<commit_message>
Añadido el saltar intro
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
+++ b/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
@@ -471,7 +471,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,8 +537,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,6 +589,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="30">
     <border>
@@ -987,7 +1001,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1231,15 +1245,57 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1255,52 +1311,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1335,7 +1358,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1363,16 +1385,16 @@
                   <c:v>89.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89.199999999999989</c:v>
+                  <c:v>89.149999999999991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89.199999999999989</c:v>
+                  <c:v>89.149999999999991</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>89.199999999999989</c:v>
+                  <c:v>89.149999999999991</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89.199999999999989</c:v>
+                  <c:v>89.149999999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1388,11 +1410,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1654616272"/>
-        <c:axId val="1654616816"/>
+        <c:axId val="-1258213216"/>
+        <c:axId val="-1258201792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1654616272"/>
+        <c:axId val="-1258213216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1401,7 +1423,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1654616816"/>
+        <c:crossAx val="-1258201792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1409,7 +1431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1654616816"/>
+        <c:axId val="-1258201792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1420,14 +1442,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1654616272"/>
+        <c:crossAx val="-1258213216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1766,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1797,19 +1818,19 @@
       <c r="J2" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
-      <c r="N2" s="108"/>
-      <c r="O2" s="108"/>
-      <c r="P2" s="108"/>
-      <c r="Q2" s="108"/>
-      <c r="R2" s="108"/>
-      <c r="S2" s="108"/>
-      <c r="T2" s="108"/>
-      <c r="U2" s="108"/>
-      <c r="V2" s="108"/>
-      <c r="W2" s="109"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98"/>
+      <c r="S2" s="98"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="98"/>
+      <c r="V2" s="98"/>
+      <c r="W2" s="99"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="64" t="s">
@@ -1880,7 +1901,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="100" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="42" t="s">
@@ -1921,7 +1942,7 @@
       <c r="W4" s="49"/>
     </row>
     <row r="5" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="104"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="37" t="s">
         <v>101</v>
       </c>
@@ -1960,7 +1981,7 @@
       <c r="W5" s="20"/>
     </row>
     <row r="6" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="104"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="37" t="s">
         <v>102</v>
       </c>
@@ -1999,7 +2020,7 @@
       <c r="W6" s="20"/>
     </row>
     <row r="7" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="104"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="37" t="s">
         <v>103</v>
       </c>
@@ -2038,7 +2059,7 @@
       <c r="W7" s="20"/>
     </row>
     <row r="8" spans="1:23" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="105"/>
+      <c r="B8" s="102"/>
       <c r="C8" s="50" t="s">
         <v>112</v>
       </c>
@@ -2077,7 +2098,7 @@
       <c r="W8" s="26"/>
     </row>
     <row r="9" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="103" t="s">
+      <c r="B9" s="100" t="s">
         <v>106</v>
       </c>
       <c r="C9" s="53" t="s">
@@ -2118,7 +2139,7 @@
       <c r="W9" s="57"/>
     </row>
     <row r="10" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="104"/>
+      <c r="B10" s="101"/>
       <c r="C10" s="36" t="s">
         <v>107</v>
       </c>
@@ -2157,7 +2178,7 @@
       <c r="W10" s="20"/>
     </row>
     <row r="11" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="104"/>
+      <c r="B11" s="101"/>
       <c r="C11" s="58" t="s">
         <v>113</v>
       </c>
@@ -2196,7 +2217,7 @@
       <c r="W11" s="20"/>
     </row>
     <row r="12" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="104"/>
+      <c r="B12" s="101"/>
       <c r="C12" s="58" t="s">
         <v>114</v>
       </c>
@@ -2215,27 +2236,53 @@
       </c>
       <c r="I12" s="63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J12" s="82">
         <v>0</v>
       </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="20"/>
+      <c r="K12" s="120">
+        <v>0.05</v>
+      </c>
+      <c r="L12" s="120">
+        <v>0</v>
+      </c>
+      <c r="M12" s="120">
+        <v>0</v>
+      </c>
+      <c r="N12" s="120">
+        <v>0</v>
+      </c>
+      <c r="O12" s="120">
+        <v>0</v>
+      </c>
+      <c r="P12" s="120">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="120">
+        <v>0</v>
+      </c>
+      <c r="R12" s="120">
+        <v>0</v>
+      </c>
+      <c r="S12" s="120">
+        <v>0</v>
+      </c>
+      <c r="T12" s="120">
+        <v>0</v>
+      </c>
+      <c r="U12" s="120">
+        <v>0</v>
+      </c>
+      <c r="V12" s="120">
+        <v>0</v>
+      </c>
+      <c r="W12" s="121">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="104"/>
+      <c r="B13" s="101"/>
       <c r="C13" s="58" t="s">
         <v>108</v>
       </c>
@@ -2259,7 +2306,7 @@
       <c r="J13" s="82">
         <v>0</v>
       </c>
-      <c r="K13" s="4"/>
+      <c r="K13" s="119"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
@@ -2274,7 +2321,7 @@
       <c r="W13" s="20"/>
     </row>
     <row r="14" spans="1:23" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="105"/>
+      <c r="B14" s="102"/>
       <c r="C14" s="59" t="s">
         <v>97</v>
       </c>
@@ -2313,7 +2360,7 @@
       <c r="W14" s="26"/>
     </row>
     <row r="15" spans="1:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B15" s="100" t="s">
+      <c r="B15" s="114" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="60" t="s">
@@ -2356,8 +2403,8 @@
       <c r="W15" s="57"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B16" s="101"/>
-      <c r="C16" s="112" t="s">
+      <c r="B16" s="115"/>
+      <c r="C16" s="105" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -2397,8 +2444,8 @@
       <c r="W16" s="20"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B17" s="101"/>
-      <c r="C17" s="113"/>
+      <c r="B17" s="115"/>
+      <c r="C17" s="106"/>
       <c r="D17" s="4" t="s">
         <v>20</v>
       </c>
@@ -2436,8 +2483,8 @@
       <c r="W17" s="20"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B18" s="101"/>
-      <c r="C18" s="113"/>
+      <c r="B18" s="115"/>
+      <c r="C18" s="106"/>
       <c r="D18" s="4" t="s">
         <v>21</v>
       </c>
@@ -2475,8 +2522,8 @@
       <c r="W18" s="20"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B19" s="101"/>
-      <c r="C19" s="113"/>
+      <c r="B19" s="115"/>
+      <c r="C19" s="106"/>
       <c r="D19" s="4" t="s">
         <v>22</v>
       </c>
@@ -2514,8 +2561,8 @@
       <c r="W19" s="20"/>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B20" s="101"/>
-      <c r="C20" s="113"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="106"/>
       <c r="D20" s="4" t="s">
         <v>23</v>
       </c>
@@ -2553,8 +2600,8 @@
       <c r="W20" s="20"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B21" s="101"/>
-      <c r="C21" s="113"/>
+      <c r="B21" s="115"/>
+      <c r="C21" s="106"/>
       <c r="D21" s="4" t="s">
         <v>24</v>
       </c>
@@ -2592,8 +2639,8 @@
       <c r="W21" s="20"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B22" s="101"/>
-      <c r="C22" s="113"/>
+      <c r="B22" s="115"/>
+      <c r="C22" s="106"/>
       <c r="D22" s="34" t="s">
         <v>36</v>
       </c>
@@ -2631,8 +2678,8 @@
       <c r="W22" s="20"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B23" s="101"/>
-      <c r="C23" s="113"/>
+      <c r="B23" s="115"/>
+      <c r="C23" s="106"/>
       <c r="D23" s="34" t="s">
         <v>37</v>
       </c>
@@ -2670,8 +2717,8 @@
       <c r="W23" s="20"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B24" s="101"/>
-      <c r="C24" s="113"/>
+      <c r="B24" s="115"/>
+      <c r="C24" s="106"/>
       <c r="D24" s="34" t="s">
         <v>38</v>
       </c>
@@ -2709,8 +2756,8 @@
       <c r="W24" s="20"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B25" s="101"/>
-      <c r="C25" s="113"/>
+      <c r="B25" s="115"/>
+      <c r="C25" s="106"/>
       <c r="D25" s="34" t="s">
         <v>39</v>
       </c>
@@ -2748,8 +2795,8 @@
       <c r="W25" s="20"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B26" s="101"/>
-      <c r="C26" s="113"/>
+      <c r="B26" s="115"/>
+      <c r="C26" s="106"/>
       <c r="D26" s="34" t="s">
         <v>40</v>
       </c>
@@ -2787,8 +2834,8 @@
       <c r="W26" s="20"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B27" s="101"/>
-      <c r="C27" s="113"/>
+      <c r="B27" s="115"/>
+      <c r="C27" s="106"/>
       <c r="D27" s="34" t="s">
         <v>41</v>
       </c>
@@ -2826,8 +2873,8 @@
       <c r="W27" s="20"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B28" s="101"/>
-      <c r="C28" s="113"/>
+      <c r="B28" s="115"/>
+      <c r="C28" s="106"/>
       <c r="D28" s="34" t="s">
         <v>42</v>
       </c>
@@ -2865,8 +2912,8 @@
       <c r="W28" s="20"/>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B29" s="101"/>
-      <c r="C29" s="113"/>
+      <c r="B29" s="115"/>
+      <c r="C29" s="106"/>
       <c r="D29" s="34" t="s">
         <v>43</v>
       </c>
@@ -2904,8 +2951,8 @@
       <c r="W29" s="20"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B30" s="101"/>
-      <c r="C30" s="113"/>
+      <c r="B30" s="115"/>
+      <c r="C30" s="106"/>
       <c r="D30" s="34" t="s">
         <v>44</v>
       </c>
@@ -2943,8 +2990,8 @@
       <c r="W30" s="20"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B31" s="101"/>
-      <c r="C31" s="113"/>
+      <c r="B31" s="115"/>
+      <c r="C31" s="106"/>
       <c r="D31" s="34" t="s">
         <v>45</v>
       </c>
@@ -2982,8 +3029,8 @@
       <c r="W31" s="20"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B32" s="101"/>
-      <c r="C32" s="113"/>
+      <c r="B32" s="115"/>
+      <c r="C32" s="106"/>
       <c r="D32" s="34" t="s">
         <v>46</v>
       </c>
@@ -3021,8 +3068,8 @@
       <c r="W32" s="20"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B33" s="101"/>
-      <c r="C33" s="113"/>
+      <c r="B33" s="115"/>
+      <c r="C33" s="106"/>
       <c r="D33" s="34" t="s">
         <v>47</v>
       </c>
@@ -3060,8 +3107,8 @@
       <c r="W33" s="20"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B34" s="101"/>
-      <c r="C34" s="113"/>
+      <c r="B34" s="115"/>
+      <c r="C34" s="106"/>
       <c r="D34" s="34" t="s">
         <v>48</v>
       </c>
@@ -3099,8 +3146,8 @@
       <c r="W34" s="20"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B35" s="101"/>
-      <c r="C35" s="113"/>
+      <c r="B35" s="115"/>
+      <c r="C35" s="106"/>
       <c r="D35" s="34" t="s">
         <v>49</v>
       </c>
@@ -3138,8 +3185,8 @@
       <c r="W35" s="20"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B36" s="101"/>
-      <c r="C36" s="113"/>
+      <c r="B36" s="115"/>
+      <c r="C36" s="106"/>
       <c r="D36" s="34" t="s">
         <v>50</v>
       </c>
@@ -3177,8 +3224,8 @@
       <c r="W36" s="20"/>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B37" s="101"/>
-      <c r="C37" s="113"/>
+      <c r="B37" s="115"/>
+      <c r="C37" s="106"/>
       <c r="D37" s="34" t="s">
         <v>51</v>
       </c>
@@ -3216,8 +3263,8 @@
       <c r="W37" s="20"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B38" s="101"/>
-      <c r="C38" s="113"/>
+      <c r="B38" s="115"/>
+      <c r="C38" s="106"/>
       <c r="D38" s="34" t="s">
         <v>52</v>
       </c>
@@ -3255,8 +3302,8 @@
       <c r="W38" s="20"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B39" s="101"/>
-      <c r="C39" s="113"/>
+      <c r="B39" s="115"/>
+      <c r="C39" s="106"/>
       <c r="D39" s="34" t="s">
         <v>53</v>
       </c>
@@ -3294,8 +3341,8 @@
       <c r="W39" s="20"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B40" s="101"/>
-      <c r="C40" s="113"/>
+      <c r="B40" s="115"/>
+      <c r="C40" s="106"/>
       <c r="D40" s="34" t="s">
         <v>54</v>
       </c>
@@ -3333,8 +3380,8 @@
       <c r="W40" s="20"/>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B41" s="101"/>
-      <c r="C41" s="113"/>
+      <c r="B41" s="115"/>
+      <c r="C41" s="106"/>
       <c r="D41" s="34" t="s">
         <v>55</v>
       </c>
@@ -3372,8 +3419,8 @@
       <c r="W41" s="20"/>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B42" s="101"/>
-      <c r="C42" s="113"/>
+      <c r="B42" s="115"/>
+      <c r="C42" s="106"/>
       <c r="D42" s="34" t="s">
         <v>56</v>
       </c>
@@ -3411,8 +3458,8 @@
       <c r="W42" s="20"/>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B43" s="101"/>
-      <c r="C43" s="113"/>
+      <c r="B43" s="115"/>
+      <c r="C43" s="106"/>
       <c r="D43" s="34" t="s">
         <v>57</v>
       </c>
@@ -3450,8 +3497,8 @@
       <c r="W43" s="20"/>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B44" s="101"/>
-      <c r="C44" s="113"/>
+      <c r="B44" s="115"/>
+      <c r="C44" s="106"/>
       <c r="D44" s="34" t="s">
         <v>58</v>
       </c>
@@ -3489,8 +3536,8 @@
       <c r="W44" s="20"/>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B45" s="101"/>
-      <c r="C45" s="113"/>
+      <c r="B45" s="115"/>
+      <c r="C45" s="106"/>
       <c r="D45" s="34" t="s">
         <v>59</v>
       </c>
@@ -3528,8 +3575,8 @@
       <c r="W45" s="20"/>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B46" s="101"/>
-      <c r="C46" s="113"/>
+      <c r="B46" s="115"/>
+      <c r="C46" s="106"/>
       <c r="D46" s="34" t="s">
         <v>60</v>
       </c>
@@ -3567,8 +3614,8 @@
       <c r="W46" s="20"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B47" s="101"/>
-      <c r="C47" s="113"/>
+      <c r="B47" s="115"/>
+      <c r="C47" s="106"/>
       <c r="D47" s="34" t="s">
         <v>61</v>
       </c>
@@ -3606,8 +3653,8 @@
       <c r="W47" s="20"/>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B48" s="101"/>
-      <c r="C48" s="113"/>
+      <c r="B48" s="115"/>
+      <c r="C48" s="106"/>
       <c r="D48" s="34" t="s">
         <v>62</v>
       </c>
@@ -3645,8 +3692,8 @@
       <c r="W48" s="20"/>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B49" s="101"/>
-      <c r="C49" s="113"/>
+      <c r="B49" s="115"/>
+      <c r="C49" s="106"/>
       <c r="D49" s="34" t="s">
         <v>63</v>
       </c>
@@ -3684,8 +3731,8 @@
       <c r="W49" s="20"/>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B50" s="101"/>
-      <c r="C50" s="113"/>
+      <c r="B50" s="115"/>
+      <c r="C50" s="106"/>
       <c r="D50" s="34" t="s">
         <v>64</v>
       </c>
@@ -3723,8 +3770,8 @@
       <c r="W50" s="20"/>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B51" s="101"/>
-      <c r="C51" s="113"/>
+      <c r="B51" s="115"/>
+      <c r="C51" s="106"/>
       <c r="D51" s="34" t="s">
         <v>65</v>
       </c>
@@ -3762,8 +3809,8 @@
       <c r="W51" s="20"/>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B52" s="101"/>
-      <c r="C52" s="113"/>
+      <c r="B52" s="115"/>
+      <c r="C52" s="106"/>
       <c r="D52" s="34" t="s">
         <v>66</v>
       </c>
@@ -3801,8 +3848,8 @@
       <c r="W52" s="20"/>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B53" s="101"/>
-      <c r="C53" s="113"/>
+      <c r="B53" s="115"/>
+      <c r="C53" s="106"/>
       <c r="D53" s="34" t="s">
         <v>67</v>
       </c>
@@ -3840,8 +3887,8 @@
       <c r="W53" s="20"/>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B54" s="101"/>
-      <c r="C54" s="113"/>
+      <c r="B54" s="115"/>
+      <c r="C54" s="106"/>
       <c r="D54" s="34" t="s">
         <v>68</v>
       </c>
@@ -3879,8 +3926,8 @@
       <c r="W54" s="20"/>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B55" s="101"/>
-      <c r="C55" s="114"/>
+      <c r="B55" s="115"/>
+      <c r="C55" s="107"/>
       <c r="D55" s="34" t="s">
         <v>69</v>
       </c>
@@ -3918,8 +3965,8 @@
       <c r="W55" s="20"/>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B56" s="101"/>
-      <c r="C56" s="110" t="s">
+      <c r="B56" s="115"/>
+      <c r="C56" s="103" t="s">
         <v>26</v>
       </c>
       <c r="D56" s="31" t="s">
@@ -3959,8 +4006,8 @@
       <c r="W56" s="20"/>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B57" s="101"/>
-      <c r="C57" s="111"/>
+      <c r="B57" s="115"/>
+      <c r="C57" s="104"/>
       <c r="D57" s="31" t="s">
         <v>29</v>
       </c>
@@ -3998,8 +4045,8 @@
       <c r="W57" s="20"/>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B58" s="101"/>
-      <c r="C58" s="111"/>
+      <c r="B58" s="115"/>
+      <c r="C58" s="104"/>
       <c r="D58" s="31" t="s">
         <v>30</v>
       </c>
@@ -4037,8 +4084,8 @@
       <c r="W58" s="20"/>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B59" s="101"/>
-      <c r="C59" s="111"/>
+      <c r="B59" s="115"/>
+      <c r="C59" s="104"/>
       <c r="D59" s="31" t="s">
         <v>31</v>
       </c>
@@ -4076,8 +4123,8 @@
       <c r="W59" s="20"/>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B60" s="101"/>
-      <c r="C60" s="111"/>
+      <c r="B60" s="115"/>
+      <c r="C60" s="104"/>
       <c r="D60" s="31" t="s">
         <v>34</v>
       </c>
@@ -4115,8 +4162,8 @@
       <c r="W60" s="20"/>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B61" s="101"/>
-      <c r="C61" s="111"/>
+      <c r="B61" s="115"/>
+      <c r="C61" s="104"/>
       <c r="D61" s="31" t="s">
         <v>32</v>
       </c>
@@ -4154,8 +4201,8 @@
       <c r="W61" s="20"/>
     </row>
     <row r="62" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="102"/>
-      <c r="C62" s="111"/>
+      <c r="B62" s="116"/>
+      <c r="C62" s="104"/>
       <c r="D62" s="74" t="s">
         <v>33</v>
       </c>
@@ -4193,10 +4240,10 @@
       <c r="W62" s="29"/>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B63" s="103" t="s">
+      <c r="B63" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="115" t="s">
+      <c r="C63" s="108" t="s">
         <v>79</v>
       </c>
       <c r="D63" s="44" t="s">
@@ -4236,8 +4283,8 @@
       <c r="W63" s="57"/>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B64" s="104"/>
-      <c r="C64" s="113"/>
+      <c r="B64" s="101"/>
+      <c r="C64" s="106"/>
       <c r="D64" s="4" t="s">
         <v>71</v>
       </c>
@@ -4275,8 +4322,8 @@
       <c r="W64" s="20"/>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B65" s="104"/>
-      <c r="C65" s="113"/>
+      <c r="B65" s="101"/>
+      <c r="C65" s="106"/>
       <c r="D65" s="4" t="s">
         <v>72</v>
       </c>
@@ -4314,8 +4361,8 @@
       <c r="W65" s="20"/>
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B66" s="104"/>
-      <c r="C66" s="114"/>
+      <c r="B66" s="101"/>
+      <c r="C66" s="107"/>
       <c r="D66" s="31" t="s">
         <v>76</v>
       </c>
@@ -4353,7 +4400,7 @@
       <c r="W66" s="20"/>
     </row>
     <row r="67" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B67" s="104"/>
+      <c r="B67" s="101"/>
       <c r="C67" s="35" t="s">
         <v>73</v>
       </c>
@@ -4392,7 +4439,7 @@
       <c r="W67" s="20"/>
     </row>
     <row r="68" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B68" s="104"/>
+      <c r="B68" s="101"/>
       <c r="C68" s="61" t="s">
         <v>81</v>
       </c>
@@ -4431,8 +4478,8 @@
       <c r="W68" s="20"/>
     </row>
     <row r="69" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="104"/>
-      <c r="C69" s="112" t="s">
+      <c r="B69" s="101"/>
+      <c r="C69" s="105" t="s">
         <v>80</v>
       </c>
       <c r="D69" s="4" t="s">
@@ -4472,8 +4519,8 @@
       <c r="W69" s="20"/>
     </row>
     <row r="70" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="104"/>
-      <c r="C70" s="113"/>
+      <c r="B70" s="101"/>
+      <c r="C70" s="106"/>
       <c r="D70" s="4" t="s">
         <v>75</v>
       </c>
@@ -4511,8 +4558,8 @@
       <c r="W70" s="20"/>
     </row>
     <row r="71" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="104"/>
-      <c r="C71" s="113"/>
+      <c r="B71" s="101"/>
+      <c r="C71" s="106"/>
       <c r="D71" s="4" t="s">
         <v>77</v>
       </c>
@@ -4550,8 +4597,8 @@
       <c r="W71" s="20"/>
     </row>
     <row r="72" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="105"/>
-      <c r="C72" s="116"/>
+      <c r="B72" s="102"/>
+      <c r="C72" s="109"/>
       <c r="D72" s="25" t="s">
         <v>78</v>
       </c>
@@ -4589,10 +4636,10 @@
       <c r="W72" s="26"/>
     </row>
     <row r="73" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="100" t="s">
+      <c r="B73" s="114" t="s">
         <v>117</v>
       </c>
-      <c r="C73" s="118" t="s">
+      <c r="C73" s="95" t="s">
         <v>118</v>
       </c>
       <c r="D73" s="44" t="s">
@@ -4632,8 +4679,8 @@
       <c r="W73" s="57"/>
     </row>
     <row r="74" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="101"/>
-      <c r="C74" s="106"/>
+      <c r="B74" s="115"/>
+      <c r="C74" s="96"/>
       <c r="D74" s="4" t="s">
         <v>134</v>
       </c>
@@ -4671,8 +4718,8 @@
       <c r="W74" s="20"/>
     </row>
     <row r="75" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="101"/>
-      <c r="C75" s="106"/>
+      <c r="B75" s="115"/>
+      <c r="C75" s="96"/>
       <c r="D75" s="4" t="s">
         <v>135</v>
       </c>
@@ -4710,8 +4757,8 @@
       <c r="W75" s="20"/>
     </row>
     <row r="76" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="101"/>
-      <c r="C76" s="106"/>
+      <c r="B76" s="115"/>
+      <c r="C76" s="96"/>
       <c r="D76" s="4" t="s">
         <v>136</v>
       </c>
@@ -4749,8 +4796,8 @@
       <c r="W76" s="20"/>
     </row>
     <row r="77" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="101"/>
-      <c r="C77" s="106" t="s">
+      <c r="B77" s="115"/>
+      <c r="C77" s="96" t="s">
         <v>119</v>
       </c>
       <c r="D77" s="4" t="s">
@@ -4790,8 +4837,8 @@
       <c r="W77" s="20"/>
     </row>
     <row r="78" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="101"/>
-      <c r="C78" s="106"/>
+      <c r="B78" s="115"/>
+      <c r="C78" s="96"/>
       <c r="D78" s="4" t="s">
         <v>134</v>
       </c>
@@ -4829,8 +4876,8 @@
       <c r="W78" s="20"/>
     </row>
     <row r="79" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="101"/>
-      <c r="C79" s="106"/>
+      <c r="B79" s="115"/>
+      <c r="C79" s="96"/>
       <c r="D79" s="4" t="s">
         <v>135</v>
       </c>
@@ -4868,8 +4915,8 @@
       <c r="W79" s="20"/>
     </row>
     <row r="80" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="101"/>
-      <c r="C80" s="106"/>
+      <c r="B80" s="115"/>
+      <c r="C80" s="96"/>
       <c r="D80" s="4" t="s">
         <v>136</v>
       </c>
@@ -4907,8 +4954,8 @@
       <c r="W80" s="20"/>
     </row>
     <row r="81" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="101"/>
-      <c r="C81" s="106" t="s">
+      <c r="B81" s="115"/>
+      <c r="C81" s="96" t="s">
         <v>120</v>
       </c>
       <c r="D81" s="4" t="s">
@@ -4948,8 +4995,8 @@
       <c r="W81" s="20"/>
     </row>
     <row r="82" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="101"/>
-      <c r="C82" s="106"/>
+      <c r="B82" s="115"/>
+      <c r="C82" s="96"/>
       <c r="D82" s="4" t="s">
         <v>134</v>
       </c>
@@ -4987,8 +5034,8 @@
       <c r="W82" s="20"/>
     </row>
     <row r="83" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="101"/>
-      <c r="C83" s="106"/>
+      <c r="B83" s="115"/>
+      <c r="C83" s="96"/>
       <c r="D83" s="4" t="s">
         <v>135</v>
       </c>
@@ -5026,8 +5073,8 @@
       <c r="W83" s="20"/>
     </row>
     <row r="84" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="101"/>
-      <c r="C84" s="106"/>
+      <c r="B84" s="115"/>
+      <c r="C84" s="96"/>
       <c r="D84" s="4" t="s">
         <v>136</v>
       </c>
@@ -5065,8 +5112,8 @@
       <c r="W84" s="20"/>
     </row>
     <row r="85" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="101"/>
-      <c r="C85" s="106" t="s">
+      <c r="B85" s="115"/>
+      <c r="C85" s="96" t="s">
         <v>121</v>
       </c>
       <c r="D85" s="4" t="s">
@@ -5106,8 +5153,8 @@
       <c r="W85" s="20"/>
     </row>
     <row r="86" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="101"/>
-      <c r="C86" s="106"/>
+      <c r="B86" s="115"/>
+      <c r="C86" s="96"/>
       <c r="D86" s="4" t="s">
         <v>134</v>
       </c>
@@ -5145,8 +5192,8 @@
       <c r="W86" s="20"/>
     </row>
     <row r="87" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="101"/>
-      <c r="C87" s="106"/>
+      <c r="B87" s="115"/>
+      <c r="C87" s="96"/>
       <c r="D87" s="4" t="s">
         <v>135</v>
       </c>
@@ -5184,8 +5231,8 @@
       <c r="W87" s="20"/>
     </row>
     <row r="88" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="101"/>
-      <c r="C88" s="106"/>
+      <c r="B88" s="115"/>
+      <c r="C88" s="96"/>
       <c r="D88" s="4" t="s">
         <v>136</v>
       </c>
@@ -5223,8 +5270,8 @@
       <c r="W88" s="20"/>
     </row>
     <row r="89" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="101"/>
-      <c r="C89" s="106" t="s">
+      <c r="B89" s="115"/>
+      <c r="C89" s="96" t="s">
         <v>122</v>
       </c>
       <c r="D89" s="4" t="s">
@@ -5264,8 +5311,8 @@
       <c r="W89" s="20"/>
     </row>
     <row r="90" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="101"/>
-      <c r="C90" s="106"/>
+      <c r="B90" s="115"/>
+      <c r="C90" s="96"/>
       <c r="D90" s="4" t="s">
         <v>134</v>
       </c>
@@ -5303,8 +5350,8 @@
       <c r="W90" s="20"/>
     </row>
     <row r="91" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="101"/>
-      <c r="C91" s="106"/>
+      <c r="B91" s="115"/>
+      <c r="C91" s="96"/>
       <c r="D91" s="4" t="s">
         <v>135</v>
       </c>
@@ -5342,8 +5389,8 @@
       <c r="W91" s="20"/>
     </row>
     <row r="92" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="101"/>
-      <c r="C92" s="106"/>
+      <c r="B92" s="115"/>
+      <c r="C92" s="96"/>
       <c r="D92" s="4" t="s">
         <v>136</v>
       </c>
@@ -5381,8 +5428,8 @@
       <c r="W92" s="20"/>
     </row>
     <row r="93" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="101"/>
-      <c r="C93" s="106" t="s">
+      <c r="B93" s="115"/>
+      <c r="C93" s="96" t="s">
         <v>123</v>
       </c>
       <c r="D93" s="4" t="s">
@@ -5422,8 +5469,8 @@
       <c r="W93" s="20"/>
     </row>
     <row r="94" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="101"/>
-      <c r="C94" s="106"/>
+      <c r="B94" s="115"/>
+      <c r="C94" s="96"/>
       <c r="D94" s="4" t="s">
         <v>134</v>
       </c>
@@ -5461,8 +5508,8 @@
       <c r="W94" s="20"/>
     </row>
     <row r="95" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="101"/>
-      <c r="C95" s="106"/>
+      <c r="B95" s="115"/>
+      <c r="C95" s="96"/>
       <c r="D95" s="4" t="s">
         <v>135</v>
       </c>
@@ -5500,8 +5547,8 @@
       <c r="W95" s="20"/>
     </row>
     <row r="96" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="101"/>
-      <c r="C96" s="106"/>
+      <c r="B96" s="115"/>
+      <c r="C96" s="96"/>
       <c r="D96" s="4" t="s">
         <v>136</v>
       </c>
@@ -5539,8 +5586,8 @@
       <c r="W96" s="20"/>
     </row>
     <row r="97" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="101"/>
-      <c r="C97" s="106" t="s">
+      <c r="B97" s="115"/>
+      <c r="C97" s="96" t="s">
         <v>124</v>
       </c>
       <c r="D97" s="4" t="s">
@@ -5580,8 +5627,8 @@
       <c r="W97" s="20"/>
     </row>
     <row r="98" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="101"/>
-      <c r="C98" s="106"/>
+      <c r="B98" s="115"/>
+      <c r="C98" s="96"/>
       <c r="D98" s="4" t="s">
         <v>134</v>
       </c>
@@ -5619,8 +5666,8 @@
       <c r="W98" s="20"/>
     </row>
     <row r="99" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="101"/>
-      <c r="C99" s="106"/>
+      <c r="B99" s="115"/>
+      <c r="C99" s="96"/>
       <c r="D99" s="4" t="s">
         <v>135</v>
       </c>
@@ -5658,8 +5705,8 @@
       <c r="W99" s="20"/>
     </row>
     <row r="100" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="101"/>
-      <c r="C100" s="106"/>
+      <c r="B100" s="115"/>
+      <c r="C100" s="96"/>
       <c r="D100" s="4" t="s">
         <v>136</v>
       </c>
@@ -5697,8 +5744,8 @@
       <c r="W100" s="20"/>
     </row>
     <row r="101" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="101"/>
-      <c r="C101" s="106" t="s">
+      <c r="B101" s="115"/>
+      <c r="C101" s="96" t="s">
         <v>125</v>
       </c>
       <c r="D101" s="4" t="s">
@@ -5738,8 +5785,8 @@
       <c r="W101" s="20"/>
     </row>
     <row r="102" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="101"/>
-      <c r="C102" s="106"/>
+      <c r="B102" s="115"/>
+      <c r="C102" s="96"/>
       <c r="D102" s="4" t="s">
         <v>134</v>
       </c>
@@ -5777,8 +5824,8 @@
       <c r="W102" s="20"/>
     </row>
     <row r="103" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="101"/>
-      <c r="C103" s="106"/>
+      <c r="B103" s="115"/>
+      <c r="C103" s="96"/>
       <c r="D103" s="4" t="s">
         <v>135</v>
       </c>
@@ -5816,8 +5863,8 @@
       <c r="W103" s="20"/>
     </row>
     <row r="104" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="101"/>
-      <c r="C104" s="106"/>
+      <c r="B104" s="115"/>
+      <c r="C104" s="96"/>
       <c r="D104" s="4" t="s">
         <v>136</v>
       </c>
@@ -5855,8 +5902,8 @@
       <c r="W104" s="20"/>
     </row>
     <row r="105" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="101"/>
-      <c r="C105" s="106" t="s">
+      <c r="B105" s="115"/>
+      <c r="C105" s="96" t="s">
         <v>126</v>
       </c>
       <c r="D105" s="4" t="s">
@@ -5896,8 +5943,8 @@
       <c r="W105" s="20"/>
     </row>
     <row r="106" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="101"/>
-      <c r="C106" s="106"/>
+      <c r="B106" s="115"/>
+      <c r="C106" s="96"/>
       <c r="D106" s="4" t="s">
         <v>134</v>
       </c>
@@ -5935,8 +5982,8 @@
       <c r="W106" s="20"/>
     </row>
     <row r="107" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="101"/>
-      <c r="C107" s="106"/>
+      <c r="B107" s="115"/>
+      <c r="C107" s="96"/>
       <c r="D107" s="4" t="s">
         <v>135</v>
       </c>
@@ -5974,8 +6021,8 @@
       <c r="W107" s="20"/>
     </row>
     <row r="108" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="101"/>
-      <c r="C108" s="106"/>
+      <c r="B108" s="115"/>
+      <c r="C108" s="96"/>
       <c r="D108" s="4" t="s">
         <v>136</v>
       </c>
@@ -6013,8 +6060,8 @@
       <c r="W108" s="20"/>
     </row>
     <row r="109" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="101"/>
-      <c r="C109" s="106" t="s">
+      <c r="B109" s="115"/>
+      <c r="C109" s="96" t="s">
         <v>127</v>
       </c>
       <c r="D109" s="4" t="s">
@@ -6054,8 +6101,8 @@
       <c r="W109" s="20"/>
     </row>
     <row r="110" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="101"/>
-      <c r="C110" s="106"/>
+      <c r="B110" s="115"/>
+      <c r="C110" s="96"/>
       <c r="D110" s="4" t="s">
         <v>134</v>
       </c>
@@ -6093,8 +6140,8 @@
       <c r="W110" s="20"/>
     </row>
     <row r="111" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="101"/>
-      <c r="C111" s="106"/>
+      <c r="B111" s="115"/>
+      <c r="C111" s="96"/>
       <c r="D111" s="4" t="s">
         <v>135</v>
       </c>
@@ -6132,8 +6179,8 @@
       <c r="W111" s="20"/>
     </row>
     <row r="112" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="101"/>
-      <c r="C112" s="106"/>
+      <c r="B112" s="115"/>
+      <c r="C112" s="96"/>
       <c r="D112" s="4" t="s">
         <v>136</v>
       </c>
@@ -6171,8 +6218,8 @@
       <c r="W112" s="20"/>
     </row>
     <row r="113" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="101"/>
-      <c r="C113" s="106" t="s">
+      <c r="B113" s="115"/>
+      <c r="C113" s="96" t="s">
         <v>128</v>
       </c>
       <c r="D113" s="4" t="s">
@@ -6212,8 +6259,8 @@
       <c r="W113" s="20"/>
     </row>
     <row r="114" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="101"/>
-      <c r="C114" s="106"/>
+      <c r="B114" s="115"/>
+      <c r="C114" s="96"/>
       <c r="D114" s="4" t="s">
         <v>134</v>
       </c>
@@ -6251,8 +6298,8 @@
       <c r="W114" s="20"/>
     </row>
     <row r="115" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="101"/>
-      <c r="C115" s="106"/>
+      <c r="B115" s="115"/>
+      <c r="C115" s="96"/>
       <c r="D115" s="4" t="s">
         <v>135</v>
       </c>
@@ -6290,8 +6337,8 @@
       <c r="W115" s="20"/>
     </row>
     <row r="116" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="101"/>
-      <c r="C116" s="106"/>
+      <c r="B116" s="115"/>
+      <c r="C116" s="96"/>
       <c r="D116" s="4" t="s">
         <v>136</v>
       </c>
@@ -6329,8 +6376,8 @@
       <c r="W116" s="20"/>
     </row>
     <row r="117" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="101"/>
-      <c r="C117" s="106" t="s">
+      <c r="B117" s="115"/>
+      <c r="C117" s="96" t="s">
         <v>129</v>
       </c>
       <c r="D117" s="4" t="s">
@@ -6370,8 +6417,8 @@
       <c r="W117" s="20"/>
     </row>
     <row r="118" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="101"/>
-      <c r="C118" s="106"/>
+      <c r="B118" s="115"/>
+      <c r="C118" s="96"/>
       <c r="D118" s="4" t="s">
         <v>134</v>
       </c>
@@ -6409,8 +6456,8 @@
       <c r="W118" s="20"/>
     </row>
     <row r="119" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="101"/>
-      <c r="C119" s="106"/>
+      <c r="B119" s="115"/>
+      <c r="C119" s="96"/>
       <c r="D119" s="4" t="s">
         <v>135</v>
       </c>
@@ -6448,8 +6495,8 @@
       <c r="W119" s="20"/>
     </row>
     <row r="120" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="101"/>
-      <c r="C120" s="106"/>
+      <c r="B120" s="115"/>
+      <c r="C120" s="96"/>
       <c r="D120" s="4" t="s">
         <v>136</v>
       </c>
@@ -6487,8 +6534,8 @@
       <c r="W120" s="20"/>
     </row>
     <row r="121" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="101"/>
-      <c r="C121" s="106" t="s">
+      <c r="B121" s="115"/>
+      <c r="C121" s="96" t="s">
         <v>130</v>
       </c>
       <c r="D121" s="4" t="s">
@@ -6528,8 +6575,8 @@
       <c r="W121" s="20"/>
     </row>
     <row r="122" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="101"/>
-      <c r="C122" s="106"/>
+      <c r="B122" s="115"/>
+      <c r="C122" s="96"/>
       <c r="D122" s="4" t="s">
         <v>134</v>
       </c>
@@ -6567,8 +6614,8 @@
       <c r="W122" s="20"/>
     </row>
     <row r="123" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="101"/>
-      <c r="C123" s="106"/>
+      <c r="B123" s="115"/>
+      <c r="C123" s="96"/>
       <c r="D123" s="4" t="s">
         <v>135</v>
       </c>
@@ -6606,8 +6653,8 @@
       <c r="W123" s="20"/>
     </row>
     <row r="124" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="101"/>
-      <c r="C124" s="106"/>
+      <c r="B124" s="115"/>
+      <c r="C124" s="96"/>
       <c r="D124" s="4" t="s">
         <v>136</v>
       </c>
@@ -6645,8 +6692,8 @@
       <c r="W124" s="20"/>
     </row>
     <row r="125" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="101"/>
-      <c r="C125" s="106" t="s">
+      <c r="B125" s="115"/>
+      <c r="C125" s="96" t="s">
         <v>131</v>
       </c>
       <c r="D125" s="4" t="s">
@@ -6686,8 +6733,8 @@
       <c r="W125" s="20"/>
     </row>
     <row r="126" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="101"/>
-      <c r="C126" s="106"/>
+      <c r="B126" s="115"/>
+      <c r="C126" s="96"/>
       <c r="D126" s="4" t="s">
         <v>134</v>
       </c>
@@ -6725,8 +6772,8 @@
       <c r="W126" s="20"/>
     </row>
     <row r="127" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="101"/>
-      <c r="C127" s="106"/>
+      <c r="B127" s="115"/>
+      <c r="C127" s="96"/>
       <c r="D127" s="4" t="s">
         <v>135</v>
       </c>
@@ -6764,8 +6811,8 @@
       <c r="W127" s="20"/>
     </row>
     <row r="128" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="101"/>
-      <c r="C128" s="106"/>
+      <c r="B128" s="115"/>
+      <c r="C128" s="96"/>
       <c r="D128" s="4" t="s">
         <v>136</v>
       </c>
@@ -6803,8 +6850,8 @@
       <c r="W128" s="20"/>
     </row>
     <row r="129" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="101"/>
-      <c r="C129" s="106" t="s">
+      <c r="B129" s="115"/>
+      <c r="C129" s="96" t="s">
         <v>132</v>
       </c>
       <c r="D129" s="4" t="s">
@@ -6844,8 +6891,8 @@
       <c r="W129" s="20"/>
     </row>
     <row r="130" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="101"/>
-      <c r="C130" s="106"/>
+      <c r="B130" s="115"/>
+      <c r="C130" s="96"/>
       <c r="D130" s="4" t="s">
         <v>134</v>
       </c>
@@ -6883,8 +6930,8 @@
       <c r="W130" s="20"/>
     </row>
     <row r="131" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="101"/>
-      <c r="C131" s="106"/>
+      <c r="B131" s="115"/>
+      <c r="C131" s="96"/>
       <c r="D131" s="4" t="s">
         <v>135</v>
       </c>
@@ -6922,8 +6969,8 @@
       <c r="W131" s="20"/>
     </row>
     <row r="132" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B132" s="107"/>
-      <c r="C132" s="117"/>
+      <c r="B132" s="117"/>
+      <c r="C132" s="118"/>
       <c r="D132" s="25" t="s">
         <v>136</v>
       </c>
@@ -6940,7 +6987,7 @@
         <v>0.25</v>
       </c>
       <c r="I132" s="21">
-        <f t="shared" ref="I132:I163" si="4">SUM(J132:W132)</f>
+        <f t="shared" ref="I132:I160" si="4">SUM(J132:W132)</f>
         <v>0</v>
       </c>
       <c r="J132" s="83">
@@ -6961,7 +7008,7 @@
       <c r="W132" s="26"/>
     </row>
     <row r="133" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B133" s="103" t="s">
+      <c r="B133" s="100" t="s">
         <v>83</v>
       </c>
       <c r="C133" s="92" t="s">
@@ -7002,7 +7049,7 @@
       <c r="W133" s="57"/>
     </row>
     <row r="134" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="104"/>
+      <c r="B134" s="101"/>
       <c r="C134" s="38" t="s">
         <v>89</v>
       </c>
@@ -7041,7 +7088,7 @@
       <c r="W134" s="20"/>
     </row>
     <row r="135" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="104"/>
+      <c r="B135" s="101"/>
       <c r="C135" s="38" t="s">
         <v>90</v>
       </c>
@@ -7080,7 +7127,7 @@
       <c r="W135" s="20"/>
     </row>
     <row r="136" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="104"/>
+      <c r="B136" s="101"/>
       <c r="C136" s="38" t="s">
         <v>91</v>
       </c>
@@ -7119,7 +7166,7 @@
       <c r="W136" s="20"/>
     </row>
     <row r="137" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="104"/>
+      <c r="B137" s="101"/>
       <c r="C137" s="38" t="s">
         <v>143</v>
       </c>
@@ -7158,7 +7205,7 @@
       <c r="W137" s="20"/>
     </row>
     <row r="138" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="104"/>
+      <c r="B138" s="101"/>
       <c r="C138" s="38" t="s">
         <v>140</v>
       </c>
@@ -7197,7 +7244,7 @@
       <c r="W138" s="20"/>
     </row>
     <row r="139" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="104"/>
+      <c r="B139" s="101"/>
       <c r="C139" s="38" t="s">
         <v>142</v>
       </c>
@@ -7236,7 +7283,7 @@
       <c r="W139" s="20"/>
     </row>
     <row r="140" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="104"/>
+      <c r="B140" s="101"/>
       <c r="C140" s="38" t="s">
         <v>141</v>
       </c>
@@ -7275,7 +7322,7 @@
       <c r="W140" s="20"/>
     </row>
     <row r="141" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="104"/>
+      <c r="B141" s="101"/>
       <c r="C141" s="38" t="s">
         <v>92</v>
       </c>
@@ -7314,7 +7361,7 @@
       <c r="W141" s="20"/>
     </row>
     <row r="142" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="104"/>
+      <c r="B142" s="101"/>
       <c r="C142" s="38" t="s">
         <v>93</v>
       </c>
@@ -7353,7 +7400,7 @@
       <c r="W142" s="20"/>
     </row>
     <row r="143" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="104"/>
+      <c r="B143" s="101"/>
       <c r="C143" s="38" t="s">
         <v>94</v>
       </c>
@@ -7392,7 +7439,7 @@
       <c r="W143" s="20"/>
     </row>
     <row r="144" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="104"/>
+      <c r="B144" s="101"/>
       <c r="C144" s="38" t="s">
         <v>98</v>
       </c>
@@ -7431,7 +7478,7 @@
       <c r="W144" s="20"/>
     </row>
     <row r="145" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B145" s="105"/>
+      <c r="B145" s="102"/>
       <c r="C145" s="62" t="s">
         <v>99</v>
       </c>
@@ -7470,7 +7517,7 @@
       <c r="W145" s="26"/>
     </row>
     <row r="146" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="100" t="s">
+      <c r="B146" s="114" t="s">
         <v>144</v>
       </c>
       <c r="C146" s="72" t="s">
@@ -7511,7 +7558,7 @@
       <c r="W146" s="57"/>
     </row>
     <row r="147" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="101"/>
+      <c r="B147" s="115"/>
       <c r="C147" s="71" t="s">
         <v>145</v>
       </c>
@@ -7550,7 +7597,7 @@
       <c r="W147" s="20"/>
     </row>
     <row r="148" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="107"/>
+      <c r="B148" s="117"/>
       <c r="C148" s="73" t="s">
         <v>146</v>
       </c>
@@ -7589,7 +7636,7 @@
       <c r="W148" s="26"/>
     </row>
     <row r="149" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="104" t="s">
+      <c r="B149" s="101" t="s">
         <v>18</v>
       </c>
       <c r="C149" s="38" t="s">
@@ -7630,7 +7677,7 @@
       <c r="W149" s="70"/>
     </row>
     <row r="150" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="104"/>
+      <c r="B150" s="101"/>
       <c r="C150" s="38" t="s">
         <v>138</v>
       </c>
@@ -7669,7 +7716,7 @@
       <c r="W150" s="70"/>
     </row>
     <row r="151" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="104"/>
+      <c r="B151" s="101"/>
       <c r="C151" s="38" t="s">
         <v>139</v>
       </c>
@@ -7708,7 +7755,7 @@
       <c r="W151" s="70"/>
     </row>
     <row r="152" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="104"/>
+      <c r="B152" s="101"/>
       <c r="C152" s="38" t="s">
         <v>147</v>
       </c>
@@ -7747,7 +7794,7 @@
       <c r="W152" s="20"/>
     </row>
     <row r="153" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="104"/>
+      <c r="B153" s="101"/>
       <c r="C153" s="35" t="s">
         <v>84</v>
       </c>
@@ -7786,7 +7833,7 @@
       <c r="W153" s="20"/>
     </row>
     <row r="154" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="104"/>
+      <c r="B154" s="101"/>
       <c r="C154" s="35" t="s">
         <v>85</v>
       </c>
@@ -7825,7 +7872,7 @@
       <c r="W154" s="20"/>
     </row>
     <row r="155" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="104"/>
+      <c r="B155" s="101"/>
       <c r="C155" s="39" t="s">
         <v>87</v>
       </c>
@@ -7864,7 +7911,7 @@
       <c r="W155" s="29"/>
     </row>
     <row r="156" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="104"/>
+      <c r="B156" s="101"/>
       <c r="C156" s="35" t="s">
         <v>86</v>
       </c>
@@ -7903,7 +7950,7 @@
       <c r="W156" s="29"/>
     </row>
     <row r="157" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="104"/>
+      <c r="B157" s="101"/>
       <c r="C157" s="41" t="s">
         <v>104</v>
       </c>
@@ -7942,7 +7989,7 @@
       <c r="W157" s="29"/>
     </row>
     <row r="158" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="104"/>
+      <c r="B158" s="101"/>
       <c r="C158" s="41" t="s">
         <v>137</v>
       </c>
@@ -7981,7 +8028,7 @@
       <c r="W158" s="29"/>
     </row>
     <row r="159" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="104"/>
+      <c r="B159" s="101"/>
       <c r="C159" s="41" t="s">
         <v>105</v>
       </c>
@@ -8020,7 +8067,7 @@
       <c r="W159" s="29"/>
     </row>
     <row r="160" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B160" s="105"/>
+      <c r="B160" s="102"/>
       <c r="C160" s="62" t="s">
         <v>100</v>
       </c>
@@ -8059,21 +8106,21 @@
       <c r="W160" s="26"/>
     </row>
     <row r="161" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B161" s="95" t="s">
+      <c r="B161" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="C161" s="98"/>
-      <c r="D161" s="96"/>
-      <c r="E161" s="96"/>
-      <c r="F161" s="96"/>
-      <c r="G161" s="99"/>
+      <c r="C161" s="112"/>
+      <c r="D161" s="111"/>
+      <c r="E161" s="111"/>
+      <c r="F161" s="111"/>
+      <c r="G161" s="113"/>
       <c r="H161" s="40">
         <f>SUM(H4:H160)</f>
         <v>89.199999999999989</v>
       </c>
       <c r="I161" s="24">
         <f>SUM(I4:I160)</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J161" s="24">
         <f>SUM(J4:J160)</f>
@@ -8081,7 +8128,7 @@
       </c>
       <c r="K161" s="24">
         <f t="shared" ref="K161:W161" si="5">SUM(K4:K160)</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="L161" s="24">
         <f t="shared" si="5"/>
@@ -8144,19 +8191,19 @@
       <c r="J162" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="K162" s="108"/>
-      <c r="L162" s="108"/>
-      <c r="M162" s="108"/>
-      <c r="N162" s="108"/>
-      <c r="O162" s="108"/>
-      <c r="P162" s="108"/>
-      <c r="Q162" s="108"/>
-      <c r="R162" s="108"/>
-      <c r="S162" s="108"/>
-      <c r="T162" s="108"/>
-      <c r="U162" s="108"/>
-      <c r="V162" s="108"/>
-      <c r="W162" s="109"/>
+      <c r="K162" s="98"/>
+      <c r="L162" s="98"/>
+      <c r="M162" s="98"/>
+      <c r="N162" s="98"/>
+      <c r="O162" s="98"/>
+      <c r="P162" s="98"/>
+      <c r="Q162" s="98"/>
+      <c r="R162" s="98"/>
+      <c r="S162" s="98"/>
+      <c r="T162" s="98"/>
+      <c r="U162" s="98"/>
+      <c r="V162" s="98"/>
+      <c r="W162" s="99"/>
     </row>
     <row r="163" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B163" s="2"/>
@@ -8180,29 +8227,29 @@
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
-      <c r="H164" s="95" t="s">
+      <c r="H164" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="I164" s="96"/>
+      <c r="I164" s="111"/>
       <c r="J164" s="10">
         <f>H161-J161</f>
         <v>89.199999999999989</v>
       </c>
       <c r="K164" s="10">
         <f>J164-K161</f>
-        <v>89.199999999999989</v>
+        <v>89.149999999999991</v>
       </c>
       <c r="L164" s="10">
         <f>K164-L161</f>
-        <v>89.199999999999989</v>
+        <v>89.149999999999991</v>
       </c>
       <c r="M164" s="10">
         <f>L164-M161</f>
-        <v>89.199999999999989</v>
+        <v>89.149999999999991</v>
       </c>
       <c r="N164" s="11">
         <f>M164-N161</f>
-        <v>89.199999999999989</v>
+        <v>89.149999999999991</v>
       </c>
     </row>
     <row r="165" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8229,15 +8276,15 @@
       <c r="H166" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="I166" s="98"/>
-      <c r="J166" s="96">
+      <c r="I166" s="112"/>
+      <c r="J166" s="111">
         <f>H161-I161</f>
-        <v>89.199999999999989</v>
-      </c>
-      <c r="K166" s="96"/>
-      <c r="L166" s="96"/>
-      <c r="M166" s="96"/>
-      <c r="N166" s="99"/>
+        <v>89.149999999999991</v>
+      </c>
+      <c r="K166" s="111"/>
+      <c r="L166" s="111"/>
+      <c r="M166" s="111"/>
+      <c r="N166" s="113"/>
     </row>
     <row r="167" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B167" s="3"/>
@@ -8341,23 +8388,6 @@
     <row r="185" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C73:C76"/>
-    <mergeCell ref="C77:C80"/>
-    <mergeCell ref="C121:C124"/>
-    <mergeCell ref="C113:C116"/>
-    <mergeCell ref="C105:C108"/>
-    <mergeCell ref="C101:C104"/>
-    <mergeCell ref="C93:C96"/>
-    <mergeCell ref="C109:C112"/>
-    <mergeCell ref="C117:C120"/>
-    <mergeCell ref="J2:W2"/>
-    <mergeCell ref="B63:B72"/>
-    <mergeCell ref="C56:C62"/>
-    <mergeCell ref="C16:C55"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="C69:C72"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B14"/>
     <mergeCell ref="H164:I164"/>
     <mergeCell ref="H166:I166"/>
     <mergeCell ref="J166:N166"/>
@@ -8374,6 +8404,23 @@
     <mergeCell ref="C89:C92"/>
     <mergeCell ref="C85:C88"/>
     <mergeCell ref="C81:C84"/>
+    <mergeCell ref="J2:W2"/>
+    <mergeCell ref="B63:B72"/>
+    <mergeCell ref="C56:C62"/>
+    <mergeCell ref="C16:C55"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C69:C72"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C73:C76"/>
+    <mergeCell ref="C77:C80"/>
+    <mergeCell ref="C121:C124"/>
+    <mergeCell ref="C113:C116"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="C101:C104"/>
+    <mergeCell ref="C93:C96"/>
+    <mergeCell ref="C109:C112"/>
+    <mergeCell ref="C117:C120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Establecido un seguimiento de la zona en la que se encuentra Link en el overworld de las 35 que hay, Introducido un objeto llamado enemySpawns con un array de 35 posiciones que contiene X bools donde X es el número de enemigos que hay en dicha zona, tiene un método para ponerlos todos en true la que se llamará en el Init y cada vez que Link muera, cuando tengamos partidas guardadas ya podrá llamarse a este método con los datos guardados. Tambien se ha introducido un comentario al lado de cada declaración de bools para cuando tenga que instanciar los enemigos sea más facil, el orden de los booleanos es de derecha a izquierda y de arriba abajo (Refiriendose a la posició original de cada enemigo en la sala)
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
+++ b/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
@@ -1001,7 +1001,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1245,85 +1245,88 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1385,16 +1388,16 @@
                   <c:v>89.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89.149999999999991</c:v>
+                  <c:v>88.266699999999986</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89.149999999999991</c:v>
+                  <c:v>88.266699999999986</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>89.149999999999991</c:v>
+                  <c:v>88.266699999999986</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89.149999999999991</c:v>
+                  <c:v>88.266699999999986</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1410,11 +1413,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1258213216"/>
-        <c:axId val="-1258201792"/>
+        <c:axId val="-1291761776"/>
+        <c:axId val="-1291761232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1258213216"/>
+        <c:axId val="-1291761776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1423,7 +1426,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1258201792"/>
+        <c:crossAx val="-1291761232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1431,7 +1434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1258201792"/>
+        <c:axId val="-1291761232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1442,7 +1445,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1258213216"/>
+        <c:crossAx val="-1291761776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1787,8 +1790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W185"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1815,22 +1818,22 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="97" t="s">
+      <c r="J2" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
-      <c r="Q2" s="98"/>
-      <c r="R2" s="98"/>
-      <c r="S2" s="98"/>
-      <c r="T2" s="98"/>
-      <c r="U2" s="98"/>
-      <c r="V2" s="98"/>
-      <c r="W2" s="99"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="111"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="112"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="64" t="s">
@@ -1901,7 +1904,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="106" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="42" t="s">
@@ -1942,7 +1945,7 @@
       <c r="W4" s="49"/>
     </row>
     <row r="5" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="101"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="37" t="s">
         <v>101</v>
       </c>
@@ -1981,7 +1984,7 @@
       <c r="W5" s="20"/>
     </row>
     <row r="6" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="101"/>
+      <c r="B6" s="107"/>
       <c r="C6" s="37" t="s">
         <v>102</v>
       </c>
@@ -2020,7 +2023,7 @@
       <c r="W6" s="20"/>
     </row>
     <row r="7" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="101"/>
+      <c r="B7" s="107"/>
       <c r="C7" s="37" t="s">
         <v>103</v>
       </c>
@@ -2059,7 +2062,7 @@
       <c r="W7" s="20"/>
     </row>
     <row r="8" spans="1:23" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="102"/>
+      <c r="B8" s="108"/>
       <c r="C8" s="50" t="s">
         <v>112</v>
       </c>
@@ -2098,7 +2101,7 @@
       <c r="W8" s="26"/>
     </row>
     <row r="9" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="100" t="s">
+      <c r="B9" s="106" t="s">
         <v>106</v>
       </c>
       <c r="C9" s="53" t="s">
@@ -2139,7 +2142,7 @@
       <c r="W9" s="57"/>
     </row>
     <row r="10" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="101"/>
+      <c r="B10" s="107"/>
       <c r="C10" s="36" t="s">
         <v>107</v>
       </c>
@@ -2178,7 +2181,7 @@
       <c r="W10" s="20"/>
     </row>
     <row r="11" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="101"/>
+      <c r="B11" s="107"/>
       <c r="C11" s="58" t="s">
         <v>113</v>
       </c>
@@ -2217,7 +2220,7 @@
       <c r="W11" s="20"/>
     </row>
     <row r="12" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="101"/>
+      <c r="B12" s="107"/>
       <c r="C12" s="58" t="s">
         <v>114</v>
       </c>
@@ -2241,48 +2244,48 @@
       <c r="J12" s="82">
         <v>0</v>
       </c>
-      <c r="K12" s="120">
+      <c r="K12" s="96">
         <v>0.05</v>
       </c>
-      <c r="L12" s="120">
-        <v>0</v>
-      </c>
-      <c r="M12" s="120">
-        <v>0</v>
-      </c>
-      <c r="N12" s="120">
-        <v>0</v>
-      </c>
-      <c r="O12" s="120">
-        <v>0</v>
-      </c>
-      <c r="P12" s="120">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="120">
-        <v>0</v>
-      </c>
-      <c r="R12" s="120">
-        <v>0</v>
-      </c>
-      <c r="S12" s="120">
-        <v>0</v>
-      </c>
-      <c r="T12" s="120">
-        <v>0</v>
-      </c>
-      <c r="U12" s="120">
-        <v>0</v>
-      </c>
-      <c r="V12" s="120">
-        <v>0</v>
-      </c>
-      <c r="W12" s="121">
+      <c r="L12" s="96">
+        <v>0</v>
+      </c>
+      <c r="M12" s="96">
+        <v>0</v>
+      </c>
+      <c r="N12" s="96">
+        <v>0</v>
+      </c>
+      <c r="O12" s="96">
+        <v>0</v>
+      </c>
+      <c r="P12" s="96">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="96">
+        <v>0</v>
+      </c>
+      <c r="R12" s="96">
+        <v>0</v>
+      </c>
+      <c r="S12" s="96">
+        <v>0</v>
+      </c>
+      <c r="T12" s="96">
+        <v>0</v>
+      </c>
+      <c r="U12" s="96">
+        <v>0</v>
+      </c>
+      <c r="V12" s="96">
+        <v>0</v>
+      </c>
+      <c r="W12" s="97">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="101"/>
+      <c r="B13" s="107"/>
       <c r="C13" s="58" t="s">
         <v>108</v>
       </c>
@@ -2306,7 +2309,7 @@
       <c r="J13" s="82">
         <v>0</v>
       </c>
-      <c r="K13" s="119"/>
+      <c r="K13" s="95"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
@@ -2321,7 +2324,7 @@
       <c r="W13" s="20"/>
     </row>
     <row r="14" spans="1:23" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="102"/>
+      <c r="B14" s="108"/>
       <c r="C14" s="59" t="s">
         <v>97</v>
       </c>
@@ -2360,7 +2363,7 @@
       <c r="W14" s="26"/>
     </row>
     <row r="15" spans="1:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="103" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="60" t="s">
@@ -2383,12 +2386,14 @@
       </c>
       <c r="I15" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.88329999999999997</v>
       </c>
       <c r="J15" s="81">
         <v>0</v>
       </c>
-      <c r="K15" s="55"/>
+      <c r="K15" s="122">
+        <v>0.88329999999999997</v>
+      </c>
       <c r="L15" s="55"/>
       <c r="M15" s="55"/>
       <c r="N15" s="44"/>
@@ -2403,8 +2408,8 @@
       <c r="W15" s="57"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B16" s="115"/>
-      <c r="C16" s="105" t="s">
+      <c r="B16" s="104"/>
+      <c r="C16" s="116" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -2444,8 +2449,8 @@
       <c r="W16" s="20"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B17" s="115"/>
-      <c r="C17" s="106"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="117"/>
       <c r="D17" s="4" t="s">
         <v>20</v>
       </c>
@@ -2483,8 +2488,8 @@
       <c r="W17" s="20"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B18" s="115"/>
-      <c r="C18" s="106"/>
+      <c r="B18" s="104"/>
+      <c r="C18" s="117"/>
       <c r="D18" s="4" t="s">
         <v>21</v>
       </c>
@@ -2522,8 +2527,8 @@
       <c r="W18" s="20"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B19" s="115"/>
-      <c r="C19" s="106"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="117"/>
       <c r="D19" s="4" t="s">
         <v>22</v>
       </c>
@@ -2561,8 +2566,8 @@
       <c r="W19" s="20"/>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B20" s="115"/>
-      <c r="C20" s="106"/>
+      <c r="B20" s="104"/>
+      <c r="C20" s="117"/>
       <c r="D20" s="4" t="s">
         <v>23</v>
       </c>
@@ -2600,8 +2605,8 @@
       <c r="W20" s="20"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B21" s="115"/>
-      <c r="C21" s="106"/>
+      <c r="B21" s="104"/>
+      <c r="C21" s="117"/>
       <c r="D21" s="4" t="s">
         <v>24</v>
       </c>
@@ -2639,8 +2644,8 @@
       <c r="W21" s="20"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B22" s="115"/>
-      <c r="C22" s="106"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="117"/>
       <c r="D22" s="34" t="s">
         <v>36</v>
       </c>
@@ -2678,8 +2683,8 @@
       <c r="W22" s="20"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B23" s="115"/>
-      <c r="C23" s="106"/>
+      <c r="B23" s="104"/>
+      <c r="C23" s="117"/>
       <c r="D23" s="34" t="s">
         <v>37</v>
       </c>
@@ -2717,8 +2722,8 @@
       <c r="W23" s="20"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B24" s="115"/>
-      <c r="C24" s="106"/>
+      <c r="B24" s="104"/>
+      <c r="C24" s="117"/>
       <c r="D24" s="34" t="s">
         <v>38</v>
       </c>
@@ -2756,8 +2761,8 @@
       <c r="W24" s="20"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B25" s="115"/>
-      <c r="C25" s="106"/>
+      <c r="B25" s="104"/>
+      <c r="C25" s="117"/>
       <c r="D25" s="34" t="s">
         <v>39</v>
       </c>
@@ -2795,8 +2800,8 @@
       <c r="W25" s="20"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B26" s="115"/>
-      <c r="C26" s="106"/>
+      <c r="B26" s="104"/>
+      <c r="C26" s="117"/>
       <c r="D26" s="34" t="s">
         <v>40</v>
       </c>
@@ -2834,8 +2839,8 @@
       <c r="W26" s="20"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B27" s="115"/>
-      <c r="C27" s="106"/>
+      <c r="B27" s="104"/>
+      <c r="C27" s="117"/>
       <c r="D27" s="34" t="s">
         <v>41</v>
       </c>
@@ -2873,8 +2878,8 @@
       <c r="W27" s="20"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B28" s="115"/>
-      <c r="C28" s="106"/>
+      <c r="B28" s="104"/>
+      <c r="C28" s="117"/>
       <c r="D28" s="34" t="s">
         <v>42</v>
       </c>
@@ -2912,8 +2917,8 @@
       <c r="W28" s="20"/>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B29" s="115"/>
-      <c r="C29" s="106"/>
+      <c r="B29" s="104"/>
+      <c r="C29" s="117"/>
       <c r="D29" s="34" t="s">
         <v>43</v>
       </c>
@@ -2951,8 +2956,8 @@
       <c r="W29" s="20"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B30" s="115"/>
-      <c r="C30" s="106"/>
+      <c r="B30" s="104"/>
+      <c r="C30" s="117"/>
       <c r="D30" s="34" t="s">
         <v>44</v>
       </c>
@@ -2990,8 +2995,8 @@
       <c r="W30" s="20"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B31" s="115"/>
-      <c r="C31" s="106"/>
+      <c r="B31" s="104"/>
+      <c r="C31" s="117"/>
       <c r="D31" s="34" t="s">
         <v>45</v>
       </c>
@@ -3029,8 +3034,8 @@
       <c r="W31" s="20"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B32" s="115"/>
-      <c r="C32" s="106"/>
+      <c r="B32" s="104"/>
+      <c r="C32" s="117"/>
       <c r="D32" s="34" t="s">
         <v>46</v>
       </c>
@@ -3068,8 +3073,8 @@
       <c r="W32" s="20"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B33" s="115"/>
-      <c r="C33" s="106"/>
+      <c r="B33" s="104"/>
+      <c r="C33" s="117"/>
       <c r="D33" s="34" t="s">
         <v>47</v>
       </c>
@@ -3107,8 +3112,8 @@
       <c r="W33" s="20"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B34" s="115"/>
-      <c r="C34" s="106"/>
+      <c r="B34" s="104"/>
+      <c r="C34" s="117"/>
       <c r="D34" s="34" t="s">
         <v>48</v>
       </c>
@@ -3146,8 +3151,8 @@
       <c r="W34" s="20"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B35" s="115"/>
-      <c r="C35" s="106"/>
+      <c r="B35" s="104"/>
+      <c r="C35" s="117"/>
       <c r="D35" s="34" t="s">
         <v>49</v>
       </c>
@@ -3185,8 +3190,8 @@
       <c r="W35" s="20"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B36" s="115"/>
-      <c r="C36" s="106"/>
+      <c r="B36" s="104"/>
+      <c r="C36" s="117"/>
       <c r="D36" s="34" t="s">
         <v>50</v>
       </c>
@@ -3224,8 +3229,8 @@
       <c r="W36" s="20"/>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B37" s="115"/>
-      <c r="C37" s="106"/>
+      <c r="B37" s="104"/>
+      <c r="C37" s="117"/>
       <c r="D37" s="34" t="s">
         <v>51</v>
       </c>
@@ -3263,8 +3268,8 @@
       <c r="W37" s="20"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B38" s="115"/>
-      <c r="C38" s="106"/>
+      <c r="B38" s="104"/>
+      <c r="C38" s="117"/>
       <c r="D38" s="34" t="s">
         <v>52</v>
       </c>
@@ -3302,8 +3307,8 @@
       <c r="W38" s="20"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B39" s="115"/>
-      <c r="C39" s="106"/>
+      <c r="B39" s="104"/>
+      <c r="C39" s="117"/>
       <c r="D39" s="34" t="s">
         <v>53</v>
       </c>
@@ -3341,8 +3346,8 @@
       <c r="W39" s="20"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B40" s="115"/>
-      <c r="C40" s="106"/>
+      <c r="B40" s="104"/>
+      <c r="C40" s="117"/>
       <c r="D40" s="34" t="s">
         <v>54</v>
       </c>
@@ -3380,8 +3385,8 @@
       <c r="W40" s="20"/>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B41" s="115"/>
-      <c r="C41" s="106"/>
+      <c r="B41" s="104"/>
+      <c r="C41" s="117"/>
       <c r="D41" s="34" t="s">
         <v>55</v>
       </c>
@@ -3419,8 +3424,8 @@
       <c r="W41" s="20"/>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B42" s="115"/>
-      <c r="C42" s="106"/>
+      <c r="B42" s="104"/>
+      <c r="C42" s="117"/>
       <c r="D42" s="34" t="s">
         <v>56</v>
       </c>
@@ -3458,8 +3463,8 @@
       <c r="W42" s="20"/>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B43" s="115"/>
-      <c r="C43" s="106"/>
+      <c r="B43" s="104"/>
+      <c r="C43" s="117"/>
       <c r="D43" s="34" t="s">
         <v>57</v>
       </c>
@@ -3497,8 +3502,8 @@
       <c r="W43" s="20"/>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B44" s="115"/>
-      <c r="C44" s="106"/>
+      <c r="B44" s="104"/>
+      <c r="C44" s="117"/>
       <c r="D44" s="34" t="s">
         <v>58</v>
       </c>
@@ -3536,8 +3541,8 @@
       <c r="W44" s="20"/>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B45" s="115"/>
-      <c r="C45" s="106"/>
+      <c r="B45" s="104"/>
+      <c r="C45" s="117"/>
       <c r="D45" s="34" t="s">
         <v>59</v>
       </c>
@@ -3575,8 +3580,8 @@
       <c r="W45" s="20"/>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B46" s="115"/>
-      <c r="C46" s="106"/>
+      <c r="B46" s="104"/>
+      <c r="C46" s="117"/>
       <c r="D46" s="34" t="s">
         <v>60</v>
       </c>
@@ -3614,8 +3619,8 @@
       <c r="W46" s="20"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B47" s="115"/>
-      <c r="C47" s="106"/>
+      <c r="B47" s="104"/>
+      <c r="C47" s="117"/>
       <c r="D47" s="34" t="s">
         <v>61</v>
       </c>
@@ -3653,8 +3658,8 @@
       <c r="W47" s="20"/>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B48" s="115"/>
-      <c r="C48" s="106"/>
+      <c r="B48" s="104"/>
+      <c r="C48" s="117"/>
       <c r="D48" s="34" t="s">
         <v>62</v>
       </c>
@@ -3692,8 +3697,8 @@
       <c r="W48" s="20"/>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B49" s="115"/>
-      <c r="C49" s="106"/>
+      <c r="B49" s="104"/>
+      <c r="C49" s="117"/>
       <c r="D49" s="34" t="s">
         <v>63</v>
       </c>
@@ -3731,8 +3736,8 @@
       <c r="W49" s="20"/>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B50" s="115"/>
-      <c r="C50" s="106"/>
+      <c r="B50" s="104"/>
+      <c r="C50" s="117"/>
       <c r="D50" s="34" t="s">
         <v>64</v>
       </c>
@@ -3770,8 +3775,8 @@
       <c r="W50" s="20"/>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B51" s="115"/>
-      <c r="C51" s="106"/>
+      <c r="B51" s="104"/>
+      <c r="C51" s="117"/>
       <c r="D51" s="34" t="s">
         <v>65</v>
       </c>
@@ -3809,8 +3814,8 @@
       <c r="W51" s="20"/>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B52" s="115"/>
-      <c r="C52" s="106"/>
+      <c r="B52" s="104"/>
+      <c r="C52" s="117"/>
       <c r="D52" s="34" t="s">
         <v>66</v>
       </c>
@@ -3848,8 +3853,8 @@
       <c r="W52" s="20"/>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B53" s="115"/>
-      <c r="C53" s="106"/>
+      <c r="B53" s="104"/>
+      <c r="C53" s="117"/>
       <c r="D53" s="34" t="s">
         <v>67</v>
       </c>
@@ -3887,8 +3892,8 @@
       <c r="W53" s="20"/>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B54" s="115"/>
-      <c r="C54" s="106"/>
+      <c r="B54" s="104"/>
+      <c r="C54" s="117"/>
       <c r="D54" s="34" t="s">
         <v>68</v>
       </c>
@@ -3926,8 +3931,8 @@
       <c r="W54" s="20"/>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B55" s="115"/>
-      <c r="C55" s="107"/>
+      <c r="B55" s="104"/>
+      <c r="C55" s="118"/>
       <c r="D55" s="34" t="s">
         <v>69</v>
       </c>
@@ -3965,8 +3970,8 @@
       <c r="W55" s="20"/>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B56" s="115"/>
-      <c r="C56" s="103" t="s">
+      <c r="B56" s="104"/>
+      <c r="C56" s="114" t="s">
         <v>26</v>
       </c>
       <c r="D56" s="31" t="s">
@@ -4006,8 +4011,8 @@
       <c r="W56" s="20"/>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B57" s="115"/>
-      <c r="C57" s="104"/>
+      <c r="B57" s="104"/>
+      <c r="C57" s="115"/>
       <c r="D57" s="31" t="s">
         <v>29</v>
       </c>
@@ -4045,8 +4050,8 @@
       <c r="W57" s="20"/>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B58" s="115"/>
-      <c r="C58" s="104"/>
+      <c r="B58" s="104"/>
+      <c r="C58" s="115"/>
       <c r="D58" s="31" t="s">
         <v>30</v>
       </c>
@@ -4084,8 +4089,8 @@
       <c r="W58" s="20"/>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B59" s="115"/>
-      <c r="C59" s="104"/>
+      <c r="B59" s="104"/>
+      <c r="C59" s="115"/>
       <c r="D59" s="31" t="s">
         <v>31</v>
       </c>
@@ -4123,8 +4128,8 @@
       <c r="W59" s="20"/>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B60" s="115"/>
-      <c r="C60" s="104"/>
+      <c r="B60" s="104"/>
+      <c r="C60" s="115"/>
       <c r="D60" s="31" t="s">
         <v>34</v>
       </c>
@@ -4162,8 +4167,8 @@
       <c r="W60" s="20"/>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B61" s="115"/>
-      <c r="C61" s="104"/>
+      <c r="B61" s="104"/>
+      <c r="C61" s="115"/>
       <c r="D61" s="31" t="s">
         <v>32</v>
       </c>
@@ -4201,8 +4206,8 @@
       <c r="W61" s="20"/>
     </row>
     <row r="62" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="116"/>
-      <c r="C62" s="104"/>
+      <c r="B62" s="105"/>
+      <c r="C62" s="115"/>
       <c r="D62" s="74" t="s">
         <v>33</v>
       </c>
@@ -4240,10 +4245,10 @@
       <c r="W62" s="29"/>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B63" s="100" t="s">
+      <c r="B63" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="108" t="s">
+      <c r="C63" s="119" t="s">
         <v>79</v>
       </c>
       <c r="D63" s="44" t="s">
@@ -4283,8 +4288,8 @@
       <c r="W63" s="57"/>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B64" s="101"/>
-      <c r="C64" s="106"/>
+      <c r="B64" s="107"/>
+      <c r="C64" s="117"/>
       <c r="D64" s="4" t="s">
         <v>71</v>
       </c>
@@ -4322,8 +4327,8 @@
       <c r="W64" s="20"/>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B65" s="101"/>
-      <c r="C65" s="106"/>
+      <c r="B65" s="107"/>
+      <c r="C65" s="117"/>
       <c r="D65" s="4" t="s">
         <v>72</v>
       </c>
@@ -4361,8 +4366,8 @@
       <c r="W65" s="20"/>
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B66" s="101"/>
-      <c r="C66" s="107"/>
+      <c r="B66" s="107"/>
+      <c r="C66" s="118"/>
       <c r="D66" s="31" t="s">
         <v>76</v>
       </c>
@@ -4400,7 +4405,7 @@
       <c r="W66" s="20"/>
     </row>
     <row r="67" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B67" s="101"/>
+      <c r="B67" s="107"/>
       <c r="C67" s="35" t="s">
         <v>73</v>
       </c>
@@ -4439,7 +4444,7 @@
       <c r="W67" s="20"/>
     </row>
     <row r="68" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B68" s="101"/>
+      <c r="B68" s="107"/>
       <c r="C68" s="61" t="s">
         <v>81</v>
       </c>
@@ -4478,8 +4483,8 @@
       <c r="W68" s="20"/>
     </row>
     <row r="69" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="101"/>
-      <c r="C69" s="105" t="s">
+      <c r="B69" s="107"/>
+      <c r="C69" s="116" t="s">
         <v>80</v>
       </c>
       <c r="D69" s="4" t="s">
@@ -4519,8 +4524,8 @@
       <c r="W69" s="20"/>
     </row>
     <row r="70" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="101"/>
-      <c r="C70" s="106"/>
+      <c r="B70" s="107"/>
+      <c r="C70" s="117"/>
       <c r="D70" s="4" t="s">
         <v>75</v>
       </c>
@@ -4558,8 +4563,8 @@
       <c r="W70" s="20"/>
     </row>
     <row r="71" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="101"/>
-      <c r="C71" s="106"/>
+      <c r="B71" s="107"/>
+      <c r="C71" s="117"/>
       <c r="D71" s="4" t="s">
         <v>77</v>
       </c>
@@ -4597,8 +4602,8 @@
       <c r="W71" s="20"/>
     </row>
     <row r="72" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="102"/>
-      <c r="C72" s="109"/>
+      <c r="B72" s="108"/>
+      <c r="C72" s="120"/>
       <c r="D72" s="25" t="s">
         <v>78</v>
       </c>
@@ -4636,10 +4641,10 @@
       <c r="W72" s="26"/>
     </row>
     <row r="73" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="114" t="s">
+      <c r="B73" s="103" t="s">
         <v>117</v>
       </c>
-      <c r="C73" s="95" t="s">
+      <c r="C73" s="121" t="s">
         <v>118</v>
       </c>
       <c r="D73" s="44" t="s">
@@ -4679,8 +4684,8 @@
       <c r="W73" s="57"/>
     </row>
     <row r="74" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="115"/>
-      <c r="C74" s="96"/>
+      <c r="B74" s="104"/>
+      <c r="C74" s="109"/>
       <c r="D74" s="4" t="s">
         <v>134</v>
       </c>
@@ -4718,8 +4723,8 @@
       <c r="W74" s="20"/>
     </row>
     <row r="75" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="115"/>
-      <c r="C75" s="96"/>
+      <c r="B75" s="104"/>
+      <c r="C75" s="109"/>
       <c r="D75" s="4" t="s">
         <v>135</v>
       </c>
@@ -4757,8 +4762,8 @@
       <c r="W75" s="20"/>
     </row>
     <row r="76" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="115"/>
-      <c r="C76" s="96"/>
+      <c r="B76" s="104"/>
+      <c r="C76" s="109"/>
       <c r="D76" s="4" t="s">
         <v>136</v>
       </c>
@@ -4796,8 +4801,8 @@
       <c r="W76" s="20"/>
     </row>
     <row r="77" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="115"/>
-      <c r="C77" s="96" t="s">
+      <c r="B77" s="104"/>
+      <c r="C77" s="109" t="s">
         <v>119</v>
       </c>
       <c r="D77" s="4" t="s">
@@ -4837,8 +4842,8 @@
       <c r="W77" s="20"/>
     </row>
     <row r="78" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="115"/>
-      <c r="C78" s="96"/>
+      <c r="B78" s="104"/>
+      <c r="C78" s="109"/>
       <c r="D78" s="4" t="s">
         <v>134</v>
       </c>
@@ -4876,8 +4881,8 @@
       <c r="W78" s="20"/>
     </row>
     <row r="79" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="115"/>
-      <c r="C79" s="96"/>
+      <c r="B79" s="104"/>
+      <c r="C79" s="109"/>
       <c r="D79" s="4" t="s">
         <v>135</v>
       </c>
@@ -4915,8 +4920,8 @@
       <c r="W79" s="20"/>
     </row>
     <row r="80" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="115"/>
-      <c r="C80" s="96"/>
+      <c r="B80" s="104"/>
+      <c r="C80" s="109"/>
       <c r="D80" s="4" t="s">
         <v>136</v>
       </c>
@@ -4954,8 +4959,8 @@
       <c r="W80" s="20"/>
     </row>
     <row r="81" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="115"/>
-      <c r="C81" s="96" t="s">
+      <c r="B81" s="104"/>
+      <c r="C81" s="109" t="s">
         <v>120</v>
       </c>
       <c r="D81" s="4" t="s">
@@ -4995,8 +5000,8 @@
       <c r="W81" s="20"/>
     </row>
     <row r="82" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="115"/>
-      <c r="C82" s="96"/>
+      <c r="B82" s="104"/>
+      <c r="C82" s="109"/>
       <c r="D82" s="4" t="s">
         <v>134</v>
       </c>
@@ -5034,8 +5039,8 @@
       <c r="W82" s="20"/>
     </row>
     <row r="83" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="115"/>
-      <c r="C83" s="96"/>
+      <c r="B83" s="104"/>
+      <c r="C83" s="109"/>
       <c r="D83" s="4" t="s">
         <v>135</v>
       </c>
@@ -5073,8 +5078,8 @@
       <c r="W83" s="20"/>
     </row>
     <row r="84" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="115"/>
-      <c r="C84" s="96"/>
+      <c r="B84" s="104"/>
+      <c r="C84" s="109"/>
       <c r="D84" s="4" t="s">
         <v>136</v>
       </c>
@@ -5112,8 +5117,8 @@
       <c r="W84" s="20"/>
     </row>
     <row r="85" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="115"/>
-      <c r="C85" s="96" t="s">
+      <c r="B85" s="104"/>
+      <c r="C85" s="109" t="s">
         <v>121</v>
       </c>
       <c r="D85" s="4" t="s">
@@ -5153,8 +5158,8 @@
       <c r="W85" s="20"/>
     </row>
     <row r="86" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="115"/>
-      <c r="C86" s="96"/>
+      <c r="B86" s="104"/>
+      <c r="C86" s="109"/>
       <c r="D86" s="4" t="s">
         <v>134</v>
       </c>
@@ -5192,8 +5197,8 @@
       <c r="W86" s="20"/>
     </row>
     <row r="87" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="115"/>
-      <c r="C87" s="96"/>
+      <c r="B87" s="104"/>
+      <c r="C87" s="109"/>
       <c r="D87" s="4" t="s">
         <v>135</v>
       </c>
@@ -5231,8 +5236,8 @@
       <c r="W87" s="20"/>
     </row>
     <row r="88" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="115"/>
-      <c r="C88" s="96"/>
+      <c r="B88" s="104"/>
+      <c r="C88" s="109"/>
       <c r="D88" s="4" t="s">
         <v>136</v>
       </c>
@@ -5270,8 +5275,8 @@
       <c r="W88" s="20"/>
     </row>
     <row r="89" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="115"/>
-      <c r="C89" s="96" t="s">
+      <c r="B89" s="104"/>
+      <c r="C89" s="109" t="s">
         <v>122</v>
       </c>
       <c r="D89" s="4" t="s">
@@ -5311,8 +5316,8 @@
       <c r="W89" s="20"/>
     </row>
     <row r="90" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="115"/>
-      <c r="C90" s="96"/>
+      <c r="B90" s="104"/>
+      <c r="C90" s="109"/>
       <c r="D90" s="4" t="s">
         <v>134</v>
       </c>
@@ -5350,8 +5355,8 @@
       <c r="W90" s="20"/>
     </row>
     <row r="91" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="115"/>
-      <c r="C91" s="96"/>
+      <c r="B91" s="104"/>
+      <c r="C91" s="109"/>
       <c r="D91" s="4" t="s">
         <v>135</v>
       </c>
@@ -5389,8 +5394,8 @@
       <c r="W91" s="20"/>
     </row>
     <row r="92" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="115"/>
-      <c r="C92" s="96"/>
+      <c r="B92" s="104"/>
+      <c r="C92" s="109"/>
       <c r="D92" s="4" t="s">
         <v>136</v>
       </c>
@@ -5428,8 +5433,8 @@
       <c r="W92" s="20"/>
     </row>
     <row r="93" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="115"/>
-      <c r="C93" s="96" t="s">
+      <c r="B93" s="104"/>
+      <c r="C93" s="109" t="s">
         <v>123</v>
       </c>
       <c r="D93" s="4" t="s">
@@ -5469,8 +5474,8 @@
       <c r="W93" s="20"/>
     </row>
     <row r="94" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="115"/>
-      <c r="C94" s="96"/>
+      <c r="B94" s="104"/>
+      <c r="C94" s="109"/>
       <c r="D94" s="4" t="s">
         <v>134</v>
       </c>
@@ -5508,8 +5513,8 @@
       <c r="W94" s="20"/>
     </row>
     <row r="95" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="115"/>
-      <c r="C95" s="96"/>
+      <c r="B95" s="104"/>
+      <c r="C95" s="109"/>
       <c r="D95" s="4" t="s">
         <v>135</v>
       </c>
@@ -5547,8 +5552,8 @@
       <c r="W95" s="20"/>
     </row>
     <row r="96" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="115"/>
-      <c r="C96" s="96"/>
+      <c r="B96" s="104"/>
+      <c r="C96" s="109"/>
       <c r="D96" s="4" t="s">
         <v>136</v>
       </c>
@@ -5586,8 +5591,8 @@
       <c r="W96" s="20"/>
     </row>
     <row r="97" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="115"/>
-      <c r="C97" s="96" t="s">
+      <c r="B97" s="104"/>
+      <c r="C97" s="109" t="s">
         <v>124</v>
       </c>
       <c r="D97" s="4" t="s">
@@ -5627,8 +5632,8 @@
       <c r="W97" s="20"/>
     </row>
     <row r="98" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="115"/>
-      <c r="C98" s="96"/>
+      <c r="B98" s="104"/>
+      <c r="C98" s="109"/>
       <c r="D98" s="4" t="s">
         <v>134</v>
       </c>
@@ -5666,8 +5671,8 @@
       <c r="W98" s="20"/>
     </row>
     <row r="99" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="115"/>
-      <c r="C99" s="96"/>
+      <c r="B99" s="104"/>
+      <c r="C99" s="109"/>
       <c r="D99" s="4" t="s">
         <v>135</v>
       </c>
@@ -5705,8 +5710,8 @@
       <c r="W99" s="20"/>
     </row>
     <row r="100" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="115"/>
-      <c r="C100" s="96"/>
+      <c r="B100" s="104"/>
+      <c r="C100" s="109"/>
       <c r="D100" s="4" t="s">
         <v>136</v>
       </c>
@@ -5744,8 +5749,8 @@
       <c r="W100" s="20"/>
     </row>
     <row r="101" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="115"/>
-      <c r="C101" s="96" t="s">
+      <c r="B101" s="104"/>
+      <c r="C101" s="109" t="s">
         <v>125</v>
       </c>
       <c r="D101" s="4" t="s">
@@ -5785,8 +5790,8 @@
       <c r="W101" s="20"/>
     </row>
     <row r="102" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="115"/>
-      <c r="C102" s="96"/>
+      <c r="B102" s="104"/>
+      <c r="C102" s="109"/>
       <c r="D102" s="4" t="s">
         <v>134</v>
       </c>
@@ -5824,8 +5829,8 @@
       <c r="W102" s="20"/>
     </row>
     <row r="103" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="115"/>
-      <c r="C103" s="96"/>
+      <c r="B103" s="104"/>
+      <c r="C103" s="109"/>
       <c r="D103" s="4" t="s">
         <v>135</v>
       </c>
@@ -5863,8 +5868,8 @@
       <c r="W103" s="20"/>
     </row>
     <row r="104" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="115"/>
-      <c r="C104" s="96"/>
+      <c r="B104" s="104"/>
+      <c r="C104" s="109"/>
       <c r="D104" s="4" t="s">
         <v>136</v>
       </c>
@@ -5902,8 +5907,8 @@
       <c r="W104" s="20"/>
     </row>
     <row r="105" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="115"/>
-      <c r="C105" s="96" t="s">
+      <c r="B105" s="104"/>
+      <c r="C105" s="109" t="s">
         <v>126</v>
       </c>
       <c r="D105" s="4" t="s">
@@ -5943,8 +5948,8 @@
       <c r="W105" s="20"/>
     </row>
     <row r="106" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="115"/>
-      <c r="C106" s="96"/>
+      <c r="B106" s="104"/>
+      <c r="C106" s="109"/>
       <c r="D106" s="4" t="s">
         <v>134</v>
       </c>
@@ -5982,8 +5987,8 @@
       <c r="W106" s="20"/>
     </row>
     <row r="107" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="115"/>
-      <c r="C107" s="96"/>
+      <c r="B107" s="104"/>
+      <c r="C107" s="109"/>
       <c r="D107" s="4" t="s">
         <v>135</v>
       </c>
@@ -6021,8 +6026,8 @@
       <c r="W107" s="20"/>
     </row>
     <row r="108" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="115"/>
-      <c r="C108" s="96"/>
+      <c r="B108" s="104"/>
+      <c r="C108" s="109"/>
       <c r="D108" s="4" t="s">
         <v>136</v>
       </c>
@@ -6060,8 +6065,8 @@
       <c r="W108" s="20"/>
     </row>
     <row r="109" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="115"/>
-      <c r="C109" s="96" t="s">
+      <c r="B109" s="104"/>
+      <c r="C109" s="109" t="s">
         <v>127</v>
       </c>
       <c r="D109" s="4" t="s">
@@ -6101,8 +6106,8 @@
       <c r="W109" s="20"/>
     </row>
     <row r="110" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="115"/>
-      <c r="C110" s="96"/>
+      <c r="B110" s="104"/>
+      <c r="C110" s="109"/>
       <c r="D110" s="4" t="s">
         <v>134</v>
       </c>
@@ -6140,8 +6145,8 @@
       <c r="W110" s="20"/>
     </row>
     <row r="111" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="115"/>
-      <c r="C111" s="96"/>
+      <c r="B111" s="104"/>
+      <c r="C111" s="109"/>
       <c r="D111" s="4" t="s">
         <v>135</v>
       </c>
@@ -6179,8 +6184,8 @@
       <c r="W111" s="20"/>
     </row>
     <row r="112" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="115"/>
-      <c r="C112" s="96"/>
+      <c r="B112" s="104"/>
+      <c r="C112" s="109"/>
       <c r="D112" s="4" t="s">
         <v>136</v>
       </c>
@@ -6218,8 +6223,8 @@
       <c r="W112" s="20"/>
     </row>
     <row r="113" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="115"/>
-      <c r="C113" s="96" t="s">
+      <c r="B113" s="104"/>
+      <c r="C113" s="109" t="s">
         <v>128</v>
       </c>
       <c r="D113" s="4" t="s">
@@ -6259,8 +6264,8 @@
       <c r="W113" s="20"/>
     </row>
     <row r="114" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="115"/>
-      <c r="C114" s="96"/>
+      <c r="B114" s="104"/>
+      <c r="C114" s="109"/>
       <c r="D114" s="4" t="s">
         <v>134</v>
       </c>
@@ -6298,8 +6303,8 @@
       <c r="W114" s="20"/>
     </row>
     <row r="115" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="115"/>
-      <c r="C115" s="96"/>
+      <c r="B115" s="104"/>
+      <c r="C115" s="109"/>
       <c r="D115" s="4" t="s">
         <v>135</v>
       </c>
@@ -6337,8 +6342,8 @@
       <c r="W115" s="20"/>
     </row>
     <row r="116" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="115"/>
-      <c r="C116" s="96"/>
+      <c r="B116" s="104"/>
+      <c r="C116" s="109"/>
       <c r="D116" s="4" t="s">
         <v>136</v>
       </c>
@@ -6376,8 +6381,8 @@
       <c r="W116" s="20"/>
     </row>
     <row r="117" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="115"/>
-      <c r="C117" s="96" t="s">
+      <c r="B117" s="104"/>
+      <c r="C117" s="109" t="s">
         <v>129</v>
       </c>
       <c r="D117" s="4" t="s">
@@ -6417,8 +6422,8 @@
       <c r="W117" s="20"/>
     </row>
     <row r="118" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="115"/>
-      <c r="C118" s="96"/>
+      <c r="B118" s="104"/>
+      <c r="C118" s="109"/>
       <c r="D118" s="4" t="s">
         <v>134</v>
       </c>
@@ -6456,8 +6461,8 @@
       <c r="W118" s="20"/>
     </row>
     <row r="119" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="115"/>
-      <c r="C119" s="96"/>
+      <c r="B119" s="104"/>
+      <c r="C119" s="109"/>
       <c r="D119" s="4" t="s">
         <v>135</v>
       </c>
@@ -6495,8 +6500,8 @@
       <c r="W119" s="20"/>
     </row>
     <row r="120" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="115"/>
-      <c r="C120" s="96"/>
+      <c r="B120" s="104"/>
+      <c r="C120" s="109"/>
       <c r="D120" s="4" t="s">
         <v>136</v>
       </c>
@@ -6534,8 +6539,8 @@
       <c r="W120" s="20"/>
     </row>
     <row r="121" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="115"/>
-      <c r="C121" s="96" t="s">
+      <c r="B121" s="104"/>
+      <c r="C121" s="109" t="s">
         <v>130</v>
       </c>
       <c r="D121" s="4" t="s">
@@ -6575,8 +6580,8 @@
       <c r="W121" s="20"/>
     </row>
     <row r="122" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="115"/>
-      <c r="C122" s="96"/>
+      <c r="B122" s="104"/>
+      <c r="C122" s="109"/>
       <c r="D122" s="4" t="s">
         <v>134</v>
       </c>
@@ -6614,8 +6619,8 @@
       <c r="W122" s="20"/>
     </row>
     <row r="123" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="115"/>
-      <c r="C123" s="96"/>
+      <c r="B123" s="104"/>
+      <c r="C123" s="109"/>
       <c r="D123" s="4" t="s">
         <v>135</v>
       </c>
@@ -6653,8 +6658,8 @@
       <c r="W123" s="20"/>
     </row>
     <row r="124" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="115"/>
-      <c r="C124" s="96"/>
+      <c r="B124" s="104"/>
+      <c r="C124" s="109"/>
       <c r="D124" s="4" t="s">
         <v>136</v>
       </c>
@@ -6692,8 +6697,8 @@
       <c r="W124" s="20"/>
     </row>
     <row r="125" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="115"/>
-      <c r="C125" s="96" t="s">
+      <c r="B125" s="104"/>
+      <c r="C125" s="109" t="s">
         <v>131</v>
       </c>
       <c r="D125" s="4" t="s">
@@ -6733,8 +6738,8 @@
       <c r="W125" s="20"/>
     </row>
     <row r="126" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="115"/>
-      <c r="C126" s="96"/>
+      <c r="B126" s="104"/>
+      <c r="C126" s="109"/>
       <c r="D126" s="4" t="s">
         <v>134</v>
       </c>
@@ -6772,8 +6777,8 @@
       <c r="W126" s="20"/>
     </row>
     <row r="127" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="115"/>
-      <c r="C127" s="96"/>
+      <c r="B127" s="104"/>
+      <c r="C127" s="109"/>
       <c r="D127" s="4" t="s">
         <v>135</v>
       </c>
@@ -6811,8 +6816,8 @@
       <c r="W127" s="20"/>
     </row>
     <row r="128" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="115"/>
-      <c r="C128" s="96"/>
+      <c r="B128" s="104"/>
+      <c r="C128" s="109"/>
       <c r="D128" s="4" t="s">
         <v>136</v>
       </c>
@@ -6850,8 +6855,8 @@
       <c r="W128" s="20"/>
     </row>
     <row r="129" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="115"/>
-      <c r="C129" s="96" t="s">
+      <c r="B129" s="104"/>
+      <c r="C129" s="109" t="s">
         <v>132</v>
       </c>
       <c r="D129" s="4" t="s">
@@ -6891,8 +6896,8 @@
       <c r="W129" s="20"/>
     </row>
     <row r="130" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="115"/>
-      <c r="C130" s="96"/>
+      <c r="B130" s="104"/>
+      <c r="C130" s="109"/>
       <c r="D130" s="4" t="s">
         <v>134</v>
       </c>
@@ -6930,8 +6935,8 @@
       <c r="W130" s="20"/>
     </row>
     <row r="131" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="115"/>
-      <c r="C131" s="96"/>
+      <c r="B131" s="104"/>
+      <c r="C131" s="109"/>
       <c r="D131" s="4" t="s">
         <v>135</v>
       </c>
@@ -6969,8 +6974,8 @@
       <c r="W131" s="20"/>
     </row>
     <row r="132" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B132" s="117"/>
-      <c r="C132" s="118"/>
+      <c r="B132" s="110"/>
+      <c r="C132" s="113"/>
       <c r="D132" s="25" t="s">
         <v>136</v>
       </c>
@@ -7008,7 +7013,7 @@
       <c r="W132" s="26"/>
     </row>
     <row r="133" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B133" s="100" t="s">
+      <c r="B133" s="106" t="s">
         <v>83</v>
       </c>
       <c r="C133" s="92" t="s">
@@ -7049,7 +7054,7 @@
       <c r="W133" s="57"/>
     </row>
     <row r="134" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="101"/>
+      <c r="B134" s="107"/>
       <c r="C134" s="38" t="s">
         <v>89</v>
       </c>
@@ -7088,7 +7093,7 @@
       <c r="W134" s="20"/>
     </row>
     <row r="135" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="101"/>
+      <c r="B135" s="107"/>
       <c r="C135" s="38" t="s">
         <v>90</v>
       </c>
@@ -7127,7 +7132,7 @@
       <c r="W135" s="20"/>
     </row>
     <row r="136" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="101"/>
+      <c r="B136" s="107"/>
       <c r="C136" s="38" t="s">
         <v>91</v>
       </c>
@@ -7166,7 +7171,7 @@
       <c r="W136" s="20"/>
     </row>
     <row r="137" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="101"/>
+      <c r="B137" s="107"/>
       <c r="C137" s="38" t="s">
         <v>143</v>
       </c>
@@ -7205,7 +7210,7 @@
       <c r="W137" s="20"/>
     </row>
     <row r="138" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="101"/>
+      <c r="B138" s="107"/>
       <c r="C138" s="38" t="s">
         <v>140</v>
       </c>
@@ -7244,7 +7249,7 @@
       <c r="W138" s="20"/>
     </row>
     <row r="139" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="101"/>
+      <c r="B139" s="107"/>
       <c r="C139" s="38" t="s">
         <v>142</v>
       </c>
@@ -7283,7 +7288,7 @@
       <c r="W139" s="20"/>
     </row>
     <row r="140" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="101"/>
+      <c r="B140" s="107"/>
       <c r="C140" s="38" t="s">
         <v>141</v>
       </c>
@@ -7322,7 +7327,7 @@
       <c r="W140" s="20"/>
     </row>
     <row r="141" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="101"/>
+      <c r="B141" s="107"/>
       <c r="C141" s="38" t="s">
         <v>92</v>
       </c>
@@ -7361,7 +7366,7 @@
       <c r="W141" s="20"/>
     </row>
     <row r="142" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="101"/>
+      <c r="B142" s="107"/>
       <c r="C142" s="38" t="s">
         <v>93</v>
       </c>
@@ -7400,7 +7405,7 @@
       <c r="W142" s="20"/>
     </row>
     <row r="143" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="101"/>
+      <c r="B143" s="107"/>
       <c r="C143" s="38" t="s">
         <v>94</v>
       </c>
@@ -7439,7 +7444,7 @@
       <c r="W143" s="20"/>
     </row>
     <row r="144" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="101"/>
+      <c r="B144" s="107"/>
       <c r="C144" s="38" t="s">
         <v>98</v>
       </c>
@@ -7478,7 +7483,7 @@
       <c r="W144" s="20"/>
     </row>
     <row r="145" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B145" s="102"/>
+      <c r="B145" s="108"/>
       <c r="C145" s="62" t="s">
         <v>99</v>
       </c>
@@ -7517,7 +7522,7 @@
       <c r="W145" s="26"/>
     </row>
     <row r="146" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="114" t="s">
+      <c r="B146" s="103" t="s">
         <v>144</v>
       </c>
       <c r="C146" s="72" t="s">
@@ -7558,7 +7563,7 @@
       <c r="W146" s="57"/>
     </row>
     <row r="147" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="115"/>
+      <c r="B147" s="104"/>
       <c r="C147" s="71" t="s">
         <v>145</v>
       </c>
@@ -7597,7 +7602,7 @@
       <c r="W147" s="20"/>
     </row>
     <row r="148" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="117"/>
+      <c r="B148" s="110"/>
       <c r="C148" s="73" t="s">
         <v>146</v>
       </c>
@@ -7636,7 +7641,7 @@
       <c r="W148" s="26"/>
     </row>
     <row r="149" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="101" t="s">
+      <c r="B149" s="107" t="s">
         <v>18</v>
       </c>
       <c r="C149" s="38" t="s">
@@ -7677,7 +7682,7 @@
       <c r="W149" s="70"/>
     </row>
     <row r="150" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="101"/>
+      <c r="B150" s="107"/>
       <c r="C150" s="38" t="s">
         <v>138</v>
       </c>
@@ -7716,7 +7721,7 @@
       <c r="W150" s="70"/>
     </row>
     <row r="151" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="101"/>
+      <c r="B151" s="107"/>
       <c r="C151" s="38" t="s">
         <v>139</v>
       </c>
@@ -7755,7 +7760,7 @@
       <c r="W151" s="70"/>
     </row>
     <row r="152" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="101"/>
+      <c r="B152" s="107"/>
       <c r="C152" s="38" t="s">
         <v>147</v>
       </c>
@@ -7794,7 +7799,7 @@
       <c r="W152" s="20"/>
     </row>
     <row r="153" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="101"/>
+      <c r="B153" s="107"/>
       <c r="C153" s="35" t="s">
         <v>84</v>
       </c>
@@ -7833,7 +7838,7 @@
       <c r="W153" s="20"/>
     </row>
     <row r="154" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="101"/>
+      <c r="B154" s="107"/>
       <c r="C154" s="35" t="s">
         <v>85</v>
       </c>
@@ -7872,7 +7877,7 @@
       <c r="W154" s="20"/>
     </row>
     <row r="155" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="101"/>
+      <c r="B155" s="107"/>
       <c r="C155" s="39" t="s">
         <v>87</v>
       </c>
@@ -7911,7 +7916,7 @@
       <c r="W155" s="29"/>
     </row>
     <row r="156" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="101"/>
+      <c r="B156" s="107"/>
       <c r="C156" s="35" t="s">
         <v>86</v>
       </c>
@@ -7950,7 +7955,7 @@
       <c r="W156" s="29"/>
     </row>
     <row r="157" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="101"/>
+      <c r="B157" s="107"/>
       <c r="C157" s="41" t="s">
         <v>104</v>
       </c>
@@ -7989,7 +7994,7 @@
       <c r="W157" s="29"/>
     </row>
     <row r="158" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="101"/>
+      <c r="B158" s="107"/>
       <c r="C158" s="41" t="s">
         <v>137</v>
       </c>
@@ -8028,7 +8033,7 @@
       <c r="W158" s="29"/>
     </row>
     <row r="159" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="101"/>
+      <c r="B159" s="107"/>
       <c r="C159" s="41" t="s">
         <v>105</v>
       </c>
@@ -8067,7 +8072,7 @@
       <c r="W159" s="29"/>
     </row>
     <row r="160" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B160" s="102"/>
+      <c r="B160" s="108"/>
       <c r="C160" s="62" t="s">
         <v>100</v>
       </c>
@@ -8106,21 +8111,21 @@
       <c r="W160" s="26"/>
     </row>
     <row r="161" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B161" s="110" t="s">
+      <c r="B161" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="C161" s="112"/>
-      <c r="D161" s="111"/>
-      <c r="E161" s="111"/>
-      <c r="F161" s="111"/>
-      <c r="G161" s="113"/>
+      <c r="C161" s="101"/>
+      <c r="D161" s="99"/>
+      <c r="E161" s="99"/>
+      <c r="F161" s="99"/>
+      <c r="G161" s="102"/>
       <c r="H161" s="40">
         <f>SUM(H4:H160)</f>
         <v>89.199999999999989</v>
       </c>
       <c r="I161" s="24">
         <f>SUM(I4:I160)</f>
-        <v>0.05</v>
+        <v>0.93330000000000002</v>
       </c>
       <c r="J161" s="24">
         <f>SUM(J4:J160)</f>
@@ -8128,7 +8133,7 @@
       </c>
       <c r="K161" s="24">
         <f t="shared" ref="K161:W161" si="5">SUM(K4:K160)</f>
-        <v>0.05</v>
+        <v>0.93330000000000002</v>
       </c>
       <c r="L161" s="24">
         <f t="shared" si="5"/>
@@ -8188,22 +8193,22 @@
       <c r="G162" s="2"/>
       <c r="H162" s="2"/>
       <c r="I162" s="2"/>
-      <c r="J162" s="97" t="s">
+      <c r="J162" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="K162" s="98"/>
-      <c r="L162" s="98"/>
-      <c r="M162" s="98"/>
-      <c r="N162" s="98"/>
-      <c r="O162" s="98"/>
-      <c r="P162" s="98"/>
-      <c r="Q162" s="98"/>
-      <c r="R162" s="98"/>
-      <c r="S162" s="98"/>
-      <c r="T162" s="98"/>
-      <c r="U162" s="98"/>
-      <c r="V162" s="98"/>
-      <c r="W162" s="99"/>
+      <c r="K162" s="111"/>
+      <c r="L162" s="111"/>
+      <c r="M162" s="111"/>
+      <c r="N162" s="111"/>
+      <c r="O162" s="111"/>
+      <c r="P162" s="111"/>
+      <c r="Q162" s="111"/>
+      <c r="R162" s="111"/>
+      <c r="S162" s="111"/>
+      <c r="T162" s="111"/>
+      <c r="U162" s="111"/>
+      <c r="V162" s="111"/>
+      <c r="W162" s="112"/>
     </row>
     <row r="163" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B163" s="2"/>
@@ -8227,29 +8232,29 @@
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
-      <c r="H164" s="110" t="s">
+      <c r="H164" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="I164" s="111"/>
+      <c r="I164" s="99"/>
       <c r="J164" s="10">
         <f>H161-J161</f>
         <v>89.199999999999989</v>
       </c>
       <c r="K164" s="10">
         <f>J164-K161</f>
-        <v>89.149999999999991</v>
+        <v>88.266699999999986</v>
       </c>
       <c r="L164" s="10">
         <f>K164-L161</f>
-        <v>89.149999999999991</v>
+        <v>88.266699999999986</v>
       </c>
       <c r="M164" s="10">
         <f>L164-M161</f>
-        <v>89.149999999999991</v>
+        <v>88.266699999999986</v>
       </c>
       <c r="N164" s="11">
         <f>M164-N161</f>
-        <v>89.149999999999991</v>
+        <v>88.266699999999986</v>
       </c>
     </row>
     <row r="165" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8273,18 +8278,18 @@
       <c r="D166" s="3"/>
       <c r="E166" s="3"/>
       <c r="F166" s="3"/>
-      <c r="H166" s="97" t="s">
+      <c r="H166" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="I166" s="112"/>
-      <c r="J166" s="111">
+      <c r="I166" s="101"/>
+      <c r="J166" s="99">
         <f>H161-I161</f>
-        <v>89.149999999999991</v>
-      </c>
-      <c r="K166" s="111"/>
-      <c r="L166" s="111"/>
-      <c r="M166" s="111"/>
-      <c r="N166" s="113"/>
+        <v>88.266699999999986</v>
+      </c>
+      <c r="K166" s="99"/>
+      <c r="L166" s="99"/>
+      <c r="M166" s="99"/>
+      <c r="N166" s="102"/>
     </row>
     <row r="167" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B167" s="3"/>
@@ -8388,6 +8393,23 @@
     <row r="185" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C73:C76"/>
+    <mergeCell ref="C77:C80"/>
+    <mergeCell ref="C121:C124"/>
+    <mergeCell ref="C113:C116"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="C101:C104"/>
+    <mergeCell ref="C93:C96"/>
+    <mergeCell ref="C109:C112"/>
+    <mergeCell ref="C117:C120"/>
+    <mergeCell ref="J2:W2"/>
+    <mergeCell ref="B63:B72"/>
+    <mergeCell ref="C56:C62"/>
+    <mergeCell ref="C16:C55"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C69:C72"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B14"/>
     <mergeCell ref="H164:I164"/>
     <mergeCell ref="H166:I166"/>
     <mergeCell ref="J166:N166"/>
@@ -8404,23 +8426,6 @@
     <mergeCell ref="C89:C92"/>
     <mergeCell ref="C85:C88"/>
     <mergeCell ref="C81:C84"/>
-    <mergeCell ref="J2:W2"/>
-    <mergeCell ref="B63:B72"/>
-    <mergeCell ref="C56:C62"/>
-    <mergeCell ref="C16:C55"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="C69:C72"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="C73:C76"/>
-    <mergeCell ref="C77:C80"/>
-    <mergeCell ref="C121:C124"/>
-    <mergeCell ref="C113:C116"/>
-    <mergeCell ref="C105:C108"/>
-    <mergeCell ref="C101:C104"/>
-    <mergeCell ref="C93:C96"/>
-    <mergeCell ref="C109:C112"/>
-    <mergeCell ref="C117:C120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Arreglada la posición de la cámara al salir de las salas secretas, la sala de la parte más alta a la izquierda al salir no reaparece Link
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
+++ b/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
@@ -1254,15 +1254,60 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1278,55 +1323,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1388,16 +1388,16 @@
                   <c:v>89.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88.266699999999986</c:v>
+                  <c:v>87.766699999999986</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88.266699999999986</c:v>
+                  <c:v>87.766699999999986</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>88.266699999999986</c:v>
+                  <c:v>87.766699999999986</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>88.266699999999986</c:v>
+                  <c:v>87.766699999999986</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1413,11 +1413,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1291761776"/>
-        <c:axId val="-1291761232"/>
+        <c:axId val="1036224592"/>
+        <c:axId val="1036214800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1291761776"/>
+        <c:axId val="1036224592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1426,7 +1426,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1291761232"/>
+        <c:crossAx val="1036214800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1434,7 +1434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1291761232"/>
+        <c:axId val="1036214800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1445,7 +1445,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1291761776"/>
+        <c:crossAx val="1036224592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1790,8 +1790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1818,22 +1818,22 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="100" t="s">
+      <c r="J2" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="112"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="102"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="102"/>
+      <c r="T2" s="102"/>
+      <c r="U2" s="102"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="103"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="64" t="s">
@@ -1904,7 +1904,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="104" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="42" t="s">
@@ -1945,7 +1945,7 @@
       <c r="W4" s="49"/>
     </row>
     <row r="5" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="107"/>
+      <c r="B5" s="105"/>
       <c r="C5" s="37" t="s">
         <v>101</v>
       </c>
@@ -1984,7 +1984,7 @@
       <c r="W5" s="20"/>
     </row>
     <row r="6" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="107"/>
+      <c r="B6" s="105"/>
       <c r="C6" s="37" t="s">
         <v>102</v>
       </c>
@@ -2023,7 +2023,7 @@
       <c r="W6" s="20"/>
     </row>
     <row r="7" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="107"/>
+      <c r="B7" s="105"/>
       <c r="C7" s="37" t="s">
         <v>103</v>
       </c>
@@ -2062,7 +2062,7 @@
       <c r="W7" s="20"/>
     </row>
     <row r="8" spans="1:23" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="108"/>
+      <c r="B8" s="106"/>
       <c r="C8" s="50" t="s">
         <v>112</v>
       </c>
@@ -2101,7 +2101,7 @@
       <c r="W8" s="26"/>
     </row>
     <row r="9" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="106" t="s">
+      <c r="B9" s="104" t="s">
         <v>106</v>
       </c>
       <c r="C9" s="53" t="s">
@@ -2142,7 +2142,7 @@
       <c r="W9" s="57"/>
     </row>
     <row r="10" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="107"/>
+      <c r="B10" s="105"/>
       <c r="C10" s="36" t="s">
         <v>107</v>
       </c>
@@ -2181,7 +2181,7 @@
       <c r="W10" s="20"/>
     </row>
     <row r="11" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="107"/>
+      <c r="B11" s="105"/>
       <c r="C11" s="58" t="s">
         <v>113</v>
       </c>
@@ -2220,7 +2220,7 @@
       <c r="W11" s="20"/>
     </row>
     <row r="12" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="107"/>
+      <c r="B12" s="105"/>
       <c r="C12" s="58" t="s">
         <v>114</v>
       </c>
@@ -2285,7 +2285,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="107"/>
+      <c r="B13" s="105"/>
       <c r="C13" s="58" t="s">
         <v>108</v>
       </c>
@@ -2324,7 +2324,7 @@
       <c r="W13" s="20"/>
     </row>
     <row r="14" spans="1:23" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="108"/>
+      <c r="B14" s="106"/>
       <c r="C14" s="59" t="s">
         <v>97</v>
       </c>
@@ -2343,12 +2343,14 @@
       </c>
       <c r="I14" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J14" s="83">
         <v>0</v>
       </c>
-      <c r="K14" s="25"/>
+      <c r="K14" s="25">
+        <v>0.5</v>
+      </c>
       <c r="L14" s="25"/>
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
@@ -2363,7 +2365,7 @@
       <c r="W14" s="26"/>
     </row>
     <row r="15" spans="1:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="118" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="60" t="s">
@@ -2391,7 +2393,7 @@
       <c r="J15" s="81">
         <v>0</v>
       </c>
-      <c r="K15" s="122">
+      <c r="K15" s="98">
         <v>0.88329999999999997</v>
       </c>
       <c r="L15" s="55"/>
@@ -2408,8 +2410,8 @@
       <c r="W15" s="57"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B16" s="104"/>
-      <c r="C16" s="116" t="s">
+      <c r="B16" s="119"/>
+      <c r="C16" s="109" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -2449,8 +2451,8 @@
       <c r="W16" s="20"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B17" s="104"/>
-      <c r="C17" s="117"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="110"/>
       <c r="D17" s="4" t="s">
         <v>20</v>
       </c>
@@ -2488,8 +2490,8 @@
       <c r="W17" s="20"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B18" s="104"/>
-      <c r="C18" s="117"/>
+      <c r="B18" s="119"/>
+      <c r="C18" s="110"/>
       <c r="D18" s="4" t="s">
         <v>21</v>
       </c>
@@ -2527,8 +2529,8 @@
       <c r="W18" s="20"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B19" s="104"/>
-      <c r="C19" s="117"/>
+      <c r="B19" s="119"/>
+      <c r="C19" s="110"/>
       <c r="D19" s="4" t="s">
         <v>22</v>
       </c>
@@ -2566,8 +2568,8 @@
       <c r="W19" s="20"/>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B20" s="104"/>
-      <c r="C20" s="117"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="110"/>
       <c r="D20" s="4" t="s">
         <v>23</v>
       </c>
@@ -2605,8 +2607,8 @@
       <c r="W20" s="20"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B21" s="104"/>
-      <c r="C21" s="117"/>
+      <c r="B21" s="119"/>
+      <c r="C21" s="110"/>
       <c r="D21" s="4" t="s">
         <v>24</v>
       </c>
@@ -2644,8 +2646,8 @@
       <c r="W21" s="20"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B22" s="104"/>
-      <c r="C22" s="117"/>
+      <c r="B22" s="119"/>
+      <c r="C22" s="110"/>
       <c r="D22" s="34" t="s">
         <v>36</v>
       </c>
@@ -2683,8 +2685,8 @@
       <c r="W22" s="20"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B23" s="104"/>
-      <c r="C23" s="117"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="110"/>
       <c r="D23" s="34" t="s">
         <v>37</v>
       </c>
@@ -2722,8 +2724,8 @@
       <c r="W23" s="20"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B24" s="104"/>
-      <c r="C24" s="117"/>
+      <c r="B24" s="119"/>
+      <c r="C24" s="110"/>
       <c r="D24" s="34" t="s">
         <v>38</v>
       </c>
@@ -2761,8 +2763,8 @@
       <c r="W24" s="20"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B25" s="104"/>
-      <c r="C25" s="117"/>
+      <c r="B25" s="119"/>
+      <c r="C25" s="110"/>
       <c r="D25" s="34" t="s">
         <v>39</v>
       </c>
@@ -2800,8 +2802,8 @@
       <c r="W25" s="20"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B26" s="104"/>
-      <c r="C26" s="117"/>
+      <c r="B26" s="119"/>
+      <c r="C26" s="110"/>
       <c r="D26" s="34" t="s">
         <v>40</v>
       </c>
@@ -2839,8 +2841,8 @@
       <c r="W26" s="20"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B27" s="104"/>
-      <c r="C27" s="117"/>
+      <c r="B27" s="119"/>
+      <c r="C27" s="110"/>
       <c r="D27" s="34" t="s">
         <v>41</v>
       </c>
@@ -2878,8 +2880,8 @@
       <c r="W27" s="20"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B28" s="104"/>
-      <c r="C28" s="117"/>
+      <c r="B28" s="119"/>
+      <c r="C28" s="110"/>
       <c r="D28" s="34" t="s">
         <v>42</v>
       </c>
@@ -2917,8 +2919,8 @@
       <c r="W28" s="20"/>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B29" s="104"/>
-      <c r="C29" s="117"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="110"/>
       <c r="D29" s="34" t="s">
         <v>43</v>
       </c>
@@ -2956,8 +2958,8 @@
       <c r="W29" s="20"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B30" s="104"/>
-      <c r="C30" s="117"/>
+      <c r="B30" s="119"/>
+      <c r="C30" s="110"/>
       <c r="D30" s="34" t="s">
         <v>44</v>
       </c>
@@ -2995,8 +2997,8 @@
       <c r="W30" s="20"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B31" s="104"/>
-      <c r="C31" s="117"/>
+      <c r="B31" s="119"/>
+      <c r="C31" s="110"/>
       <c r="D31" s="34" t="s">
         <v>45</v>
       </c>
@@ -3034,8 +3036,8 @@
       <c r="W31" s="20"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B32" s="104"/>
-      <c r="C32" s="117"/>
+      <c r="B32" s="119"/>
+      <c r="C32" s="110"/>
       <c r="D32" s="34" t="s">
         <v>46</v>
       </c>
@@ -3073,8 +3075,8 @@
       <c r="W32" s="20"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B33" s="104"/>
-      <c r="C33" s="117"/>
+      <c r="B33" s="119"/>
+      <c r="C33" s="110"/>
       <c r="D33" s="34" t="s">
         <v>47</v>
       </c>
@@ -3112,8 +3114,8 @@
       <c r="W33" s="20"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B34" s="104"/>
-      <c r="C34" s="117"/>
+      <c r="B34" s="119"/>
+      <c r="C34" s="110"/>
       <c r="D34" s="34" t="s">
         <v>48</v>
       </c>
@@ -3151,8 +3153,8 @@
       <c r="W34" s="20"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B35" s="104"/>
-      <c r="C35" s="117"/>
+      <c r="B35" s="119"/>
+      <c r="C35" s="110"/>
       <c r="D35" s="34" t="s">
         <v>49</v>
       </c>
@@ -3190,8 +3192,8 @@
       <c r="W35" s="20"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B36" s="104"/>
-      <c r="C36" s="117"/>
+      <c r="B36" s="119"/>
+      <c r="C36" s="110"/>
       <c r="D36" s="34" t="s">
         <v>50</v>
       </c>
@@ -3229,8 +3231,8 @@
       <c r="W36" s="20"/>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B37" s="104"/>
-      <c r="C37" s="117"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="110"/>
       <c r="D37" s="34" t="s">
         <v>51</v>
       </c>
@@ -3268,8 +3270,8 @@
       <c r="W37" s="20"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B38" s="104"/>
-      <c r="C38" s="117"/>
+      <c r="B38" s="119"/>
+      <c r="C38" s="110"/>
       <c r="D38" s="34" t="s">
         <v>52</v>
       </c>
@@ -3307,8 +3309,8 @@
       <c r="W38" s="20"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B39" s="104"/>
-      <c r="C39" s="117"/>
+      <c r="B39" s="119"/>
+      <c r="C39" s="110"/>
       <c r="D39" s="34" t="s">
         <v>53</v>
       </c>
@@ -3346,8 +3348,8 @@
       <c r="W39" s="20"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B40" s="104"/>
-      <c r="C40" s="117"/>
+      <c r="B40" s="119"/>
+      <c r="C40" s="110"/>
       <c r="D40" s="34" t="s">
         <v>54</v>
       </c>
@@ -3385,8 +3387,8 @@
       <c r="W40" s="20"/>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B41" s="104"/>
-      <c r="C41" s="117"/>
+      <c r="B41" s="119"/>
+      <c r="C41" s="110"/>
       <c r="D41" s="34" t="s">
         <v>55</v>
       </c>
@@ -3424,8 +3426,8 @@
       <c r="W41" s="20"/>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B42" s="104"/>
-      <c r="C42" s="117"/>
+      <c r="B42" s="119"/>
+      <c r="C42" s="110"/>
       <c r="D42" s="34" t="s">
         <v>56</v>
       </c>
@@ -3463,8 +3465,8 @@
       <c r="W42" s="20"/>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B43" s="104"/>
-      <c r="C43" s="117"/>
+      <c r="B43" s="119"/>
+      <c r="C43" s="110"/>
       <c r="D43" s="34" t="s">
         <v>57</v>
       </c>
@@ -3502,8 +3504,8 @@
       <c r="W43" s="20"/>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B44" s="104"/>
-      <c r="C44" s="117"/>
+      <c r="B44" s="119"/>
+      <c r="C44" s="110"/>
       <c r="D44" s="34" t="s">
         <v>58</v>
       </c>
@@ -3541,8 +3543,8 @@
       <c r="W44" s="20"/>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B45" s="104"/>
-      <c r="C45" s="117"/>
+      <c r="B45" s="119"/>
+      <c r="C45" s="110"/>
       <c r="D45" s="34" t="s">
         <v>59</v>
       </c>
@@ -3580,8 +3582,8 @@
       <c r="W45" s="20"/>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B46" s="104"/>
-      <c r="C46" s="117"/>
+      <c r="B46" s="119"/>
+      <c r="C46" s="110"/>
       <c r="D46" s="34" t="s">
         <v>60</v>
       </c>
@@ -3619,8 +3621,8 @@
       <c r="W46" s="20"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B47" s="104"/>
-      <c r="C47" s="117"/>
+      <c r="B47" s="119"/>
+      <c r="C47" s="110"/>
       <c r="D47" s="34" t="s">
         <v>61</v>
       </c>
@@ -3658,8 +3660,8 @@
       <c r="W47" s="20"/>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B48" s="104"/>
-      <c r="C48" s="117"/>
+      <c r="B48" s="119"/>
+      <c r="C48" s="110"/>
       <c r="D48" s="34" t="s">
         <v>62</v>
       </c>
@@ -3697,8 +3699,8 @@
       <c r="W48" s="20"/>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B49" s="104"/>
-      <c r="C49" s="117"/>
+      <c r="B49" s="119"/>
+      <c r="C49" s="110"/>
       <c r="D49" s="34" t="s">
         <v>63</v>
       </c>
@@ -3736,8 +3738,8 @@
       <c r="W49" s="20"/>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B50" s="104"/>
-      <c r="C50" s="117"/>
+      <c r="B50" s="119"/>
+      <c r="C50" s="110"/>
       <c r="D50" s="34" t="s">
         <v>64</v>
       </c>
@@ -3775,8 +3777,8 @@
       <c r="W50" s="20"/>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B51" s="104"/>
-      <c r="C51" s="117"/>
+      <c r="B51" s="119"/>
+      <c r="C51" s="110"/>
       <c r="D51" s="34" t="s">
         <v>65</v>
       </c>
@@ -3814,8 +3816,8 @@
       <c r="W51" s="20"/>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B52" s="104"/>
-      <c r="C52" s="117"/>
+      <c r="B52" s="119"/>
+      <c r="C52" s="110"/>
       <c r="D52" s="34" t="s">
         <v>66</v>
       </c>
@@ -3853,8 +3855,8 @@
       <c r="W52" s="20"/>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B53" s="104"/>
-      <c r="C53" s="117"/>
+      <c r="B53" s="119"/>
+      <c r="C53" s="110"/>
       <c r="D53" s="34" t="s">
         <v>67</v>
       </c>
@@ -3892,8 +3894,8 @@
       <c r="W53" s="20"/>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B54" s="104"/>
-      <c r="C54" s="117"/>
+      <c r="B54" s="119"/>
+      <c r="C54" s="110"/>
       <c r="D54" s="34" t="s">
         <v>68</v>
       </c>
@@ -3931,8 +3933,8 @@
       <c r="W54" s="20"/>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B55" s="104"/>
-      <c r="C55" s="118"/>
+      <c r="B55" s="119"/>
+      <c r="C55" s="111"/>
       <c r="D55" s="34" t="s">
         <v>69</v>
       </c>
@@ -3970,8 +3972,8 @@
       <c r="W55" s="20"/>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B56" s="104"/>
-      <c r="C56" s="114" t="s">
+      <c r="B56" s="119"/>
+      <c r="C56" s="107" t="s">
         <v>26</v>
       </c>
       <c r="D56" s="31" t="s">
@@ -4011,8 +4013,8 @@
       <c r="W56" s="20"/>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B57" s="104"/>
-      <c r="C57" s="115"/>
+      <c r="B57" s="119"/>
+      <c r="C57" s="108"/>
       <c r="D57" s="31" t="s">
         <v>29</v>
       </c>
@@ -4050,8 +4052,8 @@
       <c r="W57" s="20"/>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B58" s="104"/>
-      <c r="C58" s="115"/>
+      <c r="B58" s="119"/>
+      <c r="C58" s="108"/>
       <c r="D58" s="31" t="s">
         <v>30</v>
       </c>
@@ -4089,8 +4091,8 @@
       <c r="W58" s="20"/>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B59" s="104"/>
-      <c r="C59" s="115"/>
+      <c r="B59" s="119"/>
+      <c r="C59" s="108"/>
       <c r="D59" s="31" t="s">
         <v>31</v>
       </c>
@@ -4128,8 +4130,8 @@
       <c r="W59" s="20"/>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B60" s="104"/>
-      <c r="C60" s="115"/>
+      <c r="B60" s="119"/>
+      <c r="C60" s="108"/>
       <c r="D60" s="31" t="s">
         <v>34</v>
       </c>
@@ -4167,8 +4169,8 @@
       <c r="W60" s="20"/>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B61" s="104"/>
-      <c r="C61" s="115"/>
+      <c r="B61" s="119"/>
+      <c r="C61" s="108"/>
       <c r="D61" s="31" t="s">
         <v>32</v>
       </c>
@@ -4206,8 +4208,8 @@
       <c r="W61" s="20"/>
     </row>
     <row r="62" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="105"/>
-      <c r="C62" s="115"/>
+      <c r="B62" s="120"/>
+      <c r="C62" s="108"/>
       <c r="D62" s="74" t="s">
         <v>33</v>
       </c>
@@ -4245,10 +4247,10 @@
       <c r="W62" s="29"/>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B63" s="106" t="s">
+      <c r="B63" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="119" t="s">
+      <c r="C63" s="112" t="s">
         <v>79</v>
       </c>
       <c r="D63" s="44" t="s">
@@ -4288,8 +4290,8 @@
       <c r="W63" s="57"/>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B64" s="107"/>
-      <c r="C64" s="117"/>
+      <c r="B64" s="105"/>
+      <c r="C64" s="110"/>
       <c r="D64" s="4" t="s">
         <v>71</v>
       </c>
@@ -4327,8 +4329,8 @@
       <c r="W64" s="20"/>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B65" s="107"/>
-      <c r="C65" s="117"/>
+      <c r="B65" s="105"/>
+      <c r="C65" s="110"/>
       <c r="D65" s="4" t="s">
         <v>72</v>
       </c>
@@ -4366,8 +4368,8 @@
       <c r="W65" s="20"/>
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B66" s="107"/>
-      <c r="C66" s="118"/>
+      <c r="B66" s="105"/>
+      <c r="C66" s="111"/>
       <c r="D66" s="31" t="s">
         <v>76</v>
       </c>
@@ -4405,7 +4407,7 @@
       <c r="W66" s="20"/>
     </row>
     <row r="67" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B67" s="107"/>
+      <c r="B67" s="105"/>
       <c r="C67" s="35" t="s">
         <v>73</v>
       </c>
@@ -4444,7 +4446,7 @@
       <c r="W67" s="20"/>
     </row>
     <row r="68" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B68" s="107"/>
+      <c r="B68" s="105"/>
       <c r="C68" s="61" t="s">
         <v>81</v>
       </c>
@@ -4483,8 +4485,8 @@
       <c r="W68" s="20"/>
     </row>
     <row r="69" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="107"/>
-      <c r="C69" s="116" t="s">
+      <c r="B69" s="105"/>
+      <c r="C69" s="109" t="s">
         <v>80</v>
       </c>
       <c r="D69" s="4" t="s">
@@ -4524,8 +4526,8 @@
       <c r="W69" s="20"/>
     </row>
     <row r="70" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="107"/>
-      <c r="C70" s="117"/>
+      <c r="B70" s="105"/>
+      <c r="C70" s="110"/>
       <c r="D70" s="4" t="s">
         <v>75</v>
       </c>
@@ -4563,8 +4565,8 @@
       <c r="W70" s="20"/>
     </row>
     <row r="71" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="107"/>
-      <c r="C71" s="117"/>
+      <c r="B71" s="105"/>
+      <c r="C71" s="110"/>
       <c r="D71" s="4" t="s">
         <v>77</v>
       </c>
@@ -4602,8 +4604,8 @@
       <c r="W71" s="20"/>
     </row>
     <row r="72" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="108"/>
-      <c r="C72" s="120"/>
+      <c r="B72" s="106"/>
+      <c r="C72" s="113"/>
       <c r="D72" s="25" t="s">
         <v>78</v>
       </c>
@@ -4641,10 +4643,10 @@
       <c r="W72" s="26"/>
     </row>
     <row r="73" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="103" t="s">
+      <c r="B73" s="118" t="s">
         <v>117</v>
       </c>
-      <c r="C73" s="121" t="s">
+      <c r="C73" s="99" t="s">
         <v>118</v>
       </c>
       <c r="D73" s="44" t="s">
@@ -4684,8 +4686,8 @@
       <c r="W73" s="57"/>
     </row>
     <row r="74" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="104"/>
-      <c r="C74" s="109"/>
+      <c r="B74" s="119"/>
+      <c r="C74" s="100"/>
       <c r="D74" s="4" t="s">
         <v>134</v>
       </c>
@@ -4723,8 +4725,8 @@
       <c r="W74" s="20"/>
     </row>
     <row r="75" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="104"/>
-      <c r="C75" s="109"/>
+      <c r="B75" s="119"/>
+      <c r="C75" s="100"/>
       <c r="D75" s="4" t="s">
         <v>135</v>
       </c>
@@ -4762,8 +4764,8 @@
       <c r="W75" s="20"/>
     </row>
     <row r="76" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="104"/>
-      <c r="C76" s="109"/>
+      <c r="B76" s="119"/>
+      <c r="C76" s="100"/>
       <c r="D76" s="4" t="s">
         <v>136</v>
       </c>
@@ -4801,8 +4803,8 @@
       <c r="W76" s="20"/>
     </row>
     <row r="77" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="104"/>
-      <c r="C77" s="109" t="s">
+      <c r="B77" s="119"/>
+      <c r="C77" s="100" t="s">
         <v>119</v>
       </c>
       <c r="D77" s="4" t="s">
@@ -4842,8 +4844,8 @@
       <c r="W77" s="20"/>
     </row>
     <row r="78" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="104"/>
-      <c r="C78" s="109"/>
+      <c r="B78" s="119"/>
+      <c r="C78" s="100"/>
       <c r="D78" s="4" t="s">
         <v>134</v>
       </c>
@@ -4881,8 +4883,8 @@
       <c r="W78" s="20"/>
     </row>
     <row r="79" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="104"/>
-      <c r="C79" s="109"/>
+      <c r="B79" s="119"/>
+      <c r="C79" s="100"/>
       <c r="D79" s="4" t="s">
         <v>135</v>
       </c>
@@ -4920,8 +4922,8 @@
       <c r="W79" s="20"/>
     </row>
     <row r="80" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="104"/>
-      <c r="C80" s="109"/>
+      <c r="B80" s="119"/>
+      <c r="C80" s="100"/>
       <c r="D80" s="4" t="s">
         <v>136</v>
       </c>
@@ -4959,8 +4961,8 @@
       <c r="W80" s="20"/>
     </row>
     <row r="81" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="104"/>
-      <c r="C81" s="109" t="s">
+      <c r="B81" s="119"/>
+      <c r="C81" s="100" t="s">
         <v>120</v>
       </c>
       <c r="D81" s="4" t="s">
@@ -5000,8 +5002,8 @@
       <c r="W81" s="20"/>
     </row>
     <row r="82" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="104"/>
-      <c r="C82" s="109"/>
+      <c r="B82" s="119"/>
+      <c r="C82" s="100"/>
       <c r="D82" s="4" t="s">
         <v>134</v>
       </c>
@@ -5039,8 +5041,8 @@
       <c r="W82" s="20"/>
     </row>
     <row r="83" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="104"/>
-      <c r="C83" s="109"/>
+      <c r="B83" s="119"/>
+      <c r="C83" s="100"/>
       <c r="D83" s="4" t="s">
         <v>135</v>
       </c>
@@ -5078,8 +5080,8 @@
       <c r="W83" s="20"/>
     </row>
     <row r="84" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="104"/>
-      <c r="C84" s="109"/>
+      <c r="B84" s="119"/>
+      <c r="C84" s="100"/>
       <c r="D84" s="4" t="s">
         <v>136</v>
       </c>
@@ -5117,8 +5119,8 @@
       <c r="W84" s="20"/>
     </row>
     <row r="85" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="104"/>
-      <c r="C85" s="109" t="s">
+      <c r="B85" s="119"/>
+      <c r="C85" s="100" t="s">
         <v>121</v>
       </c>
       <c r="D85" s="4" t="s">
@@ -5158,8 +5160,8 @@
       <c r="W85" s="20"/>
     </row>
     <row r="86" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="104"/>
-      <c r="C86" s="109"/>
+      <c r="B86" s="119"/>
+      <c r="C86" s="100"/>
       <c r="D86" s="4" t="s">
         <v>134</v>
       </c>
@@ -5197,8 +5199,8 @@
       <c r="W86" s="20"/>
     </row>
     <row r="87" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="104"/>
-      <c r="C87" s="109"/>
+      <c r="B87" s="119"/>
+      <c r="C87" s="100"/>
       <c r="D87" s="4" t="s">
         <v>135</v>
       </c>
@@ -5236,8 +5238,8 @@
       <c r="W87" s="20"/>
     </row>
     <row r="88" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="104"/>
-      <c r="C88" s="109"/>
+      <c r="B88" s="119"/>
+      <c r="C88" s="100"/>
       <c r="D88" s="4" t="s">
         <v>136</v>
       </c>
@@ -5275,8 +5277,8 @@
       <c r="W88" s="20"/>
     </row>
     <row r="89" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="104"/>
-      <c r="C89" s="109" t="s">
+      <c r="B89" s="119"/>
+      <c r="C89" s="100" t="s">
         <v>122</v>
       </c>
       <c r="D89" s="4" t="s">
@@ -5316,8 +5318,8 @@
       <c r="W89" s="20"/>
     </row>
     <row r="90" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="104"/>
-      <c r="C90" s="109"/>
+      <c r="B90" s="119"/>
+      <c r="C90" s="100"/>
       <c r="D90" s="4" t="s">
         <v>134</v>
       </c>
@@ -5355,8 +5357,8 @@
       <c r="W90" s="20"/>
     </row>
     <row r="91" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="104"/>
-      <c r="C91" s="109"/>
+      <c r="B91" s="119"/>
+      <c r="C91" s="100"/>
       <c r="D91" s="4" t="s">
         <v>135</v>
       </c>
@@ -5394,8 +5396,8 @@
       <c r="W91" s="20"/>
     </row>
     <row r="92" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="104"/>
-      <c r="C92" s="109"/>
+      <c r="B92" s="119"/>
+      <c r="C92" s="100"/>
       <c r="D92" s="4" t="s">
         <v>136</v>
       </c>
@@ -5433,8 +5435,8 @@
       <c r="W92" s="20"/>
     </row>
     <row r="93" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="104"/>
-      <c r="C93" s="109" t="s">
+      <c r="B93" s="119"/>
+      <c r="C93" s="100" t="s">
         <v>123</v>
       </c>
       <c r="D93" s="4" t="s">
@@ -5474,8 +5476,8 @@
       <c r="W93" s="20"/>
     </row>
     <row r="94" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="104"/>
-      <c r="C94" s="109"/>
+      <c r="B94" s="119"/>
+      <c r="C94" s="100"/>
       <c r="D94" s="4" t="s">
         <v>134</v>
       </c>
@@ -5513,8 +5515,8 @@
       <c r="W94" s="20"/>
     </row>
     <row r="95" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="104"/>
-      <c r="C95" s="109"/>
+      <c r="B95" s="119"/>
+      <c r="C95" s="100"/>
       <c r="D95" s="4" t="s">
         <v>135</v>
       </c>
@@ -5552,8 +5554,8 @@
       <c r="W95" s="20"/>
     </row>
     <row r="96" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="104"/>
-      <c r="C96" s="109"/>
+      <c r="B96" s="119"/>
+      <c r="C96" s="100"/>
       <c r="D96" s="4" t="s">
         <v>136</v>
       </c>
@@ -5591,8 +5593,8 @@
       <c r="W96" s="20"/>
     </row>
     <row r="97" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="104"/>
-      <c r="C97" s="109" t="s">
+      <c r="B97" s="119"/>
+      <c r="C97" s="100" t="s">
         <v>124</v>
       </c>
       <c r="D97" s="4" t="s">
@@ -5632,8 +5634,8 @@
       <c r="W97" s="20"/>
     </row>
     <row r="98" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="104"/>
-      <c r="C98" s="109"/>
+      <c r="B98" s="119"/>
+      <c r="C98" s="100"/>
       <c r="D98" s="4" t="s">
         <v>134</v>
       </c>
@@ -5671,8 +5673,8 @@
       <c r="W98" s="20"/>
     </row>
     <row r="99" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="104"/>
-      <c r="C99" s="109"/>
+      <c r="B99" s="119"/>
+      <c r="C99" s="100"/>
       <c r="D99" s="4" t="s">
         <v>135</v>
       </c>
@@ -5710,8 +5712,8 @@
       <c r="W99" s="20"/>
     </row>
     <row r="100" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="104"/>
-      <c r="C100" s="109"/>
+      <c r="B100" s="119"/>
+      <c r="C100" s="100"/>
       <c r="D100" s="4" t="s">
         <v>136</v>
       </c>
@@ -5749,8 +5751,8 @@
       <c r="W100" s="20"/>
     </row>
     <row r="101" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="104"/>
-      <c r="C101" s="109" t="s">
+      <c r="B101" s="119"/>
+      <c r="C101" s="100" t="s">
         <v>125</v>
       </c>
       <c r="D101" s="4" t="s">
@@ -5790,8 +5792,8 @@
       <c r="W101" s="20"/>
     </row>
     <row r="102" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="104"/>
-      <c r="C102" s="109"/>
+      <c r="B102" s="119"/>
+      <c r="C102" s="100"/>
       <c r="D102" s="4" t="s">
         <v>134</v>
       </c>
@@ -5829,8 +5831,8 @@
       <c r="W102" s="20"/>
     </row>
     <row r="103" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="104"/>
-      <c r="C103" s="109"/>
+      <c r="B103" s="119"/>
+      <c r="C103" s="100"/>
       <c r="D103" s="4" t="s">
         <v>135</v>
       </c>
@@ -5868,8 +5870,8 @@
       <c r="W103" s="20"/>
     </row>
     <row r="104" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="104"/>
-      <c r="C104" s="109"/>
+      <c r="B104" s="119"/>
+      <c r="C104" s="100"/>
       <c r="D104" s="4" t="s">
         <v>136</v>
       </c>
@@ -5907,8 +5909,8 @@
       <c r="W104" s="20"/>
     </row>
     <row r="105" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="104"/>
-      <c r="C105" s="109" t="s">
+      <c r="B105" s="119"/>
+      <c r="C105" s="100" t="s">
         <v>126</v>
       </c>
       <c r="D105" s="4" t="s">
@@ -5948,8 +5950,8 @@
       <c r="W105" s="20"/>
     </row>
     <row r="106" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="104"/>
-      <c r="C106" s="109"/>
+      <c r="B106" s="119"/>
+      <c r="C106" s="100"/>
       <c r="D106" s="4" t="s">
         <v>134</v>
       </c>
@@ -5987,8 +5989,8 @@
       <c r="W106" s="20"/>
     </row>
     <row r="107" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="104"/>
-      <c r="C107" s="109"/>
+      <c r="B107" s="119"/>
+      <c r="C107" s="100"/>
       <c r="D107" s="4" t="s">
         <v>135</v>
       </c>
@@ -6026,8 +6028,8 @@
       <c r="W107" s="20"/>
     </row>
     <row r="108" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="104"/>
-      <c r="C108" s="109"/>
+      <c r="B108" s="119"/>
+      <c r="C108" s="100"/>
       <c r="D108" s="4" t="s">
         <v>136</v>
       </c>
@@ -6065,8 +6067,8 @@
       <c r="W108" s="20"/>
     </row>
     <row r="109" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="104"/>
-      <c r="C109" s="109" t="s">
+      <c r="B109" s="119"/>
+      <c r="C109" s="100" t="s">
         <v>127</v>
       </c>
       <c r="D109" s="4" t="s">
@@ -6106,8 +6108,8 @@
       <c r="W109" s="20"/>
     </row>
     <row r="110" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="104"/>
-      <c r="C110" s="109"/>
+      <c r="B110" s="119"/>
+      <c r="C110" s="100"/>
       <c r="D110" s="4" t="s">
         <v>134</v>
       </c>
@@ -6145,8 +6147,8 @@
       <c r="W110" s="20"/>
     </row>
     <row r="111" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="104"/>
-      <c r="C111" s="109"/>
+      <c r="B111" s="119"/>
+      <c r="C111" s="100"/>
       <c r="D111" s="4" t="s">
         <v>135</v>
       </c>
@@ -6184,8 +6186,8 @@
       <c r="W111" s="20"/>
     </row>
     <row r="112" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="104"/>
-      <c r="C112" s="109"/>
+      <c r="B112" s="119"/>
+      <c r="C112" s="100"/>
       <c r="D112" s="4" t="s">
         <v>136</v>
       </c>
@@ -6223,8 +6225,8 @@
       <c r="W112" s="20"/>
     </row>
     <row r="113" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="104"/>
-      <c r="C113" s="109" t="s">
+      <c r="B113" s="119"/>
+      <c r="C113" s="100" t="s">
         <v>128</v>
       </c>
       <c r="D113" s="4" t="s">
@@ -6264,8 +6266,8 @@
       <c r="W113" s="20"/>
     </row>
     <row r="114" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="104"/>
-      <c r="C114" s="109"/>
+      <c r="B114" s="119"/>
+      <c r="C114" s="100"/>
       <c r="D114" s="4" t="s">
         <v>134</v>
       </c>
@@ -6303,8 +6305,8 @@
       <c r="W114" s="20"/>
     </row>
     <row r="115" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="104"/>
-      <c r="C115" s="109"/>
+      <c r="B115" s="119"/>
+      <c r="C115" s="100"/>
       <c r="D115" s="4" t="s">
         <v>135</v>
       </c>
@@ -6342,8 +6344,8 @@
       <c r="W115" s="20"/>
     </row>
     <row r="116" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="104"/>
-      <c r="C116" s="109"/>
+      <c r="B116" s="119"/>
+      <c r="C116" s="100"/>
       <c r="D116" s="4" t="s">
         <v>136</v>
       </c>
@@ -6381,8 +6383,8 @@
       <c r="W116" s="20"/>
     </row>
     <row r="117" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="104"/>
-      <c r="C117" s="109" t="s">
+      <c r="B117" s="119"/>
+      <c r="C117" s="100" t="s">
         <v>129</v>
       </c>
       <c r="D117" s="4" t="s">
@@ -6422,8 +6424,8 @@
       <c r="W117" s="20"/>
     </row>
     <row r="118" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="104"/>
-      <c r="C118" s="109"/>
+      <c r="B118" s="119"/>
+      <c r="C118" s="100"/>
       <c r="D118" s="4" t="s">
         <v>134</v>
       </c>
@@ -6461,8 +6463,8 @@
       <c r="W118" s="20"/>
     </row>
     <row r="119" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="104"/>
-      <c r="C119" s="109"/>
+      <c r="B119" s="119"/>
+      <c r="C119" s="100"/>
       <c r="D119" s="4" t="s">
         <v>135</v>
       </c>
@@ -6500,8 +6502,8 @@
       <c r="W119" s="20"/>
     </row>
     <row r="120" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="104"/>
-      <c r="C120" s="109"/>
+      <c r="B120" s="119"/>
+      <c r="C120" s="100"/>
       <c r="D120" s="4" t="s">
         <v>136</v>
       </c>
@@ -6539,8 +6541,8 @@
       <c r="W120" s="20"/>
     </row>
     <row r="121" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="104"/>
-      <c r="C121" s="109" t="s">
+      <c r="B121" s="119"/>
+      <c r="C121" s="100" t="s">
         <v>130</v>
       </c>
       <c r="D121" s="4" t="s">
@@ -6580,8 +6582,8 @@
       <c r="W121" s="20"/>
     </row>
     <row r="122" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="104"/>
-      <c r="C122" s="109"/>
+      <c r="B122" s="119"/>
+      <c r="C122" s="100"/>
       <c r="D122" s="4" t="s">
         <v>134</v>
       </c>
@@ -6619,8 +6621,8 @@
       <c r="W122" s="20"/>
     </row>
     <row r="123" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="104"/>
-      <c r="C123" s="109"/>
+      <c r="B123" s="119"/>
+      <c r="C123" s="100"/>
       <c r="D123" s="4" t="s">
         <v>135</v>
       </c>
@@ -6658,8 +6660,8 @@
       <c r="W123" s="20"/>
     </row>
     <row r="124" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="104"/>
-      <c r="C124" s="109"/>
+      <c r="B124" s="119"/>
+      <c r="C124" s="100"/>
       <c r="D124" s="4" t="s">
         <v>136</v>
       </c>
@@ -6697,8 +6699,8 @@
       <c r="W124" s="20"/>
     </row>
     <row r="125" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="104"/>
-      <c r="C125" s="109" t="s">
+      <c r="B125" s="119"/>
+      <c r="C125" s="100" t="s">
         <v>131</v>
       </c>
       <c r="D125" s="4" t="s">
@@ -6738,8 +6740,8 @@
       <c r="W125" s="20"/>
     </row>
     <row r="126" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="104"/>
-      <c r="C126" s="109"/>
+      <c r="B126" s="119"/>
+      <c r="C126" s="100"/>
       <c r="D126" s="4" t="s">
         <v>134</v>
       </c>
@@ -6777,8 +6779,8 @@
       <c r="W126" s="20"/>
     </row>
     <row r="127" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="104"/>
-      <c r="C127" s="109"/>
+      <c r="B127" s="119"/>
+      <c r="C127" s="100"/>
       <c r="D127" s="4" t="s">
         <v>135</v>
       </c>
@@ -6816,8 +6818,8 @@
       <c r="W127" s="20"/>
     </row>
     <row r="128" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="104"/>
-      <c r="C128" s="109"/>
+      <c r="B128" s="119"/>
+      <c r="C128" s="100"/>
       <c r="D128" s="4" t="s">
         <v>136</v>
       </c>
@@ -6855,8 +6857,8 @@
       <c r="W128" s="20"/>
     </row>
     <row r="129" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="104"/>
-      <c r="C129" s="109" t="s">
+      <c r="B129" s="119"/>
+      <c r="C129" s="100" t="s">
         <v>132</v>
       </c>
       <c r="D129" s="4" t="s">
@@ -6896,8 +6898,8 @@
       <c r="W129" s="20"/>
     </row>
     <row r="130" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="104"/>
-      <c r="C130" s="109"/>
+      <c r="B130" s="119"/>
+      <c r="C130" s="100"/>
       <c r="D130" s="4" t="s">
         <v>134</v>
       </c>
@@ -6935,8 +6937,8 @@
       <c r="W130" s="20"/>
     </row>
     <row r="131" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="104"/>
-      <c r="C131" s="109"/>
+      <c r="B131" s="119"/>
+      <c r="C131" s="100"/>
       <c r="D131" s="4" t="s">
         <v>135</v>
       </c>
@@ -6974,8 +6976,8 @@
       <c r="W131" s="20"/>
     </row>
     <row r="132" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B132" s="110"/>
-      <c r="C132" s="113"/>
+      <c r="B132" s="121"/>
+      <c r="C132" s="122"/>
       <c r="D132" s="25" t="s">
         <v>136</v>
       </c>
@@ -7013,7 +7015,7 @@
       <c r="W132" s="26"/>
     </row>
     <row r="133" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B133" s="106" t="s">
+      <c r="B133" s="104" t="s">
         <v>83</v>
       </c>
       <c r="C133" s="92" t="s">
@@ -7054,7 +7056,7 @@
       <c r="W133" s="57"/>
     </row>
     <row r="134" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="107"/>
+      <c r="B134" s="105"/>
       <c r="C134" s="38" t="s">
         <v>89</v>
       </c>
@@ -7093,7 +7095,7 @@
       <c r="W134" s="20"/>
     </row>
     <row r="135" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="107"/>
+      <c r="B135" s="105"/>
       <c r="C135" s="38" t="s">
         <v>90</v>
       </c>
@@ -7132,7 +7134,7 @@
       <c r="W135" s="20"/>
     </row>
     <row r="136" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="107"/>
+      <c r="B136" s="105"/>
       <c r="C136" s="38" t="s">
         <v>91</v>
       </c>
@@ -7171,7 +7173,7 @@
       <c r="W136" s="20"/>
     </row>
     <row r="137" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="107"/>
+      <c r="B137" s="105"/>
       <c r="C137" s="38" t="s">
         <v>143</v>
       </c>
@@ -7210,7 +7212,7 @@
       <c r="W137" s="20"/>
     </row>
     <row r="138" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="107"/>
+      <c r="B138" s="105"/>
       <c r="C138" s="38" t="s">
         <v>140</v>
       </c>
@@ -7249,7 +7251,7 @@
       <c r="W138" s="20"/>
     </row>
     <row r="139" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="107"/>
+      <c r="B139" s="105"/>
       <c r="C139" s="38" t="s">
         <v>142</v>
       </c>
@@ -7288,7 +7290,7 @@
       <c r="W139" s="20"/>
     </row>
     <row r="140" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="107"/>
+      <c r="B140" s="105"/>
       <c r="C140" s="38" t="s">
         <v>141</v>
       </c>
@@ -7327,7 +7329,7 @@
       <c r="W140" s="20"/>
     </row>
     <row r="141" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="107"/>
+      <c r="B141" s="105"/>
       <c r="C141" s="38" t="s">
         <v>92</v>
       </c>
@@ -7366,7 +7368,7 @@
       <c r="W141" s="20"/>
     </row>
     <row r="142" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="107"/>
+      <c r="B142" s="105"/>
       <c r="C142" s="38" t="s">
         <v>93</v>
       </c>
@@ -7405,7 +7407,7 @@
       <c r="W142" s="20"/>
     </row>
     <row r="143" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="107"/>
+      <c r="B143" s="105"/>
       <c r="C143" s="38" t="s">
         <v>94</v>
       </c>
@@ -7444,7 +7446,7 @@
       <c r="W143" s="20"/>
     </row>
     <row r="144" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="107"/>
+      <c r="B144" s="105"/>
       <c r="C144" s="38" t="s">
         <v>98</v>
       </c>
@@ -7483,7 +7485,7 @@
       <c r="W144" s="20"/>
     </row>
     <row r="145" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B145" s="108"/>
+      <c r="B145" s="106"/>
       <c r="C145" s="62" t="s">
         <v>99</v>
       </c>
@@ -7522,7 +7524,7 @@
       <c r="W145" s="26"/>
     </row>
     <row r="146" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="103" t="s">
+      <c r="B146" s="118" t="s">
         <v>144</v>
       </c>
       <c r="C146" s="72" t="s">
@@ -7563,7 +7565,7 @@
       <c r="W146" s="57"/>
     </row>
     <row r="147" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="104"/>
+      <c r="B147" s="119"/>
       <c r="C147" s="71" t="s">
         <v>145</v>
       </c>
@@ -7602,7 +7604,7 @@
       <c r="W147" s="20"/>
     </row>
     <row r="148" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="110"/>
+      <c r="B148" s="121"/>
       <c r="C148" s="73" t="s">
         <v>146</v>
       </c>
@@ -7641,7 +7643,7 @@
       <c r="W148" s="26"/>
     </row>
     <row r="149" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="107" t="s">
+      <c r="B149" s="105" t="s">
         <v>18</v>
       </c>
       <c r="C149" s="38" t="s">
@@ -7682,7 +7684,7 @@
       <c r="W149" s="70"/>
     </row>
     <row r="150" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="107"/>
+      <c r="B150" s="105"/>
       <c r="C150" s="38" t="s">
         <v>138</v>
       </c>
@@ -7721,7 +7723,7 @@
       <c r="W150" s="70"/>
     </row>
     <row r="151" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="107"/>
+      <c r="B151" s="105"/>
       <c r="C151" s="38" t="s">
         <v>139</v>
       </c>
@@ -7760,7 +7762,7 @@
       <c r="W151" s="70"/>
     </row>
     <row r="152" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="107"/>
+      <c r="B152" s="105"/>
       <c r="C152" s="38" t="s">
         <v>147</v>
       </c>
@@ -7799,7 +7801,7 @@
       <c r="W152" s="20"/>
     </row>
     <row r="153" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="107"/>
+      <c r="B153" s="105"/>
       <c r="C153" s="35" t="s">
         <v>84</v>
       </c>
@@ -7838,7 +7840,7 @@
       <c r="W153" s="20"/>
     </row>
     <row r="154" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="107"/>
+      <c r="B154" s="105"/>
       <c r="C154" s="35" t="s">
         <v>85</v>
       </c>
@@ -7877,7 +7879,7 @@
       <c r="W154" s="20"/>
     </row>
     <row r="155" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="107"/>
+      <c r="B155" s="105"/>
       <c r="C155" s="39" t="s">
         <v>87</v>
       </c>
@@ -7916,7 +7918,7 @@
       <c r="W155" s="29"/>
     </row>
     <row r="156" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="107"/>
+      <c r="B156" s="105"/>
       <c r="C156" s="35" t="s">
         <v>86</v>
       </c>
@@ -7955,7 +7957,7 @@
       <c r="W156" s="29"/>
     </row>
     <row r="157" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="107"/>
+      <c r="B157" s="105"/>
       <c r="C157" s="41" t="s">
         <v>104</v>
       </c>
@@ -7994,7 +7996,7 @@
       <c r="W157" s="29"/>
     </row>
     <row r="158" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="107"/>
+      <c r="B158" s="105"/>
       <c r="C158" s="41" t="s">
         <v>137</v>
       </c>
@@ -8033,7 +8035,7 @@
       <c r="W158" s="29"/>
     </row>
     <row r="159" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="107"/>
+      <c r="B159" s="105"/>
       <c r="C159" s="41" t="s">
         <v>105</v>
       </c>
@@ -8072,7 +8074,7 @@
       <c r="W159" s="29"/>
     </row>
     <row r="160" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B160" s="108"/>
+      <c r="B160" s="106"/>
       <c r="C160" s="62" t="s">
         <v>100</v>
       </c>
@@ -8111,21 +8113,21 @@
       <c r="W160" s="26"/>
     </row>
     <row r="161" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B161" s="98" t="s">
+      <c r="B161" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="C161" s="101"/>
-      <c r="D161" s="99"/>
-      <c r="E161" s="99"/>
-      <c r="F161" s="99"/>
-      <c r="G161" s="102"/>
+      <c r="C161" s="116"/>
+      <c r="D161" s="115"/>
+      <c r="E161" s="115"/>
+      <c r="F161" s="115"/>
+      <c r="G161" s="117"/>
       <c r="H161" s="40">
         <f>SUM(H4:H160)</f>
         <v>89.199999999999989</v>
       </c>
       <c r="I161" s="24">
         <f>SUM(I4:I160)</f>
-        <v>0.93330000000000002</v>
+        <v>1.4333</v>
       </c>
       <c r="J161" s="24">
         <f>SUM(J4:J160)</f>
@@ -8133,7 +8135,7 @@
       </c>
       <c r="K161" s="24">
         <f t="shared" ref="K161:W161" si="5">SUM(K4:K160)</f>
-        <v>0.93330000000000002</v>
+        <v>1.4333</v>
       </c>
       <c r="L161" s="24">
         <f t="shared" si="5"/>
@@ -8193,22 +8195,22 @@
       <c r="G162" s="2"/>
       <c r="H162" s="2"/>
       <c r="I162" s="2"/>
-      <c r="J162" s="100" t="s">
+      <c r="J162" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="K162" s="111"/>
-      <c r="L162" s="111"/>
-      <c r="M162" s="111"/>
-      <c r="N162" s="111"/>
-      <c r="O162" s="111"/>
-      <c r="P162" s="111"/>
-      <c r="Q162" s="111"/>
-      <c r="R162" s="111"/>
-      <c r="S162" s="111"/>
-      <c r="T162" s="111"/>
-      <c r="U162" s="111"/>
-      <c r="V162" s="111"/>
-      <c r="W162" s="112"/>
+      <c r="K162" s="102"/>
+      <c r="L162" s="102"/>
+      <c r="M162" s="102"/>
+      <c r="N162" s="102"/>
+      <c r="O162" s="102"/>
+      <c r="P162" s="102"/>
+      <c r="Q162" s="102"/>
+      <c r="R162" s="102"/>
+      <c r="S162" s="102"/>
+      <c r="T162" s="102"/>
+      <c r="U162" s="102"/>
+      <c r="V162" s="102"/>
+      <c r="W162" s="103"/>
     </row>
     <row r="163" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B163" s="2"/>
@@ -8232,29 +8234,29 @@
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
-      <c r="H164" s="98" t="s">
+      <c r="H164" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="I164" s="99"/>
+      <c r="I164" s="115"/>
       <c r="J164" s="10">
         <f>H161-J161</f>
         <v>89.199999999999989</v>
       </c>
       <c r="K164" s="10">
         <f>J164-K161</f>
-        <v>88.266699999999986</v>
+        <v>87.766699999999986</v>
       </c>
       <c r="L164" s="10">
         <f>K164-L161</f>
-        <v>88.266699999999986</v>
+        <v>87.766699999999986</v>
       </c>
       <c r="M164" s="10">
         <f>L164-M161</f>
-        <v>88.266699999999986</v>
+        <v>87.766699999999986</v>
       </c>
       <c r="N164" s="11">
         <f>M164-N161</f>
-        <v>88.266699999999986</v>
+        <v>87.766699999999986</v>
       </c>
     </row>
     <row r="165" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8278,18 +8280,18 @@
       <c r="D166" s="3"/>
       <c r="E166" s="3"/>
       <c r="F166" s="3"/>
-      <c r="H166" s="100" t="s">
+      <c r="H166" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="I166" s="101"/>
-      <c r="J166" s="99">
+      <c r="I166" s="116"/>
+      <c r="J166" s="115">
         <f>H161-I161</f>
-        <v>88.266699999999986</v>
-      </c>
-      <c r="K166" s="99"/>
-      <c r="L166" s="99"/>
-      <c r="M166" s="99"/>
-      <c r="N166" s="102"/>
+        <v>87.766699999999986</v>
+      </c>
+      <c r="K166" s="115"/>
+      <c r="L166" s="115"/>
+      <c r="M166" s="115"/>
+      <c r="N166" s="117"/>
     </row>
     <row r="167" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B167" s="3"/>
@@ -8393,23 +8395,6 @@
     <row r="185" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C73:C76"/>
-    <mergeCell ref="C77:C80"/>
-    <mergeCell ref="C121:C124"/>
-    <mergeCell ref="C113:C116"/>
-    <mergeCell ref="C105:C108"/>
-    <mergeCell ref="C101:C104"/>
-    <mergeCell ref="C93:C96"/>
-    <mergeCell ref="C109:C112"/>
-    <mergeCell ref="C117:C120"/>
-    <mergeCell ref="J2:W2"/>
-    <mergeCell ref="B63:B72"/>
-    <mergeCell ref="C56:C62"/>
-    <mergeCell ref="C16:C55"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="C69:C72"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B14"/>
     <mergeCell ref="H164:I164"/>
     <mergeCell ref="H166:I166"/>
     <mergeCell ref="J166:N166"/>
@@ -8426,6 +8411,23 @@
     <mergeCell ref="C89:C92"/>
     <mergeCell ref="C85:C88"/>
     <mergeCell ref="C81:C84"/>
+    <mergeCell ref="J2:W2"/>
+    <mergeCell ref="B63:B72"/>
+    <mergeCell ref="C56:C62"/>
+    <mergeCell ref="C16:C55"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C69:C72"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C73:C76"/>
+    <mergeCell ref="C77:C80"/>
+    <mergeCell ref="C121:C124"/>
+    <mergeCell ref="C113:C116"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="C101:C104"/>
+    <mergeCell ref="C93:C96"/>
+    <mergeCell ref="C109:C112"/>
+    <mergeCell ref="C117:C120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Creado el prefab de Link, instanciado y funcional en OverWorld
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
+++ b/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Enti\MAP\The_Legend_of_Radev\MAP_LegendOfRadev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devildrake\Documents\MAP_LegendOfRadev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -470,7 +470,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1001,7 +1001,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1257,84 +1257,87 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1353,7 +1356,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1395,22 +1398,22 @@
                   <c:v>89.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87.666699999999992</c:v>
+                  <c:v>85.816699999999983</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87.666699999999992</c:v>
+                  <c:v>85.816699999999983</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>87.666699999999992</c:v>
+                  <c:v>85.816699999999983</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>87.666699999999992</c:v>
+                  <c:v>85.816699999999983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A091-4901-839C-4EC24FB5B5C8}"/>
             </c:ext>
@@ -1425,11 +1428,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1036224592"/>
-        <c:axId val="1036214800"/>
+        <c:axId val="958207744"/>
+        <c:axId val="958205568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1036224592"/>
+        <c:axId val="958207744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1438,7 +1441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1036214800"/>
+        <c:crossAx val="958205568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1446,7 +1449,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1036214800"/>
+        <c:axId val="958205568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1457,7 +1460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1036224592"/>
+        <c:crossAx val="958207744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1803,52 +1806,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M154" sqref="M154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1"/>
     <col min="3" max="3" width="80" customWidth="1"/>
-    <col min="4" max="4" width="57.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="57.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" customWidth="1"/>
+    <col min="16" max="16" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="101" t="s">
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J2" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="112"/>
-      <c r="P2" s="112"/>
-      <c r="Q2" s="112"/>
-      <c r="R2" s="112"/>
-      <c r="S2" s="112"/>
-      <c r="T2" s="112"/>
-      <c r="U2" s="112"/>
-      <c r="V2" s="112"/>
-      <c r="W2" s="113"/>
-    </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="107"/>
+    </row>
+    <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="63" t="s">
         <v>7</v>
       </c>
@@ -1916,8 +1919,8 @@
         <v>43067</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="107" t="s">
+    <row r="4" spans="1:23" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="108" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="42" t="s">
@@ -1957,8 +1960,8 @@
       <c r="V4" s="46"/>
       <c r="W4" s="49"/>
     </row>
-    <row r="5" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="108"/>
+    <row r="5" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="109"/>
       <c r="C5" s="37" t="s">
         <v>101</v>
       </c>
@@ -1996,8 +1999,8 @@
       <c r="V5" s="18"/>
       <c r="W5" s="20"/>
     </row>
-    <row r="6" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="108"/>
+    <row r="6" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="109"/>
       <c r="C6" s="37" t="s">
         <v>102</v>
       </c>
@@ -2035,8 +2038,8 @@
       <c r="V6" s="18"/>
       <c r="W6" s="20"/>
     </row>
-    <row r="7" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="108"/>
+    <row r="7" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="109"/>
       <c r="C7" s="37" t="s">
         <v>103</v>
       </c>
@@ -2074,8 +2077,8 @@
       <c r="V7" s="18"/>
       <c r="W7" s="20"/>
     </row>
-    <row r="8" spans="1:23" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="109"/>
+    <row r="8" spans="1:23" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="110"/>
       <c r="C8" s="50" t="s">
         <v>112</v>
       </c>
@@ -2113,8 +2116,8 @@
       <c r="V8" s="23"/>
       <c r="W8" s="26"/>
     </row>
-    <row r="9" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="107" t="s">
+    <row r="9" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="108" t="s">
         <v>106</v>
       </c>
       <c r="C9" s="53" t="s">
@@ -2146,18 +2149,18 @@
       <c r="L9" s="97"/>
       <c r="M9" s="97"/>
       <c r="N9" s="97"/>
-      <c r="O9" s="124"/>
-      <c r="P9" s="125"/>
-      <c r="Q9" s="124"/>
-      <c r="R9" s="124"/>
-      <c r="S9" s="124"/>
-      <c r="T9" s="124"/>
-      <c r="U9" s="124"/>
-      <c r="V9" s="124"/>
-      <c r="W9" s="126"/>
-    </row>
-    <row r="10" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="108"/>
+      <c r="O9" s="100"/>
+      <c r="P9" s="101"/>
+      <c r="Q9" s="100"/>
+      <c r="R9" s="100"/>
+      <c r="S9" s="100"/>
+      <c r="T9" s="100"/>
+      <c r="U9" s="100"/>
+      <c r="V9" s="100"/>
+      <c r="W9" s="102"/>
+    </row>
+    <row r="10" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="109"/>
       <c r="C10" s="36" t="s">
         <v>107</v>
       </c>
@@ -2195,9 +2198,9 @@
       <c r="V10" s="18"/>
       <c r="W10" s="20"/>
     </row>
-    <row r="11" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="108"/>
-      <c r="C11" s="123" t="s">
+    <row r="11" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="109"/>
+      <c r="C11" s="99" t="s">
         <v>113</v>
       </c>
       <c r="D11" s="5"/>
@@ -2234,9 +2237,9 @@
       <c r="V11" s="18"/>
       <c r="W11" s="20"/>
     </row>
-    <row r="12" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="108"/>
-      <c r="C12" s="123" t="s">
+    <row r="12" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="109"/>
+      <c r="C12" s="99" t="s">
         <v>114</v>
       </c>
       <c r="D12" s="5"/>
@@ -2299,8 +2302,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="108"/>
+    <row r="13" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="109"/>
       <c r="C13" s="98" t="s">
         <v>108</v>
       </c>
@@ -2338,8 +2341,8 @@
       <c r="V13" s="18"/>
       <c r="W13" s="20"/>
     </row>
-    <row r="14" spans="1:23" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="109"/>
+    <row r="14" spans="1:23" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="110"/>
       <c r="C14" s="58" t="s">
         <v>97</v>
       </c>
@@ -2379,8 +2382,8 @@
       <c r="V14" s="23"/>
       <c r="W14" s="26"/>
     </row>
-    <row r="15" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="104" t="s">
+    <row r="15" spans="1:23" ht="18" x14ac:dyDescent="0.3">
+      <c r="B15" s="122" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="59" t="s">
@@ -2424,9 +2427,9 @@
       <c r="V15" s="56"/>
       <c r="W15" s="57"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B16" s="105"/>
-      <c r="C16" s="117" t="s">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B16" s="123"/>
+      <c r="C16" s="113" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -2465,9 +2468,9 @@
       <c r="V16" s="18"/>
       <c r="W16" s="20"/>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="105"/>
-      <c r="C17" s="118"/>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B17" s="123"/>
+      <c r="C17" s="114"/>
       <c r="D17" s="4" t="s">
         <v>20</v>
       </c>
@@ -2504,9 +2507,9 @@
       <c r="V17" s="18"/>
       <c r="W17" s="20"/>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="105"/>
-      <c r="C18" s="118"/>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B18" s="123"/>
+      <c r="C18" s="114"/>
       <c r="D18" s="4" t="s">
         <v>21</v>
       </c>
@@ -2543,9 +2546,9 @@
       <c r="V18" s="18"/>
       <c r="W18" s="20"/>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B19" s="105"/>
-      <c r="C19" s="118"/>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B19" s="123"/>
+      <c r="C19" s="114"/>
       <c r="D19" s="4" t="s">
         <v>22</v>
       </c>
@@ -2582,9 +2585,9 @@
       <c r="V19" s="18"/>
       <c r="W19" s="20"/>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B20" s="105"/>
-      <c r="C20" s="118"/>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B20" s="123"/>
+      <c r="C20" s="114"/>
       <c r="D20" s="4" t="s">
         <v>23</v>
       </c>
@@ -2621,9 +2624,9 @@
       <c r="V20" s="18"/>
       <c r="W20" s="20"/>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B21" s="105"/>
-      <c r="C21" s="118"/>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B21" s="123"/>
+      <c r="C21" s="114"/>
       <c r="D21" s="4" t="s">
         <v>24</v>
       </c>
@@ -2660,9 +2663,9 @@
       <c r="V21" s="18"/>
       <c r="W21" s="20"/>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B22" s="105"/>
-      <c r="C22" s="118"/>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B22" s="123"/>
+      <c r="C22" s="114"/>
       <c r="D22" s="34" t="s">
         <v>36</v>
       </c>
@@ -2699,9 +2702,9 @@
       <c r="V22" s="18"/>
       <c r="W22" s="20"/>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B23" s="105"/>
-      <c r="C23" s="118"/>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B23" s="123"/>
+      <c r="C23" s="114"/>
       <c r="D23" s="34" t="s">
         <v>37</v>
       </c>
@@ -2738,9 +2741,9 @@
       <c r="V23" s="18"/>
       <c r="W23" s="20"/>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B24" s="105"/>
-      <c r="C24" s="118"/>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B24" s="123"/>
+      <c r="C24" s="114"/>
       <c r="D24" s="34" t="s">
         <v>38</v>
       </c>
@@ -2777,9 +2780,9 @@
       <c r="V24" s="18"/>
       <c r="W24" s="20"/>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B25" s="105"/>
-      <c r="C25" s="118"/>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B25" s="123"/>
+      <c r="C25" s="114"/>
       <c r="D25" s="34" t="s">
         <v>39</v>
       </c>
@@ -2816,9 +2819,9 @@
       <c r="V25" s="18"/>
       <c r="W25" s="20"/>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B26" s="105"/>
-      <c r="C26" s="118"/>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B26" s="123"/>
+      <c r="C26" s="114"/>
       <c r="D26" s="34" t="s">
         <v>40</v>
       </c>
@@ -2855,9 +2858,9 @@
       <c r="V26" s="18"/>
       <c r="W26" s="20"/>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B27" s="105"/>
-      <c r="C27" s="118"/>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B27" s="123"/>
+      <c r="C27" s="114"/>
       <c r="D27" s="34" t="s">
         <v>41</v>
       </c>
@@ -2894,9 +2897,9 @@
       <c r="V27" s="18"/>
       <c r="W27" s="20"/>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B28" s="105"/>
-      <c r="C28" s="118"/>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B28" s="123"/>
+      <c r="C28" s="114"/>
       <c r="D28" s="34" t="s">
         <v>42</v>
       </c>
@@ -2933,9 +2936,9 @@
       <c r="V28" s="18"/>
       <c r="W28" s="20"/>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B29" s="105"/>
-      <c r="C29" s="118"/>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B29" s="123"/>
+      <c r="C29" s="114"/>
       <c r="D29" s="34" t="s">
         <v>43</v>
       </c>
@@ -2972,9 +2975,9 @@
       <c r="V29" s="18"/>
       <c r="W29" s="20"/>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B30" s="105"/>
-      <c r="C30" s="118"/>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B30" s="123"/>
+      <c r="C30" s="114"/>
       <c r="D30" s="34" t="s">
         <v>44</v>
       </c>
@@ -3011,9 +3014,9 @@
       <c r="V30" s="18"/>
       <c r="W30" s="20"/>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B31" s="105"/>
-      <c r="C31" s="118"/>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B31" s="123"/>
+      <c r="C31" s="114"/>
       <c r="D31" s="34" t="s">
         <v>45</v>
       </c>
@@ -3050,9 +3053,9 @@
       <c r="V31" s="18"/>
       <c r="W31" s="20"/>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B32" s="105"/>
-      <c r="C32" s="118"/>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B32" s="123"/>
+      <c r="C32" s="114"/>
       <c r="D32" s="34" t="s">
         <v>46</v>
       </c>
@@ -3089,9 +3092,9 @@
       <c r="V32" s="18"/>
       <c r="W32" s="20"/>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B33" s="105"/>
-      <c r="C33" s="118"/>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B33" s="123"/>
+      <c r="C33" s="114"/>
       <c r="D33" s="34" t="s">
         <v>47</v>
       </c>
@@ -3128,9 +3131,9 @@
       <c r="V33" s="18"/>
       <c r="W33" s="20"/>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B34" s="105"/>
-      <c r="C34" s="118"/>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B34" s="123"/>
+      <c r="C34" s="114"/>
       <c r="D34" s="34" t="s">
         <v>48</v>
       </c>
@@ -3167,9 +3170,9 @@
       <c r="V34" s="18"/>
       <c r="W34" s="20"/>
     </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35" s="105"/>
-      <c r="C35" s="118"/>
+    <row r="35" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B35" s="123"/>
+      <c r="C35" s="114"/>
       <c r="D35" s="34" t="s">
         <v>49</v>
       </c>
@@ -3206,9 +3209,9 @@
       <c r="V35" s="18"/>
       <c r="W35" s="20"/>
     </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B36" s="105"/>
-      <c r="C36" s="118"/>
+    <row r="36" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B36" s="123"/>
+      <c r="C36" s="114"/>
       <c r="D36" s="34" t="s">
         <v>50</v>
       </c>
@@ -3245,9 +3248,9 @@
       <c r="V36" s="18"/>
       <c r="W36" s="20"/>
     </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B37" s="105"/>
-      <c r="C37" s="118"/>
+    <row r="37" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B37" s="123"/>
+      <c r="C37" s="114"/>
       <c r="D37" s="34" t="s">
         <v>51</v>
       </c>
@@ -3284,9 +3287,9 @@
       <c r="V37" s="18"/>
       <c r="W37" s="20"/>
     </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B38" s="105"/>
-      <c r="C38" s="118"/>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B38" s="123"/>
+      <c r="C38" s="114"/>
       <c r="D38" s="34" t="s">
         <v>52</v>
       </c>
@@ -3323,9 +3326,9 @@
       <c r="V38" s="18"/>
       <c r="W38" s="20"/>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B39" s="105"/>
-      <c r="C39" s="118"/>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B39" s="123"/>
+      <c r="C39" s="114"/>
       <c r="D39" s="34" t="s">
         <v>53</v>
       </c>
@@ -3362,9 +3365,9 @@
       <c r="V39" s="18"/>
       <c r="W39" s="20"/>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B40" s="105"/>
-      <c r="C40" s="118"/>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B40" s="123"/>
+      <c r="C40" s="114"/>
       <c r="D40" s="34" t="s">
         <v>54</v>
       </c>
@@ -3401,9 +3404,9 @@
       <c r="V40" s="18"/>
       <c r="W40" s="20"/>
     </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B41" s="105"/>
-      <c r="C41" s="118"/>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B41" s="123"/>
+      <c r="C41" s="114"/>
       <c r="D41" s="34" t="s">
         <v>55</v>
       </c>
@@ -3440,9 +3443,9 @@
       <c r="V41" s="18"/>
       <c r="W41" s="20"/>
     </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B42" s="105"/>
-      <c r="C42" s="118"/>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B42" s="123"/>
+      <c r="C42" s="114"/>
       <c r="D42" s="34" t="s">
         <v>56</v>
       </c>
@@ -3479,9 +3482,9 @@
       <c r="V42" s="18"/>
       <c r="W42" s="20"/>
     </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B43" s="105"/>
-      <c r="C43" s="118"/>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B43" s="123"/>
+      <c r="C43" s="114"/>
       <c r="D43" s="34" t="s">
         <v>57</v>
       </c>
@@ -3518,9 +3521,9 @@
       <c r="V43" s="18"/>
       <c r="W43" s="20"/>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B44" s="105"/>
-      <c r="C44" s="118"/>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B44" s="123"/>
+      <c r="C44" s="114"/>
       <c r="D44" s="34" t="s">
         <v>58</v>
       </c>
@@ -3557,9 +3560,9 @@
       <c r="V44" s="18"/>
       <c r="W44" s="20"/>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B45" s="105"/>
-      <c r="C45" s="118"/>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B45" s="123"/>
+      <c r="C45" s="114"/>
       <c r="D45" s="34" t="s">
         <v>59</v>
       </c>
@@ -3596,9 +3599,9 @@
       <c r="V45" s="18"/>
       <c r="W45" s="20"/>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B46" s="105"/>
-      <c r="C46" s="118"/>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B46" s="123"/>
+      <c r="C46" s="114"/>
       <c r="D46" s="34" t="s">
         <v>60</v>
       </c>
@@ -3635,9 +3638,9 @@
       <c r="V46" s="18"/>
       <c r="W46" s="20"/>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B47" s="105"/>
-      <c r="C47" s="118"/>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B47" s="123"/>
+      <c r="C47" s="114"/>
       <c r="D47" s="34" t="s">
         <v>61</v>
       </c>
@@ -3674,9 +3677,9 @@
       <c r="V47" s="18"/>
       <c r="W47" s="20"/>
     </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B48" s="105"/>
-      <c r="C48" s="118"/>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B48" s="123"/>
+      <c r="C48" s="114"/>
       <c r="D48" s="34" t="s">
         <v>62</v>
       </c>
@@ -3713,9 +3716,9 @@
       <c r="V48" s="18"/>
       <c r="W48" s="20"/>
     </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B49" s="105"/>
-      <c r="C49" s="118"/>
+    <row r="49" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B49" s="123"/>
+      <c r="C49" s="114"/>
       <c r="D49" s="34" t="s">
         <v>63</v>
       </c>
@@ -3752,9 +3755,9 @@
       <c r="V49" s="18"/>
       <c r="W49" s="20"/>
     </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B50" s="105"/>
-      <c r="C50" s="118"/>
+    <row r="50" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B50" s="123"/>
+      <c r="C50" s="114"/>
       <c r="D50" s="34" t="s">
         <v>64</v>
       </c>
@@ -3791,9 +3794,9 @@
       <c r="V50" s="18"/>
       <c r="W50" s="20"/>
     </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B51" s="105"/>
-      <c r="C51" s="118"/>
+    <row r="51" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B51" s="123"/>
+      <c r="C51" s="114"/>
       <c r="D51" s="34" t="s">
         <v>65</v>
       </c>
@@ -3830,9 +3833,9 @@
       <c r="V51" s="18"/>
       <c r="W51" s="20"/>
     </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B52" s="105"/>
-      <c r="C52" s="118"/>
+    <row r="52" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B52" s="123"/>
+      <c r="C52" s="114"/>
       <c r="D52" s="34" t="s">
         <v>66</v>
       </c>
@@ -3869,9 +3872,9 @@
       <c r="V52" s="18"/>
       <c r="W52" s="20"/>
     </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B53" s="105"/>
-      <c r="C53" s="118"/>
+    <row r="53" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B53" s="123"/>
+      <c r="C53" s="114"/>
       <c r="D53" s="34" t="s">
         <v>67</v>
       </c>
@@ -3908,9 +3911,9 @@
       <c r="V53" s="18"/>
       <c r="W53" s="20"/>
     </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B54" s="105"/>
-      <c r="C54" s="118"/>
+    <row r="54" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B54" s="123"/>
+      <c r="C54" s="114"/>
       <c r="D54" s="34" t="s">
         <v>68</v>
       </c>
@@ -3947,9 +3950,9 @@
       <c r="V54" s="18"/>
       <c r="W54" s="20"/>
     </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B55" s="105"/>
-      <c r="C55" s="119"/>
+    <row r="55" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B55" s="123"/>
+      <c r="C55" s="115"/>
       <c r="D55" s="34" t="s">
         <v>69</v>
       </c>
@@ -3986,9 +3989,9 @@
       <c r="V55" s="18"/>
       <c r="W55" s="20"/>
     </row>
-    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B56" s="105"/>
-      <c r="C56" s="115" t="s">
+    <row r="56" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B56" s="123"/>
+      <c r="C56" s="111" t="s">
         <v>26</v>
       </c>
       <c r="D56" s="31" t="s">
@@ -4027,9 +4030,9 @@
       <c r="V56" s="18"/>
       <c r="W56" s="20"/>
     </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B57" s="105"/>
-      <c r="C57" s="116"/>
+    <row r="57" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B57" s="123"/>
+      <c r="C57" s="112"/>
       <c r="D57" s="31" t="s">
         <v>29</v>
       </c>
@@ -4066,9 +4069,9 @@
       <c r="V57" s="18"/>
       <c r="W57" s="20"/>
     </row>
-    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B58" s="105"/>
-      <c r="C58" s="116"/>
+    <row r="58" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B58" s="123"/>
+      <c r="C58" s="112"/>
       <c r="D58" s="31" t="s">
         <v>30</v>
       </c>
@@ -4105,9 +4108,9 @@
       <c r="V58" s="18"/>
       <c r="W58" s="20"/>
     </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B59" s="105"/>
-      <c r="C59" s="116"/>
+    <row r="59" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B59" s="123"/>
+      <c r="C59" s="112"/>
       <c r="D59" s="31" t="s">
         <v>31</v>
       </c>
@@ -4144,9 +4147,9 @@
       <c r="V59" s="18"/>
       <c r="W59" s="20"/>
     </row>
-    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B60" s="105"/>
-      <c r="C60" s="116"/>
+    <row r="60" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B60" s="123"/>
+      <c r="C60" s="112"/>
       <c r="D60" s="31" t="s">
         <v>34</v>
       </c>
@@ -4183,9 +4186,9 @@
       <c r="V60" s="18"/>
       <c r="W60" s="20"/>
     </row>
-    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B61" s="105"/>
-      <c r="C61" s="116"/>
+    <row r="61" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B61" s="123"/>
+      <c r="C61" s="112"/>
       <c r="D61" s="31" t="s">
         <v>32</v>
       </c>
@@ -4222,9 +4225,9 @@
       <c r="V61" s="18"/>
       <c r="W61" s="20"/>
     </row>
-    <row r="62" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="106"/>
-      <c r="C62" s="116"/>
+    <row r="62" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="124"/>
+      <c r="C62" s="112"/>
       <c r="D62" s="73" t="s">
         <v>33</v>
       </c>
@@ -4261,11 +4264,11 @@
       <c r="V62" s="27"/>
       <c r="W62" s="29"/>
     </row>
-    <row r="63" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B63" s="107" t="s">
+    <row r="63" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B63" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="120" t="s">
+      <c r="C63" s="116" t="s">
         <v>79</v>
       </c>
       <c r="D63" s="44" t="s">
@@ -4304,9 +4307,9 @@
       <c r="V63" s="56"/>
       <c r="W63" s="57"/>
     </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B64" s="108"/>
-      <c r="C64" s="118"/>
+    <row r="64" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B64" s="109"/>
+      <c r="C64" s="114"/>
       <c r="D64" s="4" t="s">
         <v>71</v>
       </c>
@@ -4343,9 +4346,9 @@
       <c r="V64" s="18"/>
       <c r="W64" s="20"/>
     </row>
-    <row r="65" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B65" s="108"/>
-      <c r="C65" s="118"/>
+    <row r="65" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B65" s="109"/>
+      <c r="C65" s="114"/>
       <c r="D65" s="4" t="s">
         <v>72</v>
       </c>
@@ -4382,9 +4385,9 @@
       <c r="V65" s="18"/>
       <c r="W65" s="20"/>
     </row>
-    <row r="66" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B66" s="108"/>
-      <c r="C66" s="119"/>
+    <row r="66" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B66" s="109"/>
+      <c r="C66" s="115"/>
       <c r="D66" s="31" t="s">
         <v>76</v>
       </c>
@@ -4421,8 +4424,8 @@
       <c r="V66" s="18"/>
       <c r="W66" s="20"/>
     </row>
-    <row r="67" spans="2:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B67" s="108"/>
+    <row r="67" spans="2:23" ht="18" x14ac:dyDescent="0.3">
+      <c r="B67" s="109"/>
       <c r="C67" s="35" t="s">
         <v>73</v>
       </c>
@@ -4460,8 +4463,8 @@
       <c r="V67" s="18"/>
       <c r="W67" s="20"/>
     </row>
-    <row r="68" spans="2:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="108"/>
+    <row r="68" spans="2:23" ht="18" x14ac:dyDescent="0.3">
+      <c r="B68" s="109"/>
       <c r="C68" s="60" t="s">
         <v>81</v>
       </c>
@@ -4499,9 +4502,9 @@
       <c r="V68" s="18"/>
       <c r="W68" s="20"/>
     </row>
-    <row r="69" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="108"/>
-      <c r="C69" s="117" t="s">
+    <row r="69" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="109"/>
+      <c r="C69" s="113" t="s">
         <v>80</v>
       </c>
       <c r="D69" s="4" t="s">
@@ -4540,9 +4543,9 @@
       <c r="V69" s="18"/>
       <c r="W69" s="20"/>
     </row>
-    <row r="70" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="108"/>
-      <c r="C70" s="118"/>
+    <row r="70" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="109"/>
+      <c r="C70" s="114"/>
       <c r="D70" s="4" t="s">
         <v>75</v>
       </c>
@@ -4579,9 +4582,9 @@
       <c r="V70" s="18"/>
       <c r="W70" s="20"/>
     </row>
-    <row r="71" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="108"/>
-      <c r="C71" s="118"/>
+    <row r="71" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="109"/>
+      <c r="C71" s="114"/>
       <c r="D71" s="4" t="s">
         <v>77</v>
       </c>
@@ -4618,9 +4621,9 @@
       <c r="V71" s="18"/>
       <c r="W71" s="20"/>
     </row>
-    <row r="72" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="109"/>
-      <c r="C72" s="121"/>
+    <row r="72" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B72" s="110"/>
+      <c r="C72" s="117"/>
       <c r="D72" s="25" t="s">
         <v>78</v>
       </c>
@@ -4657,11 +4660,11 @@
       <c r="V72" s="23"/>
       <c r="W72" s="26"/>
     </row>
-    <row r="73" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="104" t="s">
+    <row r="73" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="122" t="s">
         <v>117</v>
       </c>
-      <c r="C73" s="122" t="s">
+      <c r="C73" s="103" t="s">
         <v>118</v>
       </c>
       <c r="D73" s="44" t="s">
@@ -4700,9 +4703,9 @@
       <c r="V73" s="56"/>
       <c r="W73" s="57"/>
     </row>
-    <row r="74" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="105"/>
-      <c r="C74" s="110"/>
+    <row r="74" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="123"/>
+      <c r="C74" s="104"/>
       <c r="D74" s="4" t="s">
         <v>134</v>
       </c>
@@ -4739,9 +4742,9 @@
       <c r="V74" s="18"/>
       <c r="W74" s="20"/>
     </row>
-    <row r="75" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="105"/>
-      <c r="C75" s="110"/>
+    <row r="75" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="123"/>
+      <c r="C75" s="104"/>
       <c r="D75" s="4" t="s">
         <v>135</v>
       </c>
@@ -4778,9 +4781,9 @@
       <c r="V75" s="18"/>
       <c r="W75" s="20"/>
     </row>
-    <row r="76" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="105"/>
-      <c r="C76" s="110"/>
+    <row r="76" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="123"/>
+      <c r="C76" s="104"/>
       <c r="D76" s="4" t="s">
         <v>136</v>
       </c>
@@ -4817,9 +4820,9 @@
       <c r="V76" s="18"/>
       <c r="W76" s="20"/>
     </row>
-    <row r="77" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="105"/>
-      <c r="C77" s="110" t="s">
+    <row r="77" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="123"/>
+      <c r="C77" s="104" t="s">
         <v>119</v>
       </c>
       <c r="D77" s="4" t="s">
@@ -4858,9 +4861,9 @@
       <c r="V77" s="18"/>
       <c r="W77" s="20"/>
     </row>
-    <row r="78" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="105"/>
-      <c r="C78" s="110"/>
+    <row r="78" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="123"/>
+      <c r="C78" s="104"/>
       <c r="D78" s="4" t="s">
         <v>134</v>
       </c>
@@ -4897,9 +4900,9 @@
       <c r="V78" s="18"/>
       <c r="W78" s="20"/>
     </row>
-    <row r="79" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="105"/>
-      <c r="C79" s="110"/>
+    <row r="79" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="123"/>
+      <c r="C79" s="104"/>
       <c r="D79" s="4" t="s">
         <v>135</v>
       </c>
@@ -4936,9 +4939,9 @@
       <c r="V79" s="18"/>
       <c r="W79" s="20"/>
     </row>
-    <row r="80" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="105"/>
-      <c r="C80" s="110"/>
+    <row r="80" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="123"/>
+      <c r="C80" s="104"/>
       <c r="D80" s="4" t="s">
         <v>136</v>
       </c>
@@ -4975,9 +4978,9 @@
       <c r="V80" s="18"/>
       <c r="W80" s="20"/>
     </row>
-    <row r="81" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="105"/>
-      <c r="C81" s="110" t="s">
+    <row r="81" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="123"/>
+      <c r="C81" s="104" t="s">
         <v>120</v>
       </c>
       <c r="D81" s="4" t="s">
@@ -5016,9 +5019,9 @@
       <c r="V81" s="18"/>
       <c r="W81" s="20"/>
     </row>
-    <row r="82" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="105"/>
-      <c r="C82" s="110"/>
+    <row r="82" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="123"/>
+      <c r="C82" s="104"/>
       <c r="D82" s="4" t="s">
         <v>134</v>
       </c>
@@ -5055,9 +5058,9 @@
       <c r="V82" s="18"/>
       <c r="W82" s="20"/>
     </row>
-    <row r="83" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="105"/>
-      <c r="C83" s="110"/>
+    <row r="83" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="123"/>
+      <c r="C83" s="104"/>
       <c r="D83" s="4" t="s">
         <v>135</v>
       </c>
@@ -5094,9 +5097,9 @@
       <c r="V83" s="18"/>
       <c r="W83" s="20"/>
     </row>
-    <row r="84" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="105"/>
-      <c r="C84" s="110"/>
+    <row r="84" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="123"/>
+      <c r="C84" s="104"/>
       <c r="D84" s="4" t="s">
         <v>136</v>
       </c>
@@ -5133,9 +5136,9 @@
       <c r="V84" s="18"/>
       <c r="W84" s="20"/>
     </row>
-    <row r="85" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="105"/>
-      <c r="C85" s="110" t="s">
+    <row r="85" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="123"/>
+      <c r="C85" s="104" t="s">
         <v>121</v>
       </c>
       <c r="D85" s="4" t="s">
@@ -5174,9 +5177,9 @@
       <c r="V85" s="18"/>
       <c r="W85" s="20"/>
     </row>
-    <row r="86" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="105"/>
-      <c r="C86" s="110"/>
+    <row r="86" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="123"/>
+      <c r="C86" s="104"/>
       <c r="D86" s="4" t="s">
         <v>134</v>
       </c>
@@ -5213,9 +5216,9 @@
       <c r="V86" s="18"/>
       <c r="W86" s="20"/>
     </row>
-    <row r="87" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="105"/>
-      <c r="C87" s="110"/>
+    <row r="87" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="123"/>
+      <c r="C87" s="104"/>
       <c r="D87" s="4" t="s">
         <v>135</v>
       </c>
@@ -5252,9 +5255,9 @@
       <c r="V87" s="18"/>
       <c r="W87" s="20"/>
     </row>
-    <row r="88" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="105"/>
-      <c r="C88" s="110"/>
+    <row r="88" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="123"/>
+      <c r="C88" s="104"/>
       <c r="D88" s="4" t="s">
         <v>136</v>
       </c>
@@ -5291,9 +5294,9 @@
       <c r="V88" s="18"/>
       <c r="W88" s="20"/>
     </row>
-    <row r="89" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="105"/>
-      <c r="C89" s="110" t="s">
+    <row r="89" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="123"/>
+      <c r="C89" s="104" t="s">
         <v>122</v>
       </c>
       <c r="D89" s="4" t="s">
@@ -5332,9 +5335,9 @@
       <c r="V89" s="18"/>
       <c r="W89" s="20"/>
     </row>
-    <row r="90" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="105"/>
-      <c r="C90" s="110"/>
+    <row r="90" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="123"/>
+      <c r="C90" s="104"/>
       <c r="D90" s="4" t="s">
         <v>134</v>
       </c>
@@ -5371,9 +5374,9 @@
       <c r="V90" s="18"/>
       <c r="W90" s="20"/>
     </row>
-    <row r="91" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="105"/>
-      <c r="C91" s="110"/>
+    <row r="91" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="123"/>
+      <c r="C91" s="104"/>
       <c r="D91" s="4" t="s">
         <v>135</v>
       </c>
@@ -5410,9 +5413,9 @@
       <c r="V91" s="18"/>
       <c r="W91" s="20"/>
     </row>
-    <row r="92" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="105"/>
-      <c r="C92" s="110"/>
+    <row r="92" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="123"/>
+      <c r="C92" s="104"/>
       <c r="D92" s="4" t="s">
         <v>136</v>
       </c>
@@ -5449,9 +5452,9 @@
       <c r="V92" s="18"/>
       <c r="W92" s="20"/>
     </row>
-    <row r="93" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="105"/>
-      <c r="C93" s="110" t="s">
+    <row r="93" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="123"/>
+      <c r="C93" s="104" t="s">
         <v>123</v>
       </c>
       <c r="D93" s="4" t="s">
@@ -5490,9 +5493,9 @@
       <c r="V93" s="18"/>
       <c r="W93" s="20"/>
     </row>
-    <row r="94" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="105"/>
-      <c r="C94" s="110"/>
+    <row r="94" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="123"/>
+      <c r="C94" s="104"/>
       <c r="D94" s="4" t="s">
         <v>134</v>
       </c>
@@ -5529,9 +5532,9 @@
       <c r="V94" s="18"/>
       <c r="W94" s="20"/>
     </row>
-    <row r="95" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="105"/>
-      <c r="C95" s="110"/>
+    <row r="95" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="123"/>
+      <c r="C95" s="104"/>
       <c r="D95" s="4" t="s">
         <v>135</v>
       </c>
@@ -5568,9 +5571,9 @@
       <c r="V95" s="18"/>
       <c r="W95" s="20"/>
     </row>
-    <row r="96" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="105"/>
-      <c r="C96" s="110"/>
+    <row r="96" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="123"/>
+      <c r="C96" s="104"/>
       <c r="D96" s="4" t="s">
         <v>136</v>
       </c>
@@ -5607,9 +5610,9 @@
       <c r="V96" s="18"/>
       <c r="W96" s="20"/>
     </row>
-    <row r="97" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="105"/>
-      <c r="C97" s="110" t="s">
+    <row r="97" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="123"/>
+      <c r="C97" s="104" t="s">
         <v>124</v>
       </c>
       <c r="D97" s="4" t="s">
@@ -5648,9 +5651,9 @@
       <c r="V97" s="18"/>
       <c r="W97" s="20"/>
     </row>
-    <row r="98" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="105"/>
-      <c r="C98" s="110"/>
+    <row r="98" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="123"/>
+      <c r="C98" s="104"/>
       <c r="D98" s="4" t="s">
         <v>134</v>
       </c>
@@ -5687,9 +5690,9 @@
       <c r="V98" s="18"/>
       <c r="W98" s="20"/>
     </row>
-    <row r="99" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="105"/>
-      <c r="C99" s="110"/>
+    <row r="99" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="123"/>
+      <c r="C99" s="104"/>
       <c r="D99" s="4" t="s">
         <v>135</v>
       </c>
@@ -5726,9 +5729,9 @@
       <c r="V99" s="18"/>
       <c r="W99" s="20"/>
     </row>
-    <row r="100" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="105"/>
-      <c r="C100" s="110"/>
+    <row r="100" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="123"/>
+      <c r="C100" s="104"/>
       <c r="D100" s="4" t="s">
         <v>136</v>
       </c>
@@ -5765,9 +5768,9 @@
       <c r="V100" s="18"/>
       <c r="W100" s="20"/>
     </row>
-    <row r="101" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="105"/>
-      <c r="C101" s="110" t="s">
+    <row r="101" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="123"/>
+      <c r="C101" s="104" t="s">
         <v>125</v>
       </c>
       <c r="D101" s="4" t="s">
@@ -5806,9 +5809,9 @@
       <c r="V101" s="18"/>
       <c r="W101" s="20"/>
     </row>
-    <row r="102" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="105"/>
-      <c r="C102" s="110"/>
+    <row r="102" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="123"/>
+      <c r="C102" s="104"/>
       <c r="D102" s="4" t="s">
         <v>134</v>
       </c>
@@ -5845,9 +5848,9 @@
       <c r="V102" s="18"/>
       <c r="W102" s="20"/>
     </row>
-    <row r="103" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="105"/>
-      <c r="C103" s="110"/>
+    <row r="103" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="123"/>
+      <c r="C103" s="104"/>
       <c r="D103" s="4" t="s">
         <v>135</v>
       </c>
@@ -5884,9 +5887,9 @@
       <c r="V103" s="18"/>
       <c r="W103" s="20"/>
     </row>
-    <row r="104" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="105"/>
-      <c r="C104" s="110"/>
+    <row r="104" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="123"/>
+      <c r="C104" s="104"/>
       <c r="D104" s="4" t="s">
         <v>136</v>
       </c>
@@ -5923,9 +5926,9 @@
       <c r="V104" s="18"/>
       <c r="W104" s="20"/>
     </row>
-    <row r="105" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="105"/>
-      <c r="C105" s="110" t="s">
+    <row r="105" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="123"/>
+      <c r="C105" s="104" t="s">
         <v>126</v>
       </c>
       <c r="D105" s="4" t="s">
@@ -5964,9 +5967,9 @@
       <c r="V105" s="18"/>
       <c r="W105" s="20"/>
     </row>
-    <row r="106" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="105"/>
-      <c r="C106" s="110"/>
+    <row r="106" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="123"/>
+      <c r="C106" s="104"/>
       <c r="D106" s="4" t="s">
         <v>134</v>
       </c>
@@ -6003,9 +6006,9 @@
       <c r="V106" s="18"/>
       <c r="W106" s="20"/>
     </row>
-    <row r="107" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="105"/>
-      <c r="C107" s="110"/>
+    <row r="107" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="123"/>
+      <c r="C107" s="104"/>
       <c r="D107" s="4" t="s">
         <v>135</v>
       </c>
@@ -6042,9 +6045,9 @@
       <c r="V107" s="18"/>
       <c r="W107" s="20"/>
     </row>
-    <row r="108" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="105"/>
-      <c r="C108" s="110"/>
+    <row r="108" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="123"/>
+      <c r="C108" s="104"/>
       <c r="D108" s="4" t="s">
         <v>136</v>
       </c>
@@ -6081,9 +6084,9 @@
       <c r="V108" s="18"/>
       <c r="W108" s="20"/>
     </row>
-    <row r="109" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="105"/>
-      <c r="C109" s="110" t="s">
+    <row r="109" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="123"/>
+      <c r="C109" s="104" t="s">
         <v>127</v>
       </c>
       <c r="D109" s="4" t="s">
@@ -6122,9 +6125,9 @@
       <c r="V109" s="18"/>
       <c r="W109" s="20"/>
     </row>
-    <row r="110" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="105"/>
-      <c r="C110" s="110"/>
+    <row r="110" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B110" s="123"/>
+      <c r="C110" s="104"/>
       <c r="D110" s="4" t="s">
         <v>134</v>
       </c>
@@ -6161,9 +6164,9 @@
       <c r="V110" s="18"/>
       <c r="W110" s="20"/>
     </row>
-    <row r="111" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="105"/>
-      <c r="C111" s="110"/>
+    <row r="111" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B111" s="123"/>
+      <c r="C111" s="104"/>
       <c r="D111" s="4" t="s">
         <v>135</v>
       </c>
@@ -6200,9 +6203,9 @@
       <c r="V111" s="18"/>
       <c r="W111" s="20"/>
     </row>
-    <row r="112" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="105"/>
-      <c r="C112" s="110"/>
+    <row r="112" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B112" s="123"/>
+      <c r="C112" s="104"/>
       <c r="D112" s="4" t="s">
         <v>136</v>
       </c>
@@ -6239,9 +6242,9 @@
       <c r="V112" s="18"/>
       <c r="W112" s="20"/>
     </row>
-    <row r="113" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="105"/>
-      <c r="C113" s="110" t="s">
+    <row r="113" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B113" s="123"/>
+      <c r="C113" s="104" t="s">
         <v>128</v>
       </c>
       <c r="D113" s="4" t="s">
@@ -6280,9 +6283,9 @@
       <c r="V113" s="18"/>
       <c r="W113" s="20"/>
     </row>
-    <row r="114" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="105"/>
-      <c r="C114" s="110"/>
+    <row r="114" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B114" s="123"/>
+      <c r="C114" s="104"/>
       <c r="D114" s="4" t="s">
         <v>134</v>
       </c>
@@ -6319,9 +6322,9 @@
       <c r="V114" s="18"/>
       <c r="W114" s="20"/>
     </row>
-    <row r="115" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="105"/>
-      <c r="C115" s="110"/>
+    <row r="115" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B115" s="123"/>
+      <c r="C115" s="104"/>
       <c r="D115" s="4" t="s">
         <v>135</v>
       </c>
@@ -6358,9 +6361,9 @@
       <c r="V115" s="18"/>
       <c r="W115" s="20"/>
     </row>
-    <row r="116" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="105"/>
-      <c r="C116" s="110"/>
+    <row r="116" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B116" s="123"/>
+      <c r="C116" s="104"/>
       <c r="D116" s="4" t="s">
         <v>136</v>
       </c>
@@ -6397,9 +6400,9 @@
       <c r="V116" s="18"/>
       <c r="W116" s="20"/>
     </row>
-    <row r="117" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="105"/>
-      <c r="C117" s="110" t="s">
+    <row r="117" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B117" s="123"/>
+      <c r="C117" s="104" t="s">
         <v>129</v>
       </c>
       <c r="D117" s="4" t="s">
@@ -6438,9 +6441,9 @@
       <c r="V117" s="18"/>
       <c r="W117" s="20"/>
     </row>
-    <row r="118" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="105"/>
-      <c r="C118" s="110"/>
+    <row r="118" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B118" s="123"/>
+      <c r="C118" s="104"/>
       <c r="D118" s="4" t="s">
         <v>134</v>
       </c>
@@ -6477,9 +6480,9 @@
       <c r="V118" s="18"/>
       <c r="W118" s="20"/>
     </row>
-    <row r="119" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="105"/>
-      <c r="C119" s="110"/>
+    <row r="119" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B119" s="123"/>
+      <c r="C119" s="104"/>
       <c r="D119" s="4" t="s">
         <v>135</v>
       </c>
@@ -6516,9 +6519,9 @@
       <c r="V119" s="18"/>
       <c r="W119" s="20"/>
     </row>
-    <row r="120" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="105"/>
-      <c r="C120" s="110"/>
+    <row r="120" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B120" s="123"/>
+      <c r="C120" s="104"/>
       <c r="D120" s="4" t="s">
         <v>136</v>
       </c>
@@ -6555,9 +6558,9 @@
       <c r="V120" s="18"/>
       <c r="W120" s="20"/>
     </row>
-    <row r="121" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="105"/>
-      <c r="C121" s="110" t="s">
+    <row r="121" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B121" s="123"/>
+      <c r="C121" s="104" t="s">
         <v>130</v>
       </c>
       <c r="D121" s="4" t="s">
@@ -6596,9 +6599,9 @@
       <c r="V121" s="18"/>
       <c r="W121" s="20"/>
     </row>
-    <row r="122" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="105"/>
-      <c r="C122" s="110"/>
+    <row r="122" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B122" s="123"/>
+      <c r="C122" s="104"/>
       <c r="D122" s="4" t="s">
         <v>134</v>
       </c>
@@ -6635,9 +6638,9 @@
       <c r="V122" s="18"/>
       <c r="W122" s="20"/>
     </row>
-    <row r="123" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="105"/>
-      <c r="C123" s="110"/>
+    <row r="123" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B123" s="123"/>
+      <c r="C123" s="104"/>
       <c r="D123" s="4" t="s">
         <v>135</v>
       </c>
@@ -6674,9 +6677,9 @@
       <c r="V123" s="18"/>
       <c r="W123" s="20"/>
     </row>
-    <row r="124" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="105"/>
-      <c r="C124" s="110"/>
+    <row r="124" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B124" s="123"/>
+      <c r="C124" s="104"/>
       <c r="D124" s="4" t="s">
         <v>136</v>
       </c>
@@ -6713,9 +6716,9 @@
       <c r="V124" s="18"/>
       <c r="W124" s="20"/>
     </row>
-    <row r="125" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="105"/>
-      <c r="C125" s="110" t="s">
+    <row r="125" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B125" s="123"/>
+      <c r="C125" s="104" t="s">
         <v>131</v>
       </c>
       <c r="D125" s="4" t="s">
@@ -6754,9 +6757,9 @@
       <c r="V125" s="18"/>
       <c r="W125" s="20"/>
     </row>
-    <row r="126" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="105"/>
-      <c r="C126" s="110"/>
+    <row r="126" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B126" s="123"/>
+      <c r="C126" s="104"/>
       <c r="D126" s="4" t="s">
         <v>134</v>
       </c>
@@ -6793,9 +6796,9 @@
       <c r="V126" s="18"/>
       <c r="W126" s="20"/>
     </row>
-    <row r="127" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="105"/>
-      <c r="C127" s="110"/>
+    <row r="127" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B127" s="123"/>
+      <c r="C127" s="104"/>
       <c r="D127" s="4" t="s">
         <v>135</v>
       </c>
@@ -6832,9 +6835,9 @@
       <c r="V127" s="18"/>
       <c r="W127" s="20"/>
     </row>
-    <row r="128" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="105"/>
-      <c r="C128" s="110"/>
+    <row r="128" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B128" s="123"/>
+      <c r="C128" s="104"/>
       <c r="D128" s="4" t="s">
         <v>136</v>
       </c>
@@ -6871,9 +6874,9 @@
       <c r="V128" s="18"/>
       <c r="W128" s="20"/>
     </row>
-    <row r="129" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="105"/>
-      <c r="C129" s="110" t="s">
+    <row r="129" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B129" s="123"/>
+      <c r="C129" s="104" t="s">
         <v>132</v>
       </c>
       <c r="D129" s="4" t="s">
@@ -6912,9 +6915,9 @@
       <c r="V129" s="18"/>
       <c r="W129" s="20"/>
     </row>
-    <row r="130" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="105"/>
-      <c r="C130" s="110"/>
+    <row r="130" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B130" s="123"/>
+      <c r="C130" s="104"/>
       <c r="D130" s="4" t="s">
         <v>134</v>
       </c>
@@ -6951,9 +6954,9 @@
       <c r="V130" s="18"/>
       <c r="W130" s="20"/>
     </row>
-    <row r="131" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="105"/>
-      <c r="C131" s="110"/>
+    <row r="131" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B131" s="123"/>
+      <c r="C131" s="104"/>
       <c r="D131" s="4" t="s">
         <v>135</v>
       </c>
@@ -6990,9 +6993,9 @@
       <c r="V131" s="18"/>
       <c r="W131" s="20"/>
     </row>
-    <row r="132" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="111"/>
-      <c r="C132" s="114"/>
+    <row r="132" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B132" s="125"/>
+      <c r="C132" s="126"/>
       <c r="D132" s="25" t="s">
         <v>136</v>
       </c>
@@ -7029,8 +7032,8 @@
       <c r="V132" s="23"/>
       <c r="W132" s="26"/>
     </row>
-    <row r="133" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="107" t="s">
+    <row r="133" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B133" s="108" t="s">
         <v>83</v>
       </c>
       <c r="C133" s="91" t="s">
@@ -7070,8 +7073,8 @@
       <c r="V133" s="56"/>
       <c r="W133" s="57"/>
     </row>
-    <row r="134" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="108"/>
+    <row r="134" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B134" s="109"/>
       <c r="C134" s="38" t="s">
         <v>89</v>
       </c>
@@ -7109,8 +7112,8 @@
       <c r="V134" s="18"/>
       <c r="W134" s="20"/>
     </row>
-    <row r="135" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="108"/>
+    <row r="135" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B135" s="109"/>
       <c r="C135" s="38" t="s">
         <v>90</v>
       </c>
@@ -7148,8 +7151,8 @@
       <c r="V135" s="18"/>
       <c r="W135" s="20"/>
     </row>
-    <row r="136" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="108"/>
+    <row r="136" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B136" s="109"/>
       <c r="C136" s="38" t="s">
         <v>91</v>
       </c>
@@ -7187,8 +7190,8 @@
       <c r="V136" s="18"/>
       <c r="W136" s="20"/>
     </row>
-    <row r="137" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="108"/>
+    <row r="137" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B137" s="109"/>
       <c r="C137" s="38" t="s">
         <v>143</v>
       </c>
@@ -7226,8 +7229,8 @@
       <c r="V137" s="18"/>
       <c r="W137" s="20"/>
     </row>
-    <row r="138" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="108"/>
+    <row r="138" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B138" s="109"/>
       <c r="C138" s="38" t="s">
         <v>140</v>
       </c>
@@ -7265,8 +7268,8 @@
       <c r="V138" s="18"/>
       <c r="W138" s="20"/>
     </row>
-    <row r="139" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="108"/>
+    <row r="139" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B139" s="109"/>
       <c r="C139" s="38" t="s">
         <v>142</v>
       </c>
@@ -7304,8 +7307,8 @@
       <c r="V139" s="18"/>
       <c r="W139" s="20"/>
     </row>
-    <row r="140" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="108"/>
+    <row r="140" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B140" s="109"/>
       <c r="C140" s="38" t="s">
         <v>141</v>
       </c>
@@ -7343,8 +7346,8 @@
       <c r="V140" s="18"/>
       <c r="W140" s="20"/>
     </row>
-    <row r="141" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="108"/>
+    <row r="141" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B141" s="109"/>
       <c r="C141" s="38" t="s">
         <v>92</v>
       </c>
@@ -7382,8 +7385,8 @@
       <c r="V141" s="18"/>
       <c r="W141" s="20"/>
     </row>
-    <row r="142" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="108"/>
+    <row r="142" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B142" s="109"/>
       <c r="C142" s="38" t="s">
         <v>93</v>
       </c>
@@ -7421,8 +7424,8 @@
       <c r="V142" s="18"/>
       <c r="W142" s="20"/>
     </row>
-    <row r="143" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="108"/>
+    <row r="143" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B143" s="109"/>
       <c r="C143" s="38" t="s">
         <v>94</v>
       </c>
@@ -7460,8 +7463,8 @@
       <c r="V143" s="18"/>
       <c r="W143" s="20"/>
     </row>
-    <row r="144" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="108"/>
+    <row r="144" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B144" s="109"/>
       <c r="C144" s="38" t="s">
         <v>98</v>
       </c>
@@ -7499,8 +7502,8 @@
       <c r="V144" s="18"/>
       <c r="W144" s="20"/>
     </row>
-    <row r="145" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="109"/>
+    <row r="145" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B145" s="110"/>
       <c r="C145" s="61" t="s">
         <v>99</v>
       </c>
@@ -7538,8 +7541,8 @@
       <c r="V145" s="23"/>
       <c r="W145" s="26"/>
     </row>
-    <row r="146" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="104" t="s">
+    <row r="146" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B146" s="122" t="s">
         <v>144</v>
       </c>
       <c r="C146" s="71" t="s">
@@ -7579,8 +7582,8 @@
       <c r="V146" s="56"/>
       <c r="W146" s="57"/>
     </row>
-    <row r="147" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="105"/>
+    <row r="147" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B147" s="123"/>
       <c r="C147" s="70" t="s">
         <v>145</v>
       </c>
@@ -7618,8 +7621,8 @@
       <c r="V147" s="18"/>
       <c r="W147" s="20"/>
     </row>
-    <row r="148" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="111"/>
+    <row r="148" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B148" s="125"/>
       <c r="C148" s="72" t="s">
         <v>146</v>
       </c>
@@ -7657,8 +7660,8 @@
       <c r="V148" s="23"/>
       <c r="W148" s="26"/>
     </row>
-    <row r="149" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="108" t="s">
+    <row r="149" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B149" s="109" t="s">
         <v>18</v>
       </c>
       <c r="C149" s="38" t="s">
@@ -7698,8 +7701,8 @@
       <c r="V149" s="67"/>
       <c r="W149" s="69"/>
     </row>
-    <row r="150" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B150" s="108"/>
+    <row r="150" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B150" s="109"/>
       <c r="C150" s="38" t="s">
         <v>138</v>
       </c>
@@ -7737,8 +7740,8 @@
       <c r="V150" s="67"/>
       <c r="W150" s="69"/>
     </row>
-    <row r="151" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="108"/>
+    <row r="151" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B151" s="109"/>
       <c r="C151" s="38" t="s">
         <v>139</v>
       </c>
@@ -7776,8 +7779,8 @@
       <c r="V151" s="67"/>
       <c r="W151" s="69"/>
     </row>
-    <row r="152" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B152" s="108"/>
+    <row r="152" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B152" s="109"/>
       <c r="C152" s="38" t="s">
         <v>147</v>
       </c>
@@ -7815,8 +7818,8 @@
       <c r="V152" s="18"/>
       <c r="W152" s="20"/>
     </row>
-    <row r="153" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="108"/>
+    <row r="153" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B153" s="109"/>
       <c r="C153" s="35" t="s">
         <v>84</v>
       </c>
@@ -7854,8 +7857,8 @@
       <c r="V153" s="18"/>
       <c r="W153" s="20"/>
     </row>
-    <row r="154" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="108"/>
+    <row r="154" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B154" s="109"/>
       <c r="C154" s="35" t="s">
         <v>85</v>
       </c>
@@ -7893,8 +7896,8 @@
       <c r="V154" s="18"/>
       <c r="W154" s="20"/>
     </row>
-    <row r="155" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="108"/>
+    <row r="155" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B155" s="109"/>
       <c r="C155" s="39" t="s">
         <v>87</v>
       </c>
@@ -7932,8 +7935,8 @@
       <c r="V155" s="27"/>
       <c r="W155" s="29"/>
     </row>
-    <row r="156" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B156" s="108"/>
+    <row r="156" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B156" s="109"/>
       <c r="C156" s="35" t="s">
         <v>86</v>
       </c>
@@ -7971,8 +7974,8 @@
       <c r="V156" s="27"/>
       <c r="W156" s="29"/>
     </row>
-    <row r="157" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="108"/>
+    <row r="157" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B157" s="109"/>
       <c r="C157" s="41" t="s">
         <v>104</v>
       </c>
@@ -8010,8 +8013,8 @@
       <c r="V157" s="27"/>
       <c r="W157" s="29"/>
     </row>
-    <row r="158" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B158" s="108"/>
+    <row r="158" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B158" s="109"/>
       <c r="C158" s="41" t="s">
         <v>137</v>
       </c>
@@ -8030,12 +8033,14 @@
       </c>
       <c r="I158" s="6">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
       <c r="J158" s="84">
         <v>0</v>
       </c>
-      <c r="K158" s="8"/>
+      <c r="K158" s="127">
+        <v>1.85</v>
+      </c>
       <c r="L158" s="8"/>
       <c r="M158" s="8"/>
       <c r="N158" s="8"/>
@@ -8049,8 +8054,8 @@
       <c r="V158" s="27"/>
       <c r="W158" s="29"/>
     </row>
-    <row r="159" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="108"/>
+    <row r="159" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B159" s="109"/>
       <c r="C159" s="41" t="s">
         <v>105</v>
       </c>
@@ -8088,8 +8093,8 @@
       <c r="V159" s="27"/>
       <c r="W159" s="29"/>
     </row>
-    <row r="160" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="109"/>
+    <row r="160" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B160" s="110"/>
       <c r="C160" s="61" t="s">
         <v>100</v>
       </c>
@@ -8127,22 +8132,22 @@
       <c r="V160" s="23"/>
       <c r="W160" s="26"/>
     </row>
-    <row r="161" spans="2:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="99" t="s">
+    <row r="161" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B161" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="C161" s="102"/>
-      <c r="D161" s="100"/>
-      <c r="E161" s="100"/>
-      <c r="F161" s="100"/>
-      <c r="G161" s="103"/>
+      <c r="C161" s="120"/>
+      <c r="D161" s="119"/>
+      <c r="E161" s="119"/>
+      <c r="F161" s="119"/>
+      <c r="G161" s="121"/>
       <c r="H161" s="40">
         <f>SUM(H4:H160)</f>
         <v>89.199999999999989</v>
       </c>
       <c r="I161" s="24">
         <f>SUM(I4:I160)</f>
-        <v>1.5333000000000001</v>
+        <v>3.3833000000000002</v>
       </c>
       <c r="J161" s="24">
         <f>SUM(J4:J160)</f>
@@ -8150,7 +8155,7 @@
       </c>
       <c r="K161" s="24">
         <f t="shared" ref="K161:W161" si="5">SUM(K4:K160)</f>
-        <v>1.5333000000000001</v>
+        <v>3.3833000000000002</v>
       </c>
       <c r="L161" s="24">
         <f t="shared" si="5"/>
@@ -8201,7 +8206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
@@ -8210,24 +8215,24 @@
       <c r="G162" s="2"/>
       <c r="H162" s="2"/>
       <c r="I162" s="2"/>
-      <c r="J162" s="101" t="s">
+      <c r="J162" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="K162" s="112"/>
-      <c r="L162" s="112"/>
-      <c r="M162" s="112"/>
-      <c r="N162" s="112"/>
-      <c r="O162" s="112"/>
-      <c r="P162" s="112"/>
-      <c r="Q162" s="112"/>
-      <c r="R162" s="112"/>
-      <c r="S162" s="112"/>
-      <c r="T162" s="112"/>
-      <c r="U162" s="112"/>
-      <c r="V162" s="112"/>
-      <c r="W162" s="113"/>
-    </row>
-    <row r="163" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K162" s="106"/>
+      <c r="L162" s="106"/>
+      <c r="M162" s="106"/>
+      <c r="N162" s="106"/>
+      <c r="O162" s="106"/>
+      <c r="P162" s="106"/>
+      <c r="Q162" s="106"/>
+      <c r="R162" s="106"/>
+      <c r="S162" s="106"/>
+      <c r="T162" s="106"/>
+      <c r="U162" s="106"/>
+      <c r="V162" s="106"/>
+      <c r="W162" s="107"/>
+    </row>
+    <row r="163" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
@@ -8242,39 +8247,39 @@
       <c r="M163" s="3"/>
       <c r="N163" s="3"/>
     </row>
-    <row r="164" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
-      <c r="H164" s="99" t="s">
+      <c r="H164" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="I164" s="100"/>
+      <c r="I164" s="119"/>
       <c r="J164" s="10">
         <f>H161-J161</f>
         <v>89.199999999999989</v>
       </c>
       <c r="K164" s="10">
         <f>J164-K161</f>
-        <v>87.666699999999992</v>
+        <v>85.816699999999983</v>
       </c>
       <c r="L164" s="10">
         <f>K164-L161</f>
-        <v>87.666699999999992</v>
+        <v>85.816699999999983</v>
       </c>
       <c r="M164" s="10">
         <f>L164-M161</f>
-        <v>87.666699999999992</v>
+        <v>85.816699999999983</v>
       </c>
       <c r="N164" s="11">
         <f>M164-N161</f>
-        <v>87.666699999999992</v>
-      </c>
-    </row>
-    <row r="165" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85.816699999999983</v>
+      </c>
+    </row>
+    <row r="165" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
       <c r="D165" s="3"/>
@@ -8289,26 +8294,26 @@
       <c r="M165" s="3"/>
       <c r="N165" s="3"/>
     </row>
-    <row r="166" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
       <c r="D166" s="3"/>
       <c r="E166" s="3"/>
       <c r="F166" s="3"/>
-      <c r="H166" s="101" t="s">
+      <c r="H166" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="I166" s="102"/>
-      <c r="J166" s="100">
+      <c r="I166" s="120"/>
+      <c r="J166" s="119">
         <f>H161-I161</f>
-        <v>87.666699999999992</v>
-      </c>
-      <c r="K166" s="100"/>
-      <c r="L166" s="100"/>
-      <c r="M166" s="100"/>
-      <c r="N166" s="103"/>
-    </row>
-    <row r="167" spans="2:23" x14ac:dyDescent="0.25">
+        <v>85.816699999999983</v>
+      </c>
+      <c r="K166" s="119"/>
+      <c r="L166" s="119"/>
+      <c r="M166" s="119"/>
+      <c r="N166" s="121"/>
+    </row>
+    <row r="167" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
       <c r="D167" s="3"/>
@@ -8323,7 +8328,7 @@
       <c r="M167" s="3"/>
       <c r="N167" s="3"/>
     </row>
-    <row r="168" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
       <c r="D168" s="3"/>
@@ -8338,7 +8343,7 @@
       <c r="M168" s="3"/>
       <c r="N168" s="3"/>
     </row>
-    <row r="169" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
       <c r="D169" s="3"/>
@@ -8353,80 +8358,63 @@
       <c r="M169" s="3"/>
       <c r="N169" s="3"/>
     </row>
-    <row r="170" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="171" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="172" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="171" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="172" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B172" s="13"/>
       <c r="C172" s="13"/>
     </row>
-    <row r="173" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B173" s="13"/>
       <c r="C173" s="13"/>
     </row>
-    <row r="174" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B174" s="13"/>
       <c r="C174" s="13"/>
     </row>
-    <row r="175" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B175" s="13"/>
       <c r="C175" s="13"/>
     </row>
-    <row r="176" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:23" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B176" s="13"/>
       <c r="C176" s="13"/>
     </row>
-    <row r="177" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B177" s="13"/>
       <c r="C177" s="13"/>
     </row>
-    <row r="178" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B178" s="13"/>
       <c r="C178" s="13"/>
     </row>
-    <row r="179" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B179" s="13"/>
       <c r="C179" s="13"/>
     </row>
-    <row r="180" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B180" s="13"/>
       <c r="C180" s="13"/>
     </row>
-    <row r="181" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B181" s="13"/>
       <c r="C181" s="13"/>
     </row>
-    <row r="182" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B182" s="13"/>
       <c r="C182" s="13"/>
     </row>
-    <row r="183" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B183" s="13"/>
       <c r="C183" s="13"/>
     </row>
-    <row r="184" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B184" s="13"/>
       <c r="C184" s="13"/>
     </row>
-    <row r="185" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="185" spans="2:3" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C73:C76"/>
-    <mergeCell ref="C77:C80"/>
-    <mergeCell ref="C121:C124"/>
-    <mergeCell ref="C113:C116"/>
-    <mergeCell ref="C105:C108"/>
-    <mergeCell ref="C101:C104"/>
-    <mergeCell ref="C93:C96"/>
-    <mergeCell ref="C109:C112"/>
-    <mergeCell ref="C117:C120"/>
-    <mergeCell ref="J2:W2"/>
-    <mergeCell ref="B63:B72"/>
-    <mergeCell ref="C56:C62"/>
-    <mergeCell ref="C16:C55"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="C69:C72"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B14"/>
     <mergeCell ref="H164:I164"/>
     <mergeCell ref="H166:I166"/>
     <mergeCell ref="J166:N166"/>
@@ -8443,6 +8431,23 @@
     <mergeCell ref="C89:C92"/>
     <mergeCell ref="C85:C88"/>
     <mergeCell ref="C81:C84"/>
+    <mergeCell ref="J2:W2"/>
+    <mergeCell ref="B63:B72"/>
+    <mergeCell ref="C56:C62"/>
+    <mergeCell ref="C16:C55"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C69:C72"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C73:C76"/>
+    <mergeCell ref="C77:C80"/>
+    <mergeCell ref="C121:C124"/>
+    <mergeCell ref="C113:C116"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="C101:C104"/>
+    <mergeCell ref="C93:C96"/>
+    <mergeCell ref="C109:C112"/>
+    <mergeCell ref="C117:C120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8456,7 +8461,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8468,7 +8473,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
El Oktorok ya genera proyectiles mediante un metodo de AIMethods, el cual puede ser detenido por Link si esta mirando en la dirección adecuada y si está quieto.
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
+++ b/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
@@ -1239,21 +1239,81 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1263,67 +1323,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1383,19 +1383,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>89.69999999999996</c:v>
+                  <c:v>96.499999999999829</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85.646699999999953</c:v>
+                  <c:v>92.446699999999822</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>84.143699999999953</c:v>
+                  <c:v>90.443699999999822</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84.143699999999953</c:v>
+                  <c:v>87.493699999999819</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84.143699999999953</c:v>
+                  <c:v>87.493699999999819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1416,11 +1416,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1221442368"/>
-        <c:axId val="-1221441824"/>
+        <c:axId val="-315111632"/>
+        <c:axId val="-315110000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1221442368"/>
+        <c:axId val="-315111632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1429,7 +1429,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1221441824"/>
+        <c:crossAx val="-315110000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1437,7 +1437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1221441824"/>
+        <c:axId val="-315110000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,7 +1448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1221442368"/>
+        <c:crossAx val="-315111632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1794,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J168" sqref="J168"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1822,22 +1822,22 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="91" t="s">
+      <c r="J2" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
-      <c r="Q2" s="92"/>
-      <c r="R2" s="92"/>
-      <c r="S2" s="92"/>
-      <c r="T2" s="92"/>
-      <c r="U2" s="92"/>
-      <c r="V2" s="92"/>
-      <c r="W2" s="93"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="103"/>
+      <c r="P2" s="103"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="103"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="103"/>
+      <c r="V2" s="103"/>
+      <c r="W2" s="104"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="56" t="s">
@@ -1908,7 +1908,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="114" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="37" t="s">
@@ -1937,7 +1937,7 @@
       <c r="K4" s="69">
         <v>0</v>
       </c>
-      <c r="L4" s="39"/>
+      <c r="L4" s="69"/>
       <c r="M4" s="39"/>
       <c r="N4" s="39"/>
       <c r="O4" s="41"/>
@@ -1951,7 +1951,7 @@
       <c r="W4" s="44"/>
     </row>
     <row r="5" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="95"/>
+      <c r="B5" s="115"/>
       <c r="C5" s="35" t="s">
         <v>101</v>
       </c>
@@ -1978,7 +1978,7 @@
       <c r="K5" s="70">
         <v>0</v>
       </c>
-      <c r="L5" s="4"/>
+      <c r="L5" s="70"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="17"/>
@@ -1992,7 +1992,7 @@
       <c r="W5" s="19"/>
     </row>
     <row r="6" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="95"/>
+      <c r="B6" s="115"/>
       <c r="C6" s="35" t="s">
         <v>102</v>
       </c>
@@ -2019,7 +2019,7 @@
       <c r="K6" s="70">
         <v>0</v>
       </c>
-      <c r="L6" s="4"/>
+      <c r="L6" s="70"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="17"/>
@@ -2033,7 +2033,7 @@
       <c r="W6" s="19"/>
     </row>
     <row r="7" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="95"/>
+      <c r="B7" s="115"/>
       <c r="C7" s="35" t="s">
         <v>103</v>
       </c>
@@ -2060,7 +2060,7 @@
       <c r="K7" s="70">
         <v>0</v>
       </c>
-      <c r="L7" s="4"/>
+      <c r="L7" s="70"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="17"/>
@@ -2074,7 +2074,7 @@
       <c r="W7" s="19"/>
     </row>
     <row r="8" spans="1:23" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="96"/>
+      <c r="B8" s="116"/>
       <c r="C8" s="45" t="s">
         <v>111</v>
       </c>
@@ -2101,7 +2101,7 @@
       <c r="K8" s="71">
         <v>0</v>
       </c>
-      <c r="L8" s="24"/>
+      <c r="L8" s="71"/>
       <c r="M8" s="24"/>
       <c r="N8" s="24"/>
       <c r="O8" s="22"/>
@@ -2115,7 +2115,7 @@
       <c r="W8" s="25"/>
     </row>
     <row r="9" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="114" t="s">
         <v>106</v>
       </c>
       <c r="C9" s="48" t="s">
@@ -2158,7 +2158,7 @@
       <c r="W9" s="86"/>
     </row>
     <row r="10" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="95"/>
+      <c r="B10" s="115"/>
       <c r="C10" s="34" t="s">
         <v>107</v>
       </c>
@@ -2185,7 +2185,7 @@
       <c r="K10" s="70">
         <v>0</v>
       </c>
-      <c r="L10" s="4"/>
+      <c r="L10" s="70"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="17"/>
@@ -2199,7 +2199,7 @@
       <c r="W10" s="19"/>
     </row>
     <row r="11" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="95"/>
+      <c r="B11" s="115"/>
       <c r="C11" s="83" t="s">
         <v>112</v>
       </c>
@@ -2226,7 +2226,7 @@
       <c r="K11" s="70">
         <v>0</v>
       </c>
-      <c r="L11" s="4"/>
+      <c r="L11" s="70"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="17"/>
@@ -2240,7 +2240,7 @@
       <c r="W11" s="19"/>
     </row>
     <row r="12" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="95"/>
+      <c r="B12" s="115"/>
       <c r="C12" s="83" t="s">
         <v>113</v>
       </c>
@@ -2305,7 +2305,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="96"/>
+      <c r="B13" s="116"/>
       <c r="C13" s="53" t="s">
         <v>97</v>
       </c>
@@ -2348,7 +2348,7 @@
       <c r="W13" s="25"/>
     </row>
     <row r="14" spans="1:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="89" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="54" t="s">
@@ -2379,7 +2379,7 @@
       <c r="K14" s="82">
         <v>0.88329999999999997</v>
       </c>
-      <c r="L14" s="50"/>
+      <c r="L14" s="69"/>
       <c r="M14" s="50"/>
       <c r="N14" s="39"/>
       <c r="O14" s="51"/>
@@ -2393,8 +2393,8 @@
       <c r="W14" s="52"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B15" s="107"/>
-      <c r="C15" s="99" t="s">
+      <c r="B15" s="90"/>
+      <c r="C15" s="108" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -2410,11 +2410,11 @@
         <v>2</v>
       </c>
       <c r="H15" s="4">
-        <v>1.2</v>
+        <v>4</v>
       </c>
       <c r="I15" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.45</v>
       </c>
       <c r="J15" s="70">
         <v>0</v>
@@ -2422,8 +2422,12 @@
       <c r="K15" s="70">
         <v>0</v>
       </c>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
+      <c r="L15" s="70">
+        <v>0.5</v>
+      </c>
+      <c r="M15" s="14">
+        <v>2.95</v>
+      </c>
       <c r="N15" s="4"/>
       <c r="O15" s="17"/>
       <c r="P15" s="16"/>
@@ -2436,8 +2440,8 @@
       <c r="W15" s="19"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B16" s="107"/>
-      <c r="C16" s="100"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="109"/>
       <c r="D16" s="4" t="s">
         <v>20</v>
       </c>
@@ -2451,7 +2455,7 @@
         <v>2</v>
       </c>
       <c r="H16" s="4">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="I16" s="55">
         <f t="shared" si="0"/>
@@ -2463,7 +2467,7 @@
       <c r="K16" s="70">
         <v>0</v>
       </c>
-      <c r="L16" s="14"/>
+      <c r="L16" s="70"/>
       <c r="M16" s="14"/>
       <c r="N16" s="4"/>
       <c r="O16" s="17"/>
@@ -2477,8 +2481,8 @@
       <c r="W16" s="19"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B17" s="107"/>
-      <c r="C17" s="100"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="109"/>
       <c r="D17" s="4" t="s">
         <v>21</v>
       </c>
@@ -2492,7 +2496,7 @@
         <v>3</v>
       </c>
       <c r="H17" s="4">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="I17" s="55">
         <f t="shared" si="0"/>
@@ -2504,7 +2508,7 @@
       <c r="K17" s="70">
         <v>0</v>
       </c>
-      <c r="L17" s="14"/>
+      <c r="L17" s="70"/>
       <c r="M17" s="14"/>
       <c r="N17" s="4"/>
       <c r="O17" s="17"/>
@@ -2518,8 +2522,8 @@
       <c r="W17" s="19"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B18" s="107"/>
-      <c r="C18" s="100"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="109"/>
       <c r="D18" s="4" t="s">
         <v>22</v>
       </c>
@@ -2533,7 +2537,7 @@
         <v>3</v>
       </c>
       <c r="H18" s="4">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="I18" s="55">
         <f t="shared" si="0"/>
@@ -2545,7 +2549,7 @@
       <c r="K18" s="70">
         <v>0</v>
       </c>
-      <c r="L18" s="14"/>
+      <c r="L18" s="70"/>
       <c r="M18" s="14"/>
       <c r="N18" s="4"/>
       <c r="O18" s="17"/>
@@ -2559,8 +2563,8 @@
       <c r="W18" s="19"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B19" s="107"/>
-      <c r="C19" s="100"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="109"/>
       <c r="D19" s="4" t="s">
         <v>23</v>
       </c>
@@ -2574,7 +2578,7 @@
         <v>3</v>
       </c>
       <c r="H19" s="4">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="I19" s="55">
         <f t="shared" si="0"/>
@@ -2586,7 +2590,7 @@
       <c r="K19" s="70">
         <v>0</v>
       </c>
-      <c r="L19" s="14"/>
+      <c r="L19" s="70"/>
       <c r="M19" s="14"/>
       <c r="N19" s="4"/>
       <c r="O19" s="17"/>
@@ -2600,8 +2604,8 @@
       <c r="W19" s="19"/>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B20" s="107"/>
-      <c r="C20" s="100"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="109"/>
       <c r="D20" s="4" t="s">
         <v>24</v>
       </c>
@@ -2615,7 +2619,7 @@
         <v>3</v>
       </c>
       <c r="H20" s="4">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="I20" s="55">
         <f t="shared" si="0"/>
@@ -2627,7 +2631,7 @@
       <c r="K20" s="70">
         <v>0</v>
       </c>
-      <c r="L20" s="14"/>
+      <c r="L20" s="70"/>
       <c r="M20" s="14"/>
       <c r="N20" s="4"/>
       <c r="O20" s="17"/>
@@ -2641,8 +2645,8 @@
       <c r="W20" s="19"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B21" s="107"/>
-      <c r="C21" s="100"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="109"/>
       <c r="D21" s="32" t="s">
         <v>36</v>
       </c>
@@ -2668,7 +2672,7 @@
       <c r="K21" s="70">
         <v>0</v>
       </c>
-      <c r="L21" s="14"/>
+      <c r="L21" s="70"/>
       <c r="M21" s="14"/>
       <c r="N21" s="4"/>
       <c r="O21" s="17"/>
@@ -2682,8 +2686,8 @@
       <c r="W21" s="19"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B22" s="107"/>
-      <c r="C22" s="100"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="109"/>
       <c r="D22" s="32" t="s">
         <v>37</v>
       </c>
@@ -2709,7 +2713,7 @@
       <c r="K22" s="70">
         <v>0</v>
       </c>
-      <c r="L22" s="14"/>
+      <c r="L22" s="70"/>
       <c r="M22" s="14"/>
       <c r="N22" s="4"/>
       <c r="O22" s="17"/>
@@ -2723,8 +2727,8 @@
       <c r="W22" s="19"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B23" s="107"/>
-      <c r="C23" s="100"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="109"/>
       <c r="D23" s="32" t="s">
         <v>38</v>
       </c>
@@ -2750,7 +2754,7 @@
       <c r="K23" s="70">
         <v>0</v>
       </c>
-      <c r="L23" s="14"/>
+      <c r="L23" s="70"/>
       <c r="M23" s="14"/>
       <c r="N23" s="4"/>
       <c r="O23" s="17"/>
@@ -2764,8 +2768,8 @@
       <c r="W23" s="19"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B24" s="107"/>
-      <c r="C24" s="100"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="109"/>
       <c r="D24" s="32" t="s">
         <v>39</v>
       </c>
@@ -2791,7 +2795,7 @@
       <c r="K24" s="70">
         <v>0</v>
       </c>
-      <c r="L24" s="14"/>
+      <c r="L24" s="70"/>
       <c r="M24" s="14"/>
       <c r="N24" s="4"/>
       <c r="O24" s="17"/>
@@ -2805,8 +2809,8 @@
       <c r="W24" s="19"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B25" s="107"/>
-      <c r="C25" s="100"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="109"/>
       <c r="D25" s="32" t="s">
         <v>40</v>
       </c>
@@ -2832,7 +2836,7 @@
       <c r="K25" s="70">
         <v>0</v>
       </c>
-      <c r="L25" s="14"/>
+      <c r="L25" s="70"/>
       <c r="M25" s="14"/>
       <c r="N25" s="4"/>
       <c r="O25" s="17"/>
@@ -2846,8 +2850,8 @@
       <c r="W25" s="19"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B26" s="107"/>
-      <c r="C26" s="100"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="109"/>
       <c r="D26" s="32" t="s">
         <v>41</v>
       </c>
@@ -2873,7 +2877,7 @@
       <c r="K26" s="70">
         <v>0</v>
       </c>
-      <c r="L26" s="14"/>
+      <c r="L26" s="70"/>
       <c r="M26" s="14"/>
       <c r="N26" s="4"/>
       <c r="O26" s="17"/>
@@ -2887,8 +2891,8 @@
       <c r="W26" s="19"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B27" s="107"/>
-      <c r="C27" s="100"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="109"/>
       <c r="D27" s="32" t="s">
         <v>42</v>
       </c>
@@ -2914,7 +2918,7 @@
       <c r="K27" s="70">
         <v>0</v>
       </c>
-      <c r="L27" s="14"/>
+      <c r="L27" s="70"/>
       <c r="M27" s="14"/>
       <c r="N27" s="4"/>
       <c r="O27" s="17"/>
@@ -2928,8 +2932,8 @@
       <c r="W27" s="19"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B28" s="107"/>
-      <c r="C28" s="100"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="109"/>
       <c r="D28" s="32" t="s">
         <v>43</v>
       </c>
@@ -2955,7 +2959,7 @@
       <c r="K28" s="70">
         <v>0</v>
       </c>
-      <c r="L28" s="14"/>
+      <c r="L28" s="70"/>
       <c r="M28" s="14"/>
       <c r="N28" s="4"/>
       <c r="O28" s="17"/>
@@ -2969,8 +2973,8 @@
       <c r="W28" s="19"/>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B29" s="107"/>
-      <c r="C29" s="100"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="109"/>
       <c r="D29" s="32" t="s">
         <v>44</v>
       </c>
@@ -2996,7 +3000,7 @@
       <c r="K29" s="70">
         <v>0</v>
       </c>
-      <c r="L29" s="14"/>
+      <c r="L29" s="70"/>
       <c r="M29" s="14"/>
       <c r="N29" s="4"/>
       <c r="O29" s="17"/>
@@ -3010,8 +3014,8 @@
       <c r="W29" s="19"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B30" s="107"/>
-      <c r="C30" s="100"/>
+      <c r="B30" s="90"/>
+      <c r="C30" s="109"/>
       <c r="D30" s="32" t="s">
         <v>45</v>
       </c>
@@ -3037,7 +3041,7 @@
       <c r="K30" s="70">
         <v>0</v>
       </c>
-      <c r="L30" s="14"/>
+      <c r="L30" s="70"/>
       <c r="M30" s="14"/>
       <c r="N30" s="4"/>
       <c r="O30" s="17"/>
@@ -3051,8 +3055,8 @@
       <c r="W30" s="19"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B31" s="107"/>
-      <c r="C31" s="100"/>
+      <c r="B31" s="90"/>
+      <c r="C31" s="109"/>
       <c r="D31" s="32" t="s">
         <v>46</v>
       </c>
@@ -3078,7 +3082,7 @@
       <c r="K31" s="70">
         <v>0</v>
       </c>
-      <c r="L31" s="14"/>
+      <c r="L31" s="70"/>
       <c r="M31" s="14"/>
       <c r="N31" s="4"/>
       <c r="O31" s="17"/>
@@ -3092,8 +3096,8 @@
       <c r="W31" s="19"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B32" s="107"/>
-      <c r="C32" s="100"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="109"/>
       <c r="D32" s="32" t="s">
         <v>47</v>
       </c>
@@ -3119,7 +3123,7 @@
       <c r="K32" s="70">
         <v>0</v>
       </c>
-      <c r="L32" s="14"/>
+      <c r="L32" s="70"/>
       <c r="M32" s="14"/>
       <c r="N32" s="4"/>
       <c r="O32" s="17"/>
@@ -3133,8 +3137,8 @@
       <c r="W32" s="19"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B33" s="107"/>
-      <c r="C33" s="100"/>
+      <c r="B33" s="90"/>
+      <c r="C33" s="109"/>
       <c r="D33" s="32" t="s">
         <v>48</v>
       </c>
@@ -3160,7 +3164,7 @@
       <c r="K33" s="70">
         <v>0</v>
       </c>
-      <c r="L33" s="14"/>
+      <c r="L33" s="70"/>
       <c r="M33" s="14"/>
       <c r="N33" s="4"/>
       <c r="O33" s="17"/>
@@ -3174,8 +3178,8 @@
       <c r="W33" s="19"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B34" s="107"/>
-      <c r="C34" s="100"/>
+      <c r="B34" s="90"/>
+      <c r="C34" s="109"/>
       <c r="D34" s="32" t="s">
         <v>49</v>
       </c>
@@ -3201,7 +3205,7 @@
       <c r="K34" s="70">
         <v>0</v>
       </c>
-      <c r="L34" s="14"/>
+      <c r="L34" s="70"/>
       <c r="M34" s="14"/>
       <c r="N34" s="4"/>
       <c r="O34" s="17"/>
@@ -3215,8 +3219,8 @@
       <c r="W34" s="19"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B35" s="107"/>
-      <c r="C35" s="100"/>
+      <c r="B35" s="90"/>
+      <c r="C35" s="109"/>
       <c r="D35" s="32" t="s">
         <v>50</v>
       </c>
@@ -3242,7 +3246,7 @@
       <c r="K35" s="70">
         <v>0</v>
       </c>
-      <c r="L35" s="14"/>
+      <c r="L35" s="70"/>
       <c r="M35" s="14"/>
       <c r="N35" s="4"/>
       <c r="O35" s="17"/>
@@ -3256,8 +3260,8 @@
       <c r="W35" s="19"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B36" s="107"/>
-      <c r="C36" s="100"/>
+      <c r="B36" s="90"/>
+      <c r="C36" s="109"/>
       <c r="D36" s="32" t="s">
         <v>51</v>
       </c>
@@ -3283,7 +3287,7 @@
       <c r="K36" s="70">
         <v>0</v>
       </c>
-      <c r="L36" s="14"/>
+      <c r="L36" s="70"/>
       <c r="M36" s="14"/>
       <c r="N36" s="4"/>
       <c r="O36" s="17"/>
@@ -3297,8 +3301,8 @@
       <c r="W36" s="19"/>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B37" s="107"/>
-      <c r="C37" s="100"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="109"/>
       <c r="D37" s="32" t="s">
         <v>52</v>
       </c>
@@ -3324,7 +3328,7 @@
       <c r="K37" s="70">
         <v>0</v>
       </c>
-      <c r="L37" s="14"/>
+      <c r="L37" s="70"/>
       <c r="M37" s="14"/>
       <c r="N37" s="4"/>
       <c r="O37" s="17"/>
@@ -3338,8 +3342,8 @@
       <c r="W37" s="19"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B38" s="107"/>
-      <c r="C38" s="100"/>
+      <c r="B38" s="90"/>
+      <c r="C38" s="109"/>
       <c r="D38" s="32" t="s">
         <v>53</v>
       </c>
@@ -3365,7 +3369,7 @@
       <c r="K38" s="70">
         <v>0</v>
       </c>
-      <c r="L38" s="14"/>
+      <c r="L38" s="70"/>
       <c r="M38" s="14"/>
       <c r="N38" s="4"/>
       <c r="O38" s="17"/>
@@ -3379,8 +3383,8 @@
       <c r="W38" s="19"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B39" s="107"/>
-      <c r="C39" s="100"/>
+      <c r="B39" s="90"/>
+      <c r="C39" s="109"/>
       <c r="D39" s="32" t="s">
         <v>54</v>
       </c>
@@ -3406,7 +3410,7 @@
       <c r="K39" s="70">
         <v>0</v>
       </c>
-      <c r="L39" s="14"/>
+      <c r="L39" s="70"/>
       <c r="M39" s="14"/>
       <c r="N39" s="4"/>
       <c r="O39" s="17"/>
@@ -3420,8 +3424,8 @@
       <c r="W39" s="19"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B40" s="107"/>
-      <c r="C40" s="100"/>
+      <c r="B40" s="90"/>
+      <c r="C40" s="109"/>
       <c r="D40" s="32" t="s">
         <v>55</v>
       </c>
@@ -3447,7 +3451,7 @@
       <c r="K40" s="70">
         <v>0</v>
       </c>
-      <c r="L40" s="14"/>
+      <c r="L40" s="70"/>
       <c r="M40" s="14"/>
       <c r="N40" s="4"/>
       <c r="O40" s="17"/>
@@ -3461,8 +3465,8 @@
       <c r="W40" s="19"/>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B41" s="107"/>
-      <c r="C41" s="100"/>
+      <c r="B41" s="90"/>
+      <c r="C41" s="109"/>
       <c r="D41" s="32" t="s">
         <v>56</v>
       </c>
@@ -3488,7 +3492,7 @@
       <c r="K41" s="70">
         <v>0</v>
       </c>
-      <c r="L41" s="14"/>
+      <c r="L41" s="70"/>
       <c r="M41" s="14"/>
       <c r="N41" s="4"/>
       <c r="O41" s="17"/>
@@ -3502,8 +3506,8 @@
       <c r="W41" s="19"/>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B42" s="107"/>
-      <c r="C42" s="100"/>
+      <c r="B42" s="90"/>
+      <c r="C42" s="109"/>
       <c r="D42" s="32" t="s">
         <v>57</v>
       </c>
@@ -3529,7 +3533,7 @@
       <c r="K42" s="70">
         <v>0</v>
       </c>
-      <c r="L42" s="14"/>
+      <c r="L42" s="70"/>
       <c r="M42" s="14"/>
       <c r="N42" s="4"/>
       <c r="O42" s="17"/>
@@ -3543,8 +3547,8 @@
       <c r="W42" s="19"/>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B43" s="107"/>
-      <c r="C43" s="100"/>
+      <c r="B43" s="90"/>
+      <c r="C43" s="109"/>
       <c r="D43" s="32" t="s">
         <v>58</v>
       </c>
@@ -3570,7 +3574,7 @@
       <c r="K43" s="70">
         <v>0</v>
       </c>
-      <c r="L43" s="14"/>
+      <c r="L43" s="70"/>
       <c r="M43" s="14"/>
       <c r="N43" s="4"/>
       <c r="O43" s="17"/>
@@ -3584,8 +3588,8 @@
       <c r="W43" s="19"/>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B44" s="107"/>
-      <c r="C44" s="100"/>
+      <c r="B44" s="90"/>
+      <c r="C44" s="109"/>
       <c r="D44" s="32" t="s">
         <v>59</v>
       </c>
@@ -3611,7 +3615,7 @@
       <c r="K44" s="70">
         <v>0</v>
       </c>
-      <c r="L44" s="14"/>
+      <c r="L44" s="70"/>
       <c r="M44" s="14"/>
       <c r="N44" s="4"/>
       <c r="O44" s="17"/>
@@ -3625,8 +3629,8 @@
       <c r="W44" s="19"/>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B45" s="107"/>
-      <c r="C45" s="100"/>
+      <c r="B45" s="90"/>
+      <c r="C45" s="109"/>
       <c r="D45" s="32" t="s">
         <v>60</v>
       </c>
@@ -3652,7 +3656,7 @@
       <c r="K45" s="70">
         <v>0</v>
       </c>
-      <c r="L45" s="14"/>
+      <c r="L45" s="70"/>
       <c r="M45" s="14"/>
       <c r="N45" s="4"/>
       <c r="O45" s="17"/>
@@ -3666,8 +3670,8 @@
       <c r="W45" s="19"/>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B46" s="107"/>
-      <c r="C46" s="100"/>
+      <c r="B46" s="90"/>
+      <c r="C46" s="109"/>
       <c r="D46" s="32" t="s">
         <v>61</v>
       </c>
@@ -3693,7 +3697,7 @@
       <c r="K46" s="70">
         <v>0</v>
       </c>
-      <c r="L46" s="14"/>
+      <c r="L46" s="70"/>
       <c r="M46" s="14"/>
       <c r="N46" s="4"/>
       <c r="O46" s="17"/>
@@ -3707,8 +3711,8 @@
       <c r="W46" s="19"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B47" s="107"/>
-      <c r="C47" s="100"/>
+      <c r="B47" s="90"/>
+      <c r="C47" s="109"/>
       <c r="D47" s="32" t="s">
         <v>62</v>
       </c>
@@ -3734,7 +3738,7 @@
       <c r="K47" s="70">
         <v>0</v>
       </c>
-      <c r="L47" s="14"/>
+      <c r="L47" s="70"/>
       <c r="M47" s="14"/>
       <c r="N47" s="4"/>
       <c r="O47" s="17"/>
@@ -3748,8 +3752,8 @@
       <c r="W47" s="19"/>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B48" s="107"/>
-      <c r="C48" s="100"/>
+      <c r="B48" s="90"/>
+      <c r="C48" s="109"/>
       <c r="D48" s="32" t="s">
         <v>63</v>
       </c>
@@ -3775,7 +3779,7 @@
       <c r="K48" s="70">
         <v>0</v>
       </c>
-      <c r="L48" s="14"/>
+      <c r="L48" s="70"/>
       <c r="M48" s="14"/>
       <c r="N48" s="4"/>
       <c r="O48" s="17"/>
@@ -3789,8 +3793,8 @@
       <c r="W48" s="19"/>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B49" s="107"/>
-      <c r="C49" s="100"/>
+      <c r="B49" s="90"/>
+      <c r="C49" s="109"/>
       <c r="D49" s="32" t="s">
         <v>64</v>
       </c>
@@ -3816,7 +3820,7 @@
       <c r="K49" s="70">
         <v>0</v>
       </c>
-      <c r="L49" s="14"/>
+      <c r="L49" s="70"/>
       <c r="M49" s="14"/>
       <c r="N49" s="4"/>
       <c r="O49" s="17"/>
@@ -3830,8 +3834,8 @@
       <c r="W49" s="19"/>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B50" s="107"/>
-      <c r="C50" s="100"/>
+      <c r="B50" s="90"/>
+      <c r="C50" s="109"/>
       <c r="D50" s="32" t="s">
         <v>65</v>
       </c>
@@ -3857,7 +3861,7 @@
       <c r="K50" s="70">
         <v>0</v>
       </c>
-      <c r="L50" s="14"/>
+      <c r="L50" s="70"/>
       <c r="M50" s="14"/>
       <c r="N50" s="4"/>
       <c r="O50" s="17"/>
@@ -3871,8 +3875,8 @@
       <c r="W50" s="19"/>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B51" s="107"/>
-      <c r="C51" s="100"/>
+      <c r="B51" s="90"/>
+      <c r="C51" s="109"/>
       <c r="D51" s="32" t="s">
         <v>66</v>
       </c>
@@ -3898,7 +3902,7 @@
       <c r="K51" s="70">
         <v>0</v>
       </c>
-      <c r="L51" s="14"/>
+      <c r="L51" s="70"/>
       <c r="M51" s="14"/>
       <c r="N51" s="4"/>
       <c r="O51" s="17"/>
@@ -3912,8 +3916,8 @@
       <c r="W51" s="19"/>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B52" s="107"/>
-      <c r="C52" s="100"/>
+      <c r="B52" s="90"/>
+      <c r="C52" s="109"/>
       <c r="D52" s="32" t="s">
         <v>67</v>
       </c>
@@ -3939,7 +3943,7 @@
       <c r="K52" s="70">
         <v>0</v>
       </c>
-      <c r="L52" s="14"/>
+      <c r="L52" s="70"/>
       <c r="M52" s="14"/>
       <c r="N52" s="4"/>
       <c r="O52" s="17"/>
@@ -3953,8 +3957,8 @@
       <c r="W52" s="19"/>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B53" s="107"/>
-      <c r="C53" s="100"/>
+      <c r="B53" s="90"/>
+      <c r="C53" s="109"/>
       <c r="D53" s="32" t="s">
         <v>68</v>
       </c>
@@ -3980,7 +3984,7 @@
       <c r="K53" s="70">
         <v>0</v>
       </c>
-      <c r="L53" s="14"/>
+      <c r="L53" s="70"/>
       <c r="M53" s="14"/>
       <c r="N53" s="4"/>
       <c r="O53" s="17"/>
@@ -3994,8 +3998,8 @@
       <c r="W53" s="19"/>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B54" s="107"/>
-      <c r="C54" s="101"/>
+      <c r="B54" s="90"/>
+      <c r="C54" s="110"/>
       <c r="D54" s="32" t="s">
         <v>69</v>
       </c>
@@ -4021,7 +4025,7 @@
       <c r="K54" s="70">
         <v>0</v>
       </c>
-      <c r="L54" s="14"/>
+      <c r="L54" s="70"/>
       <c r="M54" s="14"/>
       <c r="N54" s="4"/>
       <c r="O54" s="17"/>
@@ -4035,8 +4039,8 @@
       <c r="W54" s="19"/>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B55" s="107"/>
-      <c r="C55" s="97" t="s">
+      <c r="B55" s="90"/>
+      <c r="C55" s="106" t="s">
         <v>26</v>
       </c>
       <c r="D55" s="29" t="s">
@@ -4064,7 +4068,7 @@
       <c r="K55" s="70">
         <v>0</v>
       </c>
-      <c r="L55" s="14"/>
+      <c r="L55" s="70"/>
       <c r="M55" s="14"/>
       <c r="N55" s="4"/>
       <c r="O55" s="17"/>
@@ -4078,8 +4082,8 @@
       <c r="W55" s="19"/>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B56" s="107"/>
-      <c r="C56" s="98"/>
+      <c r="B56" s="90"/>
+      <c r="C56" s="107"/>
       <c r="D56" s="29" t="s">
         <v>29</v>
       </c>
@@ -4105,7 +4109,7 @@
       <c r="K56" s="70">
         <v>0</v>
       </c>
-      <c r="L56" s="14"/>
+      <c r="L56" s="70"/>
       <c r="M56" s="14"/>
       <c r="N56" s="4"/>
       <c r="O56" s="17"/>
@@ -4119,8 +4123,8 @@
       <c r="W56" s="19"/>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B57" s="107"/>
-      <c r="C57" s="98"/>
+      <c r="B57" s="90"/>
+      <c r="C57" s="107"/>
       <c r="D57" s="29" t="s">
         <v>30</v>
       </c>
@@ -4146,7 +4150,7 @@
       <c r="K57" s="70">
         <v>0</v>
       </c>
-      <c r="L57" s="14"/>
+      <c r="L57" s="70"/>
       <c r="M57" s="14"/>
       <c r="N57" s="4"/>
       <c r="O57" s="17"/>
@@ -4160,8 +4164,8 @@
       <c r="W57" s="19"/>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B58" s="107"/>
-      <c r="C58" s="98"/>
+      <c r="B58" s="90"/>
+      <c r="C58" s="107"/>
       <c r="D58" s="29" t="s">
         <v>31</v>
       </c>
@@ -4187,7 +4191,7 @@
       <c r="K58" s="70">
         <v>0</v>
       </c>
-      <c r="L58" s="14"/>
+      <c r="L58" s="70"/>
       <c r="M58" s="14"/>
       <c r="N58" s="4"/>
       <c r="O58" s="17"/>
@@ -4201,8 +4205,8 @@
       <c r="W58" s="19"/>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B59" s="107"/>
-      <c r="C59" s="98"/>
+      <c r="B59" s="90"/>
+      <c r="C59" s="107"/>
       <c r="D59" s="29" t="s">
         <v>34</v>
       </c>
@@ -4228,7 +4232,7 @@
       <c r="K59" s="70">
         <v>0</v>
       </c>
-      <c r="L59" s="4"/>
+      <c r="L59" s="70"/>
       <c r="M59" s="4"/>
       <c r="N59" s="14"/>
       <c r="O59" s="17"/>
@@ -4242,8 +4246,8 @@
       <c r="W59" s="19"/>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B60" s="107"/>
-      <c r="C60" s="98"/>
+      <c r="B60" s="90"/>
+      <c r="C60" s="107"/>
       <c r="D60" s="29" t="s">
         <v>32</v>
       </c>
@@ -4269,7 +4273,7 @@
       <c r="K60" s="70">
         <v>0</v>
       </c>
-      <c r="L60" s="4"/>
+      <c r="L60" s="70"/>
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
       <c r="O60" s="17"/>
@@ -4283,8 +4287,8 @@
       <c r="W60" s="19"/>
     </row>
     <row r="61" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="108"/>
-      <c r="C61" s="98"/>
+      <c r="B61" s="97"/>
+      <c r="C61" s="107"/>
       <c r="D61" s="62" t="s">
         <v>33</v>
       </c>
@@ -4310,7 +4314,7 @@
       <c r="K61" s="72">
         <v>0</v>
       </c>
-      <c r="L61" s="8"/>
+      <c r="L61" s="72"/>
       <c r="M61" s="8"/>
       <c r="N61" s="8"/>
       <c r="O61" s="26"/>
@@ -4324,10 +4328,10 @@
       <c r="W61" s="28"/>
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B62" s="106" t="s">
+      <c r="B62" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="C62" s="116" t="s">
+      <c r="C62" s="111" t="s">
         <v>79</v>
       </c>
       <c r="D62" s="39" t="s">
@@ -4355,7 +4359,7 @@
       <c r="K62" s="69">
         <v>0</v>
       </c>
-      <c r="L62" s="39"/>
+      <c r="L62" s="69"/>
       <c r="M62" s="39"/>
       <c r="N62" s="39"/>
       <c r="O62" s="51"/>
@@ -4369,8 +4373,8 @@
       <c r="W62" s="52"/>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B63" s="107"/>
-      <c r="C63" s="115"/>
+      <c r="B63" s="90"/>
+      <c r="C63" s="112"/>
       <c r="D63" s="4" t="s">
         <v>71</v>
       </c>
@@ -4396,7 +4400,7 @@
       <c r="K63" s="70">
         <v>0</v>
       </c>
-      <c r="L63" s="4"/>
+      <c r="L63" s="70"/>
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
       <c r="O63" s="17"/>
@@ -4410,8 +4414,8 @@
       <c r="W63" s="19"/>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B64" s="107"/>
-      <c r="C64" s="115"/>
+      <c r="B64" s="90"/>
+      <c r="C64" s="112"/>
       <c r="D64" s="4" t="s">
         <v>72</v>
       </c>
@@ -4437,7 +4441,7 @@
       <c r="K64" s="70">
         <v>0</v>
       </c>
-      <c r="L64" s="4"/>
+      <c r="L64" s="70"/>
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
       <c r="O64" s="17"/>
@@ -4451,8 +4455,8 @@
       <c r="W64" s="19"/>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B65" s="107"/>
-      <c r="C65" s="115"/>
+      <c r="B65" s="90"/>
+      <c r="C65" s="112"/>
       <c r="D65" s="29" t="s">
         <v>76</v>
       </c>
@@ -4478,7 +4482,7 @@
       <c r="K65" s="70">
         <v>0</v>
       </c>
-      <c r="L65" s="4"/>
+      <c r="L65" s="70"/>
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
       <c r="O65" s="17"/>
@@ -4492,7 +4496,7 @@
       <c r="W65" s="19"/>
     </row>
     <row r="66" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B66" s="107"/>
+      <c r="B66" s="90"/>
       <c r="C66" s="33" t="s">
         <v>73</v>
       </c>
@@ -4519,7 +4523,7 @@
       <c r="K66" s="70">
         <v>0</v>
       </c>
-      <c r="L66" s="4"/>
+      <c r="L66" s="70"/>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
       <c r="O66" s="17"/>
@@ -4533,7 +4537,7 @@
       <c r="W66" s="19"/>
     </row>
     <row r="67" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B67" s="107"/>
+      <c r="B67" s="90"/>
       <c r="C67" s="33" t="s">
         <v>81</v>
       </c>
@@ -4560,7 +4564,7 @@
       <c r="K67" s="70">
         <v>0</v>
       </c>
-      <c r="L67" s="4"/>
+      <c r="L67" s="70"/>
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
       <c r="O67" s="17"/>
@@ -4574,8 +4578,8 @@
       <c r="W67" s="19"/>
     </row>
     <row r="68" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="107"/>
-      <c r="C68" s="115" t="s">
+      <c r="B68" s="90"/>
+      <c r="C68" s="112" t="s">
         <v>80</v>
       </c>
       <c r="D68" s="4" t="s">
@@ -4603,7 +4607,7 @@
       <c r="K68" s="70">
         <v>0</v>
       </c>
-      <c r="L68" s="4"/>
+      <c r="L68" s="70"/>
       <c r="M68" s="4"/>
       <c r="N68" s="4"/>
       <c r="O68" s="17"/>
@@ -4617,8 +4621,8 @@
       <c r="W68" s="19"/>
     </row>
     <row r="69" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="107"/>
-      <c r="C69" s="115"/>
+      <c r="B69" s="90"/>
+      <c r="C69" s="112"/>
       <c r="D69" s="4" t="s">
         <v>75</v>
       </c>
@@ -4644,7 +4648,7 @@
       <c r="K69" s="70">
         <v>0</v>
       </c>
-      <c r="L69" s="4"/>
+      <c r="L69" s="70"/>
       <c r="M69" s="4"/>
       <c r="N69" s="4"/>
       <c r="O69" s="17"/>
@@ -4658,8 +4662,8 @@
       <c r="W69" s="19"/>
     </row>
     <row r="70" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="107"/>
-      <c r="C70" s="115"/>
+      <c r="B70" s="90"/>
+      <c r="C70" s="112"/>
       <c r="D70" s="4" t="s">
         <v>77</v>
       </c>
@@ -4685,7 +4689,7 @@
       <c r="K70" s="70">
         <v>0</v>
       </c>
-      <c r="L70" s="4"/>
+      <c r="L70" s="70"/>
       <c r="M70" s="4"/>
       <c r="N70" s="4"/>
       <c r="O70" s="17"/>
@@ -4699,8 +4703,8 @@
       <c r="W70" s="19"/>
     </row>
     <row r="71" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="109"/>
-      <c r="C71" s="117"/>
+      <c r="B71" s="91"/>
+      <c r="C71" s="113"/>
       <c r="D71" s="24" t="s">
         <v>78</v>
       </c>
@@ -4726,7 +4730,7 @@
       <c r="K71" s="71">
         <v>0</v>
       </c>
-      <c r="L71" s="24"/>
+      <c r="L71" s="71"/>
       <c r="M71" s="24"/>
       <c r="N71" s="24"/>
       <c r="O71" s="22"/>
@@ -4740,10 +4744,10 @@
       <c r="W71" s="25"/>
     </row>
     <row r="72" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="106" t="s">
+      <c r="B72" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="C72" s="89" t="s">
+      <c r="C72" s="117" t="s">
         <v>117</v>
       </c>
       <c r="D72" s="39" t="s">
@@ -4771,7 +4775,7 @@
       <c r="K72" s="69">
         <v>0</v>
       </c>
-      <c r="L72" s="39"/>
+      <c r="L72" s="69"/>
       <c r="M72" s="39"/>
       <c r="N72" s="39"/>
       <c r="O72" s="51"/>
@@ -4785,8 +4789,8 @@
       <c r="W72" s="52"/>
     </row>
     <row r="73" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="107"/>
-      <c r="C73" s="90"/>
+      <c r="B73" s="90"/>
+      <c r="C73" s="102"/>
       <c r="D73" s="4" t="s">
         <v>133</v>
       </c>
@@ -4812,7 +4816,7 @@
       <c r="K73" s="70">
         <v>0</v>
       </c>
-      <c r="L73" s="4"/>
+      <c r="L73" s="70"/>
       <c r="M73" s="4"/>
       <c r="N73" s="4"/>
       <c r="O73" s="17"/>
@@ -4826,8 +4830,8 @@
       <c r="W73" s="19"/>
     </row>
     <row r="74" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="107"/>
-      <c r="C74" s="90"/>
+      <c r="B74" s="90"/>
+      <c r="C74" s="102"/>
       <c r="D74" s="4" t="s">
         <v>156</v>
       </c>
@@ -4841,7 +4845,7 @@
       </c>
       <c r="J74" s="70"/>
       <c r="K74" s="70"/>
-      <c r="L74" s="4"/>
+      <c r="L74" s="70"/>
       <c r="M74" s="4"/>
       <c r="N74" s="4"/>
       <c r="O74" s="17"/>
@@ -4855,8 +4859,8 @@
       <c r="W74" s="19"/>
     </row>
     <row r="75" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="107"/>
-      <c r="C75" s="90"/>
+      <c r="B75" s="90"/>
+      <c r="C75" s="102"/>
       <c r="D75" s="4" t="s">
         <v>134</v>
       </c>
@@ -4882,7 +4886,7 @@
       <c r="K75" s="88">
         <v>0.67</v>
       </c>
-      <c r="L75" s="4"/>
+      <c r="L75" s="70"/>
       <c r="M75" s="4"/>
       <c r="N75" s="4"/>
       <c r="O75" s="17"/>
@@ -4896,8 +4900,8 @@
       <c r="W75" s="19"/>
     </row>
     <row r="76" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="107"/>
-      <c r="C76" s="90"/>
+      <c r="B76" s="90"/>
+      <c r="C76" s="102"/>
       <c r="D76" s="4" t="s">
         <v>135</v>
       </c>
@@ -4923,7 +4927,7 @@
       <c r="K76" s="70">
         <v>0</v>
       </c>
-      <c r="L76" s="4"/>
+      <c r="L76" s="70"/>
       <c r="M76" s="4"/>
       <c r="N76" s="4"/>
       <c r="O76" s="17"/>
@@ -4937,8 +4941,8 @@
       <c r="W76" s="19"/>
     </row>
     <row r="77" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="107"/>
-      <c r="C77" s="90" t="s">
+      <c r="B77" s="90"/>
+      <c r="C77" s="102" t="s">
         <v>118</v>
       </c>
       <c r="D77" s="4" t="s">
@@ -4966,7 +4970,7 @@
       <c r="K77" s="70">
         <v>0</v>
       </c>
-      <c r="L77" s="4"/>
+      <c r="L77" s="70"/>
       <c r="M77" s="4"/>
       <c r="N77" s="4"/>
       <c r="O77" s="17"/>
@@ -4980,8 +4984,8 @@
       <c r="W77" s="19"/>
     </row>
     <row r="78" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="107"/>
-      <c r="C78" s="90"/>
+      <c r="B78" s="90"/>
+      <c r="C78" s="102"/>
       <c r="D78" s="4" t="s">
         <v>133</v>
       </c>
@@ -5007,7 +5011,7 @@
       <c r="K78" s="70">
         <v>0</v>
       </c>
-      <c r="L78" s="4"/>
+      <c r="L78" s="70"/>
       <c r="M78" s="4"/>
       <c r="N78" s="4"/>
       <c r="O78" s="17"/>
@@ -5021,8 +5025,8 @@
       <c r="W78" s="19"/>
     </row>
     <row r="79" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="107"/>
-      <c r="C79" s="90"/>
+      <c r="B79" s="90"/>
+      <c r="C79" s="102"/>
       <c r="D79" s="4" t="s">
         <v>156</v>
       </c>
@@ -5036,7 +5040,7 @@
       </c>
       <c r="J79" s="70"/>
       <c r="K79" s="70"/>
-      <c r="L79" s="4"/>
+      <c r="L79" s="70"/>
       <c r="M79" s="4"/>
       <c r="N79" s="4"/>
       <c r="O79" s="17"/>
@@ -5050,8 +5054,8 @@
       <c r="W79" s="19"/>
     </row>
     <row r="80" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="107"/>
-      <c r="C80" s="90"/>
+      <c r="B80" s="90"/>
+      <c r="C80" s="102"/>
       <c r="D80" s="4" t="s">
         <v>134</v>
       </c>
@@ -5077,7 +5081,7 @@
       <c r="K80" s="70">
         <v>0</v>
       </c>
-      <c r="L80" s="4"/>
+      <c r="L80" s="70"/>
       <c r="M80" s="4"/>
       <c r="N80" s="4"/>
       <c r="O80" s="17"/>
@@ -5091,8 +5095,8 @@
       <c r="W80" s="19"/>
     </row>
     <row r="81" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="107"/>
-      <c r="C81" s="90"/>
+      <c r="B81" s="90"/>
+      <c r="C81" s="102"/>
       <c r="D81" s="4" t="s">
         <v>135</v>
       </c>
@@ -5118,7 +5122,7 @@
       <c r="K81" s="70">
         <v>0</v>
       </c>
-      <c r="L81" s="4"/>
+      <c r="L81" s="70"/>
       <c r="M81" s="4"/>
       <c r="N81" s="4"/>
       <c r="O81" s="17"/>
@@ -5132,8 +5136,8 @@
       <c r="W81" s="19"/>
     </row>
     <row r="82" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="107"/>
-      <c r="C82" s="90" t="s">
+      <c r="B82" s="90"/>
+      <c r="C82" s="102" t="s">
         <v>119</v>
       </c>
       <c r="D82" s="4" t="s">
@@ -5161,7 +5165,7 @@
       <c r="K82" s="70">
         <v>0</v>
       </c>
-      <c r="L82" s="4"/>
+      <c r="L82" s="70"/>
       <c r="M82" s="4"/>
       <c r="N82" s="4"/>
       <c r="O82" s="17"/>
@@ -5175,8 +5179,8 @@
       <c r="W82" s="19"/>
     </row>
     <row r="83" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="107"/>
-      <c r="C83" s="90"/>
+      <c r="B83" s="90"/>
+      <c r="C83" s="102"/>
       <c r="D83" s="4" t="s">
         <v>133</v>
       </c>
@@ -5202,7 +5206,7 @@
       <c r="K83" s="70">
         <v>0</v>
       </c>
-      <c r="L83" s="4"/>
+      <c r="L83" s="70"/>
       <c r="M83" s="4"/>
       <c r="N83" s="4"/>
       <c r="O83" s="17"/>
@@ -5216,8 +5220,8 @@
       <c r="W83" s="19"/>
     </row>
     <row r="84" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="107"/>
-      <c r="C84" s="90"/>
+      <c r="B84" s="90"/>
+      <c r="C84" s="102"/>
       <c r="D84" s="4" t="s">
         <v>156</v>
       </c>
@@ -5231,7 +5235,7 @@
       </c>
       <c r="J84" s="70"/>
       <c r="K84" s="70"/>
-      <c r="L84" s="4"/>
+      <c r="L84" s="70"/>
       <c r="M84" s="4"/>
       <c r="N84" s="4"/>
       <c r="O84" s="17"/>
@@ -5245,8 +5249,8 @@
       <c r="W84" s="19"/>
     </row>
     <row r="85" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="107"/>
-      <c r="C85" s="90"/>
+      <c r="B85" s="90"/>
+      <c r="C85" s="102"/>
       <c r="D85" s="4" t="s">
         <v>134</v>
       </c>
@@ -5272,7 +5276,7 @@
       <c r="K85" s="70">
         <v>0</v>
       </c>
-      <c r="L85" s="4"/>
+      <c r="L85" s="70"/>
       <c r="M85" s="4"/>
       <c r="N85" s="4"/>
       <c r="O85" s="17"/>
@@ -5286,8 +5290,8 @@
       <c r="W85" s="19"/>
     </row>
     <row r="86" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="107"/>
-      <c r="C86" s="90"/>
+      <c r="B86" s="90"/>
+      <c r="C86" s="102"/>
       <c r="D86" s="4" t="s">
         <v>135</v>
       </c>
@@ -5313,7 +5317,7 @@
       <c r="K86" s="70">
         <v>0</v>
       </c>
-      <c r="L86" s="4"/>
+      <c r="L86" s="70"/>
       <c r="M86" s="4"/>
       <c r="N86" s="4"/>
       <c r="O86" s="17"/>
@@ -5327,8 +5331,8 @@
       <c r="W86" s="19"/>
     </row>
     <row r="87" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="107"/>
-      <c r="C87" s="90" t="s">
+      <c r="B87" s="90"/>
+      <c r="C87" s="102" t="s">
         <v>120</v>
       </c>
       <c r="D87" s="4" t="s">
@@ -5356,7 +5360,7 @@
       <c r="K87" s="70">
         <v>0</v>
       </c>
-      <c r="L87" s="4"/>
+      <c r="L87" s="70"/>
       <c r="M87" s="4"/>
       <c r="N87" s="4"/>
       <c r="O87" s="17"/>
@@ -5370,8 +5374,8 @@
       <c r="W87" s="19"/>
     </row>
     <row r="88" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="107"/>
-      <c r="C88" s="90"/>
+      <c r="B88" s="90"/>
+      <c r="C88" s="102"/>
       <c r="D88" s="4" t="s">
         <v>133</v>
       </c>
@@ -5397,7 +5401,7 @@
       <c r="K88" s="70">
         <v>0</v>
       </c>
-      <c r="L88" s="4"/>
+      <c r="L88" s="70"/>
       <c r="M88" s="4"/>
       <c r="N88" s="4"/>
       <c r="O88" s="17"/>
@@ -5411,8 +5415,8 @@
       <c r="W88" s="19"/>
     </row>
     <row r="89" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="107"/>
-      <c r="C89" s="90"/>
+      <c r="B89" s="90"/>
+      <c r="C89" s="102"/>
       <c r="D89" s="4" t="s">
         <v>156</v>
       </c>
@@ -5426,7 +5430,7 @@
       </c>
       <c r="J89" s="70"/>
       <c r="K89" s="70"/>
-      <c r="L89" s="4"/>
+      <c r="L89" s="70"/>
       <c r="M89" s="4"/>
       <c r="N89" s="4"/>
       <c r="O89" s="17"/>
@@ -5440,8 +5444,8 @@
       <c r="W89" s="19"/>
     </row>
     <row r="90" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="107"/>
-      <c r="C90" s="90"/>
+      <c r="B90" s="90"/>
+      <c r="C90" s="102"/>
       <c r="D90" s="4" t="s">
         <v>134</v>
       </c>
@@ -5467,7 +5471,7 @@
       <c r="K90" s="70">
         <v>0</v>
       </c>
-      <c r="L90" s="4"/>
+      <c r="L90" s="70"/>
       <c r="M90" s="4"/>
       <c r="N90" s="4"/>
       <c r="O90" s="17"/>
@@ -5481,8 +5485,8 @@
       <c r="W90" s="19"/>
     </row>
     <row r="91" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="107"/>
-      <c r="C91" s="90"/>
+      <c r="B91" s="90"/>
+      <c r="C91" s="102"/>
       <c r="D91" s="4" t="s">
         <v>135</v>
       </c>
@@ -5508,7 +5512,7 @@
       <c r="K91" s="70">
         <v>0</v>
       </c>
-      <c r="L91" s="4"/>
+      <c r="L91" s="70"/>
       <c r="M91" s="4"/>
       <c r="N91" s="4"/>
       <c r="O91" s="17"/>
@@ -5522,8 +5526,8 @@
       <c r="W91" s="19"/>
     </row>
     <row r="92" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="107"/>
-      <c r="C92" s="90" t="s">
+      <c r="B92" s="90"/>
+      <c r="C92" s="102" t="s">
         <v>121</v>
       </c>
       <c r="D92" s="4" t="s">
@@ -5551,7 +5555,7 @@
       <c r="K92" s="70">
         <v>0</v>
       </c>
-      <c r="L92" s="4"/>
+      <c r="L92" s="70"/>
       <c r="M92" s="4"/>
       <c r="N92" s="4"/>
       <c r="O92" s="17"/>
@@ -5565,8 +5569,8 @@
       <c r="W92" s="19"/>
     </row>
     <row r="93" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="107"/>
-      <c r="C93" s="90"/>
+      <c r="B93" s="90"/>
+      <c r="C93" s="102"/>
       <c r="D93" s="4" t="s">
         <v>133</v>
       </c>
@@ -5592,7 +5596,7 @@
       <c r="K93" s="70">
         <v>0</v>
       </c>
-      <c r="L93" s="4"/>
+      <c r="L93" s="70"/>
       <c r="M93" s="4"/>
       <c r="N93" s="4"/>
       <c r="O93" s="17"/>
@@ -5606,8 +5610,8 @@
       <c r="W93" s="19"/>
     </row>
     <row r="94" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="107"/>
-      <c r="C94" s="90"/>
+      <c r="B94" s="90"/>
+      <c r="C94" s="102"/>
       <c r="D94" s="4" t="s">
         <v>156</v>
       </c>
@@ -5621,7 +5625,7 @@
       </c>
       <c r="J94" s="70"/>
       <c r="K94" s="70"/>
-      <c r="L94" s="4"/>
+      <c r="L94" s="70"/>
       <c r="M94" s="4"/>
       <c r="N94" s="4"/>
       <c r="O94" s="17"/>
@@ -5635,8 +5639,8 @@
       <c r="W94" s="19"/>
     </row>
     <row r="95" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="107"/>
-      <c r="C95" s="90"/>
+      <c r="B95" s="90"/>
+      <c r="C95" s="102"/>
       <c r="D95" s="4" t="s">
         <v>134</v>
       </c>
@@ -5662,7 +5666,7 @@
       <c r="K95" s="70">
         <v>0</v>
       </c>
-      <c r="L95" s="4"/>
+      <c r="L95" s="70"/>
       <c r="M95" s="4"/>
       <c r="N95" s="4"/>
       <c r="O95" s="17"/>
@@ -5676,8 +5680,8 @@
       <c r="W95" s="19"/>
     </row>
     <row r="96" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="107"/>
-      <c r="C96" s="90"/>
+      <c r="B96" s="90"/>
+      <c r="C96" s="102"/>
       <c r="D96" s="4" t="s">
         <v>135</v>
       </c>
@@ -5703,7 +5707,7 @@
       <c r="K96" s="70">
         <v>0</v>
       </c>
-      <c r="L96" s="4"/>
+      <c r="L96" s="70"/>
       <c r="M96" s="4"/>
       <c r="N96" s="4"/>
       <c r="O96" s="17"/>
@@ -5717,8 +5721,8 @@
       <c r="W96" s="19"/>
     </row>
     <row r="97" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="107"/>
-      <c r="C97" s="90" t="s">
+      <c r="B97" s="90"/>
+      <c r="C97" s="102" t="s">
         <v>122</v>
       </c>
       <c r="D97" s="4" t="s">
@@ -5746,7 +5750,7 @@
       <c r="K97" s="70">
         <v>0</v>
       </c>
-      <c r="L97" s="4"/>
+      <c r="L97" s="70"/>
       <c r="M97" s="4"/>
       <c r="N97" s="4"/>
       <c r="O97" s="17"/>
@@ -5760,8 +5764,8 @@
       <c r="W97" s="19"/>
     </row>
     <row r="98" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="107"/>
-      <c r="C98" s="90"/>
+      <c r="B98" s="90"/>
+      <c r="C98" s="102"/>
       <c r="D98" s="4" t="s">
         <v>133</v>
       </c>
@@ -5787,7 +5791,7 @@
       <c r="K98" s="70">
         <v>0</v>
       </c>
-      <c r="L98" s="4"/>
+      <c r="L98" s="70"/>
       <c r="M98" s="4"/>
       <c r="N98" s="4"/>
       <c r="O98" s="17"/>
@@ -5801,8 +5805,8 @@
       <c r="W98" s="19"/>
     </row>
     <row r="99" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="107"/>
-      <c r="C99" s="90"/>
+      <c r="B99" s="90"/>
+      <c r="C99" s="102"/>
       <c r="D99" s="4" t="s">
         <v>156</v>
       </c>
@@ -5816,7 +5820,7 @@
       </c>
       <c r="J99" s="70"/>
       <c r="K99" s="70"/>
-      <c r="L99" s="4"/>
+      <c r="L99" s="70"/>
       <c r="M99" s="4"/>
       <c r="N99" s="4"/>
       <c r="O99" s="17"/>
@@ -5830,8 +5834,8 @@
       <c r="W99" s="19"/>
     </row>
     <row r="100" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="107"/>
-      <c r="C100" s="90"/>
+      <c r="B100" s="90"/>
+      <c r="C100" s="102"/>
       <c r="D100" s="4" t="s">
         <v>134</v>
       </c>
@@ -5857,7 +5861,7 @@
       <c r="K100" s="70">
         <v>0</v>
       </c>
-      <c r="L100" s="4"/>
+      <c r="L100" s="70"/>
       <c r="M100" s="4"/>
       <c r="N100" s="4"/>
       <c r="O100" s="17"/>
@@ -5871,8 +5875,8 @@
       <c r="W100" s="19"/>
     </row>
     <row r="101" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="107"/>
-      <c r="C101" s="90"/>
+      <c r="B101" s="90"/>
+      <c r="C101" s="102"/>
       <c r="D101" s="4" t="s">
         <v>135</v>
       </c>
@@ -5898,7 +5902,7 @@
       <c r="K101" s="70">
         <v>0</v>
       </c>
-      <c r="L101" s="4"/>
+      <c r="L101" s="70"/>
       <c r="M101" s="4"/>
       <c r="N101" s="4"/>
       <c r="O101" s="17"/>
@@ -5912,8 +5916,8 @@
       <c r="W101" s="19"/>
     </row>
     <row r="102" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="107"/>
-      <c r="C102" s="90" t="s">
+      <c r="B102" s="90"/>
+      <c r="C102" s="102" t="s">
         <v>123</v>
       </c>
       <c r="D102" s="4" t="s">
@@ -5941,7 +5945,7 @@
       <c r="K102" s="70">
         <v>0</v>
       </c>
-      <c r="L102" s="4"/>
+      <c r="L102" s="70"/>
       <c r="M102" s="4"/>
       <c r="N102" s="4"/>
       <c r="O102" s="17"/>
@@ -5955,8 +5959,8 @@
       <c r="W102" s="19"/>
     </row>
     <row r="103" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="107"/>
-      <c r="C103" s="90"/>
+      <c r="B103" s="90"/>
+      <c r="C103" s="102"/>
       <c r="D103" s="4" t="s">
         <v>133</v>
       </c>
@@ -5982,7 +5986,7 @@
       <c r="K103" s="70">
         <v>0</v>
       </c>
-      <c r="L103" s="4"/>
+      <c r="L103" s="70"/>
       <c r="M103" s="4"/>
       <c r="N103" s="4"/>
       <c r="O103" s="17"/>
@@ -5996,8 +6000,8 @@
       <c r="W103" s="19"/>
     </row>
     <row r="104" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="107"/>
-      <c r="C104" s="90"/>
+      <c r="B104" s="90"/>
+      <c r="C104" s="102"/>
       <c r="D104" s="4" t="s">
         <v>156</v>
       </c>
@@ -6011,7 +6015,7 @@
       </c>
       <c r="J104" s="70"/>
       <c r="K104" s="70"/>
-      <c r="L104" s="4"/>
+      <c r="L104" s="70"/>
       <c r="M104" s="4"/>
       <c r="N104" s="4"/>
       <c r="O104" s="17"/>
@@ -6025,8 +6029,8 @@
       <c r="W104" s="19"/>
     </row>
     <row r="105" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="107"/>
-      <c r="C105" s="90"/>
+      <c r="B105" s="90"/>
+      <c r="C105" s="102"/>
       <c r="D105" s="4" t="s">
         <v>134</v>
       </c>
@@ -6052,7 +6056,7 @@
       <c r="K105" s="70">
         <v>0</v>
       </c>
-      <c r="L105" s="4"/>
+      <c r="L105" s="70"/>
       <c r="M105" s="4"/>
       <c r="N105" s="4"/>
       <c r="O105" s="17"/>
@@ -6066,8 +6070,8 @@
       <c r="W105" s="19"/>
     </row>
     <row r="106" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="107"/>
-      <c r="C106" s="90"/>
+      <c r="B106" s="90"/>
+      <c r="C106" s="102"/>
       <c r="D106" s="4" t="s">
         <v>135</v>
       </c>
@@ -6093,7 +6097,7 @@
       <c r="K106" s="70">
         <v>0</v>
       </c>
-      <c r="L106" s="4"/>
+      <c r="L106" s="70"/>
       <c r="M106" s="4"/>
       <c r="N106" s="4"/>
       <c r="O106" s="17"/>
@@ -6107,8 +6111,8 @@
       <c r="W106" s="19"/>
     </row>
     <row r="107" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="107"/>
-      <c r="C107" s="90" t="s">
+      <c r="B107" s="90"/>
+      <c r="C107" s="102" t="s">
         <v>124</v>
       </c>
       <c r="D107" s="4" t="s">
@@ -6136,7 +6140,7 @@
       <c r="K107" s="70">
         <v>0</v>
       </c>
-      <c r="L107" s="4"/>
+      <c r="L107" s="70"/>
       <c r="M107" s="4"/>
       <c r="N107" s="4"/>
       <c r="O107" s="17"/>
@@ -6150,8 +6154,8 @@
       <c r="W107" s="19"/>
     </row>
     <row r="108" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="107"/>
-      <c r="C108" s="90"/>
+      <c r="B108" s="90"/>
+      <c r="C108" s="102"/>
       <c r="D108" s="4" t="s">
         <v>133</v>
       </c>
@@ -6177,7 +6181,7 @@
       <c r="K108" s="70">
         <v>0</v>
       </c>
-      <c r="L108" s="4"/>
+      <c r="L108" s="70"/>
       <c r="M108" s="4"/>
       <c r="N108" s="4"/>
       <c r="O108" s="17"/>
@@ -6191,8 +6195,8 @@
       <c r="W108" s="19"/>
     </row>
     <row r="109" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="107"/>
-      <c r="C109" s="90"/>
+      <c r="B109" s="90"/>
+      <c r="C109" s="102"/>
       <c r="D109" s="4" t="s">
         <v>156</v>
       </c>
@@ -6206,7 +6210,7 @@
       </c>
       <c r="J109" s="70"/>
       <c r="K109" s="70"/>
-      <c r="L109" s="4"/>
+      <c r="L109" s="70"/>
       <c r="M109" s="4"/>
       <c r="N109" s="4"/>
       <c r="O109" s="17"/>
@@ -6220,8 +6224,8 @@
       <c r="W109" s="19"/>
     </row>
     <row r="110" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="107"/>
-      <c r="C110" s="90"/>
+      <c r="B110" s="90"/>
+      <c r="C110" s="102"/>
       <c r="D110" s="4" t="s">
         <v>134</v>
       </c>
@@ -6247,7 +6251,7 @@
       <c r="K110" s="70">
         <v>0</v>
       </c>
-      <c r="L110" s="4"/>
+      <c r="L110" s="70"/>
       <c r="M110" s="4"/>
       <c r="N110" s="4"/>
       <c r="O110" s="17"/>
@@ -6261,8 +6265,8 @@
       <c r="W110" s="19"/>
     </row>
     <row r="111" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="107"/>
-      <c r="C111" s="90"/>
+      <c r="B111" s="90"/>
+      <c r="C111" s="102"/>
       <c r="D111" s="4" t="s">
         <v>135</v>
       </c>
@@ -6288,7 +6292,7 @@
       <c r="K111" s="70">
         <v>0</v>
       </c>
-      <c r="L111" s="4"/>
+      <c r="L111" s="70"/>
       <c r="M111" s="4"/>
       <c r="N111" s="4"/>
       <c r="O111" s="17"/>
@@ -6302,8 +6306,8 @@
       <c r="W111" s="19"/>
     </row>
     <row r="112" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="107"/>
-      <c r="C112" s="90" t="s">
+      <c r="B112" s="90"/>
+      <c r="C112" s="102" t="s">
         <v>125</v>
       </c>
       <c r="D112" s="4" t="s">
@@ -6331,7 +6335,7 @@
       <c r="K112" s="70">
         <v>0</v>
       </c>
-      <c r="L112" s="4"/>
+      <c r="L112" s="70"/>
       <c r="M112" s="4"/>
       <c r="N112" s="4"/>
       <c r="O112" s="17"/>
@@ -6345,8 +6349,8 @@
       <c r="W112" s="19"/>
     </row>
     <row r="113" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="107"/>
-      <c r="C113" s="90"/>
+      <c r="B113" s="90"/>
+      <c r="C113" s="102"/>
       <c r="D113" s="4" t="s">
         <v>133</v>
       </c>
@@ -6372,7 +6376,7 @@
       <c r="K113" s="70">
         <v>0</v>
       </c>
-      <c r="L113" s="4"/>
+      <c r="L113" s="70"/>
       <c r="M113" s="4"/>
       <c r="N113" s="4"/>
       <c r="O113" s="17"/>
@@ -6386,8 +6390,8 @@
       <c r="W113" s="19"/>
     </row>
     <row r="114" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="107"/>
-      <c r="C114" s="90"/>
+      <c r="B114" s="90"/>
+      <c r="C114" s="102"/>
       <c r="D114" s="4" t="s">
         <v>156</v>
       </c>
@@ -6401,7 +6405,7 @@
       </c>
       <c r="J114" s="70"/>
       <c r="K114" s="70"/>
-      <c r="L114" s="4"/>
+      <c r="L114" s="70"/>
       <c r="M114" s="4"/>
       <c r="N114" s="4"/>
       <c r="O114" s="17"/>
@@ -6415,8 +6419,8 @@
       <c r="W114" s="19"/>
     </row>
     <row r="115" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="107"/>
-      <c r="C115" s="90"/>
+      <c r="B115" s="90"/>
+      <c r="C115" s="102"/>
       <c r="D115" s="4" t="s">
         <v>134</v>
       </c>
@@ -6442,7 +6446,7 @@
       <c r="K115" s="70">
         <v>0</v>
       </c>
-      <c r="L115" s="4"/>
+      <c r="L115" s="70"/>
       <c r="M115" s="4"/>
       <c r="N115" s="4"/>
       <c r="O115" s="17"/>
@@ -6456,8 +6460,8 @@
       <c r="W115" s="19"/>
     </row>
     <row r="116" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="107"/>
-      <c r="C116" s="90"/>
+      <c r="B116" s="90"/>
+      <c r="C116" s="102"/>
       <c r="D116" s="4" t="s">
         <v>135</v>
       </c>
@@ -6483,7 +6487,7 @@
       <c r="K116" s="70">
         <v>0</v>
       </c>
-      <c r="L116" s="4"/>
+      <c r="L116" s="70"/>
       <c r="M116" s="4"/>
       <c r="N116" s="4"/>
       <c r="O116" s="17"/>
@@ -6497,8 +6501,8 @@
       <c r="W116" s="19"/>
     </row>
     <row r="117" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="107"/>
-      <c r="C117" s="90" t="s">
+      <c r="B117" s="90"/>
+      <c r="C117" s="102" t="s">
         <v>126</v>
       </c>
       <c r="D117" s="4" t="s">
@@ -6526,7 +6530,7 @@
       <c r="K117" s="70">
         <v>0</v>
       </c>
-      <c r="L117" s="4"/>
+      <c r="L117" s="70"/>
       <c r="M117" s="4"/>
       <c r="N117" s="4"/>
       <c r="O117" s="17"/>
@@ -6540,8 +6544,8 @@
       <c r="W117" s="19"/>
     </row>
     <row r="118" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="107"/>
-      <c r="C118" s="90"/>
+      <c r="B118" s="90"/>
+      <c r="C118" s="102"/>
       <c r="D118" s="4" t="s">
         <v>133</v>
       </c>
@@ -6567,7 +6571,7 @@
       <c r="K118" s="70">
         <v>0</v>
       </c>
-      <c r="L118" s="4"/>
+      <c r="L118" s="70"/>
       <c r="M118" s="4"/>
       <c r="N118" s="4"/>
       <c r="O118" s="17"/>
@@ -6581,8 +6585,8 @@
       <c r="W118" s="19"/>
     </row>
     <row r="119" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="107"/>
-      <c r="C119" s="90"/>
+      <c r="B119" s="90"/>
+      <c r="C119" s="102"/>
       <c r="D119" s="4" t="s">
         <v>156</v>
       </c>
@@ -6596,7 +6600,7 @@
       </c>
       <c r="J119" s="70"/>
       <c r="K119" s="70"/>
-      <c r="L119" s="4"/>
+      <c r="L119" s="70"/>
       <c r="M119" s="4"/>
       <c r="N119" s="4"/>
       <c r="O119" s="17"/>
@@ -6610,8 +6614,8 @@
       <c r="W119" s="19"/>
     </row>
     <row r="120" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="107"/>
-      <c r="C120" s="90"/>
+      <c r="B120" s="90"/>
+      <c r="C120" s="102"/>
       <c r="D120" s="4" t="s">
         <v>134</v>
       </c>
@@ -6637,7 +6641,7 @@
       <c r="K120" s="70">
         <v>0</v>
       </c>
-      <c r="L120" s="4"/>
+      <c r="L120" s="70"/>
       <c r="M120" s="4"/>
       <c r="N120" s="4"/>
       <c r="O120" s="17"/>
@@ -6651,8 +6655,8 @@
       <c r="W120" s="19"/>
     </row>
     <row r="121" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="107"/>
-      <c r="C121" s="90"/>
+      <c r="B121" s="90"/>
+      <c r="C121" s="102"/>
       <c r="D121" s="4" t="s">
         <v>135</v>
       </c>
@@ -6678,7 +6682,7 @@
       <c r="K121" s="70">
         <v>0</v>
       </c>
-      <c r="L121" s="4"/>
+      <c r="L121" s="70"/>
       <c r="M121" s="4"/>
       <c r="N121" s="4"/>
       <c r="O121" s="17"/>
@@ -6692,8 +6696,8 @@
       <c r="W121" s="19"/>
     </row>
     <row r="122" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="107"/>
-      <c r="C122" s="90" t="s">
+      <c r="B122" s="90"/>
+      <c r="C122" s="102" t="s">
         <v>127</v>
       </c>
       <c r="D122" s="4" t="s">
@@ -6721,7 +6725,7 @@
       <c r="K122" s="70">
         <v>0</v>
       </c>
-      <c r="L122" s="4"/>
+      <c r="L122" s="70"/>
       <c r="M122" s="4"/>
       <c r="N122" s="4"/>
       <c r="O122" s="17"/>
@@ -6735,8 +6739,8 @@
       <c r="W122" s="19"/>
     </row>
     <row r="123" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="107"/>
-      <c r="C123" s="90"/>
+      <c r="B123" s="90"/>
+      <c r="C123" s="102"/>
       <c r="D123" s="4" t="s">
         <v>133</v>
       </c>
@@ -6762,7 +6766,7 @@
       <c r="K123" s="70">
         <v>0</v>
       </c>
-      <c r="L123" s="4"/>
+      <c r="L123" s="70"/>
       <c r="M123" s="4"/>
       <c r="N123" s="4"/>
       <c r="O123" s="17"/>
@@ -6776,8 +6780,8 @@
       <c r="W123" s="19"/>
     </row>
     <row r="124" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="107"/>
-      <c r="C124" s="90"/>
+      <c r="B124" s="90"/>
+      <c r="C124" s="102"/>
       <c r="D124" s="4" t="s">
         <v>156</v>
       </c>
@@ -6791,7 +6795,7 @@
       </c>
       <c r="J124" s="70"/>
       <c r="K124" s="70"/>
-      <c r="L124" s="4"/>
+      <c r="L124" s="70"/>
       <c r="M124" s="4"/>
       <c r="N124" s="4"/>
       <c r="O124" s="17"/>
@@ -6805,8 +6809,8 @@
       <c r="W124" s="19"/>
     </row>
     <row r="125" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="107"/>
-      <c r="C125" s="90"/>
+      <c r="B125" s="90"/>
+      <c r="C125" s="102"/>
       <c r="D125" s="4" t="s">
         <v>134</v>
       </c>
@@ -6832,7 +6836,7 @@
       <c r="K125" s="70">
         <v>0</v>
       </c>
-      <c r="L125" s="4"/>
+      <c r="L125" s="70"/>
       <c r="M125" s="4"/>
       <c r="N125" s="4"/>
       <c r="O125" s="17"/>
@@ -6846,8 +6850,8 @@
       <c r="W125" s="19"/>
     </row>
     <row r="126" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="107"/>
-      <c r="C126" s="90"/>
+      <c r="B126" s="90"/>
+      <c r="C126" s="102"/>
       <c r="D126" s="4" t="s">
         <v>135</v>
       </c>
@@ -6873,7 +6877,7 @@
       <c r="K126" s="70">
         <v>0</v>
       </c>
-      <c r="L126" s="4"/>
+      <c r="L126" s="70"/>
       <c r="M126" s="4"/>
       <c r="N126" s="4"/>
       <c r="O126" s="17"/>
@@ -6887,8 +6891,8 @@
       <c r="W126" s="19"/>
     </row>
     <row r="127" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="107"/>
-      <c r="C127" s="90" t="s">
+      <c r="B127" s="90"/>
+      <c r="C127" s="102" t="s">
         <v>128</v>
       </c>
       <c r="D127" s="4" t="s">
@@ -6916,7 +6920,7 @@
       <c r="K127" s="70">
         <v>0</v>
       </c>
-      <c r="L127" s="4"/>
+      <c r="L127" s="70"/>
       <c r="M127" s="4"/>
       <c r="N127" s="4"/>
       <c r="O127" s="17"/>
@@ -6930,8 +6934,8 @@
       <c r="W127" s="19"/>
     </row>
     <row r="128" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="107"/>
-      <c r="C128" s="90"/>
+      <c r="B128" s="90"/>
+      <c r="C128" s="102"/>
       <c r="D128" s="4" t="s">
         <v>133</v>
       </c>
@@ -6957,7 +6961,7 @@
       <c r="K128" s="70">
         <v>0</v>
       </c>
-      <c r="L128" s="4"/>
+      <c r="L128" s="70"/>
       <c r="M128" s="4"/>
       <c r="N128" s="4"/>
       <c r="O128" s="17"/>
@@ -6971,8 +6975,8 @@
       <c r="W128" s="19"/>
     </row>
     <row r="129" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="107"/>
-      <c r="C129" s="90"/>
+      <c r="B129" s="90"/>
+      <c r="C129" s="102"/>
       <c r="D129" s="4" t="s">
         <v>156</v>
       </c>
@@ -6986,7 +6990,7 @@
       </c>
       <c r="J129" s="70"/>
       <c r="K129" s="70"/>
-      <c r="L129" s="4"/>
+      <c r="L129" s="70"/>
       <c r="M129" s="4"/>
       <c r="N129" s="4"/>
       <c r="O129" s="17"/>
@@ -7000,8 +7004,8 @@
       <c r="W129" s="19"/>
     </row>
     <row r="130" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="107"/>
-      <c r="C130" s="90"/>
+      <c r="B130" s="90"/>
+      <c r="C130" s="102"/>
       <c r="D130" s="4" t="s">
         <v>134</v>
       </c>
@@ -7027,7 +7031,7 @@
       <c r="K130" s="70">
         <v>0</v>
       </c>
-      <c r="L130" s="4"/>
+      <c r="L130" s="70"/>
       <c r="M130" s="4"/>
       <c r="N130" s="4"/>
       <c r="O130" s="17"/>
@@ -7041,8 +7045,8 @@
       <c r="W130" s="19"/>
     </row>
     <row r="131" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="107"/>
-      <c r="C131" s="90"/>
+      <c r="B131" s="90"/>
+      <c r="C131" s="102"/>
       <c r="D131" s="4" t="s">
         <v>135</v>
       </c>
@@ -7068,7 +7072,7 @@
       <c r="K131" s="70">
         <v>0</v>
       </c>
-      <c r="L131" s="4"/>
+      <c r="L131" s="70"/>
       <c r="M131" s="4"/>
       <c r="N131" s="4"/>
       <c r="O131" s="17"/>
@@ -7082,8 +7086,8 @@
       <c r="W131" s="19"/>
     </row>
     <row r="132" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="107"/>
-      <c r="C132" s="90" t="s">
+      <c r="B132" s="90"/>
+      <c r="C132" s="102" t="s">
         <v>129</v>
       </c>
       <c r="D132" s="4" t="s">
@@ -7111,7 +7115,7 @@
       <c r="K132" s="70">
         <v>0</v>
       </c>
-      <c r="L132" s="4"/>
+      <c r="L132" s="70"/>
       <c r="M132" s="4"/>
       <c r="N132" s="4"/>
       <c r="O132" s="17"/>
@@ -7125,8 +7129,8 @@
       <c r="W132" s="19"/>
     </row>
     <row r="133" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="107"/>
-      <c r="C133" s="90"/>
+      <c r="B133" s="90"/>
+      <c r="C133" s="102"/>
       <c r="D133" s="4" t="s">
         <v>133</v>
       </c>
@@ -7152,7 +7156,7 @@
       <c r="K133" s="70">
         <v>0</v>
       </c>
-      <c r="L133" s="4"/>
+      <c r="L133" s="70"/>
       <c r="M133" s="4"/>
       <c r="N133" s="4"/>
       <c r="O133" s="17"/>
@@ -7166,8 +7170,8 @@
       <c r="W133" s="19"/>
     </row>
     <row r="134" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="107"/>
-      <c r="C134" s="90"/>
+      <c r="B134" s="90"/>
+      <c r="C134" s="102"/>
       <c r="D134" s="4" t="s">
         <v>156</v>
       </c>
@@ -7181,7 +7185,7 @@
       </c>
       <c r="J134" s="70"/>
       <c r="K134" s="70"/>
-      <c r="L134" s="4"/>
+      <c r="L134" s="70"/>
       <c r="M134" s="4"/>
       <c r="N134" s="4"/>
       <c r="O134" s="17"/>
@@ -7195,8 +7199,8 @@
       <c r="W134" s="19"/>
     </row>
     <row r="135" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="107"/>
-      <c r="C135" s="90"/>
+      <c r="B135" s="90"/>
+      <c r="C135" s="102"/>
       <c r="D135" s="4" t="s">
         <v>134</v>
       </c>
@@ -7222,7 +7226,7 @@
       <c r="K135" s="70">
         <v>0</v>
       </c>
-      <c r="L135" s="4"/>
+      <c r="L135" s="70"/>
       <c r="M135" s="4"/>
       <c r="N135" s="4"/>
       <c r="O135" s="17"/>
@@ -7236,8 +7240,8 @@
       <c r="W135" s="19"/>
     </row>
     <row r="136" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="107"/>
-      <c r="C136" s="90"/>
+      <c r="B136" s="90"/>
+      <c r="C136" s="102"/>
       <c r="D136" s="4" t="s">
         <v>135</v>
       </c>
@@ -7263,7 +7267,7 @@
       <c r="K136" s="70">
         <v>0</v>
       </c>
-      <c r="L136" s="4"/>
+      <c r="L136" s="70"/>
       <c r="M136" s="4"/>
       <c r="N136" s="4"/>
       <c r="O136" s="17"/>
@@ -7277,8 +7281,8 @@
       <c r="W136" s="19"/>
     </row>
     <row r="137" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="107"/>
-      <c r="C137" s="90" t="s">
+      <c r="B137" s="90"/>
+      <c r="C137" s="102" t="s">
         <v>130</v>
       </c>
       <c r="D137" s="4" t="s">
@@ -7306,7 +7310,7 @@
       <c r="K137" s="70">
         <v>0</v>
       </c>
-      <c r="L137" s="4"/>
+      <c r="L137" s="70"/>
       <c r="M137" s="4"/>
       <c r="N137" s="4"/>
       <c r="O137" s="17"/>
@@ -7320,8 +7324,8 @@
       <c r="W137" s="19"/>
     </row>
     <row r="138" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="107"/>
-      <c r="C138" s="90"/>
+      <c r="B138" s="90"/>
+      <c r="C138" s="102"/>
       <c r="D138" s="4" t="s">
         <v>133</v>
       </c>
@@ -7347,7 +7351,7 @@
       <c r="K138" s="70">
         <v>0</v>
       </c>
-      <c r="L138" s="4"/>
+      <c r="L138" s="70"/>
       <c r="M138" s="4"/>
       <c r="N138" s="4"/>
       <c r="O138" s="17"/>
@@ -7361,8 +7365,8 @@
       <c r="W138" s="19"/>
     </row>
     <row r="139" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="107"/>
-      <c r="C139" s="90"/>
+      <c r="B139" s="90"/>
+      <c r="C139" s="102"/>
       <c r="D139" s="4" t="s">
         <v>156</v>
       </c>
@@ -7376,7 +7380,7 @@
       </c>
       <c r="J139" s="70"/>
       <c r="K139" s="70"/>
-      <c r="L139" s="4"/>
+      <c r="L139" s="70"/>
       <c r="M139" s="4"/>
       <c r="N139" s="4"/>
       <c r="O139" s="17"/>
@@ -7390,8 +7394,8 @@
       <c r="W139" s="19"/>
     </row>
     <row r="140" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="107"/>
-      <c r="C140" s="90"/>
+      <c r="B140" s="90"/>
+      <c r="C140" s="102"/>
       <c r="D140" s="4" t="s">
         <v>134</v>
       </c>
@@ -7417,7 +7421,7 @@
       <c r="K140" s="70">
         <v>0</v>
       </c>
-      <c r="L140" s="4"/>
+      <c r="L140" s="70"/>
       <c r="M140" s="4"/>
       <c r="N140" s="4"/>
       <c r="O140" s="17"/>
@@ -7431,8 +7435,8 @@
       <c r="W140" s="19"/>
     </row>
     <row r="141" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="107"/>
-      <c r="C141" s="90"/>
+      <c r="B141" s="90"/>
+      <c r="C141" s="102"/>
       <c r="D141" s="4" t="s">
         <v>135</v>
       </c>
@@ -7458,7 +7462,7 @@
       <c r="K141" s="70">
         <v>0</v>
       </c>
-      <c r="L141" s="4"/>
+      <c r="L141" s="70"/>
       <c r="M141" s="4"/>
       <c r="N141" s="4"/>
       <c r="O141" s="17"/>
@@ -7472,8 +7476,8 @@
       <c r="W141" s="19"/>
     </row>
     <row r="142" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="107"/>
-      <c r="C142" s="90" t="s">
+      <c r="B142" s="90"/>
+      <c r="C142" s="102" t="s">
         <v>131</v>
       </c>
       <c r="D142" s="4" t="s">
@@ -7501,7 +7505,7 @@
       <c r="K142" s="70">
         <v>0</v>
       </c>
-      <c r="L142" s="4"/>
+      <c r="L142" s="70"/>
       <c r="M142" s="4"/>
       <c r="N142" s="4"/>
       <c r="O142" s="17"/>
@@ -7515,8 +7519,8 @@
       <c r="W142" s="19"/>
     </row>
     <row r="143" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="107"/>
-      <c r="C143" s="90"/>
+      <c r="B143" s="90"/>
+      <c r="C143" s="102"/>
       <c r="D143" s="4" t="s">
         <v>133</v>
       </c>
@@ -7542,7 +7546,7 @@
       <c r="K143" s="70">
         <v>0</v>
       </c>
-      <c r="L143" s="4"/>
+      <c r="L143" s="70"/>
       <c r="M143" s="4"/>
       <c r="N143" s="4"/>
       <c r="O143" s="17"/>
@@ -7556,8 +7560,8 @@
       <c r="W143" s="19"/>
     </row>
     <row r="144" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="107"/>
-      <c r="C144" s="90"/>
+      <c r="B144" s="90"/>
+      <c r="C144" s="102"/>
       <c r="D144" s="4" t="s">
         <v>156</v>
       </c>
@@ -7571,7 +7575,7 @@
       </c>
       <c r="J144" s="70"/>
       <c r="K144" s="70"/>
-      <c r="L144" s="4"/>
+      <c r="L144" s="70"/>
       <c r="M144" s="4"/>
       <c r="N144" s="4"/>
       <c r="O144" s="17"/>
@@ -7585,8 +7589,8 @@
       <c r="W144" s="19"/>
     </row>
     <row r="145" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="107"/>
-      <c r="C145" s="90"/>
+      <c r="B145" s="90"/>
+      <c r="C145" s="102"/>
       <c r="D145" s="4" t="s">
         <v>134</v>
       </c>
@@ -7603,7 +7607,7 @@
         <v>0.1</v>
       </c>
       <c r="I145" s="6">
-        <f t="shared" ref="I106:I145" si="4">SUM(J145:W145)</f>
+        <f t="shared" ref="I145" si="4">SUM(J145:W145)</f>
         <v>0</v>
       </c>
       <c r="J145" s="70">
@@ -7612,7 +7616,7 @@
       <c r="K145" s="70">
         <v>0</v>
       </c>
-      <c r="L145" s="4"/>
+      <c r="L145" s="70"/>
       <c r="M145" s="4"/>
       <c r="N145" s="4"/>
       <c r="O145" s="17"/>
@@ -7626,8 +7630,8 @@
       <c r="W145" s="19"/>
     </row>
     <row r="146" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B146" s="109"/>
-      <c r="C146" s="110"/>
+      <c r="B146" s="91"/>
+      <c r="C146" s="105"/>
       <c r="D146" s="24" t="s">
         <v>135</v>
       </c>
@@ -7653,7 +7657,7 @@
       <c r="K146" s="71">
         <v>0</v>
       </c>
-      <c r="L146" s="24"/>
+      <c r="L146" s="71"/>
       <c r="M146" s="24"/>
       <c r="N146" s="24"/>
       <c r="O146" s="22"/>
@@ -7667,7 +7671,7 @@
       <c r="W146" s="25"/>
     </row>
     <row r="147" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B147" s="106" t="s">
+      <c r="B147" s="89" t="s">
         <v>83</v>
       </c>
       <c r="C147" s="78" t="s">
@@ -7696,7 +7700,7 @@
       <c r="K147" s="69">
         <v>0</v>
       </c>
-      <c r="L147" s="39"/>
+      <c r="L147" s="69"/>
       <c r="M147" s="39"/>
       <c r="N147" s="39"/>
       <c r="O147" s="51"/>
@@ -7710,7 +7714,7 @@
       <c r="W147" s="52"/>
     </row>
     <row r="148" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="107"/>
+      <c r="B148" s="90"/>
       <c r="C148" s="33" t="s">
         <v>89</v>
       </c>
@@ -7737,7 +7741,7 @@
       <c r="K148" s="70">
         <v>0</v>
       </c>
-      <c r="L148" s="4"/>
+      <c r="L148" s="70"/>
       <c r="M148" s="4"/>
       <c r="N148" s="4"/>
       <c r="O148" s="17"/>
@@ -7751,7 +7755,7 @@
       <c r="W148" s="19"/>
     </row>
     <row r="149" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="107"/>
+      <c r="B149" s="90"/>
       <c r="C149" s="33" t="s">
         <v>90</v>
       </c>
@@ -7778,7 +7782,7 @@
       <c r="K149" s="70">
         <v>0</v>
       </c>
-      <c r="L149" s="4"/>
+      <c r="L149" s="70"/>
       <c r="M149" s="4"/>
       <c r="N149" s="4"/>
       <c r="O149" s="17"/>
@@ -7792,7 +7796,7 @@
       <c r="W149" s="19"/>
     </row>
     <row r="150" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="107"/>
+      <c r="B150" s="90"/>
       <c r="C150" s="33" t="s">
         <v>91</v>
       </c>
@@ -7819,7 +7823,7 @@
       <c r="K150" s="70">
         <v>0</v>
       </c>
-      <c r="L150" s="4"/>
+      <c r="L150" s="70"/>
       <c r="M150" s="4"/>
       <c r="N150" s="4"/>
       <c r="O150" s="17"/>
@@ -7833,7 +7837,7 @@
       <c r="W150" s="19"/>
     </row>
     <row r="151" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="107"/>
+      <c r="B151" s="90"/>
       <c r="C151" s="33" t="s">
         <v>142</v>
       </c>
@@ -7860,7 +7864,7 @@
       <c r="K151" s="70">
         <v>0</v>
       </c>
-      <c r="L151" s="4"/>
+      <c r="L151" s="70"/>
       <c r="M151" s="4"/>
       <c r="N151" s="4"/>
       <c r="O151" s="17"/>
@@ -7874,7 +7878,7 @@
       <c r="W151" s="19"/>
     </row>
     <row r="152" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="107"/>
+      <c r="B152" s="90"/>
       <c r="C152" s="33" t="s">
         <v>139</v>
       </c>
@@ -7901,7 +7905,7 @@
       <c r="K152" s="70">
         <v>0</v>
       </c>
-      <c r="L152" s="4"/>
+      <c r="L152" s="70"/>
       <c r="M152" s="4"/>
       <c r="N152" s="4"/>
       <c r="O152" s="17"/>
@@ -7915,7 +7919,7 @@
       <c r="W152" s="19"/>
     </row>
     <row r="153" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="107"/>
+      <c r="B153" s="90"/>
       <c r="C153" s="33" t="s">
         <v>141</v>
       </c>
@@ -7942,7 +7946,7 @@
       <c r="K153" s="70">
         <v>0</v>
       </c>
-      <c r="L153" s="4"/>
+      <c r="L153" s="70"/>
       <c r="M153" s="4"/>
       <c r="N153" s="4"/>
       <c r="O153" s="17"/>
@@ -7956,7 +7960,7 @@
       <c r="W153" s="19"/>
     </row>
     <row r="154" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="107"/>
+      <c r="B154" s="90"/>
       <c r="C154" s="33" t="s">
         <v>140</v>
       </c>
@@ -7983,7 +7987,7 @@
       <c r="K154" s="70">
         <v>0</v>
       </c>
-      <c r="L154" s="4"/>
+      <c r="L154" s="70"/>
       <c r="M154" s="4"/>
       <c r="N154" s="4"/>
       <c r="O154" s="17"/>
@@ -7997,7 +8001,7 @@
       <c r="W154" s="19"/>
     </row>
     <row r="155" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="107"/>
+      <c r="B155" s="90"/>
       <c r="C155" s="33" t="s">
         <v>92</v>
       </c>
@@ -8024,7 +8028,7 @@
       <c r="K155" s="70">
         <v>0</v>
       </c>
-      <c r="L155" s="4"/>
+      <c r="L155" s="70"/>
       <c r="M155" s="4"/>
       <c r="N155" s="4"/>
       <c r="O155" s="17"/>
@@ -8038,7 +8042,7 @@
       <c r="W155" s="19"/>
     </row>
     <row r="156" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="107"/>
+      <c r="B156" s="90"/>
       <c r="C156" s="33" t="s">
         <v>93</v>
       </c>
@@ -8065,7 +8069,7 @@
       <c r="K156" s="70">
         <v>0</v>
       </c>
-      <c r="L156" s="4"/>
+      <c r="L156" s="70"/>
       <c r="M156" s="4"/>
       <c r="N156" s="4"/>
       <c r="O156" s="17"/>
@@ -8079,7 +8083,7 @@
       <c r="W156" s="19"/>
     </row>
     <row r="157" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="107"/>
+      <c r="B157" s="90"/>
       <c r="C157" s="33" t="s">
         <v>94</v>
       </c>
@@ -8106,7 +8110,7 @@
       <c r="K157" s="70">
         <v>0</v>
       </c>
-      <c r="L157" s="4"/>
+      <c r="L157" s="70"/>
       <c r="M157" s="4"/>
       <c r="N157" s="4"/>
       <c r="O157" s="17"/>
@@ -8120,7 +8124,7 @@
       <c r="W157" s="19"/>
     </row>
     <row r="158" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="107"/>
+      <c r="B158" s="90"/>
       <c r="C158" s="33" t="s">
         <v>98</v>
       </c>
@@ -8147,7 +8151,7 @@
       <c r="K158" s="70">
         <v>0</v>
       </c>
-      <c r="L158" s="4"/>
+      <c r="L158" s="70"/>
       <c r="M158" s="4"/>
       <c r="N158" s="4"/>
       <c r="O158" s="17"/>
@@ -8161,7 +8165,7 @@
       <c r="W158" s="19"/>
     </row>
     <row r="159" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B159" s="109"/>
+      <c r="B159" s="91"/>
       <c r="C159" s="61" t="s">
         <v>99</v>
       </c>
@@ -8188,7 +8192,7 @@
       <c r="K159" s="71">
         <v>0</v>
       </c>
-      <c r="L159" s="24"/>
+      <c r="L159" s="71"/>
       <c r="M159" s="24"/>
       <c r="N159" s="24"/>
       <c r="O159" s="22"/>
@@ -8202,7 +8206,7 @@
       <c r="W159" s="25"/>
     </row>
     <row r="160" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="106" t="s">
+      <c r="B160" s="89" t="s">
         <v>143</v>
       </c>
       <c r="C160" s="60" t="s">
@@ -8231,7 +8235,7 @@
       <c r="K160" s="69">
         <v>0</v>
       </c>
-      <c r="L160" s="39"/>
+      <c r="L160" s="69"/>
       <c r="M160" s="39"/>
       <c r="N160" s="39"/>
       <c r="O160" s="51"/>
@@ -8245,7 +8249,7 @@
       <c r="W160" s="52"/>
     </row>
     <row r="161" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="107"/>
+      <c r="B161" s="90"/>
       <c r="C161" s="59" t="s">
         <v>144</v>
       </c>
@@ -8272,7 +8276,7 @@
       <c r="K161" s="70">
         <v>0</v>
       </c>
-      <c r="L161" s="4"/>
+      <c r="L161" s="70"/>
       <c r="M161" s="4"/>
       <c r="N161" s="4"/>
       <c r="O161" s="17"/>
@@ -8286,7 +8290,7 @@
       <c r="W161" s="19"/>
     </row>
     <row r="162" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B162" s="109"/>
+      <c r="B162" s="91"/>
       <c r="C162" s="61" t="s">
         <v>145</v>
       </c>
@@ -8313,7 +8317,7 @@
       <c r="K162" s="71">
         <v>0</v>
       </c>
-      <c r="L162" s="24"/>
+      <c r="L162" s="71"/>
       <c r="M162" s="24"/>
       <c r="N162" s="24"/>
       <c r="O162" s="22"/>
@@ -8327,7 +8331,7 @@
       <c r="W162" s="25"/>
     </row>
     <row r="163" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="106" t="s">
+      <c r="B163" s="89" t="s">
         <v>148</v>
       </c>
       <c r="C163" s="60" t="s">
@@ -8352,7 +8356,7 @@
       </c>
       <c r="J163" s="69"/>
       <c r="K163" s="69"/>
-      <c r="L163" s="39"/>
+      <c r="L163" s="69"/>
       <c r="M163" s="39"/>
       <c r="N163" s="39"/>
       <c r="O163" s="51"/>
@@ -8366,7 +8370,7 @@
       <c r="W163" s="52"/>
     </row>
     <row r="164" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="107"/>
+      <c r="B164" s="90"/>
       <c r="C164" s="59" t="s">
         <v>150</v>
       </c>
@@ -8389,7 +8393,7 @@
       </c>
       <c r="J164" s="70"/>
       <c r="K164" s="70"/>
-      <c r="L164" s="4"/>
+      <c r="L164" s="70"/>
       <c r="M164" s="4"/>
       <c r="N164" s="4"/>
       <c r="O164" s="17"/>
@@ -8403,7 +8407,7 @@
       <c r="W164" s="19"/>
     </row>
     <row r="165" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="107"/>
+      <c r="B165" s="90"/>
       <c r="C165" s="59" t="s">
         <v>151</v>
       </c>
@@ -8426,7 +8430,7 @@
       </c>
       <c r="J165" s="70"/>
       <c r="K165" s="70"/>
-      <c r="L165" s="4"/>
+      <c r="L165" s="70"/>
       <c r="M165" s="4"/>
       <c r="N165" s="4"/>
       <c r="O165" s="17"/>
@@ -8440,7 +8444,7 @@
       <c r="W165" s="19"/>
     </row>
     <row r="166" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B166" s="107"/>
+      <c r="B166" s="90"/>
       <c r="C166" s="59" t="s">
         <v>152</v>
       </c>
@@ -8463,7 +8467,7 @@
       </c>
       <c r="J166" s="70"/>
       <c r="K166" s="70"/>
-      <c r="L166" s="4"/>
+      <c r="L166" s="70"/>
       <c r="M166" s="4"/>
       <c r="N166" s="4"/>
       <c r="O166" s="17"/>
@@ -8477,7 +8481,7 @@
       <c r="W166" s="19"/>
     </row>
     <row r="167" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B167" s="107"/>
+      <c r="B167" s="90"/>
       <c r="C167" s="59" t="s">
         <v>153</v>
       </c>
@@ -8500,7 +8504,7 @@
       </c>
       <c r="J167" s="70"/>
       <c r="K167" s="70"/>
-      <c r="L167" s="4"/>
+      <c r="L167" s="70"/>
       <c r="M167" s="4"/>
       <c r="N167" s="4"/>
       <c r="O167" s="17"/>
@@ -8514,7 +8518,7 @@
       <c r="W167" s="19"/>
     </row>
     <row r="168" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B168" s="107"/>
+      <c r="B168" s="90"/>
       <c r="C168" s="59" t="s">
         <v>154</v>
       </c>
@@ -8537,7 +8541,7 @@
       </c>
       <c r="J168" s="70"/>
       <c r="K168" s="70"/>
-      <c r="L168" s="4"/>
+      <c r="L168" s="70"/>
       <c r="M168" s="4"/>
       <c r="N168" s="4"/>
       <c r="O168" s="17"/>
@@ -8551,7 +8555,7 @@
       <c r="W168" s="19"/>
     </row>
     <row r="169" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B169" s="109"/>
+      <c r="B169" s="91"/>
       <c r="C169" s="61" t="s">
         <v>155</v>
       </c>
@@ -8574,7 +8578,7 @@
       </c>
       <c r="J169" s="71"/>
       <c r="K169" s="71"/>
-      <c r="L169" s="24"/>
+      <c r="L169" s="71"/>
       <c r="M169" s="24"/>
       <c r="N169" s="24"/>
       <c r="O169" s="22"/>
@@ -8588,7 +8592,7 @@
       <c r="W169" s="25"/>
     </row>
     <row r="170" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B170" s="106" t="s">
+      <c r="B170" s="89" t="s">
         <v>18</v>
       </c>
       <c r="C170" s="54" t="s">
@@ -8617,7 +8621,7 @@
       <c r="K170" s="69">
         <v>0</v>
       </c>
-      <c r="L170" s="39"/>
+      <c r="L170" s="69"/>
       <c r="M170" s="39"/>
       <c r="N170" s="39"/>
       <c r="O170" s="51"/>
@@ -8631,7 +8635,7 @@
       <c r="W170" s="52"/>
     </row>
     <row r="171" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B171" s="107"/>
+      <c r="B171" s="90"/>
       <c r="C171" s="33" t="s">
         <v>137</v>
       </c>
@@ -8658,7 +8662,7 @@
       <c r="K171" s="70">
         <v>0</v>
       </c>
-      <c r="L171" s="4"/>
+      <c r="L171" s="70"/>
       <c r="M171" s="4"/>
       <c r="N171" s="4"/>
       <c r="O171" s="17"/>
@@ -8672,7 +8676,7 @@
       <c r="W171" s="19"/>
     </row>
     <row r="172" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="107"/>
+      <c r="B172" s="90"/>
       <c r="C172" s="33" t="s">
         <v>138</v>
       </c>
@@ -8699,7 +8703,7 @@
       <c r="K172" s="70">
         <v>0</v>
       </c>
-      <c r="L172" s="4"/>
+      <c r="L172" s="70"/>
       <c r="M172" s="4"/>
       <c r="N172" s="4"/>
       <c r="O172" s="17"/>
@@ -8713,7 +8717,7 @@
       <c r="W172" s="19"/>
     </row>
     <row r="173" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B173" s="107"/>
+      <c r="B173" s="90"/>
       <c r="C173" s="33" t="s">
         <v>146</v>
       </c>
@@ -8740,7 +8744,7 @@
       <c r="K173" s="70">
         <v>0</v>
       </c>
-      <c r="L173" s="4"/>
+      <c r="L173" s="70"/>
       <c r="M173" s="4"/>
       <c r="N173" s="4"/>
       <c r="O173" s="17"/>
@@ -8754,7 +8758,7 @@
       <c r="W173" s="19"/>
     </row>
     <row r="174" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="107"/>
+      <c r="B174" s="90"/>
       <c r="C174" s="33" t="s">
         <v>84</v>
       </c>
@@ -8781,7 +8785,7 @@
       <c r="K174" s="70">
         <v>0</v>
       </c>
-      <c r="L174" s="4"/>
+      <c r="L174" s="70"/>
       <c r="M174" s="4"/>
       <c r="N174" s="4"/>
       <c r="O174" s="17"/>
@@ -8795,7 +8799,7 @@
       <c r="W174" s="19"/>
     </row>
     <row r="175" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="107"/>
+      <c r="B175" s="90"/>
       <c r="C175" s="33" t="s">
         <v>85</v>
       </c>
@@ -8822,7 +8826,7 @@
       <c r="K175" s="70">
         <v>0</v>
       </c>
-      <c r="L175" s="4"/>
+      <c r="L175" s="70"/>
       <c r="M175" s="4"/>
       <c r="N175" s="4"/>
       <c r="O175" s="17"/>
@@ -8836,7 +8840,7 @@
       <c r="W175" s="19"/>
     </row>
     <row r="176" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="107"/>
+      <c r="B176" s="90"/>
       <c r="C176" s="33" t="s">
         <v>87</v>
       </c>
@@ -8863,7 +8867,7 @@
       <c r="K176" s="70">
         <v>0</v>
       </c>
-      <c r="L176" s="4"/>
+      <c r="L176" s="70"/>
       <c r="M176" s="4"/>
       <c r="N176" s="4"/>
       <c r="O176" s="17"/>
@@ -8877,7 +8881,7 @@
       <c r="W176" s="19"/>
     </row>
     <row r="177" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B177" s="107"/>
+      <c r="B177" s="90"/>
       <c r="C177" s="33" t="s">
         <v>86</v>
       </c>
@@ -8904,7 +8908,7 @@
       <c r="K177" s="70">
         <v>0</v>
       </c>
-      <c r="L177" s="4"/>
+      <c r="L177" s="70"/>
       <c r="M177" s="4"/>
       <c r="N177" s="4"/>
       <c r="O177" s="17"/>
@@ -8918,7 +8922,7 @@
       <c r="W177" s="19"/>
     </row>
     <row r="178" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B178" s="107"/>
+      <c r="B178" s="90"/>
       <c r="C178" s="33" t="s">
         <v>104</v>
       </c>
@@ -8945,7 +8949,7 @@
       <c r="K178" s="70">
         <v>0</v>
       </c>
-      <c r="L178" s="4"/>
+      <c r="L178" s="70"/>
       <c r="M178" s="4"/>
       <c r="N178" s="4"/>
       <c r="O178" s="17"/>
@@ -8959,7 +8963,7 @@
       <c r="W178" s="19"/>
     </row>
     <row r="179" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B179" s="107"/>
+      <c r="B179" s="90"/>
       <c r="C179" s="33" t="s">
         <v>136</v>
       </c>
@@ -8986,7 +8990,7 @@
       <c r="K179" s="80">
         <v>1.85</v>
       </c>
-      <c r="L179" s="4"/>
+      <c r="L179" s="70"/>
       <c r="M179" s="4"/>
       <c r="N179" s="4"/>
       <c r="O179" s="17"/>
@@ -9000,7 +9004,7 @@
       <c r="W179" s="19"/>
     </row>
     <row r="180" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B180" s="107"/>
+      <c r="B180" s="90"/>
       <c r="C180" s="33" t="s">
         <v>105</v>
       </c>
@@ -9027,7 +9031,7 @@
       <c r="K180" s="70">
         <v>0</v>
       </c>
-      <c r="L180" s="4"/>
+      <c r="L180" s="70"/>
       <c r="M180" s="4"/>
       <c r="N180" s="4"/>
       <c r="O180" s="17"/>
@@ -9041,7 +9045,7 @@
       <c r="W180" s="19"/>
     </row>
     <row r="181" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B181" s="109"/>
+      <c r="B181" s="91"/>
       <c r="C181" s="61" t="s">
         <v>100</v>
       </c>
@@ -9068,7 +9072,7 @@
       <c r="K181" s="71">
         <v>0</v>
       </c>
-      <c r="L181" s="24"/>
+      <c r="L181" s="71"/>
       <c r="M181" s="24"/>
       <c r="N181" s="24"/>
       <c r="O181" s="22"/>
@@ -9082,76 +9086,76 @@
       <c r="W181" s="25"/>
     </row>
     <row r="182" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B182" s="111" t="s">
+      <c r="B182" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="C182" s="112"/>
-      <c r="D182" s="113"/>
-      <c r="E182" s="113"/>
-      <c r="F182" s="113"/>
-      <c r="G182" s="114"/>
+      <c r="C182" s="99"/>
+      <c r="D182" s="100"/>
+      <c r="E182" s="100"/>
+      <c r="F182" s="100"/>
+      <c r="G182" s="101"/>
       <c r="H182" s="36">
-        <f>SUM(H4:H181)</f>
-        <v>89.69999999999996</v>
+        <f t="shared" ref="H182:W182" si="6">SUM(H4:H181)</f>
+        <v>96.499999999999829</v>
       </c>
       <c r="I182" s="23">
-        <f>SUM(I4:I181)</f>
-        <v>5.5563000000000002</v>
+        <f t="shared" si="6"/>
+        <v>9.0062999999999995</v>
       </c>
       <c r="J182" s="23">
-        <f>SUM(J4:J181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K182" s="23">
-        <f>SUM(K4:K181)</f>
+        <f t="shared" si="6"/>
         <v>4.0533000000000001</v>
       </c>
       <c r="L182" s="23">
-        <f>SUM(L4:L181)</f>
-        <v>1.5029999999999999</v>
+        <f t="shared" si="6"/>
+        <v>2.0030000000000001</v>
       </c>
       <c r="M182" s="23">
-        <f>SUM(M4:M181)</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>2.95</v>
       </c>
       <c r="N182" s="23">
-        <f>SUM(N4:N181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O182" s="23">
-        <f>SUM(O4:O181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P182" s="23">
-        <f>SUM(P4:P181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q182" s="23">
-        <f>SUM(Q4:Q181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R182" s="23">
-        <f>SUM(R4:R181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S182" s="23">
-        <f>SUM(S4:S181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T182" s="23">
-        <f>SUM(T4:T181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U182" s="23">
-        <f>SUM(U4:U181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V182" s="23">
-        <f>SUM(V4:V181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="W182" s="30">
-        <f>SUM(W4:W181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9164,22 +9168,22 @@
       <c r="G183" s="2"/>
       <c r="H183" s="2"/>
       <c r="I183" s="2"/>
-      <c r="J183" s="91" t="s">
+      <c r="J183" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="K183" s="92"/>
-      <c r="L183" s="92"/>
-      <c r="M183" s="92"/>
-      <c r="N183" s="92"/>
-      <c r="O183" s="92"/>
-      <c r="P183" s="92"/>
-      <c r="Q183" s="92"/>
-      <c r="R183" s="92"/>
-      <c r="S183" s="92"/>
-      <c r="T183" s="92"/>
-      <c r="U183" s="92"/>
-      <c r="V183" s="92"/>
-      <c r="W183" s="93"/>
+      <c r="K183" s="103"/>
+      <c r="L183" s="103"/>
+      <c r="M183" s="103"/>
+      <c r="N183" s="103"/>
+      <c r="O183" s="103"/>
+      <c r="P183" s="103"/>
+      <c r="Q183" s="103"/>
+      <c r="R183" s="103"/>
+      <c r="S183" s="103"/>
+      <c r="T183" s="103"/>
+      <c r="U183" s="103"/>
+      <c r="V183" s="103"/>
+      <c r="W183" s="104"/>
     </row>
     <row r="184" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B184" s="2"/>
@@ -9203,29 +9207,29 @@
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
-      <c r="H185" s="102" t="s">
+      <c r="H185" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="I185" s="103"/>
+      <c r="I185" s="93"/>
       <c r="J185" s="9">
         <f>H182-J182</f>
-        <v>89.69999999999996</v>
+        <v>96.499999999999829</v>
       </c>
       <c r="K185" s="9">
         <f>J185-K182</f>
-        <v>85.646699999999953</v>
+        <v>92.446699999999822</v>
       </c>
       <c r="L185" s="9">
         <f>K185-L182</f>
-        <v>84.143699999999953</v>
+        <v>90.443699999999822</v>
       </c>
       <c r="M185" s="9">
         <f>L185-M182</f>
-        <v>84.143699999999953</v>
+        <v>87.493699999999819</v>
       </c>
       <c r="N185" s="10">
         <f>M185-N182</f>
-        <v>84.143699999999953</v>
+        <v>87.493699999999819</v>
       </c>
     </row>
     <row r="186" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9249,18 +9253,18 @@
       <c r="D187" s="3"/>
       <c r="E187" s="3"/>
       <c r="F187" s="3"/>
-      <c r="H187" s="91" t="s">
+      <c r="H187" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="I187" s="104"/>
-      <c r="J187" s="103">
+      <c r="I187" s="95"/>
+      <c r="J187" s="93">
         <f>H182-I182</f>
-        <v>84.143699999999967</v>
-      </c>
-      <c r="K187" s="103"/>
-      <c r="L187" s="103"/>
-      <c r="M187" s="103"/>
-      <c r="N187" s="105"/>
+        <v>87.493699999999833</v>
+      </c>
+      <c r="K187" s="93"/>
+      <c r="L187" s="93"/>
+      <c r="M187" s="93"/>
+      <c r="N187" s="96"/>
     </row>
     <row r="188" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B188" s="3"/>
@@ -9364,6 +9368,24 @@
     <row r="206" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C132:C136"/>
+    <mergeCell ref="C122:C126"/>
+    <mergeCell ref="C112:C116"/>
+    <mergeCell ref="C107:C111"/>
+    <mergeCell ref="C97:C101"/>
+    <mergeCell ref="C117:C121"/>
+    <mergeCell ref="C127:C131"/>
+    <mergeCell ref="C82:C86"/>
+    <mergeCell ref="J2:W2"/>
+    <mergeCell ref="B62:B71"/>
+    <mergeCell ref="C55:C61"/>
+    <mergeCell ref="C15:C54"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C72:C76"/>
+    <mergeCell ref="C77:C81"/>
     <mergeCell ref="B163:B169"/>
     <mergeCell ref="H185:I185"/>
     <mergeCell ref="H187:I187"/>
@@ -9380,24 +9402,6 @@
     <mergeCell ref="C142:C146"/>
     <mergeCell ref="C92:C96"/>
     <mergeCell ref="C87:C91"/>
-    <mergeCell ref="C82:C86"/>
-    <mergeCell ref="J2:W2"/>
-    <mergeCell ref="B62:B71"/>
-    <mergeCell ref="C55:C61"/>
-    <mergeCell ref="C15:C54"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="C72:C76"/>
-    <mergeCell ref="C77:C81"/>
-    <mergeCell ref="C132:C136"/>
-    <mergeCell ref="C122:C126"/>
-    <mergeCell ref="C112:C116"/>
-    <mergeCell ref="C107:C111"/>
-    <mergeCell ref="C97:C101"/>
-    <mergeCell ref="C117:C121"/>
-    <mergeCell ref="C127:C131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Calculadas horas por individuo (Estimadas, reales y restantes)
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
+++ b/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="163">
   <si>
     <t>Subtarea</t>
   </si>
@@ -492,6 +492,24 @@
   </si>
   <si>
     <t>Implementar entrada secreta (Opertura)</t>
+  </si>
+  <si>
+    <t>Horas David</t>
+  </si>
+  <si>
+    <t>Horas Alex</t>
+  </si>
+  <si>
+    <t>Horas Carlos</t>
+  </si>
+  <si>
+    <t>Reales</t>
+  </si>
+  <si>
+    <t>Estimadas</t>
+  </si>
+  <si>
+    <t>Restantes</t>
   </si>
 </sst>
 </file>
@@ -621,7 +639,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1009,11 +1027,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1239,25 +1270,55 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1296,35 +1357,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1358,6 +1398,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1415,11 +1456,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="442743984"/>
-        <c:axId val="442742352"/>
+        <c:axId val="-1516873760"/>
+        <c:axId val="-1516873216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="442743984"/>
+        <c:axId val="-1516873760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1428,7 +1469,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442742352"/>
+        <c:crossAx val="-1516873216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1436,7 +1477,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="442742352"/>
+        <c:axId val="-1516873216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,13 +1488,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442743984"/>
+        <c:crossAx val="-1516873760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1792,8 +1834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E190" sqref="E190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1820,22 +1862,22 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="90" t="s">
+      <c r="J2" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="91"/>
-      <c r="S2" s="91"/>
-      <c r="T2" s="91"/>
-      <c r="U2" s="91"/>
-      <c r="V2" s="91"/>
-      <c r="W2" s="92"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="103"/>
+      <c r="P2" s="103"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="103"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="103"/>
+      <c r="V2" s="103"/>
+      <c r="W2" s="104"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="56" t="s">
@@ -1906,7 +1948,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="114" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="37" t="s">
@@ -1949,7 +1991,7 @@
       <c r="W4" s="44"/>
     </row>
     <row r="5" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="105"/>
+      <c r="B5" s="115"/>
       <c r="C5" s="35" t="s">
         <v>101</v>
       </c>
@@ -1990,7 +2032,7 @@
       <c r="W5" s="19"/>
     </row>
     <row r="6" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="105"/>
+      <c r="B6" s="115"/>
       <c r="C6" s="35" t="s">
         <v>102</v>
       </c>
@@ -2031,7 +2073,7 @@
       <c r="W6" s="19"/>
     </row>
     <row r="7" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="105"/>
+      <c r="B7" s="115"/>
       <c r="C7" s="35" t="s">
         <v>103</v>
       </c>
@@ -2072,7 +2114,7 @@
       <c r="W7" s="19"/>
     </row>
     <row r="8" spans="1:23" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="106"/>
+      <c r="B8" s="116"/>
       <c r="C8" s="45" t="s">
         <v>111</v>
       </c>
@@ -2113,7 +2155,7 @@
       <c r="W8" s="25"/>
     </row>
     <row r="9" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="104" t="s">
+      <c r="B9" s="114" t="s">
         <v>106</v>
       </c>
       <c r="C9" s="48" t="s">
@@ -2156,7 +2198,7 @@
       <c r="W9" s="86"/>
     </row>
     <row r="10" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="105"/>
+      <c r="B10" s="115"/>
       <c r="C10" s="34" t="s">
         <v>107</v>
       </c>
@@ -2197,7 +2239,7 @@
       <c r="W10" s="19"/>
     </row>
     <row r="11" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="105"/>
+      <c r="B11" s="115"/>
       <c r="C11" s="83" t="s">
         <v>112</v>
       </c>
@@ -2238,7 +2280,7 @@
       <c r="W11" s="19"/>
     </row>
     <row r="12" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="105"/>
+      <c r="B12" s="115"/>
       <c r="C12" s="83" t="s">
         <v>113</v>
       </c>
@@ -2303,7 +2345,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="106"/>
+      <c r="B13" s="116"/>
       <c r="C13" s="53" t="s">
         <v>97</v>
       </c>
@@ -2346,7 +2388,7 @@
       <c r="W13" s="25"/>
     </row>
     <row r="14" spans="1:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B14" s="93" t="s">
+      <c r="B14" s="89" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="54" t="s">
@@ -2391,8 +2433,8 @@
       <c r="W14" s="52"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B15" s="94"/>
-      <c r="C15" s="98" t="s">
+      <c r="B15" s="90"/>
+      <c r="C15" s="108" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -2438,8 +2480,8 @@
       <c r="W15" s="19"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B16" s="94"/>
-      <c r="C16" s="99"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="109"/>
       <c r="D16" s="4" t="s">
         <v>20</v>
       </c>
@@ -2479,8 +2521,8 @@
       <c r="W16" s="19"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B17" s="94"/>
-      <c r="C17" s="99"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="109"/>
       <c r="D17" s="4" t="s">
         <v>21</v>
       </c>
@@ -2520,8 +2562,8 @@
       <c r="W17" s="19"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B18" s="94"/>
-      <c r="C18" s="99"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="109"/>
       <c r="D18" s="4" t="s">
         <v>22</v>
       </c>
@@ -2561,8 +2603,8 @@
       <c r="W18" s="19"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B19" s="94"/>
-      <c r="C19" s="99"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="109"/>
       <c r="D19" s="4" t="s">
         <v>23</v>
       </c>
@@ -2602,8 +2644,8 @@
       <c r="W19" s="19"/>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B20" s="94"/>
-      <c r="C20" s="99"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="109"/>
       <c r="D20" s="4" t="s">
         <v>24</v>
       </c>
@@ -2643,8 +2685,8 @@
       <c r="W20" s="19"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B21" s="94"/>
-      <c r="C21" s="99"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="109"/>
       <c r="D21" s="32" t="s">
         <v>36</v>
       </c>
@@ -2684,8 +2726,8 @@
       <c r="W21" s="19"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B22" s="94"/>
-      <c r="C22" s="99"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="109"/>
       <c r="D22" s="32" t="s">
         <v>37</v>
       </c>
@@ -2725,8 +2767,8 @@
       <c r="W22" s="19"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B23" s="94"/>
-      <c r="C23" s="99"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="109"/>
       <c r="D23" s="32" t="s">
         <v>38</v>
       </c>
@@ -2766,8 +2808,8 @@
       <c r="W23" s="19"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B24" s="94"/>
-      <c r="C24" s="99"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="109"/>
       <c r="D24" s="32" t="s">
         <v>39</v>
       </c>
@@ -2807,8 +2849,8 @@
       <c r="W24" s="19"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B25" s="94"/>
-      <c r="C25" s="99"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="109"/>
       <c r="D25" s="32" t="s">
         <v>40</v>
       </c>
@@ -2848,8 +2890,8 @@
       <c r="W25" s="19"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B26" s="94"/>
-      <c r="C26" s="99"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="109"/>
       <c r="D26" s="32" t="s">
         <v>41</v>
       </c>
@@ -2889,8 +2931,8 @@
       <c r="W26" s="19"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B27" s="94"/>
-      <c r="C27" s="99"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="109"/>
       <c r="D27" s="32" t="s">
         <v>42</v>
       </c>
@@ -2930,8 +2972,8 @@
       <c r="W27" s="19"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B28" s="94"/>
-      <c r="C28" s="99"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="109"/>
       <c r="D28" s="32" t="s">
         <v>43</v>
       </c>
@@ -2971,8 +3013,8 @@
       <c r="W28" s="19"/>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B29" s="94"/>
-      <c r="C29" s="99"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="109"/>
       <c r="D29" s="32" t="s">
         <v>44</v>
       </c>
@@ -3012,8 +3054,8 @@
       <c r="W29" s="19"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B30" s="94"/>
-      <c r="C30" s="99"/>
+      <c r="B30" s="90"/>
+      <c r="C30" s="109"/>
       <c r="D30" s="32" t="s">
         <v>45</v>
       </c>
@@ -3053,8 +3095,8 @@
       <c r="W30" s="19"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B31" s="94"/>
-      <c r="C31" s="99"/>
+      <c r="B31" s="90"/>
+      <c r="C31" s="109"/>
       <c r="D31" s="32" t="s">
         <v>46</v>
       </c>
@@ -3094,8 +3136,8 @@
       <c r="W31" s="19"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B32" s="94"/>
-      <c r="C32" s="99"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="109"/>
       <c r="D32" s="32" t="s">
         <v>47</v>
       </c>
@@ -3135,8 +3177,8 @@
       <c r="W32" s="19"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B33" s="94"/>
-      <c r="C33" s="99"/>
+      <c r="B33" s="90"/>
+      <c r="C33" s="109"/>
       <c r="D33" s="32" t="s">
         <v>48</v>
       </c>
@@ -3176,8 +3218,8 @@
       <c r="W33" s="19"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B34" s="94"/>
-      <c r="C34" s="99"/>
+      <c r="B34" s="90"/>
+      <c r="C34" s="109"/>
       <c r="D34" s="32" t="s">
         <v>49</v>
       </c>
@@ -3217,8 +3259,8 @@
       <c r="W34" s="19"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B35" s="94"/>
-      <c r="C35" s="99"/>
+      <c r="B35" s="90"/>
+      <c r="C35" s="109"/>
       <c r="D35" s="32" t="s">
         <v>50</v>
       </c>
@@ -3258,8 +3300,8 @@
       <c r="W35" s="19"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B36" s="94"/>
-      <c r="C36" s="99"/>
+      <c r="B36" s="90"/>
+      <c r="C36" s="109"/>
       <c r="D36" s="32" t="s">
         <v>51</v>
       </c>
@@ -3299,8 +3341,8 @@
       <c r="W36" s="19"/>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B37" s="94"/>
-      <c r="C37" s="99"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="109"/>
       <c r="D37" s="32" t="s">
         <v>52</v>
       </c>
@@ -3340,8 +3382,8 @@
       <c r="W37" s="19"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B38" s="94"/>
-      <c r="C38" s="99"/>
+      <c r="B38" s="90"/>
+      <c r="C38" s="109"/>
       <c r="D38" s="32" t="s">
         <v>53</v>
       </c>
@@ -3381,8 +3423,8 @@
       <c r="W38" s="19"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B39" s="94"/>
-      <c r="C39" s="99"/>
+      <c r="B39" s="90"/>
+      <c r="C39" s="109"/>
       <c r="D39" s="32" t="s">
         <v>54</v>
       </c>
@@ -3422,8 +3464,8 @@
       <c r="W39" s="19"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B40" s="94"/>
-      <c r="C40" s="99"/>
+      <c r="B40" s="90"/>
+      <c r="C40" s="109"/>
       <c r="D40" s="32" t="s">
         <v>55</v>
       </c>
@@ -3463,8 +3505,8 @@
       <c r="W40" s="19"/>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B41" s="94"/>
-      <c r="C41" s="99"/>
+      <c r="B41" s="90"/>
+      <c r="C41" s="109"/>
       <c r="D41" s="32" t="s">
         <v>56</v>
       </c>
@@ -3504,8 +3546,8 @@
       <c r="W41" s="19"/>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B42" s="94"/>
-      <c r="C42" s="99"/>
+      <c r="B42" s="90"/>
+      <c r="C42" s="109"/>
       <c r="D42" s="32" t="s">
         <v>57</v>
       </c>
@@ -3545,8 +3587,8 @@
       <c r="W42" s="19"/>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B43" s="94"/>
-      <c r="C43" s="99"/>
+      <c r="B43" s="90"/>
+      <c r="C43" s="109"/>
       <c r="D43" s="32" t="s">
         <v>58</v>
       </c>
@@ -3586,8 +3628,8 @@
       <c r="W43" s="19"/>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B44" s="94"/>
-      <c r="C44" s="99"/>
+      <c r="B44" s="90"/>
+      <c r="C44" s="109"/>
       <c r="D44" s="32" t="s">
         <v>59</v>
       </c>
@@ -3627,8 +3669,8 @@
       <c r="W44" s="19"/>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B45" s="94"/>
-      <c r="C45" s="99"/>
+      <c r="B45" s="90"/>
+      <c r="C45" s="109"/>
       <c r="D45" s="32" t="s">
         <v>60</v>
       </c>
@@ -3668,8 +3710,8 @@
       <c r="W45" s="19"/>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B46" s="94"/>
-      <c r="C46" s="99"/>
+      <c r="B46" s="90"/>
+      <c r="C46" s="109"/>
       <c r="D46" s="32" t="s">
         <v>61</v>
       </c>
@@ -3709,8 +3751,8 @@
       <c r="W46" s="19"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B47" s="94"/>
-      <c r="C47" s="99"/>
+      <c r="B47" s="90"/>
+      <c r="C47" s="109"/>
       <c r="D47" s="32" t="s">
         <v>62</v>
       </c>
@@ -3750,8 +3792,8 @@
       <c r="W47" s="19"/>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B48" s="94"/>
-      <c r="C48" s="99"/>
+      <c r="B48" s="90"/>
+      <c r="C48" s="109"/>
       <c r="D48" s="32" t="s">
         <v>63</v>
       </c>
@@ -3791,8 +3833,8 @@
       <c r="W48" s="19"/>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B49" s="94"/>
-      <c r="C49" s="99"/>
+      <c r="B49" s="90"/>
+      <c r="C49" s="109"/>
       <c r="D49" s="32" t="s">
         <v>64</v>
       </c>
@@ -3832,8 +3874,8 @@
       <c r="W49" s="19"/>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B50" s="94"/>
-      <c r="C50" s="99"/>
+      <c r="B50" s="90"/>
+      <c r="C50" s="109"/>
       <c r="D50" s="32" t="s">
         <v>65</v>
       </c>
@@ -3873,8 +3915,8 @@
       <c r="W50" s="19"/>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B51" s="94"/>
-      <c r="C51" s="99"/>
+      <c r="B51" s="90"/>
+      <c r="C51" s="109"/>
       <c r="D51" s="32" t="s">
         <v>66</v>
       </c>
@@ -3914,8 +3956,8 @@
       <c r="W51" s="19"/>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B52" s="94"/>
-      <c r="C52" s="99"/>
+      <c r="B52" s="90"/>
+      <c r="C52" s="109"/>
       <c r="D52" s="32" t="s">
         <v>67</v>
       </c>
@@ -3955,8 +3997,8 @@
       <c r="W52" s="19"/>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B53" s="94"/>
-      <c r="C53" s="99"/>
+      <c r="B53" s="90"/>
+      <c r="C53" s="109"/>
       <c r="D53" s="32" t="s">
         <v>68</v>
       </c>
@@ -3996,8 +4038,8 @@
       <c r="W53" s="19"/>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B54" s="94"/>
-      <c r="C54" s="100"/>
+      <c r="B54" s="90"/>
+      <c r="C54" s="110"/>
       <c r="D54" s="32" t="s">
         <v>69</v>
       </c>
@@ -4037,8 +4079,8 @@
       <c r="W54" s="19"/>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B55" s="94"/>
-      <c r="C55" s="96" t="s">
+      <c r="B55" s="90"/>
+      <c r="C55" s="106" t="s">
         <v>26</v>
       </c>
       <c r="D55" s="29" t="s">
@@ -4080,8 +4122,8 @@
       <c r="W55" s="19"/>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B56" s="94"/>
-      <c r="C56" s="97"/>
+      <c r="B56" s="90"/>
+      <c r="C56" s="107"/>
       <c r="D56" s="29" t="s">
         <v>29</v>
       </c>
@@ -4121,8 +4163,8 @@
       <c r="W56" s="19"/>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B57" s="94"/>
-      <c r="C57" s="97"/>
+      <c r="B57" s="90"/>
+      <c r="C57" s="107"/>
       <c r="D57" s="29" t="s">
         <v>30</v>
       </c>
@@ -4162,8 +4204,8 @@
       <c r="W57" s="19"/>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B58" s="94"/>
-      <c r="C58" s="97"/>
+      <c r="B58" s="90"/>
+      <c r="C58" s="107"/>
       <c r="D58" s="29" t="s">
         <v>31</v>
       </c>
@@ -4203,8 +4245,8 @@
       <c r="W58" s="19"/>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B59" s="94"/>
-      <c r="C59" s="97"/>
+      <c r="B59" s="90"/>
+      <c r="C59" s="107"/>
       <c r="D59" s="29" t="s">
         <v>34</v>
       </c>
@@ -4244,8 +4286,8 @@
       <c r="W59" s="19"/>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B60" s="94"/>
-      <c r="C60" s="97"/>
+      <c r="B60" s="90"/>
+      <c r="C60" s="107"/>
       <c r="D60" s="29" t="s">
         <v>32</v>
       </c>
@@ -4285,8 +4327,8 @@
       <c r="W60" s="19"/>
     </row>
     <row r="61" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="112"/>
-      <c r="C61" s="97"/>
+      <c r="B61" s="97"/>
+      <c r="C61" s="107"/>
       <c r="D61" s="62" t="s">
         <v>33</v>
       </c>
@@ -4326,10 +4368,10 @@
       <c r="W61" s="28"/>
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B62" s="93" t="s">
+      <c r="B62" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="C62" s="101" t="s">
+      <c r="C62" s="111" t="s">
         <v>79</v>
       </c>
       <c r="D62" s="39" t="s">
@@ -4371,8 +4413,8 @@
       <c r="W62" s="52"/>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B63" s="94"/>
-      <c r="C63" s="102"/>
+      <c r="B63" s="90"/>
+      <c r="C63" s="112"/>
       <c r="D63" s="4" t="s">
         <v>71</v>
       </c>
@@ -4412,8 +4454,8 @@
       <c r="W63" s="19"/>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B64" s="94"/>
-      <c r="C64" s="102"/>
+      <c r="B64" s="90"/>
+      <c r="C64" s="112"/>
       <c r="D64" s="4" t="s">
         <v>72</v>
       </c>
@@ -4453,8 +4495,8 @@
       <c r="W64" s="19"/>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B65" s="94"/>
-      <c r="C65" s="102"/>
+      <c r="B65" s="90"/>
+      <c r="C65" s="112"/>
       <c r="D65" s="29" t="s">
         <v>76</v>
       </c>
@@ -4494,7 +4536,7 @@
       <c r="W65" s="19"/>
     </row>
     <row r="66" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B66" s="94"/>
+      <c r="B66" s="90"/>
       <c r="C66" s="33" t="s">
         <v>73</v>
       </c>
@@ -4535,7 +4577,7 @@
       <c r="W66" s="19"/>
     </row>
     <row r="67" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B67" s="94"/>
+      <c r="B67" s="90"/>
       <c r="C67" s="33" t="s">
         <v>81</v>
       </c>
@@ -4576,8 +4618,8 @@
       <c r="W67" s="19"/>
     </row>
     <row r="68" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="94"/>
-      <c r="C68" s="102" t="s">
+      <c r="B68" s="90"/>
+      <c r="C68" s="112" t="s">
         <v>80</v>
       </c>
       <c r="D68" s="4" t="s">
@@ -4619,8 +4661,8 @@
       <c r="W68" s="19"/>
     </row>
     <row r="69" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="94"/>
-      <c r="C69" s="102"/>
+      <c r="B69" s="90"/>
+      <c r="C69" s="112"/>
       <c r="D69" s="4" t="s">
         <v>75</v>
       </c>
@@ -4660,8 +4702,8 @@
       <c r="W69" s="19"/>
     </row>
     <row r="70" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="94"/>
-      <c r="C70" s="102"/>
+      <c r="B70" s="90"/>
+      <c r="C70" s="112"/>
       <c r="D70" s="4" t="s">
         <v>77</v>
       </c>
@@ -4701,8 +4743,8 @@
       <c r="W70" s="19"/>
     </row>
     <row r="71" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="95"/>
-      <c r="C71" s="103"/>
+      <c r="B71" s="91"/>
+      <c r="C71" s="113"/>
       <c r="D71" s="24" t="s">
         <v>78</v>
       </c>
@@ -4742,10 +4784,10 @@
       <c r="W71" s="25"/>
     </row>
     <row r="72" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="93" t="s">
+      <c r="B72" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="C72" s="107" t="s">
+      <c r="C72" s="117" t="s">
         <v>117</v>
       </c>
       <c r="D72" s="39" t="s">
@@ -4787,8 +4829,8 @@
       <c r="W72" s="52"/>
     </row>
     <row r="73" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="94"/>
-      <c r="C73" s="89"/>
+      <c r="B73" s="90"/>
+      <c r="C73" s="102"/>
       <c r="D73" s="4" t="s">
         <v>133</v>
       </c>
@@ -4828,8 +4870,8 @@
       <c r="W73" s="19"/>
     </row>
     <row r="74" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="94"/>
-      <c r="C74" s="89"/>
+      <c r="B74" s="90"/>
+      <c r="C74" s="102"/>
       <c r="D74" s="4" t="s">
         <v>156</v>
       </c>
@@ -4857,8 +4899,8 @@
       <c r="W74" s="19"/>
     </row>
     <row r="75" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="94"/>
-      <c r="C75" s="89"/>
+      <c r="B75" s="90"/>
+      <c r="C75" s="102"/>
       <c r="D75" s="4" t="s">
         <v>134</v>
       </c>
@@ -4898,8 +4940,8 @@
       <c r="W75" s="19"/>
     </row>
     <row r="76" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="94"/>
-      <c r="C76" s="89"/>
+      <c r="B76" s="90"/>
+      <c r="C76" s="102"/>
       <c r="D76" s="4" t="s">
         <v>135</v>
       </c>
@@ -4939,8 +4981,8 @@
       <c r="W76" s="19"/>
     </row>
     <row r="77" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="94"/>
-      <c r="C77" s="89" t="s">
+      <c r="B77" s="90"/>
+      <c r="C77" s="102" t="s">
         <v>118</v>
       </c>
       <c r="D77" s="4" t="s">
@@ -4982,8 +5024,8 @@
       <c r="W77" s="19"/>
     </row>
     <row r="78" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="94"/>
-      <c r="C78" s="89"/>
+      <c r="B78" s="90"/>
+      <c r="C78" s="102"/>
       <c r="D78" s="4" t="s">
         <v>133</v>
       </c>
@@ -5023,8 +5065,8 @@
       <c r="W78" s="19"/>
     </row>
     <row r="79" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="94"/>
-      <c r="C79" s="89"/>
+      <c r="B79" s="90"/>
+      <c r="C79" s="102"/>
       <c r="D79" s="4" t="s">
         <v>156</v>
       </c>
@@ -5052,8 +5094,8 @@
       <c r="W79" s="19"/>
     </row>
     <row r="80" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="94"/>
-      <c r="C80" s="89"/>
+      <c r="B80" s="90"/>
+      <c r="C80" s="102"/>
       <c r="D80" s="4" t="s">
         <v>134</v>
       </c>
@@ -5093,8 +5135,8 @@
       <c r="W80" s="19"/>
     </row>
     <row r="81" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="94"/>
-      <c r="C81" s="89"/>
+      <c r="B81" s="90"/>
+      <c r="C81" s="102"/>
       <c r="D81" s="4" t="s">
         <v>135</v>
       </c>
@@ -5134,8 +5176,8 @@
       <c r="W81" s="19"/>
     </row>
     <row r="82" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="94"/>
-      <c r="C82" s="89" t="s">
+      <c r="B82" s="90"/>
+      <c r="C82" s="102" t="s">
         <v>119</v>
       </c>
       <c r="D82" s="4" t="s">
@@ -5177,8 +5219,8 @@
       <c r="W82" s="19"/>
     </row>
     <row r="83" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="94"/>
-      <c r="C83" s="89"/>
+      <c r="B83" s="90"/>
+      <c r="C83" s="102"/>
       <c r="D83" s="4" t="s">
         <v>133</v>
       </c>
@@ -5218,8 +5260,8 @@
       <c r="W83" s="19"/>
     </row>
     <row r="84" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="94"/>
-      <c r="C84" s="89"/>
+      <c r="B84" s="90"/>
+      <c r="C84" s="102"/>
       <c r="D84" s="4" t="s">
         <v>156</v>
       </c>
@@ -5247,8 +5289,8 @@
       <c r="W84" s="19"/>
     </row>
     <row r="85" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="94"/>
-      <c r="C85" s="89"/>
+      <c r="B85" s="90"/>
+      <c r="C85" s="102"/>
       <c r="D85" s="4" t="s">
         <v>134</v>
       </c>
@@ -5288,8 +5330,8 @@
       <c r="W85" s="19"/>
     </row>
     <row r="86" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="94"/>
-      <c r="C86" s="89"/>
+      <c r="B86" s="90"/>
+      <c r="C86" s="102"/>
       <c r="D86" s="4" t="s">
         <v>135</v>
       </c>
@@ -5329,8 +5371,8 @@
       <c r="W86" s="19"/>
     </row>
     <row r="87" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="94"/>
-      <c r="C87" s="89" t="s">
+      <c r="B87" s="90"/>
+      <c r="C87" s="102" t="s">
         <v>120</v>
       </c>
       <c r="D87" s="4" t="s">
@@ -5372,8 +5414,8 @@
       <c r="W87" s="19"/>
     </row>
     <row r="88" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="94"/>
-      <c r="C88" s="89"/>
+      <c r="B88" s="90"/>
+      <c r="C88" s="102"/>
       <c r="D88" s="4" t="s">
         <v>133</v>
       </c>
@@ -5413,8 +5455,8 @@
       <c r="W88" s="19"/>
     </row>
     <row r="89" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="94"/>
-      <c r="C89" s="89"/>
+      <c r="B89" s="90"/>
+      <c r="C89" s="102"/>
       <c r="D89" s="4" t="s">
         <v>156</v>
       </c>
@@ -5442,8 +5484,8 @@
       <c r="W89" s="19"/>
     </row>
     <row r="90" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="94"/>
-      <c r="C90" s="89"/>
+      <c r="B90" s="90"/>
+      <c r="C90" s="102"/>
       <c r="D90" s="4" t="s">
         <v>134</v>
       </c>
@@ -5483,8 +5525,8 @@
       <c r="W90" s="19"/>
     </row>
     <row r="91" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="94"/>
-      <c r="C91" s="89"/>
+      <c r="B91" s="90"/>
+      <c r="C91" s="102"/>
       <c r="D91" s="4" t="s">
         <v>135</v>
       </c>
@@ -5524,8 +5566,8 @@
       <c r="W91" s="19"/>
     </row>
     <row r="92" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="94"/>
-      <c r="C92" s="89" t="s">
+      <c r="B92" s="90"/>
+      <c r="C92" s="102" t="s">
         <v>121</v>
       </c>
       <c r="D92" s="4" t="s">
@@ -5567,8 +5609,8 @@
       <c r="W92" s="19"/>
     </row>
     <row r="93" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="94"/>
-      <c r="C93" s="89"/>
+      <c r="B93" s="90"/>
+      <c r="C93" s="102"/>
       <c r="D93" s="4" t="s">
         <v>133</v>
       </c>
@@ -5608,8 +5650,8 @@
       <c r="W93" s="19"/>
     </row>
     <row r="94" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="94"/>
-      <c r="C94" s="89"/>
+      <c r="B94" s="90"/>
+      <c r="C94" s="102"/>
       <c r="D94" s="4" t="s">
         <v>156</v>
       </c>
@@ -5637,8 +5679,8 @@
       <c r="W94" s="19"/>
     </row>
     <row r="95" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="94"/>
-      <c r="C95" s="89"/>
+      <c r="B95" s="90"/>
+      <c r="C95" s="102"/>
       <c r="D95" s="4" t="s">
         <v>134</v>
       </c>
@@ -5678,8 +5720,8 @@
       <c r="W95" s="19"/>
     </row>
     <row r="96" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="94"/>
-      <c r="C96" s="89"/>
+      <c r="B96" s="90"/>
+      <c r="C96" s="102"/>
       <c r="D96" s="4" t="s">
         <v>135</v>
       </c>
@@ -5719,8 +5761,8 @@
       <c r="W96" s="19"/>
     </row>
     <row r="97" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="94"/>
-      <c r="C97" s="89" t="s">
+      <c r="B97" s="90"/>
+      <c r="C97" s="102" t="s">
         <v>122</v>
       </c>
       <c r="D97" s="4" t="s">
@@ -5762,8 +5804,8 @@
       <c r="W97" s="19"/>
     </row>
     <row r="98" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="94"/>
-      <c r="C98" s="89"/>
+      <c r="B98" s="90"/>
+      <c r="C98" s="102"/>
       <c r="D98" s="4" t="s">
         <v>133</v>
       </c>
@@ -5803,8 +5845,8 @@
       <c r="W98" s="19"/>
     </row>
     <row r="99" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="94"/>
-      <c r="C99" s="89"/>
+      <c r="B99" s="90"/>
+      <c r="C99" s="102"/>
       <c r="D99" s="4" t="s">
         <v>156</v>
       </c>
@@ -5832,8 +5874,8 @@
       <c r="W99" s="19"/>
     </row>
     <row r="100" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="94"/>
-      <c r="C100" s="89"/>
+      <c r="B100" s="90"/>
+      <c r="C100" s="102"/>
       <c r="D100" s="4" t="s">
         <v>134</v>
       </c>
@@ -5873,8 +5915,8 @@
       <c r="W100" s="19"/>
     </row>
     <row r="101" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="94"/>
-      <c r="C101" s="89"/>
+      <c r="B101" s="90"/>
+      <c r="C101" s="102"/>
       <c r="D101" s="4" t="s">
         <v>135</v>
       </c>
@@ -5914,8 +5956,8 @@
       <c r="W101" s="19"/>
     </row>
     <row r="102" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="94"/>
-      <c r="C102" s="89" t="s">
+      <c r="B102" s="90"/>
+      <c r="C102" s="102" t="s">
         <v>123</v>
       </c>
       <c r="D102" s="4" t="s">
@@ -5957,8 +5999,8 @@
       <c r="W102" s="19"/>
     </row>
     <row r="103" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="94"/>
-      <c r="C103" s="89"/>
+      <c r="B103" s="90"/>
+      <c r="C103" s="102"/>
       <c r="D103" s="4" t="s">
         <v>133</v>
       </c>
@@ -5998,8 +6040,8 @@
       <c r="W103" s="19"/>
     </row>
     <row r="104" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="94"/>
-      <c r="C104" s="89"/>
+      <c r="B104" s="90"/>
+      <c r="C104" s="102"/>
       <c r="D104" s="4" t="s">
         <v>156</v>
       </c>
@@ -6027,8 +6069,8 @@
       <c r="W104" s="19"/>
     </row>
     <row r="105" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="94"/>
-      <c r="C105" s="89"/>
+      <c r="B105" s="90"/>
+      <c r="C105" s="102"/>
       <c r="D105" s="4" t="s">
         <v>134</v>
       </c>
@@ -6068,8 +6110,8 @@
       <c r="W105" s="19"/>
     </row>
     <row r="106" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="94"/>
-      <c r="C106" s="89"/>
+      <c r="B106" s="90"/>
+      <c r="C106" s="102"/>
       <c r="D106" s="4" t="s">
         <v>135</v>
       </c>
@@ -6109,8 +6151,8 @@
       <c r="W106" s="19"/>
     </row>
     <row r="107" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="94"/>
-      <c r="C107" s="89" t="s">
+      <c r="B107" s="90"/>
+      <c r="C107" s="102" t="s">
         <v>124</v>
       </c>
       <c r="D107" s="4" t="s">
@@ -6152,8 +6194,8 @@
       <c r="W107" s="19"/>
     </row>
     <row r="108" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="94"/>
-      <c r="C108" s="89"/>
+      <c r="B108" s="90"/>
+      <c r="C108" s="102"/>
       <c r="D108" s="4" t="s">
         <v>133</v>
       </c>
@@ -6193,8 +6235,8 @@
       <c r="W108" s="19"/>
     </row>
     <row r="109" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="94"/>
-      <c r="C109" s="89"/>
+      <c r="B109" s="90"/>
+      <c r="C109" s="102"/>
       <c r="D109" s="4" t="s">
         <v>156</v>
       </c>
@@ -6222,8 +6264,8 @@
       <c r="W109" s="19"/>
     </row>
     <row r="110" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="94"/>
-      <c r="C110" s="89"/>
+      <c r="B110" s="90"/>
+      <c r="C110" s="102"/>
       <c r="D110" s="4" t="s">
         <v>134</v>
       </c>
@@ -6263,8 +6305,8 @@
       <c r="W110" s="19"/>
     </row>
     <row r="111" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="94"/>
-      <c r="C111" s="89"/>
+      <c r="B111" s="90"/>
+      <c r="C111" s="102"/>
       <c r="D111" s="4" t="s">
         <v>135</v>
       </c>
@@ -6304,8 +6346,8 @@
       <c r="W111" s="19"/>
     </row>
     <row r="112" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="94"/>
-      <c r="C112" s="89" t="s">
+      <c r="B112" s="90"/>
+      <c r="C112" s="102" t="s">
         <v>125</v>
       </c>
       <c r="D112" s="4" t="s">
@@ -6347,8 +6389,8 @@
       <c r="W112" s="19"/>
     </row>
     <row r="113" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="94"/>
-      <c r="C113" s="89"/>
+      <c r="B113" s="90"/>
+      <c r="C113" s="102"/>
       <c r="D113" s="4" t="s">
         <v>133</v>
       </c>
@@ -6388,8 +6430,8 @@
       <c r="W113" s="19"/>
     </row>
     <row r="114" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="94"/>
-      <c r="C114" s="89"/>
+      <c r="B114" s="90"/>
+      <c r="C114" s="102"/>
       <c r="D114" s="4" t="s">
         <v>156</v>
       </c>
@@ -6417,8 +6459,8 @@
       <c r="W114" s="19"/>
     </row>
     <row r="115" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="94"/>
-      <c r="C115" s="89"/>
+      <c r="B115" s="90"/>
+      <c r="C115" s="102"/>
       <c r="D115" s="4" t="s">
         <v>134</v>
       </c>
@@ -6458,8 +6500,8 @@
       <c r="W115" s="19"/>
     </row>
     <row r="116" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="94"/>
-      <c r="C116" s="89"/>
+      <c r="B116" s="90"/>
+      <c r="C116" s="102"/>
       <c r="D116" s="4" t="s">
         <v>135</v>
       </c>
@@ -6499,8 +6541,8 @@
       <c r="W116" s="19"/>
     </row>
     <row r="117" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="94"/>
-      <c r="C117" s="89" t="s">
+      <c r="B117" s="90"/>
+      <c r="C117" s="102" t="s">
         <v>126</v>
       </c>
       <c r="D117" s="4" t="s">
@@ -6542,8 +6584,8 @@
       <c r="W117" s="19"/>
     </row>
     <row r="118" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="94"/>
-      <c r="C118" s="89"/>
+      <c r="B118" s="90"/>
+      <c r="C118" s="102"/>
       <c r="D118" s="4" t="s">
         <v>133</v>
       </c>
@@ -6583,8 +6625,8 @@
       <c r="W118" s="19"/>
     </row>
     <row r="119" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="94"/>
-      <c r="C119" s="89"/>
+      <c r="B119" s="90"/>
+      <c r="C119" s="102"/>
       <c r="D119" s="4" t="s">
         <v>156</v>
       </c>
@@ -6612,8 +6654,8 @@
       <c r="W119" s="19"/>
     </row>
     <row r="120" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="94"/>
-      <c r="C120" s="89"/>
+      <c r="B120" s="90"/>
+      <c r="C120" s="102"/>
       <c r="D120" s="4" t="s">
         <v>134</v>
       </c>
@@ -6653,8 +6695,8 @@
       <c r="W120" s="19"/>
     </row>
     <row r="121" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="94"/>
-      <c r="C121" s="89"/>
+      <c r="B121" s="90"/>
+      <c r="C121" s="102"/>
       <c r="D121" s="4" t="s">
         <v>135</v>
       </c>
@@ -6694,8 +6736,8 @@
       <c r="W121" s="19"/>
     </row>
     <row r="122" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="94"/>
-      <c r="C122" s="89" t="s">
+      <c r="B122" s="90"/>
+      <c r="C122" s="102" t="s">
         <v>127</v>
       </c>
       <c r="D122" s="4" t="s">
@@ -6737,8 +6779,8 @@
       <c r="W122" s="19"/>
     </row>
     <row r="123" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="94"/>
-      <c r="C123" s="89"/>
+      <c r="B123" s="90"/>
+      <c r="C123" s="102"/>
       <c r="D123" s="4" t="s">
         <v>133</v>
       </c>
@@ -6778,8 +6820,8 @@
       <c r="W123" s="19"/>
     </row>
     <row r="124" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="94"/>
-      <c r="C124" s="89"/>
+      <c r="B124" s="90"/>
+      <c r="C124" s="102"/>
       <c r="D124" s="4" t="s">
         <v>156</v>
       </c>
@@ -6807,8 +6849,8 @@
       <c r="W124" s="19"/>
     </row>
     <row r="125" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="94"/>
-      <c r="C125" s="89"/>
+      <c r="B125" s="90"/>
+      <c r="C125" s="102"/>
       <c r="D125" s="4" t="s">
         <v>134</v>
       </c>
@@ -6848,8 +6890,8 @@
       <c r="W125" s="19"/>
     </row>
     <row r="126" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="94"/>
-      <c r="C126" s="89"/>
+      <c r="B126" s="90"/>
+      <c r="C126" s="102"/>
       <c r="D126" s="4" t="s">
         <v>135</v>
       </c>
@@ -6889,8 +6931,8 @@
       <c r="W126" s="19"/>
     </row>
     <row r="127" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="94"/>
-      <c r="C127" s="89" t="s">
+      <c r="B127" s="90"/>
+      <c r="C127" s="102" t="s">
         <v>128</v>
       </c>
       <c r="D127" s="4" t="s">
@@ -6932,8 +6974,8 @@
       <c r="W127" s="19"/>
     </row>
     <row r="128" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="94"/>
-      <c r="C128" s="89"/>
+      <c r="B128" s="90"/>
+      <c r="C128" s="102"/>
       <c r="D128" s="4" t="s">
         <v>133</v>
       </c>
@@ -6973,8 +7015,8 @@
       <c r="W128" s="19"/>
     </row>
     <row r="129" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="94"/>
-      <c r="C129" s="89"/>
+      <c r="B129" s="90"/>
+      <c r="C129" s="102"/>
       <c r="D129" s="4" t="s">
         <v>156</v>
       </c>
@@ -7002,8 +7044,8 @@
       <c r="W129" s="19"/>
     </row>
     <row r="130" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="94"/>
-      <c r="C130" s="89"/>
+      <c r="B130" s="90"/>
+      <c r="C130" s="102"/>
       <c r="D130" s="4" t="s">
         <v>134</v>
       </c>
@@ -7043,8 +7085,8 @@
       <c r="W130" s="19"/>
     </row>
     <row r="131" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="94"/>
-      <c r="C131" s="89"/>
+      <c r="B131" s="90"/>
+      <c r="C131" s="102"/>
       <c r="D131" s="4" t="s">
         <v>135</v>
       </c>
@@ -7084,8 +7126,8 @@
       <c r="W131" s="19"/>
     </row>
     <row r="132" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="94"/>
-      <c r="C132" s="89" t="s">
+      <c r="B132" s="90"/>
+      <c r="C132" s="102" t="s">
         <v>129</v>
       </c>
       <c r="D132" s="4" t="s">
@@ -7127,8 +7169,8 @@
       <c r="W132" s="19"/>
     </row>
     <row r="133" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="94"/>
-      <c r="C133" s="89"/>
+      <c r="B133" s="90"/>
+      <c r="C133" s="102"/>
       <c r="D133" s="4" t="s">
         <v>133</v>
       </c>
@@ -7168,8 +7210,8 @@
       <c r="W133" s="19"/>
     </row>
     <row r="134" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="94"/>
-      <c r="C134" s="89"/>
+      <c r="B134" s="90"/>
+      <c r="C134" s="102"/>
       <c r="D134" s="4" t="s">
         <v>156</v>
       </c>
@@ -7197,8 +7239,8 @@
       <c r="W134" s="19"/>
     </row>
     <row r="135" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="94"/>
-      <c r="C135" s="89"/>
+      <c r="B135" s="90"/>
+      <c r="C135" s="102"/>
       <c r="D135" s="4" t="s">
         <v>134</v>
       </c>
@@ -7238,8 +7280,8 @@
       <c r="W135" s="19"/>
     </row>
     <row r="136" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="94"/>
-      <c r="C136" s="89"/>
+      <c r="B136" s="90"/>
+      <c r="C136" s="102"/>
       <c r="D136" s="4" t="s">
         <v>135</v>
       </c>
@@ -7279,8 +7321,8 @@
       <c r="W136" s="19"/>
     </row>
     <row r="137" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="94"/>
-      <c r="C137" s="89" t="s">
+      <c r="B137" s="90"/>
+      <c r="C137" s="102" t="s">
         <v>130</v>
       </c>
       <c r="D137" s="4" t="s">
@@ -7322,8 +7364,8 @@
       <c r="W137" s="19"/>
     </row>
     <row r="138" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="94"/>
-      <c r="C138" s="89"/>
+      <c r="B138" s="90"/>
+      <c r="C138" s="102"/>
       <c r="D138" s="4" t="s">
         <v>133</v>
       </c>
@@ -7363,8 +7405,8 @@
       <c r="W138" s="19"/>
     </row>
     <row r="139" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="94"/>
-      <c r="C139" s="89"/>
+      <c r="B139" s="90"/>
+      <c r="C139" s="102"/>
       <c r="D139" s="4" t="s">
         <v>156</v>
       </c>
@@ -7392,8 +7434,8 @@
       <c r="W139" s="19"/>
     </row>
     <row r="140" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="94"/>
-      <c r="C140" s="89"/>
+      <c r="B140" s="90"/>
+      <c r="C140" s="102"/>
       <c r="D140" s="4" t="s">
         <v>134</v>
       </c>
@@ -7433,8 +7475,8 @@
       <c r="W140" s="19"/>
     </row>
     <row r="141" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="94"/>
-      <c r="C141" s="89"/>
+      <c r="B141" s="90"/>
+      <c r="C141" s="102"/>
       <c r="D141" s="4" t="s">
         <v>135</v>
       </c>
@@ -7474,8 +7516,8 @@
       <c r="W141" s="19"/>
     </row>
     <row r="142" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="94"/>
-      <c r="C142" s="89" t="s">
+      <c r="B142" s="90"/>
+      <c r="C142" s="102" t="s">
         <v>131</v>
       </c>
       <c r="D142" s="4" t="s">
@@ -7517,8 +7559,8 @@
       <c r="W142" s="19"/>
     </row>
     <row r="143" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="94"/>
-      <c r="C143" s="89"/>
+      <c r="B143" s="90"/>
+      <c r="C143" s="102"/>
       <c r="D143" s="4" t="s">
         <v>133</v>
       </c>
@@ -7558,8 +7600,8 @@
       <c r="W143" s="19"/>
     </row>
     <row r="144" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="94"/>
-      <c r="C144" s="89"/>
+      <c r="B144" s="90"/>
+      <c r="C144" s="102"/>
       <c r="D144" s="4" t="s">
         <v>156</v>
       </c>
@@ -7587,8 +7629,8 @@
       <c r="W144" s="19"/>
     </row>
     <row r="145" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="94"/>
-      <c r="C145" s="89"/>
+      <c r="B145" s="90"/>
+      <c r="C145" s="102"/>
       <c r="D145" s="4" t="s">
         <v>134</v>
       </c>
@@ -7628,8 +7670,8 @@
       <c r="W145" s="19"/>
     </row>
     <row r="146" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B146" s="95"/>
-      <c r="C146" s="117"/>
+      <c r="B146" s="91"/>
+      <c r="C146" s="105"/>
       <c r="D146" s="24" t="s">
         <v>135</v>
       </c>
@@ -7669,7 +7711,7 @@
       <c r="W146" s="25"/>
     </row>
     <row r="147" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B147" s="93" t="s">
+      <c r="B147" s="89" t="s">
         <v>83</v>
       </c>
       <c r="C147" s="78" t="s">
@@ -7712,7 +7754,7 @@
       <c r="W147" s="52"/>
     </row>
     <row r="148" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="94"/>
+      <c r="B148" s="90"/>
       <c r="C148" s="33" t="s">
         <v>89</v>
       </c>
@@ -7753,7 +7795,7 @@
       <c r="W148" s="19"/>
     </row>
     <row r="149" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="94"/>
+      <c r="B149" s="90"/>
       <c r="C149" s="33" t="s">
         <v>90</v>
       </c>
@@ -7794,7 +7836,7 @@
       <c r="W149" s="19"/>
     </row>
     <row r="150" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="94"/>
+      <c r="B150" s="90"/>
       <c r="C150" s="33" t="s">
         <v>91</v>
       </c>
@@ -7835,7 +7877,7 @@
       <c r="W150" s="19"/>
     </row>
     <row r="151" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="94"/>
+      <c r="B151" s="90"/>
       <c r="C151" s="33" t="s">
         <v>142</v>
       </c>
@@ -7876,7 +7918,7 @@
       <c r="W151" s="19"/>
     </row>
     <row r="152" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="94"/>
+      <c r="B152" s="90"/>
       <c r="C152" s="33" t="s">
         <v>139</v>
       </c>
@@ -7917,7 +7959,7 @@
       <c r="W152" s="19"/>
     </row>
     <row r="153" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="94"/>
+      <c r="B153" s="90"/>
       <c r="C153" s="33" t="s">
         <v>141</v>
       </c>
@@ -7958,7 +8000,7 @@
       <c r="W153" s="19"/>
     </row>
     <row r="154" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="94"/>
+      <c r="B154" s="90"/>
       <c r="C154" s="33" t="s">
         <v>140</v>
       </c>
@@ -7999,7 +8041,7 @@
       <c r="W154" s="19"/>
     </row>
     <row r="155" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="94"/>
+      <c r="B155" s="90"/>
       <c r="C155" s="33" t="s">
         <v>92</v>
       </c>
@@ -8040,7 +8082,7 @@
       <c r="W155" s="19"/>
     </row>
     <row r="156" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="94"/>
+      <c r="B156" s="90"/>
       <c r="C156" s="33" t="s">
         <v>93</v>
       </c>
@@ -8081,7 +8123,7 @@
       <c r="W156" s="19"/>
     </row>
     <row r="157" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="94"/>
+      <c r="B157" s="90"/>
       <c r="C157" s="33" t="s">
         <v>94</v>
       </c>
@@ -8122,7 +8164,7 @@
       <c r="W157" s="19"/>
     </row>
     <row r="158" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="94"/>
+      <c r="B158" s="90"/>
       <c r="C158" s="33" t="s">
         <v>98</v>
       </c>
@@ -8163,7 +8205,7 @@
       <c r="W158" s="19"/>
     </row>
     <row r="159" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B159" s="95"/>
+      <c r="B159" s="91"/>
       <c r="C159" s="61" t="s">
         <v>99</v>
       </c>
@@ -8204,7 +8246,7 @@
       <c r="W159" s="25"/>
     </row>
     <row r="160" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="93" t="s">
+      <c r="B160" s="89" t="s">
         <v>143</v>
       </c>
       <c r="C160" s="60" t="s">
@@ -8247,7 +8289,7 @@
       <c r="W160" s="52"/>
     </row>
     <row r="161" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="94"/>
+      <c r="B161" s="90"/>
       <c r="C161" s="59" t="s">
         <v>144</v>
       </c>
@@ -8288,7 +8330,7 @@
       <c r="W161" s="19"/>
     </row>
     <row r="162" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B162" s="95"/>
+      <c r="B162" s="91"/>
       <c r="C162" s="61" t="s">
         <v>145</v>
       </c>
@@ -8329,7 +8371,7 @@
       <c r="W162" s="25"/>
     </row>
     <row r="163" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="93" t="s">
+      <c r="B163" s="89" t="s">
         <v>148</v>
       </c>
       <c r="C163" s="60" t="s">
@@ -8368,7 +8410,7 @@
       <c r="W163" s="52"/>
     </row>
     <row r="164" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="94"/>
+      <c r="B164" s="90"/>
       <c r="C164" s="59" t="s">
         <v>150</v>
       </c>
@@ -8405,7 +8447,7 @@
       <c r="W164" s="19"/>
     </row>
     <row r="165" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="94"/>
+      <c r="B165" s="90"/>
       <c r="C165" s="59" t="s">
         <v>151</v>
       </c>
@@ -8442,7 +8484,7 @@
       <c r="W165" s="19"/>
     </row>
     <row r="166" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B166" s="94"/>
+      <c r="B166" s="90"/>
       <c r="C166" s="59" t="s">
         <v>152</v>
       </c>
@@ -8479,7 +8521,7 @@
       <c r="W166" s="19"/>
     </row>
     <row r="167" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B167" s="94"/>
+      <c r="B167" s="90"/>
       <c r="C167" s="59" t="s">
         <v>153</v>
       </c>
@@ -8516,7 +8558,7 @@
       <c r="W167" s="19"/>
     </row>
     <row r="168" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B168" s="94"/>
+      <c r="B168" s="90"/>
       <c r="C168" s="59" t="s">
         <v>154</v>
       </c>
@@ -8553,7 +8595,7 @@
       <c r="W168" s="19"/>
     </row>
     <row r="169" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B169" s="95"/>
+      <c r="B169" s="91"/>
       <c r="C169" s="61" t="s">
         <v>155</v>
       </c>
@@ -8590,7 +8632,7 @@
       <c r="W169" s="25"/>
     </row>
     <row r="170" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B170" s="93" t="s">
+      <c r="B170" s="89" t="s">
         <v>18</v>
       </c>
       <c r="C170" s="54" t="s">
@@ -8633,7 +8675,7 @@
       <c r="W170" s="52"/>
     </row>
     <row r="171" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B171" s="94"/>
+      <c r="B171" s="90"/>
       <c r="C171" s="33" t="s">
         <v>137</v>
       </c>
@@ -8674,7 +8716,7 @@
       <c r="W171" s="19"/>
     </row>
     <row r="172" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="94"/>
+      <c r="B172" s="90"/>
       <c r="C172" s="33" t="s">
         <v>138</v>
       </c>
@@ -8715,7 +8757,7 @@
       <c r="W172" s="19"/>
     </row>
     <row r="173" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B173" s="94"/>
+      <c r="B173" s="90"/>
       <c r="C173" s="33" t="s">
         <v>146</v>
       </c>
@@ -8756,7 +8798,7 @@
       <c r="W173" s="19"/>
     </row>
     <row r="174" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="94"/>
+      <c r="B174" s="90"/>
       <c r="C174" s="33" t="s">
         <v>84</v>
       </c>
@@ -8797,7 +8839,7 @@
       <c r="W174" s="19"/>
     </row>
     <row r="175" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="94"/>
+      <c r="B175" s="90"/>
       <c r="C175" s="33" t="s">
         <v>85</v>
       </c>
@@ -8838,7 +8880,7 @@
       <c r="W175" s="19"/>
     </row>
     <row r="176" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="94"/>
+      <c r="B176" s="90"/>
       <c r="C176" s="33" t="s">
         <v>87</v>
       </c>
@@ -8879,7 +8921,7 @@
       <c r="W176" s="19"/>
     </row>
     <row r="177" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B177" s="94"/>
+      <c r="B177" s="90"/>
       <c r="C177" s="33" t="s">
         <v>86</v>
       </c>
@@ -8920,7 +8962,7 @@
       <c r="W177" s="19"/>
     </row>
     <row r="178" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B178" s="94"/>
+      <c r="B178" s="90"/>
       <c r="C178" s="33" t="s">
         <v>104</v>
       </c>
@@ -8961,7 +9003,7 @@
       <c r="W178" s="19"/>
     </row>
     <row r="179" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B179" s="94"/>
+      <c r="B179" s="90"/>
       <c r="C179" s="33" t="s">
         <v>136</v>
       </c>
@@ -9002,7 +9044,7 @@
       <c r="W179" s="19"/>
     </row>
     <row r="180" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B180" s="94"/>
+      <c r="B180" s="90"/>
       <c r="C180" s="33" t="s">
         <v>105</v>
       </c>
@@ -9043,7 +9085,7 @@
       <c r="W180" s="19"/>
     </row>
     <row r="181" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B181" s="95"/>
+      <c r="B181" s="91"/>
       <c r="C181" s="61" t="s">
         <v>100</v>
       </c>
@@ -9084,14 +9126,14 @@
       <c r="W181" s="25"/>
     </row>
     <row r="182" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B182" s="113" t="s">
+      <c r="B182" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="C182" s="114"/>
-      <c r="D182" s="115"/>
-      <c r="E182" s="115"/>
-      <c r="F182" s="115"/>
-      <c r="G182" s="116"/>
+      <c r="C182" s="99"/>
+      <c r="D182" s="100"/>
+      <c r="E182" s="100"/>
+      <c r="F182" s="100"/>
+      <c r="G182" s="101"/>
       <c r="H182" s="36">
         <f t="shared" ref="H182:W182" si="6">SUM(H4:H181)</f>
         <v>96.499999999999829</v>
@@ -9166,28 +9208,33 @@
       <c r="G183" s="2"/>
       <c r="H183" s="2"/>
       <c r="I183" s="2"/>
-      <c r="J183" s="90" t="s">
+      <c r="J183" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="K183" s="91"/>
-      <c r="L183" s="91"/>
-      <c r="M183" s="91"/>
-      <c r="N183" s="91"/>
-      <c r="O183" s="91"/>
-      <c r="P183" s="91"/>
-      <c r="Q183" s="91"/>
-      <c r="R183" s="91"/>
-      <c r="S183" s="91"/>
-      <c r="T183" s="91"/>
-      <c r="U183" s="91"/>
-      <c r="V183" s="91"/>
-      <c r="W183" s="92"/>
-    </row>
-    <row r="184" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B184" s="2"/>
-      <c r="C184" s="2"/>
-      <c r="D184" s="2"/>
-      <c r="E184" s="2"/>
+      <c r="K183" s="103"/>
+      <c r="L183" s="103"/>
+      <c r="M183" s="103"/>
+      <c r="N183" s="103"/>
+      <c r="O183" s="103"/>
+      <c r="P183" s="103"/>
+      <c r="Q183" s="103"/>
+      <c r="R183" s="103"/>
+      <c r="S183" s="103"/>
+      <c r="T183" s="103"/>
+      <c r="U183" s="103"/>
+      <c r="V183" s="103"/>
+      <c r="W183" s="104"/>
+    </row>
+    <row r="184" spans="2:23" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C184" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="D184" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E184" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
       <c r="H184" s="2"/>
@@ -9199,16 +9246,27 @@
       <c r="N184" s="3"/>
     </row>
     <row r="185" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B185" s="2"/>
-      <c r="C185" s="2"/>
-      <c r="D185" s="2"/>
-      <c r="E185" s="2"/>
+      <c r="B185" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="C185" s="120">
+        <f>SUM(H181,H179,H175:H176,H163:H169,H159,H155:H157,H12:H61,H10)</f>
+        <v>46.899999999999984</v>
+      </c>
+      <c r="D185" s="4">
+        <f>SUM(I10,I12,I13,I14,I15:I61,I155:I157,I159,I163:I169,I175:I176,I179,I181)</f>
+        <v>8.8533000000000008</v>
+      </c>
+      <c r="E185" s="4">
+        <f>SUM(C185,-D185)</f>
+        <v>38.046699999999987</v>
+      </c>
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
-      <c r="H185" s="108" t="s">
+      <c r="H185" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="I185" s="109"/>
+      <c r="I185" s="93"/>
       <c r="J185" s="9">
         <f>H182-J182</f>
         <v>96.499999999999829</v>
@@ -9231,10 +9289,21 @@
       </c>
     </row>
     <row r="186" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B186" s="3"/>
-      <c r="C186" s="3"/>
-      <c r="D186" s="3"/>
-      <c r="E186" s="3"/>
+      <c r="B186" s="119" t="s">
+        <v>158</v>
+      </c>
+      <c r="C186" s="5">
+        <f>SUM(H160:H162,H158,H72:H147,H11,H9)</f>
+        <v>25.200000000000003</v>
+      </c>
+      <c r="D186" s="5">
+        <f>SUM(I9,I11,I72:I147,I158,I160:I162)</f>
+        <v>0.77</v>
+      </c>
+      <c r="E186" s="5">
+        <f>SUM(C186,-D186)</f>
+        <v>24.430000000000003</v>
+      </c>
       <c r="F186" s="3"/>
       <c r="G186" s="3"/>
       <c r="H186" s="3"/>
@@ -9246,23 +9315,34 @@
       <c r="N186" s="3"/>
     </row>
     <row r="187" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B187" s="3"/>
-      <c r="C187" s="3"/>
-      <c r="D187" s="3"/>
-      <c r="E187" s="3"/>
+      <c r="B187" s="119" t="s">
+        <v>159</v>
+      </c>
+      <c r="C187" s="4">
+        <f>SUM(H180,H178,H177,H170:H174,H148:H154,H62:H71,H4:H8)</f>
+        <v>24.4</v>
+      </c>
+      <c r="D187" s="5">
+        <f>SUM(I180,I177:I178,I170:I174,I148:I154,I62:I71,I4:I8)</f>
+        <v>0</v>
+      </c>
+      <c r="E187" s="5">
+        <f>SUM(C187,-D187)</f>
+        <v>24.4</v>
+      </c>
       <c r="F187" s="3"/>
-      <c r="H187" s="90" t="s">
+      <c r="H187" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="I187" s="110"/>
-      <c r="J187" s="109">
+      <c r="I187" s="95"/>
+      <c r="J187" s="93">
         <f>H182-I182</f>
         <v>86.876699999999829</v>
       </c>
-      <c r="K187" s="109"/>
-      <c r="L187" s="109"/>
-      <c r="M187" s="109"/>
-      <c r="N187" s="111"/>
+      <c r="K187" s="93"/>
+      <c r="L187" s="93"/>
+      <c r="M187" s="93"/>
+      <c r="N187" s="96"/>
     </row>
     <row r="188" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B188" s="3"/>
@@ -9366,6 +9446,24 @@
     <row r="206" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C132:C136"/>
+    <mergeCell ref="C122:C126"/>
+    <mergeCell ref="C112:C116"/>
+    <mergeCell ref="C107:C111"/>
+    <mergeCell ref="C97:C101"/>
+    <mergeCell ref="C117:C121"/>
+    <mergeCell ref="C127:C131"/>
+    <mergeCell ref="C82:C86"/>
+    <mergeCell ref="J2:W2"/>
+    <mergeCell ref="B62:B71"/>
+    <mergeCell ref="C55:C61"/>
+    <mergeCell ref="C15:C54"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C72:C76"/>
+    <mergeCell ref="C77:C81"/>
     <mergeCell ref="B163:B169"/>
     <mergeCell ref="H185:I185"/>
     <mergeCell ref="H187:I187"/>
@@ -9382,24 +9480,6 @@
     <mergeCell ref="C142:C146"/>
     <mergeCell ref="C92:C96"/>
     <mergeCell ref="C87:C91"/>
-    <mergeCell ref="C82:C86"/>
-    <mergeCell ref="J2:W2"/>
-    <mergeCell ref="B62:B71"/>
-    <mergeCell ref="C55:C61"/>
-    <mergeCell ref="C15:C54"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="C72:C76"/>
-    <mergeCell ref="C77:C81"/>
-    <mergeCell ref="C132:C136"/>
-    <mergeCell ref="C122:C126"/>
-    <mergeCell ref="C112:C116"/>
-    <mergeCell ref="C107:C111"/>
-    <mergeCell ref="C97:C101"/>
-    <mergeCell ref="C117:C121"/>
-    <mergeCell ref="C127:C131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementados corazones como grupo de prefabs, actualizado el excel
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
+++ b/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
@@ -1285,10 +1285,46 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1297,13 +1333,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1340,36 +1370,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1438,10 +1438,10 @@
                   <c:v>89.943699999999822</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85.26669999999983</c:v>
+                  <c:v>85.032699999999821</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>85.26669999999983</c:v>
+                  <c:v>85.032699999999821</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1462,11 +1462,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="327264544"/>
-        <c:axId val="327258016"/>
+        <c:axId val="-1083270528"/>
+        <c:axId val="-1083260192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="327264544"/>
+        <c:axId val="-1083270528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1475,7 +1475,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="327258016"/>
+        <c:crossAx val="-1083260192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1483,7 +1483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="327258016"/>
+        <c:axId val="-1083260192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1494,7 +1494,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="327264544"/>
+        <c:crossAx val="-1083270528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1536,7 +1536,7 @@
         <xdr:cNvPr id="4" name="3 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1846,8 +1846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C185" sqref="C185"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K156" sqref="K156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1874,22 +1874,22 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="97" t="s">
+      <c r="J2" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
-      <c r="Q2" s="98"/>
-      <c r="R2" s="98"/>
-      <c r="S2" s="98"/>
-      <c r="T2" s="98"/>
-      <c r="U2" s="98"/>
-      <c r="V2" s="98"/>
-      <c r="W2" s="99"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="110"/>
+      <c r="R2" s="110"/>
+      <c r="S2" s="110"/>
+      <c r="T2" s="110"/>
+      <c r="U2" s="110"/>
+      <c r="V2" s="110"/>
+      <c r="W2" s="111"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="56" t="s">
@@ -1960,7 +1960,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="111" t="s">
+      <c r="B4" s="121" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="37" t="s">
@@ -2005,7 +2005,7 @@
       <c r="W4" s="44"/>
     </row>
     <row r="5" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="112"/>
+      <c r="B5" s="122"/>
       <c r="C5" s="35" t="s">
         <v>100</v>
       </c>
@@ -2048,7 +2048,7 @@
       <c r="W5" s="19"/>
     </row>
     <row r="6" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="112"/>
+      <c r="B6" s="122"/>
       <c r="C6" s="35" t="s">
         <v>101</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="W6" s="19"/>
     </row>
     <row r="7" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="112"/>
+      <c r="B7" s="122"/>
       <c r="C7" s="35" t="s">
         <v>102</v>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="W7" s="19"/>
     </row>
     <row r="8" spans="1:23" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="113"/>
+      <c r="B8" s="123"/>
       <c r="C8" s="45" t="s">
         <v>110</v>
       </c>
@@ -2177,7 +2177,7 @@
       <c r="W8" s="25"/>
     </row>
     <row r="9" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="121" t="s">
         <v>105</v>
       </c>
       <c r="C9" s="48" t="s">
@@ -2222,7 +2222,7 @@
       <c r="W9" s="86"/>
     </row>
     <row r="10" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="112"/>
+      <c r="B10" s="122"/>
       <c r="C10" s="34" t="s">
         <v>106</v>
       </c>
@@ -2265,7 +2265,7 @@
       <c r="W10" s="19"/>
     </row>
     <row r="11" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="112"/>
+      <c r="B11" s="122"/>
       <c r="C11" s="83" t="s">
         <v>111</v>
       </c>
@@ -2308,7 +2308,7 @@
       <c r="W11" s="19"/>
     </row>
     <row r="12" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="112"/>
+      <c r="B12" s="122"/>
       <c r="C12" s="83" t="s">
         <v>112</v>
       </c>
@@ -2373,7 +2373,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="113"/>
+      <c r="B13" s="123"/>
       <c r="C13" s="53" t="s">
         <v>97</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="W13" s="25"/>
     </row>
     <row r="14" spans="1:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B14" s="100" t="s">
+      <c r="B14" s="96" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="54" t="s">
@@ -2463,8 +2463,8 @@
       <c r="W14" s="52"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B15" s="101"/>
-      <c r="C15" s="105" t="s">
+      <c r="B15" s="97"/>
+      <c r="C15" s="115" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -2510,8 +2510,8 @@
       <c r="W15" s="19"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B16" s="101"/>
-      <c r="C16" s="106"/>
+      <c r="B16" s="97"/>
+      <c r="C16" s="116"/>
       <c r="D16" s="4" t="s">
         <v>20</v>
       </c>
@@ -2553,8 +2553,8 @@
       <c r="W16" s="19"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B17" s="101"/>
-      <c r="C17" s="106"/>
+      <c r="B17" s="97"/>
+      <c r="C17" s="116"/>
       <c r="D17" s="4" t="s">
         <v>21</v>
       </c>
@@ -2596,8 +2596,8 @@
       <c r="W17" s="19"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B18" s="101"/>
-      <c r="C18" s="106"/>
+      <c r="B18" s="97"/>
+      <c r="C18" s="116"/>
       <c r="D18" s="4" t="s">
         <v>22</v>
       </c>
@@ -2639,8 +2639,8 @@
       <c r="W18" s="19"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B19" s="101"/>
-      <c r="C19" s="106"/>
+      <c r="B19" s="97"/>
+      <c r="C19" s="116"/>
       <c r="D19" s="4" t="s">
         <v>23</v>
       </c>
@@ -2682,8 +2682,8 @@
       <c r="W19" s="19"/>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B20" s="101"/>
-      <c r="C20" s="106"/>
+      <c r="B20" s="97"/>
+      <c r="C20" s="116"/>
       <c r="D20" s="4" t="s">
         <v>162</v>
       </c>
@@ -2725,8 +2725,8 @@
       <c r="W20" s="19"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B21" s="101"/>
-      <c r="C21" s="106"/>
+      <c r="B21" s="97"/>
+      <c r="C21" s="116"/>
       <c r="D21" s="4" t="s">
         <v>24</v>
       </c>
@@ -2768,8 +2768,8 @@
       <c r="W21" s="19"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B22" s="101"/>
-      <c r="C22" s="106"/>
+      <c r="B22" s="97"/>
+      <c r="C22" s="116"/>
       <c r="D22" s="32" t="s">
         <v>36</v>
       </c>
@@ -2811,8 +2811,8 @@
       <c r="W22" s="19"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B23" s="101"/>
-      <c r="C23" s="106"/>
+      <c r="B23" s="97"/>
+      <c r="C23" s="116"/>
       <c r="D23" s="32" t="s">
         <v>37</v>
       </c>
@@ -2854,8 +2854,8 @@
       <c r="W23" s="19"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B24" s="101"/>
-      <c r="C24" s="106"/>
+      <c r="B24" s="97"/>
+      <c r="C24" s="116"/>
       <c r="D24" s="32" t="s">
         <v>38</v>
       </c>
@@ -2897,8 +2897,8 @@
       <c r="W24" s="19"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B25" s="101"/>
-      <c r="C25" s="106"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="116"/>
       <c r="D25" s="32" t="s">
         <v>39</v>
       </c>
@@ -2940,8 +2940,8 @@
       <c r="W25" s="19"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B26" s="101"/>
-      <c r="C26" s="106"/>
+      <c r="B26" s="97"/>
+      <c r="C26" s="116"/>
       <c r="D26" s="32" t="s">
         <v>40</v>
       </c>
@@ -2983,8 +2983,8 @@
       <c r="W26" s="19"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B27" s="101"/>
-      <c r="C27" s="106"/>
+      <c r="B27" s="97"/>
+      <c r="C27" s="116"/>
       <c r="D27" s="32" t="s">
         <v>41</v>
       </c>
@@ -3026,8 +3026,8 @@
       <c r="W27" s="19"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B28" s="101"/>
-      <c r="C28" s="106"/>
+      <c r="B28" s="97"/>
+      <c r="C28" s="116"/>
       <c r="D28" s="32" t="s">
         <v>42</v>
       </c>
@@ -3069,8 +3069,8 @@
       <c r="W28" s="19"/>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B29" s="101"/>
-      <c r="C29" s="106"/>
+      <c r="B29" s="97"/>
+      <c r="C29" s="116"/>
       <c r="D29" s="32" t="s">
         <v>43</v>
       </c>
@@ -3112,8 +3112,8 @@
       <c r="W29" s="19"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B30" s="101"/>
-      <c r="C30" s="106"/>
+      <c r="B30" s="97"/>
+      <c r="C30" s="116"/>
       <c r="D30" s="32" t="s">
         <v>44</v>
       </c>
@@ -3155,8 +3155,8 @@
       <c r="W30" s="19"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B31" s="101"/>
-      <c r="C31" s="106"/>
+      <c r="B31" s="97"/>
+      <c r="C31" s="116"/>
       <c r="D31" s="32" t="s">
         <v>45</v>
       </c>
@@ -3198,8 +3198,8 @@
       <c r="W31" s="19"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B32" s="101"/>
-      <c r="C32" s="106"/>
+      <c r="B32" s="97"/>
+      <c r="C32" s="116"/>
       <c r="D32" s="32" t="s">
         <v>46</v>
       </c>
@@ -3241,8 +3241,8 @@
       <c r="W32" s="19"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B33" s="101"/>
-      <c r="C33" s="106"/>
+      <c r="B33" s="97"/>
+      <c r="C33" s="116"/>
       <c r="D33" s="32" t="s">
         <v>47</v>
       </c>
@@ -3284,8 +3284,8 @@
       <c r="W33" s="19"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B34" s="101"/>
-      <c r="C34" s="106"/>
+      <c r="B34" s="97"/>
+      <c r="C34" s="116"/>
       <c r="D34" s="32" t="s">
         <v>48</v>
       </c>
@@ -3327,8 +3327,8 @@
       <c r="W34" s="19"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B35" s="101"/>
-      <c r="C35" s="106"/>
+      <c r="B35" s="97"/>
+      <c r="C35" s="116"/>
       <c r="D35" s="32" t="s">
         <v>49</v>
       </c>
@@ -3370,8 +3370,8 @@
       <c r="W35" s="19"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B36" s="101"/>
-      <c r="C36" s="106"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="116"/>
       <c r="D36" s="32" t="s">
         <v>50</v>
       </c>
@@ -3413,8 +3413,8 @@
       <c r="W36" s="19"/>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B37" s="101"/>
-      <c r="C37" s="106"/>
+      <c r="B37" s="97"/>
+      <c r="C37" s="116"/>
       <c r="D37" s="32" t="s">
         <v>51</v>
       </c>
@@ -3456,8 +3456,8 @@
       <c r="W37" s="19"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B38" s="101"/>
-      <c r="C38" s="106"/>
+      <c r="B38" s="97"/>
+      <c r="C38" s="116"/>
       <c r="D38" s="32" t="s">
         <v>52</v>
       </c>
@@ -3499,8 +3499,8 @@
       <c r="W38" s="19"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B39" s="101"/>
-      <c r="C39" s="106"/>
+      <c r="B39" s="97"/>
+      <c r="C39" s="116"/>
       <c r="D39" s="32" t="s">
         <v>53</v>
       </c>
@@ -3542,8 +3542,8 @@
       <c r="W39" s="19"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B40" s="101"/>
-      <c r="C40" s="106"/>
+      <c r="B40" s="97"/>
+      <c r="C40" s="116"/>
       <c r="D40" s="32" t="s">
         <v>54</v>
       </c>
@@ -3585,8 +3585,8 @@
       <c r="W40" s="19"/>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B41" s="101"/>
-      <c r="C41" s="106"/>
+      <c r="B41" s="97"/>
+      <c r="C41" s="116"/>
       <c r="D41" s="32" t="s">
         <v>55</v>
       </c>
@@ -3628,8 +3628,8 @@
       <c r="W41" s="19"/>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B42" s="101"/>
-      <c r="C42" s="106"/>
+      <c r="B42" s="97"/>
+      <c r="C42" s="116"/>
       <c r="D42" s="32" t="s">
         <v>56</v>
       </c>
@@ -3671,8 +3671,8 @@
       <c r="W42" s="19"/>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B43" s="101"/>
-      <c r="C43" s="106"/>
+      <c r="B43" s="97"/>
+      <c r="C43" s="116"/>
       <c r="D43" s="32" t="s">
         <v>57</v>
       </c>
@@ -3714,8 +3714,8 @@
       <c r="W43" s="19"/>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B44" s="101"/>
-      <c r="C44" s="106"/>
+      <c r="B44" s="97"/>
+      <c r="C44" s="116"/>
       <c r="D44" s="32" t="s">
         <v>58</v>
       </c>
@@ -3757,8 +3757,8 @@
       <c r="W44" s="19"/>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B45" s="101"/>
-      <c r="C45" s="106"/>
+      <c r="B45" s="97"/>
+      <c r="C45" s="116"/>
       <c r="D45" s="32" t="s">
         <v>59</v>
       </c>
@@ -3800,8 +3800,8 @@
       <c r="W45" s="19"/>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B46" s="101"/>
-      <c r="C46" s="106"/>
+      <c r="B46" s="97"/>
+      <c r="C46" s="116"/>
       <c r="D46" s="32" t="s">
         <v>60</v>
       </c>
@@ -3843,8 +3843,8 @@
       <c r="W46" s="19"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B47" s="101"/>
-      <c r="C47" s="106"/>
+      <c r="B47" s="97"/>
+      <c r="C47" s="116"/>
       <c r="D47" s="32" t="s">
         <v>61</v>
       </c>
@@ -3886,8 +3886,8 @@
       <c r="W47" s="19"/>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B48" s="101"/>
-      <c r="C48" s="106"/>
+      <c r="B48" s="97"/>
+      <c r="C48" s="116"/>
       <c r="D48" s="32" t="s">
         <v>62</v>
       </c>
@@ -3929,8 +3929,8 @@
       <c r="W48" s="19"/>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B49" s="101"/>
-      <c r="C49" s="106"/>
+      <c r="B49" s="97"/>
+      <c r="C49" s="116"/>
       <c r="D49" s="32" t="s">
         <v>63</v>
       </c>
@@ -3972,8 +3972,8 @@
       <c r="W49" s="19"/>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B50" s="101"/>
-      <c r="C50" s="106"/>
+      <c r="B50" s="97"/>
+      <c r="C50" s="116"/>
       <c r="D50" s="32" t="s">
         <v>64</v>
       </c>
@@ -4015,8 +4015,8 @@
       <c r="W50" s="19"/>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B51" s="101"/>
-      <c r="C51" s="106"/>
+      <c r="B51" s="97"/>
+      <c r="C51" s="116"/>
       <c r="D51" s="32" t="s">
         <v>65</v>
       </c>
@@ -4058,8 +4058,8 @@
       <c r="W51" s="19"/>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B52" s="101"/>
-      <c r="C52" s="106"/>
+      <c r="B52" s="97"/>
+      <c r="C52" s="116"/>
       <c r="D52" s="32" t="s">
         <v>66</v>
       </c>
@@ -4101,8 +4101,8 @@
       <c r="W52" s="19"/>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B53" s="101"/>
-      <c r="C53" s="106"/>
+      <c r="B53" s="97"/>
+      <c r="C53" s="116"/>
       <c r="D53" s="32" t="s">
         <v>67</v>
       </c>
@@ -4144,8 +4144,8 @@
       <c r="W53" s="19"/>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B54" s="101"/>
-      <c r="C54" s="106"/>
+      <c r="B54" s="97"/>
+      <c r="C54" s="116"/>
       <c r="D54" s="32" t="s">
         <v>68</v>
       </c>
@@ -4187,8 +4187,8 @@
       <c r="W54" s="19"/>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B55" s="101"/>
-      <c r="C55" s="107"/>
+      <c r="B55" s="97"/>
+      <c r="C55" s="117"/>
       <c r="D55" s="32" t="s">
         <v>69</v>
       </c>
@@ -4230,8 +4230,8 @@
       <c r="W55" s="19"/>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B56" s="101"/>
-      <c r="C56" s="103" t="s">
+      <c r="B56" s="97"/>
+      <c r="C56" s="113" t="s">
         <v>26</v>
       </c>
       <c r="D56" s="29" t="s">
@@ -4275,8 +4275,8 @@
       <c r="W56" s="19"/>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B57" s="101"/>
-      <c r="C57" s="104"/>
+      <c r="B57" s="97"/>
+      <c r="C57" s="114"/>
       <c r="D57" s="29" t="s">
         <v>29</v>
       </c>
@@ -4318,8 +4318,8 @@
       <c r="W57" s="19"/>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B58" s="101"/>
-      <c r="C58" s="104"/>
+      <c r="B58" s="97"/>
+      <c r="C58" s="114"/>
       <c r="D58" s="29" t="s">
         <v>30</v>
       </c>
@@ -4361,8 +4361,8 @@
       <c r="W58" s="19"/>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B59" s="101"/>
-      <c r="C59" s="104"/>
+      <c r="B59" s="97"/>
+      <c r="C59" s="114"/>
       <c r="D59" s="29" t="s">
         <v>31</v>
       </c>
@@ -4404,8 +4404,8 @@
       <c r="W59" s="19"/>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B60" s="101"/>
-      <c r="C60" s="104"/>
+      <c r="B60" s="97"/>
+      <c r="C60" s="114"/>
       <c r="D60" s="29" t="s">
         <v>34</v>
       </c>
@@ -4447,8 +4447,8 @@
       <c r="W60" s="19"/>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B61" s="101"/>
-      <c r="C61" s="104"/>
+      <c r="B61" s="97"/>
+      <c r="C61" s="114"/>
       <c r="D61" s="29" t="s">
         <v>32</v>
       </c>
@@ -4490,8 +4490,8 @@
       <c r="W61" s="19"/>
     </row>
     <row r="62" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="119"/>
-      <c r="C62" s="104"/>
+      <c r="B62" s="104"/>
+      <c r="C62" s="114"/>
       <c r="D62" s="62" t="s">
         <v>33</v>
       </c>
@@ -4533,10 +4533,10 @@
       <c r="W62" s="28"/>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B63" s="100" t="s">
+      <c r="B63" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="108" t="s">
+      <c r="C63" s="118" t="s">
         <v>79</v>
       </c>
       <c r="D63" s="39" t="s">
@@ -4580,8 +4580,8 @@
       <c r="W63" s="52"/>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B64" s="101"/>
-      <c r="C64" s="109"/>
+      <c r="B64" s="97"/>
+      <c r="C64" s="119"/>
       <c r="D64" s="4" t="s">
         <v>71</v>
       </c>
@@ -4623,8 +4623,8 @@
       <c r="W64" s="19"/>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B65" s="101"/>
-      <c r="C65" s="109"/>
+      <c r="B65" s="97"/>
+      <c r="C65" s="119"/>
       <c r="D65" s="4" t="s">
         <v>72</v>
       </c>
@@ -4666,8 +4666,8 @@
       <c r="W65" s="19"/>
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B66" s="101"/>
-      <c r="C66" s="109"/>
+      <c r="B66" s="97"/>
+      <c r="C66" s="119"/>
       <c r="D66" s="29" t="s">
         <v>76</v>
       </c>
@@ -4709,7 +4709,7 @@
       <c r="W66" s="19"/>
     </row>
     <row r="67" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B67" s="101"/>
+      <c r="B67" s="97"/>
       <c r="C67" s="33" t="s">
         <v>73</v>
       </c>
@@ -4752,7 +4752,7 @@
       <c r="W67" s="19"/>
     </row>
     <row r="68" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B68" s="101"/>
+      <c r="B68" s="97"/>
       <c r="C68" s="33" t="s">
         <v>81</v>
       </c>
@@ -4795,8 +4795,8 @@
       <c r="W68" s="19"/>
     </row>
     <row r="69" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="101"/>
-      <c r="C69" s="109" t="s">
+      <c r="B69" s="97"/>
+      <c r="C69" s="119" t="s">
         <v>80</v>
       </c>
       <c r="D69" s="4" t="s">
@@ -4840,8 +4840,8 @@
       <c r="W69" s="19"/>
     </row>
     <row r="70" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="101"/>
-      <c r="C70" s="109"/>
+      <c r="B70" s="97"/>
+      <c r="C70" s="119"/>
       <c r="D70" s="4" t="s">
         <v>75</v>
       </c>
@@ -4883,8 +4883,8 @@
       <c r="W70" s="19"/>
     </row>
     <row r="71" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="101"/>
-      <c r="C71" s="109"/>
+      <c r="B71" s="97"/>
+      <c r="C71" s="119"/>
       <c r="D71" s="4" t="s">
         <v>77</v>
       </c>
@@ -4926,8 +4926,8 @@
       <c r="W71" s="19"/>
     </row>
     <row r="72" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="102"/>
-      <c r="C72" s="110"/>
+      <c r="B72" s="98"/>
+      <c r="C72" s="120"/>
       <c r="D72" s="24" t="s">
         <v>78</v>
       </c>
@@ -4969,10 +4969,10 @@
       <c r="W72" s="25"/>
     </row>
     <row r="73" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="100" t="s">
+      <c r="B73" s="96" t="s">
         <v>115</v>
       </c>
-      <c r="C73" s="114" t="s">
+      <c r="C73" s="124" t="s">
         <v>116</v>
       </c>
       <c r="D73" s="39" t="s">
@@ -5016,8 +5016,8 @@
       <c r="W73" s="52"/>
     </row>
     <row r="74" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="101"/>
-      <c r="C74" s="96"/>
+      <c r="B74" s="97"/>
+      <c r="C74" s="109"/>
       <c r="D74" s="4" t="s">
         <v>132</v>
       </c>
@@ -5059,8 +5059,8 @@
       <c r="W74" s="19"/>
     </row>
     <row r="75" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="101"/>
-      <c r="C75" s="96"/>
+      <c r="B75" s="97"/>
+      <c r="C75" s="109"/>
       <c r="D75" s="4" t="s">
         <v>161</v>
       </c>
@@ -5094,8 +5094,8 @@
       <c r="W75" s="19"/>
     </row>
     <row r="76" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="101"/>
-      <c r="C76" s="96"/>
+      <c r="B76" s="97"/>
+      <c r="C76" s="109"/>
       <c r="D76" s="4" t="s">
         <v>133</v>
       </c>
@@ -5137,8 +5137,8 @@
       <c r="W76" s="95"/>
     </row>
     <row r="77" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="101"/>
-      <c r="C77" s="96"/>
+      <c r="B77" s="97"/>
+      <c r="C77" s="109"/>
       <c r="D77" s="4" t="s">
         <v>134</v>
       </c>
@@ -5180,8 +5180,8 @@
       <c r="W77" s="19"/>
     </row>
     <row r="78" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="101"/>
-      <c r="C78" s="96" t="s">
+      <c r="B78" s="97"/>
+      <c r="C78" s="109" t="s">
         <v>117</v>
       </c>
       <c r="D78" s="4" t="s">
@@ -5225,8 +5225,8 @@
       <c r="W78" s="19"/>
     </row>
     <row r="79" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="101"/>
-      <c r="C79" s="96"/>
+      <c r="B79" s="97"/>
+      <c r="C79" s="109"/>
       <c r="D79" s="4" t="s">
         <v>132</v>
       </c>
@@ -5268,8 +5268,8 @@
       <c r="W79" s="19"/>
     </row>
     <row r="80" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="101"/>
-      <c r="C80" s="96"/>
+      <c r="B80" s="97"/>
+      <c r="C80" s="109"/>
       <c r="D80" s="4" t="s">
         <v>161</v>
       </c>
@@ -5303,8 +5303,8 @@
       <c r="W80" s="19"/>
     </row>
     <row r="81" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="101"/>
-      <c r="C81" s="96"/>
+      <c r="B81" s="97"/>
+      <c r="C81" s="109"/>
       <c r="D81" s="4" t="s">
         <v>133</v>
       </c>
@@ -5348,8 +5348,8 @@
       <c r="W81" s="95"/>
     </row>
     <row r="82" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="101"/>
-      <c r="C82" s="96"/>
+      <c r="B82" s="97"/>
+      <c r="C82" s="109"/>
       <c r="D82" s="4" t="s">
         <v>134</v>
       </c>
@@ -5391,8 +5391,8 @@
       <c r="W82" s="19"/>
     </row>
     <row r="83" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="101"/>
-      <c r="C83" s="96" t="s">
+      <c r="B83" s="97"/>
+      <c r="C83" s="109" t="s">
         <v>118</v>
       </c>
       <c r="D83" s="4" t="s">
@@ -5436,8 +5436,8 @@
       <c r="W83" s="19"/>
     </row>
     <row r="84" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="101"/>
-      <c r="C84" s="96"/>
+      <c r="B84" s="97"/>
+      <c r="C84" s="109"/>
       <c r="D84" s="4" t="s">
         <v>132</v>
       </c>
@@ -5479,8 +5479,8 @@
       <c r="W84" s="19"/>
     </row>
     <row r="85" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="101"/>
-      <c r="C85" s="96"/>
+      <c r="B85" s="97"/>
+      <c r="C85" s="109"/>
       <c r="D85" s="4" t="s">
         <v>161</v>
       </c>
@@ -5514,8 +5514,8 @@
       <c r="W85" s="19"/>
     </row>
     <row r="86" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="101"/>
-      <c r="C86" s="96"/>
+      <c r="B86" s="97"/>
+      <c r="C86" s="109"/>
       <c r="D86" s="4" t="s">
         <v>133</v>
       </c>
@@ -5559,8 +5559,8 @@
       <c r="W86" s="95"/>
     </row>
     <row r="87" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="101"/>
-      <c r="C87" s="96"/>
+      <c r="B87" s="97"/>
+      <c r="C87" s="109"/>
       <c r="D87" s="4" t="s">
         <v>134</v>
       </c>
@@ -5602,8 +5602,8 @@
       <c r="W87" s="19"/>
     </row>
     <row r="88" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="101"/>
-      <c r="C88" s="96" t="s">
+      <c r="B88" s="97"/>
+      <c r="C88" s="109" t="s">
         <v>119</v>
       </c>
       <c r="D88" s="4" t="s">
@@ -5647,8 +5647,8 @@
       <c r="W88" s="19"/>
     </row>
     <row r="89" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="101"/>
-      <c r="C89" s="96"/>
+      <c r="B89" s="97"/>
+      <c r="C89" s="109"/>
       <c r="D89" s="4" t="s">
         <v>132</v>
       </c>
@@ -5690,8 +5690,8 @@
       <c r="W89" s="19"/>
     </row>
     <row r="90" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="101"/>
-      <c r="C90" s="96"/>
+      <c r="B90" s="97"/>
+      <c r="C90" s="109"/>
       <c r="D90" s="4" t="s">
         <v>161</v>
       </c>
@@ -5725,8 +5725,8 @@
       <c r="W90" s="19"/>
     </row>
     <row r="91" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="101"/>
-      <c r="C91" s="96"/>
+      <c r="B91" s="97"/>
+      <c r="C91" s="109"/>
       <c r="D91" s="4" t="s">
         <v>133</v>
       </c>
@@ -5770,8 +5770,8 @@
       <c r="W91" s="95"/>
     </row>
     <row r="92" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="101"/>
-      <c r="C92" s="96"/>
+      <c r="B92" s="97"/>
+      <c r="C92" s="109"/>
       <c r="D92" s="4" t="s">
         <v>134</v>
       </c>
@@ -5813,8 +5813,8 @@
       <c r="W92" s="19"/>
     </row>
     <row r="93" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="101"/>
-      <c r="C93" s="96" t="s">
+      <c r="B93" s="97"/>
+      <c r="C93" s="109" t="s">
         <v>120</v>
       </c>
       <c r="D93" s="4" t="s">
@@ -5858,8 +5858,8 @@
       <c r="W93" s="19"/>
     </row>
     <row r="94" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="101"/>
-      <c r="C94" s="96"/>
+      <c r="B94" s="97"/>
+      <c r="C94" s="109"/>
       <c r="D94" s="4" t="s">
         <v>132</v>
       </c>
@@ -5901,8 +5901,8 @@
       <c r="W94" s="19"/>
     </row>
     <row r="95" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="101"/>
-      <c r="C95" s="96"/>
+      <c r="B95" s="97"/>
+      <c r="C95" s="109"/>
       <c r="D95" s="4" t="s">
         <v>161</v>
       </c>
@@ -5936,8 +5936,8 @@
       <c r="W95" s="19"/>
     </row>
     <row r="96" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="101"/>
-      <c r="C96" s="96"/>
+      <c r="B96" s="97"/>
+      <c r="C96" s="109"/>
       <c r="D96" s="4" t="s">
         <v>133</v>
       </c>
@@ -5981,8 +5981,8 @@
       <c r="W96" s="95"/>
     </row>
     <row r="97" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="101"/>
-      <c r="C97" s="96"/>
+      <c r="B97" s="97"/>
+      <c r="C97" s="109"/>
       <c r="D97" s="4" t="s">
         <v>134</v>
       </c>
@@ -6024,8 +6024,8 @@
       <c r="W97" s="19"/>
     </row>
     <row r="98" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="101"/>
-      <c r="C98" s="96" t="s">
+      <c r="B98" s="97"/>
+      <c r="C98" s="109" t="s">
         <v>121</v>
       </c>
       <c r="D98" s="4" t="s">
@@ -6069,8 +6069,8 @@
       <c r="W98" s="19"/>
     </row>
     <row r="99" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="101"/>
-      <c r="C99" s="96"/>
+      <c r="B99" s="97"/>
+      <c r="C99" s="109"/>
       <c r="D99" s="4" t="s">
         <v>132</v>
       </c>
@@ -6112,8 +6112,8 @@
       <c r="W99" s="19"/>
     </row>
     <row r="100" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="101"/>
-      <c r="C100" s="96"/>
+      <c r="B100" s="97"/>
+      <c r="C100" s="109"/>
       <c r="D100" s="4" t="s">
         <v>161</v>
       </c>
@@ -6147,8 +6147,8 @@
       <c r="W100" s="19"/>
     </row>
     <row r="101" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="101"/>
-      <c r="C101" s="96"/>
+      <c r="B101" s="97"/>
+      <c r="C101" s="109"/>
       <c r="D101" s="4" t="s">
         <v>133</v>
       </c>
@@ -6192,8 +6192,8 @@
       <c r="W101" s="95"/>
     </row>
     <row r="102" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="101"/>
-      <c r="C102" s="96"/>
+      <c r="B102" s="97"/>
+      <c r="C102" s="109"/>
       <c r="D102" s="4" t="s">
         <v>134</v>
       </c>
@@ -6235,8 +6235,8 @@
       <c r="W102" s="19"/>
     </row>
     <row r="103" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="101"/>
-      <c r="C103" s="96" t="s">
+      <c r="B103" s="97"/>
+      <c r="C103" s="109" t="s">
         <v>122</v>
       </c>
       <c r="D103" s="4" t="s">
@@ -6280,8 +6280,8 @@
       <c r="W103" s="19"/>
     </row>
     <row r="104" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="101"/>
-      <c r="C104" s="96"/>
+      <c r="B104" s="97"/>
+      <c r="C104" s="109"/>
       <c r="D104" s="4" t="s">
         <v>132</v>
       </c>
@@ -6323,8 +6323,8 @@
       <c r="W104" s="19"/>
     </row>
     <row r="105" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="101"/>
-      <c r="C105" s="96"/>
+      <c r="B105" s="97"/>
+      <c r="C105" s="109"/>
       <c r="D105" s="4" t="s">
         <v>161</v>
       </c>
@@ -6358,8 +6358,8 @@
       <c r="W105" s="19"/>
     </row>
     <row r="106" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="101"/>
-      <c r="C106" s="96"/>
+      <c r="B106" s="97"/>
+      <c r="C106" s="109"/>
       <c r="D106" s="4" t="s">
         <v>133</v>
       </c>
@@ -6403,8 +6403,8 @@
       <c r="W106" s="95"/>
     </row>
     <row r="107" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="101"/>
-      <c r="C107" s="96"/>
+      <c r="B107" s="97"/>
+      <c r="C107" s="109"/>
       <c r="D107" s="4" t="s">
         <v>134</v>
       </c>
@@ -6446,8 +6446,8 @@
       <c r="W107" s="19"/>
     </row>
     <row r="108" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="101"/>
-      <c r="C108" s="96" t="s">
+      <c r="B108" s="97"/>
+      <c r="C108" s="109" t="s">
         <v>123</v>
       </c>
       <c r="D108" s="4" t="s">
@@ -6491,8 +6491,8 @@
       <c r="W108" s="19"/>
     </row>
     <row r="109" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="101"/>
-      <c r="C109" s="96"/>
+      <c r="B109" s="97"/>
+      <c r="C109" s="109"/>
       <c r="D109" s="4" t="s">
         <v>132</v>
       </c>
@@ -6534,8 +6534,8 @@
       <c r="W109" s="19"/>
     </row>
     <row r="110" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="101"/>
-      <c r="C110" s="96"/>
+      <c r="B110" s="97"/>
+      <c r="C110" s="109"/>
       <c r="D110" s="4" t="s">
         <v>161</v>
       </c>
@@ -6569,8 +6569,8 @@
       <c r="W110" s="19"/>
     </row>
     <row r="111" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="101"/>
-      <c r="C111" s="96"/>
+      <c r="B111" s="97"/>
+      <c r="C111" s="109"/>
       <c r="D111" s="4" t="s">
         <v>133</v>
       </c>
@@ -6614,8 +6614,8 @@
       <c r="W111" s="95"/>
     </row>
     <row r="112" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="101"/>
-      <c r="C112" s="96"/>
+      <c r="B112" s="97"/>
+      <c r="C112" s="109"/>
       <c r="D112" s="4" t="s">
         <v>134</v>
       </c>
@@ -6657,8 +6657,8 @@
       <c r="W112" s="19"/>
     </row>
     <row r="113" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="101"/>
-      <c r="C113" s="96" t="s">
+      <c r="B113" s="97"/>
+      <c r="C113" s="109" t="s">
         <v>124</v>
       </c>
       <c r="D113" s="4" t="s">
@@ -6702,8 +6702,8 @@
       <c r="W113" s="19"/>
     </row>
     <row r="114" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="101"/>
-      <c r="C114" s="96"/>
+      <c r="B114" s="97"/>
+      <c r="C114" s="109"/>
       <c r="D114" s="4" t="s">
         <v>132</v>
       </c>
@@ -6745,8 +6745,8 @@
       <c r="W114" s="19"/>
     </row>
     <row r="115" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="101"/>
-      <c r="C115" s="96"/>
+      <c r="B115" s="97"/>
+      <c r="C115" s="109"/>
       <c r="D115" s="4" t="s">
         <v>161</v>
       </c>
@@ -6780,8 +6780,8 @@
       <c r="W115" s="19"/>
     </row>
     <row r="116" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="101"/>
-      <c r="C116" s="96"/>
+      <c r="B116" s="97"/>
+      <c r="C116" s="109"/>
       <c r="D116" s="4" t="s">
         <v>133</v>
       </c>
@@ -6825,8 +6825,8 @@
       <c r="W116" s="95"/>
     </row>
     <row r="117" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="101"/>
-      <c r="C117" s="96"/>
+      <c r="B117" s="97"/>
+      <c r="C117" s="109"/>
       <c r="D117" s="4" t="s">
         <v>134</v>
       </c>
@@ -6868,8 +6868,8 @@
       <c r="W117" s="19"/>
     </row>
     <row r="118" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="101"/>
-      <c r="C118" s="96" t="s">
+      <c r="B118" s="97"/>
+      <c r="C118" s="109" t="s">
         <v>125</v>
       </c>
       <c r="D118" s="4" t="s">
@@ -6913,8 +6913,8 @@
       <c r="W118" s="19"/>
     </row>
     <row r="119" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="101"/>
-      <c r="C119" s="96"/>
+      <c r="B119" s="97"/>
+      <c r="C119" s="109"/>
       <c r="D119" s="4" t="s">
         <v>132</v>
       </c>
@@ -6956,8 +6956,8 @@
       <c r="W119" s="19"/>
     </row>
     <row r="120" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="101"/>
-      <c r="C120" s="96"/>
+      <c r="B120" s="97"/>
+      <c r="C120" s="109"/>
       <c r="D120" s="4" t="s">
         <v>161</v>
       </c>
@@ -6991,8 +6991,8 @@
       <c r="W120" s="19"/>
     </row>
     <row r="121" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="101"/>
-      <c r="C121" s="96"/>
+      <c r="B121" s="97"/>
+      <c r="C121" s="109"/>
       <c r="D121" s="4" t="s">
         <v>133</v>
       </c>
@@ -7036,8 +7036,8 @@
       <c r="W121" s="95"/>
     </row>
     <row r="122" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="101"/>
-      <c r="C122" s="96"/>
+      <c r="B122" s="97"/>
+      <c r="C122" s="109"/>
       <c r="D122" s="4" t="s">
         <v>134</v>
       </c>
@@ -7079,8 +7079,8 @@
       <c r="W122" s="19"/>
     </row>
     <row r="123" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="101"/>
-      <c r="C123" s="96" t="s">
+      <c r="B123" s="97"/>
+      <c r="C123" s="109" t="s">
         <v>126</v>
       </c>
       <c r="D123" s="4" t="s">
@@ -7124,8 +7124,8 @@
       <c r="W123" s="19"/>
     </row>
     <row r="124" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="101"/>
-      <c r="C124" s="96"/>
+      <c r="B124" s="97"/>
+      <c r="C124" s="109"/>
       <c r="D124" s="4" t="s">
         <v>132</v>
       </c>
@@ -7167,8 +7167,8 @@
       <c r="W124" s="19"/>
     </row>
     <row r="125" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="101"/>
-      <c r="C125" s="96"/>
+      <c r="B125" s="97"/>
+      <c r="C125" s="109"/>
       <c r="D125" s="4" t="s">
         <v>161</v>
       </c>
@@ -7202,8 +7202,8 @@
       <c r="W125" s="19"/>
     </row>
     <row r="126" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="101"/>
-      <c r="C126" s="96"/>
+      <c r="B126" s="97"/>
+      <c r="C126" s="109"/>
       <c r="D126" s="4" t="s">
         <v>133</v>
       </c>
@@ -7247,8 +7247,8 @@
       <c r="W126" s="95"/>
     </row>
     <row r="127" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="101"/>
-      <c r="C127" s="96"/>
+      <c r="B127" s="97"/>
+      <c r="C127" s="109"/>
       <c r="D127" s="4" t="s">
         <v>134</v>
       </c>
@@ -7290,8 +7290,8 @@
       <c r="W127" s="19"/>
     </row>
     <row r="128" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="101"/>
-      <c r="C128" s="96" t="s">
+      <c r="B128" s="97"/>
+      <c r="C128" s="109" t="s">
         <v>127</v>
       </c>
       <c r="D128" s="4" t="s">
@@ -7335,8 +7335,8 @@
       <c r="W128" s="19"/>
     </row>
     <row r="129" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="101"/>
-      <c r="C129" s="96"/>
+      <c r="B129" s="97"/>
+      <c r="C129" s="109"/>
       <c r="D129" s="4" t="s">
         <v>132</v>
       </c>
@@ -7378,8 +7378,8 @@
       <c r="W129" s="19"/>
     </row>
     <row r="130" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="101"/>
-      <c r="C130" s="96"/>
+      <c r="B130" s="97"/>
+      <c r="C130" s="109"/>
       <c r="D130" s="4" t="s">
         <v>161</v>
       </c>
@@ -7413,8 +7413,8 @@
       <c r="W130" s="19"/>
     </row>
     <row r="131" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="101"/>
-      <c r="C131" s="96"/>
+      <c r="B131" s="97"/>
+      <c r="C131" s="109"/>
       <c r="D131" s="4" t="s">
         <v>133</v>
       </c>
@@ -7458,8 +7458,8 @@
       <c r="W131" s="95"/>
     </row>
     <row r="132" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="101"/>
-      <c r="C132" s="96"/>
+      <c r="B132" s="97"/>
+      <c r="C132" s="109"/>
       <c r="D132" s="4" t="s">
         <v>134</v>
       </c>
@@ -7501,8 +7501,8 @@
       <c r="W132" s="19"/>
     </row>
     <row r="133" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="101"/>
-      <c r="C133" s="96" t="s">
+      <c r="B133" s="97"/>
+      <c r="C133" s="109" t="s">
         <v>128</v>
       </c>
       <c r="D133" s="4" t="s">
@@ -7546,8 +7546,8 @@
       <c r="W133" s="19"/>
     </row>
     <row r="134" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="101"/>
-      <c r="C134" s="96"/>
+      <c r="B134" s="97"/>
+      <c r="C134" s="109"/>
       <c r="D134" s="4" t="s">
         <v>132</v>
       </c>
@@ -7589,8 +7589,8 @@
       <c r="W134" s="19"/>
     </row>
     <row r="135" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="101"/>
-      <c r="C135" s="96"/>
+      <c r="B135" s="97"/>
+      <c r="C135" s="109"/>
       <c r="D135" s="4" t="s">
         <v>161</v>
       </c>
@@ -7624,8 +7624,8 @@
       <c r="W135" s="19"/>
     </row>
     <row r="136" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="101"/>
-      <c r="C136" s="96"/>
+      <c r="B136" s="97"/>
+      <c r="C136" s="109"/>
       <c r="D136" s="4" t="s">
         <v>133</v>
       </c>
@@ -7669,8 +7669,8 @@
       <c r="W136" s="95"/>
     </row>
     <row r="137" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="101"/>
-      <c r="C137" s="96"/>
+      <c r="B137" s="97"/>
+      <c r="C137" s="109"/>
       <c r="D137" s="4" t="s">
         <v>134</v>
       </c>
@@ -7712,8 +7712,8 @@
       <c r="W137" s="19"/>
     </row>
     <row r="138" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="101"/>
-      <c r="C138" s="96" t="s">
+      <c r="B138" s="97"/>
+      <c r="C138" s="109" t="s">
         <v>129</v>
       </c>
       <c r="D138" s="4" t="s">
@@ -7757,8 +7757,8 @@
       <c r="W138" s="19"/>
     </row>
     <row r="139" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="101"/>
-      <c r="C139" s="96"/>
+      <c r="B139" s="97"/>
+      <c r="C139" s="109"/>
       <c r="D139" s="4" t="s">
         <v>132</v>
       </c>
@@ -7800,8 +7800,8 @@
       <c r="W139" s="19"/>
     </row>
     <row r="140" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="101"/>
-      <c r="C140" s="96"/>
+      <c r="B140" s="97"/>
+      <c r="C140" s="109"/>
       <c r="D140" s="4" t="s">
         <v>161</v>
       </c>
@@ -7835,8 +7835,8 @@
       <c r="W140" s="19"/>
     </row>
     <row r="141" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="101"/>
-      <c r="C141" s="96"/>
+      <c r="B141" s="97"/>
+      <c r="C141" s="109"/>
       <c r="D141" s="4" t="s">
         <v>133</v>
       </c>
@@ -7880,8 +7880,8 @@
       <c r="W141" s="95"/>
     </row>
     <row r="142" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="101"/>
-      <c r="C142" s="96"/>
+      <c r="B142" s="97"/>
+      <c r="C142" s="109"/>
       <c r="D142" s="4" t="s">
         <v>134</v>
       </c>
@@ -7923,8 +7923,8 @@
       <c r="W142" s="19"/>
     </row>
     <row r="143" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="101"/>
-      <c r="C143" s="96" t="s">
+      <c r="B143" s="97"/>
+      <c r="C143" s="109" t="s">
         <v>130</v>
       </c>
       <c r="D143" s="4" t="s">
@@ -7968,8 +7968,8 @@
       <c r="W143" s="19"/>
     </row>
     <row r="144" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="101"/>
-      <c r="C144" s="96"/>
+      <c r="B144" s="97"/>
+      <c r="C144" s="109"/>
       <c r="D144" s="4" t="s">
         <v>132</v>
       </c>
@@ -8011,8 +8011,8 @@
       <c r="W144" s="19"/>
     </row>
     <row r="145" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="101"/>
-      <c r="C145" s="96"/>
+      <c r="B145" s="97"/>
+      <c r="C145" s="109"/>
       <c r="D145" s="4" t="s">
         <v>161</v>
       </c>
@@ -8046,8 +8046,8 @@
       <c r="W145" s="19"/>
     </row>
     <row r="146" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="101"/>
-      <c r="C146" s="96"/>
+      <c r="B146" s="97"/>
+      <c r="C146" s="109"/>
       <c r="D146" s="4" t="s">
         <v>133</v>
       </c>
@@ -8091,8 +8091,8 @@
       <c r="W146" s="95"/>
     </row>
     <row r="147" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B147" s="102"/>
-      <c r="C147" s="124"/>
+      <c r="B147" s="98"/>
+      <c r="C147" s="112"/>
       <c r="D147" s="24" t="s">
         <v>134</v>
       </c>
@@ -8134,7 +8134,7 @@
       <c r="W147" s="25"/>
     </row>
     <row r="148" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="100" t="s">
+      <c r="B148" s="96" t="s">
         <v>83</v>
       </c>
       <c r="C148" s="78" t="s">
@@ -8179,7 +8179,7 @@
       <c r="W148" s="52"/>
     </row>
     <row r="149" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="101"/>
+      <c r="B149" s="97"/>
       <c r="C149" s="33" t="s">
         <v>89</v>
       </c>
@@ -8222,7 +8222,7 @@
       <c r="W149" s="19"/>
     </row>
     <row r="150" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="101"/>
+      <c r="B150" s="97"/>
       <c r="C150" s="33" t="s">
         <v>90</v>
       </c>
@@ -8265,7 +8265,7 @@
       <c r="W150" s="19"/>
     </row>
     <row r="151" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="101"/>
+      <c r="B151" s="97"/>
       <c r="C151" s="33" t="s">
         <v>91</v>
       </c>
@@ -8308,7 +8308,7 @@
       <c r="W151" s="19"/>
     </row>
     <row r="152" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="101"/>
+      <c r="B152" s="97"/>
       <c r="C152" s="33" t="s">
         <v>141</v>
       </c>
@@ -8351,7 +8351,7 @@
       <c r="W152" s="19"/>
     </row>
     <row r="153" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="101"/>
+      <c r="B153" s="97"/>
       <c r="C153" s="33" t="s">
         <v>138</v>
       </c>
@@ -8394,7 +8394,7 @@
       <c r="W153" s="19"/>
     </row>
     <row r="154" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="101"/>
+      <c r="B154" s="97"/>
       <c r="C154" s="33" t="s">
         <v>140</v>
       </c>
@@ -8437,7 +8437,7 @@
       <c r="W154" s="19"/>
     </row>
     <row r="155" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="101"/>
+      <c r="B155" s="97"/>
       <c r="C155" s="33" t="s">
         <v>139</v>
       </c>
@@ -8480,7 +8480,7 @@
       <c r="W155" s="19"/>
     </row>
     <row r="156" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="101"/>
+      <c r="B156" s="97"/>
       <c r="C156" s="33" t="s">
         <v>92</v>
       </c>
@@ -8499,7 +8499,7 @@
       </c>
       <c r="I156" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="J156" s="70">
         <v>0</v>
@@ -8510,20 +8510,42 @@
       <c r="L156" s="70">
         <v>0</v>
       </c>
-      <c r="M156" s="4"/>
-      <c r="N156" s="4"/>
-      <c r="O156" s="17"/>
-      <c r="P156" s="16"/>
-      <c r="Q156" s="17"/>
-      <c r="R156" s="17"/>
-      <c r="S156" s="17"/>
-      <c r="T156" s="17"/>
-      <c r="U156" s="17"/>
-      <c r="V156" s="17"/>
-      <c r="W156" s="19"/>
+      <c r="M156" s="80">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="N156" s="80">
+        <v>0</v>
+      </c>
+      <c r="O156" s="80">
+        <v>0</v>
+      </c>
+      <c r="P156" s="80">
+        <v>0</v>
+      </c>
+      <c r="Q156" s="80">
+        <v>0</v>
+      </c>
+      <c r="R156" s="80">
+        <v>0</v>
+      </c>
+      <c r="S156" s="80">
+        <v>0</v>
+      </c>
+      <c r="T156" s="80">
+        <v>0</v>
+      </c>
+      <c r="U156" s="80">
+        <v>0</v>
+      </c>
+      <c r="V156" s="80">
+        <v>0</v>
+      </c>
+      <c r="W156" s="80">
+        <v>0</v>
+      </c>
     </row>
     <row r="157" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="101"/>
+      <c r="B157" s="97"/>
       <c r="C157" s="33" t="s">
         <v>93</v>
       </c>
@@ -8588,7 +8610,7 @@
       </c>
     </row>
     <row r="158" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="101"/>
+      <c r="B158" s="97"/>
       <c r="C158" s="33" t="s">
         <v>94</v>
       </c>
@@ -8607,7 +8629,7 @@
       </c>
       <c r="I158" s="6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="J158" s="70">
         <v>0</v>
@@ -8618,20 +8640,42 @@
       <c r="L158" s="70">
         <v>0</v>
       </c>
-      <c r="M158" s="4"/>
-      <c r="N158" s="4"/>
-      <c r="O158" s="17"/>
-      <c r="P158" s="16"/>
-      <c r="Q158" s="17"/>
-      <c r="R158" s="17"/>
-      <c r="S158" s="17"/>
-      <c r="T158" s="17"/>
-      <c r="U158" s="17"/>
-      <c r="V158" s="17"/>
-      <c r="W158" s="19"/>
+      <c r="M158" s="80">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="N158" s="80">
+        <v>0</v>
+      </c>
+      <c r="O158" s="80">
+        <v>0</v>
+      </c>
+      <c r="P158" s="80">
+        <v>0</v>
+      </c>
+      <c r="Q158" s="80">
+        <v>0</v>
+      </c>
+      <c r="R158" s="80">
+        <v>0</v>
+      </c>
+      <c r="S158" s="80">
+        <v>0</v>
+      </c>
+      <c r="T158" s="80">
+        <v>0</v>
+      </c>
+      <c r="U158" s="80">
+        <v>0</v>
+      </c>
+      <c r="V158" s="80">
+        <v>0</v>
+      </c>
+      <c r="W158" s="80">
+        <v>0</v>
+      </c>
     </row>
     <row r="159" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="101"/>
+      <c r="B159" s="97"/>
       <c r="C159" s="33" t="s">
         <v>98</v>
       </c>
@@ -8674,7 +8718,7 @@
       <c r="W159" s="19"/>
     </row>
     <row r="160" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B160" s="102"/>
+      <c r="B160" s="98"/>
       <c r="C160" s="61" t="s">
         <v>99</v>
       </c>
@@ -8717,7 +8761,7 @@
       <c r="W160" s="25"/>
     </row>
     <row r="161" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="100" t="s">
+      <c r="B161" s="96" t="s">
         <v>142</v>
       </c>
       <c r="C161" s="60" t="s">
@@ -8762,7 +8806,7 @@
       <c r="W161" s="52"/>
     </row>
     <row r="162" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="101"/>
+      <c r="B162" s="97"/>
       <c r="C162" s="59" t="s">
         <v>143</v>
       </c>
@@ -8805,7 +8849,7 @@
       <c r="W162" s="19"/>
     </row>
     <row r="163" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B163" s="102"/>
+      <c r="B163" s="98"/>
       <c r="C163" s="61" t="s">
         <v>144</v>
       </c>
@@ -8848,7 +8892,7 @@
       <c r="W163" s="25"/>
     </row>
     <row r="164" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="100" t="s">
+      <c r="B164" s="96" t="s">
         <v>147</v>
       </c>
       <c r="C164" s="60" t="s">
@@ -8893,7 +8937,7 @@
       <c r="W164" s="52"/>
     </row>
     <row r="165" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="101"/>
+      <c r="B165" s="97"/>
       <c r="C165" s="59" t="s">
         <v>149</v>
       </c>
@@ -8936,7 +8980,7 @@
       <c r="W165" s="19"/>
     </row>
     <row r="166" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B166" s="101"/>
+      <c r="B166" s="97"/>
       <c r="C166" s="59" t="s">
         <v>150</v>
       </c>
@@ -8979,7 +9023,7 @@
       <c r="W166" s="19"/>
     </row>
     <row r="167" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B167" s="101"/>
+      <c r="B167" s="97"/>
       <c r="C167" s="59" t="s">
         <v>151</v>
       </c>
@@ -9022,7 +9066,7 @@
       <c r="W167" s="19"/>
     </row>
     <row r="168" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B168" s="101"/>
+      <c r="B168" s="97"/>
       <c r="C168" s="59" t="s">
         <v>152</v>
       </c>
@@ -9065,7 +9109,7 @@
       <c r="W168" s="19"/>
     </row>
     <row r="169" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B169" s="101"/>
+      <c r="B169" s="97"/>
       <c r="C169" s="59" t="s">
         <v>153</v>
       </c>
@@ -9108,7 +9152,7 @@
       <c r="W169" s="19"/>
     </row>
     <row r="170" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B170" s="102"/>
+      <c r="B170" s="98"/>
       <c r="C170" s="61" t="s">
         <v>154</v>
       </c>
@@ -9151,7 +9195,7 @@
       <c r="W170" s="25"/>
     </row>
     <row r="171" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B171" s="100" t="s">
+      <c r="B171" s="96" t="s">
         <v>18</v>
       </c>
       <c r="C171" s="54" t="s">
@@ -9196,7 +9240,7 @@
       <c r="W171" s="52"/>
     </row>
     <row r="172" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="101"/>
+      <c r="B172" s="97"/>
       <c r="C172" s="33" t="s">
         <v>136</v>
       </c>
@@ -9239,7 +9283,7 @@
       <c r="W172" s="19"/>
     </row>
     <row r="173" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B173" s="101"/>
+      <c r="B173" s="97"/>
       <c r="C173" s="33" t="s">
         <v>137</v>
       </c>
@@ -9282,7 +9326,7 @@
       <c r="W173" s="19"/>
     </row>
     <row r="174" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="101"/>
+      <c r="B174" s="97"/>
       <c r="C174" s="33" t="s">
         <v>145</v>
       </c>
@@ -9325,7 +9369,7 @@
       <c r="W174" s="19"/>
     </row>
     <row r="175" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="101"/>
+      <c r="B175" s="97"/>
       <c r="C175" s="33" t="s">
         <v>84</v>
       </c>
@@ -9368,7 +9412,7 @@
       <c r="W175" s="19"/>
     </row>
     <row r="176" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="101"/>
+      <c r="B176" s="97"/>
       <c r="C176" s="33" t="s">
         <v>85</v>
       </c>
@@ -9411,7 +9455,7 @@
       <c r="W176" s="19"/>
     </row>
     <row r="177" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B177" s="101"/>
+      <c r="B177" s="97"/>
       <c r="C177" s="33" t="s">
         <v>87</v>
       </c>
@@ -9454,7 +9498,7 @@
       <c r="W177" s="19"/>
     </row>
     <row r="178" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B178" s="101"/>
+      <c r="B178" s="97"/>
       <c r="C178" s="33" t="s">
         <v>86</v>
       </c>
@@ -9497,7 +9541,7 @@
       <c r="W178" s="19"/>
     </row>
     <row r="179" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B179" s="101"/>
+      <c r="B179" s="97"/>
       <c r="C179" s="33" t="s">
         <v>103</v>
       </c>
@@ -9540,7 +9584,7 @@
       <c r="W179" s="19"/>
     </row>
     <row r="180" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B180" s="101"/>
+      <c r="B180" s="97"/>
       <c r="C180" s="33" t="s">
         <v>135</v>
       </c>
@@ -9583,7 +9627,7 @@
       <c r="W180" s="19"/>
     </row>
     <row r="181" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B181" s="101"/>
+      <c r="B181" s="97"/>
       <c r="C181" s="33" t="s">
         <v>104</v>
       </c>
@@ -9626,76 +9670,76 @@
       <c r="W181" s="19"/>
     </row>
     <row r="182" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B182" s="120" t="s">
+      <c r="B182" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="C182" s="121"/>
-      <c r="D182" s="122"/>
-      <c r="E182" s="122"/>
-      <c r="F182" s="122"/>
-      <c r="G182" s="123"/>
+      <c r="C182" s="106"/>
+      <c r="D182" s="107"/>
+      <c r="E182" s="107"/>
+      <c r="F182" s="107"/>
+      <c r="G182" s="108"/>
       <c r="H182" s="36">
-        <f>SUM(H4:H181)</f>
+        <f t="shared" ref="H182:W182" si="6">SUM(H4:H181)</f>
         <v>95.999999999999829</v>
       </c>
       <c r="I182" s="23">
-        <f>SUM(I4:I181)</f>
-        <v>10.733299999999996</v>
+        <f t="shared" si="6"/>
+        <v>10.967299999999998</v>
       </c>
       <c r="J182" s="23">
-        <f>SUM(J4:J181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K182" s="23">
-        <f>SUM(K4:K181)</f>
+        <f t="shared" si="6"/>
         <v>4.0533000000000001</v>
       </c>
       <c r="L182" s="92">
-        <f>SUM(L4:L181)</f>
+        <f t="shared" si="6"/>
         <v>2.0030000000000001</v>
       </c>
       <c r="M182" s="23">
-        <f>SUM(M4:M181)</f>
-        <v>4.6769999999999969</v>
+        <f t="shared" si="6"/>
+        <v>4.9109999999999969</v>
       </c>
       <c r="N182" s="23">
-        <f>SUM(N4:N181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O182" s="23">
-        <f>SUM(O4:O181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P182" s="23">
-        <f>SUM(P4:P181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q182" s="23">
-        <f>SUM(Q4:Q181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R182" s="23">
-        <f>SUM(R4:R181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S182" s="23">
-        <f>SUM(S4:S181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T182" s="23">
-        <f>SUM(T4:T181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U182" s="23">
-        <f>SUM(U4:U181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V182" s="23">
-        <f>SUM(V4:V181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="W182" s="30">
-        <f>SUM(W4:W181)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -9708,22 +9752,22 @@
       <c r="G183" s="2"/>
       <c r="H183" s="2"/>
       <c r="I183" s="2"/>
-      <c r="J183" s="97" t="s">
+      <c r="J183" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="K183" s="98"/>
-      <c r="L183" s="98"/>
-      <c r="M183" s="98"/>
-      <c r="N183" s="98"/>
-      <c r="O183" s="98"/>
-      <c r="P183" s="98"/>
-      <c r="Q183" s="98"/>
-      <c r="R183" s="98"/>
-      <c r="S183" s="98"/>
-      <c r="T183" s="98"/>
-      <c r="U183" s="98"/>
-      <c r="V183" s="98"/>
-      <c r="W183" s="99"/>
+      <c r="K183" s="110"/>
+      <c r="L183" s="110"/>
+      <c r="M183" s="110"/>
+      <c r="N183" s="110"/>
+      <c r="O183" s="110"/>
+      <c r="P183" s="110"/>
+      <c r="Q183" s="110"/>
+      <c r="R183" s="110"/>
+      <c r="S183" s="110"/>
+      <c r="T183" s="110"/>
+      <c r="U183" s="110"/>
+      <c r="V183" s="110"/>
+      <c r="W183" s="111"/>
     </row>
     <row r="184" spans="2:23" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C184" s="59" t="s">
@@ -9755,18 +9799,18 @@
       </c>
       <c r="D185" s="4">
         <f>SUM(I10,I12,I13,I14,I15:I62,I156:I158,I160,I164:I170,I176:I177,I180)</f>
-        <v>9.1532999999999998</v>
+        <v>9.3872999999999998</v>
       </c>
       <c r="E185" s="4">
         <f>SUM(C185,-D185)</f>
-        <v>37.24669999999999</v>
+        <v>37.012699999999995</v>
       </c>
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
-      <c r="H185" s="115" t="s">
+      <c r="H185" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="I185" s="116"/>
+      <c r="I185" s="100"/>
       <c r="J185" s="9">
         <f>H182-J182</f>
         <v>95.999999999999829</v>
@@ -9781,11 +9825,11 @@
       </c>
       <c r="M185" s="9">
         <f>L185-M182</f>
-        <v>85.26669999999983</v>
+        <v>85.032699999999821</v>
       </c>
       <c r="N185" s="10">
         <f>M185-N182</f>
-        <v>85.26669999999983</v>
+        <v>85.032699999999821</v>
       </c>
     </row>
     <row r="186" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9831,18 +9875,18 @@
         <v>24.4</v>
       </c>
       <c r="F187" s="3"/>
-      <c r="H187" s="97" t="s">
+      <c r="H187" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="I187" s="117"/>
-      <c r="J187" s="116">
+      <c r="I187" s="102"/>
+      <c r="J187" s="100">
         <f>H182-I182</f>
-        <v>85.26669999999983</v>
-      </c>
-      <c r="K187" s="116"/>
-      <c r="L187" s="116"/>
-      <c r="M187" s="116"/>
-      <c r="N187" s="118"/>
+        <v>85.032699999999835</v>
+      </c>
+      <c r="K187" s="100"/>
+      <c r="L187" s="100"/>
+      <c r="M187" s="100"/>
+      <c r="N187" s="103"/>
     </row>
     <row r="188" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B188" s="3"/>
@@ -9946,6 +9990,24 @@
     <row r="206" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C133:C137"/>
+    <mergeCell ref="C123:C127"/>
+    <mergeCell ref="C113:C117"/>
+    <mergeCell ref="C108:C112"/>
+    <mergeCell ref="C98:C102"/>
+    <mergeCell ref="C118:C122"/>
+    <mergeCell ref="C128:C132"/>
+    <mergeCell ref="C83:C87"/>
+    <mergeCell ref="J2:W2"/>
+    <mergeCell ref="B63:B72"/>
+    <mergeCell ref="C56:C62"/>
+    <mergeCell ref="C15:C55"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C69:C72"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C73:C77"/>
+    <mergeCell ref="C78:C82"/>
     <mergeCell ref="B164:B170"/>
     <mergeCell ref="H185:I185"/>
     <mergeCell ref="H187:I187"/>
@@ -9962,24 +10024,6 @@
     <mergeCell ref="C143:C147"/>
     <mergeCell ref="C93:C97"/>
     <mergeCell ref="C88:C92"/>
-    <mergeCell ref="C83:C87"/>
-    <mergeCell ref="J2:W2"/>
-    <mergeCell ref="B63:B72"/>
-    <mergeCell ref="C56:C62"/>
-    <mergeCell ref="C15:C55"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="C69:C72"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="C73:C77"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="C133:C137"/>
-    <mergeCell ref="C123:C127"/>
-    <mergeCell ref="C113:C117"/>
-    <mergeCell ref="C108:C112"/>
-    <mergeCell ref="C98:C102"/>
-    <mergeCell ref="C118:C122"/>
-    <mergeCell ref="C128:C132"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tektite a medio hacer, actualizado excel captura del 18
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
+++ b/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
@@ -1285,46 +1285,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1333,7 +1297,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1370,6 +1340,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1438,10 +1438,10 @@
                   <c:v>89.943699999999822</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85.032699999999821</c:v>
+                  <c:v>83.802699999999831</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>85.032699999999821</c:v>
+                  <c:v>83.802699999999831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1462,11 +1462,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1083270528"/>
-        <c:axId val="-1083260192"/>
+        <c:axId val="-1503445520"/>
+        <c:axId val="-1503444432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1083270528"/>
+        <c:axId val="-1503445520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1475,7 +1475,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1083260192"/>
+        <c:crossAx val="-1503444432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1483,7 +1483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1083260192"/>
+        <c:axId val="-1503444432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1494,7 +1494,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1083270528"/>
+        <c:crossAx val="-1503445520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1536,7 +1536,7 @@
         <xdr:cNvPr id="4" name="3 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1846,8 +1846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K156" sqref="K156"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1874,22 +1874,22 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="101" t="s">
+      <c r="J2" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="110"/>
-      <c r="L2" s="110"/>
-      <c r="M2" s="110"/>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="110"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="110"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="110"/>
-      <c r="U2" s="110"/>
-      <c r="V2" s="110"/>
-      <c r="W2" s="111"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98"/>
+      <c r="S2" s="98"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="98"/>
+      <c r="V2" s="98"/>
+      <c r="W2" s="99"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="56" t="s">
@@ -1960,7 +1960,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="111" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="37" t="s">
@@ -2005,7 +2005,7 @@
       <c r="W4" s="44"/>
     </row>
     <row r="5" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="122"/>
+      <c r="B5" s="112"/>
       <c r="C5" s="35" t="s">
         <v>100</v>
       </c>
@@ -2048,7 +2048,7 @@
       <c r="W5" s="19"/>
     </row>
     <row r="6" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="122"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="35" t="s">
         <v>101</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="W6" s="19"/>
     </row>
     <row r="7" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="122"/>
+      <c r="B7" s="112"/>
       <c r="C7" s="35" t="s">
         <v>102</v>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="W7" s="19"/>
     </row>
     <row r="8" spans="1:23" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="123"/>
+      <c r="B8" s="113"/>
       <c r="C8" s="45" t="s">
         <v>110</v>
       </c>
@@ -2177,7 +2177,7 @@
       <c r="W8" s="25"/>
     </row>
     <row r="9" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="121" t="s">
+      <c r="B9" s="111" t="s">
         <v>105</v>
       </c>
       <c r="C9" s="48" t="s">
@@ -2222,7 +2222,7 @@
       <c r="W9" s="86"/>
     </row>
     <row r="10" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="122"/>
+      <c r="B10" s="112"/>
       <c r="C10" s="34" t="s">
         <v>106</v>
       </c>
@@ -2265,7 +2265,7 @@
       <c r="W10" s="19"/>
     </row>
     <row r="11" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="122"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="83" t="s">
         <v>111</v>
       </c>
@@ -2308,7 +2308,7 @@
       <c r="W11" s="19"/>
     </row>
     <row r="12" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="122"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="83" t="s">
         <v>112</v>
       </c>
@@ -2373,7 +2373,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="123"/>
+      <c r="B13" s="113"/>
       <c r="C13" s="53" t="s">
         <v>97</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="W13" s="25"/>
     </row>
     <row r="14" spans="1:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B14" s="96" t="s">
+      <c r="B14" s="100" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="54" t="s">
@@ -2463,8 +2463,8 @@
       <c r="W14" s="52"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B15" s="97"/>
-      <c r="C15" s="115" t="s">
+      <c r="B15" s="101"/>
+      <c r="C15" s="105" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -2510,8 +2510,8 @@
       <c r="W15" s="19"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B16" s="97"/>
-      <c r="C16" s="116"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="106"/>
       <c r="D16" s="4" t="s">
         <v>20</v>
       </c>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="I16" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.23</v>
       </c>
       <c r="J16" s="70">
         <v>0</v>
@@ -2540,7 +2540,9 @@
       <c r="L16" s="70">
         <v>0</v>
       </c>
-      <c r="M16" s="14"/>
+      <c r="M16" s="70">
+        <v>1.23</v>
+      </c>
       <c r="N16" s="4"/>
       <c r="O16" s="17"/>
       <c r="P16" s="16"/>
@@ -2553,8 +2555,8 @@
       <c r="W16" s="19"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B17" s="97"/>
-      <c r="C17" s="116"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="106"/>
       <c r="D17" s="4" t="s">
         <v>21</v>
       </c>
@@ -2596,8 +2598,8 @@
       <c r="W17" s="19"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B18" s="97"/>
-      <c r="C18" s="116"/>
+      <c r="B18" s="101"/>
+      <c r="C18" s="106"/>
       <c r="D18" s="4" t="s">
         <v>22</v>
       </c>
@@ -2639,8 +2641,8 @@
       <c r="W18" s="19"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B19" s="97"/>
-      <c r="C19" s="116"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="106"/>
       <c r="D19" s="4" t="s">
         <v>23</v>
       </c>
@@ -2682,8 +2684,8 @@
       <c r="W19" s="19"/>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B20" s="97"/>
-      <c r="C20" s="116"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="106"/>
       <c r="D20" s="4" t="s">
         <v>162</v>
       </c>
@@ -2725,8 +2727,8 @@
       <c r="W20" s="19"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B21" s="97"/>
-      <c r="C21" s="116"/>
+      <c r="B21" s="101"/>
+      <c r="C21" s="106"/>
       <c r="D21" s="4" t="s">
         <v>24</v>
       </c>
@@ -2768,8 +2770,8 @@
       <c r="W21" s="19"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B22" s="97"/>
-      <c r="C22" s="116"/>
+      <c r="B22" s="101"/>
+      <c r="C22" s="106"/>
       <c r="D22" s="32" t="s">
         <v>36</v>
       </c>
@@ -2811,8 +2813,8 @@
       <c r="W22" s="19"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B23" s="97"/>
-      <c r="C23" s="116"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="106"/>
       <c r="D23" s="32" t="s">
         <v>37</v>
       </c>
@@ -2854,8 +2856,8 @@
       <c r="W23" s="19"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B24" s="97"/>
-      <c r="C24" s="116"/>
+      <c r="B24" s="101"/>
+      <c r="C24" s="106"/>
       <c r="D24" s="32" t="s">
         <v>38</v>
       </c>
@@ -2897,8 +2899,8 @@
       <c r="W24" s="19"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B25" s="97"/>
-      <c r="C25" s="116"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="106"/>
       <c r="D25" s="32" t="s">
         <v>39</v>
       </c>
@@ -2940,8 +2942,8 @@
       <c r="W25" s="19"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B26" s="97"/>
-      <c r="C26" s="116"/>
+      <c r="B26" s="101"/>
+      <c r="C26" s="106"/>
       <c r="D26" s="32" t="s">
         <v>40</v>
       </c>
@@ -2983,8 +2985,8 @@
       <c r="W26" s="19"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B27" s="97"/>
-      <c r="C27" s="116"/>
+      <c r="B27" s="101"/>
+      <c r="C27" s="106"/>
       <c r="D27" s="32" t="s">
         <v>41</v>
       </c>
@@ -3026,8 +3028,8 @@
       <c r="W27" s="19"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B28" s="97"/>
-      <c r="C28" s="116"/>
+      <c r="B28" s="101"/>
+      <c r="C28" s="106"/>
       <c r="D28" s="32" t="s">
         <v>42</v>
       </c>
@@ -3069,8 +3071,8 @@
       <c r="W28" s="19"/>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B29" s="97"/>
-      <c r="C29" s="116"/>
+      <c r="B29" s="101"/>
+      <c r="C29" s="106"/>
       <c r="D29" s="32" t="s">
         <v>43</v>
       </c>
@@ -3112,8 +3114,8 @@
       <c r="W29" s="19"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B30" s="97"/>
-      <c r="C30" s="116"/>
+      <c r="B30" s="101"/>
+      <c r="C30" s="106"/>
       <c r="D30" s="32" t="s">
         <v>44</v>
       </c>
@@ -3155,8 +3157,8 @@
       <c r="W30" s="19"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B31" s="97"/>
-      <c r="C31" s="116"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="106"/>
       <c r="D31" s="32" t="s">
         <v>45</v>
       </c>
@@ -3198,8 +3200,8 @@
       <c r="W31" s="19"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B32" s="97"/>
-      <c r="C32" s="116"/>
+      <c r="B32" s="101"/>
+      <c r="C32" s="106"/>
       <c r="D32" s="32" t="s">
         <v>46</v>
       </c>
@@ -3241,8 +3243,8 @@
       <c r="W32" s="19"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B33" s="97"/>
-      <c r="C33" s="116"/>
+      <c r="B33" s="101"/>
+      <c r="C33" s="106"/>
       <c r="D33" s="32" t="s">
         <v>47</v>
       </c>
@@ -3284,8 +3286,8 @@
       <c r="W33" s="19"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B34" s="97"/>
-      <c r="C34" s="116"/>
+      <c r="B34" s="101"/>
+      <c r="C34" s="106"/>
       <c r="D34" s="32" t="s">
         <v>48</v>
       </c>
@@ -3327,8 +3329,8 @@
       <c r="W34" s="19"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B35" s="97"/>
-      <c r="C35" s="116"/>
+      <c r="B35" s="101"/>
+      <c r="C35" s="106"/>
       <c r="D35" s="32" t="s">
         <v>49</v>
       </c>
@@ -3370,8 +3372,8 @@
       <c r="W35" s="19"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B36" s="97"/>
-      <c r="C36" s="116"/>
+      <c r="B36" s="101"/>
+      <c r="C36" s="106"/>
       <c r="D36" s="32" t="s">
         <v>50</v>
       </c>
@@ -3413,8 +3415,8 @@
       <c r="W36" s="19"/>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B37" s="97"/>
-      <c r="C37" s="116"/>
+      <c r="B37" s="101"/>
+      <c r="C37" s="106"/>
       <c r="D37" s="32" t="s">
         <v>51</v>
       </c>
@@ -3456,8 +3458,8 @@
       <c r="W37" s="19"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B38" s="97"/>
-      <c r="C38" s="116"/>
+      <c r="B38" s="101"/>
+      <c r="C38" s="106"/>
       <c r="D38" s="32" t="s">
         <v>52</v>
       </c>
@@ -3499,8 +3501,8 @@
       <c r="W38" s="19"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B39" s="97"/>
-      <c r="C39" s="116"/>
+      <c r="B39" s="101"/>
+      <c r="C39" s="106"/>
       <c r="D39" s="32" t="s">
         <v>53</v>
       </c>
@@ -3542,8 +3544,8 @@
       <c r="W39" s="19"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B40" s="97"/>
-      <c r="C40" s="116"/>
+      <c r="B40" s="101"/>
+      <c r="C40" s="106"/>
       <c r="D40" s="32" t="s">
         <v>54</v>
       </c>
@@ -3585,8 +3587,8 @@
       <c r="W40" s="19"/>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B41" s="97"/>
-      <c r="C41" s="116"/>
+      <c r="B41" s="101"/>
+      <c r="C41" s="106"/>
       <c r="D41" s="32" t="s">
         <v>55</v>
       </c>
@@ -3628,8 +3630,8 @@
       <c r="W41" s="19"/>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B42" s="97"/>
-      <c r="C42" s="116"/>
+      <c r="B42" s="101"/>
+      <c r="C42" s="106"/>
       <c r="D42" s="32" t="s">
         <v>56</v>
       </c>
@@ -3671,8 +3673,8 @@
       <c r="W42" s="19"/>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B43" s="97"/>
-      <c r="C43" s="116"/>
+      <c r="B43" s="101"/>
+      <c r="C43" s="106"/>
       <c r="D43" s="32" t="s">
         <v>57</v>
       </c>
@@ -3714,8 +3716,8 @@
       <c r="W43" s="19"/>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B44" s="97"/>
-      <c r="C44" s="116"/>
+      <c r="B44" s="101"/>
+      <c r="C44" s="106"/>
       <c r="D44" s="32" t="s">
         <v>58</v>
       </c>
@@ -3757,8 +3759,8 @@
       <c r="W44" s="19"/>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B45" s="97"/>
-      <c r="C45" s="116"/>
+      <c r="B45" s="101"/>
+      <c r="C45" s="106"/>
       <c r="D45" s="32" t="s">
         <v>59</v>
       </c>
@@ -3800,8 +3802,8 @@
       <c r="W45" s="19"/>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B46" s="97"/>
-      <c r="C46" s="116"/>
+      <c r="B46" s="101"/>
+      <c r="C46" s="106"/>
       <c r="D46" s="32" t="s">
         <v>60</v>
       </c>
@@ -3843,8 +3845,8 @@
       <c r="W46" s="19"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B47" s="97"/>
-      <c r="C47" s="116"/>
+      <c r="B47" s="101"/>
+      <c r="C47" s="106"/>
       <c r="D47" s="32" t="s">
         <v>61</v>
       </c>
@@ -3886,8 +3888,8 @@
       <c r="W47" s="19"/>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B48" s="97"/>
-      <c r="C48" s="116"/>
+      <c r="B48" s="101"/>
+      <c r="C48" s="106"/>
       <c r="D48" s="32" t="s">
         <v>62</v>
       </c>
@@ -3929,8 +3931,8 @@
       <c r="W48" s="19"/>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B49" s="97"/>
-      <c r="C49" s="116"/>
+      <c r="B49" s="101"/>
+      <c r="C49" s="106"/>
       <c r="D49" s="32" t="s">
         <v>63</v>
       </c>
@@ -3972,8 +3974,8 @@
       <c r="W49" s="19"/>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B50" s="97"/>
-      <c r="C50" s="116"/>
+      <c r="B50" s="101"/>
+      <c r="C50" s="106"/>
       <c r="D50" s="32" t="s">
         <v>64</v>
       </c>
@@ -4015,8 +4017,8 @@
       <c r="W50" s="19"/>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B51" s="97"/>
-      <c r="C51" s="116"/>
+      <c r="B51" s="101"/>
+      <c r="C51" s="106"/>
       <c r="D51" s="32" t="s">
         <v>65</v>
       </c>
@@ -4058,8 +4060,8 @@
       <c r="W51" s="19"/>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B52" s="97"/>
-      <c r="C52" s="116"/>
+      <c r="B52" s="101"/>
+      <c r="C52" s="106"/>
       <c r="D52" s="32" t="s">
         <v>66</v>
       </c>
@@ -4101,8 +4103,8 @@
       <c r="W52" s="19"/>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B53" s="97"/>
-      <c r="C53" s="116"/>
+      <c r="B53" s="101"/>
+      <c r="C53" s="106"/>
       <c r="D53" s="32" t="s">
         <v>67</v>
       </c>
@@ -4144,8 +4146,8 @@
       <c r="W53" s="19"/>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B54" s="97"/>
-      <c r="C54" s="116"/>
+      <c r="B54" s="101"/>
+      <c r="C54" s="106"/>
       <c r="D54" s="32" t="s">
         <v>68</v>
       </c>
@@ -4187,8 +4189,8 @@
       <c r="W54" s="19"/>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B55" s="97"/>
-      <c r="C55" s="117"/>
+      <c r="B55" s="101"/>
+      <c r="C55" s="107"/>
       <c r="D55" s="32" t="s">
         <v>69</v>
       </c>
@@ -4230,8 +4232,8 @@
       <c r="W55" s="19"/>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B56" s="97"/>
-      <c r="C56" s="113" t="s">
+      <c r="B56" s="101"/>
+      <c r="C56" s="103" t="s">
         <v>26</v>
       </c>
       <c r="D56" s="29" t="s">
@@ -4275,8 +4277,8 @@
       <c r="W56" s="19"/>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B57" s="97"/>
-      <c r="C57" s="114"/>
+      <c r="B57" s="101"/>
+      <c r="C57" s="104"/>
       <c r="D57" s="29" t="s">
         <v>29</v>
       </c>
@@ -4318,8 +4320,8 @@
       <c r="W57" s="19"/>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B58" s="97"/>
-      <c r="C58" s="114"/>
+      <c r="B58" s="101"/>
+      <c r="C58" s="104"/>
       <c r="D58" s="29" t="s">
         <v>30</v>
       </c>
@@ -4361,8 +4363,8 @@
       <c r="W58" s="19"/>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B59" s="97"/>
-      <c r="C59" s="114"/>
+      <c r="B59" s="101"/>
+      <c r="C59" s="104"/>
       <c r="D59" s="29" t="s">
         <v>31</v>
       </c>
@@ -4404,8 +4406,8 @@
       <c r="W59" s="19"/>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B60" s="97"/>
-      <c r="C60" s="114"/>
+      <c r="B60" s="101"/>
+      <c r="C60" s="104"/>
       <c r="D60" s="29" t="s">
         <v>34</v>
       </c>
@@ -4447,8 +4449,8 @@
       <c r="W60" s="19"/>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B61" s="97"/>
-      <c r="C61" s="114"/>
+      <c r="B61" s="101"/>
+      <c r="C61" s="104"/>
       <c r="D61" s="29" t="s">
         <v>32</v>
       </c>
@@ -4490,8 +4492,8 @@
       <c r="W61" s="19"/>
     </row>
     <row r="62" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="104"/>
-      <c r="C62" s="114"/>
+      <c r="B62" s="119"/>
+      <c r="C62" s="104"/>
       <c r="D62" s="62" t="s">
         <v>33</v>
       </c>
@@ -4533,10 +4535,10 @@
       <c r="W62" s="28"/>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B63" s="96" t="s">
+      <c r="B63" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="118" t="s">
+      <c r="C63" s="108" t="s">
         <v>79</v>
       </c>
       <c r="D63" s="39" t="s">
@@ -4580,8 +4582,8 @@
       <c r="W63" s="52"/>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B64" s="97"/>
-      <c r="C64" s="119"/>
+      <c r="B64" s="101"/>
+      <c r="C64" s="109"/>
       <c r="D64" s="4" t="s">
         <v>71</v>
       </c>
@@ -4623,8 +4625,8 @@
       <c r="W64" s="19"/>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B65" s="97"/>
-      <c r="C65" s="119"/>
+      <c r="B65" s="101"/>
+      <c r="C65" s="109"/>
       <c r="D65" s="4" t="s">
         <v>72</v>
       </c>
@@ -4666,8 +4668,8 @@
       <c r="W65" s="19"/>
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B66" s="97"/>
-      <c r="C66" s="119"/>
+      <c r="B66" s="101"/>
+      <c r="C66" s="109"/>
       <c r="D66" s="29" t="s">
         <v>76</v>
       </c>
@@ -4709,7 +4711,7 @@
       <c r="W66" s="19"/>
     </row>
     <row r="67" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B67" s="97"/>
+      <c r="B67" s="101"/>
       <c r="C67" s="33" t="s">
         <v>73</v>
       </c>
@@ -4752,7 +4754,7 @@
       <c r="W67" s="19"/>
     </row>
     <row r="68" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B68" s="97"/>
+      <c r="B68" s="101"/>
       <c r="C68" s="33" t="s">
         <v>81</v>
       </c>
@@ -4795,8 +4797,8 @@
       <c r="W68" s="19"/>
     </row>
     <row r="69" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="97"/>
-      <c r="C69" s="119" t="s">
+      <c r="B69" s="101"/>
+      <c r="C69" s="109" t="s">
         <v>80</v>
       </c>
       <c r="D69" s="4" t="s">
@@ -4840,8 +4842,8 @@
       <c r="W69" s="19"/>
     </row>
     <row r="70" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="97"/>
-      <c r="C70" s="119"/>
+      <c r="B70" s="101"/>
+      <c r="C70" s="109"/>
       <c r="D70" s="4" t="s">
         <v>75</v>
       </c>
@@ -4883,8 +4885,8 @@
       <c r="W70" s="19"/>
     </row>
     <row r="71" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="97"/>
-      <c r="C71" s="119"/>
+      <c r="B71" s="101"/>
+      <c r="C71" s="109"/>
       <c r="D71" s="4" t="s">
         <v>77</v>
       </c>
@@ -4926,8 +4928,8 @@
       <c r="W71" s="19"/>
     </row>
     <row r="72" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="98"/>
-      <c r="C72" s="120"/>
+      <c r="B72" s="102"/>
+      <c r="C72" s="110"/>
       <c r="D72" s="24" t="s">
         <v>78</v>
       </c>
@@ -4969,10 +4971,10 @@
       <c r="W72" s="25"/>
     </row>
     <row r="73" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="96" t="s">
+      <c r="B73" s="100" t="s">
         <v>115</v>
       </c>
-      <c r="C73" s="124" t="s">
+      <c r="C73" s="114" t="s">
         <v>116</v>
       </c>
       <c r="D73" s="39" t="s">
@@ -5016,8 +5018,8 @@
       <c r="W73" s="52"/>
     </row>
     <row r="74" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="97"/>
-      <c r="C74" s="109"/>
+      <c r="B74" s="101"/>
+      <c r="C74" s="96"/>
       <c r="D74" s="4" t="s">
         <v>132</v>
       </c>
@@ -5059,8 +5061,8 @@
       <c r="W74" s="19"/>
     </row>
     <row r="75" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="97"/>
-      <c r="C75" s="109"/>
+      <c r="B75" s="101"/>
+      <c r="C75" s="96"/>
       <c r="D75" s="4" t="s">
         <v>161</v>
       </c>
@@ -5094,8 +5096,8 @@
       <c r="W75" s="19"/>
     </row>
     <row r="76" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="97"/>
-      <c r="C76" s="109"/>
+      <c r="B76" s="101"/>
+      <c r="C76" s="96"/>
       <c r="D76" s="4" t="s">
         <v>133</v>
       </c>
@@ -5137,8 +5139,8 @@
       <c r="W76" s="95"/>
     </row>
     <row r="77" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="97"/>
-      <c r="C77" s="109"/>
+      <c r="B77" s="101"/>
+      <c r="C77" s="96"/>
       <c r="D77" s="4" t="s">
         <v>134</v>
       </c>
@@ -5180,8 +5182,8 @@
       <c r="W77" s="19"/>
     </row>
     <row r="78" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="97"/>
-      <c r="C78" s="109" t="s">
+      <c r="B78" s="101"/>
+      <c r="C78" s="96" t="s">
         <v>117</v>
       </c>
       <c r="D78" s="4" t="s">
@@ -5225,8 +5227,8 @@
       <c r="W78" s="19"/>
     </row>
     <row r="79" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="97"/>
-      <c r="C79" s="109"/>
+      <c r="B79" s="101"/>
+      <c r="C79" s="96"/>
       <c r="D79" s="4" t="s">
         <v>132</v>
       </c>
@@ -5268,8 +5270,8 @@
       <c r="W79" s="19"/>
     </row>
     <row r="80" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="97"/>
-      <c r="C80" s="109"/>
+      <c r="B80" s="101"/>
+      <c r="C80" s="96"/>
       <c r="D80" s="4" t="s">
         <v>161</v>
       </c>
@@ -5303,8 +5305,8 @@
       <c r="W80" s="19"/>
     </row>
     <row r="81" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="97"/>
-      <c r="C81" s="109"/>
+      <c r="B81" s="101"/>
+      <c r="C81" s="96"/>
       <c r="D81" s="4" t="s">
         <v>133</v>
       </c>
@@ -5348,8 +5350,8 @@
       <c r="W81" s="95"/>
     </row>
     <row r="82" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="97"/>
-      <c r="C82" s="109"/>
+      <c r="B82" s="101"/>
+      <c r="C82" s="96"/>
       <c r="D82" s="4" t="s">
         <v>134</v>
       </c>
@@ -5391,8 +5393,8 @@
       <c r="W82" s="19"/>
     </row>
     <row r="83" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="97"/>
-      <c r="C83" s="109" t="s">
+      <c r="B83" s="101"/>
+      <c r="C83" s="96" t="s">
         <v>118</v>
       </c>
       <c r="D83" s="4" t="s">
@@ -5436,8 +5438,8 @@
       <c r="W83" s="19"/>
     </row>
     <row r="84" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="97"/>
-      <c r="C84" s="109"/>
+      <c r="B84" s="101"/>
+      <c r="C84" s="96"/>
       <c r="D84" s="4" t="s">
         <v>132</v>
       </c>
@@ -5479,8 +5481,8 @@
       <c r="W84" s="19"/>
     </row>
     <row r="85" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="97"/>
-      <c r="C85" s="109"/>
+      <c r="B85" s="101"/>
+      <c r="C85" s="96"/>
       <c r="D85" s="4" t="s">
         <v>161</v>
       </c>
@@ -5514,8 +5516,8 @@
       <c r="W85" s="19"/>
     </row>
     <row r="86" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="97"/>
-      <c r="C86" s="109"/>
+      <c r="B86" s="101"/>
+      <c r="C86" s="96"/>
       <c r="D86" s="4" t="s">
         <v>133</v>
       </c>
@@ -5559,8 +5561,8 @@
       <c r="W86" s="95"/>
     </row>
     <row r="87" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="97"/>
-      <c r="C87" s="109"/>
+      <c r="B87" s="101"/>
+      <c r="C87" s="96"/>
       <c r="D87" s="4" t="s">
         <v>134</v>
       </c>
@@ -5602,8 +5604,8 @@
       <c r="W87" s="19"/>
     </row>
     <row r="88" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="97"/>
-      <c r="C88" s="109" t="s">
+      <c r="B88" s="101"/>
+      <c r="C88" s="96" t="s">
         <v>119</v>
       </c>
       <c r="D88" s="4" t="s">
@@ -5647,8 +5649,8 @@
       <c r="W88" s="19"/>
     </row>
     <row r="89" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="97"/>
-      <c r="C89" s="109"/>
+      <c r="B89" s="101"/>
+      <c r="C89" s="96"/>
       <c r="D89" s="4" t="s">
         <v>132</v>
       </c>
@@ -5690,8 +5692,8 @@
       <c r="W89" s="19"/>
     </row>
     <row r="90" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="97"/>
-      <c r="C90" s="109"/>
+      <c r="B90" s="101"/>
+      <c r="C90" s="96"/>
       <c r="D90" s="4" t="s">
         <v>161</v>
       </c>
@@ -5725,8 +5727,8 @@
       <c r="W90" s="19"/>
     </row>
     <row r="91" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="97"/>
-      <c r="C91" s="109"/>
+      <c r="B91" s="101"/>
+      <c r="C91" s="96"/>
       <c r="D91" s="4" t="s">
         <v>133</v>
       </c>
@@ -5770,8 +5772,8 @@
       <c r="W91" s="95"/>
     </row>
     <row r="92" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="97"/>
-      <c r="C92" s="109"/>
+      <c r="B92" s="101"/>
+      <c r="C92" s="96"/>
       <c r="D92" s="4" t="s">
         <v>134</v>
       </c>
@@ -5813,8 +5815,8 @@
       <c r="W92" s="19"/>
     </row>
     <row r="93" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="97"/>
-      <c r="C93" s="109" t="s">
+      <c r="B93" s="101"/>
+      <c r="C93" s="96" t="s">
         <v>120</v>
       </c>
       <c r="D93" s="4" t="s">
@@ -5858,8 +5860,8 @@
       <c r="W93" s="19"/>
     </row>
     <row r="94" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="97"/>
-      <c r="C94" s="109"/>
+      <c r="B94" s="101"/>
+      <c r="C94" s="96"/>
       <c r="D94" s="4" t="s">
         <v>132</v>
       </c>
@@ -5901,8 +5903,8 @@
       <c r="W94" s="19"/>
     </row>
     <row r="95" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="97"/>
-      <c r="C95" s="109"/>
+      <c r="B95" s="101"/>
+      <c r="C95" s="96"/>
       <c r="D95" s="4" t="s">
         <v>161</v>
       </c>
@@ -5936,8 +5938,8 @@
       <c r="W95" s="19"/>
     </row>
     <row r="96" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="97"/>
-      <c r="C96" s="109"/>
+      <c r="B96" s="101"/>
+      <c r="C96" s="96"/>
       <c r="D96" s="4" t="s">
         <v>133</v>
       </c>
@@ -5981,8 +5983,8 @@
       <c r="W96" s="95"/>
     </row>
     <row r="97" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="97"/>
-      <c r="C97" s="109"/>
+      <c r="B97" s="101"/>
+      <c r="C97" s="96"/>
       <c r="D97" s="4" t="s">
         <v>134</v>
       </c>
@@ -6024,8 +6026,8 @@
       <c r="W97" s="19"/>
     </row>
     <row r="98" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="97"/>
-      <c r="C98" s="109" t="s">
+      <c r="B98" s="101"/>
+      <c r="C98" s="96" t="s">
         <v>121</v>
       </c>
       <c r="D98" s="4" t="s">
@@ -6069,8 +6071,8 @@
       <c r="W98" s="19"/>
     </row>
     <row r="99" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="97"/>
-      <c r="C99" s="109"/>
+      <c r="B99" s="101"/>
+      <c r="C99" s="96"/>
       <c r="D99" s="4" t="s">
         <v>132</v>
       </c>
@@ -6112,8 +6114,8 @@
       <c r="W99" s="19"/>
     </row>
     <row r="100" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="97"/>
-      <c r="C100" s="109"/>
+      <c r="B100" s="101"/>
+      <c r="C100" s="96"/>
       <c r="D100" s="4" t="s">
         <v>161</v>
       </c>
@@ -6147,8 +6149,8 @@
       <c r="W100" s="19"/>
     </row>
     <row r="101" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="97"/>
-      <c r="C101" s="109"/>
+      <c r="B101" s="101"/>
+      <c r="C101" s="96"/>
       <c r="D101" s="4" t="s">
         <v>133</v>
       </c>
@@ -6192,8 +6194,8 @@
       <c r="W101" s="95"/>
     </row>
     <row r="102" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="97"/>
-      <c r="C102" s="109"/>
+      <c r="B102" s="101"/>
+      <c r="C102" s="96"/>
       <c r="D102" s="4" t="s">
         <v>134</v>
       </c>
@@ -6235,8 +6237,8 @@
       <c r="W102" s="19"/>
     </row>
     <row r="103" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="97"/>
-      <c r="C103" s="109" t="s">
+      <c r="B103" s="101"/>
+      <c r="C103" s="96" t="s">
         <v>122</v>
       </c>
       <c r="D103" s="4" t="s">
@@ -6280,8 +6282,8 @@
       <c r="W103" s="19"/>
     </row>
     <row r="104" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="97"/>
-      <c r="C104" s="109"/>
+      <c r="B104" s="101"/>
+      <c r="C104" s="96"/>
       <c r="D104" s="4" t="s">
         <v>132</v>
       </c>
@@ -6323,8 +6325,8 @@
       <c r="W104" s="19"/>
     </row>
     <row r="105" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="97"/>
-      <c r="C105" s="109"/>
+      <c r="B105" s="101"/>
+      <c r="C105" s="96"/>
       <c r="D105" s="4" t="s">
         <v>161</v>
       </c>
@@ -6358,8 +6360,8 @@
       <c r="W105" s="19"/>
     </row>
     <row r="106" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="97"/>
-      <c r="C106" s="109"/>
+      <c r="B106" s="101"/>
+      <c r="C106" s="96"/>
       <c r="D106" s="4" t="s">
         <v>133</v>
       </c>
@@ -6403,8 +6405,8 @@
       <c r="W106" s="95"/>
     </row>
     <row r="107" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="97"/>
-      <c r="C107" s="109"/>
+      <c r="B107" s="101"/>
+      <c r="C107" s="96"/>
       <c r="D107" s="4" t="s">
         <v>134</v>
       </c>
@@ -6446,8 +6448,8 @@
       <c r="W107" s="19"/>
     </row>
     <row r="108" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="97"/>
-      <c r="C108" s="109" t="s">
+      <c r="B108" s="101"/>
+      <c r="C108" s="96" t="s">
         <v>123</v>
       </c>
       <c r="D108" s="4" t="s">
@@ -6491,8 +6493,8 @@
       <c r="W108" s="19"/>
     </row>
     <row r="109" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="97"/>
-      <c r="C109" s="109"/>
+      <c r="B109" s="101"/>
+      <c r="C109" s="96"/>
       <c r="D109" s="4" t="s">
         <v>132</v>
       </c>
@@ -6534,8 +6536,8 @@
       <c r="W109" s="19"/>
     </row>
     <row r="110" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="97"/>
-      <c r="C110" s="109"/>
+      <c r="B110" s="101"/>
+      <c r="C110" s="96"/>
       <c r="D110" s="4" t="s">
         <v>161</v>
       </c>
@@ -6569,8 +6571,8 @@
       <c r="W110" s="19"/>
     </row>
     <row r="111" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="97"/>
-      <c r="C111" s="109"/>
+      <c r="B111" s="101"/>
+      <c r="C111" s="96"/>
       <c r="D111" s="4" t="s">
         <v>133</v>
       </c>
@@ -6614,8 +6616,8 @@
       <c r="W111" s="95"/>
     </row>
     <row r="112" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="97"/>
-      <c r="C112" s="109"/>
+      <c r="B112" s="101"/>
+      <c r="C112" s="96"/>
       <c r="D112" s="4" t="s">
         <v>134</v>
       </c>
@@ -6657,8 +6659,8 @@
       <c r="W112" s="19"/>
     </row>
     <row r="113" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="97"/>
-      <c r="C113" s="109" t="s">
+      <c r="B113" s="101"/>
+      <c r="C113" s="96" t="s">
         <v>124</v>
       </c>
       <c r="D113" s="4" t="s">
@@ -6702,8 +6704,8 @@
       <c r="W113" s="19"/>
     </row>
     <row r="114" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="97"/>
-      <c r="C114" s="109"/>
+      <c r="B114" s="101"/>
+      <c r="C114" s="96"/>
       <c r="D114" s="4" t="s">
         <v>132</v>
       </c>
@@ -6745,8 +6747,8 @@
       <c r="W114" s="19"/>
     </row>
     <row r="115" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="97"/>
-      <c r="C115" s="109"/>
+      <c r="B115" s="101"/>
+      <c r="C115" s="96"/>
       <c r="D115" s="4" t="s">
         <v>161</v>
       </c>
@@ -6780,8 +6782,8 @@
       <c r="W115" s="19"/>
     </row>
     <row r="116" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="97"/>
-      <c r="C116" s="109"/>
+      <c r="B116" s="101"/>
+      <c r="C116" s="96"/>
       <c r="D116" s="4" t="s">
         <v>133</v>
       </c>
@@ -6825,8 +6827,8 @@
       <c r="W116" s="95"/>
     </row>
     <row r="117" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="97"/>
-      <c r="C117" s="109"/>
+      <c r="B117" s="101"/>
+      <c r="C117" s="96"/>
       <c r="D117" s="4" t="s">
         <v>134</v>
       </c>
@@ -6868,8 +6870,8 @@
       <c r="W117" s="19"/>
     </row>
     <row r="118" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="97"/>
-      <c r="C118" s="109" t="s">
+      <c r="B118" s="101"/>
+      <c r="C118" s="96" t="s">
         <v>125</v>
       </c>
       <c r="D118" s="4" t="s">
@@ -6913,8 +6915,8 @@
       <c r="W118" s="19"/>
     </row>
     <row r="119" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="97"/>
-      <c r="C119" s="109"/>
+      <c r="B119" s="101"/>
+      <c r="C119" s="96"/>
       <c r="D119" s="4" t="s">
         <v>132</v>
       </c>
@@ -6956,8 +6958,8 @@
       <c r="W119" s="19"/>
     </row>
     <row r="120" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="97"/>
-      <c r="C120" s="109"/>
+      <c r="B120" s="101"/>
+      <c r="C120" s="96"/>
       <c r="D120" s="4" t="s">
         <v>161</v>
       </c>
@@ -6991,8 +6993,8 @@
       <c r="W120" s="19"/>
     </row>
     <row r="121" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="97"/>
-      <c r="C121" s="109"/>
+      <c r="B121" s="101"/>
+      <c r="C121" s="96"/>
       <c r="D121" s="4" t="s">
         <v>133</v>
       </c>
@@ -7036,8 +7038,8 @@
       <c r="W121" s="95"/>
     </row>
     <row r="122" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="97"/>
-      <c r="C122" s="109"/>
+      <c r="B122" s="101"/>
+      <c r="C122" s="96"/>
       <c r="D122" s="4" t="s">
         <v>134</v>
       </c>
@@ -7079,8 +7081,8 @@
       <c r="W122" s="19"/>
     </row>
     <row r="123" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="97"/>
-      <c r="C123" s="109" t="s">
+      <c r="B123" s="101"/>
+      <c r="C123" s="96" t="s">
         <v>126</v>
       </c>
       <c r="D123" s="4" t="s">
@@ -7124,8 +7126,8 @@
       <c r="W123" s="19"/>
     </row>
     <row r="124" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="97"/>
-      <c r="C124" s="109"/>
+      <c r="B124" s="101"/>
+      <c r="C124" s="96"/>
       <c r="D124" s="4" t="s">
         <v>132</v>
       </c>
@@ -7167,8 +7169,8 @@
       <c r="W124" s="19"/>
     </row>
     <row r="125" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="97"/>
-      <c r="C125" s="109"/>
+      <c r="B125" s="101"/>
+      <c r="C125" s="96"/>
       <c r="D125" s="4" t="s">
         <v>161</v>
       </c>
@@ -7202,8 +7204,8 @@
       <c r="W125" s="19"/>
     </row>
     <row r="126" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="97"/>
-      <c r="C126" s="109"/>
+      <c r="B126" s="101"/>
+      <c r="C126" s="96"/>
       <c r="D126" s="4" t="s">
         <v>133</v>
       </c>
@@ -7247,8 +7249,8 @@
       <c r="W126" s="95"/>
     </row>
     <row r="127" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="97"/>
-      <c r="C127" s="109"/>
+      <c r="B127" s="101"/>
+      <c r="C127" s="96"/>
       <c r="D127" s="4" t="s">
         <v>134</v>
       </c>
@@ -7290,8 +7292,8 @@
       <c r="W127" s="19"/>
     </row>
     <row r="128" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="97"/>
-      <c r="C128" s="109" t="s">
+      <c r="B128" s="101"/>
+      <c r="C128" s="96" t="s">
         <v>127</v>
       </c>
       <c r="D128" s="4" t="s">
@@ -7335,8 +7337,8 @@
       <c r="W128" s="19"/>
     </row>
     <row r="129" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="97"/>
-      <c r="C129" s="109"/>
+      <c r="B129" s="101"/>
+      <c r="C129" s="96"/>
       <c r="D129" s="4" t="s">
         <v>132</v>
       </c>
@@ -7378,8 +7380,8 @@
       <c r="W129" s="19"/>
     </row>
     <row r="130" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="97"/>
-      <c r="C130" s="109"/>
+      <c r="B130" s="101"/>
+      <c r="C130" s="96"/>
       <c r="D130" s="4" t="s">
         <v>161</v>
       </c>
@@ -7413,8 +7415,8 @@
       <c r="W130" s="19"/>
     </row>
     <row r="131" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="97"/>
-      <c r="C131" s="109"/>
+      <c r="B131" s="101"/>
+      <c r="C131" s="96"/>
       <c r="D131" s="4" t="s">
         <v>133</v>
       </c>
@@ -7458,8 +7460,8 @@
       <c r="W131" s="95"/>
     </row>
     <row r="132" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="97"/>
-      <c r="C132" s="109"/>
+      <c r="B132" s="101"/>
+      <c r="C132" s="96"/>
       <c r="D132" s="4" t="s">
         <v>134</v>
       </c>
@@ -7501,8 +7503,8 @@
       <c r="W132" s="19"/>
     </row>
     <row r="133" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="97"/>
-      <c r="C133" s="109" t="s">
+      <c r="B133" s="101"/>
+      <c r="C133" s="96" t="s">
         <v>128</v>
       </c>
       <c r="D133" s="4" t="s">
@@ -7546,8 +7548,8 @@
       <c r="W133" s="19"/>
     </row>
     <row r="134" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="97"/>
-      <c r="C134" s="109"/>
+      <c r="B134" s="101"/>
+      <c r="C134" s="96"/>
       <c r="D134" s="4" t="s">
         <v>132</v>
       </c>
@@ -7589,8 +7591,8 @@
       <c r="W134" s="19"/>
     </row>
     <row r="135" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="97"/>
-      <c r="C135" s="109"/>
+      <c r="B135" s="101"/>
+      <c r="C135" s="96"/>
       <c r="D135" s="4" t="s">
         <v>161</v>
       </c>
@@ -7624,8 +7626,8 @@
       <c r="W135" s="19"/>
     </row>
     <row r="136" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="97"/>
-      <c r="C136" s="109"/>
+      <c r="B136" s="101"/>
+      <c r="C136" s="96"/>
       <c r="D136" s="4" t="s">
         <v>133</v>
       </c>
@@ -7669,8 +7671,8 @@
       <c r="W136" s="95"/>
     </row>
     <row r="137" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="97"/>
-      <c r="C137" s="109"/>
+      <c r="B137" s="101"/>
+      <c r="C137" s="96"/>
       <c r="D137" s="4" t="s">
         <v>134</v>
       </c>
@@ -7712,8 +7714,8 @@
       <c r="W137" s="19"/>
     </row>
     <row r="138" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="97"/>
-      <c r="C138" s="109" t="s">
+      <c r="B138" s="101"/>
+      <c r="C138" s="96" t="s">
         <v>129</v>
       </c>
       <c r="D138" s="4" t="s">
@@ -7757,8 +7759,8 @@
       <c r="W138" s="19"/>
     </row>
     <row r="139" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="97"/>
-      <c r="C139" s="109"/>
+      <c r="B139" s="101"/>
+      <c r="C139" s="96"/>
       <c r="D139" s="4" t="s">
         <v>132</v>
       </c>
@@ -7800,8 +7802,8 @@
       <c r="W139" s="19"/>
     </row>
     <row r="140" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="97"/>
-      <c r="C140" s="109"/>
+      <c r="B140" s="101"/>
+      <c r="C140" s="96"/>
       <c r="D140" s="4" t="s">
         <v>161</v>
       </c>
@@ -7835,8 +7837,8 @@
       <c r="W140" s="19"/>
     </row>
     <row r="141" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="97"/>
-      <c r="C141" s="109"/>
+      <c r="B141" s="101"/>
+      <c r="C141" s="96"/>
       <c r="D141" s="4" t="s">
         <v>133</v>
       </c>
@@ -7880,8 +7882,8 @@
       <c r="W141" s="95"/>
     </row>
     <row r="142" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="97"/>
-      <c r="C142" s="109"/>
+      <c r="B142" s="101"/>
+      <c r="C142" s="96"/>
       <c r="D142" s="4" t="s">
         <v>134</v>
       </c>
@@ -7923,8 +7925,8 @@
       <c r="W142" s="19"/>
     </row>
     <row r="143" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="97"/>
-      <c r="C143" s="109" t="s">
+      <c r="B143" s="101"/>
+      <c r="C143" s="96" t="s">
         <v>130</v>
       </c>
       <c r="D143" s="4" t="s">
@@ -7968,8 +7970,8 @@
       <c r="W143" s="19"/>
     </row>
     <row r="144" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="97"/>
-      <c r="C144" s="109"/>
+      <c r="B144" s="101"/>
+      <c r="C144" s="96"/>
       <c r="D144" s="4" t="s">
         <v>132</v>
       </c>
@@ -8011,8 +8013,8 @@
       <c r="W144" s="19"/>
     </row>
     <row r="145" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="97"/>
-      <c r="C145" s="109"/>
+      <c r="B145" s="101"/>
+      <c r="C145" s="96"/>
       <c r="D145" s="4" t="s">
         <v>161</v>
       </c>
@@ -8046,8 +8048,8 @@
       <c r="W145" s="19"/>
     </row>
     <row r="146" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="97"/>
-      <c r="C146" s="109"/>
+      <c r="B146" s="101"/>
+      <c r="C146" s="96"/>
       <c r="D146" s="4" t="s">
         <v>133</v>
       </c>
@@ -8091,8 +8093,8 @@
       <c r="W146" s="95"/>
     </row>
     <row r="147" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B147" s="98"/>
-      <c r="C147" s="112"/>
+      <c r="B147" s="102"/>
+      <c r="C147" s="124"/>
       <c r="D147" s="24" t="s">
         <v>134</v>
       </c>
@@ -8134,7 +8136,7 @@
       <c r="W147" s="25"/>
     </row>
     <row r="148" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="96" t="s">
+      <c r="B148" s="100" t="s">
         <v>83</v>
       </c>
       <c r="C148" s="78" t="s">
@@ -8179,7 +8181,7 @@
       <c r="W148" s="52"/>
     </row>
     <row r="149" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="97"/>
+      <c r="B149" s="101"/>
       <c r="C149" s="33" t="s">
         <v>89</v>
       </c>
@@ -8222,7 +8224,7 @@
       <c r="W149" s="19"/>
     </row>
     <row r="150" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="97"/>
+      <c r="B150" s="101"/>
       <c r="C150" s="33" t="s">
         <v>90</v>
       </c>
@@ -8265,7 +8267,7 @@
       <c r="W150" s="19"/>
     </row>
     <row r="151" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="97"/>
+      <c r="B151" s="101"/>
       <c r="C151" s="33" t="s">
         <v>91</v>
       </c>
@@ -8308,7 +8310,7 @@
       <c r="W151" s="19"/>
     </row>
     <row r="152" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="97"/>
+      <c r="B152" s="101"/>
       <c r="C152" s="33" t="s">
         <v>141</v>
       </c>
@@ -8351,7 +8353,7 @@
       <c r="W152" s="19"/>
     </row>
     <row r="153" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="97"/>
+      <c r="B153" s="101"/>
       <c r="C153" s="33" t="s">
         <v>138</v>
       </c>
@@ -8394,7 +8396,7 @@
       <c r="W153" s="19"/>
     </row>
     <row r="154" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="97"/>
+      <c r="B154" s="101"/>
       <c r="C154" s="33" t="s">
         <v>140</v>
       </c>
@@ -8437,7 +8439,7 @@
       <c r="W154" s="19"/>
     </row>
     <row r="155" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="97"/>
+      <c r="B155" s="101"/>
       <c r="C155" s="33" t="s">
         <v>139</v>
       </c>
@@ -8480,7 +8482,7 @@
       <c r="W155" s="19"/>
     </row>
     <row r="156" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="97"/>
+      <c r="B156" s="101"/>
       <c r="C156" s="33" t="s">
         <v>92</v>
       </c>
@@ -8545,7 +8547,7 @@
       </c>
     </row>
     <row r="157" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="97"/>
+      <c r="B157" s="101"/>
       <c r="C157" s="33" t="s">
         <v>93</v>
       </c>
@@ -8610,7 +8612,7 @@
       </c>
     </row>
     <row r="158" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="97"/>
+      <c r="B158" s="101"/>
       <c r="C158" s="33" t="s">
         <v>94</v>
       </c>
@@ -8675,7 +8677,7 @@
       </c>
     </row>
     <row r="159" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="97"/>
+      <c r="B159" s="101"/>
       <c r="C159" s="33" t="s">
         <v>98</v>
       </c>
@@ -8718,7 +8720,7 @@
       <c r="W159" s="19"/>
     </row>
     <row r="160" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B160" s="98"/>
+      <c r="B160" s="102"/>
       <c r="C160" s="61" t="s">
         <v>99</v>
       </c>
@@ -8761,7 +8763,7 @@
       <c r="W160" s="25"/>
     </row>
     <row r="161" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="96" t="s">
+      <c r="B161" s="100" t="s">
         <v>142</v>
       </c>
       <c r="C161" s="60" t="s">
@@ -8806,7 +8808,7 @@
       <c r="W161" s="52"/>
     </row>
     <row r="162" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="97"/>
+      <c r="B162" s="101"/>
       <c r="C162" s="59" t="s">
         <v>143</v>
       </c>
@@ -8849,7 +8851,7 @@
       <c r="W162" s="19"/>
     </row>
     <row r="163" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B163" s="98"/>
+      <c r="B163" s="102"/>
       <c r="C163" s="61" t="s">
         <v>144</v>
       </c>
@@ -8892,7 +8894,7 @@
       <c r="W163" s="25"/>
     </row>
     <row r="164" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="96" t="s">
+      <c r="B164" s="100" t="s">
         <v>147</v>
       </c>
       <c r="C164" s="60" t="s">
@@ -8937,7 +8939,7 @@
       <c r="W164" s="52"/>
     </row>
     <row r="165" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="97"/>
+      <c r="B165" s="101"/>
       <c r="C165" s="59" t="s">
         <v>149</v>
       </c>
@@ -8980,7 +8982,7 @@
       <c r="W165" s="19"/>
     </row>
     <row r="166" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B166" s="97"/>
+      <c r="B166" s="101"/>
       <c r="C166" s="59" t="s">
         <v>150</v>
       </c>
@@ -9023,7 +9025,7 @@
       <c r="W166" s="19"/>
     </row>
     <row r="167" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B167" s="97"/>
+      <c r="B167" s="101"/>
       <c r="C167" s="59" t="s">
         <v>151</v>
       </c>
@@ -9066,7 +9068,7 @@
       <c r="W167" s="19"/>
     </row>
     <row r="168" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B168" s="97"/>
+      <c r="B168" s="101"/>
       <c r="C168" s="59" t="s">
         <v>152</v>
       </c>
@@ -9109,7 +9111,7 @@
       <c r="W168" s="19"/>
     </row>
     <row r="169" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B169" s="97"/>
+      <c r="B169" s="101"/>
       <c r="C169" s="59" t="s">
         <v>153</v>
       </c>
@@ -9152,7 +9154,7 @@
       <c r="W169" s="19"/>
     </row>
     <row r="170" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B170" s="98"/>
+      <c r="B170" s="102"/>
       <c r="C170" s="61" t="s">
         <v>154</v>
       </c>
@@ -9195,7 +9197,7 @@
       <c r="W170" s="25"/>
     </row>
     <row r="171" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B171" s="96" t="s">
+      <c r="B171" s="100" t="s">
         <v>18</v>
       </c>
       <c r="C171" s="54" t="s">
@@ -9240,7 +9242,7 @@
       <c r="W171" s="52"/>
     </row>
     <row r="172" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="97"/>
+      <c r="B172" s="101"/>
       <c r="C172" s="33" t="s">
         <v>136</v>
       </c>
@@ -9283,7 +9285,7 @@
       <c r="W172" s="19"/>
     </row>
     <row r="173" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B173" s="97"/>
+      <c r="B173" s="101"/>
       <c r="C173" s="33" t="s">
         <v>137</v>
       </c>
@@ -9326,7 +9328,7 @@
       <c r="W173" s="19"/>
     </row>
     <row r="174" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="97"/>
+      <c r="B174" s="101"/>
       <c r="C174" s="33" t="s">
         <v>145</v>
       </c>
@@ -9369,7 +9371,7 @@
       <c r="W174" s="19"/>
     </row>
     <row r="175" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="97"/>
+      <c r="B175" s="101"/>
       <c r="C175" s="33" t="s">
         <v>84</v>
       </c>
@@ -9412,7 +9414,7 @@
       <c r="W175" s="19"/>
     </row>
     <row r="176" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="97"/>
+      <c r="B176" s="101"/>
       <c r="C176" s="33" t="s">
         <v>85</v>
       </c>
@@ -9455,7 +9457,7 @@
       <c r="W176" s="19"/>
     </row>
     <row r="177" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B177" s="97"/>
+      <c r="B177" s="101"/>
       <c r="C177" s="33" t="s">
         <v>87</v>
       </c>
@@ -9498,7 +9500,7 @@
       <c r="W177" s="19"/>
     </row>
     <row r="178" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B178" s="97"/>
+      <c r="B178" s="101"/>
       <c r="C178" s="33" t="s">
         <v>86</v>
       </c>
@@ -9541,7 +9543,7 @@
       <c r="W178" s="19"/>
     </row>
     <row r="179" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B179" s="97"/>
+      <c r="B179" s="101"/>
       <c r="C179" s="33" t="s">
         <v>103</v>
       </c>
@@ -9584,7 +9586,7 @@
       <c r="W179" s="19"/>
     </row>
     <row r="180" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B180" s="97"/>
+      <c r="B180" s="101"/>
       <c r="C180" s="33" t="s">
         <v>135</v>
       </c>
@@ -9627,7 +9629,7 @@
       <c r="W180" s="19"/>
     </row>
     <row r="181" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B181" s="97"/>
+      <c r="B181" s="101"/>
       <c r="C181" s="33" t="s">
         <v>104</v>
       </c>
@@ -9670,21 +9672,21 @@
       <c r="W181" s="19"/>
     </row>
     <row r="182" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B182" s="105" t="s">
+      <c r="B182" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="C182" s="106"/>
-      <c r="D182" s="107"/>
-      <c r="E182" s="107"/>
-      <c r="F182" s="107"/>
-      <c r="G182" s="108"/>
+      <c r="C182" s="121"/>
+      <c r="D182" s="122"/>
+      <c r="E182" s="122"/>
+      <c r="F182" s="122"/>
+      <c r="G182" s="123"/>
       <c r="H182" s="36">
         <f t="shared" ref="H182:W182" si="6">SUM(H4:H181)</f>
         <v>95.999999999999829</v>
       </c>
       <c r="I182" s="23">
         <f t="shared" si="6"/>
-        <v>10.967299999999998</v>
+        <v>12.197299999999998</v>
       </c>
       <c r="J182" s="23">
         <f t="shared" si="6"/>
@@ -9700,7 +9702,7 @@
       </c>
       <c r="M182" s="23">
         <f t="shared" si="6"/>
-        <v>4.9109999999999969</v>
+        <v>6.1409999999999973</v>
       </c>
       <c r="N182" s="23">
         <f t="shared" si="6"/>
@@ -9752,22 +9754,22 @@
       <c r="G183" s="2"/>
       <c r="H183" s="2"/>
       <c r="I183" s="2"/>
-      <c r="J183" s="101" t="s">
+      <c r="J183" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="K183" s="110"/>
-      <c r="L183" s="110"/>
-      <c r="M183" s="110"/>
-      <c r="N183" s="110"/>
-      <c r="O183" s="110"/>
-      <c r="P183" s="110"/>
-      <c r="Q183" s="110"/>
-      <c r="R183" s="110"/>
-      <c r="S183" s="110"/>
-      <c r="T183" s="110"/>
-      <c r="U183" s="110"/>
-      <c r="V183" s="110"/>
-      <c r="W183" s="111"/>
+      <c r="K183" s="98"/>
+      <c r="L183" s="98"/>
+      <c r="M183" s="98"/>
+      <c r="N183" s="98"/>
+      <c r="O183" s="98"/>
+      <c r="P183" s="98"/>
+      <c r="Q183" s="98"/>
+      <c r="R183" s="98"/>
+      <c r="S183" s="98"/>
+      <c r="T183" s="98"/>
+      <c r="U183" s="98"/>
+      <c r="V183" s="98"/>
+      <c r="W183" s="99"/>
     </row>
     <row r="184" spans="2:23" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C184" s="59" t="s">
@@ -9799,18 +9801,18 @@
       </c>
       <c r="D185" s="4">
         <f>SUM(I10,I12,I13,I14,I15:I62,I156:I158,I160,I164:I170,I176:I177,I180)</f>
-        <v>9.3872999999999998</v>
+        <v>10.617300000000002</v>
       </c>
       <c r="E185" s="4">
         <f>SUM(C185,-D185)</f>
-        <v>37.012699999999995</v>
+        <v>35.782699999999991</v>
       </c>
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
-      <c r="H185" s="99" t="s">
+      <c r="H185" s="115" t="s">
         <v>12</v>
       </c>
-      <c r="I185" s="100"/>
+      <c r="I185" s="116"/>
       <c r="J185" s="9">
         <f>H182-J182</f>
         <v>95.999999999999829</v>
@@ -9825,11 +9827,11 @@
       </c>
       <c r="M185" s="9">
         <f>L185-M182</f>
-        <v>85.032699999999821</v>
+        <v>83.802699999999831</v>
       </c>
       <c r="N185" s="10">
         <f>M185-N182</f>
-        <v>85.032699999999821</v>
+        <v>83.802699999999831</v>
       </c>
     </row>
     <row r="186" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9875,18 +9877,18 @@
         <v>24.4</v>
       </c>
       <c r="F187" s="3"/>
-      <c r="H187" s="101" t="s">
+      <c r="H187" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="I187" s="102"/>
-      <c r="J187" s="100">
+      <c r="I187" s="117"/>
+      <c r="J187" s="116">
         <f>H182-I182</f>
-        <v>85.032699999999835</v>
-      </c>
-      <c r="K187" s="100"/>
-      <c r="L187" s="100"/>
-      <c r="M187" s="100"/>
-      <c r="N187" s="103"/>
+        <v>83.802699999999831</v>
+      </c>
+      <c r="K187" s="116"/>
+      <c r="L187" s="116"/>
+      <c r="M187" s="116"/>
+      <c r="N187" s="118"/>
     </row>
     <row r="188" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B188" s="3"/>
@@ -9990,24 +9992,6 @@
     <row r="206" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="C133:C137"/>
-    <mergeCell ref="C123:C127"/>
-    <mergeCell ref="C113:C117"/>
-    <mergeCell ref="C108:C112"/>
-    <mergeCell ref="C98:C102"/>
-    <mergeCell ref="C118:C122"/>
-    <mergeCell ref="C128:C132"/>
-    <mergeCell ref="C83:C87"/>
-    <mergeCell ref="J2:W2"/>
-    <mergeCell ref="B63:B72"/>
-    <mergeCell ref="C56:C62"/>
-    <mergeCell ref="C15:C55"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="C69:C72"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="C73:C77"/>
-    <mergeCell ref="C78:C82"/>
     <mergeCell ref="B164:B170"/>
     <mergeCell ref="H185:I185"/>
     <mergeCell ref="H187:I187"/>
@@ -10024,6 +10008,24 @@
     <mergeCell ref="C143:C147"/>
     <mergeCell ref="C93:C97"/>
     <mergeCell ref="C88:C92"/>
+    <mergeCell ref="C83:C87"/>
+    <mergeCell ref="J2:W2"/>
+    <mergeCell ref="B63:B72"/>
+    <mergeCell ref="C56:C62"/>
+    <mergeCell ref="C15:C55"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C69:C72"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C73:C77"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="C133:C137"/>
+    <mergeCell ref="C123:C127"/>
+    <mergeCell ref="C113:C117"/>
+    <mergeCell ref="C108:C112"/>
+    <mergeCell ref="C98:C102"/>
+    <mergeCell ref="C118:C122"/>
+    <mergeCell ref="C128:C132"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
tocandome con el excell
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
+++ b/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devildrake\Documents\MAP_LegendOfRadev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\MAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="166">
   <si>
     <t>Subtarea</t>
   </si>
@@ -516,12 +516,15 @@
   </si>
   <si>
     <t>Limitar el movimiento por la sala</t>
+  </si>
+  <si>
+    <t>0.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1095,7 +1098,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1346,10 +1349,43 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1358,13 +1394,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1403,35 +1436,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1451,9 +1457,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1465,7 +1471,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1508,7 +1513,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A091-4901-839C-4EC24FB5B5C8}"/>
             </c:ext>
@@ -1562,7 +1567,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1597,7 +1601,7 @@
         <xdr:cNvPr id="4" name="3 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1619,7 +1623,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1694,6 +1698,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1729,6 +1750,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1907,52 +1945,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="D175" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P205" sqref="P205"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.109375" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
     <col min="3" max="3" width="80" customWidth="1"/>
-    <col min="4" max="4" width="57.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="57.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" customWidth="1"/>
-    <col min="16" max="16" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="107" t="s">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
-      <c r="N2" s="108"/>
-      <c r="O2" s="108"/>
-      <c r="P2" s="108"/>
-      <c r="Q2" s="108"/>
-      <c r="R2" s="108"/>
-      <c r="S2" s="108"/>
-      <c r="T2" s="108"/>
-      <c r="U2" s="108"/>
-      <c r="V2" s="108"/>
-      <c r="W2" s="109"/>
-    </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="119"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="119"/>
+      <c r="P2" s="119"/>
+      <c r="Q2" s="119"/>
+      <c r="R2" s="119"/>
+      <c r="S2" s="119"/>
+      <c r="T2" s="119"/>
+      <c r="U2" s="119"/>
+      <c r="V2" s="119"/>
+      <c r="W2" s="120"/>
+    </row>
+    <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="49" t="s">
         <v>7</v>
       </c>
@@ -2020,8 +2058,8 @@
         <v>43067</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="121" t="s">
+    <row r="4" spans="1:23" s="1" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="131" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="32" t="s">
@@ -2042,7 +2080,7 @@
       </c>
       <c r="I4" s="35">
         <f t="shared" ref="I4:I35" si="0">SUM(J4:W4)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J4" s="72">
         <v>0</v>
@@ -2060,7 +2098,7 @@
         <v>0</v>
       </c>
       <c r="O4" s="62">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P4" s="103"/>
       <c r="Q4" s="37"/>
@@ -2071,8 +2109,8 @@
       <c r="V4" s="36"/>
       <c r="W4" s="38"/>
     </row>
-    <row r="5" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="122"/>
+    <row r="5" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="132"/>
       <c r="C5" s="30" t="s">
         <v>100</v>
       </c>
@@ -2091,7 +2129,7 @@
       </c>
       <c r="I5" s="48">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="J5" s="63">
         <v>0</v>
@@ -2111,7 +2149,9 @@
       <c r="O5" s="63">
         <v>0</v>
       </c>
-      <c r="P5" s="94"/>
+      <c r="P5" s="94">
+        <v>3.5</v>
+      </c>
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
       <c r="S5" s="15"/>
@@ -2120,8 +2160,8 @@
       <c r="V5" s="15"/>
       <c r="W5" s="16"/>
     </row>
-    <row r="6" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="122"/>
+    <row r="6" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="132"/>
       <c r="C6" s="30" t="s">
         <v>101</v>
       </c>
@@ -2169,8 +2209,8 @@
       <c r="V6" s="15"/>
       <c r="W6" s="16"/>
     </row>
-    <row r="7" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="122"/>
+    <row r="7" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="132"/>
       <c r="C7" s="30" t="s">
         <v>102</v>
       </c>
@@ -2218,8 +2258,8 @@
       <c r="V7" s="15"/>
       <c r="W7" s="16"/>
     </row>
-    <row r="8" spans="1:23" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="123"/>
+    <row r="8" spans="1:23" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="133"/>
       <c r="C8" s="39" t="s">
         <v>110</v>
       </c>
@@ -2238,7 +2278,7 @@
       </c>
       <c r="I8" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J8" s="64">
         <v>0</v>
@@ -2256,9 +2296,11 @@
         <v>0</v>
       </c>
       <c r="O8" s="64">
-        <v>0</v>
-      </c>
-      <c r="P8" s="95"/>
+        <v>0.5</v>
+      </c>
+      <c r="P8" s="95">
+        <v>1</v>
+      </c>
       <c r="Q8" s="18"/>
       <c r="R8" s="18"/>
       <c r="S8" s="18"/>
@@ -2267,8 +2309,8 @@
       <c r="V8" s="18"/>
       <c r="W8" s="21"/>
     </row>
-    <row r="9" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="121" t="s">
+    <row r="9" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="131" t="s">
         <v>105</v>
       </c>
       <c r="C9" s="42" t="s">
@@ -2312,8 +2354,8 @@
       <c r="V9" s="77"/>
       <c r="W9" s="78"/>
     </row>
-    <row r="10" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="122"/>
+    <row r="10" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="132"/>
       <c r="C10" s="29" t="s">
         <v>106</v>
       </c>
@@ -2361,8 +2403,8 @@
       <c r="V10" s="15"/>
       <c r="W10" s="16"/>
     </row>
-    <row r="11" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="122"/>
+    <row r="11" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="132"/>
       <c r="C11" s="76" t="s">
         <v>111</v>
       </c>
@@ -2410,8 +2452,8 @@
       <c r="V11" s="15"/>
       <c r="W11" s="16"/>
     </row>
-    <row r="12" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="122"/>
+    <row r="12" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="132"/>
       <c r="C12" s="76" t="s">
         <v>112</v>
       </c>
@@ -2475,8 +2517,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="123"/>
+    <row r="13" spans="1:23" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="133"/>
       <c r="C13" s="46" t="s">
         <v>97</v>
       </c>
@@ -2524,8 +2566,8 @@
       <c r="V13" s="18"/>
       <c r="W13" s="21"/>
     </row>
-    <row r="14" spans="1:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B14" s="110" t="s">
+    <row r="14" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="47" t="s">
@@ -2577,9 +2619,9 @@
       <c r="V14" s="44"/>
       <c r="W14" s="45"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B15" s="111"/>
-      <c r="C15" s="115" t="s">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="107"/>
+      <c r="C15" s="125" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -2628,9 +2670,9 @@
       <c r="V15" s="15"/>
       <c r="W15" s="16"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B16" s="111"/>
-      <c r="C16" s="116"/>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B16" s="107"/>
+      <c r="C16" s="126"/>
       <c r="D16" s="4" t="s">
         <v>20</v>
       </c>
@@ -2677,9 +2719,9 @@
       <c r="V16" s="15"/>
       <c r="W16" s="16"/>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B17" s="111"/>
-      <c r="C17" s="116"/>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" s="107"/>
+      <c r="C17" s="126"/>
       <c r="D17" s="4" t="s">
         <v>21</v>
       </c>
@@ -2728,9 +2770,9 @@
       <c r="V17" s="15"/>
       <c r="W17" s="16"/>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B18" s="111"/>
-      <c r="C18" s="116"/>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B18" s="107"/>
+      <c r="C18" s="126"/>
       <c r="D18" s="4" t="s">
         <v>22</v>
       </c>
@@ -2779,9 +2821,9 @@
       <c r="V18" s="15"/>
       <c r="W18" s="16"/>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B19" s="111"/>
-      <c r="C19" s="116"/>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B19" s="107"/>
+      <c r="C19" s="126"/>
       <c r="D19" s="4" t="s">
         <v>23</v>
       </c>
@@ -2828,9 +2870,9 @@
       <c r="V19" s="15"/>
       <c r="W19" s="16"/>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B20" s="111"/>
-      <c r="C20" s="116"/>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B20" s="107"/>
+      <c r="C20" s="126"/>
       <c r="D20" s="4" t="s">
         <v>162</v>
       </c>
@@ -2877,9 +2919,9 @@
       <c r="V20" s="15"/>
       <c r="W20" s="16"/>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B21" s="111"/>
-      <c r="C21" s="116"/>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B21" s="107"/>
+      <c r="C21" s="126"/>
       <c r="D21" s="4" t="s">
         <v>24</v>
       </c>
@@ -2926,9 +2968,9 @@
       <c r="V21" s="15"/>
       <c r="W21" s="16"/>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B22" s="111"/>
-      <c r="C22" s="116"/>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B22" s="107"/>
+      <c r="C22" s="126"/>
       <c r="D22" s="27" t="s">
         <v>36</v>
       </c>
@@ -2975,9 +3017,9 @@
       <c r="V22" s="15"/>
       <c r="W22" s="16"/>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B23" s="111"/>
-      <c r="C23" s="116"/>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B23" s="107"/>
+      <c r="C23" s="126"/>
       <c r="D23" s="27" t="s">
         <v>37</v>
       </c>
@@ -3024,9 +3066,9 @@
       <c r="V23" s="15"/>
       <c r="W23" s="16"/>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B24" s="111"/>
-      <c r="C24" s="116"/>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B24" s="107"/>
+      <c r="C24" s="126"/>
       <c r="D24" s="27" t="s">
         <v>38</v>
       </c>
@@ -3073,9 +3115,9 @@
       <c r="V24" s="15"/>
       <c r="W24" s="16"/>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B25" s="111"/>
-      <c r="C25" s="116"/>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B25" s="107"/>
+      <c r="C25" s="126"/>
       <c r="D25" s="27" t="s">
         <v>39</v>
       </c>
@@ -3122,9 +3164,9 @@
       <c r="V25" s="15"/>
       <c r="W25" s="16"/>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B26" s="111"/>
-      <c r="C26" s="116"/>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B26" s="107"/>
+      <c r="C26" s="126"/>
       <c r="D26" s="27" t="s">
         <v>40</v>
       </c>
@@ -3171,9 +3213,9 @@
       <c r="V26" s="15"/>
       <c r="W26" s="16"/>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B27" s="111"/>
-      <c r="C27" s="116"/>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B27" s="107"/>
+      <c r="C27" s="126"/>
       <c r="D27" s="27" t="s">
         <v>41</v>
       </c>
@@ -3220,9 +3262,9 @@
       <c r="V27" s="15"/>
       <c r="W27" s="16"/>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B28" s="111"/>
-      <c r="C28" s="116"/>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B28" s="107"/>
+      <c r="C28" s="126"/>
       <c r="D28" s="27" t="s">
         <v>42</v>
       </c>
@@ -3269,9 +3311,9 @@
       <c r="V28" s="15"/>
       <c r="W28" s="16"/>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B29" s="111"/>
-      <c r="C29" s="116"/>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B29" s="107"/>
+      <c r="C29" s="126"/>
       <c r="D29" s="27" t="s">
         <v>43</v>
       </c>
@@ -3318,9 +3360,9 @@
       <c r="V29" s="15"/>
       <c r="W29" s="16"/>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B30" s="111"/>
-      <c r="C30" s="116"/>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B30" s="107"/>
+      <c r="C30" s="126"/>
       <c r="D30" s="27" t="s">
         <v>44</v>
       </c>
@@ -3367,9 +3409,9 @@
       <c r="V30" s="15"/>
       <c r="W30" s="16"/>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B31" s="111"/>
-      <c r="C31" s="116"/>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B31" s="107"/>
+      <c r="C31" s="126"/>
       <c r="D31" s="27" t="s">
         <v>45</v>
       </c>
@@ -3416,9 +3458,9 @@
       <c r="V31" s="15"/>
       <c r="W31" s="16"/>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B32" s="111"/>
-      <c r="C32" s="116"/>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B32" s="107"/>
+      <c r="C32" s="126"/>
       <c r="D32" s="27" t="s">
         <v>46</v>
       </c>
@@ -3465,9 +3507,9 @@
       <c r="V32" s="15"/>
       <c r="W32" s="16"/>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B33" s="111"/>
-      <c r="C33" s="116"/>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B33" s="107"/>
+      <c r="C33" s="126"/>
       <c r="D33" s="27" t="s">
         <v>47</v>
       </c>
@@ -3514,9 +3556,9 @@
       <c r="V33" s="15"/>
       <c r="W33" s="16"/>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B34" s="111"/>
-      <c r="C34" s="116"/>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B34" s="107"/>
+      <c r="C34" s="126"/>
       <c r="D34" s="27" t="s">
         <v>48</v>
       </c>
@@ -3563,9 +3605,9 @@
       <c r="V34" s="15"/>
       <c r="W34" s="16"/>
     </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B35" s="111"/>
-      <c r="C35" s="116"/>
+    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B35" s="107"/>
+      <c r="C35" s="126"/>
       <c r="D35" s="27" t="s">
         <v>49</v>
       </c>
@@ -3612,9 +3654,9 @@
       <c r="V35" s="15"/>
       <c r="W35" s="16"/>
     </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B36" s="111"/>
-      <c r="C36" s="116"/>
+    <row r="36" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B36" s="107"/>
+      <c r="C36" s="126"/>
       <c r="D36" s="27" t="s">
         <v>50</v>
       </c>
@@ -3661,9 +3703,9 @@
       <c r="V36" s="15"/>
       <c r="W36" s="16"/>
     </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B37" s="111"/>
-      <c r="C37" s="116"/>
+    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B37" s="107"/>
+      <c r="C37" s="126"/>
       <c r="D37" s="27" t="s">
         <v>51</v>
       </c>
@@ -3710,9 +3752,9 @@
       <c r="V37" s="15"/>
       <c r="W37" s="16"/>
     </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B38" s="111"/>
-      <c r="C38" s="116"/>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B38" s="107"/>
+      <c r="C38" s="126"/>
       <c r="D38" s="27" t="s">
         <v>52</v>
       </c>
@@ -3759,9 +3801,9 @@
       <c r="V38" s="15"/>
       <c r="W38" s="16"/>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B39" s="111"/>
-      <c r="C39" s="116"/>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B39" s="107"/>
+      <c r="C39" s="126"/>
       <c r="D39" s="27" t="s">
         <v>53</v>
       </c>
@@ -3808,9 +3850,9 @@
       <c r="V39" s="15"/>
       <c r="W39" s="16"/>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B40" s="111"/>
-      <c r="C40" s="116"/>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B40" s="107"/>
+      <c r="C40" s="126"/>
       <c r="D40" s="27" t="s">
         <v>54</v>
       </c>
@@ -3857,9 +3899,9 @@
       <c r="V40" s="15"/>
       <c r="W40" s="16"/>
     </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B41" s="111"/>
-      <c r="C41" s="116"/>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B41" s="107"/>
+      <c r="C41" s="126"/>
       <c r="D41" s="27" t="s">
         <v>55</v>
       </c>
@@ -3906,9 +3948,9 @@
       <c r="V41" s="15"/>
       <c r="W41" s="16"/>
     </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B42" s="111"/>
-      <c r="C42" s="116"/>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B42" s="107"/>
+      <c r="C42" s="126"/>
       <c r="D42" s="27" t="s">
         <v>56</v>
       </c>
@@ -3955,9 +3997,9 @@
       <c r="V42" s="15"/>
       <c r="W42" s="16"/>
     </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B43" s="111"/>
-      <c r="C43" s="116"/>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B43" s="107"/>
+      <c r="C43" s="126"/>
       <c r="D43" s="27" t="s">
         <v>57</v>
       </c>
@@ -4004,9 +4046,9 @@
       <c r="V43" s="15"/>
       <c r="W43" s="16"/>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B44" s="111"/>
-      <c r="C44" s="116"/>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B44" s="107"/>
+      <c r="C44" s="126"/>
       <c r="D44" s="27" t="s">
         <v>58</v>
       </c>
@@ -4053,9 +4095,9 @@
       <c r="V44" s="15"/>
       <c r="W44" s="16"/>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B45" s="111"/>
-      <c r="C45" s="116"/>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B45" s="107"/>
+      <c r="C45" s="126"/>
       <c r="D45" s="27" t="s">
         <v>59</v>
       </c>
@@ -4102,9 +4144,9 @@
       <c r="V45" s="15"/>
       <c r="W45" s="16"/>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B46" s="111"/>
-      <c r="C46" s="116"/>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B46" s="107"/>
+      <c r="C46" s="126"/>
       <c r="D46" s="27" t="s">
         <v>60</v>
       </c>
@@ -4151,9 +4193,9 @@
       <c r="V46" s="15"/>
       <c r="W46" s="16"/>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B47" s="111"/>
-      <c r="C47" s="116"/>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B47" s="107"/>
+      <c r="C47" s="126"/>
       <c r="D47" s="27" t="s">
         <v>61</v>
       </c>
@@ -4200,9 +4242,9 @@
       <c r="V47" s="15"/>
       <c r="W47" s="16"/>
     </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B48" s="111"/>
-      <c r="C48" s="116"/>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B48" s="107"/>
+      <c r="C48" s="126"/>
       <c r="D48" s="27" t="s">
         <v>62</v>
       </c>
@@ -4249,9 +4291,9 @@
       <c r="V48" s="15"/>
       <c r="W48" s="16"/>
     </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B49" s="111"/>
-      <c r="C49" s="116"/>
+    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B49" s="107"/>
+      <c r="C49" s="126"/>
       <c r="D49" s="27" t="s">
         <v>63</v>
       </c>
@@ -4298,9 +4340,9 @@
       <c r="V49" s="15"/>
       <c r="W49" s="16"/>
     </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B50" s="111"/>
-      <c r="C50" s="116"/>
+    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B50" s="107"/>
+      <c r="C50" s="126"/>
       <c r="D50" s="27" t="s">
         <v>64</v>
       </c>
@@ -4347,9 +4389,9 @@
       <c r="V50" s="15"/>
       <c r="W50" s="16"/>
     </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B51" s="111"/>
-      <c r="C51" s="116"/>
+    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B51" s="107"/>
+      <c r="C51" s="126"/>
       <c r="D51" s="27" t="s">
         <v>65</v>
       </c>
@@ -4396,9 +4438,9 @@
       <c r="V51" s="15"/>
       <c r="W51" s="16"/>
     </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B52" s="111"/>
-      <c r="C52" s="116"/>
+    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B52" s="107"/>
+      <c r="C52" s="126"/>
       <c r="D52" s="27" t="s">
         <v>66</v>
       </c>
@@ -4445,9 +4487,9 @@
       <c r="V52" s="15"/>
       <c r="W52" s="16"/>
     </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B53" s="111"/>
-      <c r="C53" s="116"/>
+    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B53" s="107"/>
+      <c r="C53" s="126"/>
       <c r="D53" s="27" t="s">
         <v>67</v>
       </c>
@@ -4494,9 +4536,9 @@
       <c r="V53" s="15"/>
       <c r="W53" s="16"/>
     </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B54" s="111"/>
-      <c r="C54" s="116"/>
+    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B54" s="107"/>
+      <c r="C54" s="126"/>
       <c r="D54" s="27" t="s">
         <v>68</v>
       </c>
@@ -4543,9 +4585,9 @@
       <c r="V54" s="15"/>
       <c r="W54" s="16"/>
     </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B55" s="111"/>
-      <c r="C55" s="117"/>
+    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B55" s="107"/>
+      <c r="C55" s="127"/>
       <c r="D55" s="27" t="s">
         <v>69</v>
       </c>
@@ -4592,9 +4634,9 @@
       <c r="V55" s="15"/>
       <c r="W55" s="16"/>
     </row>
-    <row r="56" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B56" s="111"/>
-      <c r="C56" s="113" t="s">
+    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B56" s="107"/>
+      <c r="C56" s="123" t="s">
         <v>26</v>
       </c>
       <c r="D56" s="24" t="s">
@@ -4643,9 +4685,9 @@
       <c r="V56" s="15"/>
       <c r="W56" s="16"/>
     </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B57" s="111"/>
-      <c r="C57" s="114"/>
+    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B57" s="107"/>
+      <c r="C57" s="124"/>
       <c r="D57" s="24" t="s">
         <v>29</v>
       </c>
@@ -4692,9 +4734,9 @@
       <c r="V57" s="15"/>
       <c r="W57" s="16"/>
     </row>
-    <row r="58" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B58" s="111"/>
-      <c r="C58" s="114"/>
+    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B58" s="107"/>
+      <c r="C58" s="124"/>
       <c r="D58" s="24" t="s">
         <v>30</v>
       </c>
@@ -4741,9 +4783,9 @@
       <c r="V58" s="15"/>
       <c r="W58" s="16"/>
     </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B59" s="111"/>
-      <c r="C59" s="114"/>
+    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B59" s="107"/>
+      <c r="C59" s="124"/>
       <c r="D59" s="24" t="s">
         <v>31</v>
       </c>
@@ -4790,9 +4832,9 @@
       <c r="V59" s="15"/>
       <c r="W59" s="16"/>
     </row>
-    <row r="60" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B60" s="111"/>
-      <c r="C60" s="114"/>
+    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B60" s="107"/>
+      <c r="C60" s="124"/>
       <c r="D60" s="24" t="s">
         <v>34</v>
       </c>
@@ -4839,9 +4881,9 @@
       <c r="V60" s="15"/>
       <c r="W60" s="16"/>
     </row>
-    <row r="61" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B61" s="111"/>
-      <c r="C61" s="114"/>
+    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B61" s="107"/>
+      <c r="C61" s="124"/>
       <c r="D61" s="24" t="s">
         <v>32</v>
       </c>
@@ -4888,9 +4930,9 @@
       <c r="V61" s="15"/>
       <c r="W61" s="16"/>
     </row>
-    <row r="62" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="129"/>
-      <c r="C62" s="114"/>
+    <row r="62" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="114"/>
+      <c r="C62" s="124"/>
       <c r="D62" s="55" t="s">
         <v>33</v>
       </c>
@@ -4937,11 +4979,11 @@
       <c r="V62" s="22"/>
       <c r="W62" s="23"/>
     </row>
-    <row r="63" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B63" s="110" t="s">
+    <row r="63" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B63" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="118" t="s">
+      <c r="C63" s="128" t="s">
         <v>79</v>
       </c>
       <c r="D63" s="34" t="s">
@@ -4990,9 +5032,9 @@
       <c r="V63" s="44"/>
       <c r="W63" s="45"/>
     </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B64" s="111"/>
-      <c r="C64" s="119"/>
+    <row r="64" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B64" s="107"/>
+      <c r="C64" s="129"/>
       <c r="D64" s="4" t="s">
         <v>71</v>
       </c>
@@ -5039,9 +5081,9 @@
       <c r="V64" s="15"/>
       <c r="W64" s="16"/>
     </row>
-    <row r="65" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B65" s="111"/>
-      <c r="C65" s="119"/>
+    <row r="65" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B65" s="107"/>
+      <c r="C65" s="129"/>
       <c r="D65" s="4" t="s">
         <v>72</v>
       </c>
@@ -5088,9 +5130,9 @@
       <c r="V65" s="15"/>
       <c r="W65" s="16"/>
     </row>
-    <row r="66" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B66" s="111"/>
-      <c r="C66" s="119"/>
+    <row r="66" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B66" s="107"/>
+      <c r="C66" s="129"/>
       <c r="D66" s="24" t="s">
         <v>76</v>
       </c>
@@ -5137,8 +5179,8 @@
       <c r="V66" s="15"/>
       <c r="W66" s="16"/>
     </row>
-    <row r="67" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B67" s="111"/>
+    <row r="67" spans="2:23" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B67" s="107"/>
       <c r="C67" s="28" t="s">
         <v>73</v>
       </c>
@@ -5186,8 +5228,8 @@
       <c r="V67" s="15"/>
       <c r="W67" s="16"/>
     </row>
-    <row r="68" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B68" s="111"/>
+    <row r="68" spans="2:23" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B68" s="107"/>
       <c r="C68" s="28" t="s">
         <v>81</v>
       </c>
@@ -5235,9 +5277,9 @@
       <c r="V68" s="15"/>
       <c r="W68" s="16"/>
     </row>
-    <row r="69" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="111"/>
-      <c r="C69" s="119" t="s">
+    <row r="69" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="107"/>
+      <c r="C69" s="129" t="s">
         <v>80</v>
       </c>
       <c r="D69" s="4" t="s">
@@ -5286,9 +5328,9 @@
       <c r="V69" s="15"/>
       <c r="W69" s="16"/>
     </row>
-    <row r="70" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="111"/>
-      <c r="C70" s="119"/>
+    <row r="70" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="107"/>
+      <c r="C70" s="129"/>
       <c r="D70" s="4" t="s">
         <v>75</v>
       </c>
@@ -5335,9 +5377,9 @@
       <c r="V70" s="15"/>
       <c r="W70" s="16"/>
     </row>
-    <row r="71" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="111"/>
-      <c r="C71" s="119"/>
+    <row r="71" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="107"/>
+      <c r="C71" s="129"/>
       <c r="D71" s="4" t="s">
         <v>77</v>
       </c>
@@ -5384,9 +5426,9 @@
       <c r="V71" s="15"/>
       <c r="W71" s="16"/>
     </row>
-    <row r="72" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="112"/>
-      <c r="C72" s="120"/>
+    <row r="72" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="108"/>
+      <c r="C72" s="130"/>
       <c r="D72" s="20" t="s">
         <v>78</v>
       </c>
@@ -5433,11 +5475,11 @@
       <c r="V72" s="18"/>
       <c r="W72" s="21"/>
     </row>
-    <row r="73" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="110" t="s">
+    <row r="73" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="106" t="s">
         <v>115</v>
       </c>
-      <c r="C73" s="124" t="s">
+      <c r="C73" s="134" t="s">
         <v>116</v>
       </c>
       <c r="D73" s="34" t="s">
@@ -5484,9 +5526,9 @@
       <c r="V73" s="77"/>
       <c r="W73" s="78"/>
     </row>
-    <row r="74" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="111"/>
-      <c r="C74" s="106"/>
+    <row r="74" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="107"/>
+      <c r="C74" s="118"/>
       <c r="D74" s="4" t="s">
         <v>132</v>
       </c>
@@ -5533,9 +5575,9 @@
       <c r="V74" s="15"/>
       <c r="W74" s="16"/>
     </row>
-    <row r="75" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="111"/>
-      <c r="C75" s="106"/>
+    <row r="75" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="107"/>
+      <c r="C75" s="118"/>
       <c r="D75" s="4" t="s">
         <v>161</v>
       </c>
@@ -5582,9 +5624,9 @@
       <c r="V75" s="15"/>
       <c r="W75" s="16"/>
     </row>
-    <row r="76" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="111"/>
-      <c r="C76" s="106"/>
+    <row r="76" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="107"/>
+      <c r="C76" s="118"/>
       <c r="D76" s="4" t="s">
         <v>133</v>
       </c>
@@ -5627,9 +5669,9 @@
       <c r="V76" s="84"/>
       <c r="W76" s="85"/>
     </row>
-    <row r="77" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="111"/>
-      <c r="C77" s="106"/>
+    <row r="77" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="107"/>
+      <c r="C77" s="118"/>
       <c r="D77" s="4" t="s">
         <v>164</v>
       </c>
@@ -5676,9 +5718,9 @@
       <c r="V77" s="91"/>
       <c r="W77" s="92"/>
     </row>
-    <row r="78" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="111"/>
-      <c r="C78" s="106"/>
+    <row r="78" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="107"/>
+      <c r="C78" s="118"/>
       <c r="D78" s="4" t="s">
         <v>163</v>
       </c>
@@ -5725,9 +5767,9 @@
       <c r="V78" s="91"/>
       <c r="W78" s="92"/>
     </row>
-    <row r="79" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B79" s="111"/>
-      <c r="C79" s="106"/>
+    <row r="79" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="107"/>
+      <c r="C79" s="118"/>
       <c r="D79" s="4" t="s">
         <v>134</v>
       </c>
@@ -5774,9 +5816,9 @@
       <c r="V79" s="15"/>
       <c r="W79" s="16"/>
     </row>
-    <row r="80" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B80" s="111"/>
-      <c r="C80" s="106" t="s">
+    <row r="80" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="107"/>
+      <c r="C80" s="118" t="s">
         <v>117</v>
       </c>
       <c r="D80" s="4" t="s">
@@ -5823,9 +5865,9 @@
       <c r="V80" s="84"/>
       <c r="W80" s="85"/>
     </row>
-    <row r="81" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B81" s="111"/>
-      <c r="C81" s="106"/>
+    <row r="81" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="107"/>
+      <c r="C81" s="118"/>
       <c r="D81" s="4" t="s">
         <v>132</v>
       </c>
@@ -5872,9 +5914,9 @@
       <c r="V81" s="15"/>
       <c r="W81" s="16"/>
     </row>
-    <row r="82" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B82" s="111"/>
-      <c r="C82" s="106"/>
+    <row r="82" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="107"/>
+      <c r="C82" s="118"/>
       <c r="D82" s="4" t="s">
         <v>161</v>
       </c>
@@ -5921,9 +5963,9 @@
       <c r="V82" s="15"/>
       <c r="W82" s="16"/>
     </row>
-    <row r="83" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="111"/>
-      <c r="C83" s="106"/>
+    <row r="83" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="107"/>
+      <c r="C83" s="118"/>
       <c r="D83" s="4" t="s">
         <v>164</v>
       </c>
@@ -5970,9 +6012,9 @@
       <c r="V83" s="15"/>
       <c r="W83" s="16"/>
     </row>
-    <row r="84" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B84" s="111"/>
-      <c r="C84" s="106"/>
+    <row r="84" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="107"/>
+      <c r="C84" s="118"/>
       <c r="D84" s="4" t="s">
         <v>163</v>
       </c>
@@ -6019,9 +6061,9 @@
       <c r="V84" s="15"/>
       <c r="W84" s="16"/>
     </row>
-    <row r="85" spans="2:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="111"/>
-      <c r="C85" s="106"/>
+    <row r="85" spans="2:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="107"/>
+      <c r="C85" s="118"/>
       <c r="D85" s="4" t="s">
         <v>133</v>
       </c>
@@ -6064,9 +6106,9 @@
       <c r="V85" s="84"/>
       <c r="W85" s="85"/>
     </row>
-    <row r="86" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="111"/>
-      <c r="C86" s="106"/>
+    <row r="86" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="107"/>
+      <c r="C86" s="118"/>
       <c r="D86" s="4" t="s">
         <v>134</v>
       </c>
@@ -6113,9 +6155,9 @@
       <c r="V86" s="15"/>
       <c r="W86" s="16"/>
     </row>
-    <row r="87" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B87" s="111"/>
-      <c r="C87" s="106" t="s">
+    <row r="87" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="107"/>
+      <c r="C87" s="118" t="s">
         <v>118</v>
       </c>
       <c r="D87" s="4" t="s">
@@ -6164,9 +6206,9 @@
       <c r="V87" s="15"/>
       <c r="W87" s="16"/>
     </row>
-    <row r="88" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B88" s="111"/>
-      <c r="C88" s="106"/>
+    <row r="88" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="107"/>
+      <c r="C88" s="118"/>
       <c r="D88" s="4" t="s">
         <v>132</v>
       </c>
@@ -6213,9 +6255,9 @@
       <c r="V88" s="15"/>
       <c r="W88" s="16"/>
     </row>
-    <row r="89" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="111"/>
-      <c r="C89" s="106"/>
+    <row r="89" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="107"/>
+      <c r="C89" s="118"/>
       <c r="D89" s="4" t="s">
         <v>161</v>
       </c>
@@ -6262,9 +6304,9 @@
       <c r="V89" s="15"/>
       <c r="W89" s="16"/>
     </row>
-    <row r="90" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="111"/>
-      <c r="C90" s="106"/>
+    <row r="90" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="107"/>
+      <c r="C90" s="118"/>
       <c r="D90" s="4" t="s">
         <v>133</v>
       </c>
@@ -6307,9 +6349,9 @@
       <c r="V90" s="84"/>
       <c r="W90" s="85"/>
     </row>
-    <row r="91" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="111"/>
-      <c r="C91" s="106"/>
+    <row r="91" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="107"/>
+      <c r="C91" s="118"/>
       <c r="D91" s="4" t="s">
         <v>164</v>
       </c>
@@ -6356,9 +6398,9 @@
       <c r="V91" s="91"/>
       <c r="W91" s="92"/>
     </row>
-    <row r="92" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="111"/>
-      <c r="C92" s="106"/>
+    <row r="92" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="107"/>
+      <c r="C92" s="118"/>
       <c r="D92" s="4" t="s">
         <v>163</v>
       </c>
@@ -6405,9 +6447,9 @@
       <c r="V92" s="91"/>
       <c r="W92" s="92"/>
     </row>
-    <row r="93" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B93" s="111"/>
-      <c r="C93" s="106"/>
+    <row r="93" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="107"/>
+      <c r="C93" s="118"/>
       <c r="D93" s="4" t="s">
         <v>134</v>
       </c>
@@ -6454,9 +6496,9 @@
       <c r="V93" s="15"/>
       <c r="W93" s="16"/>
     </row>
-    <row r="94" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B94" s="111"/>
-      <c r="C94" s="106" t="s">
+    <row r="94" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="107"/>
+      <c r="C94" s="118" t="s">
         <v>119</v>
       </c>
       <c r="D94" s="4" t="s">
@@ -6505,9 +6547,9 @@
       <c r="V94" s="15"/>
       <c r="W94" s="16"/>
     </row>
-    <row r="95" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B95" s="111"/>
-      <c r="C95" s="106"/>
+    <row r="95" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="107"/>
+      <c r="C95" s="118"/>
       <c r="D95" s="4" t="s">
         <v>132</v>
       </c>
@@ -6554,9 +6596,9 @@
       <c r="V95" s="15"/>
       <c r="W95" s="16"/>
     </row>
-    <row r="96" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B96" s="111"/>
-      <c r="C96" s="106"/>
+    <row r="96" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="107"/>
+      <c r="C96" s="118"/>
       <c r="D96" s="4" t="s">
         <v>161</v>
       </c>
@@ -6603,9 +6645,9 @@
       <c r="V96" s="15"/>
       <c r="W96" s="16"/>
     </row>
-    <row r="97" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B97" s="111"/>
-      <c r="C97" s="106"/>
+    <row r="97" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="107"/>
+      <c r="C97" s="118"/>
       <c r="D97" s="4" t="s">
         <v>133</v>
       </c>
@@ -6648,9 +6690,9 @@
       <c r="V97" s="84"/>
       <c r="W97" s="85"/>
     </row>
-    <row r="98" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B98" s="111"/>
-      <c r="C98" s="106"/>
+    <row r="98" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="107"/>
+      <c r="C98" s="118"/>
       <c r="D98" s="4" t="s">
         <v>164</v>
       </c>
@@ -6697,9 +6739,9 @@
       <c r="V98" s="91"/>
       <c r="W98" s="92"/>
     </row>
-    <row r="99" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B99" s="111"/>
-      <c r="C99" s="106"/>
+    <row r="99" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="107"/>
+      <c r="C99" s="118"/>
       <c r="D99" s="4" t="s">
         <v>163</v>
       </c>
@@ -6746,9 +6788,9 @@
       <c r="V99" s="91"/>
       <c r="W99" s="92"/>
     </row>
-    <row r="100" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B100" s="111"/>
-      <c r="C100" s="106"/>
+    <row r="100" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="107"/>
+      <c r="C100" s="118"/>
       <c r="D100" s="4" t="s">
         <v>134</v>
       </c>
@@ -6795,9 +6837,9 @@
       <c r="V100" s="15"/>
       <c r="W100" s="16"/>
     </row>
-    <row r="101" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B101" s="111"/>
-      <c r="C101" s="106" t="s">
+    <row r="101" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="107"/>
+      <c r="C101" s="118" t="s">
         <v>120</v>
       </c>
       <c r="D101" s="4" t="s">
@@ -6846,9 +6888,9 @@
       <c r="V101" s="15"/>
       <c r="W101" s="16"/>
     </row>
-    <row r="102" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B102" s="111"/>
-      <c r="C102" s="106"/>
+    <row r="102" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="107"/>
+      <c r="C102" s="118"/>
       <c r="D102" s="4" t="s">
         <v>132</v>
       </c>
@@ -6895,9 +6937,9 @@
       <c r="V102" s="15"/>
       <c r="W102" s="16"/>
     </row>
-    <row r="103" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="111"/>
-      <c r="C103" s="106"/>
+    <row r="103" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="107"/>
+      <c r="C103" s="118"/>
       <c r="D103" s="4" t="s">
         <v>161</v>
       </c>
@@ -6944,9 +6986,9 @@
       <c r="V103" s="15"/>
       <c r="W103" s="16"/>
     </row>
-    <row r="104" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B104" s="111"/>
-      <c r="C104" s="106"/>
+    <row r="104" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="107"/>
+      <c r="C104" s="118"/>
       <c r="D104" s="4" t="s">
         <v>133</v>
       </c>
@@ -6989,9 +7031,9 @@
       <c r="V104" s="84"/>
       <c r="W104" s="85"/>
     </row>
-    <row r="105" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B105" s="111"/>
-      <c r="C105" s="106"/>
+    <row r="105" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="107"/>
+      <c r="C105" s="118"/>
       <c r="D105" s="4" t="s">
         <v>164</v>
       </c>
@@ -7038,9 +7080,9 @@
       <c r="V105" s="91"/>
       <c r="W105" s="92"/>
     </row>
-    <row r="106" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B106" s="111"/>
-      <c r="C106" s="106"/>
+    <row r="106" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="107"/>
+      <c r="C106" s="118"/>
       <c r="D106" s="4" t="s">
         <v>163</v>
       </c>
@@ -7087,9 +7129,9 @@
       <c r="V106" s="91"/>
       <c r="W106" s="92"/>
     </row>
-    <row r="107" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="111"/>
-      <c r="C107" s="106"/>
+    <row r="107" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="107"/>
+      <c r="C107" s="118"/>
       <c r="D107" s="4" t="s">
         <v>134</v>
       </c>
@@ -7138,9 +7180,9 @@
       <c r="V107" s="15"/>
       <c r="W107" s="16"/>
     </row>
-    <row r="108" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B108" s="111"/>
-      <c r="C108" s="106" t="s">
+    <row r="108" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="107"/>
+      <c r="C108" s="118" t="s">
         <v>121</v>
       </c>
       <c r="D108" s="4" t="s">
@@ -7189,9 +7231,9 @@
       <c r="V108" s="15"/>
       <c r="W108" s="16"/>
     </row>
-    <row r="109" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B109" s="111"/>
-      <c r="C109" s="106"/>
+    <row r="109" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="107"/>
+      <c r="C109" s="118"/>
       <c r="D109" s="4" t="s">
         <v>132</v>
       </c>
@@ -7238,9 +7280,9 @@
       <c r="V109" s="15"/>
       <c r="W109" s="16"/>
     </row>
-    <row r="110" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B110" s="111"/>
-      <c r="C110" s="106"/>
+    <row r="110" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B110" s="107"/>
+      <c r="C110" s="118"/>
       <c r="D110" s="4" t="s">
         <v>161</v>
       </c>
@@ -7287,9 +7329,9 @@
       <c r="V110" s="15"/>
       <c r="W110" s="16"/>
     </row>
-    <row r="111" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B111" s="111"/>
-      <c r="C111" s="106"/>
+    <row r="111" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B111" s="107"/>
+      <c r="C111" s="118"/>
       <c r="D111" s="4" t="s">
         <v>133</v>
       </c>
@@ -7332,9 +7374,9 @@
       <c r="V111" s="84"/>
       <c r="W111" s="85"/>
     </row>
-    <row r="112" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B112" s="111"/>
-      <c r="C112" s="106"/>
+    <row r="112" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B112" s="107"/>
+      <c r="C112" s="118"/>
       <c r="D112" s="4" t="s">
         <v>164</v>
       </c>
@@ -7381,9 +7423,9 @@
       <c r="V112" s="91"/>
       <c r="W112" s="92"/>
     </row>
-    <row r="113" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B113" s="111"/>
-      <c r="C113" s="106"/>
+    <row r="113" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B113" s="107"/>
+      <c r="C113" s="118"/>
       <c r="D113" s="4" t="s">
         <v>163</v>
       </c>
@@ -7430,9 +7472,9 @@
       <c r="V113" s="91"/>
       <c r="W113" s="92"/>
     </row>
-    <row r="114" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B114" s="111"/>
-      <c r="C114" s="106"/>
+    <row r="114" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B114" s="107"/>
+      <c r="C114" s="118"/>
       <c r="D114" s="4" t="s">
         <v>134</v>
       </c>
@@ -7481,9 +7523,9 @@
       <c r="V114" s="15"/>
       <c r="W114" s="16"/>
     </row>
-    <row r="115" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B115" s="111"/>
-      <c r="C115" s="106" t="s">
+    <row r="115" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B115" s="107"/>
+      <c r="C115" s="118" t="s">
         <v>122</v>
       </c>
       <c r="D115" s="4" t="s">
@@ -7532,9 +7574,9 @@
       <c r="V115" s="15"/>
       <c r="W115" s="16"/>
     </row>
-    <row r="116" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B116" s="111"/>
-      <c r="C116" s="106"/>
+    <row r="116" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B116" s="107"/>
+      <c r="C116" s="118"/>
       <c r="D116" s="4" t="s">
         <v>132</v>
       </c>
@@ -7581,9 +7623,9 @@
       <c r="V116" s="15"/>
       <c r="W116" s="16"/>
     </row>
-    <row r="117" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B117" s="111"/>
-      <c r="C117" s="106"/>
+    <row r="117" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B117" s="107"/>
+      <c r="C117" s="118"/>
       <c r="D117" s="4" t="s">
         <v>161</v>
       </c>
@@ -7630,9 +7672,9 @@
       <c r="V117" s="15"/>
       <c r="W117" s="16"/>
     </row>
-    <row r="118" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B118" s="111"/>
-      <c r="C118" s="106"/>
+    <row r="118" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B118" s="107"/>
+      <c r="C118" s="118"/>
       <c r="D118" s="4" t="s">
         <v>133</v>
       </c>
@@ -7675,9 +7717,9 @@
       <c r="V118" s="84"/>
       <c r="W118" s="85"/>
     </row>
-    <row r="119" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B119" s="111"/>
-      <c r="C119" s="106"/>
+    <row r="119" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B119" s="107"/>
+      <c r="C119" s="118"/>
       <c r="D119" s="4" t="s">
         <v>164</v>
       </c>
@@ -7724,9 +7766,9 @@
       <c r="V119" s="91"/>
       <c r="W119" s="92"/>
     </row>
-    <row r="120" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B120" s="111"/>
-      <c r="C120" s="106"/>
+    <row r="120" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B120" s="107"/>
+      <c r="C120" s="118"/>
       <c r="D120" s="4" t="s">
         <v>163</v>
       </c>
@@ -7773,9 +7815,9 @@
       <c r="V120" s="91"/>
       <c r="W120" s="92"/>
     </row>
-    <row r="121" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B121" s="111"/>
-      <c r="C121" s="106"/>
+    <row r="121" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B121" s="107"/>
+      <c r="C121" s="118"/>
       <c r="D121" s="4" t="s">
         <v>134</v>
       </c>
@@ -7824,9 +7866,9 @@
       <c r="V121" s="15"/>
       <c r="W121" s="16"/>
     </row>
-    <row r="122" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B122" s="111"/>
-      <c r="C122" s="106" t="s">
+    <row r="122" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B122" s="107"/>
+      <c r="C122" s="118" t="s">
         <v>123</v>
       </c>
       <c r="D122" s="4" t="s">
@@ -7875,9 +7917,9 @@
       <c r="V122" s="15"/>
       <c r="W122" s="16"/>
     </row>
-    <row r="123" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B123" s="111"/>
-      <c r="C123" s="106"/>
+    <row r="123" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B123" s="107"/>
+      <c r="C123" s="118"/>
       <c r="D123" s="4" t="s">
         <v>132</v>
       </c>
@@ -7924,9 +7966,9 @@
       <c r="V123" s="15"/>
       <c r="W123" s="16"/>
     </row>
-    <row r="124" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B124" s="111"/>
-      <c r="C124" s="106"/>
+    <row r="124" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B124" s="107"/>
+      <c r="C124" s="118"/>
       <c r="D124" s="4" t="s">
         <v>161</v>
       </c>
@@ -7973,9 +8015,9 @@
       <c r="V124" s="15"/>
       <c r="W124" s="16"/>
     </row>
-    <row r="125" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B125" s="111"/>
-      <c r="C125" s="106"/>
+    <row r="125" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B125" s="107"/>
+      <c r="C125" s="118"/>
       <c r="D125" s="4" t="s">
         <v>133</v>
       </c>
@@ -8018,9 +8060,9 @@
       <c r="V125" s="84"/>
       <c r="W125" s="85"/>
     </row>
-    <row r="126" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B126" s="111"/>
-      <c r="C126" s="106"/>
+    <row r="126" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B126" s="107"/>
+      <c r="C126" s="118"/>
       <c r="D126" s="4" t="s">
         <v>164</v>
       </c>
@@ -8067,9 +8109,9 @@
       <c r="V126" s="91"/>
       <c r="W126" s="92"/>
     </row>
-    <row r="127" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B127" s="111"/>
-      <c r="C127" s="106"/>
+    <row r="127" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B127" s="107"/>
+      <c r="C127" s="118"/>
       <c r="D127" s="4" t="s">
         <v>163</v>
       </c>
@@ -8116,9 +8158,9 @@
       <c r="V127" s="91"/>
       <c r="W127" s="92"/>
     </row>
-    <row r="128" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B128" s="111"/>
-      <c r="C128" s="106"/>
+    <row r="128" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B128" s="107"/>
+      <c r="C128" s="118"/>
       <c r="D128" s="4" t="s">
         <v>134</v>
       </c>
@@ -8167,9 +8209,9 @@
       <c r="V128" s="15"/>
       <c r="W128" s="16"/>
     </row>
-    <row r="129" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B129" s="111"/>
-      <c r="C129" s="106" t="s">
+    <row r="129" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B129" s="107"/>
+      <c r="C129" s="118" t="s">
         <v>124</v>
       </c>
       <c r="D129" s="4" t="s">
@@ -8218,9 +8260,9 @@
       <c r="V129" s="15"/>
       <c r="W129" s="16"/>
     </row>
-    <row r="130" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B130" s="111"/>
-      <c r="C130" s="106"/>
+    <row r="130" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B130" s="107"/>
+      <c r="C130" s="118"/>
       <c r="D130" s="4" t="s">
         <v>132</v>
       </c>
@@ -8267,9 +8309,9 @@
       <c r="V130" s="15"/>
       <c r="W130" s="16"/>
     </row>
-    <row r="131" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B131" s="111"/>
-      <c r="C131" s="106"/>
+    <row r="131" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B131" s="107"/>
+      <c r="C131" s="118"/>
       <c r="D131" s="4" t="s">
         <v>161</v>
       </c>
@@ -8316,9 +8358,9 @@
       <c r="V131" s="15"/>
       <c r="W131" s="16"/>
     </row>
-    <row r="132" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B132" s="111"/>
-      <c r="C132" s="106"/>
+    <row r="132" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B132" s="107"/>
+      <c r="C132" s="118"/>
       <c r="D132" s="4" t="s">
         <v>133</v>
       </c>
@@ -8361,9 +8403,9 @@
       <c r="V132" s="84"/>
       <c r="W132" s="85"/>
     </row>
-    <row r="133" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B133" s="111"/>
-      <c r="C133" s="106"/>
+    <row r="133" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B133" s="107"/>
+      <c r="C133" s="118"/>
       <c r="D133" s="4" t="s">
         <v>164</v>
       </c>
@@ -8410,9 +8452,9 @@
       <c r="V133" s="91"/>
       <c r="W133" s="92"/>
     </row>
-    <row r="134" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B134" s="111"/>
-      <c r="C134" s="106"/>
+    <row r="134" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B134" s="107"/>
+      <c r="C134" s="118"/>
       <c r="D134" s="4" t="s">
         <v>163</v>
       </c>
@@ -8459,9 +8501,9 @@
       <c r="V134" s="91"/>
       <c r="W134" s="92"/>
     </row>
-    <row r="135" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B135" s="111"/>
-      <c r="C135" s="106"/>
+    <row r="135" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B135" s="107"/>
+      <c r="C135" s="118"/>
       <c r="D135" s="4" t="s">
         <v>134</v>
       </c>
@@ -8510,9 +8552,9 @@
       <c r="V135" s="15"/>
       <c r="W135" s="16"/>
     </row>
-    <row r="136" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B136" s="111"/>
-      <c r="C136" s="106" t="s">
+    <row r="136" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B136" s="107"/>
+      <c r="C136" s="118" t="s">
         <v>125</v>
       </c>
       <c r="D136" s="4" t="s">
@@ -8561,9 +8603,9 @@
       <c r="V136" s="15"/>
       <c r="W136" s="16"/>
     </row>
-    <row r="137" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B137" s="111"/>
-      <c r="C137" s="106"/>
+    <row r="137" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B137" s="107"/>
+      <c r="C137" s="118"/>
       <c r="D137" s="4" t="s">
         <v>132</v>
       </c>
@@ -8610,9 +8652,9 @@
       <c r="V137" s="15"/>
       <c r="W137" s="16"/>
     </row>
-    <row r="138" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B138" s="111"/>
-      <c r="C138" s="106"/>
+    <row r="138" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B138" s="107"/>
+      <c r="C138" s="118"/>
       <c r="D138" s="4" t="s">
         <v>161</v>
       </c>
@@ -8659,9 +8701,9 @@
       <c r="V138" s="15"/>
       <c r="W138" s="16"/>
     </row>
-    <row r="139" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B139" s="111"/>
-      <c r="C139" s="106"/>
+    <row r="139" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B139" s="107"/>
+      <c r="C139" s="118"/>
       <c r="D139" s="4" t="s">
         <v>133</v>
       </c>
@@ -8704,9 +8746,9 @@
       <c r="V139" s="84"/>
       <c r="W139" s="85"/>
     </row>
-    <row r="140" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B140" s="111"/>
-      <c r="C140" s="106"/>
+    <row r="140" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B140" s="107"/>
+      <c r="C140" s="118"/>
       <c r="D140" s="4" t="s">
         <v>164</v>
       </c>
@@ -8753,9 +8795,9 @@
       <c r="V140" s="91"/>
       <c r="W140" s="92"/>
     </row>
-    <row r="141" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B141" s="111"/>
-      <c r="C141" s="106"/>
+    <row r="141" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B141" s="107"/>
+      <c r="C141" s="118"/>
       <c r="D141" s="4" t="s">
         <v>163</v>
       </c>
@@ -8802,9 +8844,9 @@
       <c r="V141" s="91"/>
       <c r="W141" s="92"/>
     </row>
-    <row r="142" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B142" s="111"/>
-      <c r="C142" s="106"/>
+    <row r="142" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B142" s="107"/>
+      <c r="C142" s="118"/>
       <c r="D142" s="4" t="s">
         <v>134</v>
       </c>
@@ -8853,9 +8895,9 @@
       <c r="V142" s="15"/>
       <c r="W142" s="16"/>
     </row>
-    <row r="143" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B143" s="111"/>
-      <c r="C143" s="106" t="s">
+    <row r="143" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B143" s="107"/>
+      <c r="C143" s="118" t="s">
         <v>126</v>
       </c>
       <c r="D143" s="4" t="s">
@@ -8904,9 +8946,9 @@
       <c r="V143" s="15"/>
       <c r="W143" s="16"/>
     </row>
-    <row r="144" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B144" s="111"/>
-      <c r="C144" s="106"/>
+    <row r="144" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B144" s="107"/>
+      <c r="C144" s="118"/>
       <c r="D144" s="4" t="s">
         <v>132</v>
       </c>
@@ -8953,9 +8995,9 @@
       <c r="V144" s="15"/>
       <c r="W144" s="16"/>
     </row>
-    <row r="145" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B145" s="111"/>
-      <c r="C145" s="106"/>
+    <row r="145" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B145" s="107"/>
+      <c r="C145" s="118"/>
       <c r="D145" s="4" t="s">
         <v>161</v>
       </c>
@@ -9002,9 +9044,9 @@
       <c r="V145" s="15"/>
       <c r="W145" s="16"/>
     </row>
-    <row r="146" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B146" s="111"/>
-      <c r="C146" s="106"/>
+    <row r="146" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B146" s="107"/>
+      <c r="C146" s="118"/>
       <c r="D146" s="4" t="s">
         <v>133</v>
       </c>
@@ -9047,9 +9089,9 @@
       <c r="V146" s="84"/>
       <c r="W146" s="85"/>
     </row>
-    <row r="147" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B147" s="111"/>
-      <c r="C147" s="106"/>
+    <row r="147" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B147" s="107"/>
+      <c r="C147" s="118"/>
       <c r="D147" s="4" t="s">
         <v>164</v>
       </c>
@@ -9096,9 +9138,9 @@
       <c r="V147" s="91"/>
       <c r="W147" s="92"/>
     </row>
-    <row r="148" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="111"/>
-      <c r="C148" s="106"/>
+    <row r="148" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B148" s="107"/>
+      <c r="C148" s="118"/>
       <c r="D148" s="4" t="s">
         <v>163</v>
       </c>
@@ -9145,9 +9187,9 @@
       <c r="V148" s="91"/>
       <c r="W148" s="92"/>
     </row>
-    <row r="149" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B149" s="111"/>
-      <c r="C149" s="106"/>
+    <row r="149" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B149" s="107"/>
+      <c r="C149" s="118"/>
       <c r="D149" s="4" t="s">
         <v>134</v>
       </c>
@@ -9196,9 +9238,9 @@
       <c r="V149" s="15"/>
       <c r="W149" s="16"/>
     </row>
-    <row r="150" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B150" s="111"/>
-      <c r="C150" s="106" t="s">
+    <row r="150" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B150" s="107"/>
+      <c r="C150" s="118" t="s">
         <v>127</v>
       </c>
       <c r="D150" s="4" t="s">
@@ -9247,9 +9289,9 @@
       <c r="V150" s="15"/>
       <c r="W150" s="16"/>
     </row>
-    <row r="151" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B151" s="111"/>
-      <c r="C151" s="106"/>
+    <row r="151" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B151" s="107"/>
+      <c r="C151" s="118"/>
       <c r="D151" s="4" t="s">
         <v>132</v>
       </c>
@@ -9296,9 +9338,9 @@
       <c r="V151" s="15"/>
       <c r="W151" s="16"/>
     </row>
-    <row r="152" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B152" s="111"/>
-      <c r="C152" s="106"/>
+    <row r="152" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B152" s="107"/>
+      <c r="C152" s="118"/>
       <c r="D152" s="4" t="s">
         <v>161</v>
       </c>
@@ -9345,9 +9387,9 @@
       <c r="V152" s="15"/>
       <c r="W152" s="16"/>
     </row>
-    <row r="153" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B153" s="111"/>
-      <c r="C153" s="106"/>
+    <row r="153" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B153" s="107"/>
+      <c r="C153" s="118"/>
       <c r="D153" s="4" t="s">
         <v>133</v>
       </c>
@@ -9390,9 +9432,9 @@
       <c r="V153" s="84"/>
       <c r="W153" s="85"/>
     </row>
-    <row r="154" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B154" s="111"/>
-      <c r="C154" s="106"/>
+    <row r="154" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B154" s="107"/>
+      <c r="C154" s="118"/>
       <c r="D154" s="4" t="s">
         <v>164</v>
       </c>
@@ -9439,9 +9481,9 @@
       <c r="V154" s="91"/>
       <c r="W154" s="92"/>
     </row>
-    <row r="155" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B155" s="111"/>
-      <c r="C155" s="106"/>
+    <row r="155" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B155" s="107"/>
+      <c r="C155" s="118"/>
       <c r="D155" s="4" t="s">
         <v>163</v>
       </c>
@@ -9488,9 +9530,9 @@
       <c r="V155" s="91"/>
       <c r="W155" s="92"/>
     </row>
-    <row r="156" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B156" s="111"/>
-      <c r="C156" s="106"/>
+    <row r="156" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B156" s="107"/>
+      <c r="C156" s="118"/>
       <c r="D156" s="4" t="s">
         <v>134</v>
       </c>
@@ -9539,9 +9581,9 @@
       <c r="V156" s="15"/>
       <c r="W156" s="16"/>
     </row>
-    <row r="157" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B157" s="111"/>
-      <c r="C157" s="106" t="s">
+    <row r="157" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B157" s="107"/>
+      <c r="C157" s="118" t="s">
         <v>128</v>
       </c>
       <c r="D157" s="4" t="s">
@@ -9590,9 +9632,9 @@
       <c r="V157" s="15"/>
       <c r="W157" s="16"/>
     </row>
-    <row r="158" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B158" s="111"/>
-      <c r="C158" s="106"/>
+    <row r="158" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B158" s="107"/>
+      <c r="C158" s="118"/>
       <c r="D158" s="4" t="s">
         <v>132</v>
       </c>
@@ -9639,9 +9681,9 @@
       <c r="V158" s="15"/>
       <c r="W158" s="16"/>
     </row>
-    <row r="159" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B159" s="111"/>
-      <c r="C159" s="106"/>
+    <row r="159" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B159" s="107"/>
+      <c r="C159" s="118"/>
       <c r="D159" s="4" t="s">
         <v>161</v>
       </c>
@@ -9688,9 +9730,9 @@
       <c r="V159" s="15"/>
       <c r="W159" s="16"/>
     </row>
-    <row r="160" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B160" s="111"/>
-      <c r="C160" s="106"/>
+    <row r="160" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B160" s="107"/>
+      <c r="C160" s="118"/>
       <c r="D160" s="4" t="s">
         <v>133</v>
       </c>
@@ -9733,9 +9775,9 @@
       <c r="V160" s="84"/>
       <c r="W160" s="85"/>
     </row>
-    <row r="161" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B161" s="111"/>
-      <c r="C161" s="106"/>
+    <row r="161" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B161" s="107"/>
+      <c r="C161" s="118"/>
       <c r="D161" s="4" t="s">
         <v>164</v>
       </c>
@@ -9782,9 +9824,9 @@
       <c r="V161" s="91"/>
       <c r="W161" s="92"/>
     </row>
-    <row r="162" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B162" s="111"/>
-      <c r="C162" s="106"/>
+    <row r="162" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B162" s="107"/>
+      <c r="C162" s="118"/>
       <c r="D162" s="4" t="s">
         <v>163</v>
       </c>
@@ -9831,9 +9873,9 @@
       <c r="V162" s="91"/>
       <c r="W162" s="92"/>
     </row>
-    <row r="163" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B163" s="111"/>
-      <c r="C163" s="106"/>
+    <row r="163" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B163" s="107"/>
+      <c r="C163" s="118"/>
       <c r="D163" s="4" t="s">
         <v>134</v>
       </c>
@@ -9882,9 +9924,9 @@
       <c r="V163" s="15"/>
       <c r="W163" s="16"/>
     </row>
-    <row r="164" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B164" s="111"/>
-      <c r="C164" s="106" t="s">
+    <row r="164" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B164" s="107"/>
+      <c r="C164" s="118" t="s">
         <v>129</v>
       </c>
       <c r="D164" s="4" t="s">
@@ -9933,9 +9975,9 @@
       <c r="V164" s="15"/>
       <c r="W164" s="16"/>
     </row>
-    <row r="165" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B165" s="111"/>
-      <c r="C165" s="106"/>
+    <row r="165" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B165" s="107"/>
+      <c r="C165" s="118"/>
       <c r="D165" s="4" t="s">
         <v>132</v>
       </c>
@@ -9982,9 +10024,9 @@
       <c r="V165" s="15"/>
       <c r="W165" s="16"/>
     </row>
-    <row r="166" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B166" s="111"/>
-      <c r="C166" s="106"/>
+    <row r="166" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B166" s="107"/>
+      <c r="C166" s="118"/>
       <c r="D166" s="4" t="s">
         <v>161</v>
       </c>
@@ -10031,9 +10073,9 @@
       <c r="V166" s="15"/>
       <c r="W166" s="16"/>
     </row>
-    <row r="167" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B167" s="111"/>
-      <c r="C167" s="106"/>
+    <row r="167" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B167" s="107"/>
+      <c r="C167" s="118"/>
       <c r="D167" s="4" t="s">
         <v>133</v>
       </c>
@@ -10076,9 +10118,9 @@
       <c r="V167" s="84"/>
       <c r="W167" s="85"/>
     </row>
-    <row r="168" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B168" s="111"/>
-      <c r="C168" s="106"/>
+    <row r="168" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B168" s="107"/>
+      <c r="C168" s="118"/>
       <c r="D168" s="4" t="s">
         <v>164</v>
       </c>
@@ -10125,9 +10167,9 @@
       <c r="V168" s="91"/>
       <c r="W168" s="92"/>
     </row>
-    <row r="169" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B169" s="111"/>
-      <c r="C169" s="106"/>
+    <row r="169" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B169" s="107"/>
+      <c r="C169" s="118"/>
       <c r="D169" s="4" t="s">
         <v>163</v>
       </c>
@@ -10174,9 +10216,9 @@
       <c r="V169" s="91"/>
       <c r="W169" s="92"/>
     </row>
-    <row r="170" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B170" s="111"/>
-      <c r="C170" s="106"/>
+    <row r="170" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B170" s="107"/>
+      <c r="C170" s="118"/>
       <c r="D170" s="4" t="s">
         <v>134</v>
       </c>
@@ -10225,9 +10267,9 @@
       <c r="V170" s="15"/>
       <c r="W170" s="16"/>
     </row>
-    <row r="171" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B171" s="111"/>
-      <c r="C171" s="106" t="s">
+    <row r="171" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B171" s="107"/>
+      <c r="C171" s="118" t="s">
         <v>130</v>
       </c>
       <c r="D171" s="4" t="s">
@@ -10276,9 +10318,9 @@
       <c r="V171" s="15"/>
       <c r="W171" s="16"/>
     </row>
-    <row r="172" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B172" s="111"/>
-      <c r="C172" s="106"/>
+    <row r="172" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B172" s="107"/>
+      <c r="C172" s="118"/>
       <c r="D172" s="4" t="s">
         <v>132</v>
       </c>
@@ -10325,9 +10367,9 @@
       <c r="V172" s="15"/>
       <c r="W172" s="16"/>
     </row>
-    <row r="173" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B173" s="111"/>
-      <c r="C173" s="106"/>
+    <row r="173" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B173" s="107"/>
+      <c r="C173" s="118"/>
       <c r="D173" s="4" t="s">
         <v>161</v>
       </c>
@@ -10374,9 +10416,9 @@
       <c r="V173" s="15"/>
       <c r="W173" s="16"/>
     </row>
-    <row r="174" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B174" s="111"/>
-      <c r="C174" s="106"/>
+    <row r="174" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B174" s="107"/>
+      <c r="C174" s="118"/>
       <c r="D174" s="4" t="s">
         <v>133</v>
       </c>
@@ -10419,9 +10461,9 @@
       <c r="V174" s="84"/>
       <c r="W174" s="85"/>
     </row>
-    <row r="175" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B175" s="129"/>
-      <c r="C175" s="133"/>
+    <row r="175" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B175" s="114"/>
+      <c r="C175" s="121"/>
       <c r="D175" s="4" t="s">
         <v>164</v>
       </c>
@@ -10468,9 +10510,9 @@
       <c r="V175" s="89"/>
       <c r="W175" s="90"/>
     </row>
-    <row r="176" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B176" s="129"/>
-      <c r="C176" s="133"/>
+    <row r="176" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B176" s="114"/>
+      <c r="C176" s="121"/>
       <c r="D176" s="4" t="s">
         <v>163</v>
       </c>
@@ -10517,9 +10559,9 @@
       <c r="V176" s="89"/>
       <c r="W176" s="90"/>
     </row>
-    <row r="177" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B177" s="112"/>
-      <c r="C177" s="134"/>
+    <row r="177" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B177" s="108"/>
+      <c r="C177" s="122"/>
       <c r="D177" s="20" t="s">
         <v>134</v>
       </c>
@@ -10568,8 +10610,8 @@
       <c r="V177" s="18"/>
       <c r="W177" s="21"/>
     </row>
-    <row r="178" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B178" s="110" t="s">
+    <row r="178" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B178" s="106" t="s">
         <v>83</v>
       </c>
       <c r="C178" s="71" t="s">
@@ -10619,8 +10661,8 @@
       <c r="V178" s="44"/>
       <c r="W178" s="45"/>
     </row>
-    <row r="179" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B179" s="111"/>
+    <row r="179" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B179" s="107"/>
       <c r="C179" s="28" t="s">
         <v>89</v>
       </c>
@@ -10668,8 +10710,8 @@
       <c r="V179" s="15"/>
       <c r="W179" s="16"/>
     </row>
-    <row r="180" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B180" s="111"/>
+    <row r="180" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B180" s="107"/>
       <c r="C180" s="28" t="s">
         <v>90</v>
       </c>
@@ -10717,8 +10759,8 @@
       <c r="V180" s="15"/>
       <c r="W180" s="16"/>
     </row>
-    <row r="181" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B181" s="111"/>
+    <row r="181" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B181" s="107"/>
       <c r="C181" s="28" t="s">
         <v>91</v>
       </c>
@@ -10766,8 +10808,8 @@
       <c r="V181" s="15"/>
       <c r="W181" s="16"/>
     </row>
-    <row r="182" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B182" s="111"/>
+    <row r="182" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B182" s="107"/>
       <c r="C182" s="28" t="s">
         <v>141</v>
       </c>
@@ -10815,8 +10857,8 @@
       <c r="V182" s="15"/>
       <c r="W182" s="16"/>
     </row>
-    <row r="183" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B183" s="111"/>
+    <row r="183" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B183" s="107"/>
       <c r="C183" s="28" t="s">
         <v>138</v>
       </c>
@@ -10864,8 +10906,8 @@
       <c r="V183" s="15"/>
       <c r="W183" s="16"/>
     </row>
-    <row r="184" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B184" s="111"/>
+    <row r="184" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B184" s="107"/>
       <c r="C184" s="28" t="s">
         <v>140</v>
       </c>
@@ -10913,8 +10955,8 @@
       <c r="V184" s="15"/>
       <c r="W184" s="16"/>
     </row>
-    <row r="185" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B185" s="111"/>
+    <row r="185" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B185" s="107"/>
       <c r="C185" s="28" t="s">
         <v>139</v>
       </c>
@@ -10962,8 +11004,8 @@
       <c r="V185" s="15"/>
       <c r="W185" s="16"/>
     </row>
-    <row r="186" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B186" s="111"/>
+    <row r="186" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B186" s="107"/>
       <c r="C186" s="28" t="s">
         <v>92</v>
       </c>
@@ -11027,8 +11069,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B187" s="111"/>
+    <row r="187" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B187" s="107"/>
       <c r="C187" s="28" t="s">
         <v>93</v>
       </c>
@@ -11092,8 +11134,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B188" s="111"/>
+    <row r="188" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B188" s="107"/>
       <c r="C188" s="28" t="s">
         <v>94</v>
       </c>
@@ -11157,8 +11199,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B189" s="111"/>
+    <row r="189" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B189" s="107"/>
       <c r="C189" s="28" t="s">
         <v>98</v>
       </c>
@@ -11206,8 +11248,8 @@
       <c r="V189" s="15"/>
       <c r="W189" s="16"/>
     </row>
-    <row r="190" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B190" s="112"/>
+    <row r="190" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B190" s="108"/>
       <c r="C190" s="54" t="s">
         <v>99</v>
       </c>
@@ -11255,8 +11297,8 @@
       <c r="V190" s="18"/>
       <c r="W190" s="21"/>
     </row>
-    <row r="191" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B191" s="110" t="s">
+    <row r="191" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B191" s="106" t="s">
         <v>142</v>
       </c>
       <c r="C191" s="53" t="s">
@@ -11306,8 +11348,8 @@
       <c r="V191" s="44"/>
       <c r="W191" s="45"/>
     </row>
-    <row r="192" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B192" s="111"/>
+    <row r="192" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B192" s="107"/>
       <c r="C192" s="52" t="s">
         <v>143</v>
       </c>
@@ -11355,8 +11397,8 @@
       <c r="V192" s="15"/>
       <c r="W192" s="16"/>
     </row>
-    <row r="193" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B193" s="112"/>
+    <row r="193" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B193" s="108"/>
       <c r="C193" s="54" t="s">
         <v>144</v>
       </c>
@@ -11404,8 +11446,8 @@
       <c r="V193" s="18"/>
       <c r="W193" s="21"/>
     </row>
-    <row r="194" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B194" s="110" t="s">
+    <row r="194" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B194" s="106" t="s">
         <v>147</v>
       </c>
       <c r="C194" s="53" t="s">
@@ -11455,8 +11497,8 @@
       <c r="V194" s="44"/>
       <c r="W194" s="45"/>
     </row>
-    <row r="195" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B195" s="111"/>
+    <row r="195" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B195" s="107"/>
       <c r="C195" s="52" t="s">
         <v>149</v>
       </c>
@@ -11504,8 +11546,8 @@
       <c r="V195" s="15"/>
       <c r="W195" s="16"/>
     </row>
-    <row r="196" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B196" s="111"/>
+    <row r="196" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B196" s="107"/>
       <c r="C196" s="52" t="s">
         <v>150</v>
       </c>
@@ -11553,8 +11595,8 @@
       <c r="V196" s="15"/>
       <c r="W196" s="16"/>
     </row>
-    <row r="197" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B197" s="111"/>
+    <row r="197" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B197" s="107"/>
       <c r="C197" s="52" t="s">
         <v>151</v>
       </c>
@@ -11602,8 +11644,8 @@
       <c r="V197" s="15"/>
       <c r="W197" s="16"/>
     </row>
-    <row r="198" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B198" s="111"/>
+    <row r="198" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B198" s="107"/>
       <c r="C198" s="52" t="s">
         <v>152</v>
       </c>
@@ -11651,8 +11693,8 @@
       <c r="V198" s="15"/>
       <c r="W198" s="16"/>
     </row>
-    <row r="199" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B199" s="111"/>
+    <row r="199" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B199" s="107"/>
       <c r="C199" s="52" t="s">
         <v>153</v>
       </c>
@@ -11700,8 +11742,8 @@
       <c r="V199" s="15"/>
       <c r="W199" s="16"/>
     </row>
-    <row r="200" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B200" s="112"/>
+    <row r="200" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B200" s="108"/>
       <c r="C200" s="54" t="s">
         <v>154</v>
       </c>
@@ -11749,8 +11791,8 @@
       <c r="V200" s="18"/>
       <c r="W200" s="21"/>
     </row>
-    <row r="201" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B201" s="110" t="s">
+    <row r="201" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B201" s="106" t="s">
         <v>18</v>
       </c>
       <c r="C201" s="47" t="s">
@@ -11800,8 +11842,8 @@
       <c r="V201" s="44"/>
       <c r="W201" s="45"/>
     </row>
-    <row r="202" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B202" s="111"/>
+    <row r="202" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B202" s="107"/>
       <c r="C202" s="28" t="s">
         <v>136</v>
       </c>
@@ -11849,8 +11891,8 @@
       <c r="V202" s="15"/>
       <c r="W202" s="16"/>
     </row>
-    <row r="203" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B203" s="111"/>
+    <row r="203" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B203" s="107"/>
       <c r="C203" s="28" t="s">
         <v>137</v>
       </c>
@@ -11898,8 +11940,8 @@
       <c r="V203" s="15"/>
       <c r="W203" s="16"/>
     </row>
-    <row r="204" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B204" s="111"/>
+    <row r="204" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B204" s="107"/>
       <c r="C204" s="28" t="s">
         <v>145</v>
       </c>
@@ -11947,8 +11989,8 @@
       <c r="V204" s="15"/>
       <c r="W204" s="16"/>
     </row>
-    <row r="205" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B205" s="111"/>
+    <row r="205" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B205" s="107"/>
       <c r="C205" s="28" t="s">
         <v>84</v>
       </c>
@@ -11996,8 +12038,8 @@
       <c r="V205" s="15"/>
       <c r="W205" s="16"/>
     </row>
-    <row r="206" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B206" s="111"/>
+    <row r="206" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B206" s="107"/>
       <c r="C206" s="28" t="s">
         <v>85</v>
       </c>
@@ -12045,8 +12087,8 @@
       <c r="V206" s="15"/>
       <c r="W206" s="16"/>
     </row>
-    <row r="207" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B207" s="111"/>
+    <row r="207" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B207" s="107"/>
       <c r="C207" s="28" t="s">
         <v>87</v>
       </c>
@@ -12094,8 +12136,8 @@
       <c r="V207" s="15"/>
       <c r="W207" s="16"/>
     </row>
-    <row r="208" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B208" s="111"/>
+    <row r="208" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B208" s="107"/>
       <c r="C208" s="28" t="s">
         <v>86</v>
       </c>
@@ -12143,8 +12185,8 @@
       <c r="V208" s="15"/>
       <c r="W208" s="16"/>
     </row>
-    <row r="209" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B209" s="111"/>
+    <row r="209" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B209" s="107"/>
       <c r="C209" s="28" t="s">
         <v>103</v>
       </c>
@@ -12192,8 +12234,8 @@
       <c r="V209" s="15"/>
       <c r="W209" s="16"/>
     </row>
-    <row r="210" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B210" s="111"/>
+    <row r="210" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B210" s="107"/>
       <c r="C210" s="28" t="s">
         <v>135</v>
       </c>
@@ -12241,8 +12283,8 @@
       <c r="V210" s="15"/>
       <c r="W210" s="16"/>
     </row>
-    <row r="211" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B211" s="111"/>
+    <row r="211" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B211" s="107"/>
       <c r="C211" s="28" t="s">
         <v>104</v>
       </c>
@@ -12281,7 +12323,9 @@
       <c r="O211" s="63">
         <v>0</v>
       </c>
-      <c r="P211" s="94"/>
+      <c r="P211" s="135" t="s">
+        <v>165</v>
+      </c>
       <c r="Q211" s="15"/>
       <c r="R211" s="15"/>
       <c r="S211" s="15"/>
@@ -12290,22 +12334,22 @@
       <c r="V211" s="15"/>
       <c r="W211" s="16"/>
     </row>
-    <row r="212" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B212" s="130" t="s">
+    <row r="212" spans="2:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B212" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="C212" s="131"/>
-      <c r="D212" s="131"/>
-      <c r="E212" s="131"/>
-      <c r="F212" s="131"/>
-      <c r="G212" s="132"/>
+      <c r="C212" s="116"/>
+      <c r="D212" s="116"/>
+      <c r="E212" s="116"/>
+      <c r="F212" s="116"/>
+      <c r="G212" s="117"/>
       <c r="H212" s="31">
         <f t="shared" ref="H212:W212" si="5">SUM(H4:H211)</f>
         <v>114.84999999999995</v>
       </c>
       <c r="I212" s="19">
         <f t="shared" si="5"/>
-        <v>20.200300000000009</v>
+        <v>25.700300000000013</v>
       </c>
       <c r="J212" s="19">
         <f t="shared" si="5"/>
@@ -12329,11 +12373,11 @@
       </c>
       <c r="O212" s="19">
         <f t="shared" si="5"/>
-        <v>1.5170000000000001</v>
+        <v>2.5169999999999999</v>
       </c>
       <c r="P212" s="19">
         <f t="shared" si="5"/>
-        <v>4.0429999999999993</v>
+        <v>8.5430000000000028</v>
       </c>
       <c r="Q212" s="19">
         <f t="shared" si="5"/>
@@ -12364,7 +12408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
@@ -12373,24 +12417,24 @@
       <c r="G213" s="2"/>
       <c r="H213" s="2"/>
       <c r="I213" s="2"/>
-      <c r="J213" s="107" t="s">
+      <c r="J213" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="K213" s="108"/>
-      <c r="L213" s="108"/>
-      <c r="M213" s="108"/>
-      <c r="N213" s="108"/>
-      <c r="O213" s="108"/>
-      <c r="P213" s="108"/>
-      <c r="Q213" s="108"/>
-      <c r="R213" s="108"/>
-      <c r="S213" s="108"/>
-      <c r="T213" s="108"/>
-      <c r="U213" s="108"/>
-      <c r="V213" s="108"/>
-      <c r="W213" s="109"/>
-    </row>
-    <row r="214" spans="2:23" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K213" s="119"/>
+      <c r="L213" s="119"/>
+      <c r="M213" s="119"/>
+      <c r="N213" s="119"/>
+      <c r="O213" s="119"/>
+      <c r="P213" s="119"/>
+      <c r="Q213" s="119"/>
+      <c r="R213" s="119"/>
+      <c r="S213" s="119"/>
+      <c r="T213" s="119"/>
+      <c r="U213" s="119"/>
+      <c r="V213" s="119"/>
+      <c r="W213" s="120"/>
+    </row>
+    <row r="214" spans="2:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C214" s="52" t="s">
         <v>159</v>
       </c>
@@ -12410,7 +12454,7 @@
       <c r="M214" s="3"/>
       <c r="N214" s="3"/>
     </row>
-    <row r="215" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B215" s="81" t="s">
         <v>155</v>
       </c>
@@ -12428,10 +12472,10 @@
       </c>
       <c r="F215" s="2"/>
       <c r="G215" s="2"/>
-      <c r="H215" s="125" t="s">
+      <c r="H215" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="I215" s="126"/>
+      <c r="I215" s="110"/>
       <c r="J215" s="9">
         <f>H212-J212</f>
         <v>114.84999999999995</v>
@@ -12454,42 +12498,42 @@
       </c>
       <c r="O215" s="86">
         <f t="shared" ref="O215:W215" si="6">N215-O212</f>
-        <v>98.692699999999974</v>
+        <v>97.692699999999974</v>
       </c>
       <c r="P215" s="86">
         <f t="shared" si="6"/>
-        <v>94.649699999999967</v>
+        <v>89.149699999999967</v>
       </c>
       <c r="Q215" s="86">
         <f t="shared" si="6"/>
-        <v>94.649699999999967</v>
+        <v>89.149699999999967</v>
       </c>
       <c r="R215" s="86">
         <f t="shared" si="6"/>
-        <v>94.649699999999967</v>
+        <v>89.149699999999967</v>
       </c>
       <c r="S215" s="86">
         <f t="shared" si="6"/>
-        <v>94.649699999999967</v>
+        <v>89.149699999999967</v>
       </c>
       <c r="T215" s="86">
         <f t="shared" si="6"/>
-        <v>94.649699999999967</v>
+        <v>89.149699999999967</v>
       </c>
       <c r="U215" s="86">
         <f t="shared" si="6"/>
-        <v>94.649699999999967</v>
+        <v>89.149699999999967</v>
       </c>
       <c r="V215" s="86">
         <f t="shared" si="6"/>
-        <v>94.649699999999967</v>
+        <v>89.149699999999967</v>
       </c>
       <c r="W215" s="86">
         <f t="shared" si="6"/>
-        <v>94.649699999999967</v>
-      </c>
-    </row>
-    <row r="216" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>89.149699999999967</v>
+      </c>
+    </row>
+    <row r="216" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B216" s="82" t="s">
         <v>156</v>
       </c>
@@ -12515,7 +12559,7 @@
       <c r="M216" s="3"/>
       <c r="N216" s="3"/>
     </row>
-    <row r="217" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B217" s="82" t="s">
         <v>157</v>
       </c>
@@ -12525,27 +12569,27 @@
       </c>
       <c r="D217" s="5">
         <f>SUM(I211,I208:I209,I201:I205,I179:I185,I63:I72,I4:I8)</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="E217" s="5">
         <f>SUM(C217,-D217)</f>
-        <v>24.4</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="F217" s="3"/>
-      <c r="H217" s="107" t="s">
+      <c r="H217" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="I217" s="127"/>
-      <c r="J217" s="126">
+      <c r="I217" s="112"/>
+      <c r="J217" s="110">
         <f>H212-I212</f>
-        <v>94.649699999999939</v>
-      </c>
-      <c r="K217" s="126"/>
-      <c r="L217" s="126"/>
-      <c r="M217" s="126"/>
-      <c r="N217" s="128"/>
-    </row>
-    <row r="218" spans="2:23" x14ac:dyDescent="0.3">
+        <v>89.149699999999939</v>
+      </c>
+      <c r="K217" s="110"/>
+      <c r="L217" s="110"/>
+      <c r="M217" s="110"/>
+      <c r="N217" s="113"/>
+    </row>
+    <row r="218" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B218" s="3"/>
       <c r="C218" s="3"/>
       <c r="D218" s="3"/>
@@ -12560,7 +12604,7 @@
       <c r="M218" s="3"/>
       <c r="N218" s="3"/>
     </row>
-    <row r="219" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B219" s="3"/>
       <c r="C219" s="3"/>
       <c r="D219" s="3"/>
@@ -12575,7 +12619,7 @@
       <c r="M219" s="3"/>
       <c r="N219" s="3"/>
     </row>
-    <row r="220" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B220" s="3"/>
       <c r="C220" s="3"/>
       <c r="D220" s="3"/>
@@ -12590,63 +12634,81 @@
       <c r="M220" s="3"/>
       <c r="N220" s="3"/>
     </row>
-    <row r="221" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="222" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="223" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B223" s="12"/>
       <c r="C223" s="12"/>
     </row>
-    <row r="224" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B224" s="12"/>
       <c r="C224" s="12"/>
     </row>
-    <row r="225" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B225" s="12"/>
       <c r="C225" s="12"/>
     </row>
-    <row r="226" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B226" s="12"/>
       <c r="C226" s="12"/>
     </row>
-    <row r="227" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B227" s="12"/>
       <c r="C227" s="12"/>
     </row>
-    <row r="228" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B228" s="12"/>
       <c r="C228" s="12"/>
     </row>
-    <row r="229" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B229" s="12"/>
       <c r="C229" s="12"/>
     </row>
-    <row r="230" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B230" s="12"/>
       <c r="C230" s="12"/>
     </row>
-    <row r="231" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B231" s="12"/>
       <c r="C231" s="12"/>
     </row>
-    <row r="232" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B232" s="12"/>
       <c r="C232" s="12"/>
     </row>
-    <row r="233" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B233" s="12"/>
       <c r="C233" s="12"/>
     </row>
-    <row r="234" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B234" s="12"/>
       <c r="C234" s="12"/>
     </row>
-    <row r="235" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B235" s="12"/>
       <c r="C235" s="12"/>
     </row>
-    <row r="236" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="236" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C157:C163"/>
+    <mergeCell ref="C143:C149"/>
+    <mergeCell ref="C129:C135"/>
+    <mergeCell ref="C122:C128"/>
+    <mergeCell ref="C108:C114"/>
+    <mergeCell ref="C136:C142"/>
+    <mergeCell ref="C150:C156"/>
+    <mergeCell ref="C87:C93"/>
+    <mergeCell ref="J2:W2"/>
+    <mergeCell ref="B63:B72"/>
+    <mergeCell ref="C56:C62"/>
+    <mergeCell ref="C15:C55"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C69:C72"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C73:C79"/>
+    <mergeCell ref="C80:C86"/>
     <mergeCell ref="B194:B200"/>
     <mergeCell ref="H215:I215"/>
     <mergeCell ref="H217:I217"/>
@@ -12663,24 +12725,6 @@
     <mergeCell ref="C171:C177"/>
     <mergeCell ref="C101:C107"/>
     <mergeCell ref="C94:C100"/>
-    <mergeCell ref="C87:C93"/>
-    <mergeCell ref="J2:W2"/>
-    <mergeCell ref="B63:B72"/>
-    <mergeCell ref="C56:C62"/>
-    <mergeCell ref="C15:C55"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="C69:C72"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="C73:C79"/>
-    <mergeCell ref="C80:C86"/>
-    <mergeCell ref="C157:C163"/>
-    <mergeCell ref="C143:C149"/>
-    <mergeCell ref="C129:C135"/>
-    <mergeCell ref="C122:C128"/>
-    <mergeCell ref="C108:C114"/>
-    <mergeCell ref="C136:C142"/>
-    <mergeCell ref="C150:C156"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12694,7 +12738,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12706,7 +12750,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado el excel, acabado de implementar el sistema de spawn/despawn de enemigos, establecida zona 31 (Derecha del principio)
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
+++ b/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Enti\MAP\The_Legend_of_Radev\MAP_LegendOfRadev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devildrake\Documents\MAP_LegendOfRadev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -530,7 +530,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1090,7 +1090,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1350,10 +1350,43 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1362,13 +1395,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1407,34 +1437,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1455,7 +1458,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1512,7 +1515,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A091-4901-839C-4EC24FB5B5C8}"/>
             </c:ext>
@@ -1527,11 +1530,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-971319520"/>
-        <c:axId val="-971325504"/>
+        <c:axId val="-215243664"/>
+        <c:axId val="-215242576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-971319520"/>
+        <c:axId val="-215243664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1540,7 +1543,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-971325504"/>
+        <c:crossAx val="-215242576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1548,7 +1551,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-971325504"/>
+        <c:axId val="-215242576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1562,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-971319520"/>
+        <c:crossAx val="-215243664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1601,7 +1604,7 @@
         <xdr:cNvPr id="4" name="3 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1911,52 +1914,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C190" sqref="C190:I190"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C223" sqref="C223"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" customWidth="1"/>
     <col min="3" max="3" width="80" customWidth="1"/>
-    <col min="4" max="4" width="57.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="57.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" customWidth="1"/>
+    <col min="16" max="16" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="90" t="s">
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J2" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="91"/>
-      <c r="S2" s="91"/>
-      <c r="T2" s="91"/>
-      <c r="U2" s="91"/>
-      <c r="V2" s="91"/>
-      <c r="W2" s="92"/>
-    </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="102"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="102"/>
+      <c r="T2" s="102"/>
+      <c r="U2" s="102"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="103"/>
+    </row>
+    <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="38" t="s">
         <v>7</v>
       </c>
@@ -2024,8 +2027,8 @@
         <v>43067</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="104" t="s">
+    <row r="4" spans="1:23" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="114" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="26" t="s">
@@ -2072,7 +2075,7 @@
       <c r="Q4" s="51">
         <v>0</v>
       </c>
-      <c r="R4" s="27">
+      <c r="R4" s="118">
         <v>1</v>
       </c>
       <c r="S4" s="27"/>
@@ -2081,8 +2084,8 @@
       <c r="V4" s="27"/>
       <c r="W4" s="77"/>
     </row>
-    <row r="5" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="105"/>
+    <row r="5" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="115"/>
       <c r="C5" s="24" t="s">
         <v>100</v>
       </c>
@@ -2146,8 +2149,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="105"/>
+    <row r="6" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="115"/>
       <c r="C6" s="24" t="s">
         <v>101</v>
       </c>
@@ -2192,15 +2195,17 @@
       <c r="Q6" s="74">
         <v>0</v>
       </c>
-      <c r="R6" s="5"/>
+      <c r="R6" s="74">
+        <v>0</v>
+      </c>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
       <c r="W6" s="78"/>
     </row>
-    <row r="7" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="105"/>
+    <row r="7" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="115"/>
       <c r="C7" s="24" t="s">
         <v>102</v>
       </c>
@@ -2245,15 +2250,17 @@
       <c r="Q7" s="74">
         <v>0</v>
       </c>
-      <c r="R7" s="5"/>
+      <c r="R7" s="74">
+        <v>0</v>
+      </c>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="78"/>
     </row>
-    <row r="8" spans="1:23" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="106"/>
+    <row r="8" spans="1:23" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="116"/>
       <c r="C8" s="30" t="s">
         <v>110</v>
       </c>
@@ -2317,8 +2324,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="104" t="s">
+    <row r="9" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="114" t="s">
         <v>105</v>
       </c>
       <c r="C9" s="33" t="s">
@@ -2384,8 +2391,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="105"/>
+    <row r="10" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="115"/>
       <c r="C10" s="23" t="s">
         <v>106</v>
       </c>
@@ -2430,15 +2437,17 @@
       <c r="Q10" s="74">
         <v>0</v>
       </c>
-      <c r="R10" s="5"/>
+      <c r="R10" s="74">
+        <v>0</v>
+      </c>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
       <c r="W10" s="78"/>
     </row>
-    <row r="11" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="105"/>
+    <row r="11" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="115"/>
       <c r="C11" s="65" t="s">
         <v>111</v>
       </c>
@@ -2502,8 +2511,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="105"/>
+    <row r="12" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="115"/>
       <c r="C12" s="65" t="s">
         <v>112</v>
       </c>
@@ -2567,8 +2576,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="106"/>
+    <row r="13" spans="1:23" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="116"/>
       <c r="C13" s="35" t="s">
         <v>97</v>
       </c>
@@ -2632,8 +2641,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="93" t="s">
+    <row r="14" spans="1:23" ht="18" x14ac:dyDescent="0.3">
+      <c r="B14" s="89" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="36" t="s">
@@ -2701,9 +2710,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B15" s="94"/>
-      <c r="C15" s="98" t="s">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B15" s="90"/>
+      <c r="C15" s="108" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -2768,9 +2777,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B16" s="94"/>
-      <c r="C16" s="99"/>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B16" s="90"/>
+      <c r="C16" s="109"/>
       <c r="D16" s="4" t="s">
         <v>20</v>
       </c>
@@ -2833,9 +2842,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="94"/>
-      <c r="C17" s="99"/>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B17" s="90"/>
+      <c r="C17" s="109"/>
       <c r="D17" s="4" t="s">
         <v>21</v>
       </c>
@@ -2898,9 +2907,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="94"/>
-      <c r="C18" s="99"/>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B18" s="90"/>
+      <c r="C18" s="109"/>
       <c r="D18" s="4" t="s">
         <v>22</v>
       </c>
@@ -2963,9 +2972,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B19" s="94"/>
-      <c r="C19" s="99"/>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B19" s="90"/>
+      <c r="C19" s="109"/>
       <c r="D19" s="4" t="s">
         <v>23</v>
       </c>
@@ -3028,9 +3037,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B20" s="94"/>
-      <c r="C20" s="99"/>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B20" s="90"/>
+      <c r="C20" s="109"/>
       <c r="D20" s="4" t="s">
         <v>162</v>
       </c>
@@ -3074,16 +3083,18 @@
       <c r="Q20" s="52">
         <v>0</v>
       </c>
-      <c r="R20" s="5"/>
+      <c r="R20" s="52">
+        <v>0</v>
+      </c>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
       <c r="U20" s="5"/>
       <c r="V20" s="5"/>
       <c r="W20" s="78"/>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B21" s="94"/>
-      <c r="C21" s="99"/>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B21" s="90"/>
+      <c r="C21" s="109"/>
       <c r="D21" s="4" t="s">
         <v>24</v>
       </c>
@@ -3146,9 +3157,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B22" s="94"/>
-      <c r="C22" s="99"/>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B22" s="90"/>
+      <c r="C22" s="109"/>
       <c r="D22" s="21" t="s">
         <v>167</v>
       </c>
@@ -3166,7 +3177,7 @@
       </c>
       <c r="I22" s="37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.73299999999999998</v>
       </c>
       <c r="J22" s="52">
         <v>0</v>
@@ -3192,16 +3203,18 @@
       <c r="Q22" s="52">
         <v>0</v>
       </c>
-      <c r="R22" s="5"/>
+      <c r="R22" s="73">
+        <v>0.73299999999999998</v>
+      </c>
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
       <c r="V22" s="5"/>
       <c r="W22" s="78"/>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B23" s="94"/>
-      <c r="C23" s="99"/>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B23" s="90"/>
+      <c r="C23" s="109"/>
       <c r="D23" s="21" t="s">
         <v>36</v>
       </c>
@@ -3219,7 +3232,7 @@
       </c>
       <c r="I23" s="37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.016</v>
       </c>
       <c r="J23" s="52">
         <v>0</v>
@@ -3245,16 +3258,20 @@
       <c r="Q23" s="52">
         <v>0</v>
       </c>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
+      <c r="R23" s="74">
+        <v>1.4</v>
+      </c>
+      <c r="S23" s="73">
+        <v>0.61599999999999999</v>
+      </c>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
       <c r="V23" s="5"/>
       <c r="W23" s="78"/>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B24" s="94"/>
-      <c r="C24" s="99"/>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B24" s="90"/>
+      <c r="C24" s="109"/>
       <c r="D24" s="21" t="s">
         <v>37</v>
       </c>
@@ -3298,16 +3315,18 @@
       <c r="Q24" s="52">
         <v>0</v>
       </c>
-      <c r="R24" s="5"/>
+      <c r="R24" s="52">
+        <v>0</v>
+      </c>
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
       <c r="U24" s="5"/>
       <c r="V24" s="5"/>
       <c r="W24" s="78"/>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B25" s="94"/>
-      <c r="C25" s="99"/>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B25" s="90"/>
+      <c r="C25" s="109"/>
       <c r="D25" s="21" t="s">
         <v>38</v>
       </c>
@@ -3351,16 +3370,18 @@
       <c r="Q25" s="52">
         <v>0</v>
       </c>
-      <c r="R25" s="5"/>
+      <c r="R25" s="52">
+        <v>0</v>
+      </c>
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
       <c r="W25" s="78"/>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B26" s="94"/>
-      <c r="C26" s="99"/>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B26" s="90"/>
+      <c r="C26" s="109"/>
       <c r="D26" s="21" t="s">
         <v>39</v>
       </c>
@@ -3404,16 +3425,18 @@
       <c r="Q26" s="52">
         <v>0</v>
       </c>
-      <c r="R26" s="5"/>
+      <c r="R26" s="52">
+        <v>0</v>
+      </c>
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
       <c r="V26" s="5"/>
       <c r="W26" s="78"/>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B27" s="94"/>
-      <c r="C27" s="99"/>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B27" s="90"/>
+      <c r="C27" s="109"/>
       <c r="D27" s="21" t="s">
         <v>40</v>
       </c>
@@ -3457,16 +3480,18 @@
       <c r="Q27" s="52">
         <v>0</v>
       </c>
-      <c r="R27" s="5"/>
+      <c r="R27" s="52">
+        <v>0</v>
+      </c>
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
       <c r="V27" s="5"/>
       <c r="W27" s="78"/>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B28" s="94"/>
-      <c r="C28" s="99"/>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B28" s="90"/>
+      <c r="C28" s="109"/>
       <c r="D28" s="21" t="s">
         <v>41</v>
       </c>
@@ -3510,16 +3535,18 @@
       <c r="Q28" s="52">
         <v>0</v>
       </c>
-      <c r="R28" s="5"/>
+      <c r="R28" s="52">
+        <v>0</v>
+      </c>
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>
       <c r="W28" s="78"/>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B29" s="94"/>
-      <c r="C29" s="99"/>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B29" s="90"/>
+      <c r="C29" s="109"/>
       <c r="D29" s="21" t="s">
         <v>42</v>
       </c>
@@ -3563,16 +3590,18 @@
       <c r="Q29" s="52">
         <v>0</v>
       </c>
-      <c r="R29" s="5"/>
+      <c r="R29" s="52">
+        <v>0</v>
+      </c>
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
       <c r="U29" s="5"/>
       <c r="V29" s="5"/>
       <c r="W29" s="78"/>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B30" s="94"/>
-      <c r="C30" s="99"/>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B30" s="90"/>
+      <c r="C30" s="109"/>
       <c r="D30" s="21" t="s">
         <v>43</v>
       </c>
@@ -3616,16 +3645,18 @@
       <c r="Q30" s="52">
         <v>0</v>
       </c>
-      <c r="R30" s="5"/>
+      <c r="R30" s="52">
+        <v>0</v>
+      </c>
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
       <c r="V30" s="5"/>
       <c r="W30" s="78"/>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B31" s="94"/>
-      <c r="C31" s="99"/>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B31" s="90"/>
+      <c r="C31" s="109"/>
       <c r="D31" s="21" t="s">
         <v>44</v>
       </c>
@@ -3669,16 +3700,18 @@
       <c r="Q31" s="52">
         <v>0</v>
       </c>
-      <c r="R31" s="5"/>
+      <c r="R31" s="52">
+        <v>0</v>
+      </c>
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
       <c r="V31" s="5"/>
       <c r="W31" s="78"/>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B32" s="94"/>
-      <c r="C32" s="99"/>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B32" s="90"/>
+      <c r="C32" s="109"/>
       <c r="D32" s="21" t="s">
         <v>45</v>
       </c>
@@ -3722,16 +3755,18 @@
       <c r="Q32" s="52">
         <v>0</v>
       </c>
-      <c r="R32" s="5"/>
+      <c r="R32" s="52">
+        <v>0</v>
+      </c>
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
       <c r="V32" s="5"/>
       <c r="W32" s="78"/>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B33" s="94"/>
-      <c r="C33" s="99"/>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B33" s="90"/>
+      <c r="C33" s="109"/>
       <c r="D33" s="21" t="s">
         <v>46</v>
       </c>
@@ -3775,16 +3810,18 @@
       <c r="Q33" s="52">
         <v>0</v>
       </c>
-      <c r="R33" s="5"/>
+      <c r="R33" s="52">
+        <v>0</v>
+      </c>
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
       <c r="V33" s="5"/>
       <c r="W33" s="78"/>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B34" s="94"/>
-      <c r="C34" s="99"/>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B34" s="90"/>
+      <c r="C34" s="109"/>
       <c r="D34" s="21" t="s">
         <v>47</v>
       </c>
@@ -3828,16 +3865,18 @@
       <c r="Q34" s="52">
         <v>0</v>
       </c>
-      <c r="R34" s="5"/>
+      <c r="R34" s="52">
+        <v>0</v>
+      </c>
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
       <c r="U34" s="5"/>
       <c r="V34" s="5"/>
       <c r="W34" s="78"/>
     </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35" s="94"/>
-      <c r="C35" s="99"/>
+    <row r="35" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B35" s="90"/>
+      <c r="C35" s="109"/>
       <c r="D35" s="21" t="s">
         <v>48</v>
       </c>
@@ -3881,16 +3920,18 @@
       <c r="Q35" s="52">
         <v>0</v>
       </c>
-      <c r="R35" s="5"/>
+      <c r="R35" s="52">
+        <v>0</v>
+      </c>
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
       <c r="U35" s="5"/>
       <c r="V35" s="5"/>
       <c r="W35" s="78"/>
     </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B36" s="94"/>
-      <c r="C36" s="99"/>
+    <row r="36" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B36" s="90"/>
+      <c r="C36" s="109"/>
       <c r="D36" s="21" t="s">
         <v>49</v>
       </c>
@@ -3934,16 +3975,18 @@
       <c r="Q36" s="52">
         <v>0</v>
       </c>
-      <c r="R36" s="5"/>
+      <c r="R36" s="52">
+        <v>0</v>
+      </c>
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
       <c r="U36" s="5"/>
       <c r="V36" s="5"/>
       <c r="W36" s="78"/>
     </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B37" s="94"/>
-      <c r="C37" s="99"/>
+    <row r="37" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B37" s="90"/>
+      <c r="C37" s="109"/>
       <c r="D37" s="21" t="s">
         <v>50</v>
       </c>
@@ -3987,16 +4030,18 @@
       <c r="Q37" s="52">
         <v>0</v>
       </c>
-      <c r="R37" s="5"/>
+      <c r="R37" s="52">
+        <v>0</v>
+      </c>
       <c r="S37" s="5"/>
       <c r="T37" s="5"/>
       <c r="U37" s="5"/>
       <c r="V37" s="5"/>
       <c r="W37" s="78"/>
     </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B38" s="94"/>
-      <c r="C38" s="99"/>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B38" s="90"/>
+      <c r="C38" s="109"/>
       <c r="D38" s="21" t="s">
         <v>51</v>
       </c>
@@ -4040,16 +4085,18 @@
       <c r="Q38" s="52">
         <v>0</v>
       </c>
-      <c r="R38" s="5"/>
+      <c r="R38" s="52">
+        <v>0</v>
+      </c>
       <c r="S38" s="5"/>
       <c r="T38" s="5"/>
       <c r="U38" s="5"/>
       <c r="V38" s="5"/>
       <c r="W38" s="78"/>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B39" s="94"/>
-      <c r="C39" s="99"/>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B39" s="90"/>
+      <c r="C39" s="109"/>
       <c r="D39" s="21" t="s">
         <v>52</v>
       </c>
@@ -4093,16 +4140,18 @@
       <c r="Q39" s="52">
         <v>0</v>
       </c>
-      <c r="R39" s="5"/>
+      <c r="R39" s="52">
+        <v>0</v>
+      </c>
       <c r="S39" s="5"/>
       <c r="T39" s="5"/>
       <c r="U39" s="5"/>
       <c r="V39" s="5"/>
       <c r="W39" s="78"/>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B40" s="94"/>
-      <c r="C40" s="99"/>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B40" s="90"/>
+      <c r="C40" s="109"/>
       <c r="D40" s="21" t="s">
         <v>53</v>
       </c>
@@ -4146,16 +4195,18 @@
       <c r="Q40" s="52">
         <v>0</v>
       </c>
-      <c r="R40" s="5"/>
+      <c r="R40" s="52">
+        <v>0</v>
+      </c>
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
       <c r="U40" s="5"/>
       <c r="V40" s="5"/>
       <c r="W40" s="78"/>
     </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B41" s="94"/>
-      <c r="C41" s="99"/>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B41" s="90"/>
+      <c r="C41" s="109"/>
       <c r="D41" s="21" t="s">
         <v>54</v>
       </c>
@@ -4199,16 +4250,18 @@
       <c r="Q41" s="52">
         <v>0</v>
       </c>
-      <c r="R41" s="5"/>
+      <c r="R41" s="52">
+        <v>0</v>
+      </c>
       <c r="S41" s="5"/>
       <c r="T41" s="5"/>
       <c r="U41" s="5"/>
       <c r="V41" s="5"/>
       <c r="W41" s="78"/>
     </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B42" s="94"/>
-      <c r="C42" s="99"/>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B42" s="90"/>
+      <c r="C42" s="109"/>
       <c r="D42" s="21" t="s">
         <v>55</v>
       </c>
@@ -4252,16 +4305,18 @@
       <c r="Q42" s="52">
         <v>0</v>
       </c>
-      <c r="R42" s="5"/>
+      <c r="R42" s="52">
+        <v>0</v>
+      </c>
       <c r="S42" s="5"/>
       <c r="T42" s="5"/>
       <c r="U42" s="5"/>
       <c r="V42" s="5"/>
       <c r="W42" s="78"/>
     </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B43" s="94"/>
-      <c r="C43" s="99"/>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B43" s="90"/>
+      <c r="C43" s="109"/>
       <c r="D43" s="21" t="s">
         <v>56</v>
       </c>
@@ -4305,16 +4360,18 @@
       <c r="Q43" s="52">
         <v>0</v>
       </c>
-      <c r="R43" s="5"/>
+      <c r="R43" s="52">
+        <v>0</v>
+      </c>
       <c r="S43" s="5"/>
       <c r="T43" s="5"/>
       <c r="U43" s="5"/>
       <c r="V43" s="5"/>
       <c r="W43" s="78"/>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B44" s="94"/>
-      <c r="C44" s="99"/>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B44" s="90"/>
+      <c r="C44" s="109"/>
       <c r="D44" s="21" t="s">
         <v>57</v>
       </c>
@@ -4358,16 +4415,18 @@
       <c r="Q44" s="52">
         <v>0</v>
       </c>
-      <c r="R44" s="5"/>
+      <c r="R44" s="52">
+        <v>0</v>
+      </c>
       <c r="S44" s="5"/>
       <c r="T44" s="5"/>
       <c r="U44" s="5"/>
       <c r="V44" s="5"/>
       <c r="W44" s="78"/>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B45" s="94"/>
-      <c r="C45" s="99"/>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B45" s="90"/>
+      <c r="C45" s="109"/>
       <c r="D45" s="21" t="s">
         <v>58</v>
       </c>
@@ -4411,16 +4470,18 @@
       <c r="Q45" s="52">
         <v>0</v>
       </c>
-      <c r="R45" s="5"/>
+      <c r="R45" s="52">
+        <v>0</v>
+      </c>
       <c r="S45" s="5"/>
       <c r="T45" s="5"/>
       <c r="U45" s="5"/>
       <c r="V45" s="5"/>
       <c r="W45" s="78"/>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B46" s="94"/>
-      <c r="C46" s="99"/>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B46" s="90"/>
+      <c r="C46" s="109"/>
       <c r="D46" s="21" t="s">
         <v>59</v>
       </c>
@@ -4464,16 +4525,18 @@
       <c r="Q46" s="52">
         <v>0</v>
       </c>
-      <c r="R46" s="5"/>
+      <c r="R46" s="52">
+        <v>0</v>
+      </c>
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
       <c r="U46" s="5"/>
       <c r="V46" s="5"/>
       <c r="W46" s="78"/>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B47" s="94"/>
-      <c r="C47" s="99"/>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B47" s="90"/>
+      <c r="C47" s="109"/>
       <c r="D47" s="21" t="s">
         <v>60</v>
       </c>
@@ -4517,16 +4580,18 @@
       <c r="Q47" s="52">
         <v>0</v>
       </c>
-      <c r="R47" s="5"/>
+      <c r="R47" s="52">
+        <v>0</v>
+      </c>
       <c r="S47" s="5"/>
       <c r="T47" s="5"/>
       <c r="U47" s="5"/>
       <c r="V47" s="5"/>
       <c r="W47" s="78"/>
     </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B48" s="94"/>
-      <c r="C48" s="99"/>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B48" s="90"/>
+      <c r="C48" s="109"/>
       <c r="D48" s="21" t="s">
         <v>61</v>
       </c>
@@ -4570,16 +4635,18 @@
       <c r="Q48" s="52">
         <v>0</v>
       </c>
-      <c r="R48" s="5"/>
+      <c r="R48" s="52">
+        <v>0</v>
+      </c>
       <c r="S48" s="5"/>
       <c r="T48" s="5"/>
       <c r="U48" s="5"/>
       <c r="V48" s="5"/>
       <c r="W48" s="78"/>
     </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B49" s="94"/>
-      <c r="C49" s="99"/>
+    <row r="49" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B49" s="90"/>
+      <c r="C49" s="109"/>
       <c r="D49" s="21" t="s">
         <v>62</v>
       </c>
@@ -4623,16 +4690,18 @@
       <c r="Q49" s="52">
         <v>0</v>
       </c>
-      <c r="R49" s="5"/>
+      <c r="R49" s="52">
+        <v>0</v>
+      </c>
       <c r="S49" s="5"/>
       <c r="T49" s="5"/>
       <c r="U49" s="5"/>
       <c r="V49" s="5"/>
       <c r="W49" s="78"/>
     </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B50" s="94"/>
-      <c r="C50" s="99"/>
+    <row r="50" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B50" s="90"/>
+      <c r="C50" s="109"/>
       <c r="D50" s="21" t="s">
         <v>63</v>
       </c>
@@ -4676,16 +4745,18 @@
       <c r="Q50" s="52">
         <v>0</v>
       </c>
-      <c r="R50" s="5"/>
+      <c r="R50" s="52">
+        <v>0</v>
+      </c>
       <c r="S50" s="5"/>
       <c r="T50" s="5"/>
       <c r="U50" s="5"/>
       <c r="V50" s="5"/>
       <c r="W50" s="78"/>
     </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B51" s="94"/>
-      <c r="C51" s="99"/>
+    <row r="51" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B51" s="90"/>
+      <c r="C51" s="109"/>
       <c r="D51" s="21" t="s">
         <v>64</v>
       </c>
@@ -4729,16 +4800,18 @@
       <c r="Q51" s="52">
         <v>0</v>
       </c>
-      <c r="R51" s="5"/>
+      <c r="R51" s="52">
+        <v>0</v>
+      </c>
       <c r="S51" s="5"/>
       <c r="T51" s="5"/>
       <c r="U51" s="5"/>
       <c r="V51" s="5"/>
       <c r="W51" s="78"/>
     </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B52" s="94"/>
-      <c r="C52" s="99"/>
+    <row r="52" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B52" s="90"/>
+      <c r="C52" s="109"/>
       <c r="D52" s="21" t="s">
         <v>65</v>
       </c>
@@ -4782,16 +4855,18 @@
       <c r="Q52" s="52">
         <v>0</v>
       </c>
-      <c r="R52" s="5"/>
+      <c r="R52" s="52">
+        <v>0</v>
+      </c>
       <c r="S52" s="5"/>
       <c r="T52" s="5"/>
       <c r="U52" s="5"/>
       <c r="V52" s="5"/>
       <c r="W52" s="78"/>
     </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B53" s="94"/>
-      <c r="C53" s="99"/>
+    <row r="53" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B53" s="90"/>
+      <c r="C53" s="109"/>
       <c r="D53" s="21" t="s">
         <v>66</v>
       </c>
@@ -4835,16 +4910,18 @@
       <c r="Q53" s="52">
         <v>0</v>
       </c>
-      <c r="R53" s="5"/>
+      <c r="R53" s="52">
+        <v>0</v>
+      </c>
       <c r="S53" s="5"/>
       <c r="T53" s="5"/>
       <c r="U53" s="5"/>
       <c r="V53" s="5"/>
       <c r="W53" s="78"/>
     </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B54" s="94"/>
-      <c r="C54" s="99"/>
+    <row r="54" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B54" s="90"/>
+      <c r="C54" s="109"/>
       <c r="D54" s="21" t="s">
         <v>67</v>
       </c>
@@ -4888,16 +4965,18 @@
       <c r="Q54" s="52">
         <v>0</v>
       </c>
-      <c r="R54" s="5"/>
+      <c r="R54" s="52">
+        <v>0</v>
+      </c>
       <c r="S54" s="5"/>
       <c r="T54" s="5"/>
       <c r="U54" s="5"/>
       <c r="V54" s="5"/>
       <c r="W54" s="78"/>
     </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B55" s="94"/>
-      <c r="C55" s="99"/>
+    <row r="55" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B55" s="90"/>
+      <c r="C55" s="109"/>
       <c r="D55" s="21" t="s">
         <v>68</v>
       </c>
@@ -4941,16 +5020,18 @@
       <c r="Q55" s="52">
         <v>0</v>
       </c>
-      <c r="R55" s="5"/>
+      <c r="R55" s="52">
+        <v>0</v>
+      </c>
       <c r="S55" s="5"/>
       <c r="T55" s="5"/>
       <c r="U55" s="5"/>
       <c r="V55" s="5"/>
       <c r="W55" s="78"/>
     </row>
-    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B56" s="94"/>
-      <c r="C56" s="100"/>
+    <row r="56" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B56" s="90"/>
+      <c r="C56" s="110"/>
       <c r="D56" s="21" t="s">
         <v>69</v>
       </c>
@@ -4994,16 +5075,18 @@
       <c r="Q56" s="52">
         <v>0</v>
       </c>
-      <c r="R56" s="5"/>
+      <c r="R56" s="52">
+        <v>0</v>
+      </c>
       <c r="S56" s="5"/>
       <c r="T56" s="5"/>
       <c r="U56" s="5"/>
       <c r="V56" s="5"/>
       <c r="W56" s="78"/>
     </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B57" s="94"/>
-      <c r="C57" s="96" t="s">
+    <row r="57" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B57" s="90"/>
+      <c r="C57" s="106" t="s">
         <v>26</v>
       </c>
       <c r="D57" s="18" t="s">
@@ -5049,16 +5132,18 @@
       <c r="Q57" s="52">
         <v>0</v>
       </c>
-      <c r="R57" s="5"/>
+      <c r="R57" s="52">
+        <v>0</v>
+      </c>
       <c r="S57" s="5"/>
       <c r="T57" s="5"/>
       <c r="U57" s="5"/>
       <c r="V57" s="5"/>
       <c r="W57" s="78"/>
     </row>
-    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B58" s="94"/>
-      <c r="C58" s="97"/>
+    <row r="58" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B58" s="90"/>
+      <c r="C58" s="107"/>
       <c r="D58" s="18" t="s">
         <v>29</v>
       </c>
@@ -5102,16 +5187,18 @@
       <c r="Q58" s="52">
         <v>0</v>
       </c>
-      <c r="R58" s="5"/>
+      <c r="R58" s="52">
+        <v>0</v>
+      </c>
       <c r="S58" s="5"/>
       <c r="T58" s="5"/>
       <c r="U58" s="5"/>
       <c r="V58" s="5"/>
       <c r="W58" s="78"/>
     </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B59" s="94"/>
-      <c r="C59" s="97"/>
+    <row r="59" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B59" s="90"/>
+      <c r="C59" s="107"/>
       <c r="D59" s="18" t="s">
         <v>30</v>
       </c>
@@ -5155,16 +5242,18 @@
       <c r="Q59" s="52">
         <v>0</v>
       </c>
-      <c r="R59" s="5"/>
+      <c r="R59" s="52">
+        <v>0</v>
+      </c>
       <c r="S59" s="5"/>
       <c r="T59" s="5"/>
       <c r="U59" s="5"/>
       <c r="V59" s="5"/>
       <c r="W59" s="78"/>
     </row>
-    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B60" s="94"/>
-      <c r="C60" s="97"/>
+    <row r="60" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B60" s="90"/>
+      <c r="C60" s="107"/>
       <c r="D60" s="18" t="s">
         <v>31</v>
       </c>
@@ -5208,16 +5297,18 @@
       <c r="Q60" s="52">
         <v>0</v>
       </c>
-      <c r="R60" s="5"/>
+      <c r="R60" s="52">
+        <v>0</v>
+      </c>
       <c r="S60" s="5"/>
       <c r="T60" s="5"/>
       <c r="U60" s="5"/>
       <c r="V60" s="5"/>
       <c r="W60" s="78"/>
     </row>
-    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B61" s="94"/>
-      <c r="C61" s="97"/>
+    <row r="61" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B61" s="90"/>
+      <c r="C61" s="107"/>
       <c r="D61" s="18" t="s">
         <v>34</v>
       </c>
@@ -5261,16 +5352,18 @@
       <c r="Q61" s="52">
         <v>0</v>
       </c>
-      <c r="R61" s="5"/>
+      <c r="R61" s="52">
+        <v>0</v>
+      </c>
       <c r="S61" s="5"/>
       <c r="T61" s="5"/>
       <c r="U61" s="5"/>
       <c r="V61" s="5"/>
       <c r="W61" s="78"/>
     </row>
-    <row r="62" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B62" s="94"/>
-      <c r="C62" s="97"/>
+    <row r="62" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B62" s="90"/>
+      <c r="C62" s="107"/>
       <c r="D62" s="18" t="s">
         <v>32</v>
       </c>
@@ -5314,16 +5407,18 @@
       <c r="Q62" s="52">
         <v>0</v>
       </c>
-      <c r="R62" s="5"/>
+      <c r="R62" s="52">
+        <v>0</v>
+      </c>
       <c r="S62" s="5"/>
       <c r="T62" s="5"/>
       <c r="U62" s="5"/>
       <c r="V62" s="5"/>
       <c r="W62" s="78"/>
     </row>
-    <row r="63" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="112"/>
-      <c r="C63" s="97"/>
+    <row r="63" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="97"/>
+      <c r="C63" s="107"/>
       <c r="D63" s="44" t="s">
         <v>33</v>
       </c>
@@ -5367,18 +5462,20 @@
       <c r="Q63" s="54">
         <v>0</v>
       </c>
-      <c r="R63" s="80"/>
+      <c r="R63" s="54">
+        <v>0</v>
+      </c>
       <c r="S63" s="80"/>
       <c r="T63" s="80"/>
       <c r="U63" s="80"/>
       <c r="V63" s="80"/>
       <c r="W63" s="81"/>
     </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B64" s="93" t="s">
+    <row r="64" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B64" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="C64" s="101" t="s">
+      <c r="C64" s="111" t="s">
         <v>79</v>
       </c>
       <c r="D64" s="28" t="s">
@@ -5424,16 +5521,18 @@
       <c r="Q64" s="51">
         <v>0</v>
       </c>
-      <c r="R64" s="34"/>
+      <c r="R64" s="51">
+        <v>0</v>
+      </c>
       <c r="S64" s="34"/>
       <c r="T64" s="34"/>
       <c r="U64" s="34"/>
       <c r="V64" s="34"/>
       <c r="W64" s="82"/>
     </row>
-    <row r="65" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B65" s="94"/>
-      <c r="C65" s="102"/>
+    <row r="65" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B65" s="90"/>
+      <c r="C65" s="112"/>
       <c r="D65" s="4" t="s">
         <v>71</v>
       </c>
@@ -5477,16 +5576,18 @@
       <c r="Q65" s="52">
         <v>0</v>
       </c>
-      <c r="R65" s="5"/>
+      <c r="R65" s="52">
+        <v>0</v>
+      </c>
       <c r="S65" s="5"/>
       <c r="T65" s="5"/>
       <c r="U65" s="5"/>
       <c r="V65" s="5"/>
       <c r="W65" s="78"/>
     </row>
-    <row r="66" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B66" s="94"/>
-      <c r="C66" s="102"/>
+    <row r="66" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B66" s="90"/>
+      <c r="C66" s="112"/>
       <c r="D66" s="4" t="s">
         <v>72</v>
       </c>
@@ -5530,16 +5631,18 @@
       <c r="Q66" s="52">
         <v>0</v>
       </c>
-      <c r="R66" s="5"/>
+      <c r="R66" s="52">
+        <v>0</v>
+      </c>
       <c r="S66" s="5"/>
       <c r="T66" s="5"/>
       <c r="U66" s="5"/>
       <c r="V66" s="5"/>
       <c r="W66" s="78"/>
     </row>
-    <row r="67" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B67" s="94"/>
-      <c r="C67" s="102"/>
+    <row r="67" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B67" s="90"/>
+      <c r="C67" s="112"/>
       <c r="D67" s="18" t="s">
         <v>76</v>
       </c>
@@ -5583,15 +5686,17 @@
       <c r="Q67" s="52">
         <v>0</v>
       </c>
-      <c r="R67" s="5"/>
+      <c r="R67" s="52">
+        <v>0</v>
+      </c>
       <c r="S67" s="5"/>
       <c r="T67" s="5"/>
       <c r="U67" s="5"/>
       <c r="V67" s="5"/>
       <c r="W67" s="78"/>
     </row>
-    <row r="68" spans="2:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="94"/>
+    <row r="68" spans="2:23" ht="18" x14ac:dyDescent="0.3">
+      <c r="B68" s="90"/>
       <c r="C68" s="22" t="s">
         <v>73</v>
       </c>
@@ -5636,15 +5741,17 @@
       <c r="Q68" s="52">
         <v>0</v>
       </c>
-      <c r="R68" s="5"/>
+      <c r="R68" s="52">
+        <v>0</v>
+      </c>
       <c r="S68" s="5"/>
       <c r="T68" s="5"/>
       <c r="U68" s="5"/>
       <c r="V68" s="5"/>
       <c r="W68" s="78"/>
     </row>
-    <row r="69" spans="2:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B69" s="94"/>
+    <row r="69" spans="2:23" ht="18" x14ac:dyDescent="0.3">
+      <c r="B69" s="90"/>
       <c r="C69" s="22" t="s">
         <v>81</v>
       </c>
@@ -5689,16 +5796,18 @@
       <c r="Q69" s="52">
         <v>0</v>
       </c>
-      <c r="R69" s="5"/>
+      <c r="R69" s="52">
+        <v>0</v>
+      </c>
       <c r="S69" s="5"/>
       <c r="T69" s="5"/>
       <c r="U69" s="5"/>
       <c r="V69" s="5"/>
       <c r="W69" s="78"/>
     </row>
-    <row r="70" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="94"/>
-      <c r="C70" s="102" t="s">
+    <row r="70" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="90"/>
+      <c r="C70" s="112" t="s">
         <v>80</v>
       </c>
       <c r="D70" s="4" t="s">
@@ -5744,16 +5853,18 @@
       <c r="Q70" s="52">
         <v>0</v>
       </c>
-      <c r="R70" s="5"/>
+      <c r="R70" s="52">
+        <v>0</v>
+      </c>
       <c r="S70" s="5"/>
       <c r="T70" s="5"/>
       <c r="U70" s="5"/>
       <c r="V70" s="5"/>
       <c r="W70" s="78"/>
     </row>
-    <row r="71" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="94"/>
-      <c r="C71" s="102"/>
+    <row r="71" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="90"/>
+      <c r="C71" s="112"/>
       <c r="D71" s="4" t="s">
         <v>75</v>
       </c>
@@ -5797,16 +5908,18 @@
       <c r="Q71" s="52">
         <v>0</v>
       </c>
-      <c r="R71" s="5"/>
+      <c r="R71" s="52">
+        <v>0</v>
+      </c>
       <c r="S71" s="5"/>
       <c r="T71" s="5"/>
       <c r="U71" s="5"/>
       <c r="V71" s="5"/>
       <c r="W71" s="78"/>
     </row>
-    <row r="72" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="94"/>
-      <c r="C72" s="102"/>
+    <row r="72" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="90"/>
+      <c r="C72" s="112"/>
       <c r="D72" s="4" t="s">
         <v>77</v>
       </c>
@@ -5850,16 +5963,18 @@
       <c r="Q72" s="52">
         <v>0</v>
       </c>
-      <c r="R72" s="5"/>
+      <c r="R72" s="52">
+        <v>0</v>
+      </c>
       <c r="S72" s="5"/>
       <c r="T72" s="5"/>
       <c r="U72" s="5"/>
       <c r="V72" s="5"/>
       <c r="W72" s="78"/>
     </row>
-    <row r="73" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="95"/>
-      <c r="C73" s="103"/>
+    <row r="73" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B73" s="91"/>
+      <c r="C73" s="113"/>
       <c r="D73" s="17" t="s">
         <v>78</v>
       </c>
@@ -5903,18 +6018,20 @@
       <c r="Q73" s="53">
         <v>0</v>
       </c>
-      <c r="R73" s="31"/>
+      <c r="R73" s="53">
+        <v>0</v>
+      </c>
       <c r="S73" s="31"/>
       <c r="T73" s="31"/>
       <c r="U73" s="31"/>
       <c r="V73" s="31"/>
       <c r="W73" s="79"/>
     </row>
-    <row r="74" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="93" t="s">
+    <row r="74" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="89" t="s">
         <v>115</v>
       </c>
-      <c r="C74" s="107" t="s">
+      <c r="C74" s="117" t="s">
         <v>116</v>
       </c>
       <c r="D74" s="28" t="s">
@@ -5979,9 +6096,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="94"/>
-      <c r="C75" s="89"/>
+    <row r="75" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B75" s="90"/>
+      <c r="C75" s="101"/>
       <c r="D75" s="4" t="s">
         <v>132</v>
       </c>
@@ -6025,16 +6142,18 @@
       <c r="Q75" s="52">
         <v>0</v>
       </c>
-      <c r="R75" s="5"/>
+      <c r="R75" s="52">
+        <v>0</v>
+      </c>
       <c r="S75" s="5"/>
       <c r="T75" s="5"/>
       <c r="U75" s="5"/>
       <c r="V75" s="5"/>
       <c r="W75" s="78"/>
     </row>
-    <row r="76" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="94"/>
-      <c r="C76" s="89"/>
+    <row r="76" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B76" s="90"/>
+      <c r="C76" s="101"/>
       <c r="D76" s="4" t="s">
         <v>161</v>
       </c>
@@ -6078,16 +6197,18 @@
       <c r="Q76" s="52">
         <v>0</v>
       </c>
-      <c r="R76" s="5"/>
+      <c r="R76" s="52">
+        <v>0</v>
+      </c>
       <c r="S76" s="5"/>
       <c r="T76" s="5"/>
       <c r="U76" s="5"/>
       <c r="V76" s="5"/>
       <c r="W76" s="78"/>
     </row>
-    <row r="77" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="94"/>
-      <c r="C77" s="89"/>
+    <row r="77" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B77" s="90"/>
+      <c r="C77" s="101"/>
       <c r="D77" s="4" t="s">
         <v>133</v>
       </c>
@@ -6150,9 +6271,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="94"/>
-      <c r="C78" s="89"/>
+    <row r="78" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B78" s="90"/>
+      <c r="C78" s="101"/>
       <c r="D78" s="4" t="s">
         <v>164</v>
       </c>
@@ -6196,16 +6317,18 @@
       <c r="Q78" s="52">
         <v>0</v>
       </c>
-      <c r="R78" s="83"/>
+      <c r="R78" s="52">
+        <v>0</v>
+      </c>
       <c r="S78" s="83"/>
       <c r="T78" s="83"/>
       <c r="U78" s="83"/>
       <c r="V78" s="83"/>
       <c r="W78" s="84"/>
     </row>
-    <row r="79" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="94"/>
-      <c r="C79" s="89"/>
+    <row r="79" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B79" s="90"/>
+      <c r="C79" s="101"/>
       <c r="D79" s="4" t="s">
         <v>163</v>
       </c>
@@ -6249,16 +6372,18 @@
       <c r="Q79" s="52">
         <v>0</v>
       </c>
-      <c r="R79" s="83"/>
+      <c r="R79" s="52">
+        <v>0</v>
+      </c>
       <c r="S79" s="83"/>
       <c r="T79" s="83"/>
       <c r="U79" s="83"/>
       <c r="V79" s="83"/>
       <c r="W79" s="84"/>
     </row>
-    <row r="80" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="94"/>
-      <c r="C80" s="89"/>
+    <row r="80" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B80" s="90"/>
+      <c r="C80" s="101"/>
       <c r="D80" s="4" t="s">
         <v>134</v>
       </c>
@@ -6302,16 +6427,18 @@
       <c r="Q80" s="52">
         <v>0</v>
       </c>
-      <c r="R80" s="5"/>
+      <c r="R80" s="52">
+        <v>0</v>
+      </c>
       <c r="S80" s="5"/>
       <c r="T80" s="5"/>
       <c r="U80" s="5"/>
       <c r="V80" s="5"/>
       <c r="W80" s="78"/>
     </row>
-    <row r="81" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="94"/>
-      <c r="C81" s="89" t="s">
+    <row r="81" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B81" s="90"/>
+      <c r="C81" s="101" t="s">
         <v>117</v>
       </c>
       <c r="D81" s="4" t="s">
@@ -6376,9 +6503,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="94"/>
-      <c r="C82" s="89"/>
+    <row r="82" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B82" s="90"/>
+      <c r="C82" s="101"/>
       <c r="D82" s="4" t="s">
         <v>132</v>
       </c>
@@ -6422,16 +6549,18 @@
       <c r="Q82" s="74">
         <v>0</v>
       </c>
-      <c r="R82" s="5"/>
+      <c r="R82" s="74">
+        <v>0</v>
+      </c>
       <c r="S82" s="5"/>
       <c r="T82" s="5"/>
       <c r="U82" s="5"/>
       <c r="V82" s="5"/>
       <c r="W82" s="78"/>
     </row>
-    <row r="83" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="94"/>
-      <c r="C83" s="89"/>
+    <row r="83" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B83" s="90"/>
+      <c r="C83" s="101"/>
       <c r="D83" s="4" t="s">
         <v>161</v>
       </c>
@@ -6475,16 +6604,18 @@
       <c r="Q83" s="52">
         <v>0</v>
       </c>
-      <c r="R83" s="5"/>
+      <c r="R83" s="52">
+        <v>0</v>
+      </c>
       <c r="S83" s="5"/>
       <c r="T83" s="5"/>
       <c r="U83" s="5"/>
       <c r="V83" s="5"/>
       <c r="W83" s="78"/>
     </row>
-    <row r="84" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="94"/>
-      <c r="C84" s="89"/>
+    <row r="84" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B84" s="90"/>
+      <c r="C84" s="101"/>
       <c r="D84" s="4" t="s">
         <v>164</v>
       </c>
@@ -6528,16 +6659,18 @@
       <c r="Q84" s="52">
         <v>0</v>
       </c>
-      <c r="R84" s="5"/>
+      <c r="R84" s="52">
+        <v>0</v>
+      </c>
       <c r="S84" s="5"/>
       <c r="T84" s="5"/>
       <c r="U84" s="5"/>
       <c r="V84" s="5"/>
       <c r="W84" s="78"/>
     </row>
-    <row r="85" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="94"/>
-      <c r="C85" s="89"/>
+    <row r="85" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B85" s="90"/>
+      <c r="C85" s="101"/>
       <c r="D85" s="4" t="s">
         <v>163</v>
       </c>
@@ -6581,16 +6714,18 @@
       <c r="Q85" s="52">
         <v>0</v>
       </c>
-      <c r="R85" s="5"/>
+      <c r="R85" s="52">
+        <v>0</v>
+      </c>
       <c r="S85" s="5"/>
       <c r="T85" s="5"/>
       <c r="U85" s="5"/>
       <c r="V85" s="5"/>
       <c r="W85" s="78"/>
     </row>
-    <row r="86" spans="2:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="94"/>
-      <c r="C86" s="89"/>
+    <row r="86" spans="2:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B86" s="90"/>
+      <c r="C86" s="101"/>
       <c r="D86" s="4" t="s">
         <v>133</v>
       </c>
@@ -6653,9 +6788,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="94"/>
-      <c r="C87" s="89"/>
+    <row r="87" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B87" s="90"/>
+      <c r="C87" s="101"/>
       <c r="D87" s="4" t="s">
         <v>134</v>
       </c>
@@ -6699,16 +6834,18 @@
       <c r="Q87" s="52">
         <v>0</v>
       </c>
-      <c r="R87" s="5"/>
+      <c r="R87" s="52">
+        <v>0</v>
+      </c>
       <c r="S87" s="5"/>
       <c r="T87" s="5"/>
       <c r="U87" s="5"/>
       <c r="V87" s="5"/>
       <c r="W87" s="78"/>
     </row>
-    <row r="88" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="94"/>
-      <c r="C88" s="89" t="s">
+    <row r="88" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="90"/>
+      <c r="C88" s="101" t="s">
         <v>118</v>
       </c>
       <c r="D88" s="4" t="s">
@@ -6773,9 +6910,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="94"/>
-      <c r="C89" s="89"/>
+    <row r="89" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B89" s="90"/>
+      <c r="C89" s="101"/>
       <c r="D89" s="4" t="s">
         <v>132</v>
       </c>
@@ -6819,16 +6956,18 @@
       <c r="Q89" s="52">
         <v>0</v>
       </c>
-      <c r="R89" s="5"/>
+      <c r="R89" s="52">
+        <v>0</v>
+      </c>
       <c r="S89" s="5"/>
       <c r="T89" s="5"/>
       <c r="U89" s="5"/>
       <c r="V89" s="5"/>
       <c r="W89" s="78"/>
     </row>
-    <row r="90" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="94"/>
-      <c r="C90" s="89"/>
+    <row r="90" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B90" s="90"/>
+      <c r="C90" s="101"/>
       <c r="D90" s="4" t="s">
         <v>161</v>
       </c>
@@ -6872,16 +7011,18 @@
       <c r="Q90" s="52">
         <v>0</v>
       </c>
-      <c r="R90" s="5"/>
+      <c r="R90" s="52">
+        <v>0</v>
+      </c>
       <c r="S90" s="5"/>
       <c r="T90" s="5"/>
       <c r="U90" s="5"/>
       <c r="V90" s="5"/>
       <c r="W90" s="78"/>
     </row>
-    <row r="91" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="94"/>
-      <c r="C91" s="89"/>
+    <row r="91" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B91" s="90"/>
+      <c r="C91" s="101"/>
       <c r="D91" s="4" t="s">
         <v>133</v>
       </c>
@@ -6944,9 +7085,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="94"/>
-      <c r="C92" s="89"/>
+    <row r="92" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B92" s="90"/>
+      <c r="C92" s="101"/>
       <c r="D92" s="4" t="s">
         <v>164</v>
       </c>
@@ -6990,16 +7131,18 @@
       <c r="Q92" s="52">
         <v>0</v>
       </c>
-      <c r="R92" s="83"/>
+      <c r="R92" s="52">
+        <v>0</v>
+      </c>
       <c r="S92" s="83"/>
       <c r="T92" s="83"/>
       <c r="U92" s="83"/>
       <c r="V92" s="83"/>
       <c r="W92" s="84"/>
     </row>
-    <row r="93" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="94"/>
-      <c r="C93" s="89"/>
+    <row r="93" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B93" s="90"/>
+      <c r="C93" s="101"/>
       <c r="D93" s="4" t="s">
         <v>163</v>
       </c>
@@ -7043,16 +7186,18 @@
       <c r="Q93" s="52">
         <v>0</v>
       </c>
-      <c r="R93" s="83"/>
+      <c r="R93" s="52">
+        <v>0</v>
+      </c>
       <c r="S93" s="83"/>
       <c r="T93" s="83"/>
       <c r="U93" s="83"/>
       <c r="V93" s="83"/>
       <c r="W93" s="84"/>
     </row>
-    <row r="94" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="94"/>
-      <c r="C94" s="89"/>
+    <row r="94" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B94" s="90"/>
+      <c r="C94" s="101"/>
       <c r="D94" s="4" t="s">
         <v>134</v>
       </c>
@@ -7096,16 +7241,18 @@
       <c r="Q94" s="52">
         <v>0</v>
       </c>
-      <c r="R94" s="5"/>
+      <c r="R94" s="52">
+        <v>0</v>
+      </c>
       <c r="S94" s="5"/>
       <c r="T94" s="5"/>
       <c r="U94" s="5"/>
       <c r="V94" s="5"/>
       <c r="W94" s="78"/>
     </row>
-    <row r="95" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="94"/>
-      <c r="C95" s="89" t="s">
+    <row r="95" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B95" s="90"/>
+      <c r="C95" s="101" t="s">
         <v>119</v>
       </c>
       <c r="D95" s="4" t="s">
@@ -7170,9 +7317,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="94"/>
-      <c r="C96" s="89"/>
+    <row r="96" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B96" s="90"/>
+      <c r="C96" s="101"/>
       <c r="D96" s="4" t="s">
         <v>132</v>
       </c>
@@ -7216,16 +7363,18 @@
       <c r="Q96" s="52">
         <v>0</v>
       </c>
-      <c r="R96" s="5"/>
+      <c r="R96" s="52">
+        <v>0</v>
+      </c>
       <c r="S96" s="5"/>
       <c r="T96" s="5"/>
       <c r="U96" s="5"/>
       <c r="V96" s="5"/>
       <c r="W96" s="78"/>
     </row>
-    <row r="97" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="94"/>
-      <c r="C97" s="89"/>
+    <row r="97" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B97" s="90"/>
+      <c r="C97" s="101"/>
       <c r="D97" s="4" t="s">
         <v>161</v>
       </c>
@@ -7269,16 +7418,18 @@
       <c r="Q97" s="52">
         <v>0</v>
       </c>
-      <c r="R97" s="5"/>
+      <c r="R97" s="52">
+        <v>0</v>
+      </c>
       <c r="S97" s="5"/>
       <c r="T97" s="5"/>
       <c r="U97" s="5"/>
       <c r="V97" s="5"/>
       <c r="W97" s="78"/>
     </row>
-    <row r="98" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="94"/>
-      <c r="C98" s="89"/>
+    <row r="98" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B98" s="90"/>
+      <c r="C98" s="101"/>
       <c r="D98" s="4" t="s">
         <v>133</v>
       </c>
@@ -7341,9 +7492,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="94"/>
-      <c r="C99" s="89"/>
+    <row r="99" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B99" s="90"/>
+      <c r="C99" s="101"/>
       <c r="D99" s="4" t="s">
         <v>164</v>
       </c>
@@ -7387,16 +7538,18 @@
       <c r="Q99" s="52">
         <v>0</v>
       </c>
-      <c r="R99" s="83"/>
+      <c r="R99" s="52">
+        <v>0</v>
+      </c>
       <c r="S99" s="83"/>
       <c r="T99" s="83"/>
       <c r="U99" s="83"/>
       <c r="V99" s="83"/>
       <c r="W99" s="84"/>
     </row>
-    <row r="100" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="94"/>
-      <c r="C100" s="89"/>
+    <row r="100" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B100" s="90"/>
+      <c r="C100" s="101"/>
       <c r="D100" s="4" t="s">
         <v>163</v>
       </c>
@@ -7440,16 +7593,18 @@
       <c r="Q100" s="52">
         <v>0</v>
       </c>
-      <c r="R100" s="83"/>
+      <c r="R100" s="52">
+        <v>0</v>
+      </c>
       <c r="S100" s="83"/>
       <c r="T100" s="83"/>
       <c r="U100" s="83"/>
       <c r="V100" s="83"/>
       <c r="W100" s="84"/>
     </row>
-    <row r="101" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="94"/>
-      <c r="C101" s="89"/>
+    <row r="101" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B101" s="90"/>
+      <c r="C101" s="101"/>
       <c r="D101" s="4" t="s">
         <v>134</v>
       </c>
@@ -7493,16 +7648,18 @@
       <c r="Q101" s="52">
         <v>0</v>
       </c>
-      <c r="R101" s="5"/>
+      <c r="R101" s="52">
+        <v>0</v>
+      </c>
       <c r="S101" s="5"/>
       <c r="T101" s="5"/>
       <c r="U101" s="5"/>
       <c r="V101" s="5"/>
       <c r="W101" s="78"/>
     </row>
-    <row r="102" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="94"/>
-      <c r="C102" s="89" t="s">
+    <row r="102" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B102" s="90"/>
+      <c r="C102" s="101" t="s">
         <v>120</v>
       </c>
       <c r="D102" s="4" t="s">
@@ -7557,9 +7714,9 @@
       <c r="V102" s="73"/>
       <c r="W102" s="63"/>
     </row>
-    <row r="103" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="94"/>
-      <c r="C103" s="89"/>
+    <row r="103" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="90"/>
+      <c r="C103" s="101"/>
       <c r="D103" s="4" t="s">
         <v>132</v>
       </c>
@@ -7603,16 +7760,18 @@
       <c r="Q103" s="52">
         <v>0</v>
       </c>
-      <c r="R103" s="5"/>
+      <c r="R103" s="52">
+        <v>0</v>
+      </c>
       <c r="S103" s="5"/>
       <c r="T103" s="5"/>
       <c r="U103" s="5"/>
       <c r="V103" s="5"/>
       <c r="W103" s="78"/>
     </row>
-    <row r="104" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="94"/>
-      <c r="C104" s="89"/>
+    <row r="104" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B104" s="90"/>
+      <c r="C104" s="101"/>
       <c r="D104" s="4" t="s">
         <v>161</v>
       </c>
@@ -7656,16 +7815,18 @@
       <c r="Q104" s="52">
         <v>0</v>
       </c>
-      <c r="R104" s="5"/>
+      <c r="R104" s="52">
+        <v>0</v>
+      </c>
       <c r="S104" s="5"/>
       <c r="T104" s="5"/>
       <c r="U104" s="5"/>
       <c r="V104" s="5"/>
       <c r="W104" s="78"/>
     </row>
-    <row r="105" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="94"/>
-      <c r="C105" s="89"/>
+    <row r="105" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B105" s="90"/>
+      <c r="C105" s="101"/>
       <c r="D105" s="4" t="s">
         <v>133</v>
       </c>
@@ -7728,9 +7889,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="94"/>
-      <c r="C106" s="89"/>
+    <row r="106" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B106" s="90"/>
+      <c r="C106" s="101"/>
       <c r="D106" s="4" t="s">
         <v>164</v>
       </c>
@@ -7774,16 +7935,18 @@
       <c r="Q106" s="52">
         <v>0</v>
       </c>
-      <c r="R106" s="83"/>
+      <c r="R106" s="52">
+        <v>0</v>
+      </c>
       <c r="S106" s="83"/>
       <c r="T106" s="83"/>
       <c r="U106" s="83"/>
       <c r="V106" s="83"/>
       <c r="W106" s="84"/>
     </row>
-    <row r="107" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="94"/>
-      <c r="C107" s="89"/>
+    <row r="107" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B107" s="90"/>
+      <c r="C107" s="101"/>
       <c r="D107" s="4" t="s">
         <v>163</v>
       </c>
@@ -7827,16 +7990,18 @@
       <c r="Q107" s="52">
         <v>0</v>
       </c>
-      <c r="R107" s="83"/>
+      <c r="R107" s="52">
+        <v>0</v>
+      </c>
       <c r="S107" s="83"/>
       <c r="T107" s="83"/>
       <c r="U107" s="83"/>
       <c r="V107" s="83"/>
       <c r="W107" s="84"/>
     </row>
-    <row r="108" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="94"/>
-      <c r="C108" s="89"/>
+    <row r="108" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B108" s="90"/>
+      <c r="C108" s="101"/>
       <c r="D108" s="4" t="s">
         <v>134</v>
       </c>
@@ -7880,16 +8045,18 @@
       <c r="Q108" s="52">
         <v>0</v>
       </c>
-      <c r="R108" s="5"/>
+      <c r="R108" s="52">
+        <v>0</v>
+      </c>
       <c r="S108" s="5"/>
       <c r="T108" s="5"/>
       <c r="U108" s="5"/>
       <c r="V108" s="5"/>
       <c r="W108" s="78"/>
     </row>
-    <row r="109" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="94"/>
-      <c r="C109" s="89" t="s">
+    <row r="109" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B109" s="90"/>
+      <c r="C109" s="101" t="s">
         <v>121</v>
       </c>
       <c r="D109" s="4" t="s">
@@ -7944,9 +8111,9 @@
       <c r="V109" s="73"/>
       <c r="W109" s="63"/>
     </row>
-    <row r="110" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="94"/>
-      <c r="C110" s="89"/>
+    <row r="110" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B110" s="90"/>
+      <c r="C110" s="101"/>
       <c r="D110" s="4" t="s">
         <v>132</v>
       </c>
@@ -7990,16 +8157,18 @@
       <c r="Q110" s="52">
         <v>0</v>
       </c>
-      <c r="R110" s="5"/>
+      <c r="R110" s="52">
+        <v>0</v>
+      </c>
       <c r="S110" s="5"/>
       <c r="T110" s="5"/>
       <c r="U110" s="5"/>
       <c r="V110" s="5"/>
       <c r="W110" s="78"/>
     </row>
-    <row r="111" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="94"/>
-      <c r="C111" s="89"/>
+    <row r="111" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B111" s="90"/>
+      <c r="C111" s="101"/>
       <c r="D111" s="4" t="s">
         <v>161</v>
       </c>
@@ -8043,16 +8212,18 @@
       <c r="Q111" s="52">
         <v>0</v>
       </c>
-      <c r="R111" s="5"/>
+      <c r="R111" s="52">
+        <v>0</v>
+      </c>
       <c r="S111" s="5"/>
       <c r="T111" s="5"/>
       <c r="U111" s="5"/>
       <c r="V111" s="5"/>
       <c r="W111" s="78"/>
     </row>
-    <row r="112" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="94"/>
-      <c r="C112" s="89"/>
+    <row r="112" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B112" s="90"/>
+      <c r="C112" s="101"/>
       <c r="D112" s="4" t="s">
         <v>133</v>
       </c>
@@ -8115,9 +8286,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="94"/>
-      <c r="C113" s="89"/>
+    <row r="113" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B113" s="90"/>
+      <c r="C113" s="101"/>
       <c r="D113" s="4" t="s">
         <v>164</v>
       </c>
@@ -8161,16 +8332,18 @@
       <c r="Q113" s="52">
         <v>0</v>
       </c>
-      <c r="R113" s="83"/>
+      <c r="R113" s="52">
+        <v>0</v>
+      </c>
       <c r="S113" s="83"/>
       <c r="T113" s="83"/>
       <c r="U113" s="83"/>
       <c r="V113" s="83"/>
       <c r="W113" s="84"/>
     </row>
-    <row r="114" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="94"/>
-      <c r="C114" s="89"/>
+    <row r="114" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B114" s="90"/>
+      <c r="C114" s="101"/>
       <c r="D114" s="4" t="s">
         <v>163</v>
       </c>
@@ -8214,16 +8387,18 @@
       <c r="Q114" s="52">
         <v>0</v>
       </c>
-      <c r="R114" s="83"/>
+      <c r="R114" s="52">
+        <v>0</v>
+      </c>
       <c r="S114" s="83"/>
       <c r="T114" s="83"/>
       <c r="U114" s="83"/>
       <c r="V114" s="83"/>
       <c r="W114" s="84"/>
     </row>
-    <row r="115" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="94"/>
-      <c r="C115" s="89"/>
+    <row r="115" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B115" s="90"/>
+      <c r="C115" s="101"/>
       <c r="D115" s="4" t="s">
         <v>134</v>
       </c>
@@ -8267,16 +8442,18 @@
       <c r="Q115" s="52">
         <v>0</v>
       </c>
-      <c r="R115" s="5"/>
+      <c r="R115" s="52">
+        <v>0</v>
+      </c>
       <c r="S115" s="5"/>
       <c r="T115" s="5"/>
       <c r="U115" s="5"/>
       <c r="V115" s="5"/>
       <c r="W115" s="78"/>
     </row>
-    <row r="116" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="94"/>
-      <c r="C116" s="89" t="s">
+    <row r="116" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B116" s="90"/>
+      <c r="C116" s="101" t="s">
         <v>122</v>
       </c>
       <c r="D116" s="4" t="s">
@@ -8331,9 +8508,9 @@
       <c r="V116" s="73"/>
       <c r="W116" s="63"/>
     </row>
-    <row r="117" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="94"/>
-      <c r="C117" s="89"/>
+    <row r="117" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B117" s="90"/>
+      <c r="C117" s="101"/>
       <c r="D117" s="4" t="s">
         <v>132</v>
       </c>
@@ -8377,16 +8554,18 @@
       <c r="Q117" s="52">
         <v>0</v>
       </c>
-      <c r="R117" s="5"/>
+      <c r="R117" s="52">
+        <v>0</v>
+      </c>
       <c r="S117" s="5"/>
       <c r="T117" s="5"/>
       <c r="U117" s="5"/>
       <c r="V117" s="5"/>
       <c r="W117" s="78"/>
     </row>
-    <row r="118" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="94"/>
-      <c r="C118" s="89"/>
+    <row r="118" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B118" s="90"/>
+      <c r="C118" s="101"/>
       <c r="D118" s="4" t="s">
         <v>161</v>
       </c>
@@ -8430,16 +8609,18 @@
       <c r="Q118" s="52">
         <v>0</v>
       </c>
-      <c r="R118" s="5"/>
+      <c r="R118" s="52">
+        <v>0</v>
+      </c>
       <c r="S118" s="5"/>
       <c r="T118" s="5"/>
       <c r="U118" s="5"/>
       <c r="V118" s="5"/>
       <c r="W118" s="78"/>
     </row>
-    <row r="119" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="94"/>
-      <c r="C119" s="89"/>
+    <row r="119" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B119" s="90"/>
+      <c r="C119" s="101"/>
       <c r="D119" s="4" t="s">
         <v>133</v>
       </c>
@@ -8502,9 +8683,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="94"/>
-      <c r="C120" s="89"/>
+    <row r="120" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B120" s="90"/>
+      <c r="C120" s="101"/>
       <c r="D120" s="4" t="s">
         <v>164</v>
       </c>
@@ -8548,16 +8729,18 @@
       <c r="Q120" s="52">
         <v>0</v>
       </c>
-      <c r="R120" s="83"/>
+      <c r="R120" s="52">
+        <v>0</v>
+      </c>
       <c r="S120" s="83"/>
       <c r="T120" s="83"/>
       <c r="U120" s="83"/>
       <c r="V120" s="83"/>
       <c r="W120" s="84"/>
     </row>
-    <row r="121" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="94"/>
-      <c r="C121" s="89"/>
+    <row r="121" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B121" s="90"/>
+      <c r="C121" s="101"/>
       <c r="D121" s="4" t="s">
         <v>163</v>
       </c>
@@ -8601,16 +8784,18 @@
       <c r="Q121" s="52">
         <v>0</v>
       </c>
-      <c r="R121" s="83"/>
+      <c r="R121" s="52">
+        <v>0</v>
+      </c>
       <c r="S121" s="83"/>
       <c r="T121" s="83"/>
       <c r="U121" s="83"/>
       <c r="V121" s="83"/>
       <c r="W121" s="84"/>
     </row>
-    <row r="122" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="94"/>
-      <c r="C122" s="89"/>
+    <row r="122" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B122" s="90"/>
+      <c r="C122" s="101"/>
       <c r="D122" s="4" t="s">
         <v>134</v>
       </c>
@@ -8654,16 +8839,18 @@
       <c r="Q122" s="52">
         <v>0</v>
       </c>
-      <c r="R122" s="5"/>
+      <c r="R122" s="52">
+        <v>0</v>
+      </c>
       <c r="S122" s="5"/>
       <c r="T122" s="5"/>
       <c r="U122" s="5"/>
       <c r="V122" s="5"/>
       <c r="W122" s="78"/>
     </row>
-    <row r="123" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="94"/>
-      <c r="C123" s="89" t="s">
+    <row r="123" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B123" s="90"/>
+      <c r="C123" s="101" t="s">
         <v>123</v>
       </c>
       <c r="D123" s="4" t="s">
@@ -8718,9 +8905,9 @@
       <c r="V123" s="73"/>
       <c r="W123" s="63"/>
     </row>
-    <row r="124" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="94"/>
-      <c r="C124" s="89"/>
+    <row r="124" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B124" s="90"/>
+      <c r="C124" s="101"/>
       <c r="D124" s="4" t="s">
         <v>132</v>
       </c>
@@ -8764,16 +8951,18 @@
       <c r="Q124" s="52">
         <v>0</v>
       </c>
-      <c r="R124" s="5"/>
+      <c r="R124" s="52">
+        <v>0</v>
+      </c>
       <c r="S124" s="5"/>
       <c r="T124" s="5"/>
       <c r="U124" s="5"/>
       <c r="V124" s="5"/>
       <c r="W124" s="78"/>
     </row>
-    <row r="125" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="94"/>
-      <c r="C125" s="89"/>
+    <row r="125" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B125" s="90"/>
+      <c r="C125" s="101"/>
       <c r="D125" s="4" t="s">
         <v>161</v>
       </c>
@@ -8817,16 +9006,18 @@
       <c r="Q125" s="52">
         <v>0</v>
       </c>
-      <c r="R125" s="5"/>
+      <c r="R125" s="52">
+        <v>0</v>
+      </c>
       <c r="S125" s="5"/>
       <c r="T125" s="5"/>
       <c r="U125" s="5"/>
       <c r="V125" s="5"/>
       <c r="W125" s="78"/>
     </row>
-    <row r="126" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="94"/>
-      <c r="C126" s="89"/>
+    <row r="126" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B126" s="90"/>
+      <c r="C126" s="101"/>
       <c r="D126" s="4" t="s">
         <v>133</v>
       </c>
@@ -8889,9 +9080,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="94"/>
-      <c r="C127" s="89"/>
+    <row r="127" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B127" s="90"/>
+      <c r="C127" s="101"/>
       <c r="D127" s="4" t="s">
         <v>164</v>
       </c>
@@ -8935,16 +9126,18 @@
       <c r="Q127" s="52">
         <v>0</v>
       </c>
-      <c r="R127" s="83"/>
+      <c r="R127" s="52">
+        <v>0</v>
+      </c>
       <c r="S127" s="83"/>
       <c r="T127" s="83"/>
       <c r="U127" s="83"/>
       <c r="V127" s="83"/>
       <c r="W127" s="84"/>
     </row>
-    <row r="128" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="94"/>
-      <c r="C128" s="89"/>
+    <row r="128" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B128" s="90"/>
+      <c r="C128" s="101"/>
       <c r="D128" s="4" t="s">
         <v>163</v>
       </c>
@@ -8988,16 +9181,18 @@
       <c r="Q128" s="52">
         <v>0</v>
       </c>
-      <c r="R128" s="83"/>
+      <c r="R128" s="52">
+        <v>0</v>
+      </c>
       <c r="S128" s="83"/>
       <c r="T128" s="83"/>
       <c r="U128" s="83"/>
       <c r="V128" s="83"/>
       <c r="W128" s="84"/>
     </row>
-    <row r="129" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="94"/>
-      <c r="C129" s="89"/>
+    <row r="129" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B129" s="90"/>
+      <c r="C129" s="101"/>
       <c r="D129" s="4" t="s">
         <v>134</v>
       </c>
@@ -9041,16 +9236,18 @@
       <c r="Q129" s="52">
         <v>0</v>
       </c>
-      <c r="R129" s="5"/>
+      <c r="R129" s="52">
+        <v>0</v>
+      </c>
       <c r="S129" s="5"/>
       <c r="T129" s="5"/>
       <c r="U129" s="5"/>
       <c r="V129" s="5"/>
       <c r="W129" s="78"/>
     </row>
-    <row r="130" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="94"/>
-      <c r="C130" s="89" t="s">
+    <row r="130" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B130" s="90"/>
+      <c r="C130" s="101" t="s">
         <v>124</v>
       </c>
       <c r="D130" s="4" t="s">
@@ -9105,9 +9302,9 @@
       <c r="V130" s="73"/>
       <c r="W130" s="63"/>
     </row>
-    <row r="131" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="94"/>
-      <c r="C131" s="89"/>
+    <row r="131" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B131" s="90"/>
+      <c r="C131" s="101"/>
       <c r="D131" s="4" t="s">
         <v>132</v>
       </c>
@@ -9151,16 +9348,18 @@
       <c r="Q131" s="52">
         <v>0</v>
       </c>
-      <c r="R131" s="5"/>
+      <c r="R131" s="52">
+        <v>0</v>
+      </c>
       <c r="S131" s="5"/>
       <c r="T131" s="5"/>
       <c r="U131" s="5"/>
       <c r="V131" s="5"/>
       <c r="W131" s="78"/>
     </row>
-    <row r="132" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="94"/>
-      <c r="C132" s="89"/>
+    <row r="132" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B132" s="90"/>
+      <c r="C132" s="101"/>
       <c r="D132" s="4" t="s">
         <v>161</v>
       </c>
@@ -9204,16 +9403,18 @@
       <c r="Q132" s="52">
         <v>0</v>
       </c>
-      <c r="R132" s="5"/>
+      <c r="R132" s="52">
+        <v>0</v>
+      </c>
       <c r="S132" s="5"/>
       <c r="T132" s="5"/>
       <c r="U132" s="5"/>
       <c r="V132" s="5"/>
       <c r="W132" s="78"/>
     </row>
-    <row r="133" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="94"/>
-      <c r="C133" s="89"/>
+    <row r="133" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B133" s="90"/>
+      <c r="C133" s="101"/>
       <c r="D133" s="4" t="s">
         <v>133</v>
       </c>
@@ -9276,9 +9477,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="94"/>
-      <c r="C134" s="89"/>
+    <row r="134" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B134" s="90"/>
+      <c r="C134" s="101"/>
       <c r="D134" s="4" t="s">
         <v>164</v>
       </c>
@@ -9322,16 +9523,18 @@
       <c r="Q134" s="52">
         <v>0</v>
       </c>
-      <c r="R134" s="83"/>
+      <c r="R134" s="52">
+        <v>0</v>
+      </c>
       <c r="S134" s="83"/>
       <c r="T134" s="83"/>
       <c r="U134" s="83"/>
       <c r="V134" s="83"/>
       <c r="W134" s="84"/>
     </row>
-    <row r="135" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="94"/>
-      <c r="C135" s="89"/>
+    <row r="135" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B135" s="90"/>
+      <c r="C135" s="101"/>
       <c r="D135" s="4" t="s">
         <v>163</v>
       </c>
@@ -9375,16 +9578,18 @@
       <c r="Q135" s="52">
         <v>0</v>
       </c>
-      <c r="R135" s="83"/>
+      <c r="R135" s="52">
+        <v>0</v>
+      </c>
       <c r="S135" s="83"/>
       <c r="T135" s="83"/>
       <c r="U135" s="83"/>
       <c r="V135" s="83"/>
       <c r="W135" s="84"/>
     </row>
-    <row r="136" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="94"/>
-      <c r="C136" s="89"/>
+    <row r="136" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B136" s="90"/>
+      <c r="C136" s="101"/>
       <c r="D136" s="4" t="s">
         <v>134</v>
       </c>
@@ -9428,16 +9633,18 @@
       <c r="Q136" s="52">
         <v>0</v>
       </c>
-      <c r="R136" s="5"/>
+      <c r="R136" s="52">
+        <v>0</v>
+      </c>
       <c r="S136" s="5"/>
       <c r="T136" s="5"/>
       <c r="U136" s="5"/>
       <c r="V136" s="5"/>
       <c r="W136" s="78"/>
     </row>
-    <row r="137" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="94"/>
-      <c r="C137" s="89" t="s">
+    <row r="137" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B137" s="90"/>
+      <c r="C137" s="101" t="s">
         <v>125</v>
       </c>
       <c r="D137" s="4" t="s">
@@ -9483,16 +9690,18 @@
       <c r="Q137" s="52">
         <v>0</v>
       </c>
-      <c r="R137" s="5"/>
+      <c r="R137" s="52">
+        <v>0</v>
+      </c>
       <c r="S137" s="5"/>
       <c r="T137" s="5"/>
       <c r="U137" s="5"/>
       <c r="V137" s="5"/>
       <c r="W137" s="78"/>
     </row>
-    <row r="138" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="94"/>
-      <c r="C138" s="89"/>
+    <row r="138" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B138" s="90"/>
+      <c r="C138" s="101"/>
       <c r="D138" s="4" t="s">
         <v>132</v>
       </c>
@@ -9536,16 +9745,18 @@
       <c r="Q138" s="52">
         <v>0</v>
       </c>
-      <c r="R138" s="5"/>
+      <c r="R138" s="52">
+        <v>0</v>
+      </c>
       <c r="S138" s="5"/>
       <c r="T138" s="5"/>
       <c r="U138" s="5"/>
       <c r="V138" s="5"/>
       <c r="W138" s="78"/>
     </row>
-    <row r="139" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="94"/>
-      <c r="C139" s="89"/>
+    <row r="139" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B139" s="90"/>
+      <c r="C139" s="101"/>
       <c r="D139" s="4" t="s">
         <v>161</v>
       </c>
@@ -9589,16 +9800,18 @@
       <c r="Q139" s="52">
         <v>0</v>
       </c>
-      <c r="R139" s="5"/>
+      <c r="R139" s="52">
+        <v>0</v>
+      </c>
       <c r="S139" s="5"/>
       <c r="T139" s="5"/>
       <c r="U139" s="5"/>
       <c r="V139" s="5"/>
       <c r="W139" s="78"/>
     </row>
-    <row r="140" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="94"/>
-      <c r="C140" s="89"/>
+    <row r="140" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B140" s="90"/>
+      <c r="C140" s="101"/>
       <c r="D140" s="4" t="s">
         <v>133</v>
       </c>
@@ -9661,9 +9874,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="94"/>
-      <c r="C141" s="89"/>
+    <row r="141" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B141" s="90"/>
+      <c r="C141" s="101"/>
       <c r="D141" s="4" t="s">
         <v>164</v>
       </c>
@@ -9707,16 +9920,18 @@
       <c r="Q141" s="52">
         <v>0</v>
       </c>
-      <c r="R141" s="83"/>
+      <c r="R141" s="52">
+        <v>0</v>
+      </c>
       <c r="S141" s="83"/>
       <c r="T141" s="83"/>
       <c r="U141" s="83"/>
       <c r="V141" s="83"/>
       <c r="W141" s="84"/>
     </row>
-    <row r="142" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="94"/>
-      <c r="C142" s="89"/>
+    <row r="142" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B142" s="90"/>
+      <c r="C142" s="101"/>
       <c r="D142" s="4" t="s">
         <v>163</v>
       </c>
@@ -9760,16 +9975,18 @@
       <c r="Q142" s="52">
         <v>0</v>
       </c>
-      <c r="R142" s="83"/>
+      <c r="R142" s="52">
+        <v>0</v>
+      </c>
       <c r="S142" s="83"/>
       <c r="T142" s="83"/>
       <c r="U142" s="83"/>
       <c r="V142" s="83"/>
       <c r="W142" s="84"/>
     </row>
-    <row r="143" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="94"/>
-      <c r="C143" s="89"/>
+    <row r="143" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B143" s="90"/>
+      <c r="C143" s="101"/>
       <c r="D143" s="4" t="s">
         <v>134</v>
       </c>
@@ -9813,16 +10030,18 @@
       <c r="Q143" s="52">
         <v>0</v>
       </c>
-      <c r="R143" s="5"/>
+      <c r="R143" s="52">
+        <v>0</v>
+      </c>
       <c r="S143" s="5"/>
       <c r="T143" s="5"/>
       <c r="U143" s="5"/>
       <c r="V143" s="5"/>
       <c r="W143" s="78"/>
     </row>
-    <row r="144" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="94"/>
-      <c r="C144" s="89" t="s">
+    <row r="144" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B144" s="90"/>
+      <c r="C144" s="101" t="s">
         <v>126</v>
       </c>
       <c r="D144" s="4" t="s">
@@ -9868,16 +10087,18 @@
       <c r="Q144" s="52">
         <v>0</v>
       </c>
-      <c r="R144" s="5"/>
+      <c r="R144" s="52">
+        <v>0</v>
+      </c>
       <c r="S144" s="5"/>
       <c r="T144" s="5"/>
       <c r="U144" s="5"/>
       <c r="V144" s="5"/>
       <c r="W144" s="78"/>
     </row>
-    <row r="145" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="94"/>
-      <c r="C145" s="89"/>
+    <row r="145" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B145" s="90"/>
+      <c r="C145" s="101"/>
       <c r="D145" s="4" t="s">
         <v>132</v>
       </c>
@@ -9921,16 +10142,18 @@
       <c r="Q145" s="52">
         <v>0</v>
       </c>
-      <c r="R145" s="5"/>
+      <c r="R145" s="52">
+        <v>0</v>
+      </c>
       <c r="S145" s="5"/>
       <c r="T145" s="5"/>
       <c r="U145" s="5"/>
       <c r="V145" s="5"/>
       <c r="W145" s="78"/>
     </row>
-    <row r="146" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="94"/>
-      <c r="C146" s="89"/>
+    <row r="146" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B146" s="90"/>
+      <c r="C146" s="101"/>
       <c r="D146" s="4" t="s">
         <v>161</v>
       </c>
@@ -9974,16 +10197,18 @@
       <c r="Q146" s="52">
         <v>0</v>
       </c>
-      <c r="R146" s="5"/>
+      <c r="R146" s="52">
+        <v>0</v>
+      </c>
       <c r="S146" s="5"/>
       <c r="T146" s="5"/>
       <c r="U146" s="5"/>
       <c r="V146" s="5"/>
       <c r="W146" s="78"/>
     </row>
-    <row r="147" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="94"/>
-      <c r="C147" s="89"/>
+    <row r="147" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B147" s="90"/>
+      <c r="C147" s="101"/>
       <c r="D147" s="4" t="s">
         <v>133</v>
       </c>
@@ -10046,9 +10271,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="94"/>
-      <c r="C148" s="89"/>
+    <row r="148" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B148" s="90"/>
+      <c r="C148" s="101"/>
       <c r="D148" s="4" t="s">
         <v>164</v>
       </c>
@@ -10092,16 +10317,18 @@
       <c r="Q148" s="52">
         <v>0</v>
       </c>
-      <c r="R148" s="83"/>
+      <c r="R148" s="52">
+        <v>0</v>
+      </c>
       <c r="S148" s="83"/>
       <c r="T148" s="83"/>
       <c r="U148" s="83"/>
       <c r="V148" s="83"/>
       <c r="W148" s="84"/>
     </row>
-    <row r="149" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="94"/>
-      <c r="C149" s="89"/>
+    <row r="149" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B149" s="90"/>
+      <c r="C149" s="101"/>
       <c r="D149" s="4" t="s">
         <v>163</v>
       </c>
@@ -10145,16 +10372,18 @@
       <c r="Q149" s="52">
         <v>0</v>
       </c>
-      <c r="R149" s="83"/>
+      <c r="R149" s="52">
+        <v>0</v>
+      </c>
       <c r="S149" s="83"/>
       <c r="T149" s="83"/>
       <c r="U149" s="83"/>
       <c r="V149" s="83"/>
       <c r="W149" s="84"/>
     </row>
-    <row r="150" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="94"/>
-      <c r="C150" s="89"/>
+    <row r="150" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B150" s="90"/>
+      <c r="C150" s="101"/>
       <c r="D150" s="4" t="s">
         <v>134</v>
       </c>
@@ -10198,16 +10427,18 @@
       <c r="Q150" s="52">
         <v>0</v>
       </c>
-      <c r="R150" s="5"/>
+      <c r="R150" s="52">
+        <v>0</v>
+      </c>
       <c r="S150" s="5"/>
       <c r="T150" s="5"/>
       <c r="U150" s="5"/>
       <c r="V150" s="5"/>
       <c r="W150" s="78"/>
     </row>
-    <row r="151" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="94"/>
-      <c r="C151" s="89" t="s">
+    <row r="151" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B151" s="90"/>
+      <c r="C151" s="101" t="s">
         <v>127</v>
       </c>
       <c r="D151" s="4" t="s">
@@ -10253,16 +10484,18 @@
       <c r="Q151" s="52">
         <v>0</v>
       </c>
-      <c r="R151" s="5"/>
+      <c r="R151" s="52">
+        <v>0</v>
+      </c>
       <c r="S151" s="5"/>
       <c r="T151" s="5"/>
       <c r="U151" s="5"/>
       <c r="V151" s="5"/>
       <c r="W151" s="78"/>
     </row>
-    <row r="152" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="94"/>
-      <c r="C152" s="89"/>
+    <row r="152" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B152" s="90"/>
+      <c r="C152" s="101"/>
       <c r="D152" s="4" t="s">
         <v>132</v>
       </c>
@@ -10306,16 +10539,18 @@
       <c r="Q152" s="52">
         <v>0</v>
       </c>
-      <c r="R152" s="5"/>
+      <c r="R152" s="52">
+        <v>0</v>
+      </c>
       <c r="S152" s="5"/>
       <c r="T152" s="5"/>
       <c r="U152" s="5"/>
       <c r="V152" s="5"/>
       <c r="W152" s="78"/>
     </row>
-    <row r="153" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="94"/>
-      <c r="C153" s="89"/>
+    <row r="153" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B153" s="90"/>
+      <c r="C153" s="101"/>
       <c r="D153" s="4" t="s">
         <v>161</v>
       </c>
@@ -10359,16 +10594,18 @@
       <c r="Q153" s="52">
         <v>0</v>
       </c>
-      <c r="R153" s="5"/>
+      <c r="R153" s="52">
+        <v>0</v>
+      </c>
       <c r="S153" s="5"/>
       <c r="T153" s="5"/>
       <c r="U153" s="5"/>
       <c r="V153" s="5"/>
       <c r="W153" s="78"/>
     </row>
-    <row r="154" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="94"/>
-      <c r="C154" s="89"/>
+    <row r="154" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B154" s="90"/>
+      <c r="C154" s="101"/>
       <c r="D154" s="4" t="s">
         <v>133</v>
       </c>
@@ -10431,9 +10668,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="94"/>
-      <c r="C155" s="89"/>
+    <row r="155" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B155" s="90"/>
+      <c r="C155" s="101"/>
       <c r="D155" s="4" t="s">
         <v>164</v>
       </c>
@@ -10477,16 +10714,18 @@
       <c r="Q155" s="52">
         <v>0</v>
       </c>
-      <c r="R155" s="83"/>
+      <c r="R155" s="52">
+        <v>0</v>
+      </c>
       <c r="S155" s="83"/>
       <c r="T155" s="83"/>
       <c r="U155" s="83"/>
       <c r="V155" s="83"/>
       <c r="W155" s="84"/>
     </row>
-    <row r="156" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="94"/>
-      <c r="C156" s="89"/>
+    <row r="156" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B156" s="90"/>
+      <c r="C156" s="101"/>
       <c r="D156" s="4" t="s">
         <v>163</v>
       </c>
@@ -10530,16 +10769,18 @@
       <c r="Q156" s="52">
         <v>0</v>
       </c>
-      <c r="R156" s="83"/>
+      <c r="R156" s="52">
+        <v>0</v>
+      </c>
       <c r="S156" s="83"/>
       <c r="T156" s="83"/>
       <c r="U156" s="83"/>
       <c r="V156" s="83"/>
       <c r="W156" s="84"/>
     </row>
-    <row r="157" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="94"/>
-      <c r="C157" s="89"/>
+    <row r="157" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B157" s="90"/>
+      <c r="C157" s="101"/>
       <c r="D157" s="4" t="s">
         <v>134</v>
       </c>
@@ -10583,16 +10824,18 @@
       <c r="Q157" s="52">
         <v>0</v>
       </c>
-      <c r="R157" s="5"/>
+      <c r="R157" s="52">
+        <v>0</v>
+      </c>
       <c r="S157" s="5"/>
       <c r="T157" s="5"/>
       <c r="U157" s="5"/>
       <c r="V157" s="5"/>
       <c r="W157" s="78"/>
     </row>
-    <row r="158" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="94"/>
-      <c r="C158" s="89" t="s">
+    <row r="158" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B158" s="90"/>
+      <c r="C158" s="101" t="s">
         <v>128</v>
       </c>
       <c r="D158" s="4" t="s">
@@ -10638,16 +10881,18 @@
       <c r="Q158" s="52">
         <v>0</v>
       </c>
-      <c r="R158" s="5"/>
+      <c r="R158" s="52">
+        <v>0</v>
+      </c>
       <c r="S158" s="5"/>
       <c r="T158" s="5"/>
       <c r="U158" s="5"/>
       <c r="V158" s="5"/>
       <c r="W158" s="78"/>
     </row>
-    <row r="159" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="94"/>
-      <c r="C159" s="89"/>
+    <row r="159" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B159" s="90"/>
+      <c r="C159" s="101"/>
       <c r="D159" s="4" t="s">
         <v>132</v>
       </c>
@@ -10691,16 +10936,18 @@
       <c r="Q159" s="52">
         <v>0</v>
       </c>
-      <c r="R159" s="5"/>
+      <c r="R159" s="52">
+        <v>0</v>
+      </c>
       <c r="S159" s="5"/>
       <c r="T159" s="5"/>
       <c r="U159" s="5"/>
       <c r="V159" s="5"/>
       <c r="W159" s="78"/>
     </row>
-    <row r="160" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="94"/>
-      <c r="C160" s="89"/>
+    <row r="160" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B160" s="90"/>
+      <c r="C160" s="101"/>
       <c r="D160" s="4" t="s">
         <v>161</v>
       </c>
@@ -10744,16 +10991,18 @@
       <c r="Q160" s="52">
         <v>0</v>
       </c>
-      <c r="R160" s="5"/>
+      <c r="R160" s="52">
+        <v>0</v>
+      </c>
       <c r="S160" s="5"/>
       <c r="T160" s="5"/>
       <c r="U160" s="5"/>
       <c r="V160" s="5"/>
       <c r="W160" s="78"/>
     </row>
-    <row r="161" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="94"/>
-      <c r="C161" s="89"/>
+    <row r="161" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B161" s="90"/>
+      <c r="C161" s="101"/>
       <c r="D161" s="4" t="s">
         <v>133</v>
       </c>
@@ -10816,9 +11065,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="94"/>
-      <c r="C162" s="89"/>
+    <row r="162" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B162" s="90"/>
+      <c r="C162" s="101"/>
       <c r="D162" s="4" t="s">
         <v>164</v>
       </c>
@@ -10862,16 +11111,18 @@
       <c r="Q162" s="52">
         <v>0</v>
       </c>
-      <c r="R162" s="83"/>
+      <c r="R162" s="52">
+        <v>0</v>
+      </c>
       <c r="S162" s="83"/>
       <c r="T162" s="83"/>
       <c r="U162" s="83"/>
       <c r="V162" s="83"/>
       <c r="W162" s="84"/>
     </row>
-    <row r="163" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="94"/>
-      <c r="C163" s="89"/>
+    <row r="163" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B163" s="90"/>
+      <c r="C163" s="101"/>
       <c r="D163" s="4" t="s">
         <v>163</v>
       </c>
@@ -10915,16 +11166,18 @@
       <c r="Q163" s="52">
         <v>0</v>
       </c>
-      <c r="R163" s="83"/>
+      <c r="R163" s="52">
+        <v>0</v>
+      </c>
       <c r="S163" s="83"/>
       <c r="T163" s="83"/>
       <c r="U163" s="83"/>
       <c r="V163" s="83"/>
       <c r="W163" s="84"/>
     </row>
-    <row r="164" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="94"/>
-      <c r="C164" s="89"/>
+    <row r="164" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B164" s="90"/>
+      <c r="C164" s="101"/>
       <c r="D164" s="4" t="s">
         <v>134</v>
       </c>
@@ -10968,16 +11221,18 @@
       <c r="Q164" s="52">
         <v>0</v>
       </c>
-      <c r="R164" s="5"/>
+      <c r="R164" s="52">
+        <v>0</v>
+      </c>
       <c r="S164" s="5"/>
       <c r="T164" s="5"/>
       <c r="U164" s="5"/>
       <c r="V164" s="5"/>
       <c r="W164" s="78"/>
     </row>
-    <row r="165" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="94"/>
-      <c r="C165" s="89" t="s">
+    <row r="165" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B165" s="90"/>
+      <c r="C165" s="101" t="s">
         <v>129</v>
       </c>
       <c r="D165" s="4" t="s">
@@ -11023,16 +11278,18 @@
       <c r="Q165" s="52">
         <v>0</v>
       </c>
-      <c r="R165" s="5"/>
+      <c r="R165" s="52">
+        <v>0</v>
+      </c>
       <c r="S165" s="5"/>
       <c r="T165" s="5"/>
       <c r="U165" s="5"/>
       <c r="V165" s="5"/>
       <c r="W165" s="78"/>
     </row>
-    <row r="166" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B166" s="94"/>
-      <c r="C166" s="89"/>
+    <row r="166" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B166" s="90"/>
+      <c r="C166" s="101"/>
       <c r="D166" s="4" t="s">
         <v>132</v>
       </c>
@@ -11076,16 +11333,18 @@
       <c r="Q166" s="52">
         <v>0</v>
       </c>
-      <c r="R166" s="5"/>
+      <c r="R166" s="52">
+        <v>0</v>
+      </c>
       <c r="S166" s="5"/>
       <c r="T166" s="5"/>
       <c r="U166" s="5"/>
       <c r="V166" s="5"/>
       <c r="W166" s="78"/>
     </row>
-    <row r="167" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B167" s="94"/>
-      <c r="C167" s="89"/>
+    <row r="167" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B167" s="90"/>
+      <c r="C167" s="101"/>
       <c r="D167" s="4" t="s">
         <v>161</v>
       </c>
@@ -11129,16 +11388,18 @@
       <c r="Q167" s="52">
         <v>0</v>
       </c>
-      <c r="R167" s="5"/>
+      <c r="R167" s="52">
+        <v>0</v>
+      </c>
       <c r="S167" s="5"/>
       <c r="T167" s="5"/>
       <c r="U167" s="5"/>
       <c r="V167" s="5"/>
       <c r="W167" s="78"/>
     </row>
-    <row r="168" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B168" s="94"/>
-      <c r="C168" s="89"/>
+    <row r="168" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B168" s="90"/>
+      <c r="C168" s="101"/>
       <c r="D168" s="4" t="s">
         <v>133</v>
       </c>
@@ -11201,9 +11462,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B169" s="94"/>
-      <c r="C169" s="89"/>
+    <row r="169" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B169" s="90"/>
+      <c r="C169" s="101"/>
       <c r="D169" s="4" t="s">
         <v>164</v>
       </c>
@@ -11247,16 +11508,18 @@
       <c r="Q169" s="52">
         <v>0</v>
       </c>
-      <c r="R169" s="83"/>
+      <c r="R169" s="52">
+        <v>0</v>
+      </c>
       <c r="S169" s="83"/>
       <c r="T169" s="83"/>
       <c r="U169" s="83"/>
       <c r="V169" s="83"/>
       <c r="W169" s="84"/>
     </row>
-    <row r="170" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B170" s="94"/>
-      <c r="C170" s="89"/>
+    <row r="170" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B170" s="90"/>
+      <c r="C170" s="101"/>
       <c r="D170" s="4" t="s">
         <v>163</v>
       </c>
@@ -11300,16 +11563,18 @@
       <c r="Q170" s="52">
         <v>0</v>
       </c>
-      <c r="R170" s="83"/>
+      <c r="R170" s="52">
+        <v>0</v>
+      </c>
       <c r="S170" s="83"/>
       <c r="T170" s="83"/>
       <c r="U170" s="83"/>
       <c r="V170" s="83"/>
       <c r="W170" s="84"/>
     </row>
-    <row r="171" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B171" s="94"/>
-      <c r="C171" s="89"/>
+    <row r="171" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B171" s="90"/>
+      <c r="C171" s="101"/>
       <c r="D171" s="4" t="s">
         <v>134</v>
       </c>
@@ -11353,16 +11618,18 @@
       <c r="Q171" s="52">
         <v>0</v>
       </c>
-      <c r="R171" s="5"/>
+      <c r="R171" s="52">
+        <v>0</v>
+      </c>
       <c r="S171" s="5"/>
       <c r="T171" s="5"/>
       <c r="U171" s="5"/>
       <c r="V171" s="5"/>
       <c r="W171" s="78"/>
     </row>
-    <row r="172" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="94"/>
-      <c r="C172" s="89" t="s">
+    <row r="172" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B172" s="90"/>
+      <c r="C172" s="101" t="s">
         <v>130</v>
       </c>
       <c r="D172" s="4" t="s">
@@ -11408,16 +11675,18 @@
       <c r="Q172" s="52">
         <v>0</v>
       </c>
-      <c r="R172" s="5"/>
+      <c r="R172" s="52">
+        <v>0</v>
+      </c>
       <c r="S172" s="5"/>
       <c r="T172" s="5"/>
       <c r="U172" s="5"/>
       <c r="V172" s="5"/>
       <c r="W172" s="78"/>
     </row>
-    <row r="173" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B173" s="94"/>
-      <c r="C173" s="89"/>
+    <row r="173" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B173" s="90"/>
+      <c r="C173" s="101"/>
       <c r="D173" s="4" t="s">
         <v>132</v>
       </c>
@@ -11461,16 +11730,18 @@
       <c r="Q173" s="52">
         <v>0</v>
       </c>
-      <c r="R173" s="5"/>
+      <c r="R173" s="52">
+        <v>0</v>
+      </c>
       <c r="S173" s="5"/>
       <c r="T173" s="5"/>
       <c r="U173" s="5"/>
       <c r="V173" s="5"/>
       <c r="W173" s="78"/>
     </row>
-    <row r="174" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="94"/>
-      <c r="C174" s="89"/>
+    <row r="174" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B174" s="90"/>
+      <c r="C174" s="101"/>
       <c r="D174" s="4" t="s">
         <v>161</v>
       </c>
@@ -11514,16 +11785,18 @@
       <c r="Q174" s="52">
         <v>0</v>
       </c>
-      <c r="R174" s="5"/>
+      <c r="R174" s="52">
+        <v>0</v>
+      </c>
       <c r="S174" s="5"/>
       <c r="T174" s="5"/>
       <c r="U174" s="5"/>
       <c r="V174" s="5"/>
       <c r="W174" s="78"/>
     </row>
-    <row r="175" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="94"/>
-      <c r="C175" s="89"/>
+    <row r="175" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B175" s="90"/>
+      <c r="C175" s="101"/>
       <c r="D175" s="4" t="s">
         <v>133</v>
       </c>
@@ -11586,9 +11859,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="112"/>
-      <c r="C176" s="116"/>
+    <row r="176" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B176" s="97"/>
+      <c r="C176" s="104"/>
       <c r="D176" s="4" t="s">
         <v>164</v>
       </c>
@@ -11632,16 +11905,18 @@
       <c r="Q176" s="54">
         <v>0</v>
       </c>
-      <c r="R176" s="85"/>
+      <c r="R176" s="54">
+        <v>0</v>
+      </c>
       <c r="S176" s="85"/>
       <c r="T176" s="85"/>
       <c r="U176" s="85"/>
       <c r="V176" s="85"/>
       <c r="W176" s="86"/>
     </row>
-    <row r="177" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B177" s="112"/>
-      <c r="C177" s="116"/>
+    <row r="177" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B177" s="97"/>
+      <c r="C177" s="104"/>
       <c r="D177" s="4" t="s">
         <v>163</v>
       </c>
@@ -11685,16 +11960,18 @@
       <c r="Q177" s="54">
         <v>0</v>
       </c>
-      <c r="R177" s="85"/>
+      <c r="R177" s="54">
+        <v>0</v>
+      </c>
       <c r="S177" s="85"/>
       <c r="T177" s="85"/>
       <c r="U177" s="85"/>
       <c r="V177" s="85"/>
       <c r="W177" s="86"/>
     </row>
-    <row r="178" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B178" s="95"/>
-      <c r="C178" s="117"/>
+    <row r="178" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B178" s="91"/>
+      <c r="C178" s="105"/>
       <c r="D178" s="17" t="s">
         <v>134</v>
       </c>
@@ -11738,15 +12015,17 @@
       <c r="Q178" s="76">
         <v>0</v>
       </c>
-      <c r="R178" s="31"/>
+      <c r="R178" s="76">
+        <v>0</v>
+      </c>
       <c r="S178" s="31"/>
       <c r="T178" s="31"/>
       <c r="U178" s="31"/>
       <c r="V178" s="31"/>
       <c r="W178" s="79"/>
     </row>
-    <row r="179" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B179" s="93" t="s">
+    <row r="179" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B179" s="89" t="s">
         <v>83</v>
       </c>
       <c r="C179" s="60" t="s">
@@ -11793,15 +12072,17 @@
       <c r="Q179" s="51">
         <v>0</v>
       </c>
-      <c r="R179" s="34"/>
+      <c r="R179" s="51">
+        <v>0</v>
+      </c>
       <c r="S179" s="34"/>
       <c r="T179" s="34"/>
       <c r="U179" s="34"/>
       <c r="V179" s="34"/>
       <c r="W179" s="82"/>
     </row>
-    <row r="180" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B180" s="94"/>
+    <row r="180" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B180" s="90"/>
       <c r="C180" s="22" t="s">
         <v>89</v>
       </c>
@@ -11846,15 +12127,17 @@
       <c r="Q180" s="52">
         <v>0</v>
       </c>
-      <c r="R180" s="5"/>
+      <c r="R180" s="52">
+        <v>0</v>
+      </c>
       <c r="S180" s="5"/>
       <c r="T180" s="5"/>
       <c r="U180" s="5"/>
       <c r="V180" s="5"/>
       <c r="W180" s="78"/>
     </row>
-    <row r="181" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B181" s="94"/>
+    <row r="181" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B181" s="90"/>
       <c r="C181" s="22" t="s">
         <v>90</v>
       </c>
@@ -11899,15 +12182,17 @@
       <c r="Q181" s="52">
         <v>0</v>
       </c>
-      <c r="R181" s="5"/>
+      <c r="R181" s="52">
+        <v>0</v>
+      </c>
       <c r="S181" s="5"/>
       <c r="T181" s="5"/>
       <c r="U181" s="5"/>
       <c r="V181" s="5"/>
       <c r="W181" s="78"/>
     </row>
-    <row r="182" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B182" s="94"/>
+    <row r="182" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B182" s="90"/>
       <c r="C182" s="22" t="s">
         <v>91</v>
       </c>
@@ -11952,15 +12237,17 @@
       <c r="Q182" s="52">
         <v>0</v>
       </c>
-      <c r="R182" s="5"/>
+      <c r="R182" s="52">
+        <v>0</v>
+      </c>
       <c r="S182" s="5"/>
       <c r="T182" s="5"/>
       <c r="U182" s="5"/>
       <c r="V182" s="5"/>
       <c r="W182" s="78"/>
     </row>
-    <row r="183" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B183" s="94"/>
+    <row r="183" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B183" s="90"/>
       <c r="C183" s="22" t="s">
         <v>141</v>
       </c>
@@ -12005,15 +12292,17 @@
       <c r="Q183" s="52">
         <v>0</v>
       </c>
-      <c r="R183" s="5"/>
+      <c r="R183" s="52">
+        <v>0</v>
+      </c>
       <c r="S183" s="5"/>
       <c r="T183" s="5"/>
       <c r="U183" s="5"/>
       <c r="V183" s="5"/>
       <c r="W183" s="78"/>
     </row>
-    <row r="184" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B184" s="94"/>
+    <row r="184" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B184" s="90"/>
       <c r="C184" s="22" t="s">
         <v>138</v>
       </c>
@@ -12058,15 +12347,17 @@
       <c r="Q184" s="52">
         <v>0</v>
       </c>
-      <c r="R184" s="5"/>
+      <c r="R184" s="52">
+        <v>0</v>
+      </c>
       <c r="S184" s="5"/>
       <c r="T184" s="5"/>
       <c r="U184" s="5"/>
       <c r="V184" s="5"/>
       <c r="W184" s="78"/>
     </row>
-    <row r="185" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="94"/>
+    <row r="185" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B185" s="90"/>
       <c r="C185" s="22" t="s">
         <v>140</v>
       </c>
@@ -12111,15 +12402,17 @@
       <c r="Q185" s="52">
         <v>0</v>
       </c>
-      <c r="R185" s="5"/>
+      <c r="R185" s="52">
+        <v>0</v>
+      </c>
       <c r="S185" s="5"/>
       <c r="T185" s="5"/>
       <c r="U185" s="5"/>
       <c r="V185" s="5"/>
       <c r="W185" s="78"/>
     </row>
-    <row r="186" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="94"/>
+    <row r="186" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B186" s="90"/>
       <c r="C186" s="22" t="s">
         <v>139</v>
       </c>
@@ -12164,15 +12457,17 @@
       <c r="Q186" s="52">
         <v>0</v>
       </c>
-      <c r="R186" s="5"/>
+      <c r="R186" s="52">
+        <v>0</v>
+      </c>
       <c r="S186" s="5"/>
       <c r="T186" s="5"/>
       <c r="U186" s="5"/>
       <c r="V186" s="5"/>
       <c r="W186" s="78"/>
     </row>
-    <row r="187" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B187" s="94"/>
+    <row r="187" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B187" s="90"/>
       <c r="C187" s="22" t="s">
         <v>92</v>
       </c>
@@ -12236,8 +12531,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B188" s="94"/>
+    <row r="188" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B188" s="90"/>
       <c r="C188" s="22" t="s">
         <v>93</v>
       </c>
@@ -12301,8 +12596,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B189" s="94"/>
+    <row r="189" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B189" s="90"/>
       <c r="C189" s="22" t="s">
         <v>94</v>
       </c>
@@ -12366,8 +12661,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B190" s="94"/>
+    <row r="190" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B190" s="90"/>
       <c r="C190" s="22" t="s">
         <v>98</v>
       </c>
@@ -12412,15 +12707,17 @@
       <c r="Q190" s="52">
         <v>0</v>
       </c>
-      <c r="R190" s="5"/>
+      <c r="R190" s="52">
+        <v>0</v>
+      </c>
       <c r="S190" s="5"/>
       <c r="T190" s="5"/>
       <c r="U190" s="5"/>
       <c r="V190" s="5"/>
       <c r="W190" s="78"/>
     </row>
-    <row r="191" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B191" s="95"/>
+    <row r="191" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B191" s="91"/>
       <c r="C191" s="43" t="s">
         <v>99</v>
       </c>
@@ -12465,15 +12762,17 @@
       <c r="Q191" s="53">
         <v>0</v>
       </c>
-      <c r="R191" s="31"/>
+      <c r="R191" s="53">
+        <v>0</v>
+      </c>
       <c r="S191" s="31"/>
       <c r="T191" s="31"/>
       <c r="U191" s="31"/>
       <c r="V191" s="31"/>
       <c r="W191" s="79"/>
     </row>
-    <row r="192" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B192" s="93" t="s">
+    <row r="192" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B192" s="89" t="s">
         <v>142</v>
       </c>
       <c r="C192" s="42" t="s">
@@ -12520,15 +12819,17 @@
       <c r="Q192" s="51">
         <v>0</v>
       </c>
-      <c r="R192" s="34"/>
+      <c r="R192" s="51">
+        <v>0</v>
+      </c>
       <c r="S192" s="34"/>
       <c r="T192" s="34"/>
       <c r="U192" s="34"/>
       <c r="V192" s="34"/>
       <c r="W192" s="82"/>
     </row>
-    <row r="193" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="94"/>
+    <row r="193" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B193" s="90"/>
       <c r="C193" s="41" t="s">
         <v>143</v>
       </c>
@@ -12573,15 +12874,17 @@
       <c r="Q193" s="52">
         <v>0</v>
       </c>
-      <c r="R193" s="5"/>
+      <c r="R193" s="52">
+        <v>0</v>
+      </c>
       <c r="S193" s="5"/>
       <c r="T193" s="5"/>
       <c r="U193" s="5"/>
       <c r="V193" s="5"/>
       <c r="W193" s="78"/>
     </row>
-    <row r="194" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B194" s="95"/>
+    <row r="194" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B194" s="91"/>
       <c r="C194" s="43" t="s">
         <v>144</v>
       </c>
@@ -12626,15 +12929,17 @@
       <c r="Q194" s="53">
         <v>0</v>
       </c>
-      <c r="R194" s="31"/>
+      <c r="R194" s="53">
+        <v>0</v>
+      </c>
       <c r="S194" s="31"/>
       <c r="T194" s="31"/>
       <c r="U194" s="31"/>
       <c r="V194" s="31"/>
       <c r="W194" s="79"/>
     </row>
-    <row r="195" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="93" t="s">
+    <row r="195" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B195" s="89" t="s">
         <v>147</v>
       </c>
       <c r="C195" s="42" t="s">
@@ -12681,15 +12986,17 @@
       <c r="Q195" s="51">
         <v>0</v>
       </c>
-      <c r="R195" s="34"/>
+      <c r="R195" s="51">
+        <v>0</v>
+      </c>
       <c r="S195" s="34"/>
       <c r="T195" s="34"/>
       <c r="U195" s="34"/>
       <c r="V195" s="34"/>
       <c r="W195" s="82"/>
     </row>
-    <row r="196" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="94"/>
+    <row r="196" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B196" s="90"/>
       <c r="C196" s="41" t="s">
         <v>149</v>
       </c>
@@ -12734,15 +13041,17 @@
       <c r="Q196" s="52">
         <v>0</v>
       </c>
-      <c r="R196" s="5"/>
+      <c r="R196" s="52">
+        <v>0</v>
+      </c>
       <c r="S196" s="5"/>
       <c r="T196" s="5"/>
       <c r="U196" s="5"/>
       <c r="V196" s="5"/>
       <c r="W196" s="78"/>
     </row>
-    <row r="197" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="94"/>
+    <row r="197" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B197" s="90"/>
       <c r="C197" s="41" t="s">
         <v>150</v>
       </c>
@@ -12787,15 +13096,17 @@
       <c r="Q197" s="52">
         <v>0</v>
       </c>
-      <c r="R197" s="5"/>
+      <c r="R197" s="52">
+        <v>0</v>
+      </c>
       <c r="S197" s="5"/>
       <c r="T197" s="5"/>
       <c r="U197" s="5"/>
       <c r="V197" s="5"/>
       <c r="W197" s="78"/>
     </row>
-    <row r="198" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B198" s="94"/>
+    <row r="198" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B198" s="90"/>
       <c r="C198" s="41" t="s">
         <v>151</v>
       </c>
@@ -12840,15 +13151,17 @@
       <c r="Q198" s="52">
         <v>0</v>
       </c>
-      <c r="R198" s="5"/>
+      <c r="R198" s="52">
+        <v>0</v>
+      </c>
       <c r="S198" s="5"/>
       <c r="T198" s="5"/>
       <c r="U198" s="5"/>
       <c r="V198" s="5"/>
       <c r="W198" s="78"/>
     </row>
-    <row r="199" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B199" s="94"/>
+    <row r="199" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B199" s="90"/>
       <c r="C199" s="41" t="s">
         <v>152</v>
       </c>
@@ -12893,15 +13206,17 @@
       <c r="Q199" s="62">
         <v>0</v>
       </c>
-      <c r="R199" s="5"/>
+      <c r="R199" s="62">
+        <v>0</v>
+      </c>
       <c r="S199" s="5"/>
       <c r="T199" s="5"/>
       <c r="U199" s="5"/>
       <c r="V199" s="5"/>
       <c r="W199" s="78"/>
     </row>
-    <row r="200" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B200" s="94"/>
+    <row r="200" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B200" s="90"/>
       <c r="C200" s="41" t="s">
         <v>153</v>
       </c>
@@ -12946,15 +13261,17 @@
       <c r="Q200" s="52">
         <v>0</v>
       </c>
-      <c r="R200" s="5"/>
+      <c r="R200" s="52">
+        <v>0</v>
+      </c>
       <c r="S200" s="5"/>
       <c r="T200" s="5"/>
       <c r="U200" s="5"/>
       <c r="V200" s="5"/>
       <c r="W200" s="78"/>
     </row>
-    <row r="201" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B201" s="95"/>
+    <row r="201" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B201" s="91"/>
       <c r="C201" s="43" t="s">
         <v>154</v>
       </c>
@@ -12999,15 +13316,17 @@
       <c r="Q201" s="53">
         <v>0</v>
       </c>
-      <c r="R201" s="31"/>
+      <c r="R201" s="53">
+        <v>0</v>
+      </c>
       <c r="S201" s="31"/>
       <c r="T201" s="31"/>
       <c r="U201" s="31"/>
       <c r="V201" s="31"/>
       <c r="W201" s="79"/>
     </row>
-    <row r="202" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B202" s="93" t="s">
+    <row r="202" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B202" s="89" t="s">
         <v>18</v>
       </c>
       <c r="C202" s="36" t="s">
@@ -13054,15 +13373,17 @@
       <c r="Q202" s="51">
         <v>0</v>
       </c>
-      <c r="R202" s="34"/>
+      <c r="R202" s="51">
+        <v>0</v>
+      </c>
       <c r="S202" s="34"/>
       <c r="T202" s="34"/>
       <c r="U202" s="34"/>
       <c r="V202" s="34"/>
       <c r="W202" s="82"/>
     </row>
-    <row r="203" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B203" s="94"/>
+    <row r="203" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B203" s="90"/>
       <c r="C203" s="22" t="s">
         <v>136</v>
       </c>
@@ -13107,15 +13428,17 @@
       <c r="Q203" s="52">
         <v>0</v>
       </c>
-      <c r="R203" s="5"/>
+      <c r="R203" s="52">
+        <v>0</v>
+      </c>
       <c r="S203" s="5"/>
       <c r="T203" s="5"/>
       <c r="U203" s="5"/>
       <c r="V203" s="5"/>
       <c r="W203" s="78"/>
     </row>
-    <row r="204" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B204" s="94"/>
+    <row r="204" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B204" s="90"/>
       <c r="C204" s="22" t="s">
         <v>137</v>
       </c>
@@ -13160,15 +13483,17 @@
       <c r="Q204" s="52">
         <v>0</v>
       </c>
-      <c r="R204" s="5"/>
+      <c r="R204" s="52">
+        <v>0</v>
+      </c>
       <c r="S204" s="5"/>
       <c r="T204" s="5"/>
       <c r="U204" s="5"/>
       <c r="V204" s="5"/>
       <c r="W204" s="78"/>
     </row>
-    <row r="205" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B205" s="94"/>
+    <row r="205" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B205" s="90"/>
       <c r="C205" s="22" t="s">
         <v>145</v>
       </c>
@@ -13213,15 +13538,17 @@
       <c r="Q205" s="52">
         <v>0</v>
       </c>
-      <c r="R205" s="5"/>
+      <c r="R205" s="52">
+        <v>0</v>
+      </c>
       <c r="S205" s="5"/>
       <c r="T205" s="5"/>
       <c r="U205" s="5"/>
       <c r="V205" s="5"/>
       <c r="W205" s="78"/>
     </row>
-    <row r="206" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B206" s="94"/>
+    <row r="206" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B206" s="90"/>
       <c r="C206" s="22" t="s">
         <v>84</v>
       </c>
@@ -13266,15 +13593,17 @@
       <c r="Q206" s="52">
         <v>0</v>
       </c>
-      <c r="R206" s="5"/>
+      <c r="R206" s="52">
+        <v>0</v>
+      </c>
       <c r="S206" s="5"/>
       <c r="T206" s="5"/>
       <c r="U206" s="5"/>
       <c r="V206" s="5"/>
       <c r="W206" s="78"/>
     </row>
-    <row r="207" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B207" s="94"/>
+    <row r="207" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B207" s="90"/>
       <c r="C207" s="22" t="s">
         <v>85</v>
       </c>
@@ -13319,15 +13648,17 @@
       <c r="Q207" s="62">
         <v>0</v>
       </c>
-      <c r="R207" s="5"/>
+      <c r="R207" s="62">
+        <v>0</v>
+      </c>
       <c r="S207" s="5"/>
       <c r="T207" s="5"/>
       <c r="U207" s="5"/>
       <c r="V207" s="5"/>
       <c r="W207" s="78"/>
     </row>
-    <row r="208" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B208" s="94"/>
+    <row r="208" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B208" s="90"/>
       <c r="C208" s="22" t="s">
         <v>87</v>
       </c>
@@ -13372,15 +13703,17 @@
       <c r="Q208" s="52">
         <v>0</v>
       </c>
-      <c r="R208" s="5"/>
+      <c r="R208" s="52">
+        <v>0</v>
+      </c>
       <c r="S208" s="5"/>
       <c r="T208" s="5"/>
       <c r="U208" s="5"/>
       <c r="V208" s="5"/>
       <c r="W208" s="78"/>
     </row>
-    <row r="209" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B209" s="94"/>
+    <row r="209" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B209" s="90"/>
       <c r="C209" s="22" t="s">
         <v>86</v>
       </c>
@@ -13425,15 +13758,17 @@
       <c r="Q209" s="52">
         <v>0</v>
       </c>
-      <c r="R209" s="5"/>
+      <c r="R209" s="52">
+        <v>0</v>
+      </c>
       <c r="S209" s="5"/>
       <c r="T209" s="5"/>
       <c r="U209" s="5"/>
       <c r="V209" s="5"/>
       <c r="W209" s="78"/>
     </row>
-    <row r="210" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B210" s="94"/>
+    <row r="210" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B210" s="90"/>
       <c r="C210" s="22" t="s">
         <v>103</v>
       </c>
@@ -13478,15 +13813,17 @@
       <c r="Q210" s="52">
         <v>0</v>
       </c>
-      <c r="R210" s="5"/>
+      <c r="R210" s="52">
+        <v>0</v>
+      </c>
       <c r="S210" s="5"/>
       <c r="T210" s="5"/>
       <c r="U210" s="5"/>
       <c r="V210" s="5"/>
       <c r="W210" s="78"/>
     </row>
-    <row r="211" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B211" s="94"/>
+    <row r="211" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B211" s="90"/>
       <c r="C211" s="22" t="s">
         <v>135</v>
       </c>
@@ -13531,15 +13868,17 @@
       <c r="Q211" s="62">
         <v>0</v>
       </c>
-      <c r="R211" s="5"/>
+      <c r="R211" s="62">
+        <v>0</v>
+      </c>
       <c r="S211" s="5"/>
       <c r="T211" s="5"/>
       <c r="U211" s="5"/>
       <c r="V211" s="5"/>
       <c r="W211" s="78"/>
     </row>
-    <row r="212" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B212" s="94"/>
+    <row r="212" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B212" s="90"/>
       <c r="C212" s="22" t="s">
         <v>104</v>
       </c>
@@ -13584,29 +13923,31 @@
       <c r="Q212" s="74">
         <v>0</v>
       </c>
-      <c r="R212" s="5"/>
+      <c r="R212" s="74">
+        <v>0</v>
+      </c>
       <c r="S212" s="5"/>
       <c r="T212" s="5"/>
       <c r="U212" s="5"/>
       <c r="V212" s="5"/>
       <c r="W212" s="78"/>
     </row>
-    <row r="213" spans="2:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B213" s="113" t="s">
+    <row r="213" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B213" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="C213" s="114"/>
-      <c r="D213" s="114"/>
-      <c r="E213" s="114"/>
-      <c r="F213" s="114"/>
-      <c r="G213" s="115"/>
+      <c r="C213" s="99"/>
+      <c r="D213" s="99"/>
+      <c r="E213" s="99"/>
+      <c r="F213" s="99"/>
+      <c r="G213" s="100"/>
       <c r="H213" s="25">
         <f t="shared" ref="H213:W213" si="5">SUM(H4:H212)</f>
         <v>115.84999999999995</v>
       </c>
       <c r="I213" s="16">
         <f t="shared" si="5"/>
-        <v>35.82030000000001</v>
+        <v>38.56930000000002</v>
       </c>
       <c r="J213" s="16">
         <f t="shared" si="5"/>
@@ -13642,11 +13983,11 @@
       </c>
       <c r="R213" s="16">
         <f t="shared" si="5"/>
-        <v>6.6999999999999993</v>
+        <v>8.8329999999999984</v>
       </c>
       <c r="S213" s="16">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.61599999999999999</v>
       </c>
       <c r="T213" s="16">
         <f t="shared" si="5"/>
@@ -13665,7 +14006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
@@ -13674,24 +14015,24 @@
       <c r="G214" s="2"/>
       <c r="H214" s="2"/>
       <c r="I214" s="2"/>
-      <c r="J214" s="90" t="s">
+      <c r="J214" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="K214" s="91"/>
-      <c r="L214" s="91"/>
-      <c r="M214" s="91"/>
-      <c r="N214" s="91"/>
-      <c r="O214" s="91"/>
-      <c r="P214" s="91"/>
-      <c r="Q214" s="91"/>
-      <c r="R214" s="91"/>
-      <c r="S214" s="91"/>
-      <c r="T214" s="91"/>
-      <c r="U214" s="91"/>
-      <c r="V214" s="91"/>
-      <c r="W214" s="92"/>
-    </row>
-    <row r="215" spans="2:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K214" s="102"/>
+      <c r="L214" s="102"/>
+      <c r="M214" s="102"/>
+      <c r="N214" s="102"/>
+      <c r="O214" s="102"/>
+      <c r="P214" s="102"/>
+      <c r="Q214" s="102"/>
+      <c r="R214" s="102"/>
+      <c r="S214" s="102"/>
+      <c r="T214" s="102"/>
+      <c r="U214" s="102"/>
+      <c r="V214" s="102"/>
+      <c r="W214" s="103"/>
+    </row>
+    <row r="215" spans="2:23" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C215" s="41" t="s">
         <v>159</v>
       </c>
@@ -13711,7 +14052,7 @@
       <c r="M215" s="3"/>
       <c r="N215" s="3"/>
     </row>
-    <row r="216" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B216" s="68" t="s">
         <v>155</v>
       </c>
@@ -13721,18 +14062,18 @@
       </c>
       <c r="D216" s="4">
         <f>SUM(I10,I12,I13,I14,I15:I63,I187:I189,I191,I195:I201,I207:I208,I211)</f>
-        <v>16.880300000000002</v>
+        <v>19.629300000000008</v>
       </c>
       <c r="E216" s="4">
         <f>SUM(C216,-D216)</f>
-        <v>30.519699999999983</v>
+        <v>27.770699999999977</v>
       </c>
       <c r="F216" s="2"/>
       <c r="G216" s="2"/>
-      <c r="H216" s="108" t="s">
+      <c r="H216" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="I216" s="109"/>
+      <c r="I216" s="93"/>
       <c r="J216" s="9">
         <f>H213-J213</f>
         <v>115.84999999999995</v>
@@ -13767,30 +14108,30 @@
       </c>
       <c r="R216" s="71">
         <f t="shared" si="6"/>
-        <v>80.029699999999963</v>
+        <v>77.896699999999967</v>
       </c>
       <c r="S216" s="71">
         <f t="shared" si="6"/>
-        <v>80.029699999999963</v>
+        <v>77.280699999999968</v>
       </c>
       <c r="T216" s="71">
         <f t="shared" si="6"/>
-        <v>80.029699999999963</v>
+        <v>77.280699999999968</v>
       </c>
       <c r="U216" s="71">
         <f t="shared" si="6"/>
-        <v>80.029699999999963</v>
+        <v>77.280699999999968</v>
       </c>
       <c r="V216" s="71">
         <f t="shared" si="6"/>
-        <v>80.029699999999963</v>
+        <v>77.280699999999968</v>
       </c>
       <c r="W216" s="71">
         <f t="shared" si="6"/>
-        <v>80.029699999999963</v>
-      </c>
-    </row>
-    <row r="217" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>77.280699999999968</v>
+      </c>
+    </row>
+    <row r="217" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B217" s="69" t="s">
         <v>156</v>
       </c>
@@ -13816,7 +14157,7 @@
       <c r="M217" s="3"/>
       <c r="N217" s="3"/>
     </row>
-    <row r="218" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B218" s="69" t="s">
         <v>157</v>
       </c>
@@ -13833,20 +14174,20 @@
         <v>14.149999999999999</v>
       </c>
       <c r="F218" s="3"/>
-      <c r="H218" s="90" t="s">
+      <c r="H218" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="I218" s="110"/>
-      <c r="J218" s="109">
+      <c r="I218" s="95"/>
+      <c r="J218" s="93">
         <f>H213-I213</f>
-        <v>80.029699999999934</v>
-      </c>
-      <c r="K218" s="109"/>
-      <c r="L218" s="109"/>
-      <c r="M218" s="109"/>
-      <c r="N218" s="111"/>
-    </row>
-    <row r="219" spans="2:23" x14ac:dyDescent="0.25">
+        <v>77.280699999999939</v>
+      </c>
+      <c r="K218" s="93"/>
+      <c r="L218" s="93"/>
+      <c r="M218" s="93"/>
+      <c r="N218" s="96"/>
+    </row>
+    <row r="219" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B219" s="3"/>
       <c r="C219" s="3"/>
       <c r="D219" s="3"/>
@@ -13861,7 +14202,7 @@
       <c r="M219" s="3"/>
       <c r="N219" s="3"/>
     </row>
-    <row r="220" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B220" s="3"/>
       <c r="C220" s="3"/>
       <c r="D220" s="3"/>
@@ -13876,7 +14217,7 @@
       <c r="M220" s="3"/>
       <c r="N220" s="3"/>
     </row>
-    <row r="221" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B221" s="3"/>
       <c r="C221" s="3"/>
       <c r="D221" s="3"/>
@@ -13891,63 +14232,81 @@
       <c r="M221" s="3"/>
       <c r="N221" s="3"/>
     </row>
-    <row r="222" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="223" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="224" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="223" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="224" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B224" s="12"/>
       <c r="C224" s="12"/>
     </row>
-    <row r="225" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B225" s="12"/>
       <c r="C225" s="12"/>
     </row>
-    <row r="226" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B226" s="12"/>
       <c r="C226" s="12"/>
     </row>
-    <row r="227" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B227" s="12"/>
       <c r="C227" s="12"/>
     </row>
-    <row r="228" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B228" s="12"/>
       <c r="C228" s="12"/>
     </row>
-    <row r="229" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B229" s="12"/>
       <c r="C229" s="12"/>
     </row>
-    <row r="230" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B230" s="12"/>
       <c r="C230" s="12"/>
     </row>
-    <row r="231" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B231" s="12"/>
       <c r="C231" s="12"/>
     </row>
-    <row r="232" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B232" s="12"/>
       <c r="C232" s="12"/>
     </row>
-    <row r="233" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B233" s="12"/>
       <c r="C233" s="12"/>
     </row>
-    <row r="234" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B234" s="12"/>
       <c r="C234" s="12"/>
     </row>
-    <row r="235" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B235" s="12"/>
       <c r="C235" s="12"/>
     </row>
-    <row r="236" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B236" s="12"/>
       <c r="C236" s="12"/>
     </row>
-    <row r="237" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="237" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C158:C164"/>
+    <mergeCell ref="C144:C150"/>
+    <mergeCell ref="C130:C136"/>
+    <mergeCell ref="C123:C129"/>
+    <mergeCell ref="C109:C115"/>
+    <mergeCell ref="C137:C143"/>
+    <mergeCell ref="C151:C157"/>
+    <mergeCell ref="C88:C94"/>
+    <mergeCell ref="J2:W2"/>
+    <mergeCell ref="B64:B73"/>
+    <mergeCell ref="C57:C63"/>
+    <mergeCell ref="C15:C56"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C74:C80"/>
+    <mergeCell ref="C81:C87"/>
     <mergeCell ref="B195:B201"/>
     <mergeCell ref="H216:I216"/>
     <mergeCell ref="H218:I218"/>
@@ -13964,24 +14323,6 @@
     <mergeCell ref="C172:C178"/>
     <mergeCell ref="C102:C108"/>
     <mergeCell ref="C95:C101"/>
-    <mergeCell ref="C88:C94"/>
-    <mergeCell ref="J2:W2"/>
-    <mergeCell ref="B64:B73"/>
-    <mergeCell ref="C57:C63"/>
-    <mergeCell ref="C15:C56"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="C74:C80"/>
-    <mergeCell ref="C81:C87"/>
-    <mergeCell ref="C158:C164"/>
-    <mergeCell ref="C144:C150"/>
-    <mergeCell ref="C130:C136"/>
-    <mergeCell ref="C123:C129"/>
-    <mergeCell ref="C109:C115"/>
-    <mergeCell ref="C137:C143"/>
-    <mergeCell ref="C151:C157"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13995,7 +14336,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14007,7 +14348,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizando excel, introducido sonido de proyectil espada
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
+++ b/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="159">
   <si>
     <t>Subtarea</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t>Crear Animación Spawn Enemigos</t>
+  </si>
+  <si>
+    <t>Sonido atacar</t>
   </si>
 </sst>
 </file>
@@ -1323,43 +1326,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1368,10 +1338,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1405,6 +1378,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1459,24 +1462,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$J$208:$N$208</c:f>
+              <c:f>Hoja1!$J$209:$N$209</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>113.44999999999997</c:v>
+                  <c:v>113.54999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>109.39669999999998</c:v>
+                  <c:v>109.49669999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>107.39369999999998</c:v>
+                  <c:v>107.49369999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>101.25269999999999</c:v>
+                  <c:v>101.35269999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>98.809699999999992</c:v>
+                  <c:v>98.909699999999987</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1497,11 +1500,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="472228576"/>
-        <c:axId val="472234016"/>
+        <c:axId val="-941709808"/>
+        <c:axId val="-941708176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="472228576"/>
+        <c:axId val="-941709808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1510,7 +1513,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="472234016"/>
+        <c:crossAx val="-941708176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1518,7 +1521,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="472234016"/>
+        <c:axId val="-941708176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1529,7 +1532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="472228576"/>
+        <c:crossAx val="-941709808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1557,13 +1560,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>532721</xdr:colOff>
-      <xdr:row>217</xdr:row>
+      <xdr:row>218</xdr:row>
       <xdr:rowOff>120667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>138546</xdr:colOff>
-      <xdr:row>234</xdr:row>
+      <xdr:row>235</xdr:row>
       <xdr:rowOff>32068</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1571,7 +1574,7 @@
         <xdr:cNvPr id="4" name="3 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1879,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W229"/>
+  <dimension ref="A1:W230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C154" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="T200" sqref="T200"/>
+    <sheetView tabSelected="1" topLeftCell="C169" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T189" sqref="T189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1912,22 +1915,22 @@
       <c r="I2" s="37">
         <v>3</v>
       </c>
-      <c r="J2" s="95" t="s">
+      <c r="J2" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="104"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="W2" s="93"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="38" t="s">
@@ -1998,7 +2001,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="114" t="s">
+      <c r="B4" s="104" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="26" t="s">
@@ -2056,7 +2059,7 @@
       <c r="W4" s="77"/>
     </row>
     <row r="5" spans="1:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="115"/>
+      <c r="B5" s="105"/>
       <c r="C5" s="24" t="s">
         <v>91</v>
       </c>
@@ -2121,7 +2124,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="115"/>
+      <c r="B6" s="105"/>
       <c r="C6" s="24" t="s">
         <v>92</v>
       </c>
@@ -2178,7 +2181,7 @@
       <c r="W6" s="78"/>
     </row>
     <row r="7" spans="1:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="115"/>
+      <c r="B7" s="105"/>
       <c r="C7" s="24" t="s">
         <v>93</v>
       </c>
@@ -2235,7 +2238,7 @@
       <c r="W7" s="78"/>
     </row>
     <row r="8" spans="1:23" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="116"/>
+      <c r="B8" s="106"/>
       <c r="C8" s="30" t="s">
         <v>101</v>
       </c>
@@ -2300,7 +2303,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="114" t="s">
+      <c r="B9" s="104" t="s">
         <v>96</v>
       </c>
       <c r="C9" s="33" t="s">
@@ -2367,7 +2370,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="115"/>
+      <c r="B10" s="105"/>
       <c r="C10" s="23" t="s">
         <v>97</v>
       </c>
@@ -2424,7 +2427,7 @@
       <c r="W10" s="78"/>
     </row>
     <row r="11" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="115"/>
+      <c r="B11" s="105"/>
       <c r="C11" s="65" t="s">
         <v>102</v>
       </c>
@@ -2489,7 +2492,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="115"/>
+      <c r="B12" s="105"/>
       <c r="C12" s="65" t="s">
         <v>103</v>
       </c>
@@ -2554,7 +2557,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="116"/>
+      <c r="B13" s="106"/>
       <c r="C13" s="35" t="s">
         <v>88</v>
       </c>
@@ -2619,7 +2622,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="94" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="36" t="s">
@@ -2688,8 +2691,8 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B15" s="91"/>
-      <c r="C15" s="109" t="s">
+      <c r="B15" s="95"/>
+      <c r="C15" s="99" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -2755,8 +2758,8 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B16" s="91"/>
-      <c r="C16" s="110"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="100"/>
       <c r="D16" s="4" t="s">
         <v>19</v>
       </c>
@@ -2820,8 +2823,8 @@
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B17" s="91"/>
-      <c r="C17" s="110"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="100"/>
       <c r="D17" s="4" t="s">
         <v>20</v>
       </c>
@@ -2885,8 +2888,8 @@
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B18" s="91"/>
-      <c r="C18" s="110"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="100"/>
       <c r="D18" s="4" t="s">
         <v>21</v>
       </c>
@@ -2950,8 +2953,8 @@
       </c>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B19" s="91"/>
-      <c r="C19" s="110"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="100"/>
       <c r="D19" s="4" t="s">
         <v>22</v>
       </c>
@@ -3015,8 +3018,8 @@
       </c>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B20" s="91"/>
-      <c r="C20" s="110"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="100"/>
       <c r="D20" s="4" t="s">
         <v>153</v>
       </c>
@@ -3072,8 +3075,8 @@
       <c r="W20" s="78"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B21" s="91"/>
-      <c r="C21" s="110"/>
+      <c r="B21" s="95"/>
+      <c r="C21" s="100"/>
       <c r="D21" s="4" t="s">
         <v>23</v>
       </c>
@@ -3137,8 +3140,8 @@
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B22" s="91"/>
-      <c r="C22" s="110"/>
+      <c r="B22" s="95"/>
+      <c r="C22" s="100"/>
       <c r="D22" s="21" t="s">
         <v>157</v>
       </c>
@@ -3194,8 +3197,8 @@
       <c r="W22" s="78"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B23" s="91"/>
-      <c r="C23" s="110"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="100"/>
       <c r="D23" s="21" t="s">
         <v>35</v>
       </c>
@@ -3251,8 +3254,8 @@
       <c r="W23" s="78"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B24" s="91"/>
-      <c r="C24" s="110"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="100"/>
       <c r="D24" s="21" t="s">
         <v>36</v>
       </c>
@@ -3308,8 +3311,8 @@
       <c r="W24" s="78"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B25" s="91"/>
-      <c r="C25" s="110"/>
+      <c r="B25" s="95"/>
+      <c r="C25" s="100"/>
       <c r="D25" s="21" t="s">
         <v>37</v>
       </c>
@@ -3365,8 +3368,8 @@
       <c r="W25" s="78"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B26" s="91"/>
-      <c r="C26" s="110"/>
+      <c r="B26" s="95"/>
+      <c r="C26" s="100"/>
       <c r="D26" s="21" t="s">
         <v>38</v>
       </c>
@@ -3422,8 +3425,8 @@
       <c r="W26" s="78"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B27" s="91"/>
-      <c r="C27" s="110"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="100"/>
       <c r="D27" s="21" t="s">
         <v>39</v>
       </c>
@@ -3479,8 +3482,8 @@
       <c r="W27" s="78"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B28" s="91"/>
-      <c r="C28" s="110"/>
+      <c r="B28" s="95"/>
+      <c r="C28" s="100"/>
       <c r="D28" s="21" t="s">
         <v>40</v>
       </c>
@@ -3536,8 +3539,8 @@
       <c r="W28" s="78"/>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B29" s="91"/>
-      <c r="C29" s="110"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="100"/>
       <c r="D29" s="21" t="s">
         <v>41</v>
       </c>
@@ -3593,8 +3596,8 @@
       <c r="W29" s="78"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B30" s="91"/>
-      <c r="C30" s="110"/>
+      <c r="B30" s="95"/>
+      <c r="C30" s="100"/>
       <c r="D30" s="21" t="s">
         <v>42</v>
       </c>
@@ -3650,8 +3653,8 @@
       <c r="W30" s="78"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B31" s="91"/>
-      <c r="C31" s="110"/>
+      <c r="B31" s="95"/>
+      <c r="C31" s="100"/>
       <c r="D31" s="21" t="s">
         <v>43</v>
       </c>
@@ -3707,8 +3710,8 @@
       <c r="W31" s="78"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B32" s="91"/>
-      <c r="C32" s="110"/>
+      <c r="B32" s="95"/>
+      <c r="C32" s="100"/>
       <c r="D32" s="21" t="s">
         <v>44</v>
       </c>
@@ -3764,8 +3767,8 @@
       <c r="W32" s="78"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B33" s="91"/>
-      <c r="C33" s="110"/>
+      <c r="B33" s="95"/>
+      <c r="C33" s="100"/>
       <c r="D33" s="21" t="s">
         <v>45</v>
       </c>
@@ -3821,8 +3824,8 @@
       <c r="W33" s="78"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B34" s="91"/>
-      <c r="C34" s="110"/>
+      <c r="B34" s="95"/>
+      <c r="C34" s="100"/>
       <c r="D34" s="21" t="s">
         <v>46</v>
       </c>
@@ -3878,8 +3881,8 @@
       <c r="W34" s="78"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B35" s="91"/>
-      <c r="C35" s="110"/>
+      <c r="B35" s="95"/>
+      <c r="C35" s="100"/>
       <c r="D35" s="21" t="s">
         <v>47</v>
       </c>
@@ -3935,8 +3938,8 @@
       <c r="W35" s="78"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B36" s="91"/>
-      <c r="C36" s="110"/>
+      <c r="B36" s="95"/>
+      <c r="C36" s="100"/>
       <c r="D36" s="21" t="s">
         <v>48</v>
       </c>
@@ -3992,8 +3995,8 @@
       <c r="W36" s="78"/>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B37" s="91"/>
-      <c r="C37" s="110"/>
+      <c r="B37" s="95"/>
+      <c r="C37" s="100"/>
       <c r="D37" s="21" t="s">
         <v>49</v>
       </c>
@@ -4049,8 +4052,8 @@
       <c r="W37" s="78"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B38" s="91"/>
-      <c r="C38" s="110"/>
+      <c r="B38" s="95"/>
+      <c r="C38" s="100"/>
       <c r="D38" s="21" t="s">
         <v>50</v>
       </c>
@@ -4106,8 +4109,8 @@
       <c r="W38" s="78"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B39" s="91"/>
-      <c r="C39" s="110"/>
+      <c r="B39" s="95"/>
+      <c r="C39" s="100"/>
       <c r="D39" s="21" t="s">
         <v>51</v>
       </c>
@@ -4163,8 +4166,8 @@
       <c r="W39" s="78"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B40" s="91"/>
-      <c r="C40" s="110"/>
+      <c r="B40" s="95"/>
+      <c r="C40" s="100"/>
       <c r="D40" s="21" t="s">
         <v>52</v>
       </c>
@@ -4220,8 +4223,8 @@
       <c r="W40" s="78"/>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B41" s="91"/>
-      <c r="C41" s="110"/>
+      <c r="B41" s="95"/>
+      <c r="C41" s="100"/>
       <c r="D41" s="21" t="s">
         <v>53</v>
       </c>
@@ -4277,8 +4280,8 @@
       <c r="W41" s="78"/>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B42" s="91"/>
-      <c r="C42" s="110"/>
+      <c r="B42" s="95"/>
+      <c r="C42" s="100"/>
       <c r="D42" s="21" t="s">
         <v>54</v>
       </c>
@@ -4334,8 +4337,8 @@
       <c r="W42" s="78"/>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B43" s="91"/>
-      <c r="C43" s="110"/>
+      <c r="B43" s="95"/>
+      <c r="C43" s="100"/>
       <c r="D43" s="21" t="s">
         <v>55</v>
       </c>
@@ -4391,8 +4394,8 @@
       <c r="W43" s="78"/>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B44" s="91"/>
-      <c r="C44" s="110"/>
+      <c r="B44" s="95"/>
+      <c r="C44" s="100"/>
       <c r="D44" s="21" t="s">
         <v>56</v>
       </c>
@@ -4448,8 +4451,8 @@
       <c r="W44" s="78"/>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B45" s="91"/>
-      <c r="C45" s="110"/>
+      <c r="B45" s="95"/>
+      <c r="C45" s="100"/>
       <c r="D45" s="21" t="s">
         <v>57</v>
       </c>
@@ -4505,8 +4508,8 @@
       <c r="W45" s="78"/>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B46" s="91"/>
-      <c r="C46" s="110"/>
+      <c r="B46" s="95"/>
+      <c r="C46" s="100"/>
       <c r="D46" s="21" t="s">
         <v>58</v>
       </c>
@@ -4562,8 +4565,8 @@
       <c r="W46" s="78"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B47" s="91"/>
-      <c r="C47" s="110"/>
+      <c r="B47" s="95"/>
+      <c r="C47" s="100"/>
       <c r="D47" s="21" t="s">
         <v>59</v>
       </c>
@@ -4619,8 +4622,8 @@
       <c r="W47" s="78"/>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B48" s="91"/>
-      <c r="C48" s="110"/>
+      <c r="B48" s="95"/>
+      <c r="C48" s="100"/>
       <c r="D48" s="21" t="s">
         <v>60</v>
       </c>
@@ -4676,8 +4679,8 @@
       <c r="W48" s="78"/>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B49" s="91"/>
-      <c r="C49" s="107" t="s">
+      <c r="B49" s="95"/>
+      <c r="C49" s="97" t="s">
         <v>25</v>
       </c>
       <c r="D49" s="18" t="s">
@@ -4735,8 +4738,8 @@
       <c r="W49" s="78"/>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B50" s="91"/>
-      <c r="C50" s="108"/>
+      <c r="B50" s="95"/>
+      <c r="C50" s="98"/>
       <c r="D50" s="18" t="s">
         <v>28</v>
       </c>
@@ -4792,8 +4795,8 @@
       <c r="W50" s="78"/>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B51" s="91"/>
-      <c r="C51" s="108"/>
+      <c r="B51" s="95"/>
+      <c r="C51" s="98"/>
       <c r="D51" s="18" t="s">
         <v>29</v>
       </c>
@@ -4849,8 +4852,8 @@
       <c r="W51" s="78"/>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B52" s="91"/>
-      <c r="C52" s="108"/>
+      <c r="B52" s="95"/>
+      <c r="C52" s="98"/>
       <c r="D52" s="18" t="s">
         <v>30</v>
       </c>
@@ -4906,8 +4909,8 @@
       <c r="W52" s="78"/>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B53" s="91"/>
-      <c r="C53" s="108"/>
+      <c r="B53" s="95"/>
+      <c r="C53" s="98"/>
       <c r="D53" s="18" t="s">
         <v>33</v>
       </c>
@@ -4963,8 +4966,8 @@
       <c r="W53" s="78"/>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B54" s="91"/>
-      <c r="C54" s="108"/>
+      <c r="B54" s="95"/>
+      <c r="C54" s="98"/>
       <c r="D54" s="18" t="s">
         <v>31</v>
       </c>
@@ -5020,8 +5023,8 @@
       <c r="W54" s="78"/>
     </row>
     <row r="55" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="98"/>
-      <c r="C55" s="108"/>
+      <c r="B55" s="112"/>
+      <c r="C55" s="98"/>
       <c r="D55" s="44" t="s">
         <v>32</v>
       </c>
@@ -5077,10 +5080,10 @@
       <c r="W55" s="81"/>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B56" s="90" t="s">
+      <c r="B56" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="111" t="s">
+      <c r="C56" s="101" t="s">
         <v>70</v>
       </c>
       <c r="D56" s="28" t="s">
@@ -5138,8 +5141,8 @@
       <c r="W56" s="82"/>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B57" s="91"/>
-      <c r="C57" s="112"/>
+      <c r="B57" s="95"/>
+      <c r="C57" s="102"/>
       <c r="D57" s="4" t="s">
         <v>62</v>
       </c>
@@ -5195,8 +5198,8 @@
       <c r="W57" s="78"/>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B58" s="91"/>
-      <c r="C58" s="112"/>
+      <c r="B58" s="95"/>
+      <c r="C58" s="102"/>
       <c r="D58" s="4" t="s">
         <v>63</v>
       </c>
@@ -5252,8 +5255,8 @@
       <c r="W58" s="78"/>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B59" s="91"/>
-      <c r="C59" s="112"/>
+      <c r="B59" s="95"/>
+      <c r="C59" s="102"/>
       <c r="D59" s="18" t="s">
         <v>67</v>
       </c>
@@ -5309,7 +5312,7 @@
       <c r="W59" s="78"/>
     </row>
     <row r="60" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B60" s="91"/>
+      <c r="B60" s="95"/>
       <c r="C60" s="22" t="s">
         <v>64</v>
       </c>
@@ -5366,7 +5369,7 @@
       <c r="W60" s="78"/>
     </row>
     <row r="61" spans="2:23" ht="18" x14ac:dyDescent="0.3">
-      <c r="B61" s="91"/>
+      <c r="B61" s="95"/>
       <c r="C61" s="22" t="s">
         <v>72</v>
       </c>
@@ -5423,8 +5426,8 @@
       <c r="W61" s="78"/>
     </row>
     <row r="62" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="91"/>
-      <c r="C62" s="112" t="s">
+      <c r="B62" s="95"/>
+      <c r="C62" s="102" t="s">
         <v>71</v>
       </c>
       <c r="D62" s="4" t="s">
@@ -5482,8 +5485,8 @@
       <c r="W62" s="78"/>
     </row>
     <row r="63" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="91"/>
-      <c r="C63" s="112"/>
+      <c r="B63" s="95"/>
+      <c r="C63" s="102"/>
       <c r="D63" s="4" t="s">
         <v>66</v>
       </c>
@@ -5539,8 +5542,8 @@
       <c r="W63" s="78"/>
     </row>
     <row r="64" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="91"/>
-      <c r="C64" s="112"/>
+      <c r="B64" s="95"/>
+      <c r="C64" s="102"/>
       <c r="D64" s="4" t="s">
         <v>68</v>
       </c>
@@ -5596,8 +5599,8 @@
       <c r="W64" s="78"/>
     </row>
     <row r="65" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="92"/>
-      <c r="C65" s="113"/>
+      <c r="B65" s="96"/>
+      <c r="C65" s="103"/>
       <c r="D65" s="17" t="s">
         <v>69</v>
       </c>
@@ -5653,10 +5656,10 @@
       <c r="W65" s="79"/>
     </row>
     <row r="66" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="90" t="s">
+      <c r="B66" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="C66" s="117" t="s">
+      <c r="C66" s="107" t="s">
         <v>107</v>
       </c>
       <c r="D66" s="28" t="s">
@@ -5722,8 +5725,8 @@
       </c>
     </row>
     <row r="67" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="91"/>
-      <c r="C67" s="102"/>
+      <c r="B67" s="95"/>
+      <c r="C67" s="90"/>
       <c r="D67" s="4" t="s">
         <v>123</v>
       </c>
@@ -5779,8 +5782,8 @@
       <c r="W67" s="63"/>
     </row>
     <row r="68" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="91"/>
-      <c r="C68" s="102"/>
+      <c r="B68" s="95"/>
+      <c r="C68" s="90"/>
       <c r="D68" s="4" t="s">
         <v>152</v>
       </c>
@@ -5836,8 +5839,8 @@
       <c r="W68" s="78"/>
     </row>
     <row r="69" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="91"/>
-      <c r="C69" s="102"/>
+      <c r="B69" s="95"/>
+      <c r="C69" s="90"/>
       <c r="D69" s="4" t="s">
         <v>124</v>
       </c>
@@ -5901,8 +5904,8 @@
       </c>
     </row>
     <row r="70" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="91"/>
-      <c r="C70" s="102"/>
+      <c r="B70" s="95"/>
+      <c r="C70" s="90"/>
       <c r="D70" s="4" t="s">
         <v>155</v>
       </c>
@@ -5958,8 +5961,8 @@
       <c r="W70" s="84"/>
     </row>
     <row r="71" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="91"/>
-      <c r="C71" s="102"/>
+      <c r="B71" s="95"/>
+      <c r="C71" s="90"/>
       <c r="D71" s="4" t="s">
         <v>154</v>
       </c>
@@ -6015,8 +6018,8 @@
       <c r="W71" s="84"/>
     </row>
     <row r="72" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="91"/>
-      <c r="C72" s="102"/>
+      <c r="B72" s="95"/>
+      <c r="C72" s="90"/>
       <c r="D72" s="4" t="s">
         <v>125</v>
       </c>
@@ -6072,8 +6075,8 @@
       <c r="W72" s="78"/>
     </row>
     <row r="73" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="91"/>
-      <c r="C73" s="102" t="s">
+      <c r="B73" s="95"/>
+      <c r="C73" s="90" t="s">
         <v>108</v>
       </c>
       <c r="D73" s="4" t="s">
@@ -6139,8 +6142,8 @@
       </c>
     </row>
     <row r="74" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="91"/>
-      <c r="C74" s="102"/>
+      <c r="B74" s="95"/>
+      <c r="C74" s="90"/>
       <c r="D74" s="4" t="s">
         <v>123</v>
       </c>
@@ -6196,8 +6199,8 @@
       <c r="W74" s="78"/>
     </row>
     <row r="75" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="91"/>
-      <c r="C75" s="102"/>
+      <c r="B75" s="95"/>
+      <c r="C75" s="90"/>
       <c r="D75" s="4" t="s">
         <v>152</v>
       </c>
@@ -6253,8 +6256,8 @@
       <c r="W75" s="78"/>
     </row>
     <row r="76" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="91"/>
-      <c r="C76" s="102"/>
+      <c r="B76" s="95"/>
+      <c r="C76" s="90"/>
       <c r="D76" s="4" t="s">
         <v>155</v>
       </c>
@@ -6310,8 +6313,8 @@
       <c r="W76" s="78"/>
     </row>
     <row r="77" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="91"/>
-      <c r="C77" s="102"/>
+      <c r="B77" s="95"/>
+      <c r="C77" s="90"/>
       <c r="D77" s="4" t="s">
         <v>154</v>
       </c>
@@ -6367,8 +6370,8 @@
       <c r="W77" s="78"/>
     </row>
     <row r="78" spans="2:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="91"/>
-      <c r="C78" s="102"/>
+      <c r="B78" s="95"/>
+      <c r="C78" s="90"/>
       <c r="D78" s="4" t="s">
         <v>124</v>
       </c>
@@ -6432,8 +6435,8 @@
       </c>
     </row>
     <row r="79" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B79" s="91"/>
-      <c r="C79" s="102"/>
+      <c r="B79" s="95"/>
+      <c r="C79" s="90"/>
       <c r="D79" s="4" t="s">
         <v>125</v>
       </c>
@@ -6489,8 +6492,8 @@
       <c r="W79" s="78"/>
     </row>
     <row r="80" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B80" s="91"/>
-      <c r="C80" s="102" t="s">
+      <c r="B80" s="95"/>
+      <c r="C80" s="90" t="s">
         <v>109</v>
       </c>
       <c r="D80" s="4" t="s">
@@ -6556,8 +6559,8 @@
       </c>
     </row>
     <row r="81" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B81" s="91"/>
-      <c r="C81" s="102"/>
+      <c r="B81" s="95"/>
+      <c r="C81" s="90"/>
       <c r="D81" s="4" t="s">
         <v>123</v>
       </c>
@@ -6613,8 +6616,8 @@
       <c r="W81" s="78"/>
     </row>
     <row r="82" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B82" s="91"/>
-      <c r="C82" s="102"/>
+      <c r="B82" s="95"/>
+      <c r="C82" s="90"/>
       <c r="D82" s="4" t="s">
         <v>152</v>
       </c>
@@ -6670,8 +6673,8 @@
       <c r="W82" s="78"/>
     </row>
     <row r="83" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="91"/>
-      <c r="C83" s="102"/>
+      <c r="B83" s="95"/>
+      <c r="C83" s="90"/>
       <c r="D83" s="4" t="s">
         <v>124</v>
       </c>
@@ -6735,8 +6738,8 @@
       </c>
     </row>
     <row r="84" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B84" s="91"/>
-      <c r="C84" s="102"/>
+      <c r="B84" s="95"/>
+      <c r="C84" s="90"/>
       <c r="D84" s="4" t="s">
         <v>155</v>
       </c>
@@ -6792,8 +6795,8 @@
       <c r="W84" s="84"/>
     </row>
     <row r="85" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="91"/>
-      <c r="C85" s="102"/>
+      <c r="B85" s="95"/>
+      <c r="C85" s="90"/>
       <c r="D85" s="4" t="s">
         <v>154</v>
       </c>
@@ -6849,8 +6852,8 @@
       <c r="W85" s="84"/>
     </row>
     <row r="86" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="91"/>
-      <c r="C86" s="102"/>
+      <c r="B86" s="95"/>
+      <c r="C86" s="90"/>
       <c r="D86" s="4" t="s">
         <v>125</v>
       </c>
@@ -6906,8 +6909,8 @@
       <c r="W86" s="78"/>
     </row>
     <row r="87" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B87" s="91"/>
-      <c r="C87" s="102" t="s">
+      <c r="B87" s="95"/>
+      <c r="C87" s="90" t="s">
         <v>110</v>
       </c>
       <c r="D87" s="4" t="s">
@@ -6973,8 +6976,8 @@
       </c>
     </row>
     <row r="88" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B88" s="91"/>
-      <c r="C88" s="102"/>
+      <c r="B88" s="95"/>
+      <c r="C88" s="90"/>
       <c r="D88" s="4" t="s">
         <v>123</v>
       </c>
@@ -7030,8 +7033,8 @@
       <c r="W88" s="78"/>
     </row>
     <row r="89" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="91"/>
-      <c r="C89" s="102"/>
+      <c r="B89" s="95"/>
+      <c r="C89" s="90"/>
       <c r="D89" s="4" t="s">
         <v>152</v>
       </c>
@@ -7087,8 +7090,8 @@
       <c r="W89" s="78"/>
     </row>
     <row r="90" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="91"/>
-      <c r="C90" s="102"/>
+      <c r="B90" s="95"/>
+      <c r="C90" s="90"/>
       <c r="D90" s="4" t="s">
         <v>124</v>
       </c>
@@ -7152,8 +7155,8 @@
       </c>
     </row>
     <row r="91" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="91"/>
-      <c r="C91" s="102"/>
+      <c r="B91" s="95"/>
+      <c r="C91" s="90"/>
       <c r="D91" s="4" t="s">
         <v>155</v>
       </c>
@@ -7209,8 +7212,8 @@
       <c r="W91" s="84"/>
     </row>
     <row r="92" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="91"/>
-      <c r="C92" s="102"/>
+      <c r="B92" s="95"/>
+      <c r="C92" s="90"/>
       <c r="D92" s="4" t="s">
         <v>154</v>
       </c>
@@ -7266,8 +7269,8 @@
       <c r="W92" s="84"/>
     </row>
     <row r="93" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B93" s="91"/>
-      <c r="C93" s="102"/>
+      <c r="B93" s="95"/>
+      <c r="C93" s="90"/>
       <c r="D93" s="4" t="s">
         <v>125</v>
       </c>
@@ -7323,8 +7326,8 @@
       <c r="W93" s="78"/>
     </row>
     <row r="94" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B94" s="91"/>
-      <c r="C94" s="102" t="s">
+      <c r="B94" s="95"/>
+      <c r="C94" s="90" t="s">
         <v>111</v>
       </c>
       <c r="D94" s="4" t="s">
@@ -7380,8 +7383,8 @@
       <c r="W94" s="63"/>
     </row>
     <row r="95" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B95" s="91"/>
-      <c r="C95" s="102"/>
+      <c r="B95" s="95"/>
+      <c r="C95" s="90"/>
       <c r="D95" s="4" t="s">
         <v>123</v>
       </c>
@@ -7437,8 +7440,8 @@
       <c r="W95" s="78"/>
     </row>
     <row r="96" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B96" s="91"/>
-      <c r="C96" s="102"/>
+      <c r="B96" s="95"/>
+      <c r="C96" s="90"/>
       <c r="D96" s="4" t="s">
         <v>152</v>
       </c>
@@ -7494,8 +7497,8 @@
       <c r="W96" s="78"/>
     </row>
     <row r="97" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B97" s="91"/>
-      <c r="C97" s="102"/>
+      <c r="B97" s="95"/>
+      <c r="C97" s="90"/>
       <c r="D97" s="4" t="s">
         <v>124</v>
       </c>
@@ -7559,8 +7562,8 @@
       </c>
     </row>
     <row r="98" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B98" s="91"/>
-      <c r="C98" s="102"/>
+      <c r="B98" s="95"/>
+      <c r="C98" s="90"/>
       <c r="D98" s="4" t="s">
         <v>155</v>
       </c>
@@ -7616,8 +7619,8 @@
       <c r="W98" s="84"/>
     </row>
     <row r="99" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B99" s="91"/>
-      <c r="C99" s="102"/>
+      <c r="B99" s="95"/>
+      <c r="C99" s="90"/>
       <c r="D99" s="4" t="s">
         <v>154</v>
       </c>
@@ -7673,8 +7676,8 @@
       <c r="W99" s="84"/>
     </row>
     <row r="100" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B100" s="91"/>
-      <c r="C100" s="102"/>
+      <c r="B100" s="95"/>
+      <c r="C100" s="90"/>
       <c r="D100" s="4" t="s">
         <v>125</v>
       </c>
@@ -7730,8 +7733,8 @@
       <c r="W100" s="78"/>
     </row>
     <row r="101" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B101" s="91"/>
-      <c r="C101" s="102" t="s">
+      <c r="B101" s="95"/>
+      <c r="C101" s="90" t="s">
         <v>112</v>
       </c>
       <c r="D101" s="4" t="s">
@@ -7789,8 +7792,8 @@
       <c r="W101" s="63"/>
     </row>
     <row r="102" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B102" s="91"/>
-      <c r="C102" s="102"/>
+      <c r="B102" s="95"/>
+      <c r="C102" s="90"/>
       <c r="D102" s="4" t="s">
         <v>123</v>
       </c>
@@ -7846,8 +7849,8 @@
       <c r="W102" s="78"/>
     </row>
     <row r="103" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="91"/>
-      <c r="C103" s="102"/>
+      <c r="B103" s="95"/>
+      <c r="C103" s="90"/>
       <c r="D103" s="4" t="s">
         <v>152</v>
       </c>
@@ -7903,8 +7906,8 @@
       <c r="W103" s="78"/>
     </row>
     <row r="104" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B104" s="91"/>
-      <c r="C104" s="102"/>
+      <c r="B104" s="95"/>
+      <c r="C104" s="90"/>
       <c r="D104" s="4" t="s">
         <v>124</v>
       </c>
@@ -7968,8 +7971,8 @@
       </c>
     </row>
     <row r="105" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B105" s="91"/>
-      <c r="C105" s="102"/>
+      <c r="B105" s="95"/>
+      <c r="C105" s="90"/>
       <c r="D105" s="4" t="s">
         <v>155</v>
       </c>
@@ -8025,8 +8028,8 @@
       <c r="W105" s="84"/>
     </row>
     <row r="106" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B106" s="91"/>
-      <c r="C106" s="102"/>
+      <c r="B106" s="95"/>
+      <c r="C106" s="90"/>
       <c r="D106" s="4" t="s">
         <v>154</v>
       </c>
@@ -8082,8 +8085,8 @@
       <c r="W106" s="84"/>
     </row>
     <row r="107" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="91"/>
-      <c r="C107" s="102"/>
+      <c r="B107" s="95"/>
+      <c r="C107" s="90"/>
       <c r="D107" s="4" t="s">
         <v>125</v>
       </c>
@@ -8139,8 +8142,8 @@
       <c r="W107" s="78"/>
     </row>
     <row r="108" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B108" s="91"/>
-      <c r="C108" s="102" t="s">
+      <c r="B108" s="95"/>
+      <c r="C108" s="90" t="s">
         <v>113</v>
       </c>
       <c r="D108" s="4" t="s">
@@ -8198,8 +8201,8 @@
       <c r="W108" s="63"/>
     </row>
     <row r="109" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B109" s="91"/>
-      <c r="C109" s="102"/>
+      <c r="B109" s="95"/>
+      <c r="C109" s="90"/>
       <c r="D109" s="4" t="s">
         <v>123</v>
       </c>
@@ -8255,8 +8258,8 @@
       <c r="W109" s="78"/>
     </row>
     <row r="110" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B110" s="91"/>
-      <c r="C110" s="102"/>
+      <c r="B110" s="95"/>
+      <c r="C110" s="90"/>
       <c r="D110" s="4" t="s">
         <v>152</v>
       </c>
@@ -8312,8 +8315,8 @@
       <c r="W110" s="78"/>
     </row>
     <row r="111" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B111" s="91"/>
-      <c r="C111" s="102"/>
+      <c r="B111" s="95"/>
+      <c r="C111" s="90"/>
       <c r="D111" s="4" t="s">
         <v>124</v>
       </c>
@@ -8377,8 +8380,8 @@
       </c>
     </row>
     <row r="112" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B112" s="91"/>
-      <c r="C112" s="102"/>
+      <c r="B112" s="95"/>
+      <c r="C112" s="90"/>
       <c r="D112" s="4" t="s">
         <v>155</v>
       </c>
@@ -8434,8 +8437,8 @@
       <c r="W112" s="84"/>
     </row>
     <row r="113" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B113" s="91"/>
-      <c r="C113" s="102"/>
+      <c r="B113" s="95"/>
+      <c r="C113" s="90"/>
       <c r="D113" s="4" t="s">
         <v>154</v>
       </c>
@@ -8491,8 +8494,8 @@
       <c r="W113" s="84"/>
     </row>
     <row r="114" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B114" s="91"/>
-      <c r="C114" s="102"/>
+      <c r="B114" s="95"/>
+      <c r="C114" s="90"/>
       <c r="D114" s="4" t="s">
         <v>125</v>
       </c>
@@ -8548,8 +8551,8 @@
       <c r="W114" s="78"/>
     </row>
     <row r="115" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B115" s="91"/>
-      <c r="C115" s="102" t="s">
+      <c r="B115" s="95"/>
+      <c r="C115" s="90" t="s">
         <v>114</v>
       </c>
       <c r="D115" s="4" t="s">
@@ -8607,8 +8610,8 @@
       <c r="W115" s="63"/>
     </row>
     <row r="116" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B116" s="91"/>
-      <c r="C116" s="102"/>
+      <c r="B116" s="95"/>
+      <c r="C116" s="90"/>
       <c r="D116" s="4" t="s">
         <v>123</v>
       </c>
@@ -8664,8 +8667,8 @@
       <c r="W116" s="78"/>
     </row>
     <row r="117" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B117" s="91"/>
-      <c r="C117" s="102"/>
+      <c r="B117" s="95"/>
+      <c r="C117" s="90"/>
       <c r="D117" s="4" t="s">
         <v>152</v>
       </c>
@@ -8721,8 +8724,8 @@
       <c r="W117" s="78"/>
     </row>
     <row r="118" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B118" s="91"/>
-      <c r="C118" s="102"/>
+      <c r="B118" s="95"/>
+      <c r="C118" s="90"/>
       <c r="D118" s="4" t="s">
         <v>124</v>
       </c>
@@ -8786,8 +8789,8 @@
       </c>
     </row>
     <row r="119" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B119" s="91"/>
-      <c r="C119" s="102"/>
+      <c r="B119" s="95"/>
+      <c r="C119" s="90"/>
       <c r="D119" s="4" t="s">
         <v>155</v>
       </c>
@@ -8843,8 +8846,8 @@
       <c r="W119" s="84"/>
     </row>
     <row r="120" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B120" s="91"/>
-      <c r="C120" s="102"/>
+      <c r="B120" s="95"/>
+      <c r="C120" s="90"/>
       <c r="D120" s="4" t="s">
         <v>154</v>
       </c>
@@ -8900,8 +8903,8 @@
       <c r="W120" s="84"/>
     </row>
     <row r="121" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B121" s="91"/>
-      <c r="C121" s="102"/>
+      <c r="B121" s="95"/>
+      <c r="C121" s="90"/>
       <c r="D121" s="4" t="s">
         <v>125</v>
       </c>
@@ -8957,8 +8960,8 @@
       <c r="W121" s="78"/>
     </row>
     <row r="122" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B122" s="91"/>
-      <c r="C122" s="102" t="s">
+      <c r="B122" s="95"/>
+      <c r="C122" s="90" t="s">
         <v>115</v>
       </c>
       <c r="D122" s="4" t="s">
@@ -9014,8 +9017,8 @@
       <c r="W122" s="63"/>
     </row>
     <row r="123" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B123" s="91"/>
-      <c r="C123" s="102"/>
+      <c r="B123" s="95"/>
+      <c r="C123" s="90"/>
       <c r="D123" s="4" t="s">
         <v>123</v>
       </c>
@@ -9071,8 +9074,8 @@
       <c r="W123" s="78"/>
     </row>
     <row r="124" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B124" s="91"/>
-      <c r="C124" s="102"/>
+      <c r="B124" s="95"/>
+      <c r="C124" s="90"/>
       <c r="D124" s="4" t="s">
         <v>152</v>
       </c>
@@ -9128,8 +9131,8 @@
       <c r="W124" s="78"/>
     </row>
     <row r="125" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B125" s="91"/>
-      <c r="C125" s="102"/>
+      <c r="B125" s="95"/>
+      <c r="C125" s="90"/>
       <c r="D125" s="4" t="s">
         <v>124</v>
       </c>
@@ -9193,8 +9196,8 @@
       </c>
     </row>
     <row r="126" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B126" s="91"/>
-      <c r="C126" s="102"/>
+      <c r="B126" s="95"/>
+      <c r="C126" s="90"/>
       <c r="D126" s="4" t="s">
         <v>155</v>
       </c>
@@ -9250,8 +9253,8 @@
       <c r="W126" s="84"/>
     </row>
     <row r="127" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B127" s="91"/>
-      <c r="C127" s="102"/>
+      <c r="B127" s="95"/>
+      <c r="C127" s="90"/>
       <c r="D127" s="4" t="s">
         <v>154</v>
       </c>
@@ -9307,8 +9310,8 @@
       <c r="W127" s="84"/>
     </row>
     <row r="128" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B128" s="91"/>
-      <c r="C128" s="102"/>
+      <c r="B128" s="95"/>
+      <c r="C128" s="90"/>
       <c r="D128" s="4" t="s">
         <v>125</v>
       </c>
@@ -9364,8 +9367,8 @@
       <c r="W128" s="78"/>
     </row>
     <row r="129" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B129" s="91"/>
-      <c r="C129" s="102" t="s">
+      <c r="B129" s="95"/>
+      <c r="C129" s="90" t="s">
         <v>116</v>
       </c>
       <c r="D129" s="4" t="s">
@@ -9423,8 +9426,8 @@
       <c r="W129" s="63"/>
     </row>
     <row r="130" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B130" s="91"/>
-      <c r="C130" s="102"/>
+      <c r="B130" s="95"/>
+      <c r="C130" s="90"/>
       <c r="D130" s="4" t="s">
         <v>123</v>
       </c>
@@ -9480,8 +9483,8 @@
       <c r="W130" s="78"/>
     </row>
     <row r="131" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B131" s="91"/>
-      <c r="C131" s="102"/>
+      <c r="B131" s="95"/>
+      <c r="C131" s="90"/>
       <c r="D131" s="4" t="s">
         <v>152</v>
       </c>
@@ -9537,8 +9540,8 @@
       <c r="W131" s="78"/>
     </row>
     <row r="132" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B132" s="91"/>
-      <c r="C132" s="102"/>
+      <c r="B132" s="95"/>
+      <c r="C132" s="90"/>
       <c r="D132" s="4" t="s">
         <v>124</v>
       </c>
@@ -9602,8 +9605,8 @@
       </c>
     </row>
     <row r="133" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B133" s="91"/>
-      <c r="C133" s="102"/>
+      <c r="B133" s="95"/>
+      <c r="C133" s="90"/>
       <c r="D133" s="4" t="s">
         <v>155</v>
       </c>
@@ -9659,8 +9662,8 @@
       <c r="W133" s="84"/>
     </row>
     <row r="134" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B134" s="91"/>
-      <c r="C134" s="102"/>
+      <c r="B134" s="95"/>
+      <c r="C134" s="90"/>
       <c r="D134" s="4" t="s">
         <v>154</v>
       </c>
@@ -9716,8 +9719,8 @@
       <c r="W134" s="84"/>
     </row>
     <row r="135" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B135" s="91"/>
-      <c r="C135" s="102"/>
+      <c r="B135" s="95"/>
+      <c r="C135" s="90"/>
       <c r="D135" s="4" t="s">
         <v>125</v>
       </c>
@@ -9773,8 +9776,8 @@
       <c r="W135" s="78"/>
     </row>
     <row r="136" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B136" s="91"/>
-      <c r="C136" s="102" t="s">
+      <c r="B136" s="95"/>
+      <c r="C136" s="90" t="s">
         <v>117</v>
       </c>
       <c r="D136" s="4" t="s">
@@ -9832,8 +9835,8 @@
       <c r="W136" s="63"/>
     </row>
     <row r="137" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B137" s="91"/>
-      <c r="C137" s="102"/>
+      <c r="B137" s="95"/>
+      <c r="C137" s="90"/>
       <c r="D137" s="4" t="s">
         <v>123</v>
       </c>
@@ -9889,8 +9892,8 @@
       <c r="W137" s="78"/>
     </row>
     <row r="138" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B138" s="91"/>
-      <c r="C138" s="102"/>
+      <c r="B138" s="95"/>
+      <c r="C138" s="90"/>
       <c r="D138" s="4" t="s">
         <v>152</v>
       </c>
@@ -9946,8 +9949,8 @@
       <c r="W138" s="78"/>
     </row>
     <row r="139" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B139" s="91"/>
-      <c r="C139" s="102"/>
+      <c r="B139" s="95"/>
+      <c r="C139" s="90"/>
       <c r="D139" s="4" t="s">
         <v>124</v>
       </c>
@@ -10011,8 +10014,8 @@
       </c>
     </row>
     <row r="140" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B140" s="91"/>
-      <c r="C140" s="102"/>
+      <c r="B140" s="95"/>
+      <c r="C140" s="90"/>
       <c r="D140" s="4" t="s">
         <v>155</v>
       </c>
@@ -10068,8 +10071,8 @@
       <c r="W140" s="84"/>
     </row>
     <row r="141" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B141" s="91"/>
-      <c r="C141" s="102"/>
+      <c r="B141" s="95"/>
+      <c r="C141" s="90"/>
       <c r="D141" s="4" t="s">
         <v>154</v>
       </c>
@@ -10125,8 +10128,8 @@
       <c r="W141" s="84"/>
     </row>
     <row r="142" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B142" s="91"/>
-      <c r="C142" s="102"/>
+      <c r="B142" s="95"/>
+      <c r="C142" s="90"/>
       <c r="D142" s="4" t="s">
         <v>125</v>
       </c>
@@ -10182,8 +10185,8 @@
       <c r="W142" s="78"/>
     </row>
     <row r="143" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B143" s="91"/>
-      <c r="C143" s="102" t="s">
+      <c r="B143" s="95"/>
+      <c r="C143" s="90" t="s">
         <v>118</v>
       </c>
       <c r="D143" s="4" t="s">
@@ -10241,8 +10244,8 @@
       <c r="W143" s="63"/>
     </row>
     <row r="144" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B144" s="91"/>
-      <c r="C144" s="102"/>
+      <c r="B144" s="95"/>
+      <c r="C144" s="90"/>
       <c r="D144" s="4" t="s">
         <v>123</v>
       </c>
@@ -10298,8 +10301,8 @@
       <c r="W144" s="78"/>
     </row>
     <row r="145" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B145" s="91"/>
-      <c r="C145" s="102"/>
+      <c r="B145" s="95"/>
+      <c r="C145" s="90"/>
       <c r="D145" s="4" t="s">
         <v>152</v>
       </c>
@@ -10355,8 +10358,8 @@
       <c r="W145" s="78"/>
     </row>
     <row r="146" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B146" s="91"/>
-      <c r="C146" s="102"/>
+      <c r="B146" s="95"/>
+      <c r="C146" s="90"/>
       <c r="D146" s="4" t="s">
         <v>124</v>
       </c>
@@ -10420,8 +10423,8 @@
       </c>
     </row>
     <row r="147" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B147" s="91"/>
-      <c r="C147" s="102"/>
+      <c r="B147" s="95"/>
+      <c r="C147" s="90"/>
       <c r="D147" s="4" t="s">
         <v>155</v>
       </c>
@@ -10477,8 +10480,8 @@
       <c r="W147" s="84"/>
     </row>
     <row r="148" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="91"/>
-      <c r="C148" s="102"/>
+      <c r="B148" s="95"/>
+      <c r="C148" s="90"/>
       <c r="D148" s="4" t="s">
         <v>154</v>
       </c>
@@ -10534,8 +10537,8 @@
       <c r="W148" s="84"/>
     </row>
     <row r="149" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B149" s="91"/>
-      <c r="C149" s="102"/>
+      <c r="B149" s="95"/>
+      <c r="C149" s="90"/>
       <c r="D149" s="4" t="s">
         <v>125</v>
       </c>
@@ -10591,8 +10594,8 @@
       <c r="W149" s="78"/>
     </row>
     <row r="150" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B150" s="91"/>
-      <c r="C150" s="102" t="s">
+      <c r="B150" s="95"/>
+      <c r="C150" s="90" t="s">
         <v>119</v>
       </c>
       <c r="D150" s="4" t="s">
@@ -10650,8 +10653,8 @@
       <c r="W150" s="63"/>
     </row>
     <row r="151" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B151" s="91"/>
-      <c r="C151" s="102"/>
+      <c r="B151" s="95"/>
+      <c r="C151" s="90"/>
       <c r="D151" s="4" t="s">
         <v>123</v>
       </c>
@@ -10707,8 +10710,8 @@
       <c r="W151" s="78"/>
     </row>
     <row r="152" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B152" s="91"/>
-      <c r="C152" s="102"/>
+      <c r="B152" s="95"/>
+      <c r="C152" s="90"/>
       <c r="D152" s="4" t="s">
         <v>152</v>
       </c>
@@ -10764,8 +10767,8 @@
       <c r="W152" s="78"/>
     </row>
     <row r="153" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B153" s="91"/>
-      <c r="C153" s="102"/>
+      <c r="B153" s="95"/>
+      <c r="C153" s="90"/>
       <c r="D153" s="4" t="s">
         <v>124</v>
       </c>
@@ -10829,8 +10832,8 @@
       </c>
     </row>
     <row r="154" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B154" s="91"/>
-      <c r="C154" s="102"/>
+      <c r="B154" s="95"/>
+      <c r="C154" s="90"/>
       <c r="D154" s="4" t="s">
         <v>155</v>
       </c>
@@ -10886,8 +10889,8 @@
       <c r="W154" s="84"/>
     </row>
     <row r="155" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B155" s="91"/>
-      <c r="C155" s="102"/>
+      <c r="B155" s="95"/>
+      <c r="C155" s="90"/>
       <c r="D155" s="4" t="s">
         <v>154</v>
       </c>
@@ -10943,8 +10946,8 @@
       <c r="W155" s="84"/>
     </row>
     <row r="156" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B156" s="91"/>
-      <c r="C156" s="102"/>
+      <c r="B156" s="95"/>
+      <c r="C156" s="90"/>
       <c r="D156" s="4" t="s">
         <v>125</v>
       </c>
@@ -11000,8 +11003,8 @@
       <c r="W156" s="78"/>
     </row>
     <row r="157" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B157" s="91"/>
-      <c r="C157" s="102" t="s">
+      <c r="B157" s="95"/>
+      <c r="C157" s="90" t="s">
         <v>120</v>
       </c>
       <c r="D157" s="4" t="s">
@@ -11059,8 +11062,8 @@
       <c r="W157" s="63"/>
     </row>
     <row r="158" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B158" s="91"/>
-      <c r="C158" s="102"/>
+      <c r="B158" s="95"/>
+      <c r="C158" s="90"/>
       <c r="D158" s="4" t="s">
         <v>123</v>
       </c>
@@ -11116,8 +11119,8 @@
       <c r="W158" s="78"/>
     </row>
     <row r="159" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B159" s="91"/>
-      <c r="C159" s="102"/>
+      <c r="B159" s="95"/>
+      <c r="C159" s="90"/>
       <c r="D159" s="4" t="s">
         <v>152</v>
       </c>
@@ -11173,8 +11176,8 @@
       <c r="W159" s="78"/>
     </row>
     <row r="160" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B160" s="91"/>
-      <c r="C160" s="102"/>
+      <c r="B160" s="95"/>
+      <c r="C160" s="90"/>
       <c r="D160" s="4" t="s">
         <v>124</v>
       </c>
@@ -11238,8 +11241,8 @@
       </c>
     </row>
     <row r="161" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B161" s="91"/>
-      <c r="C161" s="102"/>
+      <c r="B161" s="95"/>
+      <c r="C161" s="90"/>
       <c r="D161" s="4" t="s">
         <v>155</v>
       </c>
@@ -11295,8 +11298,8 @@
       <c r="W161" s="84"/>
     </row>
     <row r="162" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B162" s="91"/>
-      <c r="C162" s="102"/>
+      <c r="B162" s="95"/>
+      <c r="C162" s="90"/>
       <c r="D162" s="4" t="s">
         <v>154</v>
       </c>
@@ -11352,8 +11355,8 @@
       <c r="W162" s="84"/>
     </row>
     <row r="163" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B163" s="91"/>
-      <c r="C163" s="102"/>
+      <c r="B163" s="95"/>
+      <c r="C163" s="90"/>
       <c r="D163" s="4" t="s">
         <v>125</v>
       </c>
@@ -11409,8 +11412,8 @@
       <c r="W163" s="78"/>
     </row>
     <row r="164" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B164" s="91"/>
-      <c r="C164" s="102" t="s">
+      <c r="B164" s="95"/>
+      <c r="C164" s="90" t="s">
         <v>121</v>
       </c>
       <c r="D164" s="4" t="s">
@@ -11468,8 +11471,8 @@
       <c r="W164" s="63"/>
     </row>
     <row r="165" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B165" s="91"/>
-      <c r="C165" s="102"/>
+      <c r="B165" s="95"/>
+      <c r="C165" s="90"/>
       <c r="D165" s="4" t="s">
         <v>123</v>
       </c>
@@ -11525,8 +11528,8 @@
       <c r="W165" s="78"/>
     </row>
     <row r="166" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B166" s="91"/>
-      <c r="C166" s="102"/>
+      <c r="B166" s="95"/>
+      <c r="C166" s="90"/>
       <c r="D166" s="4" t="s">
         <v>152</v>
       </c>
@@ -11582,8 +11585,8 @@
       <c r="W166" s="78"/>
     </row>
     <row r="167" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B167" s="91"/>
-      <c r="C167" s="102"/>
+      <c r="B167" s="95"/>
+      <c r="C167" s="90"/>
       <c r="D167" s="4" t="s">
         <v>124</v>
       </c>
@@ -11647,8 +11650,8 @@
       </c>
     </row>
     <row r="168" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B168" s="98"/>
-      <c r="C168" s="105"/>
+      <c r="B168" s="112"/>
+      <c r="C168" s="116"/>
       <c r="D168" s="4" t="s">
         <v>155</v>
       </c>
@@ -11704,8 +11707,8 @@
       <c r="W168" s="86"/>
     </row>
     <row r="169" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B169" s="98"/>
-      <c r="C169" s="105"/>
+      <c r="B169" s="112"/>
+      <c r="C169" s="116"/>
       <c r="D169" s="4" t="s">
         <v>154</v>
       </c>
@@ -11761,8 +11764,8 @@
       <c r="W169" s="86"/>
     </row>
     <row r="170" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B170" s="92"/>
-      <c r="C170" s="106"/>
+      <c r="B170" s="96"/>
+      <c r="C170" s="117"/>
       <c r="D170" s="17" t="s">
         <v>125</v>
       </c>
@@ -11818,7 +11821,7 @@
       <c r="W170" s="79"/>
     </row>
     <row r="171" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B171" s="90" t="s">
+      <c r="B171" s="94" t="s">
         <v>74</v>
       </c>
       <c r="C171" s="60" t="s">
@@ -11838,7 +11841,7 @@
         <v>3</v>
       </c>
       <c r="I171" s="29">
-        <f t="shared" ref="I171:I204" si="4">SUM(J171:W171)</f>
+        <f t="shared" ref="I171:I205" si="4">SUM(J171:W171)</f>
         <v>0</v>
       </c>
       <c r="J171" s="51">
@@ -11877,7 +11880,7 @@
       <c r="W171" s="82"/>
     </row>
     <row r="172" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="91"/>
+      <c r="B172" s="95"/>
       <c r="C172" s="22" t="s">
         <v>80</v>
       </c>
@@ -11934,7 +11937,7 @@
       <c r="W172" s="78"/>
     </row>
     <row r="173" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B173" s="91"/>
+      <c r="B173" s="95"/>
       <c r="C173" s="22" t="s">
         <v>81</v>
       </c>
@@ -11991,7 +11994,7 @@
       <c r="W173" s="78"/>
     </row>
     <row r="174" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="91"/>
+      <c r="B174" s="95"/>
       <c r="C174" s="22" t="s">
         <v>82</v>
       </c>
@@ -12048,7 +12051,7 @@
       <c r="W174" s="78"/>
     </row>
     <row r="175" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="91"/>
+      <c r="B175" s="95"/>
       <c r="C175" s="22" t="s">
         <v>132</v>
       </c>
@@ -12105,7 +12108,7 @@
       <c r="W175" s="78"/>
     </row>
     <row r="176" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="91"/>
+      <c r="B176" s="95"/>
       <c r="C176" s="22" t="s">
         <v>129</v>
       </c>
@@ -12162,7 +12165,7 @@
       <c r="W176" s="78"/>
     </row>
     <row r="177" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B177" s="91"/>
+      <c r="B177" s="95"/>
       <c r="C177" s="22" t="s">
         <v>131</v>
       </c>
@@ -12219,7 +12222,7 @@
       <c r="W177" s="78"/>
     </row>
     <row r="178" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B178" s="91"/>
+      <c r="B178" s="95"/>
       <c r="C178" s="22" t="s">
         <v>130</v>
       </c>
@@ -12276,7 +12279,7 @@
       <c r="W178" s="78"/>
     </row>
     <row r="179" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B179" s="91"/>
+      <c r="B179" s="95"/>
       <c r="C179" s="22" t="s">
         <v>83</v>
       </c>
@@ -12341,7 +12344,7 @@
       </c>
     </row>
     <row r="180" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B180" s="91"/>
+      <c r="B180" s="95"/>
       <c r="C180" s="22" t="s">
         <v>84</v>
       </c>
@@ -12406,7 +12409,7 @@
       </c>
     </row>
     <row r="181" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B181" s="91"/>
+      <c r="B181" s="95"/>
       <c r="C181" s="22" t="s">
         <v>85</v>
       </c>
@@ -12471,7 +12474,7 @@
       </c>
     </row>
     <row r="182" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B182" s="91"/>
+      <c r="B182" s="95"/>
       <c r="C182" s="22" t="s">
         <v>89</v>
       </c>
@@ -12528,7 +12531,7 @@
       <c r="W182" s="78"/>
     </row>
     <row r="183" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B183" s="92"/>
+      <c r="B183" s="96"/>
       <c r="C183" s="43" t="s">
         <v>90</v>
       </c>
@@ -12587,7 +12590,7 @@
       <c r="W183" s="79"/>
     </row>
     <row r="184" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B184" s="90" t="s">
+      <c r="B184" s="94" t="s">
         <v>133</v>
       </c>
       <c r="C184" s="42" t="s">
@@ -12646,7 +12649,7 @@
       <c r="W184" s="82"/>
     </row>
     <row r="185" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B185" s="91"/>
+      <c r="B185" s="95"/>
       <c r="C185" s="41" t="s">
         <v>134</v>
       </c>
@@ -12703,7 +12706,7 @@
       <c r="W185" s="78"/>
     </row>
     <row r="186" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B186" s="92"/>
+      <c r="B186" s="96"/>
       <c r="C186" s="43" t="s">
         <v>135</v>
       </c>
@@ -12760,7 +12763,7 @@
       <c r="W186" s="79"/>
     </row>
     <row r="187" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B187" s="90" t="s">
+      <c r="B187" s="94" t="s">
         <v>138</v>
       </c>
       <c r="C187" s="42" t="s">
@@ -12821,7 +12824,7 @@
       <c r="W187" s="82"/>
     </row>
     <row r="188" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B188" s="91"/>
+      <c r="B188" s="95"/>
       <c r="C188" s="41" t="s">
         <v>140</v>
       </c>
@@ -12878,9 +12881,9 @@
       <c r="W188" s="78"/>
     </row>
     <row r="189" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B189" s="91"/>
+      <c r="B189" s="95"/>
       <c r="C189" s="41" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="D189" s="4"/>
       <c r="E189" s="4" t="s">
@@ -12935,9 +12938,9 @@
       <c r="W189" s="78"/>
     </row>
     <row r="190" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B190" s="91"/>
+      <c r="B190" s="95"/>
       <c r="C190" s="41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D190" s="4"/>
       <c r="E190" s="4" t="s">
@@ -12992,9 +12995,9 @@
       <c r="W190" s="78"/>
     </row>
     <row r="191" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B191" s="91"/>
+      <c r="B191" s="95"/>
       <c r="C191" s="41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D191" s="4"/>
       <c r="E191" s="4" t="s">
@@ -13011,7 +13014,7 @@
       </c>
       <c r="I191" s="40">
         <f t="shared" si="4"/>
-        <v>0.16700000000000001</v>
+        <v>0</v>
       </c>
       <c r="J191" s="52">
         <v>0</v>
@@ -13028,19 +13031,19 @@
       <c r="N191" s="52">
         <v>0</v>
       </c>
-      <c r="O191" s="73">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="P191" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q191" s="62">
-        <v>0</v>
-      </c>
-      <c r="R191" s="62">
-        <v>0</v>
-      </c>
-      <c r="S191" s="62">
+      <c r="O191" s="52">
+        <v>0</v>
+      </c>
+      <c r="P191" s="52">
+        <v>0</v>
+      </c>
+      <c r="Q191" s="52">
+        <v>0</v>
+      </c>
+      <c r="R191" s="52">
+        <v>0</v>
+      </c>
+      <c r="S191" s="52">
         <v>0</v>
       </c>
       <c r="T191" s="5"/>
@@ -13049,9 +13052,9 @@
       <c r="W191" s="78"/>
     </row>
     <row r="192" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B192" s="91"/>
+      <c r="B192" s="95"/>
       <c r="C192" s="41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D192" s="4"/>
       <c r="E192" s="4" t="s">
@@ -13068,7 +13071,7 @@
       </c>
       <c r="I192" s="40">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="J192" s="52">
         <v>0</v>
@@ -13085,19 +13088,19 @@
       <c r="N192" s="52">
         <v>0</v>
       </c>
-      <c r="O192" s="52">
-        <v>0</v>
-      </c>
-      <c r="P192" s="52">
-        <v>0</v>
-      </c>
-      <c r="Q192" s="52">
-        <v>0</v>
-      </c>
-      <c r="R192" s="52">
-        <v>0</v>
-      </c>
-      <c r="S192" s="52">
+      <c r="O192" s="73">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="P192" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q192" s="62">
+        <v>0</v>
+      </c>
+      <c r="R192" s="62">
+        <v>0</v>
+      </c>
+      <c r="S192" s="62">
         <v>0</v>
       </c>
       <c r="T192" s="5"/>
@@ -13105,183 +13108,183 @@
       <c r="V192" s="5"/>
       <c r="W192" s="78"/>
     </row>
-    <row r="193" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B193" s="92"/>
-      <c r="C193" s="43" t="s">
-        <v>145</v>
-      </c>
-      <c r="D193" s="17"/>
-      <c r="E193" s="17" t="s">
+    <row r="193" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B193" s="95"/>
+      <c r="C193" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="D193" s="4"/>
+      <c r="E193" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F193" s="50" t="s">
+      <c r="F193" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="G193" s="17">
-        <v>7</v>
-      </c>
-      <c r="H193" s="17">
+      <c r="G193" s="4">
+        <v>7</v>
+      </c>
+      <c r="H193" s="4">
         <v>0.1</v>
       </c>
       <c r="I193" s="40">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J193" s="53">
-        <v>0</v>
-      </c>
-      <c r="K193" s="53">
-        <v>0</v>
-      </c>
-      <c r="L193" s="53">
-        <v>0</v>
-      </c>
-      <c r="M193" s="53">
-        <v>0</v>
-      </c>
-      <c r="N193" s="53">
-        <v>0</v>
-      </c>
-      <c r="O193" s="53">
-        <v>0</v>
-      </c>
-      <c r="P193" s="53">
-        <v>0</v>
-      </c>
-      <c r="Q193" s="53">
-        <v>0</v>
-      </c>
-      <c r="R193" s="53">
-        <v>0</v>
-      </c>
-      <c r="S193" s="53">
-        <v>0</v>
-      </c>
-      <c r="T193" s="31"/>
-      <c r="U193" s="31"/>
-      <c r="V193" s="31"/>
-      <c r="W193" s="79"/>
-    </row>
-    <row r="194" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B194" s="90" t="s">
+      <c r="J193" s="52">
+        <v>0</v>
+      </c>
+      <c r="K193" s="52">
+        <v>0</v>
+      </c>
+      <c r="L193" s="52">
+        <v>0</v>
+      </c>
+      <c r="M193" s="52">
+        <v>0</v>
+      </c>
+      <c r="N193" s="52">
+        <v>0</v>
+      </c>
+      <c r="O193" s="52">
+        <v>0</v>
+      </c>
+      <c r="P193" s="52">
+        <v>0</v>
+      </c>
+      <c r="Q193" s="52">
+        <v>0</v>
+      </c>
+      <c r="R193" s="52">
+        <v>0</v>
+      </c>
+      <c r="S193" s="52">
+        <v>0</v>
+      </c>
+      <c r="T193" s="5"/>
+      <c r="U193" s="5"/>
+      <c r="V193" s="5"/>
+      <c r="W193" s="78"/>
+    </row>
+    <row r="194" spans="2:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B194" s="96"/>
+      <c r="C194" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="D194" s="17"/>
+      <c r="E194" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="F194" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="G194" s="17">
+        <v>7</v>
+      </c>
+      <c r="H194" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="I194" s="40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J194" s="53">
+        <v>0</v>
+      </c>
+      <c r="K194" s="53">
+        <v>0</v>
+      </c>
+      <c r="L194" s="53">
+        <v>0</v>
+      </c>
+      <c r="M194" s="53">
+        <v>0</v>
+      </c>
+      <c r="N194" s="53">
+        <v>0</v>
+      </c>
+      <c r="O194" s="53">
+        <v>0</v>
+      </c>
+      <c r="P194" s="53">
+        <v>0</v>
+      </c>
+      <c r="Q194" s="53">
+        <v>0</v>
+      </c>
+      <c r="R194" s="53">
+        <v>0</v>
+      </c>
+      <c r="S194" s="53">
+        <v>0</v>
+      </c>
+      <c r="T194" s="31"/>
+      <c r="U194" s="31"/>
+      <c r="V194" s="31"/>
+      <c r="W194" s="79"/>
+    </row>
+    <row r="195" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B195" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="C194" s="36" t="s">
+      <c r="C195" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="D194" s="28"/>
-      <c r="E194" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="F194" s="57" t="s">
+      <c r="D195" s="28"/>
+      <c r="E195" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F195" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="G194" s="28">
+      <c r="G195" s="28">
         <v>3</v>
       </c>
-      <c r="H194" s="28">
+      <c r="H195" s="28">
         <v>0.4</v>
       </c>
-      <c r="I194" s="29">
+      <c r="I195" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J194" s="51">
-        <v>0</v>
-      </c>
-      <c r="K194" s="51">
-        <v>0</v>
-      </c>
-      <c r="L194" s="51">
-        <v>0</v>
-      </c>
-      <c r="M194" s="51">
-        <v>0</v>
-      </c>
-      <c r="N194" s="51">
-        <v>0</v>
-      </c>
-      <c r="O194" s="51">
-        <v>0</v>
-      </c>
-      <c r="P194" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q194" s="51">
-        <v>0</v>
-      </c>
-      <c r="R194" s="51">
-        <v>0</v>
-      </c>
-      <c r="S194" s="51">
-        <v>0</v>
-      </c>
-      <c r="T194" s="34"/>
-      <c r="U194" s="34"/>
-      <c r="V194" s="34"/>
-      <c r="W194" s="82"/>
-    </row>
-    <row r="195" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B195" s="91"/>
-      <c r="C195" s="22" t="s">
+      <c r="J195" s="51">
+        <v>0</v>
+      </c>
+      <c r="K195" s="51">
+        <v>0</v>
+      </c>
+      <c r="L195" s="51">
+        <v>0</v>
+      </c>
+      <c r="M195" s="51">
+        <v>0</v>
+      </c>
+      <c r="N195" s="51">
+        <v>0</v>
+      </c>
+      <c r="O195" s="51">
+        <v>0</v>
+      </c>
+      <c r="P195" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q195" s="51">
+        <v>0</v>
+      </c>
+      <c r="R195" s="51">
+        <v>0</v>
+      </c>
+      <c r="S195" s="51">
+        <v>0</v>
+      </c>
+      <c r="T195" s="34"/>
+      <c r="U195" s="34"/>
+      <c r="V195" s="34"/>
+      <c r="W195" s="82"/>
+    </row>
+    <row r="196" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B196" s="95"/>
+      <c r="C196" s="22" t="s">
         <v>127</v>
-      </c>
-      <c r="D195" s="4"/>
-      <c r="E195" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F195" s="56" t="s">
-        <v>100</v>
-      </c>
-      <c r="G195" s="4">
-        <v>3</v>
-      </c>
-      <c r="H195" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="I195" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J195" s="52">
-        <v>0</v>
-      </c>
-      <c r="K195" s="52">
-        <v>0</v>
-      </c>
-      <c r="L195" s="52">
-        <v>0</v>
-      </c>
-      <c r="M195" s="52">
-        <v>0</v>
-      </c>
-      <c r="N195" s="52">
-        <v>0</v>
-      </c>
-      <c r="O195" s="52">
-        <v>0</v>
-      </c>
-      <c r="P195" s="52">
-        <v>0</v>
-      </c>
-      <c r="Q195" s="52">
-        <v>0</v>
-      </c>
-      <c r="R195" s="52">
-        <v>0</v>
-      </c>
-      <c r="S195" s="52">
-        <v>0</v>
-      </c>
-      <c r="T195" s="5"/>
-      <c r="U195" s="5"/>
-      <c r="V195" s="5"/>
-      <c r="W195" s="78"/>
-    </row>
-    <row r="196" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B196" s="91"/>
-      <c r="C196" s="22" t="s">
-        <v>128</v>
       </c>
       <c r="D196" s="4"/>
       <c r="E196" s="4" t="s">
@@ -13336,9 +13339,9 @@
       <c r="W196" s="78"/>
     </row>
     <row r="197" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B197" s="91"/>
+      <c r="B197" s="95"/>
       <c r="C197" s="22" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D197" s="4"/>
       <c r="E197" s="4" t="s">
@@ -13393,11 +13396,11 @@
       <c r="W197" s="78"/>
     </row>
     <row r="198" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B198" s="91"/>
+      <c r="B198" s="95"/>
       <c r="C198" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D198" s="5"/>
+        <v>136</v>
+      </c>
+      <c r="D198" s="4"/>
       <c r="E198" s="4" t="s">
         <v>7</v>
       </c>
@@ -13450,16 +13453,16 @@
       <c r="W198" s="78"/>
     </row>
     <row r="199" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B199" s="91"/>
+      <c r="B199" s="95"/>
       <c r="C199" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D199" s="5"/>
       <c r="E199" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F199" s="49" t="s">
-        <v>104</v>
+      <c r="F199" s="56" t="s">
+        <v>100</v>
       </c>
       <c r="G199" s="4">
         <v>3</v>
@@ -13469,7 +13472,7 @@
       </c>
       <c r="I199" s="6">
         <f t="shared" si="4"/>
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="J199" s="52">
         <v>0</v>
@@ -13486,19 +13489,19 @@
       <c r="N199" s="52">
         <v>0</v>
       </c>
-      <c r="O199" s="73">
-        <v>0.48</v>
-      </c>
-      <c r="P199" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q199" s="62">
-        <v>0</v>
-      </c>
-      <c r="R199" s="62">
-        <v>0</v>
-      </c>
-      <c r="S199" s="62">
+      <c r="O199" s="52">
+        <v>0</v>
+      </c>
+      <c r="P199" s="52">
+        <v>0</v>
+      </c>
+      <c r="Q199" s="52">
+        <v>0</v>
+      </c>
+      <c r="R199" s="52">
+        <v>0</v>
+      </c>
+      <c r="S199" s="52">
         <v>0</v>
       </c>
       <c r="T199" s="5"/>
@@ -13507,9 +13510,9 @@
       <c r="W199" s="78"/>
     </row>
     <row r="200" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B200" s="91"/>
+      <c r="B200" s="95"/>
       <c r="C200" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D200" s="5"/>
       <c r="E200" s="4" t="s">
@@ -13519,14 +13522,14 @@
         <v>104</v>
       </c>
       <c r="G200" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H200" s="4">
         <v>0.4</v>
       </c>
       <c r="I200" s="6">
         <f t="shared" si="4"/>
-        <v>1.5</v>
+        <v>0.48</v>
       </c>
       <c r="J200" s="52">
         <v>0</v>
@@ -13543,49 +13546,47 @@
       <c r="N200" s="52">
         <v>0</v>
       </c>
-      <c r="O200" s="52">
-        <v>0</v>
-      </c>
-      <c r="P200" s="52">
-        <v>0</v>
-      </c>
-      <c r="Q200" s="52">
-        <v>0</v>
-      </c>
-      <c r="R200" s="52">
-        <v>0</v>
-      </c>
-      <c r="S200" s="52">
-        <v>0</v>
-      </c>
-      <c r="T200" s="73">
-        <v>1.5</v>
-      </c>
+      <c r="O200" s="73">
+        <v>0.48</v>
+      </c>
+      <c r="P200" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q200" s="62">
+        <v>0</v>
+      </c>
+      <c r="R200" s="62">
+        <v>0</v>
+      </c>
+      <c r="S200" s="62">
+        <v>0</v>
+      </c>
+      <c r="T200" s="5"/>
       <c r="U200" s="5"/>
       <c r="V200" s="5"/>
       <c r="W200" s="78"/>
     </row>
     <row r="201" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B201" s="91"/>
+      <c r="B201" s="95"/>
       <c r="C201" s="22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D201" s="5"/>
       <c r="E201" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F201" s="56" t="s">
-        <v>100</v>
+      <c r="F201" s="49" t="s">
+        <v>104</v>
       </c>
       <c r="G201" s="4">
         <v>5</v>
       </c>
       <c r="H201" s="4">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="I201" s="6">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J201" s="52">
         <v>0</v>
@@ -13617,15 +13618,17 @@
       <c r="S201" s="52">
         <v>0</v>
       </c>
-      <c r="T201" s="5"/>
+      <c r="T201" s="73">
+        <v>1.5</v>
+      </c>
       <c r="U201" s="5"/>
       <c r="V201" s="5"/>
       <c r="W201" s="78"/>
     </row>
     <row r="202" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B202" s="91"/>
+      <c r="B202" s="95"/>
       <c r="C202" s="22" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="D202" s="5"/>
       <c r="E202" s="4" t="s">
@@ -13635,10 +13638,10 @@
         <v>100</v>
       </c>
       <c r="G202" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H202" s="4">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="I202" s="6">
         <f t="shared" si="4"/>
@@ -13680,55 +13683,55 @@
       <c r="W202" s="78"/>
     </row>
     <row r="203" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B203" s="91"/>
+      <c r="B203" s="95"/>
       <c r="C203" s="22" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="D203" s="5"/>
       <c r="E203" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F203" s="49" t="s">
-        <v>104</v>
+      <c r="F203" s="56" t="s">
+        <v>100</v>
       </c>
       <c r="G203" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H203" s="4">
-        <v>3</v>
+        <v>0.7</v>
       </c>
       <c r="I203" s="6">
         <f t="shared" si="4"/>
-        <v>1.85</v>
+        <v>0</v>
       </c>
       <c r="J203" s="52">
         <v>0</v>
       </c>
-      <c r="K203" s="62">
-        <v>1.85</v>
-      </c>
-      <c r="L203" s="62">
-        <v>0</v>
-      </c>
-      <c r="M203" s="62">
-        <v>0</v>
-      </c>
-      <c r="N203" s="62">
-        <v>0</v>
-      </c>
-      <c r="O203" s="62">
-        <v>0</v>
-      </c>
-      <c r="P203" s="62">
-        <v>0</v>
-      </c>
-      <c r="Q203" s="62">
-        <v>0</v>
-      </c>
-      <c r="R203" s="62">
-        <v>0</v>
-      </c>
-      <c r="S203" s="62">
+      <c r="K203" s="52">
+        <v>0</v>
+      </c>
+      <c r="L203" s="52">
+        <v>0</v>
+      </c>
+      <c r="M203" s="52">
+        <v>0</v>
+      </c>
+      <c r="N203" s="52">
+        <v>0</v>
+      </c>
+      <c r="O203" s="52">
+        <v>0</v>
+      </c>
+      <c r="P203" s="52">
+        <v>0</v>
+      </c>
+      <c r="Q203" s="52">
+        <v>0</v>
+      </c>
+      <c r="R203" s="52">
+        <v>0</v>
+      </c>
+      <c r="S203" s="52">
         <v>0</v>
       </c>
       <c r="T203" s="5"/>
@@ -13737,55 +13740,55 @@
       <c r="W203" s="78"/>
     </row>
     <row r="204" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B204" s="91"/>
+      <c r="B204" s="95"/>
       <c r="C204" s="22" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="D204" s="5"/>
       <c r="E204" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F204" s="56" t="s">
-        <v>100</v>
+      <c r="F204" s="49" t="s">
+        <v>104</v>
       </c>
       <c r="G204" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H204" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I204" s="6">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
       <c r="J204" s="52">
         <v>0</v>
       </c>
-      <c r="K204" s="52">
-        <v>0</v>
-      </c>
-      <c r="L204" s="52">
-        <v>0</v>
-      </c>
-      <c r="M204" s="52">
-        <v>0</v>
-      </c>
-      <c r="N204" s="52">
-        <v>0</v>
-      </c>
-      <c r="O204" s="52">
-        <v>0</v>
-      </c>
-      <c r="P204" s="52" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q204" s="74">
-        <v>0</v>
-      </c>
-      <c r="R204" s="74">
-        <v>0</v>
-      </c>
-      <c r="S204" s="74">
+      <c r="K204" s="62">
+        <v>1.85</v>
+      </c>
+      <c r="L204" s="62">
+        <v>0</v>
+      </c>
+      <c r="M204" s="62">
+        <v>0</v>
+      </c>
+      <c r="N204" s="62">
+        <v>0</v>
+      </c>
+      <c r="O204" s="62">
+        <v>0</v>
+      </c>
+      <c r="P204" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q204" s="62">
+        <v>0</v>
+      </c>
+      <c r="R204" s="62">
+        <v>0</v>
+      </c>
+      <c r="S204" s="62">
         <v>0</v>
       </c>
       <c r="T204" s="5"/>
@@ -13793,277 +13796,319 @@
       <c r="V204" s="5"/>
       <c r="W204" s="78"/>
     </row>
-    <row r="205" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B205" s="99" t="s">
+    <row r="205" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B205" s="95"/>
+      <c r="C205" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D205" s="5"/>
+      <c r="E205" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F205" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="G205" s="4">
+        <v>2</v>
+      </c>
+      <c r="H205" s="4">
+        <v>2</v>
+      </c>
+      <c r="I205" s="6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J205" s="52">
+        <v>0</v>
+      </c>
+      <c r="K205" s="52">
+        <v>0</v>
+      </c>
+      <c r="L205" s="52">
+        <v>0</v>
+      </c>
+      <c r="M205" s="52">
+        <v>0</v>
+      </c>
+      <c r="N205" s="52">
+        <v>0</v>
+      </c>
+      <c r="O205" s="52">
+        <v>0</v>
+      </c>
+      <c r="P205" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q205" s="74">
+        <v>0</v>
+      </c>
+      <c r="R205" s="74">
+        <v>0</v>
+      </c>
+      <c r="S205" s="74">
+        <v>0</v>
+      </c>
+      <c r="T205" s="5"/>
+      <c r="U205" s="5"/>
+      <c r="V205" s="5"/>
+      <c r="W205" s="78"/>
+    </row>
+    <row r="206" spans="2:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B206" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="C205" s="100"/>
-      <c r="D205" s="100"/>
-      <c r="E205" s="100"/>
-      <c r="F205" s="100"/>
-      <c r="G205" s="101"/>
-      <c r="H205" s="25">
-        <f t="shared" ref="H205:W205" si="5">SUM(H4:H204)</f>
-        <v>113.44999999999997</v>
-      </c>
-      <c r="I205" s="16">
+      <c r="C206" s="114"/>
+      <c r="D206" s="114"/>
+      <c r="E206" s="114"/>
+      <c r="F206" s="114"/>
+      <c r="G206" s="115"/>
+      <c r="H206" s="25">
+        <f t="shared" ref="H206:W206" si="5">SUM(H4:H205)</f>
+        <v>113.54999999999997</v>
+      </c>
+      <c r="I206" s="16">
         <f t="shared" si="5"/>
         <v>48.17530000000005</v>
       </c>
-      <c r="J205" s="16">
+      <c r="J206" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K205" s="16">
+      <c r="K206" s="16">
         <f t="shared" si="5"/>
         <v>4.0533000000000001</v>
       </c>
-      <c r="L205" s="70">
+      <c r="L206" s="70">
         <f t="shared" si="5"/>
         <v>2.0030000000000001</v>
       </c>
-      <c r="M205" s="16">
+      <c r="M206" s="16">
         <f t="shared" si="5"/>
         <v>6.1409999999999973</v>
       </c>
-      <c r="N205" s="16">
+      <c r="N206" s="16">
         <f t="shared" si="5"/>
         <v>2.4430000000000001</v>
       </c>
-      <c r="O205" s="16">
+      <c r="O206" s="16">
         <f t="shared" si="5"/>
         <v>3.0169999999999995</v>
       </c>
-      <c r="P205" s="16">
+      <c r="P206" s="16">
         <f t="shared" si="5"/>
         <v>9.2930000000000028</v>
       </c>
-      <c r="Q205" s="16">
+      <c r="Q206" s="16">
         <f t="shared" si="5"/>
         <v>2.4700000000000002</v>
       </c>
-      <c r="R205" s="16">
+      <c r="R206" s="16">
         <f t="shared" si="5"/>
         <v>8.8329999999999984</v>
       </c>
-      <c r="S205" s="16">
+      <c r="S206" s="16">
         <f t="shared" si="5"/>
         <v>6.5919999999999987</v>
       </c>
-      <c r="T205" s="16">
+      <c r="T206" s="16">
         <f t="shared" si="5"/>
         <v>1.83</v>
       </c>
-      <c r="U205" s="16">
+      <c r="U206" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V205" s="16">
+      <c r="V206" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W205" s="19">
+      <c r="W206" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B206" s="2"/>
-      <c r="C206" s="2"/>
-      <c r="D206" s="2"/>
-      <c r="E206" s="2"/>
-      <c r="F206" s="2"/>
-      <c r="G206" s="2"/>
-      <c r="H206" s="2"/>
-      <c r="I206" s="2"/>
-      <c r="J206" s="95" t="s">
-        <v>9</v>
-      </c>
-      <c r="K206" s="103"/>
-      <c r="L206" s="103"/>
-      <c r="M206" s="103"/>
-      <c r="N206" s="103"/>
-      <c r="O206" s="103"/>
-      <c r="P206" s="103"/>
-      <c r="Q206" s="103"/>
-      <c r="R206" s="103"/>
-      <c r="S206" s="103"/>
-      <c r="T206" s="103"/>
-      <c r="U206" s="103"/>
-      <c r="V206" s="103"/>
-      <c r="W206" s="104"/>
-    </row>
-    <row r="207" spans="2:23" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C207" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="D207" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E207" s="4" t="s">
-        <v>151</v>
-      </c>
+    <row r="207" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B207" s="2"/>
+      <c r="C207" s="2"/>
+      <c r="D207" s="2"/>
+      <c r="E207" s="2"/>
       <c r="F207" s="2"/>
       <c r="G207" s="2"/>
       <c r="H207" s="2"/>
       <c r="I207" s="2"/>
-      <c r="J207" s="3"/>
-      <c r="K207" s="3"/>
-      <c r="L207" s="3"/>
-      <c r="M207" s="3"/>
-      <c r="N207" s="3"/>
-    </row>
-    <row r="208" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B208" s="68" t="s">
-        <v>146</v>
-      </c>
-      <c r="C208" s="72">
-        <f>SUM(H203,H199:H200,H187:H193,H183,H179:H181,H12:H55,H10)</f>
-        <v>45.000000000000007</v>
-      </c>
-      <c r="D208" s="4">
-        <f>SUM(I10,I12,I13,I14,I15:I55,I179:I181,I183,I187:I193,I199:I200,I203)</f>
-        <v>23.865300000000026</v>
-      </c>
-      <c r="E208" s="4">
-        <f>SUM(C208,-D208)</f>
-        <v>21.134699999999981</v>
+      <c r="J207" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="K207" s="92"/>
+      <c r="L207" s="92"/>
+      <c r="M207" s="92"/>
+      <c r="N207" s="92"/>
+      <c r="O207" s="92"/>
+      <c r="P207" s="92"/>
+      <c r="Q207" s="92"/>
+      <c r="R207" s="92"/>
+      <c r="S207" s="92"/>
+      <c r="T207" s="92"/>
+      <c r="U207" s="92"/>
+      <c r="V207" s="92"/>
+      <c r="W207" s="93"/>
+    </row>
+    <row r="208" spans="2:23" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C208" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="D208" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E208" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="F208" s="2"/>
       <c r="G208" s="2"/>
-      <c r="H208" s="93" t="s">
+      <c r="H208" s="2"/>
+      <c r="I208" s="2"/>
+      <c r="J208" s="3"/>
+      <c r="K208" s="3"/>
+      <c r="L208" s="3"/>
+      <c r="M208" s="3"/>
+      <c r="N208" s="3"/>
+    </row>
+    <row r="209" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B209" s="68" t="s">
+        <v>146</v>
+      </c>
+      <c r="C209" s="72">
+        <f>SUM(H204,H200:H201,H187:H194,H183,H179:H181,H12:H55,H10)</f>
+        <v>45.1</v>
+      </c>
+      <c r="D209" s="4">
+        <f>SUM(I10,I12,I13,I14,I15:I55,I179:I181,I183,I187:I194,I200:I201,I204)</f>
+        <v>23.865300000000026</v>
+      </c>
+      <c r="E209" s="4">
+        <f>SUM(C209,-D209)</f>
+        <v>21.234699999999975</v>
+      </c>
+      <c r="F209" s="2"/>
+      <c r="G209" s="2"/>
+      <c r="H209" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="I208" s="94"/>
-      <c r="J208" s="9">
-        <f>H205-J205</f>
-        <v>113.44999999999997</v>
-      </c>
-      <c r="K208" s="9">
-        <f>J208-K205</f>
-        <v>109.39669999999998</v>
-      </c>
-      <c r="L208" s="9">
-        <f>K208-L205</f>
-        <v>107.39369999999998</v>
-      </c>
-      <c r="M208" s="9">
-        <f>L208-M205</f>
-        <v>101.25269999999999</v>
-      </c>
-      <c r="N208" s="10">
-        <f>M208-N205</f>
-        <v>98.809699999999992</v>
-      </c>
-      <c r="O208" s="71">
-        <f t="shared" ref="O208:W208" si="6">N208-O205</f>
-        <v>95.792699999999996</v>
-      </c>
-      <c r="P208" s="71">
+      <c r="I209" s="109"/>
+      <c r="J209" s="9">
+        <f>H206-J206</f>
+        <v>113.54999999999997</v>
+      </c>
+      <c r="K209" s="9">
+        <f>J209-K206</f>
+        <v>109.49669999999998</v>
+      </c>
+      <c r="L209" s="9">
+        <f>K209-L206</f>
+        <v>107.49369999999998</v>
+      </c>
+      <c r="M209" s="9">
+        <f>L209-M206</f>
+        <v>101.35269999999998</v>
+      </c>
+      <c r="N209" s="10">
+        <f>M209-N206</f>
+        <v>98.909699999999987</v>
+      </c>
+      <c r="O209" s="71">
+        <f t="shared" ref="O209:W209" si="6">N209-O206</f>
+        <v>95.892699999999991</v>
+      </c>
+      <c r="P209" s="71">
         <f t="shared" si="6"/>
-        <v>86.49969999999999</v>
-      </c>
-      <c r="Q208" s="71">
+        <v>86.599699999999984</v>
+      </c>
+      <c r="Q209" s="71">
         <f t="shared" si="6"/>
-        <v>84.029699999999991</v>
-      </c>
-      <c r="R208" s="71">
+        <v>84.129699999999985</v>
+      </c>
+      <c r="R209" s="71">
         <f t="shared" si="6"/>
-        <v>75.196699999999993</v>
-      </c>
-      <c r="S208" s="71">
+        <v>75.296699999999987</v>
+      </c>
+      <c r="S209" s="71">
         <f t="shared" si="6"/>
-        <v>68.604699999999994</v>
-      </c>
-      <c r="T208" s="71">
+        <v>68.704699999999988</v>
+      </c>
+      <c r="T209" s="71">
         <f t="shared" si="6"/>
-        <v>66.774699999999996</v>
-      </c>
-      <c r="U208" s="71">
+        <v>66.87469999999999</v>
+      </c>
+      <c r="U209" s="71">
         <f t="shared" si="6"/>
-        <v>66.774699999999996</v>
-      </c>
-      <c r="V208" s="71">
+        <v>66.87469999999999</v>
+      </c>
+      <c r="V209" s="71">
         <f t="shared" si="6"/>
-        <v>66.774699999999996</v>
-      </c>
-      <c r="W208" s="71">
+        <v>66.87469999999999</v>
+      </c>
+      <c r="W209" s="71">
         <f t="shared" si="6"/>
-        <v>66.774699999999996</v>
-      </c>
-    </row>
-    <row r="209" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B209" s="69" t="s">
+        <v>66.87469999999999</v>
+      </c>
+    </row>
+    <row r="210" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B210" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="C209" s="5">
+      <c r="C210" s="5">
         <f>SUM(H184:H186,H182,H66:H171,H11,H9)</f>
         <v>44.050000000000004</v>
       </c>
-      <c r="D209" s="5">
+      <c r="D210" s="5">
         <f>SUM(I9,I11,I66:I171,I182,I184:I186)</f>
         <v>12.26</v>
       </c>
-      <c r="E209" s="5">
-        <f>SUM(C209,-D209)</f>
-        <v>31.790000000000006</v>
-      </c>
-      <c r="F209" s="3"/>
-      <c r="G209" s="3"/>
-      <c r="H209" s="3"/>
-      <c r="I209" s="3"/>
-      <c r="J209" s="3"/>
-      <c r="K209" s="3"/>
-      <c r="L209" s="3"/>
-      <c r="M209" s="3"/>
-      <c r="N209" s="3"/>
-    </row>
-    <row r="210" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B210" s="69" t="s">
-        <v>148</v>
-      </c>
-      <c r="C210" s="4">
-        <f>SUM(H204,H202,H201,H194:H198,H172:H178,H56:H65,H4:H8)</f>
-        <v>24.4</v>
-      </c>
-      <c r="D210" s="5">
-        <f>SUM(I204,I201:I202,I194:I198,I172:I178,I56:I65,I4:I8)</f>
-        <v>12.05</v>
-      </c>
       <c r="E210" s="5">
         <f>SUM(C210,-D210)</f>
+        <v>31.790000000000006</v>
+      </c>
+      <c r="F210" s="3"/>
+      <c r="G210" s="3"/>
+      <c r="H210" s="3"/>
+      <c r="I210" s="3"/>
+      <c r="J210" s="3"/>
+      <c r="K210" s="3"/>
+      <c r="L210" s="3"/>
+      <c r="M210" s="3"/>
+      <c r="N210" s="3"/>
+    </row>
+    <row r="211" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B211" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="C211" s="4">
+        <f>SUM(H205,H203,H202,H195:H199,H172:H178,H56:H65,H4:H8)</f>
+        <v>24.4</v>
+      </c>
+      <c r="D211" s="5">
+        <f>SUM(I205,I202:I203,I195:I199,I172:I178,I56:I65,I4:I8)</f>
+        <v>12.05</v>
+      </c>
+      <c r="E211" s="5">
+        <f>SUM(C211,-D211)</f>
         <v>12.349999999999998</v>
       </c>
-      <c r="F210" s="3"/>
-      <c r="H210" s="95" t="s">
+      <c r="F211" s="3"/>
+      <c r="H211" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="I210" s="96"/>
-      <c r="J210" s="94">
-        <f>H205-I205</f>
-        <v>65.274699999999925</v>
-      </c>
-      <c r="K210" s="94"/>
-      <c r="L210" s="94"/>
-      <c r="M210" s="94"/>
-      <c r="N210" s="97"/>
-    </row>
-    <row r="211" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B211" s="3"/>
-      <c r="C211" s="3"/>
-      <c r="D211" s="3"/>
-      <c r="E211" s="3"/>
-      <c r="F211" s="3"/>
-      <c r="G211" s="3"/>
-      <c r="H211" s="3"/>
-      <c r="I211" s="3"/>
-      <c r="J211" s="3"/>
-      <c r="K211" s="3"/>
-      <c r="L211" s="3"/>
-      <c r="M211" s="3"/>
-      <c r="N211" s="3"/>
-    </row>
-    <row r="212" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="I211" s="110"/>
+      <c r="J211" s="109">
+        <f>H206-I206</f>
+        <v>65.374699999999919</v>
+      </c>
+      <c r="K211" s="109"/>
+      <c r="L211" s="109"/>
+      <c r="M211" s="109"/>
+      <c r="N211" s="111"/>
+    </row>
+    <row r="212" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B212" s="3"/>
       <c r="C212" s="3"/>
       <c r="D212" s="3"/>
@@ -14078,7 +14123,7 @@
       <c r="M212" s="3"/>
       <c r="N212" s="3"/>
     </row>
-    <row r="213" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B213" s="3"/>
       <c r="C213" s="3"/>
       <c r="D213" s="3"/>
@@ -14093,41 +14138,52 @@
       <c r="M213" s="3"/>
       <c r="N213" s="3"/>
     </row>
-    <row r="214" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="215" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="216" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B216" s="12"/>
-      <c r="C216" s="12"/>
-    </row>
-    <row r="217" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B214" s="3"/>
+      <c r="C214" s="3"/>
+      <c r="D214" s="3"/>
+      <c r="E214" s="3"/>
+      <c r="F214" s="3"/>
+      <c r="G214" s="3"/>
+      <c r="H214" s="3"/>
+      <c r="I214" s="3"/>
+      <c r="J214" s="3"/>
+      <c r="K214" s="3"/>
+      <c r="L214" s="3"/>
+      <c r="M214" s="3"/>
+      <c r="N214" s="3"/>
+    </row>
+    <row r="215" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="216" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="217" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B217" s="12"/>
       <c r="C217" s="12"/>
     </row>
-    <row r="218" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B218" s="12"/>
       <c r="C218" s="12"/>
     </row>
-    <row r="219" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B219" s="12"/>
       <c r="C219" s="12"/>
     </row>
-    <row r="220" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B220" s="12"/>
       <c r="C220" s="12"/>
     </row>
-    <row r="221" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B221" s="12"/>
       <c r="C221" s="12"/>
     </row>
-    <row r="222" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B222" s="12"/>
       <c r="C222" s="12"/>
     </row>
-    <row r="223" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B223" s="12"/>
       <c r="C223" s="12"/>
     </row>
-    <row r="224" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B224" s="12"/>
       <c r="C224" s="12"/>
     </row>
@@ -14147,16 +14203,29 @@
       <c r="B228" s="12"/>
       <c r="C228" s="12"/>
     </row>
-    <row r="229" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="229" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B229" s="12"/>
+      <c r="C229" s="12"/>
+    </row>
+    <row r="230" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="C150:C156"/>
-    <mergeCell ref="C136:C142"/>
-    <mergeCell ref="C122:C128"/>
-    <mergeCell ref="C115:C121"/>
-    <mergeCell ref="C101:C107"/>
-    <mergeCell ref="C129:C135"/>
-    <mergeCell ref="C143:C149"/>
+    <mergeCell ref="B187:B194"/>
+    <mergeCell ref="H209:I209"/>
+    <mergeCell ref="H211:I211"/>
+    <mergeCell ref="J211:N211"/>
+    <mergeCell ref="B14:B55"/>
+    <mergeCell ref="B206:G206"/>
+    <mergeCell ref="B171:B183"/>
+    <mergeCell ref="B195:B205"/>
+    <mergeCell ref="C108:C114"/>
+    <mergeCell ref="B184:B186"/>
+    <mergeCell ref="J207:W207"/>
+    <mergeCell ref="B66:B170"/>
+    <mergeCell ref="C157:C163"/>
+    <mergeCell ref="C164:C170"/>
+    <mergeCell ref="C94:C100"/>
+    <mergeCell ref="C87:C93"/>
     <mergeCell ref="C80:C86"/>
     <mergeCell ref="J2:W2"/>
     <mergeCell ref="B56:B65"/>
@@ -14168,22 +14237,13 @@
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="C66:C72"/>
     <mergeCell ref="C73:C79"/>
-    <mergeCell ref="B187:B193"/>
-    <mergeCell ref="H208:I208"/>
-    <mergeCell ref="H210:I210"/>
-    <mergeCell ref="J210:N210"/>
-    <mergeCell ref="B14:B55"/>
-    <mergeCell ref="B205:G205"/>
-    <mergeCell ref="B171:B183"/>
-    <mergeCell ref="B194:B204"/>
-    <mergeCell ref="C108:C114"/>
-    <mergeCell ref="B184:B186"/>
-    <mergeCell ref="J206:W206"/>
-    <mergeCell ref="B66:B170"/>
-    <mergeCell ref="C157:C163"/>
-    <mergeCell ref="C164:C170"/>
-    <mergeCell ref="C94:C100"/>
-    <mergeCell ref="C87:C93"/>
+    <mergeCell ref="C150:C156"/>
+    <mergeCell ref="C136:C142"/>
+    <mergeCell ref="C122:C128"/>
+    <mergeCell ref="C115:C121"/>
+    <mergeCell ref="C101:C107"/>
+    <mergeCell ref="C129:C135"/>
+    <mergeCell ref="C143:C149"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
excel y ya no peta al recibir y curarse a la vez
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
+++ b/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ENTI\MAP\MAP_LegendOfRadev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="162">
   <si>
     <t>Subtarea</t>
   </si>
@@ -491,9 +491,6 @@
     <t>Limitar el movimiento por la sala</t>
   </si>
   <si>
-    <t>0.2</t>
-  </si>
-  <si>
     <t>Crear Animación Spawn Enemigos</t>
   </si>
   <si>
@@ -507,9 +504,6 @@
   </si>
   <si>
     <t>Sonido vida baja</t>
-  </si>
-  <si>
-    <t>0.7</t>
   </si>
   <si>
     <t>0.5</t>
@@ -1078,7 +1072,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1302,9 +1296,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1351,10 +1342,43 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1363,13 +1387,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1405,34 +1426,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1503,28 +1500,28 @@
                   <c:v>95.792699999999968</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>86.499699999999962</c:v>
+                  <c:v>86.299699999999973</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>84.029699999999963</c:v>
+                  <c:v>83.829699999999974</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75.196699999999964</c:v>
+                  <c:v>74.996699999999976</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>68.004699999999971</c:v>
+                  <c:v>67.804699999999983</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>58.575699999999969</c:v>
+                  <c:v>57.675699999999985</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55.185699999999969</c:v>
+                  <c:v>45.785699999999984</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>55.185699999999969</c:v>
+                  <c:v>41.785699999999984</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>55.185699999999969</c:v>
+                  <c:v>41.785699999999984</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1584,6 +1581,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1928,8 +1926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W75" sqref="W75"/>
+    <sheetView tabSelected="1" topLeftCell="C160" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,22 +1957,22 @@
       <c r="I2" s="37">
         <v>3</v>
       </c>
-      <c r="J2" s="95" t="s">
+      <c r="J2" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="96"/>
-      <c r="U2" s="96"/>
-      <c r="V2" s="96"/>
-      <c r="W2" s="97"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="107"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="38" t="s">
@@ -2045,7 +2043,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="108" t="s">
+      <c r="B4" s="117" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="26" t="s">
@@ -2092,21 +2090,21 @@
       <c r="Q4" s="51">
         <v>0</v>
       </c>
-      <c r="R4" s="89">
+      <c r="R4" s="88">
         <v>1</v>
       </c>
-      <c r="S4" s="89" t="s">
-        <v>163</v>
-      </c>
-      <c r="T4" s="89" t="s">
-        <v>163</v>
-      </c>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="77"/>
+      <c r="S4" s="88" t="s">
+        <v>161</v>
+      </c>
+      <c r="T4" s="88" t="s">
+        <v>161</v>
+      </c>
+      <c r="U4" s="121"/>
+      <c r="V4" s="121"/>
+      <c r="W4" s="122"/>
     </row>
     <row r="5" spans="1:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="109"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="24" t="s">
         <v>91</v>
       </c>
@@ -2171,7 +2169,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="109"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="24" t="s">
         <v>92</v>
       </c>
@@ -2190,7 +2188,7 @@
       </c>
       <c r="I6" s="70">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J6" s="52">
         <v>0</v>
@@ -2225,12 +2223,18 @@
       <c r="T6" s="74">
         <v>6</v>
       </c>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="78"/>
+      <c r="U6" s="73">
+        <v>1</v>
+      </c>
+      <c r="V6" s="73">
+        <v>0</v>
+      </c>
+      <c r="W6" s="63">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="109"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="24" t="s">
         <v>93</v>
       </c>
@@ -2295,7 +2299,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="110"/>
+      <c r="B8" s="119"/>
       <c r="C8" s="30" t="s">
         <v>101</v>
       </c>
@@ -2314,7 +2318,7 @@
       </c>
       <c r="I8" s="16">
         <f t="shared" si="0"/>
-        <v>5.75</v>
+        <v>7.75</v>
       </c>
       <c r="J8" s="53">
         <v>0</v>
@@ -2340,27 +2344,27 @@
       <c r="Q8" s="76">
         <v>0.7</v>
       </c>
-      <c r="R8" s="87">
+      <c r="R8" s="86">
         <v>3.05</v>
       </c>
-      <c r="S8" s="87">
-        <v>0</v>
-      </c>
-      <c r="T8" s="87">
-        <v>0</v>
-      </c>
-      <c r="U8" s="87">
-        <v>0</v>
-      </c>
-      <c r="V8" s="87">
-        <v>0</v>
-      </c>
-      <c r="W8" s="88">
+      <c r="S8" s="86">
+        <v>0</v>
+      </c>
+      <c r="T8" s="86">
+        <v>0</v>
+      </c>
+      <c r="U8" s="86">
+        <v>2</v>
+      </c>
+      <c r="V8" s="86">
+        <v>0</v>
+      </c>
+      <c r="W8" s="87">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="117" t="s">
         <v>96</v>
       </c>
       <c r="C9" s="33" t="s">
@@ -2427,7 +2431,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="109"/>
+      <c r="B10" s="118"/>
       <c r="C10" s="23" t="s">
         <v>97</v>
       </c>
@@ -2483,10 +2487,10 @@
       </c>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
-      <c r="W10" s="78"/>
+      <c r="W10" s="77"/>
     </row>
     <row r="11" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="109"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="65" t="s">
         <v>102</v>
       </c>
@@ -2551,7 +2555,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="109"/>
+      <c r="B12" s="118"/>
       <c r="C12" s="65" t="s">
         <v>103</v>
       </c>
@@ -2616,7 +2620,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="110"/>
+      <c r="B13" s="119"/>
       <c r="C13" s="35" t="s">
         <v>88</v>
       </c>
@@ -2681,7 +2685,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="93" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="36" t="s">
@@ -2750,8 +2754,8 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B15" s="99"/>
-      <c r="C15" s="103" t="s">
+      <c r="B15" s="94"/>
+      <c r="C15" s="112" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -2817,8 +2821,8 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B16" s="99"/>
-      <c r="C16" s="104"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="113"/>
       <c r="D16" s="4" t="s">
         <v>19</v>
       </c>
@@ -2882,8 +2886,8 @@
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="99"/>
-      <c r="C17" s="104"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="113"/>
       <c r="D17" s="4" t="s">
         <v>20</v>
       </c>
@@ -2947,8 +2951,8 @@
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="99"/>
-      <c r="C18" s="104"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="113"/>
       <c r="D18" s="4" t="s">
         <v>21</v>
       </c>
@@ -3012,8 +3016,8 @@
       </c>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B19" s="99"/>
-      <c r="C19" s="104"/>
+      <c r="B19" s="94"/>
+      <c r="C19" s="113"/>
       <c r="D19" s="4" t="s">
         <v>22</v>
       </c>
@@ -3077,8 +3081,8 @@
       </c>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B20" s="99"/>
-      <c r="C20" s="104"/>
+      <c r="B20" s="94"/>
+      <c r="C20" s="113"/>
       <c r="D20" s="4" t="s">
         <v>153</v>
       </c>
@@ -3133,11 +3137,11 @@
       </c>
       <c r="U20" s="5"/>
       <c r="V20" s="5"/>
-      <c r="W20" s="78"/>
+      <c r="W20" s="77"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B21" s="99"/>
-      <c r="C21" s="104"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="113"/>
       <c r="D21" s="4" t="s">
         <v>23</v>
       </c>
@@ -3201,10 +3205,10 @@
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B22" s="99"/>
-      <c r="C22" s="104"/>
+      <c r="B22" s="94"/>
+      <c r="C22" s="113"/>
       <c r="D22" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>98</v>
@@ -3257,11 +3261,11 @@
       </c>
       <c r="U22" s="5"/>
       <c r="V22" s="5"/>
-      <c r="W22" s="78"/>
+      <c r="W22" s="77"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B23" s="99"/>
-      <c r="C23" s="104"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="113"/>
       <c r="D23" s="21" t="s">
         <v>35</v>
       </c>
@@ -3316,11 +3320,11 @@
       </c>
       <c r="U23" s="5"/>
       <c r="V23" s="5"/>
-      <c r="W23" s="78"/>
+      <c r="W23" s="77"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B24" s="99"/>
-      <c r="C24" s="104"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="113"/>
       <c r="D24" s="21" t="s">
         <v>36</v>
       </c>
@@ -3375,11 +3379,11 @@
       </c>
       <c r="U24" s="5"/>
       <c r="V24" s="5"/>
-      <c r="W24" s="78"/>
+      <c r="W24" s="77"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B25" s="99"/>
-      <c r="C25" s="104"/>
+      <c r="B25" s="94"/>
+      <c r="C25" s="113"/>
       <c r="D25" s="21" t="s">
         <v>37</v>
       </c>
@@ -3434,11 +3438,11 @@
       </c>
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
-      <c r="W25" s="78"/>
+      <c r="W25" s="77"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B26" s="99"/>
-      <c r="C26" s="104"/>
+      <c r="B26" s="94"/>
+      <c r="C26" s="113"/>
       <c r="D26" s="21" t="s">
         <v>38</v>
       </c>
@@ -3493,11 +3497,11 @@
       </c>
       <c r="U26" s="5"/>
       <c r="V26" s="5"/>
-      <c r="W26" s="78"/>
+      <c r="W26" s="77"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B27" s="99"/>
-      <c r="C27" s="104"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="113"/>
       <c r="D27" s="21" t="s">
         <v>39</v>
       </c>
@@ -3552,11 +3556,11 @@
       </c>
       <c r="U27" s="5"/>
       <c r="V27" s="5"/>
-      <c r="W27" s="78"/>
+      <c r="W27" s="77"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B28" s="99"/>
-      <c r="C28" s="104"/>
+      <c r="B28" s="94"/>
+      <c r="C28" s="113"/>
       <c r="D28" s="21" t="s">
         <v>40</v>
       </c>
@@ -3611,11 +3615,11 @@
       </c>
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>
-      <c r="W28" s="78"/>
+      <c r="W28" s="77"/>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B29" s="99"/>
-      <c r="C29" s="104"/>
+      <c r="B29" s="94"/>
+      <c r="C29" s="113"/>
       <c r="D29" s="21" t="s">
         <v>41</v>
       </c>
@@ -3670,11 +3674,11 @@
       </c>
       <c r="U29" s="5"/>
       <c r="V29" s="5"/>
-      <c r="W29" s="78"/>
+      <c r="W29" s="77"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B30" s="99"/>
-      <c r="C30" s="104"/>
+      <c r="B30" s="94"/>
+      <c r="C30" s="113"/>
       <c r="D30" s="21" t="s">
         <v>42</v>
       </c>
@@ -3729,11 +3733,11 @@
       </c>
       <c r="U30" s="5"/>
       <c r="V30" s="5"/>
-      <c r="W30" s="78"/>
+      <c r="W30" s="77"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B31" s="99"/>
-      <c r="C31" s="104"/>
+      <c r="B31" s="94"/>
+      <c r="C31" s="113"/>
       <c r="D31" s="21" t="s">
         <v>43</v>
       </c>
@@ -3788,11 +3792,11 @@
       </c>
       <c r="U31" s="5"/>
       <c r="V31" s="5"/>
-      <c r="W31" s="78"/>
+      <c r="W31" s="77"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B32" s="99"/>
-      <c r="C32" s="104"/>
+      <c r="B32" s="94"/>
+      <c r="C32" s="113"/>
       <c r="D32" s="21" t="s">
         <v>44</v>
       </c>
@@ -3847,11 +3851,11 @@
       </c>
       <c r="U32" s="5"/>
       <c r="V32" s="5"/>
-      <c r="W32" s="78"/>
+      <c r="W32" s="77"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B33" s="99"/>
-      <c r="C33" s="104"/>
+      <c r="B33" s="94"/>
+      <c r="C33" s="113"/>
       <c r="D33" s="21" t="s">
         <v>45</v>
       </c>
@@ -3906,11 +3910,11 @@
       </c>
       <c r="U33" s="5"/>
       <c r="V33" s="5"/>
-      <c r="W33" s="78"/>
+      <c r="W33" s="77"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B34" s="99"/>
-      <c r="C34" s="104"/>
+      <c r="B34" s="94"/>
+      <c r="C34" s="113"/>
       <c r="D34" s="21" t="s">
         <v>46</v>
       </c>
@@ -3965,11 +3969,11 @@
       </c>
       <c r="U34" s="5"/>
       <c r="V34" s="5"/>
-      <c r="W34" s="78"/>
+      <c r="W34" s="77"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35" s="99"/>
-      <c r="C35" s="104"/>
+      <c r="B35" s="94"/>
+      <c r="C35" s="113"/>
       <c r="D35" s="21" t="s">
         <v>47</v>
       </c>
@@ -4024,11 +4028,11 @@
       </c>
       <c r="U35" s="5"/>
       <c r="V35" s="5"/>
-      <c r="W35" s="78"/>
+      <c r="W35" s="77"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B36" s="99"/>
-      <c r="C36" s="104"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="113"/>
       <c r="D36" s="21" t="s">
         <v>48</v>
       </c>
@@ -4083,11 +4087,11 @@
       </c>
       <c r="U36" s="5"/>
       <c r="V36" s="5"/>
-      <c r="W36" s="78"/>
+      <c r="W36" s="77"/>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B37" s="99"/>
-      <c r="C37" s="104"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="113"/>
       <c r="D37" s="21" t="s">
         <v>49</v>
       </c>
@@ -4142,11 +4146,11 @@
       </c>
       <c r="U37" s="5"/>
       <c r="V37" s="5"/>
-      <c r="W37" s="78"/>
+      <c r="W37" s="77"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B38" s="99"/>
-      <c r="C38" s="104"/>
+      <c r="B38" s="94"/>
+      <c r="C38" s="113"/>
       <c r="D38" s="21" t="s">
         <v>50</v>
       </c>
@@ -4201,11 +4205,11 @@
       </c>
       <c r="U38" s="5"/>
       <c r="V38" s="5"/>
-      <c r="W38" s="78"/>
+      <c r="W38" s="77"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B39" s="99"/>
-      <c r="C39" s="104"/>
+      <c r="B39" s="94"/>
+      <c r="C39" s="113"/>
       <c r="D39" s="21" t="s">
         <v>51</v>
       </c>
@@ -4260,11 +4264,11 @@
       </c>
       <c r="U39" s="5"/>
       <c r="V39" s="5"/>
-      <c r="W39" s="78"/>
+      <c r="W39" s="77"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B40" s="99"/>
-      <c r="C40" s="104"/>
+      <c r="B40" s="94"/>
+      <c r="C40" s="113"/>
       <c r="D40" s="21" t="s">
         <v>52</v>
       </c>
@@ -4319,11 +4323,11 @@
       </c>
       <c r="U40" s="5"/>
       <c r="V40" s="5"/>
-      <c r="W40" s="78"/>
+      <c r="W40" s="77"/>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B41" s="99"/>
-      <c r="C41" s="104"/>
+      <c r="B41" s="94"/>
+      <c r="C41" s="113"/>
       <c r="D41" s="21" t="s">
         <v>53</v>
       </c>
@@ -4378,11 +4382,11 @@
       </c>
       <c r="U41" s="5"/>
       <c r="V41" s="5"/>
-      <c r="W41" s="78"/>
+      <c r="W41" s="77"/>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B42" s="99"/>
-      <c r="C42" s="104"/>
+      <c r="B42" s="94"/>
+      <c r="C42" s="113"/>
       <c r="D42" s="21" t="s">
         <v>54</v>
       </c>
@@ -4437,11 +4441,11 @@
       </c>
       <c r="U42" s="5"/>
       <c r="V42" s="5"/>
-      <c r="W42" s="78"/>
+      <c r="W42" s="77"/>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B43" s="99"/>
-      <c r="C43" s="104"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="113"/>
       <c r="D43" s="21" t="s">
         <v>55</v>
       </c>
@@ -4496,11 +4500,11 @@
       </c>
       <c r="U43" s="5"/>
       <c r="V43" s="5"/>
-      <c r="W43" s="78"/>
+      <c r="W43" s="77"/>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B44" s="99"/>
-      <c r="C44" s="104"/>
+      <c r="B44" s="94"/>
+      <c r="C44" s="113"/>
       <c r="D44" s="21" t="s">
         <v>56</v>
       </c>
@@ -4555,11 +4559,11 @@
       </c>
       <c r="U44" s="5"/>
       <c r="V44" s="5"/>
-      <c r="W44" s="78"/>
+      <c r="W44" s="77"/>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B45" s="99"/>
-      <c r="C45" s="104"/>
+      <c r="B45" s="94"/>
+      <c r="C45" s="113"/>
       <c r="D45" s="21" t="s">
         <v>57</v>
       </c>
@@ -4614,11 +4618,11 @@
       </c>
       <c r="U45" s="5"/>
       <c r="V45" s="5"/>
-      <c r="W45" s="78"/>
+      <c r="W45" s="77"/>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B46" s="99"/>
-      <c r="C46" s="104"/>
+      <c r="B46" s="94"/>
+      <c r="C46" s="113"/>
       <c r="D46" s="21" t="s">
         <v>58</v>
       </c>
@@ -4673,11 +4677,11 @@
       </c>
       <c r="U46" s="5"/>
       <c r="V46" s="5"/>
-      <c r="W46" s="78"/>
+      <c r="W46" s="77"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B47" s="99"/>
-      <c r="C47" s="104"/>
+      <c r="B47" s="94"/>
+      <c r="C47" s="113"/>
       <c r="D47" s="21" t="s">
         <v>59</v>
       </c>
@@ -4732,11 +4736,11 @@
       </c>
       <c r="U47" s="5"/>
       <c r="V47" s="5"/>
-      <c r="W47" s="78"/>
+      <c r="W47" s="77"/>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B48" s="99"/>
-      <c r="C48" s="104"/>
+      <c r="B48" s="94"/>
+      <c r="C48" s="113"/>
       <c r="D48" s="21" t="s">
         <v>60</v>
       </c>
@@ -4791,11 +4795,11 @@
       </c>
       <c r="U48" s="5"/>
       <c r="V48" s="5"/>
-      <c r="W48" s="78"/>
+      <c r="W48" s="77"/>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B49" s="99"/>
-      <c r="C49" s="101" t="s">
+      <c r="B49" s="94"/>
+      <c r="C49" s="110" t="s">
         <v>25</v>
       </c>
       <c r="D49" s="18" t="s">
@@ -4852,11 +4856,11 @@
       </c>
       <c r="U49" s="5"/>
       <c r="V49" s="5"/>
-      <c r="W49" s="78"/>
+      <c r="W49" s="77"/>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B50" s="99"/>
-      <c r="C50" s="102"/>
+      <c r="B50" s="94"/>
+      <c r="C50" s="111"/>
       <c r="D50" s="18" t="s">
         <v>28</v>
       </c>
@@ -4911,11 +4915,11 @@
       </c>
       <c r="U50" s="5"/>
       <c r="V50" s="5"/>
-      <c r="W50" s="78"/>
+      <c r="W50" s="77"/>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B51" s="99"/>
-      <c r="C51" s="102"/>
+      <c r="B51" s="94"/>
+      <c r="C51" s="111"/>
       <c r="D51" s="18" t="s">
         <v>29</v>
       </c>
@@ -4970,11 +4974,11 @@
       </c>
       <c r="U51" s="5"/>
       <c r="V51" s="5"/>
-      <c r="W51" s="78"/>
+      <c r="W51" s="77"/>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B52" s="99"/>
-      <c r="C52" s="102"/>
+      <c r="B52" s="94"/>
+      <c r="C52" s="111"/>
       <c r="D52" s="18" t="s">
         <v>30</v>
       </c>
@@ -5029,11 +5033,11 @@
       </c>
       <c r="U52" s="5"/>
       <c r="V52" s="5"/>
-      <c r="W52" s="78"/>
+      <c r="W52" s="77"/>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B53" s="99"/>
-      <c r="C53" s="102"/>
+      <c r="B53" s="94"/>
+      <c r="C53" s="111"/>
       <c r="D53" s="18" t="s">
         <v>33</v>
       </c>
@@ -5088,11 +5092,11 @@
       </c>
       <c r="U53" s="5"/>
       <c r="V53" s="5"/>
-      <c r="W53" s="78"/>
+      <c r="W53" s="77"/>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B54" s="99"/>
-      <c r="C54" s="102"/>
+      <c r="B54" s="94"/>
+      <c r="C54" s="111"/>
       <c r="D54" s="18" t="s">
         <v>31</v>
       </c>
@@ -5147,11 +5151,11 @@
       </c>
       <c r="U54" s="5"/>
       <c r="V54" s="5"/>
-      <c r="W54" s="78"/>
+      <c r="W54" s="77"/>
     </row>
     <row r="55" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="116"/>
-      <c r="C55" s="102"/>
+      <c r="B55" s="101"/>
+      <c r="C55" s="111"/>
       <c r="D55" s="44" t="s">
         <v>32</v>
       </c>
@@ -5204,15 +5208,15 @@
       <c r="T55" s="54">
         <v>0</v>
       </c>
-      <c r="U55" s="80"/>
-      <c r="V55" s="80"/>
-      <c r="W55" s="81"/>
+      <c r="U55" s="79"/>
+      <c r="V55" s="79"/>
+      <c r="W55" s="80"/>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B56" s="98" t="s">
+      <c r="B56" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="105" t="s">
+      <c r="C56" s="114" t="s">
         <v>70</v>
       </c>
       <c r="D56" s="28" t="s">
@@ -5269,11 +5273,11 @@
       </c>
       <c r="U56" s="34"/>
       <c r="V56" s="34"/>
-      <c r="W56" s="82"/>
+      <c r="W56" s="81"/>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B57" s="99"/>
-      <c r="C57" s="106"/>
+      <c r="B57" s="94"/>
+      <c r="C57" s="115"/>
       <c r="D57" s="4" t="s">
         <v>62</v>
       </c>
@@ -5328,11 +5332,11 @@
       </c>
       <c r="U57" s="5"/>
       <c r="V57" s="5"/>
-      <c r="W57" s="78"/>
+      <c r="W57" s="77"/>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B58" s="99"/>
-      <c r="C58" s="106"/>
+      <c r="B58" s="94"/>
+      <c r="C58" s="115"/>
       <c r="D58" s="4" t="s">
         <v>63</v>
       </c>
@@ -5387,11 +5391,11 @@
       </c>
       <c r="U58" s="5"/>
       <c r="V58" s="5"/>
-      <c r="W58" s="78"/>
+      <c r="W58" s="77"/>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B59" s="99"/>
-      <c r="C59" s="106"/>
+      <c r="B59" s="94"/>
+      <c r="C59" s="115"/>
       <c r="D59" s="18" t="s">
         <v>67</v>
       </c>
@@ -5446,10 +5450,10 @@
       </c>
       <c r="U59" s="5"/>
       <c r="V59" s="5"/>
-      <c r="W59" s="78"/>
+      <c r="W59" s="77"/>
     </row>
     <row r="60" spans="2:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B60" s="99"/>
+      <c r="B60" s="94"/>
       <c r="C60" s="22" t="s">
         <v>64</v>
       </c>
@@ -5505,10 +5509,10 @@
       </c>
       <c r="U60" s="5"/>
       <c r="V60" s="5"/>
-      <c r="W60" s="78"/>
+      <c r="W60" s="77"/>
     </row>
     <row r="61" spans="2:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B61" s="99"/>
+      <c r="B61" s="94"/>
       <c r="C61" s="22" t="s">
         <v>72</v>
       </c>
@@ -5564,11 +5568,11 @@
       </c>
       <c r="U61" s="5"/>
       <c r="V61" s="5"/>
-      <c r="W61" s="78"/>
+      <c r="W61" s="77"/>
     </row>
     <row r="62" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="99"/>
-      <c r="C62" s="106" t="s">
+      <c r="B62" s="94"/>
+      <c r="C62" s="115" t="s">
         <v>71</v>
       </c>
       <c r="D62" s="4" t="s">
@@ -5625,11 +5629,11 @@
       </c>
       <c r="U62" s="5"/>
       <c r="V62" s="5"/>
-      <c r="W62" s="78"/>
+      <c r="W62" s="77"/>
     </row>
     <row r="63" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="99"/>
-      <c r="C63" s="106"/>
+      <c r="B63" s="94"/>
+      <c r="C63" s="115"/>
       <c r="D63" s="4" t="s">
         <v>66</v>
       </c>
@@ -5684,11 +5688,11 @@
       </c>
       <c r="U63" s="5"/>
       <c r="V63" s="5"/>
-      <c r="W63" s="78"/>
+      <c r="W63" s="77"/>
     </row>
     <row r="64" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="99"/>
-      <c r="C64" s="106"/>
+      <c r="B64" s="94"/>
+      <c r="C64" s="115"/>
       <c r="D64" s="4" t="s">
         <v>68</v>
       </c>
@@ -5743,11 +5747,11 @@
       </c>
       <c r="U64" s="5"/>
       <c r="V64" s="5"/>
-      <c r="W64" s="78"/>
+      <c r="W64" s="77"/>
     </row>
     <row r="65" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="100"/>
-      <c r="C65" s="107"/>
+      <c r="B65" s="95"/>
+      <c r="C65" s="116"/>
       <c r="D65" s="17" t="s">
         <v>69</v>
       </c>
@@ -5802,13 +5806,13 @@
       </c>
       <c r="U65" s="31"/>
       <c r="V65" s="31"/>
-      <c r="W65" s="79"/>
+      <c r="W65" s="78"/>
     </row>
     <row r="66" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="98" t="s">
+      <c r="B66" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="C66" s="111" t="s">
+      <c r="C66" s="120" t="s">
         <v>107</v>
       </c>
       <c r="D66" s="28" t="s">
@@ -5874,8 +5878,8 @@
       </c>
     </row>
     <row r="67" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="99"/>
-      <c r="C67" s="94"/>
+      <c r="B67" s="94"/>
+      <c r="C67" s="105"/>
       <c r="D67" s="4" t="s">
         <v>123</v>
       </c>
@@ -5939,8 +5943,8 @@
       </c>
     </row>
     <row r="68" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="99"/>
-      <c r="C68" s="94"/>
+      <c r="B68" s="94"/>
+      <c r="C68" s="105"/>
       <c r="D68" s="4" t="s">
         <v>152</v>
       </c>
@@ -5995,11 +5999,11 @@
       </c>
       <c r="U68" s="5"/>
       <c r="V68" s="5"/>
-      <c r="W68" s="78"/>
+      <c r="W68" s="77"/>
     </row>
     <row r="69" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="99"/>
-      <c r="C69" s="94"/>
+      <c r="B69" s="94"/>
+      <c r="C69" s="105"/>
       <c r="D69" s="4" t="s">
         <v>124</v>
       </c>
@@ -6063,8 +6067,8 @@
       </c>
     </row>
     <row r="70" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="99"/>
-      <c r="C70" s="94"/>
+      <c r="B70" s="94"/>
+      <c r="C70" s="105"/>
       <c r="D70" s="4" t="s">
         <v>155</v>
       </c>
@@ -6117,13 +6121,13 @@
       <c r="T70" s="52">
         <v>0</v>
       </c>
-      <c r="U70" s="83"/>
-      <c r="V70" s="83"/>
-      <c r="W70" s="84"/>
+      <c r="U70" s="82"/>
+      <c r="V70" s="82"/>
+      <c r="W70" s="83"/>
     </row>
     <row r="71" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="99"/>
-      <c r="C71" s="94"/>
+      <c r="B71" s="94"/>
+      <c r="C71" s="105"/>
       <c r="D71" s="4" t="s">
         <v>154</v>
       </c>
@@ -6187,8 +6191,8 @@
       </c>
     </row>
     <row r="72" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="99"/>
-      <c r="C72" s="94"/>
+      <c r="B72" s="94"/>
+      <c r="C72" s="105"/>
       <c r="D72" s="4" t="s">
         <v>125</v>
       </c>
@@ -6243,11 +6247,11 @@
       </c>
       <c r="U72" s="5"/>
       <c r="V72" s="5"/>
-      <c r="W72" s="78"/>
+      <c r="W72" s="77"/>
     </row>
     <row r="73" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="99"/>
-      <c r="C73" s="94" t="s">
+      <c r="B73" s="94"/>
+      <c r="C73" s="105" t="s">
         <v>108</v>
       </c>
       <c r="D73" s="4" t="s">
@@ -6313,8 +6317,8 @@
       </c>
     </row>
     <row r="74" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="99"/>
-      <c r="C74" s="94"/>
+      <c r="B74" s="94"/>
+      <c r="C74" s="105"/>
       <c r="D74" s="4" t="s">
         <v>123</v>
       </c>
@@ -6369,11 +6373,11 @@
       </c>
       <c r="U74" s="5"/>
       <c r="V74" s="5"/>
-      <c r="W74" s="78"/>
+      <c r="W74" s="77"/>
     </row>
     <row r="75" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="99"/>
-      <c r="C75" s="94"/>
+      <c r="B75" s="94"/>
+      <c r="C75" s="105"/>
       <c r="D75" s="4" t="s">
         <v>152</v>
       </c>
@@ -6428,11 +6432,11 @@
       </c>
       <c r="U75" s="5"/>
       <c r="V75" s="5"/>
-      <c r="W75" s="78"/>
+      <c r="W75" s="77"/>
     </row>
     <row r="76" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="99"/>
-      <c r="C76" s="94"/>
+      <c r="B76" s="94"/>
+      <c r="C76" s="105"/>
       <c r="D76" s="4" t="s">
         <v>155</v>
       </c>
@@ -6487,11 +6491,11 @@
       </c>
       <c r="U76" s="5"/>
       <c r="V76" s="5"/>
-      <c r="W76" s="78"/>
+      <c r="W76" s="77"/>
     </row>
     <row r="77" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="99"/>
-      <c r="C77" s="94"/>
+      <c r="B77" s="94"/>
+      <c r="C77" s="105"/>
       <c r="D77" s="4" t="s">
         <v>154</v>
       </c>
@@ -6551,8 +6555,8 @@
       <c r="W77" s="63"/>
     </row>
     <row r="78" spans="2:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="99"/>
-      <c r="C78" s="94"/>
+      <c r="B78" s="94"/>
+      <c r="C78" s="105"/>
       <c r="D78" s="4" t="s">
         <v>124</v>
       </c>
@@ -6616,8 +6620,8 @@
       </c>
     </row>
     <row r="79" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="99"/>
-      <c r="C79" s="94"/>
+      <c r="B79" s="94"/>
+      <c r="C79" s="105"/>
       <c r="D79" s="4" t="s">
         <v>125</v>
       </c>
@@ -6672,11 +6676,11 @@
       </c>
       <c r="U79" s="5"/>
       <c r="V79" s="5"/>
-      <c r="W79" s="78"/>
+      <c r="W79" s="77"/>
     </row>
     <row r="80" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="99"/>
-      <c r="C80" s="94" t="s">
+      <c r="B80" s="94"/>
+      <c r="C80" s="105" t="s">
         <v>109</v>
       </c>
       <c r="D80" s="4" t="s">
@@ -6742,8 +6746,8 @@
       </c>
     </row>
     <row r="81" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="99"/>
-      <c r="C81" s="94"/>
+      <c r="B81" s="94"/>
+      <c r="C81" s="105"/>
       <c r="D81" s="4" t="s">
         <v>123</v>
       </c>
@@ -6798,11 +6802,11 @@
       </c>
       <c r="U81" s="5"/>
       <c r="V81" s="5"/>
-      <c r="W81" s="78"/>
+      <c r="W81" s="77"/>
     </row>
     <row r="82" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="99"/>
-      <c r="C82" s="94"/>
+      <c r="B82" s="94"/>
+      <c r="C82" s="105"/>
       <c r="D82" s="4" t="s">
         <v>152</v>
       </c>
@@ -6857,11 +6861,11 @@
       </c>
       <c r="U82" s="5"/>
       <c r="V82" s="5"/>
-      <c r="W82" s="78"/>
+      <c r="W82" s="77"/>
     </row>
     <row r="83" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="99"/>
-      <c r="C83" s="94"/>
+      <c r="B83" s="94"/>
+      <c r="C83" s="105"/>
       <c r="D83" s="4" t="s">
         <v>124</v>
       </c>
@@ -6925,8 +6929,8 @@
       </c>
     </row>
     <row r="84" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="99"/>
-      <c r="C84" s="94"/>
+      <c r="B84" s="94"/>
+      <c r="C84" s="105"/>
       <c r="D84" s="4" t="s">
         <v>155</v>
       </c>
@@ -6979,13 +6983,13 @@
       <c r="T84" s="52">
         <v>0</v>
       </c>
-      <c r="U84" s="83"/>
-      <c r="V84" s="83"/>
-      <c r="W84" s="84"/>
+      <c r="U84" s="82"/>
+      <c r="V84" s="82"/>
+      <c r="W84" s="83"/>
     </row>
     <row r="85" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="99"/>
-      <c r="C85" s="94"/>
+      <c r="B85" s="94"/>
+      <c r="C85" s="105"/>
       <c r="D85" s="4" t="s">
         <v>154</v>
       </c>
@@ -7049,8 +7053,8 @@
       </c>
     </row>
     <row r="86" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="99"/>
-      <c r="C86" s="94"/>
+      <c r="B86" s="94"/>
+      <c r="C86" s="105"/>
       <c r="D86" s="4" t="s">
         <v>125</v>
       </c>
@@ -7105,11 +7109,11 @@
       </c>
       <c r="U86" s="5"/>
       <c r="V86" s="5"/>
-      <c r="W86" s="78"/>
+      <c r="W86" s="77"/>
     </row>
     <row r="87" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="99"/>
-      <c r="C87" s="94" t="s">
+      <c r="B87" s="94"/>
+      <c r="C87" s="105" t="s">
         <v>110</v>
       </c>
       <c r="D87" s="4" t="s">
@@ -7175,8 +7179,8 @@
       </c>
     </row>
     <row r="88" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="99"/>
-      <c r="C88" s="94"/>
+      <c r="B88" s="94"/>
+      <c r="C88" s="105"/>
       <c r="D88" s="4" t="s">
         <v>123</v>
       </c>
@@ -7231,11 +7235,11 @@
       </c>
       <c r="U88" s="5"/>
       <c r="V88" s="5"/>
-      <c r="W88" s="78"/>
+      <c r="W88" s="77"/>
     </row>
     <row r="89" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="99"/>
-      <c r="C89" s="94"/>
+      <c r="B89" s="94"/>
+      <c r="C89" s="105"/>
       <c r="D89" s="4" t="s">
         <v>152</v>
       </c>
@@ -7290,11 +7294,11 @@
       </c>
       <c r="U89" s="5"/>
       <c r="V89" s="5"/>
-      <c r="W89" s="78"/>
+      <c r="W89" s="77"/>
     </row>
     <row r="90" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="99"/>
-      <c r="C90" s="94"/>
+      <c r="B90" s="94"/>
+      <c r="C90" s="105"/>
       <c r="D90" s="4" t="s">
         <v>124</v>
       </c>
@@ -7358,8 +7362,8 @@
       </c>
     </row>
     <row r="91" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="99"/>
-      <c r="C91" s="94"/>
+      <c r="B91" s="94"/>
+      <c r="C91" s="105"/>
       <c r="D91" s="4" t="s">
         <v>155</v>
       </c>
@@ -7412,13 +7416,13 @@
       <c r="T91" s="52">
         <v>0</v>
       </c>
-      <c r="U91" s="83"/>
-      <c r="V91" s="83"/>
-      <c r="W91" s="84"/>
+      <c r="U91" s="82"/>
+      <c r="V91" s="82"/>
+      <c r="W91" s="83"/>
     </row>
     <row r="92" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="99"/>
-      <c r="C92" s="94"/>
+      <c r="B92" s="94"/>
+      <c r="C92" s="105"/>
       <c r="D92" s="4" t="s">
         <v>154</v>
       </c>
@@ -7478,8 +7482,8 @@
       <c r="W92" s="63"/>
     </row>
     <row r="93" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="99"/>
-      <c r="C93" s="94"/>
+      <c r="B93" s="94"/>
+      <c r="C93" s="105"/>
       <c r="D93" s="4" t="s">
         <v>125</v>
       </c>
@@ -7534,11 +7538,11 @@
       </c>
       <c r="U93" s="5"/>
       <c r="V93" s="5"/>
-      <c r="W93" s="78"/>
+      <c r="W93" s="77"/>
     </row>
     <row r="94" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="99"/>
-      <c r="C94" s="94" t="s">
+      <c r="B94" s="94"/>
+      <c r="C94" s="105" t="s">
         <v>111</v>
       </c>
       <c r="D94" s="4" t="s">
@@ -7604,8 +7608,8 @@
       </c>
     </row>
     <row r="95" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="99"/>
-      <c r="C95" s="94"/>
+      <c r="B95" s="94"/>
+      <c r="C95" s="105"/>
       <c r="D95" s="4" t="s">
         <v>123</v>
       </c>
@@ -7660,11 +7664,11 @@
       </c>
       <c r="U95" s="5"/>
       <c r="V95" s="5"/>
-      <c r="W95" s="78"/>
+      <c r="W95" s="77"/>
     </row>
     <row r="96" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="99"/>
-      <c r="C96" s="94"/>
+      <c r="B96" s="94"/>
+      <c r="C96" s="105"/>
       <c r="D96" s="4" t="s">
         <v>152</v>
       </c>
@@ -7719,11 +7723,11 @@
       </c>
       <c r="U96" s="5"/>
       <c r="V96" s="5"/>
-      <c r="W96" s="78"/>
+      <c r="W96" s="77"/>
     </row>
     <row r="97" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="99"/>
-      <c r="C97" s="94"/>
+      <c r="B97" s="94"/>
+      <c r="C97" s="105"/>
       <c r="D97" s="4" t="s">
         <v>124</v>
       </c>
@@ -7787,8 +7791,8 @@
       </c>
     </row>
     <row r="98" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="99"/>
-      <c r="C98" s="94"/>
+      <c r="B98" s="94"/>
+      <c r="C98" s="105"/>
       <c r="D98" s="4" t="s">
         <v>155</v>
       </c>
@@ -7841,13 +7845,13 @@
       <c r="T98" s="52">
         <v>0</v>
       </c>
-      <c r="U98" s="83"/>
-      <c r="V98" s="83"/>
-      <c r="W98" s="84"/>
+      <c r="U98" s="82"/>
+      <c r="V98" s="82"/>
+      <c r="W98" s="83"/>
     </row>
     <row r="99" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="99"/>
-      <c r="C99" s="94"/>
+      <c r="B99" s="94"/>
+      <c r="C99" s="105"/>
       <c r="D99" s="4" t="s">
         <v>154</v>
       </c>
@@ -7911,8 +7915,8 @@
       </c>
     </row>
     <row r="100" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="99"/>
-      <c r="C100" s="94"/>
+      <c r="B100" s="94"/>
+      <c r="C100" s="105"/>
       <c r="D100" s="4" t="s">
         <v>125</v>
       </c>
@@ -7967,11 +7971,11 @@
       </c>
       <c r="U100" s="5"/>
       <c r="V100" s="5"/>
-      <c r="W100" s="78"/>
+      <c r="W100" s="77"/>
     </row>
     <row r="101" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="99"/>
-      <c r="C101" s="94" t="s">
+      <c r="B101" s="94"/>
+      <c r="C101" s="105" t="s">
         <v>112</v>
       </c>
       <c r="D101" s="4" t="s">
@@ -8037,8 +8041,8 @@
       </c>
     </row>
     <row r="102" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="99"/>
-      <c r="C102" s="94"/>
+      <c r="B102" s="94"/>
+      <c r="C102" s="105"/>
       <c r="D102" s="4" t="s">
         <v>123</v>
       </c>
@@ -8093,11 +8097,11 @@
       </c>
       <c r="U102" s="5"/>
       <c r="V102" s="5"/>
-      <c r="W102" s="78"/>
+      <c r="W102" s="77"/>
     </row>
     <row r="103" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="99"/>
-      <c r="C103" s="94"/>
+      <c r="B103" s="94"/>
+      <c r="C103" s="105"/>
       <c r="D103" s="4" t="s">
         <v>152</v>
       </c>
@@ -8152,11 +8156,11 @@
       </c>
       <c r="U103" s="5"/>
       <c r="V103" s="5"/>
-      <c r="W103" s="78"/>
+      <c r="W103" s="77"/>
     </row>
     <row r="104" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="99"/>
-      <c r="C104" s="94"/>
+      <c r="B104" s="94"/>
+      <c r="C104" s="105"/>
       <c r="D104" s="4" t="s">
         <v>124</v>
       </c>
@@ -8220,8 +8224,8 @@
       </c>
     </row>
     <row r="105" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="99"/>
-      <c r="C105" s="94"/>
+      <c r="B105" s="94"/>
+      <c r="C105" s="105"/>
       <c r="D105" s="4" t="s">
         <v>155</v>
       </c>
@@ -8274,13 +8278,13 @@
       <c r="T105" s="52">
         <v>0</v>
       </c>
-      <c r="U105" s="83"/>
-      <c r="V105" s="83"/>
-      <c r="W105" s="84"/>
+      <c r="U105" s="82"/>
+      <c r="V105" s="82"/>
+      <c r="W105" s="83"/>
     </row>
     <row r="106" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="99"/>
-      <c r="C106" s="94"/>
+      <c r="B106" s="94"/>
+      <c r="C106" s="105"/>
       <c r="D106" s="4" t="s">
         <v>154</v>
       </c>
@@ -8340,8 +8344,8 @@
       <c r="W106" s="63"/>
     </row>
     <row r="107" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="99"/>
-      <c r="C107" s="94"/>
+      <c r="B107" s="94"/>
+      <c r="C107" s="105"/>
       <c r="D107" s="4" t="s">
         <v>125</v>
       </c>
@@ -8394,14 +8398,14 @@
       <c r="T107" s="52">
         <v>0</v>
       </c>
-      <c r="U107" s="83"/>
-      <c r="V107" s="83"/>
-      <c r="W107" s="84"/>
-      <c r="X107" s="93"/>
+      <c r="U107" s="82"/>
+      <c r="V107" s="82"/>
+      <c r="W107" s="83"/>
+      <c r="X107" s="92"/>
     </row>
     <row r="108" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="99"/>
-      <c r="C108" s="94" t="s">
+      <c r="B108" s="94"/>
+      <c r="C108" s="105" t="s">
         <v>113</v>
       </c>
       <c r="D108" s="4" t="s">
@@ -8467,8 +8471,8 @@
       </c>
     </row>
     <row r="109" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="99"/>
-      <c r="C109" s="94"/>
+      <c r="B109" s="94"/>
+      <c r="C109" s="105"/>
       <c r="D109" s="4" t="s">
         <v>123</v>
       </c>
@@ -8523,11 +8527,11 @@
       </c>
       <c r="U109" s="5"/>
       <c r="V109" s="5"/>
-      <c r="W109" s="78"/>
+      <c r="W109" s="77"/>
     </row>
     <row r="110" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="99"/>
-      <c r="C110" s="94"/>
+      <c r="B110" s="94"/>
+      <c r="C110" s="105"/>
       <c r="D110" s="4" t="s">
         <v>152</v>
       </c>
@@ -8582,11 +8586,11 @@
       </c>
       <c r="U110" s="5"/>
       <c r="V110" s="5"/>
-      <c r="W110" s="78"/>
+      <c r="W110" s="77"/>
     </row>
     <row r="111" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="99"/>
-      <c r="C111" s="94"/>
+      <c r="B111" s="94"/>
+      <c r="C111" s="105"/>
       <c r="D111" s="4" t="s">
         <v>124</v>
       </c>
@@ -8650,8 +8654,8 @@
       </c>
     </row>
     <row r="112" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="99"/>
-      <c r="C112" s="94"/>
+      <c r="B112" s="94"/>
+      <c r="C112" s="105"/>
       <c r="D112" s="4" t="s">
         <v>155</v>
       </c>
@@ -8704,13 +8708,13 @@
       <c r="T112" s="52">
         <v>0</v>
       </c>
-      <c r="U112" s="83"/>
-      <c r="V112" s="83"/>
-      <c r="W112" s="84"/>
+      <c r="U112" s="82"/>
+      <c r="V112" s="82"/>
+      <c r="W112" s="83"/>
     </row>
     <row r="113" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="99"/>
-      <c r="C113" s="94"/>
+      <c r="B113" s="94"/>
+      <c r="C113" s="105"/>
       <c r="D113" s="4" t="s">
         <v>154</v>
       </c>
@@ -8770,8 +8774,8 @@
       <c r="W113" s="63"/>
     </row>
     <row r="114" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="99"/>
-      <c r="C114" s="94"/>
+      <c r="B114" s="94"/>
+      <c r="C114" s="105"/>
       <c r="D114" s="4" t="s">
         <v>125</v>
       </c>
@@ -8826,11 +8830,11 @@
       </c>
       <c r="U114" s="5"/>
       <c r="V114" s="5"/>
-      <c r="W114" s="78"/>
+      <c r="W114" s="77"/>
     </row>
     <row r="115" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="99"/>
-      <c r="C115" s="94" t="s">
+      <c r="B115" s="94"/>
+      <c r="C115" s="105" t="s">
         <v>114</v>
       </c>
       <c r="D115" s="4" t="s">
@@ -8896,8 +8900,8 @@
       </c>
     </row>
     <row r="116" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="99"/>
-      <c r="C116" s="94"/>
+      <c r="B116" s="94"/>
+      <c r="C116" s="105"/>
       <c r="D116" s="4" t="s">
         <v>123</v>
       </c>
@@ -8952,11 +8956,11 @@
       </c>
       <c r="U116" s="5"/>
       <c r="V116" s="5"/>
-      <c r="W116" s="78"/>
+      <c r="W116" s="77"/>
     </row>
     <row r="117" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="99"/>
-      <c r="C117" s="94"/>
+      <c r="B117" s="94"/>
+      <c r="C117" s="105"/>
       <c r="D117" s="4" t="s">
         <v>152</v>
       </c>
@@ -9011,11 +9015,11 @@
       </c>
       <c r="U117" s="5"/>
       <c r="V117" s="5"/>
-      <c r="W117" s="78"/>
+      <c r="W117" s="77"/>
     </row>
     <row r="118" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="99"/>
-      <c r="C118" s="94"/>
+      <c r="B118" s="94"/>
+      <c r="C118" s="105"/>
       <c r="D118" s="4" t="s">
         <v>124</v>
       </c>
@@ -9079,8 +9083,8 @@
       </c>
     </row>
     <row r="119" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="99"/>
-      <c r="C119" s="94"/>
+      <c r="B119" s="94"/>
+      <c r="C119" s="105"/>
       <c r="D119" s="4" t="s">
         <v>155</v>
       </c>
@@ -9133,13 +9137,13 @@
       <c r="T119" s="52">
         <v>0</v>
       </c>
-      <c r="U119" s="83"/>
-      <c r="V119" s="83"/>
-      <c r="W119" s="84"/>
+      <c r="U119" s="82"/>
+      <c r="V119" s="82"/>
+      <c r="W119" s="83"/>
     </row>
     <row r="120" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="99"/>
-      <c r="C120" s="94"/>
+      <c r="B120" s="94"/>
+      <c r="C120" s="105"/>
       <c r="D120" s="4" t="s">
         <v>154</v>
       </c>
@@ -9203,8 +9207,8 @@
       </c>
     </row>
     <row r="121" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="99"/>
-      <c r="C121" s="94"/>
+      <c r="B121" s="94"/>
+      <c r="C121" s="105"/>
       <c r="D121" s="4" t="s">
         <v>125</v>
       </c>
@@ -9259,11 +9263,11 @@
       </c>
       <c r="U121" s="5"/>
       <c r="V121" s="5"/>
-      <c r="W121" s="78"/>
+      <c r="W121" s="77"/>
     </row>
     <row r="122" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="99"/>
-      <c r="C122" s="94" t="s">
+      <c r="B122" s="94"/>
+      <c r="C122" s="105" t="s">
         <v>115</v>
       </c>
       <c r="D122" s="4" t="s">
@@ -9329,8 +9333,8 @@
       </c>
     </row>
     <row r="123" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="99"/>
-      <c r="C123" s="94"/>
+      <c r="B123" s="94"/>
+      <c r="C123" s="105"/>
       <c r="D123" s="4" t="s">
         <v>123</v>
       </c>
@@ -9385,11 +9389,11 @@
       </c>
       <c r="U123" s="5"/>
       <c r="V123" s="5"/>
-      <c r="W123" s="78"/>
+      <c r="W123" s="77"/>
     </row>
     <row r="124" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="99"/>
-      <c r="C124" s="94"/>
+      <c r="B124" s="94"/>
+      <c r="C124" s="105"/>
       <c r="D124" s="4" t="s">
         <v>152</v>
       </c>
@@ -9444,11 +9448,11 @@
       </c>
       <c r="U124" s="5"/>
       <c r="V124" s="5"/>
-      <c r="W124" s="78"/>
+      <c r="W124" s="77"/>
     </row>
     <row r="125" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="99"/>
-      <c r="C125" s="94"/>
+      <c r="B125" s="94"/>
+      <c r="C125" s="105"/>
       <c r="D125" s="4" t="s">
         <v>124</v>
       </c>
@@ -9512,8 +9516,8 @@
       </c>
     </row>
     <row r="126" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="99"/>
-      <c r="C126" s="94"/>
+      <c r="B126" s="94"/>
+      <c r="C126" s="105"/>
       <c r="D126" s="4" t="s">
         <v>155</v>
       </c>
@@ -9566,13 +9570,13 @@
       <c r="T126" s="52">
         <v>0</v>
       </c>
-      <c r="U126" s="83"/>
-      <c r="V126" s="83"/>
-      <c r="W126" s="84"/>
+      <c r="U126" s="82"/>
+      <c r="V126" s="82"/>
+      <c r="W126" s="83"/>
     </row>
     <row r="127" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="99"/>
-      <c r="C127" s="94"/>
+      <c r="B127" s="94"/>
+      <c r="C127" s="105"/>
       <c r="D127" s="4" t="s">
         <v>154</v>
       </c>
@@ -9632,8 +9636,8 @@
       <c r="W127" s="63"/>
     </row>
     <row r="128" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="99"/>
-      <c r="C128" s="94"/>
+      <c r="B128" s="94"/>
+      <c r="C128" s="105"/>
       <c r="D128" s="4" t="s">
         <v>125</v>
       </c>
@@ -9688,11 +9692,11 @@
       </c>
       <c r="U128" s="5"/>
       <c r="V128" s="5"/>
-      <c r="W128" s="78"/>
+      <c r="W128" s="77"/>
     </row>
     <row r="129" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="99"/>
-      <c r="C129" s="94" t="s">
+      <c r="B129" s="94"/>
+      <c r="C129" s="105" t="s">
         <v>116</v>
       </c>
       <c r="D129" s="4" t="s">
@@ -9758,8 +9762,8 @@
       </c>
     </row>
     <row r="130" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="99"/>
-      <c r="C130" s="94"/>
+      <c r="B130" s="94"/>
+      <c r="C130" s="105"/>
       <c r="D130" s="4" t="s">
         <v>123</v>
       </c>
@@ -9814,11 +9818,11 @@
       </c>
       <c r="U130" s="5"/>
       <c r="V130" s="5"/>
-      <c r="W130" s="78"/>
+      <c r="W130" s="77"/>
     </row>
     <row r="131" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="99"/>
-      <c r="C131" s="94"/>
+      <c r="B131" s="94"/>
+      <c r="C131" s="105"/>
       <c r="D131" s="4" t="s">
         <v>152</v>
       </c>
@@ -9873,11 +9877,11 @@
       </c>
       <c r="U131" s="5"/>
       <c r="V131" s="5"/>
-      <c r="W131" s="78"/>
+      <c r="W131" s="77"/>
     </row>
     <row r="132" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="99"/>
-      <c r="C132" s="94"/>
+      <c r="B132" s="94"/>
+      <c r="C132" s="105"/>
       <c r="D132" s="4" t="s">
         <v>124</v>
       </c>
@@ -9941,8 +9945,8 @@
       </c>
     </row>
     <row r="133" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="99"/>
-      <c r="C133" s="94"/>
+      <c r="B133" s="94"/>
+      <c r="C133" s="105"/>
       <c r="D133" s="4" t="s">
         <v>155</v>
       </c>
@@ -9995,13 +9999,13 @@
       <c r="T133" s="52">
         <v>0</v>
       </c>
-      <c r="U133" s="83"/>
-      <c r="V133" s="83"/>
-      <c r="W133" s="84"/>
+      <c r="U133" s="82"/>
+      <c r="V133" s="82"/>
+      <c r="W133" s="83"/>
     </row>
     <row r="134" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="99"/>
-      <c r="C134" s="94"/>
+      <c r="B134" s="94"/>
+      <c r="C134" s="105"/>
       <c r="D134" s="4" t="s">
         <v>154</v>
       </c>
@@ -10065,8 +10069,8 @@
       </c>
     </row>
     <row r="135" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="99"/>
-      <c r="C135" s="94"/>
+      <c r="B135" s="94"/>
+      <c r="C135" s="105"/>
       <c r="D135" s="4" t="s">
         <v>125</v>
       </c>
@@ -10121,11 +10125,11 @@
       </c>
       <c r="U135" s="5"/>
       <c r="V135" s="5"/>
-      <c r="W135" s="78"/>
+      <c r="W135" s="77"/>
     </row>
     <row r="136" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="99"/>
-      <c r="C136" s="94" t="s">
+      <c r="B136" s="94"/>
+      <c r="C136" s="105" t="s">
         <v>117</v>
       </c>
       <c r="D136" s="4" t="s">
@@ -10191,8 +10195,8 @@
       </c>
     </row>
     <row r="137" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="99"/>
-      <c r="C137" s="94"/>
+      <c r="B137" s="94"/>
+      <c r="C137" s="105"/>
       <c r="D137" s="4" t="s">
         <v>123</v>
       </c>
@@ -10247,11 +10251,11 @@
       </c>
       <c r="U137" s="5"/>
       <c r="V137" s="5"/>
-      <c r="W137" s="78"/>
+      <c r="W137" s="77"/>
     </row>
     <row r="138" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="99"/>
-      <c r="C138" s="94"/>
+      <c r="B138" s="94"/>
+      <c r="C138" s="105"/>
       <c r="D138" s="4" t="s">
         <v>152</v>
       </c>
@@ -10306,11 +10310,11 @@
       </c>
       <c r="U138" s="5"/>
       <c r="V138" s="5"/>
-      <c r="W138" s="78"/>
+      <c r="W138" s="77"/>
     </row>
     <row r="139" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="99"/>
-      <c r="C139" s="94"/>
+      <c r="B139" s="94"/>
+      <c r="C139" s="105"/>
       <c r="D139" s="4" t="s">
         <v>124</v>
       </c>
@@ -10374,8 +10378,8 @@
       </c>
     </row>
     <row r="140" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="99"/>
-      <c r="C140" s="94"/>
+      <c r="B140" s="94"/>
+      <c r="C140" s="105"/>
       <c r="D140" s="4" t="s">
         <v>155</v>
       </c>
@@ -10428,13 +10432,13 @@
       <c r="T140" s="52">
         <v>0</v>
       </c>
-      <c r="U140" s="83"/>
-      <c r="V140" s="83"/>
-      <c r="W140" s="84"/>
+      <c r="U140" s="82"/>
+      <c r="V140" s="82"/>
+      <c r="W140" s="83"/>
     </row>
     <row r="141" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="99"/>
-      <c r="C141" s="94"/>
+      <c r="B141" s="94"/>
+      <c r="C141" s="105"/>
       <c r="D141" s="4" t="s">
         <v>154</v>
       </c>
@@ -10498,8 +10502,8 @@
       </c>
     </row>
     <row r="142" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="99"/>
-      <c r="C142" s="94"/>
+      <c r="B142" s="94"/>
+      <c r="C142" s="105"/>
       <c r="D142" s="4" t="s">
         <v>125</v>
       </c>
@@ -10554,11 +10558,11 @@
       </c>
       <c r="U142" s="5"/>
       <c r="V142" s="5"/>
-      <c r="W142" s="78"/>
+      <c r="W142" s="77"/>
     </row>
     <row r="143" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="99"/>
-      <c r="C143" s="94" t="s">
+      <c r="B143" s="94"/>
+      <c r="C143" s="105" t="s">
         <v>118</v>
       </c>
       <c r="D143" s="4" t="s">
@@ -10624,8 +10628,8 @@
       </c>
     </row>
     <row r="144" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="99"/>
-      <c r="C144" s="94"/>
+      <c r="B144" s="94"/>
+      <c r="C144" s="105"/>
       <c r="D144" s="4" t="s">
         <v>123</v>
       </c>
@@ -10680,11 +10684,11 @@
       </c>
       <c r="U144" s="5"/>
       <c r="V144" s="5"/>
-      <c r="W144" s="78"/>
+      <c r="W144" s="77"/>
     </row>
     <row r="145" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="99"/>
-      <c r="C145" s="94"/>
+      <c r="B145" s="94"/>
+      <c r="C145" s="105"/>
       <c r="D145" s="4" t="s">
         <v>152</v>
       </c>
@@ -10739,11 +10743,11 @@
       </c>
       <c r="U145" s="5"/>
       <c r="V145" s="5"/>
-      <c r="W145" s="78"/>
+      <c r="W145" s="77"/>
     </row>
     <row r="146" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="99"/>
-      <c r="C146" s="94"/>
+      <c r="B146" s="94"/>
+      <c r="C146" s="105"/>
       <c r="D146" s="4" t="s">
         <v>124</v>
       </c>
@@ -10807,8 +10811,8 @@
       </c>
     </row>
     <row r="147" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="99"/>
-      <c r="C147" s="94"/>
+      <c r="B147" s="94"/>
+      <c r="C147" s="105"/>
       <c r="D147" s="4" t="s">
         <v>155</v>
       </c>
@@ -10861,13 +10865,13 @@
       <c r="T147" s="52">
         <v>0</v>
       </c>
-      <c r="U147" s="83"/>
-      <c r="V147" s="83"/>
-      <c r="W147" s="84"/>
+      <c r="U147" s="82"/>
+      <c r="V147" s="82"/>
+      <c r="W147" s="83"/>
     </row>
     <row r="148" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="99"/>
-      <c r="C148" s="94"/>
+      <c r="B148" s="94"/>
+      <c r="C148" s="105"/>
       <c r="D148" s="4" t="s">
         <v>154</v>
       </c>
@@ -10931,8 +10935,8 @@
       </c>
     </row>
     <row r="149" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="99"/>
-      <c r="C149" s="94"/>
+      <c r="B149" s="94"/>
+      <c r="C149" s="105"/>
       <c r="D149" s="4" t="s">
         <v>125</v>
       </c>
@@ -10987,11 +10991,11 @@
       </c>
       <c r="U149" s="5"/>
       <c r="V149" s="5"/>
-      <c r="W149" s="78"/>
+      <c r="W149" s="77"/>
     </row>
     <row r="150" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="99"/>
-      <c r="C150" s="94" t="s">
+      <c r="B150" s="94"/>
+      <c r="C150" s="105" t="s">
         <v>119</v>
       </c>
       <c r="D150" s="4" t="s">
@@ -11057,8 +11061,8 @@
       </c>
     </row>
     <row r="151" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="99"/>
-      <c r="C151" s="94"/>
+      <c r="B151" s="94"/>
+      <c r="C151" s="105"/>
       <c r="D151" s="4" t="s">
         <v>123</v>
       </c>
@@ -11113,11 +11117,11 @@
       </c>
       <c r="U151" s="5"/>
       <c r="V151" s="5"/>
-      <c r="W151" s="78"/>
+      <c r="W151" s="77"/>
     </row>
     <row r="152" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="99"/>
-      <c r="C152" s="94"/>
+      <c r="B152" s="94"/>
+      <c r="C152" s="105"/>
       <c r="D152" s="4" t="s">
         <v>152</v>
       </c>
@@ -11172,11 +11176,11 @@
       </c>
       <c r="U152" s="5"/>
       <c r="V152" s="5"/>
-      <c r="W152" s="78"/>
+      <c r="W152" s="77"/>
     </row>
     <row r="153" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="99"/>
-      <c r="C153" s="94"/>
+      <c r="B153" s="94"/>
+      <c r="C153" s="105"/>
       <c r="D153" s="4" t="s">
         <v>124</v>
       </c>
@@ -11240,8 +11244,8 @@
       </c>
     </row>
     <row r="154" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="99"/>
-      <c r="C154" s="94"/>
+      <c r="B154" s="94"/>
+      <c r="C154" s="105"/>
       <c r="D154" s="4" t="s">
         <v>155</v>
       </c>
@@ -11294,13 +11298,13 @@
       <c r="T154" s="52">
         <v>0</v>
       </c>
-      <c r="U154" s="83"/>
-      <c r="V154" s="83"/>
-      <c r="W154" s="84"/>
+      <c r="U154" s="82"/>
+      <c r="V154" s="82"/>
+      <c r="W154" s="83"/>
     </row>
     <row r="155" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="99"/>
-      <c r="C155" s="94"/>
+      <c r="B155" s="94"/>
+      <c r="C155" s="105"/>
       <c r="D155" s="4" t="s">
         <v>154</v>
       </c>
@@ -11360,8 +11364,8 @@
       <c r="W155" s="63"/>
     </row>
     <row r="156" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="99"/>
-      <c r="C156" s="94"/>
+      <c r="B156" s="94"/>
+      <c r="C156" s="105"/>
       <c r="D156" s="4" t="s">
         <v>125</v>
       </c>
@@ -11416,11 +11420,11 @@
       </c>
       <c r="U156" s="5"/>
       <c r="V156" s="5"/>
-      <c r="W156" s="78"/>
+      <c r="W156" s="77"/>
     </row>
     <row r="157" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="99"/>
-      <c r="C157" s="94" t="s">
+      <c r="B157" s="94"/>
+      <c r="C157" s="105" t="s">
         <v>120</v>
       </c>
       <c r="D157" s="4" t="s">
@@ -11486,8 +11490,8 @@
       </c>
     </row>
     <row r="158" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="99"/>
-      <c r="C158" s="94"/>
+      <c r="B158" s="94"/>
+      <c r="C158" s="105"/>
       <c r="D158" s="4" t="s">
         <v>123</v>
       </c>
@@ -11542,11 +11546,11 @@
       </c>
       <c r="U158" s="5"/>
       <c r="V158" s="5"/>
-      <c r="W158" s="78"/>
+      <c r="W158" s="77"/>
     </row>
     <row r="159" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="99"/>
-      <c r="C159" s="94"/>
+      <c r="B159" s="94"/>
+      <c r="C159" s="105"/>
       <c r="D159" s="4" t="s">
         <v>152</v>
       </c>
@@ -11601,11 +11605,11 @@
       </c>
       <c r="U159" s="5"/>
       <c r="V159" s="5"/>
-      <c r="W159" s="78"/>
+      <c r="W159" s="77"/>
     </row>
     <row r="160" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="99"/>
-      <c r="C160" s="94"/>
+      <c r="B160" s="94"/>
+      <c r="C160" s="105"/>
       <c r="D160" s="4" t="s">
         <v>124</v>
       </c>
@@ -11669,8 +11673,8 @@
       </c>
     </row>
     <row r="161" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="99"/>
-      <c r="C161" s="94"/>
+      <c r="B161" s="94"/>
+      <c r="C161" s="105"/>
       <c r="D161" s="4" t="s">
         <v>155</v>
       </c>
@@ -11723,13 +11727,13 @@
       <c r="T161" s="52">
         <v>0</v>
       </c>
-      <c r="U161" s="83"/>
-      <c r="V161" s="83"/>
-      <c r="W161" s="84"/>
+      <c r="U161" s="82"/>
+      <c r="V161" s="82"/>
+      <c r="W161" s="83"/>
     </row>
     <row r="162" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="99"/>
-      <c r="C162" s="94"/>
+      <c r="B162" s="94"/>
+      <c r="C162" s="105"/>
       <c r="D162" s="4" t="s">
         <v>154</v>
       </c>
@@ -11793,8 +11797,8 @@
       </c>
     </row>
     <row r="163" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="99"/>
-      <c r="C163" s="94"/>
+      <c r="B163" s="94"/>
+      <c r="C163" s="105"/>
       <c r="D163" s="4" t="s">
         <v>125</v>
       </c>
@@ -11849,11 +11853,11 @@
       </c>
       <c r="U163" s="5"/>
       <c r="V163" s="5"/>
-      <c r="W163" s="78"/>
+      <c r="W163" s="77"/>
     </row>
     <row r="164" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="99"/>
-      <c r="C164" s="94" t="s">
+      <c r="B164" s="94"/>
+      <c r="C164" s="105" t="s">
         <v>121</v>
       </c>
       <c r="D164" s="4" t="s">
@@ -11919,8 +11923,8 @@
       </c>
     </row>
     <row r="165" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="99"/>
-      <c r="C165" s="94"/>
+      <c r="B165" s="94"/>
+      <c r="C165" s="105"/>
       <c r="D165" s="4" t="s">
         <v>123</v>
       </c>
@@ -11975,11 +11979,11 @@
       </c>
       <c r="U165" s="5"/>
       <c r="V165" s="5"/>
-      <c r="W165" s="78"/>
+      <c r="W165" s="77"/>
     </row>
     <row r="166" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B166" s="99"/>
-      <c r="C166" s="94"/>
+      <c r="B166" s="94"/>
+      <c r="C166" s="105"/>
       <c r="D166" s="4" t="s">
         <v>152</v>
       </c>
@@ -12034,11 +12038,11 @@
       </c>
       <c r="U166" s="5"/>
       <c r="V166" s="5"/>
-      <c r="W166" s="78"/>
+      <c r="W166" s="77"/>
     </row>
     <row r="167" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B167" s="99"/>
-      <c r="C167" s="94"/>
+      <c r="B167" s="94"/>
+      <c r="C167" s="105"/>
       <c r="D167" s="4" t="s">
         <v>124</v>
       </c>
@@ -12102,8 +12106,8 @@
       </c>
     </row>
     <row r="168" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B168" s="116"/>
-      <c r="C168" s="120"/>
+      <c r="B168" s="101"/>
+      <c r="C168" s="108"/>
       <c r="D168" s="4" t="s">
         <v>155</v>
       </c>
@@ -12156,13 +12160,13 @@
       <c r="T168" s="54">
         <v>0</v>
       </c>
-      <c r="U168" s="85"/>
-      <c r="V168" s="85"/>
-      <c r="W168" s="86"/>
+      <c r="U168" s="84"/>
+      <c r="V168" s="84"/>
+      <c r="W168" s="85"/>
     </row>
     <row r="169" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B169" s="116"/>
-      <c r="C169" s="120"/>
+      <c r="B169" s="101"/>
+      <c r="C169" s="108"/>
       <c r="D169" s="4" t="s">
         <v>154</v>
       </c>
@@ -12215,19 +12219,19 @@
       <c r="T169" s="54">
         <v>0</v>
       </c>
-      <c r="U169" s="91">
+      <c r="U169" s="90">
         <v>0.03</v>
       </c>
-      <c r="V169" s="91">
-        <v>0</v>
-      </c>
-      <c r="W169" s="92">
+      <c r="V169" s="90">
+        <v>0</v>
+      </c>
+      <c r="W169" s="91">
         <v>0</v>
       </c>
     </row>
     <row r="170" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B170" s="100"/>
-      <c r="C170" s="121"/>
+      <c r="B170" s="95"/>
+      <c r="C170" s="109"/>
       <c r="D170" s="17" t="s">
         <v>125</v>
       </c>
@@ -12282,10 +12286,10 @@
       </c>
       <c r="U170" s="31"/>
       <c r="V170" s="31"/>
-      <c r="W170" s="79"/>
+      <c r="W170" s="78"/>
     </row>
     <row r="171" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B171" s="98" t="s">
+      <c r="B171" s="93" t="s">
         <v>74</v>
       </c>
       <c r="C171" s="60" t="s">
@@ -12347,12 +12351,12 @@
       <c r="V171" s="75">
         <v>0</v>
       </c>
-      <c r="W171" s="90">
+      <c r="W171" s="89">
         <v>0</v>
       </c>
     </row>
     <row r="172" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B172" s="99"/>
+      <c r="B172" s="94"/>
       <c r="C172" s="22" t="s">
         <v>80</v>
       </c>
@@ -12408,10 +12412,10 @@
       </c>
       <c r="U172" s="5"/>
       <c r="V172" s="5"/>
-      <c r="W172" s="78"/>
+      <c r="W172" s="77"/>
     </row>
     <row r="173" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B173" s="99"/>
+      <c r="B173" s="94"/>
       <c r="C173" s="22" t="s">
         <v>81</v>
       </c>
@@ -12467,10 +12471,10 @@
       </c>
       <c r="U173" s="5"/>
       <c r="V173" s="5"/>
-      <c r="W173" s="78"/>
+      <c r="W173" s="77"/>
     </row>
     <row r="174" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B174" s="99"/>
+      <c r="B174" s="94"/>
       <c r="C174" s="22" t="s">
         <v>82</v>
       </c>
@@ -12526,10 +12530,10 @@
       </c>
       <c r="U174" s="5"/>
       <c r="V174" s="5"/>
-      <c r="W174" s="78"/>
+      <c r="W174" s="77"/>
     </row>
     <row r="175" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B175" s="99"/>
+      <c r="B175" s="94"/>
       <c r="C175" s="22" t="s">
         <v>132</v>
       </c>
@@ -12585,10 +12589,10 @@
       </c>
       <c r="U175" s="5"/>
       <c r="V175" s="5"/>
-      <c r="W175" s="78"/>
+      <c r="W175" s="77"/>
     </row>
     <row r="176" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="99"/>
+      <c r="B176" s="94"/>
       <c r="C176" s="22" t="s">
         <v>129</v>
       </c>
@@ -12644,10 +12648,10 @@
       </c>
       <c r="U176" s="5"/>
       <c r="V176" s="5"/>
-      <c r="W176" s="78"/>
+      <c r="W176" s="77"/>
     </row>
     <row r="177" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B177" s="99"/>
+      <c r="B177" s="94"/>
       <c r="C177" s="22" t="s">
         <v>131</v>
       </c>
@@ -12703,10 +12707,10 @@
       </c>
       <c r="U177" s="5"/>
       <c r="V177" s="5"/>
-      <c r="W177" s="78"/>
+      <c r="W177" s="77"/>
     </row>
     <row r="178" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B178" s="99"/>
+      <c r="B178" s="94"/>
       <c r="C178" s="22" t="s">
         <v>130</v>
       </c>
@@ -12762,10 +12766,10 @@
       </c>
       <c r="U178" s="5"/>
       <c r="V178" s="5"/>
-      <c r="W178" s="78"/>
+      <c r="W178" s="77"/>
     </row>
     <row r="179" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B179" s="99"/>
+      <c r="B179" s="94"/>
       <c r="C179" s="22" t="s">
         <v>83</v>
       </c>
@@ -12830,7 +12834,7 @@
       </c>
     </row>
     <row r="180" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B180" s="99"/>
+      <c r="B180" s="94"/>
       <c r="C180" s="22" t="s">
         <v>84</v>
       </c>
@@ -12895,7 +12899,7 @@
       </c>
     </row>
     <row r="181" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B181" s="99"/>
+      <c r="B181" s="94"/>
       <c r="C181" s="22" t="s">
         <v>85</v>
       </c>
@@ -12960,7 +12964,7 @@
       </c>
     </row>
     <row r="182" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B182" s="99"/>
+      <c r="B182" s="94"/>
       <c r="C182" s="22" t="s">
         <v>89</v>
       </c>
@@ -13025,7 +13029,7 @@
       </c>
     </row>
     <row r="183" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B183" s="100"/>
+      <c r="B183" s="95"/>
       <c r="C183" s="43" t="s">
         <v>90</v>
       </c>
@@ -13076,15 +13080,15 @@
       <c r="S183" s="53">
         <v>0</v>
       </c>
-      <c r="T183" s="87">
+      <c r="T183" s="86">
         <v>0.03</v>
       </c>
       <c r="U183" s="31"/>
       <c r="V183" s="31"/>
-      <c r="W183" s="79"/>
+      <c r="W183" s="78"/>
     </row>
     <row r="184" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B184" s="98" t="s">
+      <c r="B184" s="93" t="s">
         <v>133</v>
       </c>
       <c r="C184" s="42" t="s">
@@ -13142,10 +13146,10 @@
       </c>
       <c r="U184" s="34"/>
       <c r="V184" s="34"/>
-      <c r="W184" s="82"/>
+      <c r="W184" s="81"/>
     </row>
     <row r="185" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="99"/>
+      <c r="B185" s="94"/>
       <c r="C185" s="41" t="s">
         <v>134</v>
       </c>
@@ -13201,10 +13205,10 @@
       </c>
       <c r="U185" s="5"/>
       <c r="V185" s="5"/>
-      <c r="W185" s="78"/>
+      <c r="W185" s="77"/>
     </row>
     <row r="186" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B186" s="100"/>
+      <c r="B186" s="95"/>
       <c r="C186" s="43" t="s">
         <v>135</v>
       </c>
@@ -13260,10 +13264,10 @@
       </c>
       <c r="U186" s="31"/>
       <c r="V186" s="31"/>
-      <c r="W186" s="79"/>
+      <c r="W186" s="78"/>
     </row>
     <row r="187" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B187" s="98" t="s">
+      <c r="B187" s="93" t="s">
         <v>138</v>
       </c>
       <c r="C187" s="42" t="s">
@@ -13321,10 +13325,10 @@
       </c>
       <c r="U187" s="34"/>
       <c r="V187" s="34"/>
-      <c r="W187" s="82"/>
+      <c r="W187" s="81"/>
     </row>
     <row r="188" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B188" s="99"/>
+      <c r="B188" s="94"/>
       <c r="C188" s="41" t="s">
         <v>140</v>
       </c>
@@ -13380,12 +13384,12 @@
       </c>
       <c r="U188" s="5"/>
       <c r="V188" s="5"/>
-      <c r="W188" s="78"/>
+      <c r="W188" s="77"/>
     </row>
     <row r="189" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B189" s="99"/>
+      <c r="B189" s="94"/>
       <c r="C189" s="41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D189" s="4"/>
       <c r="E189" s="4" t="s">
@@ -13439,10 +13443,10 @@
       </c>
       <c r="U189" s="5"/>
       <c r="V189" s="5"/>
-      <c r="W189" s="78"/>
+      <c r="W189" s="77"/>
     </row>
     <row r="190" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B190" s="99"/>
+      <c r="B190" s="94"/>
       <c r="C190" s="41" t="s">
         <v>141</v>
       </c>
@@ -13498,10 +13502,10 @@
       </c>
       <c r="U190" s="5"/>
       <c r="V190" s="5"/>
-      <c r="W190" s="78"/>
+      <c r="W190" s="77"/>
     </row>
     <row r="191" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B191" s="99"/>
+      <c r="B191" s="94"/>
       <c r="C191" s="41" t="s">
         <v>142</v>
       </c>
@@ -13557,12 +13561,12 @@
       </c>
       <c r="U191" s="5"/>
       <c r="V191" s="5"/>
-      <c r="W191" s="78"/>
+      <c r="W191" s="77"/>
     </row>
     <row r="192" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B192" s="99"/>
+      <c r="B192" s="94"/>
       <c r="C192" s="41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D192" s="4"/>
       <c r="E192" s="4" t="s">
@@ -13616,12 +13620,12 @@
       </c>
       <c r="U192" s="5"/>
       <c r="V192" s="5"/>
-      <c r="W192" s="78"/>
+      <c r="W192" s="77"/>
     </row>
     <row r="193" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="99"/>
+      <c r="B193" s="94"/>
       <c r="C193" s="41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D193" s="4"/>
       <c r="E193" s="4" t="s">
@@ -13675,12 +13679,12 @@
       </c>
       <c r="U193" s="5"/>
       <c r="V193" s="5"/>
-      <c r="W193" s="78"/>
+      <c r="W193" s="77"/>
     </row>
     <row r="194" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B194" s="99"/>
+      <c r="B194" s="94"/>
       <c r="C194" s="41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D194" s="4"/>
       <c r="E194" s="4" t="s">
@@ -13734,10 +13738,10 @@
       </c>
       <c r="U194" s="5"/>
       <c r="V194" s="5"/>
-      <c r="W194" s="78"/>
+      <c r="W194" s="77"/>
     </row>
     <row r="195" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="99"/>
+      <c r="B195" s="94"/>
       <c r="C195" s="41" t="s">
         <v>143</v>
       </c>
@@ -13793,10 +13797,10 @@
       </c>
       <c r="U195" s="5"/>
       <c r="V195" s="5"/>
-      <c r="W195" s="78"/>
+      <c r="W195" s="77"/>
     </row>
     <row r="196" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="99"/>
+      <c r="B196" s="94"/>
       <c r="C196" s="41" t="s">
         <v>144</v>
       </c>
@@ -13852,10 +13856,10 @@
       </c>
       <c r="U196" s="5"/>
       <c r="V196" s="5"/>
-      <c r="W196" s="78"/>
+      <c r="W196" s="77"/>
     </row>
     <row r="197" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B197" s="100"/>
+      <c r="B197" s="95"/>
       <c r="C197" s="43" t="s">
         <v>145</v>
       </c>
@@ -13911,10 +13915,10 @@
       </c>
       <c r="U197" s="31"/>
       <c r="V197" s="31"/>
-      <c r="W197" s="79"/>
+      <c r="W197" s="78"/>
     </row>
     <row r="198" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B198" s="98" t="s">
+      <c r="B198" s="93" t="s">
         <v>17</v>
       </c>
       <c r="C198" s="36" t="s">
@@ -13972,10 +13976,10 @@
       </c>
       <c r="U198" s="34"/>
       <c r="V198" s="34"/>
-      <c r="W198" s="82"/>
+      <c r="W198" s="81"/>
     </row>
     <row r="199" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B199" s="99"/>
+      <c r="B199" s="94"/>
       <c r="C199" s="22" t="s">
         <v>127</v>
       </c>
@@ -14031,10 +14035,10 @@
       </c>
       <c r="U199" s="5"/>
       <c r="V199" s="5"/>
-      <c r="W199" s="78"/>
+      <c r="W199" s="77"/>
     </row>
     <row r="200" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B200" s="99"/>
+      <c r="B200" s="94"/>
       <c r="C200" s="22" t="s">
         <v>128</v>
       </c>
@@ -14090,10 +14094,10 @@
       </c>
       <c r="U200" s="5"/>
       <c r="V200" s="5"/>
-      <c r="W200" s="78"/>
+      <c r="W200" s="77"/>
     </row>
     <row r="201" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B201" s="99"/>
+      <c r="B201" s="94"/>
       <c r="C201" s="22" t="s">
         <v>136</v>
       </c>
@@ -14149,10 +14153,10 @@
       </c>
       <c r="U201" s="5"/>
       <c r="V201" s="5"/>
-      <c r="W201" s="78"/>
+      <c r="W201" s="77"/>
     </row>
     <row r="202" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B202" s="99"/>
+      <c r="B202" s="94"/>
       <c r="C202" s="22" t="s">
         <v>75</v>
       </c>
@@ -14208,10 +14212,10 @@
       </c>
       <c r="U202" s="5"/>
       <c r="V202" s="5"/>
-      <c r="W202" s="78"/>
+      <c r="W202" s="77"/>
     </row>
     <row r="203" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B203" s="99"/>
+      <c r="B203" s="94"/>
       <c r="C203" s="22" t="s">
         <v>76</v>
       </c>
@@ -14267,10 +14271,10 @@
       </c>
       <c r="U203" s="5"/>
       <c r="V203" s="5"/>
-      <c r="W203" s="78"/>
+      <c r="W203" s="77"/>
     </row>
     <row r="204" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B204" s="99"/>
+      <c r="B204" s="94"/>
       <c r="C204" s="22" t="s">
         <v>78</v>
       </c>
@@ -14326,10 +14330,10 @@
       </c>
       <c r="U204" s="5"/>
       <c r="V204" s="5"/>
-      <c r="W204" s="78"/>
+      <c r="W204" s="77"/>
     </row>
     <row r="205" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B205" s="99"/>
+      <c r="B205" s="94"/>
       <c r="C205" s="22" t="s">
         <v>77</v>
       </c>
@@ -14385,10 +14389,10 @@
       </c>
       <c r="U205" s="5"/>
       <c r="V205" s="5"/>
-      <c r="W205" s="78"/>
+      <c r="W205" s="77"/>
     </row>
     <row r="206" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B206" s="99"/>
+      <c r="B206" s="94"/>
       <c r="C206" s="22" t="s">
         <v>94</v>
       </c>
@@ -14444,10 +14448,10 @@
       </c>
       <c r="U206" s="5"/>
       <c r="V206" s="5"/>
-      <c r="W206" s="78"/>
+      <c r="W206" s="77"/>
     </row>
     <row r="207" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B207" s="99"/>
+      <c r="B207" s="94"/>
       <c r="C207" s="22" t="s">
         <v>126</v>
       </c>
@@ -14503,10 +14507,10 @@
       </c>
       <c r="U207" s="5"/>
       <c r="V207" s="5"/>
-      <c r="W207" s="78"/>
+      <c r="W207" s="77"/>
     </row>
     <row r="208" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B208" s="99"/>
+      <c r="B208" s="94"/>
       <c r="C208" s="22" t="s">
         <v>95</v>
       </c>
@@ -14525,7 +14529,7 @@
       </c>
       <c r="I208" s="6">
         <f>SUM(J208:W208)</f>
-        <v>0</v>
+        <v>10.4</v>
       </c>
       <c r="J208" s="52">
         <v>0</v>
@@ -14545,8 +14549,8 @@
       <c r="O208" s="52">
         <v>0</v>
       </c>
-      <c r="P208" s="52" t="s">
-        <v>156</v>
+      <c r="P208" s="52">
+        <v>0.2</v>
       </c>
       <c r="Q208" s="74">
         <v>0</v>
@@ -14557,29 +14561,33 @@
       <c r="S208" s="74">
         <v>0</v>
       </c>
-      <c r="T208" s="74" t="s">
-        <v>162</v>
-      </c>
-      <c r="U208" s="5"/>
-      <c r="V208" s="5"/>
-      <c r="W208" s="78"/>
+      <c r="T208" s="74">
+        <v>0.7</v>
+      </c>
+      <c r="U208" s="74">
+        <v>5.5</v>
+      </c>
+      <c r="V208" s="74">
+        <v>4</v>
+      </c>
+      <c r="W208" s="77"/>
     </row>
     <row r="209" spans="2:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B209" s="117" t="s">
+      <c r="B209" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="C209" s="118"/>
-      <c r="D209" s="118"/>
-      <c r="E209" s="118"/>
-      <c r="F209" s="118"/>
-      <c r="G209" s="119"/>
+      <c r="C209" s="103"/>
+      <c r="D209" s="103"/>
+      <c r="E209" s="103"/>
+      <c r="F209" s="103"/>
+      <c r="G209" s="104"/>
       <c r="H209" s="25">
         <f t="shared" ref="H209:W209" si="7">SUM(H4:H208)</f>
         <v>113.84999999999995</v>
       </c>
       <c r="I209" s="16">
         <f t="shared" si="7"/>
-        <v>58.664300000000026</v>
+        <v>72.064300000000031</v>
       </c>
       <c r="J209" s="16">
         <f t="shared" si="7"/>
@@ -14607,7 +14615,7 @@
       </c>
       <c r="P209" s="16">
         <f t="shared" si="7"/>
-        <v>9.2930000000000028</v>
+        <v>9.4930000000000021</v>
       </c>
       <c r="Q209" s="16">
         <f t="shared" si="7"/>
@@ -14623,15 +14631,15 @@
       </c>
       <c r="T209" s="16">
         <f t="shared" si="7"/>
-        <v>9.4290000000000003</v>
+        <v>10.129</v>
       </c>
       <c r="U209" s="16">
         <f t="shared" si="7"/>
-        <v>3.3900000000000006</v>
+        <v>11.889999999999999</v>
       </c>
       <c r="V209" s="16">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W209" s="19">
         <f t="shared" si="7"/>
@@ -14647,22 +14655,22 @@
       <c r="G210" s="2"/>
       <c r="H210" s="2"/>
       <c r="I210" s="2"/>
-      <c r="J210" s="95" t="s">
+      <c r="J210" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="K210" s="96"/>
-      <c r="L210" s="96"/>
-      <c r="M210" s="96"/>
-      <c r="N210" s="96"/>
-      <c r="O210" s="96"/>
-      <c r="P210" s="96"/>
-      <c r="Q210" s="96"/>
-      <c r="R210" s="96"/>
-      <c r="S210" s="96"/>
-      <c r="T210" s="96"/>
-      <c r="U210" s="96"/>
-      <c r="V210" s="96"/>
-      <c r="W210" s="97"/>
+      <c r="K210" s="106"/>
+      <c r="L210" s="106"/>
+      <c r="M210" s="106"/>
+      <c r="N210" s="106"/>
+      <c r="O210" s="106"/>
+      <c r="P210" s="106"/>
+      <c r="Q210" s="106"/>
+      <c r="R210" s="106"/>
+      <c r="S210" s="106"/>
+      <c r="T210" s="106"/>
+      <c r="U210" s="106"/>
+      <c r="V210" s="106"/>
+      <c r="W210" s="107"/>
     </row>
     <row r="211" spans="2:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C211" s="41" t="s">
@@ -14702,10 +14710,10 @@
       </c>
       <c r="F212" s="2"/>
       <c r="G212" s="2"/>
-      <c r="H212" s="112" t="s">
+      <c r="H212" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="I212" s="113"/>
+      <c r="I212" s="97"/>
       <c r="J212" s="9">
         <f>H209-J209</f>
         <v>113.84999999999995</v>
@@ -14732,35 +14740,35 @@
       </c>
       <c r="P212" s="71">
         <f t="shared" si="8"/>
-        <v>86.499699999999962</v>
+        <v>86.299699999999973</v>
       </c>
       <c r="Q212" s="71">
         <f t="shared" si="8"/>
-        <v>84.029699999999963</v>
+        <v>83.829699999999974</v>
       </c>
       <c r="R212" s="71">
         <f t="shared" si="8"/>
-        <v>75.196699999999964</v>
+        <v>74.996699999999976</v>
       </c>
       <c r="S212" s="71">
         <f t="shared" si="8"/>
-        <v>68.004699999999971</v>
+        <v>67.804699999999983</v>
       </c>
       <c r="T212" s="71">
         <f t="shared" si="8"/>
-        <v>58.575699999999969</v>
+        <v>57.675699999999985</v>
       </c>
       <c r="U212" s="71">
         <f t="shared" si="8"/>
-        <v>55.185699999999969</v>
+        <v>45.785699999999984</v>
       </c>
       <c r="V212" s="71">
         <f t="shared" si="8"/>
-        <v>55.185699999999969</v>
+        <v>41.785699999999984</v>
       </c>
       <c r="W212" s="71">
         <f t="shared" si="8"/>
-        <v>55.185699999999969</v>
+        <v>41.785699999999984</v>
       </c>
     </row>
     <row r="213" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14799,25 +14807,25 @@
       </c>
       <c r="D214" s="5">
         <f>SUM(I208,I205:I206,I198:I202,I172:I178,I56:I65,I4:I8)</f>
-        <v>17.55</v>
+        <v>30.95</v>
       </c>
       <c r="E214" s="5">
         <f>SUM(C214,-D214)</f>
-        <v>6.8499999999999979</v>
+        <v>-6.5500000000000007</v>
       </c>
       <c r="F214" s="3"/>
-      <c r="H214" s="95" t="s">
+      <c r="H214" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="I214" s="114"/>
-      <c r="J214" s="113">
+      <c r="I214" s="99"/>
+      <c r="J214" s="97">
         <f>H209-I209</f>
-        <v>55.185699999999926</v>
-      </c>
-      <c r="K214" s="113"/>
-      <c r="L214" s="113"/>
-      <c r="M214" s="113"/>
-      <c r="N214" s="115"/>
+        <v>41.78569999999992</v>
+      </c>
+      <c r="K214" s="97"/>
+      <c r="L214" s="97"/>
+      <c r="M214" s="97"/>
+      <c r="N214" s="100"/>
     </row>
     <row r="215" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B215" s="3"/>
@@ -14921,6 +14929,24 @@
     <row r="233" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C150:C156"/>
+    <mergeCell ref="C136:C142"/>
+    <mergeCell ref="C122:C128"/>
+    <mergeCell ref="C115:C121"/>
+    <mergeCell ref="C101:C107"/>
+    <mergeCell ref="C129:C135"/>
+    <mergeCell ref="C143:C149"/>
+    <mergeCell ref="C80:C86"/>
+    <mergeCell ref="J2:W2"/>
+    <mergeCell ref="B56:B65"/>
+    <mergeCell ref="C49:C55"/>
+    <mergeCell ref="C15:C48"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C66:C72"/>
+    <mergeCell ref="C73:C79"/>
     <mergeCell ref="B187:B197"/>
     <mergeCell ref="H212:I212"/>
     <mergeCell ref="H214:I214"/>
@@ -14937,24 +14963,6 @@
     <mergeCell ref="C164:C170"/>
     <mergeCell ref="C94:C100"/>
     <mergeCell ref="C87:C93"/>
-    <mergeCell ref="C80:C86"/>
-    <mergeCell ref="J2:W2"/>
-    <mergeCell ref="B56:B65"/>
-    <mergeCell ref="C49:C55"/>
-    <mergeCell ref="C15:C48"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="C66:C72"/>
-    <mergeCell ref="C73:C79"/>
-    <mergeCell ref="C150:C156"/>
-    <mergeCell ref="C136:C142"/>
-    <mergeCell ref="C122:C128"/>
-    <mergeCell ref="C115:C121"/>
-    <mergeCell ref="C101:C107"/>
-    <mergeCell ref="C129:C135"/>
-    <mergeCell ref="C143:C149"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
MORE THINGS! HAHAHAH. hay sonido en el filescene
</commit_message>
<xml_diff>
--- a/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
+++ b/tabla scrum backlog + burndown chart _SPRINT 3_by SampleText.xlsx
@@ -1351,43 +1351,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1396,10 +1363,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1433,6 +1403,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1524,7 +1524,7 @@
                   <c:v>32.185699999999983</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26.935699999999983</c:v>
+                  <c:v>25.635699999999982</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1928,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W61" sqref="W61"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,22 +1959,22 @@
       <c r="I2" s="37">
         <v>3</v>
       </c>
-      <c r="J2" s="102" t="s">
+      <c r="J2" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="110"/>
-      <c r="L2" s="110"/>
-      <c r="M2" s="110"/>
-      <c r="N2" s="110"/>
-      <c r="O2" s="110"/>
-      <c r="P2" s="110"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="110"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="110"/>
-      <c r="U2" s="110"/>
-      <c r="V2" s="110"/>
-      <c r="W2" s="111"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
+      <c r="Q2" s="99"/>
+      <c r="R2" s="99"/>
+      <c r="S2" s="99"/>
+      <c r="T2" s="99"/>
+      <c r="U2" s="99"/>
+      <c r="V2" s="99"/>
+      <c r="W2" s="100"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="38" t="s">
@@ -2045,7 +2045,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="111" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="26" t="s">
@@ -2106,7 +2106,7 @@
       <c r="W4" s="94"/>
     </row>
     <row r="5" spans="1:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="122"/>
+      <c r="B5" s="112"/>
       <c r="C5" s="24" t="s">
         <v>91</v>
       </c>
@@ -2171,7 +2171,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="122"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="24" t="s">
         <v>92</v>
       </c>
@@ -2236,7 +2236,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="122"/>
+      <c r="B7" s="112"/>
       <c r="C7" s="24" t="s">
         <v>93</v>
       </c>
@@ -2301,7 +2301,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="123"/>
+      <c r="B8" s="113"/>
       <c r="C8" s="30" t="s">
         <v>101</v>
       </c>
@@ -2366,7 +2366,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="121" t="s">
+      <c r="B9" s="111" t="s">
         <v>96</v>
       </c>
       <c r="C9" s="33" t="s">
@@ -2433,7 +2433,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="122"/>
+      <c r="B10" s="112"/>
       <c r="C10" s="23" t="s">
         <v>97</v>
       </c>
@@ -2492,7 +2492,7 @@
       <c r="W10" s="77"/>
     </row>
     <row r="11" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="122"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="65" t="s">
         <v>102</v>
       </c>
@@ -2557,7 +2557,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="122"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="65" t="s">
         <v>103</v>
       </c>
@@ -2622,7 +2622,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="123"/>
+      <c r="B13" s="113"/>
       <c r="C13" s="35" t="s">
         <v>88</v>
       </c>
@@ -2687,7 +2687,7 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="101" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="36" t="s">
@@ -2756,8 +2756,8 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B15" s="98"/>
-      <c r="C15" s="116" t="s">
+      <c r="B15" s="102"/>
+      <c r="C15" s="106" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -2823,8 +2823,8 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B16" s="98"/>
-      <c r="C16" s="117"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="107"/>
       <c r="D16" s="4" t="s">
         <v>19</v>
       </c>
@@ -2888,8 +2888,8 @@
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B17" s="98"/>
-      <c r="C17" s="117"/>
+      <c r="B17" s="102"/>
+      <c r="C17" s="107"/>
       <c r="D17" s="4" t="s">
         <v>20</v>
       </c>
@@ -2953,8 +2953,8 @@
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="98"/>
-      <c r="C18" s="117"/>
+      <c r="B18" s="102"/>
+      <c r="C18" s="107"/>
       <c r="D18" s="4" t="s">
         <v>21</v>
       </c>
@@ -3018,8 +3018,8 @@
       </c>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B19" s="98"/>
-      <c r="C19" s="117"/>
+      <c r="B19" s="102"/>
+      <c r="C19" s="107"/>
       <c r="D19" s="4" t="s">
         <v>22</v>
       </c>
@@ -3083,8 +3083,8 @@
       </c>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B20" s="98"/>
-      <c r="C20" s="117"/>
+      <c r="B20" s="102"/>
+      <c r="C20" s="107"/>
       <c r="D20" s="4" t="s">
         <v>153</v>
       </c>
@@ -3142,8 +3142,8 @@
       <c r="W20" s="77"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B21" s="98"/>
-      <c r="C21" s="117"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="107"/>
       <c r="D21" s="4" t="s">
         <v>23</v>
       </c>
@@ -3207,8 +3207,8 @@
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B22" s="98"/>
-      <c r="C22" s="117"/>
+      <c r="B22" s="102"/>
+      <c r="C22" s="107"/>
       <c r="D22" s="21" t="s">
         <v>156</v>
       </c>
@@ -3266,8 +3266,8 @@
       <c r="W22" s="77"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B23" s="98"/>
-      <c r="C23" s="117"/>
+      <c r="B23" s="102"/>
+      <c r="C23" s="107"/>
       <c r="D23" s="21" t="s">
         <v>35</v>
       </c>
@@ -3325,8 +3325,8 @@
       <c r="W23" s="77"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B24" s="98"/>
-      <c r="C24" s="117"/>
+      <c r="B24" s="102"/>
+      <c r="C24" s="107"/>
       <c r="D24" s="21" t="s">
         <v>36</v>
       </c>
@@ -3384,8 +3384,8 @@
       <c r="W24" s="77"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B25" s="98"/>
-      <c r="C25" s="117"/>
+      <c r="B25" s="102"/>
+      <c r="C25" s="107"/>
       <c r="D25" s="21" t="s">
         <v>37</v>
       </c>
@@ -3443,8 +3443,8 @@
       <c r="W25" s="77"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B26" s="98"/>
-      <c r="C26" s="117"/>
+      <c r="B26" s="102"/>
+      <c r="C26" s="107"/>
       <c r="D26" s="21" t="s">
         <v>38</v>
       </c>
@@ -3502,8 +3502,8 @@
       <c r="W26" s="77"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B27" s="98"/>
-      <c r="C27" s="117"/>
+      <c r="B27" s="102"/>
+      <c r="C27" s="107"/>
       <c r="D27" s="21" t="s">
         <v>39</v>
       </c>
@@ -3561,8 +3561,8 @@
       <c r="W27" s="77"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B28" s="98"/>
-      <c r="C28" s="117"/>
+      <c r="B28" s="102"/>
+      <c r="C28" s="107"/>
       <c r="D28" s="21" t="s">
         <v>40</v>
       </c>
@@ -3620,8 +3620,8 @@
       <c r="W28" s="77"/>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B29" s="98"/>
-      <c r="C29" s="117"/>
+      <c r="B29" s="102"/>
+      <c r="C29" s="107"/>
       <c r="D29" s="21" t="s">
         <v>41</v>
       </c>
@@ -3679,8 +3679,8 @@
       <c r="W29" s="77"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B30" s="98"/>
-      <c r="C30" s="117"/>
+      <c r="B30" s="102"/>
+      <c r="C30" s="107"/>
       <c r="D30" s="21" t="s">
         <v>42</v>
       </c>
@@ -3738,8 +3738,8 @@
       <c r="W30" s="77"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B31" s="98"/>
-      <c r="C31" s="117"/>
+      <c r="B31" s="102"/>
+      <c r="C31" s="107"/>
       <c r="D31" s="21" t="s">
         <v>43</v>
       </c>
@@ -3797,8 +3797,8 @@
       <c r="W31" s="77"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B32" s="98"/>
-      <c r="C32" s="117"/>
+      <c r="B32" s="102"/>
+      <c r="C32" s="107"/>
       <c r="D32" s="21" t="s">
         <v>44</v>
       </c>
@@ -3856,8 +3856,8 @@
       <c r="W32" s="77"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B33" s="98"/>
-      <c r="C33" s="117"/>
+      <c r="B33" s="102"/>
+      <c r="C33" s="107"/>
       <c r="D33" s="21" t="s">
         <v>45</v>
       </c>
@@ -3915,8 +3915,8 @@
       <c r="W33" s="77"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B34" s="98"/>
-      <c r="C34" s="117"/>
+      <c r="B34" s="102"/>
+      <c r="C34" s="107"/>
       <c r="D34" s="21" t="s">
         <v>46</v>
       </c>
@@ -3974,8 +3974,8 @@
       <c r="W34" s="77"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35" s="98"/>
-      <c r="C35" s="117"/>
+      <c r="B35" s="102"/>
+      <c r="C35" s="107"/>
       <c r="D35" s="21" t="s">
         <v>47</v>
       </c>
@@ -4033,8 +4033,8 @@
       <c r="W35" s="77"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B36" s="98"/>
-      <c r="C36" s="117"/>
+      <c r="B36" s="102"/>
+      <c r="C36" s="107"/>
       <c r="D36" s="21" t="s">
         <v>48</v>
       </c>
@@ -4092,8 +4092,8 @@
       <c r="W36" s="77"/>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B37" s="98"/>
-      <c r="C37" s="117"/>
+      <c r="B37" s="102"/>
+      <c r="C37" s="107"/>
       <c r="D37" s="21" t="s">
         <v>49</v>
       </c>
@@ -4151,8 +4151,8 @@
       <c r="W37" s="77"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B38" s="98"/>
-      <c r="C38" s="117"/>
+      <c r="B38" s="102"/>
+      <c r="C38" s="107"/>
       <c r="D38" s="21" t="s">
         <v>50</v>
       </c>
@@ -4210,8 +4210,8 @@
       <c r="W38" s="77"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B39" s="98"/>
-      <c r="C39" s="117"/>
+      <c r="B39" s="102"/>
+      <c r="C39" s="107"/>
       <c r="D39" s="21" t="s">
         <v>51</v>
       </c>
@@ -4269,8 +4269,8 @@
       <c r="W39" s="77"/>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B40" s="98"/>
-      <c r="C40" s="117"/>
+      <c r="B40" s="102"/>
+      <c r="C40" s="107"/>
       <c r="D40" s="21" t="s">
         <v>52</v>
       </c>
@@ -4328,8 +4328,8 @@
       <c r="W40" s="77"/>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B41" s="98"/>
-      <c r="C41" s="117"/>
+      <c r="B41" s="102"/>
+      <c r="C41" s="107"/>
       <c r="D41" s="21" t="s">
         <v>53</v>
       </c>
@@ -4387,8 +4387,8 @@
       <c r="W41" s="77"/>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B42" s="98"/>
-      <c r="C42" s="117"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="107"/>
       <c r="D42" s="21" t="s">
         <v>54</v>
       </c>
@@ -4446,8 +4446,8 @@
       <c r="W42" s="77"/>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B43" s="98"/>
-      <c r="C43" s="117"/>
+      <c r="B43" s="102"/>
+      <c r="C43" s="107"/>
       <c r="D43" s="21" t="s">
         <v>55</v>
       </c>
@@ -4505,8 +4505,8 @@
       <c r="W43" s="77"/>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B44" s="98"/>
-      <c r="C44" s="117"/>
+      <c r="B44" s="102"/>
+      <c r="C44" s="107"/>
       <c r="D44" s="21" t="s">
         <v>56</v>
       </c>
@@ -4564,8 +4564,8 @@
       <c r="W44" s="77"/>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B45" s="98"/>
-      <c r="C45" s="117"/>
+      <c r="B45" s="102"/>
+      <c r="C45" s="107"/>
       <c r="D45" s="21" t="s">
         <v>57</v>
       </c>
@@ -4623,8 +4623,8 @@
       <c r="W45" s="77"/>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B46" s="98"/>
-      <c r="C46" s="117"/>
+      <c r="B46" s="102"/>
+      <c r="C46" s="107"/>
       <c r="D46" s="21" t="s">
         <v>58</v>
       </c>
@@ -4682,8 +4682,8 @@
       <c r="W46" s="77"/>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B47" s="98"/>
-      <c r="C47" s="117"/>
+      <c r="B47" s="102"/>
+      <c r="C47" s="107"/>
       <c r="D47" s="21" t="s">
         <v>59</v>
       </c>
@@ -4741,8 +4741,8 @@
       <c r="W47" s="77"/>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B48" s="98"/>
-      <c r="C48" s="117"/>
+      <c r="B48" s="102"/>
+      <c r="C48" s="107"/>
       <c r="D48" s="21" t="s">
         <v>60</v>
       </c>
@@ -4800,8 +4800,8 @@
       <c r="W48" s="77"/>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B49" s="98"/>
-      <c r="C49" s="114" t="s">
+      <c r="B49" s="102"/>
+      <c r="C49" s="104" t="s">
         <v>25</v>
       </c>
       <c r="D49" s="18" t="s">
@@ -4861,8 +4861,8 @@
       <c r="W49" s="77"/>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B50" s="98"/>
-      <c r="C50" s="115"/>
+      <c r="B50" s="102"/>
+      <c r="C50" s="105"/>
       <c r="D50" s="18" t="s">
         <v>28</v>
       </c>
@@ -4920,8 +4920,8 @@
       <c r="W50" s="77"/>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B51" s="98"/>
-      <c r="C51" s="115"/>
+      <c r="B51" s="102"/>
+      <c r="C51" s="105"/>
       <c r="D51" s="18" t="s">
         <v>29</v>
       </c>
@@ -4979,8 +4979,8 @@
       <c r="W51" s="77"/>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B52" s="98"/>
-      <c r="C52" s="115"/>
+      <c r="B52" s="102"/>
+      <c r="C52" s="105"/>
       <c r="D52" s="18" t="s">
         <v>30</v>
       </c>
@@ -5038,8 +5038,8 @@
       <c r="W52" s="77"/>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B53" s="98"/>
-      <c r="C53" s="115"/>
+      <c r="B53" s="102"/>
+      <c r="C53" s="105"/>
       <c r="D53" s="18" t="s">
         <v>33</v>
       </c>
@@ -5097,8 +5097,8 @@
       <c r="W53" s="77"/>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B54" s="98"/>
-      <c r="C54" s="115"/>
+      <c r="B54" s="102"/>
+      <c r="C54" s="105"/>
       <c r="D54" s="18" t="s">
         <v>31</v>
       </c>
@@ -5156,8 +5156,8 @@
       <c r="W54" s="77"/>
     </row>
     <row r="55" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="105"/>
-      <c r="C55" s="115"/>
+      <c r="B55" s="119"/>
+      <c r="C55" s="105"/>
       <c r="D55" s="44" t="s">
         <v>32</v>
       </c>
@@ -5215,10 +5215,10 @@
       <c r="W55" s="80"/>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B56" s="97" t="s">
+      <c r="B56" s="101" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="118" t="s">
+      <c r="C56" s="108" t="s">
         <v>70</v>
       </c>
       <c r="D56" s="28" t="s">
@@ -5284,8 +5284,8 @@
       </c>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B57" s="98"/>
-      <c r="C57" s="119"/>
+      <c r="B57" s="102"/>
+      <c r="C57" s="109"/>
       <c r="D57" s="4" t="s">
         <v>62</v>
       </c>
@@ -5349,8 +5349,8 @@
       </c>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B58" s="98"/>
-      <c r="C58" s="119"/>
+      <c r="B58" s="102"/>
+      <c r="C58" s="109"/>
       <c r="D58" s="4" t="s">
         <v>63</v>
       </c>
@@ -5368,7 +5368,7 @@
       </c>
       <c r="I58" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J58" s="52">
         <v>0</v>
@@ -5406,12 +5406,16 @@
       <c r="U58" s="74">
         <v>0</v>
       </c>
-      <c r="V58" s="74"/>
-      <c r="W58" s="77"/>
+      <c r="V58" s="74">
+        <v>0</v>
+      </c>
+      <c r="W58" s="63">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B59" s="98"/>
-      <c r="C59" s="119"/>
+      <c r="B59" s="102"/>
+      <c r="C59" s="109"/>
       <c r="D59" s="18" t="s">
         <v>67</v>
       </c>
@@ -5475,7 +5479,7 @@
       </c>
     </row>
     <row r="60" spans="2:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B60" s="98"/>
+      <c r="B60" s="102"/>
       <c r="C60" s="22" t="s">
         <v>64</v>
       </c>
@@ -5535,10 +5539,12 @@
       <c r="V60" s="73">
         <v>4.0999999999999996</v>
       </c>
-      <c r="W60" s="63"/>
+      <c r="W60" s="63">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="2:23" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B61" s="98"/>
+      <c r="B61" s="102"/>
       <c r="C61" s="22" t="s">
         <v>72</v>
       </c>
@@ -5603,8 +5609,8 @@
       </c>
     </row>
     <row r="62" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="98"/>
-      <c r="C62" s="119" t="s">
+      <c r="B62" s="102"/>
+      <c r="C62" s="109" t="s">
         <v>71</v>
       </c>
       <c r="D62" s="4" t="s">
@@ -5670,8 +5676,8 @@
       </c>
     </row>
     <row r="63" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="98"/>
-      <c r="C63" s="119"/>
+      <c r="B63" s="102"/>
+      <c r="C63" s="109"/>
       <c r="D63" s="4" t="s">
         <v>66</v>
       </c>
@@ -5735,8 +5741,8 @@
       </c>
     </row>
     <row r="64" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="98"/>
-      <c r="C64" s="119"/>
+      <c r="B64" s="102"/>
+      <c r="C64" s="109"/>
       <c r="D64" s="4" t="s">
         <v>68</v>
       </c>
@@ -5754,7 +5760,7 @@
       </c>
       <c r="I64" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J64" s="52">
         <v>0</v>
@@ -5796,12 +5802,12 @@
         <v>0</v>
       </c>
       <c r="W64" s="63">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="99"/>
-      <c r="C65" s="120"/>
+      <c r="B65" s="103"/>
+      <c r="C65" s="110"/>
       <c r="D65" s="17" t="s">
         <v>69</v>
       </c>
@@ -5819,7 +5825,7 @@
       </c>
       <c r="I65" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J65" s="53">
         <v>0</v>
@@ -5854,15 +5860,21 @@
       <c r="T65" s="53">
         <v>0</v>
       </c>
-      <c r="U65" s="31"/>
-      <c r="V65" s="31"/>
-      <c r="W65" s="78"/>
+      <c r="U65" s="76">
+        <v>0</v>
+      </c>
+      <c r="V65" s="76">
+        <v>0</v>
+      </c>
+      <c r="W65" s="87">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="66" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="97" t="s">
+      <c r="B66" s="101" t="s">
         <v>106</v>
       </c>
-      <c r="C66" s="124" t="s">
+      <c r="C66" s="114" t="s">
         <v>107</v>
       </c>
       <c r="D66" s="28" t="s">
@@ -5928,8 +5940,8 @@
       </c>
     </row>
     <row r="67" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="98"/>
-      <c r="C67" s="109"/>
+      <c r="B67" s="102"/>
+      <c r="C67" s="97"/>
       <c r="D67" s="4" t="s">
         <v>123</v>
       </c>
@@ -5993,8 +6005,8 @@
       </c>
     </row>
     <row r="68" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="98"/>
-      <c r="C68" s="109"/>
+      <c r="B68" s="102"/>
+      <c r="C68" s="97"/>
       <c r="D68" s="4" t="s">
         <v>152</v>
       </c>
@@ -6052,8 +6064,8 @@
       <c r="W68" s="77"/>
     </row>
     <row r="69" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="98"/>
-      <c r="C69" s="109"/>
+      <c r="B69" s="102"/>
+      <c r="C69" s="97"/>
       <c r="D69" s="4" t="s">
         <v>124</v>
       </c>
@@ -6117,8 +6129,8 @@
       </c>
     </row>
     <row r="70" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="98"/>
-      <c r="C70" s="109"/>
+      <c r="B70" s="102"/>
+      <c r="C70" s="97"/>
       <c r="D70" s="4" t="s">
         <v>155</v>
       </c>
@@ -6176,8 +6188,8 @@
       <c r="W70" s="83"/>
     </row>
     <row r="71" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="98"/>
-      <c r="C71" s="109"/>
+      <c r="B71" s="102"/>
+      <c r="C71" s="97"/>
       <c r="D71" s="4" t="s">
         <v>154</v>
       </c>
@@ -6241,8 +6253,8 @@
       </c>
     </row>
     <row r="72" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="98"/>
-      <c r="C72" s="109"/>
+      <c r="B72" s="102"/>
+      <c r="C72" s="97"/>
       <c r="D72" s="4" t="s">
         <v>125</v>
       </c>
@@ -6300,8 +6312,8 @@
       <c r="W72" s="77"/>
     </row>
     <row r="73" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="98"/>
-      <c r="C73" s="109" t="s">
+      <c r="B73" s="102"/>
+      <c r="C73" s="97" t="s">
         <v>108</v>
       </c>
       <c r="D73" s="4" t="s">
@@ -6367,8 +6379,8 @@
       </c>
     </row>
     <row r="74" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="98"/>
-      <c r="C74" s="109"/>
+      <c r="B74" s="102"/>
+      <c r="C74" s="97"/>
       <c r="D74" s="4" t="s">
         <v>123</v>
       </c>
@@ -6426,8 +6438,8 @@
       <c r="W74" s="77"/>
     </row>
     <row r="75" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="98"/>
-      <c r="C75" s="109"/>
+      <c r="B75" s="102"/>
+      <c r="C75" s="97"/>
       <c r="D75" s="4" t="s">
         <v>152</v>
       </c>
@@ -6485,8 +6497,8 @@
       <c r="W75" s="77"/>
     </row>
     <row r="76" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="98"/>
-      <c r="C76" s="109"/>
+      <c r="B76" s="102"/>
+      <c r="C76" s="97"/>
       <c r="D76" s="4" t="s">
         <v>155</v>
       </c>
@@ -6544,8 +6556,8 @@
       <c r="W76" s="77"/>
     </row>
     <row r="77" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="98"/>
-      <c r="C77" s="109"/>
+      <c r="B77" s="102"/>
+      <c r="C77" s="97"/>
       <c r="D77" s="4" t="s">
         <v>154</v>
       </c>
@@ -6605,8 +6617,8 @@
       <c r="W77" s="63"/>
     </row>
     <row r="78" spans="2:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="98"/>
-      <c r="C78" s="109"/>
+      <c r="B78" s="102"/>
+      <c r="C78" s="97"/>
       <c r="D78" s="4" t="s">
         <v>124</v>
       </c>
@@ -6670,8 +6682,8 @@
       </c>
     </row>
     <row r="79" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="98"/>
-      <c r="C79" s="109"/>
+      <c r="B79" s="102"/>
+      <c r="C79" s="97"/>
       <c r="D79" s="4" t="s">
         <v>125</v>
       </c>
@@ -6729,8 +6741,8 @@
       <c r="W79" s="77"/>
     </row>
     <row r="80" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="98"/>
-      <c r="C80" s="109" t="s">
+      <c r="B80" s="102"/>
+      <c r="C80" s="97" t="s">
         <v>109</v>
       </c>
       <c r="D80" s="4" t="s">
@@ -6796,8 +6808,8 @@
       </c>
     </row>
     <row r="81" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="98"/>
-      <c r="C81" s="109"/>
+      <c r="B81" s="102"/>
+      <c r="C81" s="97"/>
       <c r="D81" s="4" t="s">
         <v>123</v>
       </c>
@@ -6855,8 +6867,8 @@
       <c r="W81" s="77"/>
     </row>
     <row r="82" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="98"/>
-      <c r="C82" s="109"/>
+      <c r="B82" s="102"/>
+      <c r="C82" s="97"/>
       <c r="D82" s="4" t="s">
         <v>152</v>
       </c>
@@ -6914,8 +6926,8 @@
       <c r="W82" s="77"/>
     </row>
     <row r="83" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="98"/>
-      <c r="C83" s="109"/>
+      <c r="B83" s="102"/>
+      <c r="C83" s="97"/>
       <c r="D83" s="4" t="s">
         <v>124</v>
       </c>
@@ -6979,8 +6991,8 @@
       </c>
     </row>
     <row r="84" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="98"/>
-      <c r="C84" s="109"/>
+      <c r="B84" s="102"/>
+      <c r="C84" s="97"/>
       <c r="D84" s="4" t="s">
         <v>155</v>
       </c>
@@ -7038,8 +7050,8 @@
       <c r="W84" s="83"/>
     </row>
     <row r="85" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="98"/>
-      <c r="C85" s="109"/>
+      <c r="B85" s="102"/>
+      <c r="C85" s="97"/>
       <c r="D85" s="4" t="s">
         <v>154</v>
       </c>
@@ -7103,8 +7115,8 @@
       </c>
     </row>
     <row r="86" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="98"/>
-      <c r="C86" s="109"/>
+      <c r="B86" s="102"/>
+      <c r="C86" s="97"/>
       <c r="D86" s="4" t="s">
         <v>125</v>
       </c>
@@ -7162,8 +7174,8 @@
       <c r="W86" s="77"/>
     </row>
     <row r="87" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="98"/>
-      <c r="C87" s="109" t="s">
+      <c r="B87" s="102"/>
+      <c r="C87" s="97" t="s">
         <v>110</v>
       </c>
       <c r="D87" s="4" t="s">
@@ -7229,8 +7241,8 @@
       </c>
     </row>
     <row r="88" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="98"/>
-      <c r="C88" s="109"/>
+      <c r="B88" s="102"/>
+      <c r="C88" s="97"/>
       <c r="D88" s="4" t="s">
         <v>123</v>
       </c>
@@ -7288,8 +7300,8 @@
       <c r="W88" s="77"/>
     </row>
     <row r="89" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="98"/>
-      <c r="C89" s="109"/>
+      <c r="B89" s="102"/>
+      <c r="C89" s="97"/>
       <c r="D89" s="4" t="s">
         <v>152</v>
       </c>
@@ -7347,8 +7359,8 @@
       <c r="W89" s="77"/>
     </row>
     <row r="90" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="98"/>
-      <c r="C90" s="109"/>
+      <c r="B90" s="102"/>
+      <c r="C90" s="97"/>
       <c r="D90" s="4" t="s">
         <v>124</v>
       </c>
@@ -7412,8 +7424,8 @@
       </c>
     </row>
     <row r="91" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="98"/>
-      <c r="C91" s="109"/>
+      <c r="B91" s="102"/>
+      <c r="C91" s="97"/>
       <c r="D91" s="4" t="s">
         <v>155</v>
       </c>
@@ -7471,8 +7483,8 @@
       <c r="W91" s="83"/>
     </row>
     <row r="92" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="98"/>
-      <c r="C92" s="109"/>
+      <c r="B92" s="102"/>
+      <c r="C92" s="97"/>
       <c r="D92" s="4" t="s">
         <v>154</v>
       </c>
@@ -7532,8 +7544,8 @@
       <c r="W92" s="63"/>
     </row>
     <row r="93" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="98"/>
-      <c r="C93" s="109"/>
+      <c r="B93" s="102"/>
+      <c r="C93" s="97"/>
       <c r="D93" s="4" t="s">
         <v>125</v>
       </c>
@@ -7591,8 +7603,8 @@
       <c r="W93" s="77"/>
     </row>
     <row r="94" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="98"/>
-      <c r="C94" s="109" t="s">
+      <c r="B94" s="102"/>
+      <c r="C94" s="97" t="s">
         <v>111</v>
       </c>
       <c r="D94" s="4" t="s">
@@ -7658,8 +7670,8 @@
       </c>
     </row>
     <row r="95" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="98"/>
-      <c r="C95" s="109"/>
+      <c r="B95" s="102"/>
+      <c r="C95" s="97"/>
       <c r="D95" s="4" t="s">
         <v>123</v>
       </c>
@@ -7717,8 +7729,8 @@
       <c r="W95" s="77"/>
     </row>
     <row r="96" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="98"/>
-      <c r="C96" s="109"/>
+      <c r="B96" s="102"/>
+      <c r="C96" s="97"/>
       <c r="D96" s="4" t="s">
         <v>152</v>
       </c>
@@ -7776,8 +7788,8 @@
       <c r="W96" s="77"/>
     </row>
     <row r="97" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="98"/>
-      <c r="C97" s="109"/>
+      <c r="B97" s="102"/>
+      <c r="C97" s="97"/>
       <c r="D97" s="4" t="s">
         <v>124</v>
       </c>
@@ -7841,8 +7853,8 @@
       </c>
     </row>
     <row r="98" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="98"/>
-      <c r="C98" s="109"/>
+      <c r="B98" s="102"/>
+      <c r="C98" s="97"/>
       <c r="D98" s="4" t="s">
         <v>155</v>
       </c>
@@ -7900,8 +7912,8 @@
       <c r="W98" s="83"/>
     </row>
     <row r="99" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="98"/>
-      <c r="C99" s="109"/>
+      <c r="B99" s="102"/>
+      <c r="C99" s="97"/>
       <c r="D99" s="4" t="s">
         <v>154</v>
       </c>
@@ -7965,8 +7977,8 @@
       </c>
     </row>
     <row r="100" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="98"/>
-      <c r="C100" s="109"/>
+      <c r="B100" s="102"/>
+      <c r="C100" s="97"/>
       <c r="D100" s="4" t="s">
         <v>125</v>
       </c>
@@ -8024,8 +8036,8 @@
       <c r="W100" s="77"/>
     </row>
     <row r="101" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="98"/>
-      <c r="C101" s="109" t="s">
+      <c r="B101" s="102"/>
+      <c r="C101" s="97" t="s">
         <v>112</v>
       </c>
       <c r="D101" s="4" t="s">
@@ -8091,8 +8103,8 @@
       </c>
     </row>
     <row r="102" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="98"/>
-      <c r="C102" s="109"/>
+      <c r="B102" s="102"/>
+      <c r="C102" s="97"/>
       <c r="D102" s="4" t="s">
         <v>123</v>
       </c>
@@ -8150,8 +8162,8 @@
       <c r="W102" s="77"/>
     </row>
     <row r="103" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="98"/>
-      <c r="C103" s="109"/>
+      <c r="B103" s="102"/>
+      <c r="C103" s="97"/>
       <c r="D103" s="4" t="s">
         <v>152</v>
       </c>
@@ -8209,8 +8221,8 @@
       <c r="W103" s="77"/>
     </row>
     <row r="104" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="98"/>
-      <c r="C104" s="109"/>
+      <c r="B104" s="102"/>
+      <c r="C104" s="97"/>
       <c r="D104" s="4" t="s">
         <v>124</v>
       </c>
@@ -8274,8 +8286,8 @@
       </c>
     </row>
     <row r="105" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="98"/>
-      <c r="C105" s="109"/>
+      <c r="B105" s="102"/>
+      <c r="C105" s="97"/>
       <c r="D105" s="4" t="s">
         <v>155</v>
       </c>
@@ -8333,8 +8345,8 @@
       <c r="W105" s="83"/>
     </row>
     <row r="106" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="98"/>
-      <c r="C106" s="109"/>
+      <c r="B106" s="102"/>
+      <c r="C106" s="97"/>
       <c r="D106" s="4" t="s">
         <v>154</v>
       </c>
@@ -8394,8 +8406,8 @@
       <c r="W106" s="63"/>
     </row>
     <row r="107" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="98"/>
-      <c r="C107" s="109"/>
+      <c r="B107" s="102"/>
+      <c r="C107" s="97"/>
       <c r="D107" s="4" t="s">
         <v>125</v>
       </c>
@@ -8454,8 +8466,8 @@
       <c r="X107" s="92"/>
     </row>
     <row r="108" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="98"/>
-      <c r="C108" s="109" t="s">
+      <c r="B108" s="102"/>
+      <c r="C108" s="97" t="s">
         <v>113</v>
       </c>
       <c r="D108" s="4" t="s">
@@ -8521,8 +8533,8 @@
       </c>
     </row>
     <row r="109" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="98"/>
-      <c r="C109" s="109"/>
+      <c r="B109" s="102"/>
+      <c r="C109" s="97"/>
       <c r="D109" s="4" t="s">
         <v>123</v>
       </c>
@@ -8580,8 +8592,8 @@
       <c r="W109" s="77"/>
     </row>
     <row r="110" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="98"/>
-      <c r="C110" s="109"/>
+      <c r="B110" s="102"/>
+      <c r="C110" s="97"/>
       <c r="D110" s="4" t="s">
         <v>152</v>
       </c>
@@ -8639,8 +8651,8 @@
       <c r="W110" s="77"/>
     </row>
     <row r="111" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="98"/>
-      <c r="C111" s="109"/>
+      <c r="B111" s="102"/>
+      <c r="C111" s="97"/>
       <c r="D111" s="4" t="s">
         <v>124</v>
       </c>
@@ -8704,8 +8716,8 @@
       </c>
     </row>
     <row r="112" spans="2:24" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="98"/>
-      <c r="C112" s="109"/>
+      <c r="B112" s="102"/>
+      <c r="C112" s="97"/>
       <c r="D112" s="4" t="s">
         <v>155</v>
       </c>
@@ -8763,8 +8775,8 @@
       <c r="W112" s="83"/>
     </row>
     <row r="113" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="98"/>
-      <c r="C113" s="109"/>
+      <c r="B113" s="102"/>
+      <c r="C113" s="97"/>
       <c r="D113" s="4" t="s">
         <v>154</v>
       </c>
@@ -8824,8 +8836,8 @@
       <c r="W113" s="63"/>
     </row>
     <row r="114" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="98"/>
-      <c r="C114" s="109"/>
+      <c r="B114" s="102"/>
+      <c r="C114" s="97"/>
       <c r="D114" s="4" t="s">
         <v>125</v>
       </c>
@@ -8883,8 +8895,8 @@
       <c r="W114" s="77"/>
     </row>
     <row r="115" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="98"/>
-      <c r="C115" s="109" t="s">
+      <c r="B115" s="102"/>
+      <c r="C115" s="97" t="s">
         <v>114</v>
       </c>
       <c r="D115" s="4" t="s">
@@ -8950,8 +8962,8 @@
       </c>
     </row>
     <row r="116" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="98"/>
-      <c r="C116" s="109"/>
+      <c r="B116" s="102"/>
+      <c r="C116" s="97"/>
       <c r="D116" s="4" t="s">
         <v>123</v>
       </c>
@@ -9009,8 +9021,8 @@
       <c r="W116" s="77"/>
     </row>
     <row r="117" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="98"/>
-      <c r="C117" s="109"/>
+      <c r="B117" s="102"/>
+      <c r="C117" s="97"/>
       <c r="D117" s="4" t="s">
         <v>152</v>
       </c>
@@ -9068,8 +9080,8 @@
       <c r="W117" s="77"/>
     </row>
     <row r="118" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="98"/>
-      <c r="C118" s="109"/>
+      <c r="B118" s="102"/>
+      <c r="C118" s="97"/>
       <c r="D118" s="4" t="s">
         <v>124</v>
       </c>
@@ -9133,8 +9145,8 @@
       </c>
     </row>
     <row r="119" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="98"/>
-      <c r="C119" s="109"/>
+      <c r="B119" s="102"/>
+      <c r="C119" s="97"/>
       <c r="D119" s="4" t="s">
         <v>155</v>
       </c>
@@ -9192,8 +9204,8 @@
       <c r="W119" s="83"/>
     </row>
     <row r="120" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="98"/>
-      <c r="C120" s="109"/>
+      <c r="B120" s="102"/>
+      <c r="C120" s="97"/>
       <c r="D120" s="4" t="s">
         <v>154</v>
       </c>
@@ -9257,8 +9269,8 @@
       </c>
     </row>
     <row r="121" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="98"/>
-      <c r="C121" s="109"/>
+      <c r="B121" s="102"/>
+      <c r="C121" s="97"/>
       <c r="D121" s="4" t="s">
         <v>125</v>
       </c>
@@ -9316,8 +9328,8 @@
       <c r="W121" s="77"/>
     </row>
     <row r="122" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="98"/>
-      <c r="C122" s="109" t="s">
+      <c r="B122" s="102"/>
+      <c r="C122" s="97" t="s">
         <v>115</v>
       </c>
       <c r="D122" s="4" t="s">
@@ -9383,8 +9395,8 @@
       </c>
     </row>
     <row r="123" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="98"/>
-      <c r="C123" s="109"/>
+      <c r="B123" s="102"/>
+      <c r="C123" s="97"/>
       <c r="D123" s="4" t="s">
         <v>123</v>
       </c>
@@ -9442,8 +9454,8 @@
       <c r="W123" s="77"/>
     </row>
     <row r="124" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="98"/>
-      <c r="C124" s="109"/>
+      <c r="B124" s="102"/>
+      <c r="C124" s="97"/>
       <c r="D124" s="4" t="s">
         <v>152</v>
       </c>
@@ -9501,8 +9513,8 @@
       <c r="W124" s="77"/>
     </row>
     <row r="125" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="98"/>
-      <c r="C125" s="109"/>
+      <c r="B125" s="102"/>
+      <c r="C125" s="97"/>
       <c r="D125" s="4" t="s">
         <v>124</v>
       </c>
@@ -9566,8 +9578,8 @@
       </c>
     </row>
     <row r="126" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="98"/>
-      <c r="C126" s="109"/>
+      <c r="B126" s="102"/>
+      <c r="C126" s="97"/>
       <c r="D126" s="4" t="s">
         <v>155</v>
       </c>
@@ -9625,8 +9637,8 @@
       <c r="W126" s="83"/>
     </row>
     <row r="127" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="98"/>
-      <c r="C127" s="109"/>
+      <c r="B127" s="102"/>
+      <c r="C127" s="97"/>
       <c r="D127" s="4" t="s">
         <v>154</v>
       </c>
@@ -9686,8 +9698,8 @@
       <c r="W127" s="63"/>
     </row>
     <row r="128" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="98"/>
-      <c r="C128" s="109"/>
+      <c r="B128" s="102"/>
+      <c r="C128" s="97"/>
       <c r="D128" s="4" t="s">
         <v>125</v>
       </c>
@@ -9745,8 +9757,8 @@
       <c r="W128" s="77"/>
     </row>
     <row r="129" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="98"/>
-      <c r="C129" s="109" t="s">
+      <c r="B129" s="102"/>
+      <c r="C129" s="97" t="s">
         <v>116</v>
       </c>
       <c r="D129" s="4" t="s">
@@ -9812,8 +9824,8 @@
       </c>
     </row>
     <row r="130" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="98"/>
-      <c r="C130" s="109"/>
+      <c r="B130" s="102"/>
+      <c r="C130" s="97"/>
       <c r="D130" s="4" t="s">
         <v>123</v>
       </c>
@@ -9871,8 +9883,8 @@
       <c r="W130" s="77"/>
     </row>
     <row r="131" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="98"/>
-      <c r="C131" s="109"/>
+      <c r="B131" s="102"/>
+      <c r="C131" s="97"/>
       <c r="D131" s="4" t="s">
         <v>152</v>
       </c>
@@ -9930,8 +9942,8 @@
       <c r="W131" s="77"/>
     </row>
     <row r="132" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="98"/>
-      <c r="C132" s="109"/>
+      <c r="B132" s="102"/>
+      <c r="C132" s="97"/>
       <c r="D132" s="4" t="s">
         <v>124</v>
       </c>
@@ -9995,8 +10007,8 @@
       </c>
     </row>
     <row r="133" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="98"/>
-      <c r="C133" s="109"/>
+      <c r="B133" s="102"/>
+      <c r="C133" s="97"/>
       <c r="D133" s="4" t="s">
         <v>155</v>
       </c>
@@ -10054,8 +10066,8 @@
       <c r="W133" s="83"/>
     </row>
     <row r="134" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="98"/>
-      <c r="C134" s="109"/>
+      <c r="B134" s="102"/>
+      <c r="C134" s="97"/>
       <c r="D134" s="4" t="s">
         <v>154</v>
       </c>
@@ -10119,8 +10131,8 @@
       </c>
     </row>
     <row r="135" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="98"/>
-      <c r="C135" s="109"/>
+      <c r="B135" s="102"/>
+      <c r="C135" s="97"/>
       <c r="D135" s="4" t="s">
         <v>125</v>
       </c>
@@ -10178,8 +10190,8 @@
       <c r="W135" s="77"/>
     </row>
     <row r="136" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="98"/>
-      <c r="C136" s="109" t="s">
+      <c r="B136" s="102"/>
+      <c r="C136" s="97" t="s">
         <v>117</v>
       </c>
       <c r="D136" s="4" t="s">
@@ -10245,8 +10257,8 @@
       </c>
     </row>
     <row r="137" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="98"/>
-      <c r="C137" s="109"/>
+      <c r="B137" s="102"/>
+      <c r="C137" s="97"/>
       <c r="D137" s="4" t="s">
         <v>123</v>
       </c>
@@ -10304,8 +10316,8 @@
       <c r="W137" s="77"/>
     </row>
     <row r="138" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="98"/>
-      <c r="C138" s="109"/>
+      <c r="B138" s="102"/>
+      <c r="C138" s="97"/>
       <c r="D138" s="4" t="s">
         <v>152</v>
       </c>
@@ -10363,8 +10375,8 @@
       <c r="W138" s="77"/>
     </row>
     <row r="139" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="98"/>
-      <c r="C139" s="109"/>
+      <c r="B139" s="102"/>
+      <c r="C139" s="97"/>
       <c r="D139" s="4" t="s">
         <v>124</v>
       </c>
@@ -10428,8 +10440,8 @@
       </c>
     </row>
     <row r="140" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="98"/>
-      <c r="C140" s="109"/>
+      <c r="B140" s="102"/>
+      <c r="C140" s="97"/>
       <c r="D140" s="4" t="s">
         <v>155</v>
       </c>
@@ -10487,8 +10499,8 @@
       <c r="W140" s="83"/>
     </row>
     <row r="141" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="98"/>
-      <c r="C141" s="109"/>
+      <c r="B141" s="102"/>
+      <c r="C141" s="97"/>
       <c r="D141" s="4" t="s">
         <v>154</v>
       </c>
@@ -10552,8 +10564,8 @@
       </c>
     </row>
     <row r="142" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="98"/>
-      <c r="C142" s="109"/>
+      <c r="B142" s="102"/>
+      <c r="C142" s="97"/>
       <c r="D142" s="4" t="s">
         <v>125</v>
       </c>
@@ -10611,8 +10623,8 @@
       <c r="W142" s="77"/>
     </row>
     <row r="143" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="98"/>
-      <c r="C143" s="109" t="s">
+      <c r="B143" s="102"/>
+      <c r="C143" s="97" t="s">
         <v>118</v>
       </c>
       <c r="D143" s="4" t="s">
@@ -10678,8 +10690,8 @@
       </c>
     </row>
     <row r="144" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="98"/>
-      <c r="C144" s="109"/>
+      <c r="B144" s="102"/>
+      <c r="C144" s="97"/>
       <c r="D144" s="4" t="s">
         <v>123</v>
       </c>
@@ -10737,8 +10749,8 @@
       <c r="W144" s="77"/>
     </row>
     <row r="145" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="98"/>
-      <c r="C145" s="109"/>
+      <c r="B145" s="102"/>
+      <c r="C145" s="97"/>
       <c r="D145" s="4" t="s">
         <v>152</v>
       </c>
@@ -10796,8 +10808,8 @@
       <c r="W145" s="77"/>
     </row>
     <row r="146" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="98"/>
-      <c r="C146" s="109"/>
+      <c r="B146" s="102"/>
+      <c r="C146" s="97"/>
       <c r="D146" s="4" t="s">
         <v>124</v>
       </c>
@@ -10861,8 +10873,8 @@
       </c>
     </row>
     <row r="147" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="98"/>
-      <c r="C147" s="109"/>
+      <c r="B147" s="102"/>
+      <c r="C147" s="97"/>
       <c r="D147" s="4" t="s">
         <v>155</v>
       </c>
@@ -10920,8 +10932,8 @@
       <c r="W147" s="83"/>
     </row>
     <row r="148" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="98"/>
-      <c r="C148" s="109"/>
+      <c r="B148" s="102"/>
+      <c r="C148" s="97"/>
       <c r="D148" s="4" t="s">
         <v>154</v>
       </c>
@@ -10985,8 +10997,8 @@
       </c>
     </row>
     <row r="149" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="98"/>
-      <c r="C149" s="109"/>
+      <c r="B149" s="102"/>
+      <c r="C149" s="97"/>
       <c r="D149" s="4" t="s">
         <v>125</v>
       </c>
@@ -11044,8 +11056,8 @@
       <c r="W149" s="77"/>
     </row>
     <row r="150" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="98"/>
-      <c r="C150" s="109" t="s">
+      <c r="B150" s="102"/>
+      <c r="C150" s="97" t="s">
         <v>119</v>
       </c>
       <c r="D150" s="4" t="s">
@@ -11111,8 +11123,8 @@
       </c>
     </row>
     <row r="151" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="98"/>
-      <c r="C151" s="109"/>
+      <c r="B151" s="102"/>
+      <c r="C151" s="97"/>
       <c r="D151" s="4" t="s">
         <v>123</v>
       </c>
@@ -11170,8 +11182,8 @@
       <c r="W151" s="77"/>
     </row>
     <row r="152" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="98"/>
-      <c r="C152" s="109"/>
+      <c r="B152" s="102"/>
+      <c r="C152" s="97"/>
       <c r="D152" s="4" t="s">
         <v>152</v>
       </c>
@@ -11229,8 +11241,8 @@
       <c r="W152" s="77"/>
     </row>
     <row r="153" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="98"/>
-      <c r="C153" s="109"/>
+      <c r="B153" s="102"/>
+      <c r="C153" s="97"/>
       <c r="D153" s="4" t="s">
         <v>124</v>
       </c>
@@ -11294,8 +11306,8 @@
       </c>
     </row>
     <row r="154" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="98"/>
-      <c r="C154" s="109"/>
+      <c r="B154" s="102"/>
+      <c r="C154" s="97"/>
       <c r="D154" s="4" t="s">
         <v>155</v>
       </c>
@@ -11353,8 +11365,8 @@
       <c r="W154" s="83"/>
     </row>
     <row r="155" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="98"/>
-      <c r="C155" s="109"/>
+      <c r="B155" s="102"/>
+      <c r="C155" s="97"/>
       <c r="D155" s="4" t="s">
         <v>154</v>
       </c>
@@ -11414,8 +11426,8 @@
       <c r="W155" s="63"/>
     </row>
     <row r="156" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="98"/>
-      <c r="C156" s="109"/>
+      <c r="B156" s="102"/>
+      <c r="C156" s="97"/>
       <c r="D156" s="4" t="s">
         <v>125</v>
       </c>
@@ -11473,8 +11485,8 @@
       <c r="W156" s="77"/>
     </row>
     <row r="157" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="98"/>
-      <c r="C157" s="109" t="s">
+      <c r="B157" s="102"/>
+      <c r="C157" s="97" t="s">
         <v>120</v>
       </c>
       <c r="D157" s="4" t="s">
@@ -11540,8 +11552,8 @@
       </c>
     </row>
     <row r="158" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="98"/>
-      <c r="C158" s="109"/>
+      <c r="B158" s="102"/>
+      <c r="C158" s="97"/>
       <c r="D158" s="4" t="s">
         <v>123</v>
       </c>
@@ -11599,8 +11611,8 @@
       <c r="W158" s="77"/>
     </row>
     <row r="159" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="98"/>
-      <c r="C159" s="109"/>
+      <c r="B159" s="102"/>
+      <c r="C159" s="97"/>
       <c r="D159" s="4" t="s">
         <v>152</v>
       </c>
@@ -11658,8 +11670,8 @@
       <c r="W159" s="77"/>
     </row>
     <row r="160" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="98"/>
-      <c r="C160" s="109"/>
+      <c r="B160" s="102"/>
+      <c r="C160" s="97"/>
       <c r="D160" s="4" t="s">
         <v>124</v>
       </c>
@@ -11723,8 +11735,8 @@
       </c>
     </row>
     <row r="161" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="98"/>
-      <c r="C161" s="109"/>
+      <c r="B161" s="102"/>
+      <c r="C161" s="97"/>
       <c r="D161" s="4" t="s">
         <v>155</v>
       </c>
@@ -11782,8 +11794,8 @@
       <c r="W161" s="83"/>
     </row>
     <row r="162" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="98"/>
-      <c r="C162" s="109"/>
+      <c r="B162" s="102"/>
+      <c r="C162" s="97"/>
       <c r="D162" s="4" t="s">
         <v>154</v>
       </c>
@@ -11847,8 +11859,8 @@
       </c>
     </row>
     <row r="163" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="98"/>
-      <c r="C163" s="109"/>
+      <c r="B163" s="102"/>
+      <c r="C163" s="97"/>
       <c r="D163" s="4" t="s">
         <v>125</v>
       </c>
@@ -11906,8 +11918,8 @@
       <c r="W163" s="77"/>
     </row>
     <row r="164" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="98"/>
-      <c r="C164" s="109" t="s">
+      <c r="B164" s="102"/>
+      <c r="C164" s="97" t="s">
         <v>121</v>
       </c>
       <c r="D164" s="4" t="s">
@@ -11973,8 +11985,8 @@
       </c>
     </row>
     <row r="165" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="98"/>
-      <c r="C165" s="109"/>
+      <c r="B165" s="102"/>
+      <c r="C165" s="97"/>
       <c r="D165" s="4" t="s">
         <v>123</v>
       </c>
@@ -12032,8 +12044,8 @@
       <c r="W165" s="77"/>
     </row>
     <row r="166" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B166" s="98"/>
-      <c r="C166" s="109"/>
+      <c r="B166" s="102"/>
+      <c r="C166" s="97"/>
       <c r="D166" s="4" t="s">
         <v>152</v>
       </c>
@@ -12091,8 +12103,8 @@
       <c r="W166" s="77"/>
     </row>
     <row r="167" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B167" s="98"/>
-      <c r="C167" s="109"/>
+      <c r="B167" s="102"/>
+      <c r="C167" s="97"/>
       <c r="D167" s="4" t="s">
         <v>124</v>
       </c>
@@ -12156,8 +12168,8 @@
       </c>
     </row>
     <row r="168" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B168" s="105"/>
-      <c r="C168" s="112"/>
+      <c r="B168" s="119"/>
+      <c r="C168" s="123"/>
       <c r="D168" s="4" t="s">
         <v>155</v>
       </c>
@@ -12215,8 +12227,8 @@
       <c r="W168" s="85"/>
     </row>
     <row r="169" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B169" s="105"/>
-      <c r="C169" s="112"/>
+      <c r="B169" s="119"/>
+      <c r="C169" s="123"/>
       <c r="D169" s="4" t="s">
         <v>154</v>
       </c>
@@ -12280,8 +12292,8 @@
       </c>
     </row>
     <row r="170" spans="2:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B170" s="99"/>
-      <c r="C170" s="113"/>
+      <c r="B170" s="103"/>
+      <c r="C170" s="124"/>
       <c r="D170" s="17" t="s">
         <v>125</v>
       </c>
@@ -12339,7 +12351,7 @@
       <c r="W170" s="78"/>
     </row>
     <row r="171" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B171" s="97" t="s">
+      <c r="B171" s="101" t="s">
         <v>74</v>
       </c>
       <c r="C171" s="60" t="s">
@@ -12406,7 +12418,7 @@
       </c>
     </row>
     <row r="172" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B172" s="98"/>
+      <c r="B172" s="102"/>
       <c r="C172" s="22" t="s">
         <v>80</v>
       </c>
@@ -12465,7 +12477,7 @@
       <c r="W172" s="77"/>
     </row>
     <row r="173" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B173" s="98"/>
+      <c r="B173" s="102"/>
       <c r="C173" s="22" t="s">
         <v>81</v>
       </c>
@@ -12524,7 +12536,7 @@
       <c r="W173" s="77"/>
     </row>
     <row r="174" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B174" s="98"/>
+      <c r="B174" s="102"/>
       <c r="C174" s="22" t="s">
         <v>82</v>
       </c>
@@ -12583,7 +12595,7 @@
       <c r="W174" s="77"/>
     </row>
     <row r="175" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B175" s="98"/>
+      <c r="B175" s="102"/>
       <c r="C175" s="22" t="s">
         <v>132</v>
       </c>
@@ -12642,7 +12654,7 @@
       <c r="W175" s="77"/>
     </row>
     <row r="176" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="98"/>
+      <c r="B176" s="102"/>
       <c r="C176" s="22" t="s">
         <v>129</v>
       </c>
@@ -12701,7 +12713,7 @@
       <c r="W176" s="77"/>
     </row>
     <row r="177" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B177" s="98"/>
+      <c r="B177" s="102"/>
       <c r="C177" s="22" t="s">
         <v>131</v>
       </c>
@@ -12760,7 +12772,7 @@
       <c r="W177" s="77"/>
     </row>
     <row r="178" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B178" s="98"/>
+      <c r="B178" s="102"/>
       <c r="C178" s="22" t="s">
         <v>130</v>
       </c>
@@ -12819,7 +12831,7 @@
       <c r="W178" s="77"/>
     </row>
     <row r="179" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B179" s="98"/>
+      <c r="B179" s="102"/>
       <c r="C179" s="22" t="s">
         <v>83</v>
       </c>
@@ -12884,7 +12896,7 @@
       </c>
     </row>
     <row r="180" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B180" s="98"/>
+      <c r="B180" s="102"/>
       <c r="C180" s="22" t="s">
         <v>84</v>
       </c>
@@ -12949,7 +12961,7 @@
       </c>
     </row>
     <row r="181" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B181" s="98"/>
+      <c r="B181" s="102"/>
       <c r="C181" s="22" t="s">
         <v>85</v>
       </c>
@@ -13014,7 +13026,7 @@
       </c>
     </row>
     <row r="182" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B182" s="98"/>
+      <c r="B182" s="102"/>
       <c r="C182" s="22" t="s">
         <v>89</v>
       </c>
@@ -13079,7 +13091,7 @@
       </c>
     </row>
     <row r="183" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B183" s="99"/>
+      <c r="B183" s="103"/>
       <c r="C183" s="43" t="s">
         <v>90</v>
       </c>
@@ -13138,7 +13150,7 @@
       <c r="W183" s="78"/>
     </row>
     <row r="184" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B184" s="97" t="s">
+      <c r="B184" s="101" t="s">
         <v>133</v>
       </c>
       <c r="C184" s="42" t="s">
@@ -13199,7 +13211,7 @@
       <c r="W184" s="81"/>
     </row>
     <row r="185" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="98"/>
+      <c r="B185" s="102"/>
       <c r="C185" s="41" t="s">
         <v>134</v>
       </c>
@@ -13258,7 +13270,7 @@
       <c r="W185" s="77"/>
     </row>
     <row r="186" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B186" s="99"/>
+      <c r="B186" s="103"/>
       <c r="C186" s="43" t="s">
         <v>135</v>
       </c>
@@ -13317,7 +13329,7 @@
       <c r="W186" s="78"/>
     </row>
     <row r="187" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B187" s="97" t="s">
+      <c r="B187" s="101" t="s">
         <v>138</v>
       </c>
       <c r="C187" s="42" t="s">
@@ -13378,7 +13390,7 @@
       <c r="W187" s="81"/>
     </row>
     <row r="188" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B188" s="98"/>
+      <c r="B188" s="102"/>
       <c r="C188" s="41" t="s">
         <v>140</v>
       </c>
@@ -13437,7 +13449,7 @@
       <c r="W188" s="77"/>
     </row>
     <row r="189" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B189" s="98"/>
+      <c r="B189" s="102"/>
       <c r="C189" s="41" t="s">
         <v>157</v>
       </c>
@@ -13496,7 +13508,7 @@
       <c r="W189" s="77"/>
     </row>
     <row r="190" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B190" s="98"/>
+      <c r="B190" s="102"/>
       <c r="C190" s="41" t="s">
         <v>141</v>
       </c>
@@ -13555,7 +13567,7 @@
       <c r="W190" s="77"/>
     </row>
     <row r="191" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B191" s="98"/>
+      <c r="B191" s="102"/>
       <c r="C191" s="41" t="s">
         <v>142</v>
       </c>
@@ -13614,7 +13626,7 @@
       <c r="W191" s="77"/>
     </row>
     <row r="192" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B192" s="98"/>
+      <c r="B192" s="102"/>
       <c r="C192" s="41" t="s">
         <v>160</v>
       </c>
@@ -13673,7 +13685,7 @@
       <c r="W192" s="77"/>
     </row>
     <row r="193" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="98"/>
+      <c r="B193" s="102"/>
       <c r="C193" s="41" t="s">
         <v>159</v>
       </c>
@@ -13732,7 +13744,7 @@
       <c r="W193" s="77"/>
     </row>
     <row r="194" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B194" s="98"/>
+      <c r="B194" s="102"/>
       <c r="C194" s="41" t="s">
         <v>158</v>
       </c>
@@ -13791,7 +13803,7 @@
       <c r="W194" s="77"/>
     </row>
     <row r="195" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="98"/>
+      <c r="B195" s="102"/>
       <c r="C195" s="41" t="s">
         <v>143</v>
       </c>
@@ -13850,7 +13862,7 @@
       <c r="W195" s="77"/>
     </row>
     <row r="196" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="98"/>
+      <c r="B196" s="102"/>
       <c r="C196" s="41" t="s">
         <v>144</v>
       </c>
@@ -13909,7 +13921,7 @@
       <c r="W196" s="77"/>
     </row>
     <row r="197" spans="2:23" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B197" s="99"/>
+      <c r="B197" s="103"/>
       <c r="C197" s="43" t="s">
         <v>145</v>
       </c>
@@ -13968,7 +13980,7 @@
       <c r="W197" s="78"/>
     </row>
     <row r="198" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B198" s="97" t="s">
+      <c r="B198" s="101" t="s">
         <v>17</v>
       </c>
       <c r="C198" s="36" t="s">
@@ -14029,7 +14041,7 @@
       <c r="W198" s="81"/>
     </row>
     <row r="199" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B199" s="98"/>
+      <c r="B199" s="102"/>
       <c r="C199" s="22" t="s">
         <v>127</v>
       </c>
@@ -14088,7 +14100,7 @@
       <c r="W199" s="77"/>
     </row>
     <row r="200" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B200" s="98"/>
+      <c r="B200" s="102"/>
       <c r="C200" s="22" t="s">
         <v>128</v>
       </c>
@@ -14147,7 +14159,7 @@
       <c r="W200" s="77"/>
     </row>
     <row r="201" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B201" s="98"/>
+      <c r="B201" s="102"/>
       <c r="C201" s="22" t="s">
         <v>136</v>
       </c>
@@ -14206,7 +14218,7 @@
       <c r="W201" s="77"/>
     </row>
     <row r="202" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B202" s="98"/>
+      <c r="B202" s="102"/>
       <c r="C202" s="22" t="s">
         <v>75</v>
       </c>
@@ -14265,7 +14277,7 @@
       <c r="W202" s="77"/>
     </row>
     <row r="203" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B203" s="98"/>
+      <c r="B203" s="102"/>
       <c r="C203" s="22" t="s">
         <v>76</v>
       </c>
@@ -14324,7 +14336,7 @@
       <c r="W203" s="77"/>
     </row>
     <row r="204" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B204" s="98"/>
+      <c r="B204" s="102"/>
       <c r="C204" s="22" t="s">
         <v>78</v>
       </c>
@@ -14383,7 +14395,7 @@
       <c r="W204" s="77"/>
     </row>
     <row r="205" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B205" s="98"/>
+      <c r="B205" s="102"/>
       <c r="C205" s="22" t="s">
         <v>77</v>
       </c>
@@ -14442,7 +14454,7 @@
       <c r="W205" s="77"/>
     </row>
     <row r="206" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B206" s="98"/>
+      <c r="B206" s="102"/>
       <c r="C206" s="22" t="s">
         <v>94</v>
       </c>
@@ -14501,7 +14513,7 @@
       <c r="W206" s="77"/>
     </row>
     <row r="207" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B207" s="98"/>
+      <c r="B207" s="102"/>
       <c r="C207" s="22" t="s">
         <v>126</v>
       </c>
@@ -14560,7 +14572,7 @@
       <c r="W207" s="77"/>
     </row>
     <row r="208" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B208" s="98"/>
+      <c r="B208" s="102"/>
       <c r="C208" s="22" t="s">
         <v>95</v>
       </c>
@@ -14623,21 +14635,21 @@
       <c r="W208" s="63"/>
     </row>
     <row r="209" spans="2:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B209" s="106" t="s">
+      <c r="B209" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="C209" s="107"/>
-      <c r="D209" s="107"/>
-      <c r="E209" s="107"/>
-      <c r="F209" s="107"/>
-      <c r="G209" s="108"/>
+      <c r="C209" s="121"/>
+      <c r="D209" s="121"/>
+      <c r="E209" s="121"/>
+      <c r="F209" s="121"/>
+      <c r="G209" s="122"/>
       <c r="H209" s="25">
         <f t="shared" ref="H209:W209" si="7">SUM(H4:H208)</f>
         <v>113.84999999999995</v>
       </c>
       <c r="I209" s="16">
         <f t="shared" si="7"/>
-        <v>86.914299999999983</v>
+        <v>88.214299999999952</v>
       </c>
       <c r="J209" s="16">
         <f t="shared" si="7"/>
@@ -14693,7 +14705,7 @@
       </c>
       <c r="W209" s="19">
         <f t="shared" si="7"/>
-        <v>5.25</v>
+        <v>6.55</v>
       </c>
     </row>
     <row r="210" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14705,22 +14717,22 @@
       <c r="G210" s="2"/>
       <c r="H210" s="2"/>
       <c r="I210" s="2"/>
-      <c r="J210" s="102" t="s">
+      <c r="J210" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="K210" s="110"/>
-      <c r="L210" s="110"/>
-      <c r="M210" s="110"/>
-      <c r="N210" s="110"/>
-      <c r="O210" s="110"/>
-      <c r="P210" s="110"/>
-      <c r="Q210" s="110"/>
-      <c r="R210" s="110"/>
-      <c r="S210" s="110"/>
-      <c r="T210" s="110"/>
-      <c r="U210" s="110"/>
-      <c r="V210" s="110"/>
-      <c r="W210" s="111"/>
+      <c r="K210" s="99"/>
+      <c r="L210" s="99"/>
+      <c r="M210" s="99"/>
+      <c r="N210" s="99"/>
+      <c r="O210" s="99"/>
+      <c r="P210" s="99"/>
+      <c r="Q210" s="99"/>
+      <c r="R210" s="99"/>
+      <c r="S210" s="99"/>
+      <c r="T210" s="99"/>
+      <c r="U210" s="99"/>
+      <c r="V210" s="99"/>
+      <c r="W210" s="100"/>
     </row>
     <row r="211" spans="2:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C211" s="41" t="s">
@@ -14760,10 +14772,10 @@
       </c>
       <c r="F212" s="2"/>
       <c r="G212" s="2"/>
-      <c r="H212" s="100" t="s">
+      <c r="H212" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="I212" s="101"/>
+      <c r="I212" s="116"/>
       <c r="J212" s="9">
         <f>H209-J209</f>
         <v>113.84999999999995</v>
@@ -14818,7 +14830,7 @@
       </c>
       <c r="W212" s="71">
         <f t="shared" si="8"/>
-        <v>26.935699999999983</v>
+        <v>25.635699999999982</v>
       </c>
     </row>
     <row r="213" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14857,25 +14869,25 @@
       </c>
       <c r="D214" s="5">
         <f>SUM(I208,I205:I206,I198:I202,I172:I178,I56:I65,I4:I8)</f>
-        <v>45.8</v>
+        <v>47.099999999999994</v>
       </c>
       <c r="E214" s="5">
         <f>SUM(C214,-D214)</f>
-        <v>-21.4</v>
+        <v>-22.699999999999996</v>
       </c>
       <c r="F214" s="3"/>
-      <c r="H214" s="102" t="s">
+      <c r="H214" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="I214" s="103"/>
-      <c r="J214" s="101">
+      <c r="I214" s="117"/>
+      <c r="J214" s="116">
         <f>H209-I209</f>
-        <v>26.935699999999969</v>
-      </c>
-      <c r="K214" s="101"/>
-      <c r="L214" s="101"/>
-      <c r="M214" s="101"/>
-      <c r="N214" s="104"/>
+        <v>25.6357</v>
+      </c>
+      <c r="K214" s="116"/>
+      <c r="L214" s="116"/>
+      <c r="M214" s="116"/>
+      <c r="N214" s="118"/>
     </row>
     <row r="215" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B215" s="3"/>
@@ -14979,24 +14991,6 @@
     <row r="233" spans="2:3" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="C150:C156"/>
-    <mergeCell ref="C136:C142"/>
-    <mergeCell ref="C122:C128"/>
-    <mergeCell ref="C115:C121"/>
-    <mergeCell ref="C101:C107"/>
-    <mergeCell ref="C129:C135"/>
-    <mergeCell ref="C143:C149"/>
-    <mergeCell ref="C80:C86"/>
-    <mergeCell ref="J2:W2"/>
-    <mergeCell ref="B56:B65"/>
-    <mergeCell ref="C49:C55"/>
-    <mergeCell ref="C15:C48"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="C66:C72"/>
-    <mergeCell ref="C73:C79"/>
     <mergeCell ref="B187:B197"/>
     <mergeCell ref="H212:I212"/>
     <mergeCell ref="H214:I214"/>
@@ -15013,6 +15007,24 @@
     <mergeCell ref="C164:C170"/>
     <mergeCell ref="C94:C100"/>
     <mergeCell ref="C87:C93"/>
+    <mergeCell ref="C80:C86"/>
+    <mergeCell ref="J2:W2"/>
+    <mergeCell ref="B56:B65"/>
+    <mergeCell ref="C49:C55"/>
+    <mergeCell ref="C15:C48"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C66:C72"/>
+    <mergeCell ref="C73:C79"/>
+    <mergeCell ref="C150:C156"/>
+    <mergeCell ref="C136:C142"/>
+    <mergeCell ref="C122:C128"/>
+    <mergeCell ref="C115:C121"/>
+    <mergeCell ref="C101:C107"/>
+    <mergeCell ref="C129:C135"/>
+    <mergeCell ref="C143:C149"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>